<commit_message>
Let "TBD" return a false value
</commit_message>
<xml_diff>
--- a/report/merged_configurations.xlsx
+++ b/report/merged_configurations.xlsx
@@ -3712,7 +3712,7 @@
         <v>41</v>
       </c>
       <c r="E4" s="2">
-        <v>45222</v>
+        <v>45221.91666666667</v>
       </c>
       <c r="G4" t="s">
         <v>42</v>
@@ -3768,7 +3768,7 @@
         <v>41</v>
       </c>
       <c r="E5" s="2">
-        <v>45118</v>
+        <v>45117.91666666667</v>
       </c>
       <c r="F5" t="s">
         <v>50</v>
@@ -3801,7 +3801,7 @@
         <v>57</v>
       </c>
       <c r="P5" s="2">
-        <v>44974</v>
+        <v>44973.95833333333</v>
       </c>
       <c r="Q5" t="s">
         <v>26</v>
@@ -5556,7 +5556,7 @@
         <v>149</v>
       </c>
       <c r="E32" s="2">
-        <v>44679</v>
+        <v>44678.91666666667</v>
       </c>
       <c r="F32" t="s">
         <v>50</v>
@@ -5627,7 +5627,7 @@
         <v>164</v>
       </c>
       <c r="E33" s="2">
-        <v>44455</v>
+        <v>44454.91666666667</v>
       </c>
       <c r="F33" t="s">
         <v>50</v>
@@ -5660,7 +5660,7 @@
         <v>171</v>
       </c>
       <c r="P33" s="2">
-        <v>44455</v>
+        <v>44454.91666666667</v>
       </c>
       <c r="Q33" t="s">
         <v>172</v>
@@ -5669,7 +5669,7 @@
         <v>26</v>
       </c>
       <c r="S33" s="2">
-        <v>44730</v>
+        <v>44729.91666666667</v>
       </c>
       <c r="T33" t="s">
         <v>36</v>
@@ -5698,7 +5698,7 @@
         <v>164</v>
       </c>
       <c r="E34" s="2">
-        <v>44455</v>
+        <v>44454.91666666667</v>
       </c>
       <c r="F34" t="s">
         <v>50</v>
@@ -5731,7 +5731,7 @@
         <v>171</v>
       </c>
       <c r="P34" s="2">
-        <v>44455</v>
+        <v>44454.91666666667</v>
       </c>
       <c r="Q34" t="s">
         <v>172</v>
@@ -5740,7 +5740,7 @@
         <v>26</v>
       </c>
       <c r="S34" s="2">
-        <v>44730</v>
+        <v>44729.91666666667</v>
       </c>
       <c r="T34" t="s">
         <v>36</v>
@@ -5766,7 +5766,7 @@
         <v>149</v>
       </c>
       <c r="E35" s="2">
-        <v>44595</v>
+        <v>44594.95833333333</v>
       </c>
       <c r="F35" t="s">
         <v>26</v>
@@ -5834,7 +5834,7 @@
         <v>149</v>
       </c>
       <c r="E36" s="2">
-        <v>44595</v>
+        <v>44594.95833333333</v>
       </c>
       <c r="F36" t="s">
         <v>26</v>
@@ -5905,7 +5905,7 @@
         <v>191</v>
       </c>
       <c r="E37" s="2">
-        <v>44672</v>
+        <v>44671.91666666667</v>
       </c>
       <c r="F37" t="s">
         <v>192</v>
@@ -5938,13 +5938,13 @@
         <v>65</v>
       </c>
       <c r="P37" s="2">
-        <v>44147</v>
+        <v>44146.95833333333</v>
       </c>
       <c r="Q37" s="2">
-        <v>44637</v>
+        <v>44636.95833333333</v>
       </c>
       <c r="R37" s="2">
-        <v>44672</v>
+        <v>44671.91666666667</v>
       </c>
       <c r="S37" t="s">
         <v>36</v>
@@ -5976,7 +5976,7 @@
         <v>191</v>
       </c>
       <c r="E38" s="2">
-        <v>44672</v>
+        <v>44671.91666666667</v>
       </c>
       <c r="F38" t="s">
         <v>192</v>
@@ -6009,13 +6009,13 @@
         <v>65</v>
       </c>
       <c r="P38" s="2">
-        <v>44147</v>
+        <v>44146.95833333333</v>
       </c>
       <c r="Q38" s="2">
-        <v>44637</v>
+        <v>44636.95833333333</v>
       </c>
       <c r="R38" s="2">
-        <v>44672</v>
+        <v>44671.91666666667</v>
       </c>
       <c r="S38" t="s">
         <v>36</v>
@@ -6047,7 +6047,7 @@
         <v>191</v>
       </c>
       <c r="E39" s="2">
-        <v>44672</v>
+        <v>44671.91666666667</v>
       </c>
       <c r="F39" t="s">
         <v>192</v>
@@ -6080,13 +6080,13 @@
         <v>65</v>
       </c>
       <c r="P39" s="2">
-        <v>44147</v>
+        <v>44146.95833333333</v>
       </c>
       <c r="Q39" s="2">
-        <v>44637</v>
+        <v>44636.95833333333</v>
       </c>
       <c r="R39" s="2">
-        <v>44672</v>
+        <v>44671.91666666667</v>
       </c>
       <c r="S39" t="s">
         <v>36</v>
@@ -6118,7 +6118,7 @@
         <v>191</v>
       </c>
       <c r="E40" s="2">
-        <v>44672</v>
+        <v>44671.91666666667</v>
       </c>
       <c r="F40" t="s">
         <v>192</v>
@@ -6151,13 +6151,13 @@
         <v>65</v>
       </c>
       <c r="P40" s="2">
-        <v>44147</v>
+        <v>44146.95833333333</v>
       </c>
       <c r="Q40" s="2">
-        <v>44637</v>
+        <v>44636.95833333333</v>
       </c>
       <c r="R40" s="2">
-        <v>44672</v>
+        <v>44671.91666666667</v>
       </c>
       <c r="S40" t="s">
         <v>36</v>
@@ -6189,7 +6189,7 @@
         <v>41</v>
       </c>
       <c r="E41" s="2">
-        <v>43284</v>
+        <v>43283.91666666667</v>
       </c>
       <c r="F41" t="s">
         <v>50</v>
@@ -6331,7 +6331,7 @@
         <v>41</v>
       </c>
       <c r="E43" s="2">
-        <v>43431</v>
+        <v>43430.95833333333</v>
       </c>
       <c r="F43" t="s">
         <v>50</v>
@@ -6473,7 +6473,7 @@
         <v>41</v>
       </c>
       <c r="E45" s="2">
-        <v>43503</v>
+        <v>43502.95833333333</v>
       </c>
       <c r="F45" t="s">
         <v>50</v>
@@ -6544,7 +6544,7 @@
         <v>41</v>
       </c>
       <c r="E46" s="2">
-        <v>43503</v>
+        <v>43502.95833333333</v>
       </c>
       <c r="F46" t="s">
         <v>50</v>
@@ -6615,7 +6615,7 @@
         <v>41</v>
       </c>
       <c r="E47" s="2">
-        <v>43284</v>
+        <v>43283.91666666667</v>
       </c>
       <c r="F47" t="s">
         <v>50</v>
@@ -6757,7 +6757,7 @@
         <v>269</v>
       </c>
       <c r="E49" s="2">
-        <v>43503</v>
+        <v>43502.95833333333</v>
       </c>
       <c r="F49" t="s">
         <v>50</v>
@@ -6828,7 +6828,7 @@
         <v>41</v>
       </c>
       <c r="E50" s="2">
-        <v>43284</v>
+        <v>43283.91666666667</v>
       </c>
       <c r="F50" t="s">
         <v>50</v>
@@ -6970,7 +6970,7 @@
         <v>296</v>
       </c>
       <c r="E52" s="2">
-        <v>43804</v>
+        <v>43803.95833333333</v>
       </c>
       <c r="F52" t="s">
         <v>50</v>
@@ -7041,7 +7041,7 @@
         <v>296</v>
       </c>
       <c r="E53" s="2">
-        <v>43804</v>
+        <v>43803.95833333333</v>
       </c>
       <c r="F53" t="s">
         <v>50</v>
@@ -7183,7 +7183,7 @@
         <v>41</v>
       </c>
       <c r="E55" s="2">
-        <v>43284</v>
+        <v>43283.91666666667</v>
       </c>
       <c r="F55" t="s">
         <v>50</v>
@@ -7254,7 +7254,7 @@
         <v>41</v>
       </c>
       <c r="E56" s="2">
-        <v>43412</v>
+        <v>43411.95833333333</v>
       </c>
       <c r="F56" t="s">
         <v>50</v>
@@ -7325,7 +7325,7 @@
         <v>41</v>
       </c>
       <c r="E57" s="2">
-        <v>43412</v>
+        <v>43411.95833333333</v>
       </c>
       <c r="F57" t="s">
         <v>50</v>
@@ -7467,7 +7467,7 @@
         <v>41</v>
       </c>
       <c r="E59" s="2">
-        <v>43503</v>
+        <v>43502.95833333333</v>
       </c>
       <c r="F59" t="s">
         <v>50</v>
@@ -7538,7 +7538,7 @@
         <v>41</v>
       </c>
       <c r="E60" s="2">
-        <v>43503</v>
+        <v>43502.95833333333</v>
       </c>
       <c r="F60" t="s">
         <v>50</v>
@@ -7609,7 +7609,7 @@
         <v>41</v>
       </c>
       <c r="E61" s="2">
-        <v>43503</v>
+        <v>43502.95833333333</v>
       </c>
       <c r="F61" t="s">
         <v>50</v>
@@ -7680,7 +7680,7 @@
         <v>41</v>
       </c>
       <c r="E62" s="2">
-        <v>43503</v>
+        <v>43502.95833333333</v>
       </c>
       <c r="F62" t="s">
         <v>50</v>
@@ -7751,7 +7751,7 @@
         <v>41</v>
       </c>
       <c r="E63" s="2">
-        <v>43503</v>
+        <v>43502.95833333333</v>
       </c>
       <c r="F63" t="s">
         <v>50</v>
@@ -7819,7 +7819,7 @@
         <v>369</v>
       </c>
       <c r="E64" s="2">
-        <v>45194</v>
+        <v>45193.91666666667</v>
       </c>
       <c r="F64" t="s">
         <v>50</v>
@@ -7887,7 +7887,7 @@
         <v>369</v>
       </c>
       <c r="E65" s="2">
-        <v>45194</v>
+        <v>45193.91666666667</v>
       </c>
       <c r="F65" t="s">
         <v>50</v>
@@ -8100,7 +8100,7 @@
         <v>400</v>
       </c>
       <c r="E68" s="2">
-        <v>43944</v>
+        <v>43943.91666666667</v>
       </c>
       <c r="F68" t="s">
         <v>50</v>
@@ -8171,7 +8171,7 @@
         <v>400</v>
       </c>
       <c r="E69" s="2">
-        <v>43944</v>
+        <v>43943.91666666667</v>
       </c>
       <c r="F69" t="s">
         <v>50</v>
@@ -8242,7 +8242,7 @@
         <v>400</v>
       </c>
       <c r="E70" s="2">
-        <v>43944</v>
+        <v>43943.91666666667</v>
       </c>
       <c r="F70" t="s">
         <v>50</v>
@@ -8313,7 +8313,7 @@
         <v>400</v>
       </c>
       <c r="E71" s="2">
-        <v>43944</v>
+        <v>43943.91666666667</v>
       </c>
       <c r="F71" t="s">
         <v>50</v>
@@ -8384,7 +8384,7 @@
         <v>41</v>
       </c>
       <c r="E72" s="2">
-        <v>44532</v>
+        <v>44531.95833333333</v>
       </c>
       <c r="F72" t="s">
         <v>50</v>
@@ -8452,7 +8452,7 @@
         <v>41</v>
       </c>
       <c r="E73" s="2">
-        <v>43503</v>
+        <v>43502.95833333333</v>
       </c>
       <c r="F73" t="s">
         <v>50</v>
@@ -8523,7 +8523,7 @@
         <v>41</v>
       </c>
       <c r="E74" s="2">
-        <v>43503</v>
+        <v>43502.95833333333</v>
       </c>
       <c r="F74" t="s">
         <v>50</v>
@@ -8594,7 +8594,7 @@
         <v>41</v>
       </c>
       <c r="E75" s="2">
-        <v>43503</v>
+        <v>43502.95833333333</v>
       </c>
       <c r="F75" t="s">
         <v>50</v>
@@ -8665,7 +8665,7 @@
         <v>463</v>
       </c>
       <c r="E76" s="2">
-        <v>44000</v>
+        <v>43999.91666666667</v>
       </c>
       <c r="F76" t="s">
         <v>50</v>
@@ -8736,7 +8736,7 @@
         <v>463</v>
       </c>
       <c r="E77" s="2">
-        <v>44000</v>
+        <v>43999.91666666667</v>
       </c>
       <c r="F77" t="s">
         <v>50</v>
@@ -8807,7 +8807,7 @@
         <v>463</v>
       </c>
       <c r="E78" s="2">
-        <v>44000</v>
+        <v>43999.91666666667</v>
       </c>
       <c r="F78" t="s">
         <v>50</v>
@@ -8878,7 +8878,7 @@
         <v>463</v>
       </c>
       <c r="E79" s="2">
-        <v>44000</v>
+        <v>43999.91666666667</v>
       </c>
       <c r="F79" t="s">
         <v>50</v>
@@ -8949,7 +8949,7 @@
         <v>490</v>
       </c>
       <c r="E80" s="2">
-        <v>43301</v>
+        <v>43300.91666666667</v>
       </c>
       <c r="F80" t="s">
         <v>50</v>
@@ -9020,7 +9020,7 @@
         <v>490</v>
       </c>
       <c r="E81" s="2">
-        <v>43301</v>
+        <v>43300.91666666667</v>
       </c>
       <c r="F81" t="s">
         <v>498</v>
@@ -9091,7 +9091,7 @@
         <v>490</v>
       </c>
       <c r="E82" s="2">
-        <v>43301</v>
+        <v>43300.91666666667</v>
       </c>
       <c r="F82" t="s">
         <v>50</v>
@@ -9162,7 +9162,7 @@
         <v>490</v>
       </c>
       <c r="E83" s="2">
-        <v>43301</v>
+        <v>43300.91666666667</v>
       </c>
       <c r="F83" t="s">
         <v>498</v>
@@ -9233,7 +9233,7 @@
         <v>490</v>
       </c>
       <c r="E84" s="2">
-        <v>43277</v>
+        <v>43276.91666666667</v>
       </c>
       <c r="F84" t="s">
         <v>498</v>
@@ -9301,7 +9301,7 @@
         <v>41</v>
       </c>
       <c r="E85" s="2">
-        <v>43242</v>
+        <v>43241.91666666667</v>
       </c>
       <c r="F85" t="s">
         <v>520</v>
@@ -9369,7 +9369,7 @@
         <v>41</v>
       </c>
       <c r="E86" s="2">
-        <v>43242</v>
+        <v>43241.91666666667</v>
       </c>
       <c r="F86" t="s">
         <v>520</v>
@@ -9437,7 +9437,7 @@
         <v>41</v>
       </c>
       <c r="E87" s="2">
-        <v>43242</v>
+        <v>43241.91666666667</v>
       </c>
       <c r="F87" t="s">
         <v>50</v>
@@ -9508,7 +9508,7 @@
         <v>41</v>
       </c>
       <c r="E88" s="2">
-        <v>43431</v>
+        <v>43430.95833333333</v>
       </c>
       <c r="F88" t="s">
         <v>50</v>
@@ -9579,7 +9579,7 @@
         <v>41</v>
       </c>
       <c r="E89" s="2">
-        <v>43431</v>
+        <v>43430.95833333333</v>
       </c>
       <c r="F89" t="s">
         <v>50</v>
@@ -9650,7 +9650,7 @@
         <v>41</v>
       </c>
       <c r="E90" s="2">
-        <v>43431</v>
+        <v>43430.95833333333</v>
       </c>
       <c r="F90" t="s">
         <v>50</v>
@@ -9721,7 +9721,7 @@
         <v>41</v>
       </c>
       <c r="E91" s="2">
-        <v>43431</v>
+        <v>43430.95833333333</v>
       </c>
       <c r="F91" t="s">
         <v>50</v>
@@ -9792,7 +9792,7 @@
         <v>41</v>
       </c>
       <c r="E92" s="2">
-        <v>43431</v>
+        <v>43430.95833333333</v>
       </c>
       <c r="F92" t="s">
         <v>50</v>
@@ -9863,7 +9863,7 @@
         <v>41</v>
       </c>
       <c r="E93" s="2">
-        <v>43431</v>
+        <v>43430.95833333333</v>
       </c>
       <c r="F93" t="s">
         <v>50</v>
@@ -9934,7 +9934,7 @@
         <v>41</v>
       </c>
       <c r="E94" s="2">
-        <v>43431</v>
+        <v>43430.95833333333</v>
       </c>
       <c r="F94" t="s">
         <v>50</v>
@@ -10005,7 +10005,7 @@
         <v>41</v>
       </c>
       <c r="E95" s="2">
-        <v>43431</v>
+        <v>43430.95833333333</v>
       </c>
       <c r="F95" t="s">
         <v>50</v>
@@ -10076,7 +10076,7 @@
         <v>41</v>
       </c>
       <c r="E96" s="2">
-        <v>43431</v>
+        <v>43430.95833333333</v>
       </c>
       <c r="F96" t="s">
         <v>50</v>
@@ -10147,7 +10147,7 @@
         <v>41</v>
       </c>
       <c r="E97" s="2">
-        <v>43431</v>
+        <v>43430.95833333333</v>
       </c>
       <c r="F97" t="s">
         <v>50</v>
@@ -10218,7 +10218,7 @@
         <v>41</v>
       </c>
       <c r="E98" s="2">
-        <v>43431</v>
+        <v>43430.95833333333</v>
       </c>
       <c r="F98" t="s">
         <v>50</v>
@@ -10289,7 +10289,7 @@
         <v>41</v>
       </c>
       <c r="E99" s="2">
-        <v>43431</v>
+        <v>43430.95833333333</v>
       </c>
       <c r="F99" t="s">
         <v>50</v>
@@ -10360,7 +10360,7 @@
         <v>41</v>
       </c>
       <c r="E100" s="2">
-        <v>43431</v>
+        <v>43430.95833333333</v>
       </c>
       <c r="F100" t="s">
         <v>50</v>
@@ -10431,7 +10431,7 @@
         <v>41</v>
       </c>
       <c r="E101" s="2">
-        <v>43431</v>
+        <v>43430.95833333333</v>
       </c>
       <c r="F101" t="s">
         <v>50</v>
@@ -10502,7 +10502,7 @@
         <v>41</v>
       </c>
       <c r="E102" s="2">
-        <v>43431</v>
+        <v>43430.95833333333</v>
       </c>
       <c r="F102" t="s">
         <v>50</v>
@@ -10573,7 +10573,7 @@
         <v>41</v>
       </c>
       <c r="E103" s="2">
-        <v>43431</v>
+        <v>43430.95833333333</v>
       </c>
       <c r="F103" t="s">
         <v>50</v>
@@ -10715,7 +10715,7 @@
         <v>269</v>
       </c>
       <c r="E105" s="2">
-        <v>44231</v>
+        <v>44230.95833333333</v>
       </c>
       <c r="F105" t="s">
         <v>50</v>
@@ -10786,7 +10786,7 @@
         <v>269</v>
       </c>
       <c r="E106" s="2">
-        <v>44231</v>
+        <v>44230.95833333333</v>
       </c>
       <c r="F106" t="s">
         <v>50</v>
@@ -10857,7 +10857,7 @@
         <v>149</v>
       </c>
       <c r="E107" s="2">
-        <v>44308</v>
+        <v>44307.91666666667</v>
       </c>
       <c r="F107" t="s">
         <v>192</v>
@@ -10893,10 +10893,10 @@
         <v>609</v>
       </c>
       <c r="Q107" s="2">
-        <v>44266</v>
+        <v>44265.95833333333</v>
       </c>
       <c r="R107" s="2">
-        <v>44308</v>
+        <v>44307.91666666667</v>
       </c>
       <c r="S107" t="s">
         <v>36</v>
@@ -10928,7 +10928,7 @@
         <v>149</v>
       </c>
       <c r="E108" s="2">
-        <v>44308</v>
+        <v>44307.91666666667</v>
       </c>
       <c r="F108" t="s">
         <v>192</v>
@@ -10964,10 +10964,10 @@
         <v>609</v>
       </c>
       <c r="Q108" s="2">
-        <v>44266</v>
+        <v>44265.95833333333</v>
       </c>
       <c r="R108" s="2">
-        <v>44308</v>
+        <v>44307.91666666667</v>
       </c>
       <c r="S108" t="s">
         <v>36</v>
@@ -10999,7 +10999,7 @@
         <v>149</v>
       </c>
       <c r="E109" s="2">
-        <v>44308</v>
+        <v>44307.91666666667</v>
       </c>
       <c r="F109" t="s">
         <v>50</v>
@@ -11032,13 +11032,13 @@
         <v>65</v>
       </c>
       <c r="P109" s="2">
-        <v>43789</v>
+        <v>43788.95833333333</v>
       </c>
       <c r="Q109" s="2">
-        <v>44266</v>
+        <v>44265.95833333333</v>
       </c>
       <c r="R109" s="2">
-        <v>44308</v>
+        <v>44307.91666666667</v>
       </c>
       <c r="S109" t="s">
         <v>36</v>
@@ -11212,7 +11212,7 @@
         <v>41</v>
       </c>
       <c r="E112" s="2">
-        <v>42817</v>
+        <v>42816.95833333333</v>
       </c>
       <c r="F112" t="s">
         <v>50</v>
@@ -11274,7 +11274,7 @@
         <v>41</v>
       </c>
       <c r="E113" s="2">
-        <v>42825</v>
+        <v>42824.91666666667</v>
       </c>
       <c r="F113" t="s">
         <v>50</v>
@@ -12966,7 +12966,7 @@
         <v>25</v>
       </c>
       <c r="E137" s="2">
-        <v>44308</v>
+        <v>44307.91666666667</v>
       </c>
       <c r="F137" t="s">
         <v>192</v>
@@ -12999,13 +12999,13 @@
         <v>34</v>
       </c>
       <c r="P137" s="2">
-        <v>44032</v>
+        <v>44031.91666666667</v>
       </c>
       <c r="Q137" s="2">
-        <v>44266</v>
+        <v>44265.95833333333</v>
       </c>
       <c r="R137" s="2">
-        <v>44308</v>
+        <v>44307.91666666667</v>
       </c>
       <c r="S137" t="s">
         <v>36</v>
@@ -13037,7 +13037,7 @@
         <v>25</v>
       </c>
       <c r="E138" s="2">
-        <v>44308</v>
+        <v>44307.91666666667</v>
       </c>
       <c r="F138" t="s">
         <v>192</v>
@@ -13070,13 +13070,13 @@
         <v>34</v>
       </c>
       <c r="P138" s="2">
-        <v>44397</v>
+        <v>44396.91666666667</v>
       </c>
       <c r="Q138" s="2">
-        <v>44266</v>
+        <v>44265.95833333333</v>
       </c>
       <c r="R138" s="2">
-        <v>44308</v>
+        <v>44307.91666666667</v>
       </c>
       <c r="S138" t="s">
         <v>36</v>
@@ -13173,7 +13173,7 @@
         <v>582</v>
       </c>
       <c r="E140" s="2">
-        <v>44167</v>
+        <v>44166.95833333333</v>
       </c>
       <c r="F140" t="s">
         <v>50</v>
@@ -13241,7 +13241,7 @@
         <v>582</v>
       </c>
       <c r="E141" s="2">
-        <v>44167</v>
+        <v>44166.95833333333</v>
       </c>
       <c r="F141" t="s">
         <v>50</v>
@@ -13309,7 +13309,7 @@
         <v>582</v>
       </c>
       <c r="E142" s="2">
-        <v>44167</v>
+        <v>44166.95833333333</v>
       </c>
       <c r="F142" t="s">
         <v>50</v>
@@ -13377,7 +13377,7 @@
         <v>582</v>
       </c>
       <c r="E143" s="2">
-        <v>44167</v>
+        <v>44166.95833333333</v>
       </c>
       <c r="F143" t="s">
         <v>50</v>
@@ -13445,7 +13445,7 @@
         <v>582</v>
       </c>
       <c r="E144" s="2">
-        <v>44167</v>
+        <v>44166.95833333333</v>
       </c>
       <c r="F144" t="s">
         <v>50</v>
@@ -13513,7 +13513,7 @@
         <v>582</v>
       </c>
       <c r="E145" s="2">
-        <v>44167</v>
+        <v>44166.95833333333</v>
       </c>
       <c r="F145" t="s">
         <v>50</v>
@@ -13581,7 +13581,7 @@
         <v>582</v>
       </c>
       <c r="E146" s="2">
-        <v>44167</v>
+        <v>44166.95833333333</v>
       </c>
       <c r="F146" t="s">
         <v>50</v>
@@ -13649,7 +13649,7 @@
         <v>582</v>
       </c>
       <c r="E147" s="2">
-        <v>44167</v>
+        <v>44166.95833333333</v>
       </c>
       <c r="F147" t="s">
         <v>50</v>
@@ -13717,7 +13717,7 @@
         <v>582</v>
       </c>
       <c r="E148" s="2">
-        <v>44167</v>
+        <v>44166.95833333333</v>
       </c>
       <c r="F148" t="s">
         <v>50</v>
@@ -13785,7 +13785,7 @@
         <v>582</v>
       </c>
       <c r="E149" s="2">
-        <v>44167</v>
+        <v>44166.95833333333</v>
       </c>
       <c r="F149" t="s">
         <v>50</v>
@@ -13853,7 +13853,7 @@
         <v>582</v>
       </c>
       <c r="E150" s="2">
-        <v>44167</v>
+        <v>44166.95833333333</v>
       </c>
       <c r="F150" t="s">
         <v>50</v>
@@ -13921,7 +13921,7 @@
         <v>582</v>
       </c>
       <c r="E151" s="2">
-        <v>44167</v>
+        <v>44166.95833333333</v>
       </c>
       <c r="F151" t="s">
         <v>50</v>
@@ -13989,7 +13989,7 @@
         <v>582</v>
       </c>
       <c r="E152" s="2">
-        <v>44167</v>
+        <v>44166.95833333333</v>
       </c>
       <c r="F152" t="s">
         <v>50</v>
@@ -14057,7 +14057,7 @@
         <v>582</v>
       </c>
       <c r="E153" s="2">
-        <v>44167</v>
+        <v>44166.95833333333</v>
       </c>
       <c r="F153" t="s">
         <v>50</v>
@@ -14125,7 +14125,7 @@
         <v>582</v>
       </c>
       <c r="E154" s="2">
-        <v>44167</v>
+        <v>44166.95833333333</v>
       </c>
       <c r="F154" t="s">
         <v>50</v>
@@ -14193,7 +14193,7 @@
         <v>582</v>
       </c>
       <c r="E155" s="2">
-        <v>44167</v>
+        <v>44166.95833333333</v>
       </c>
       <c r="F155" t="s">
         <v>50</v>
@@ -14261,7 +14261,7 @@
         <v>582</v>
       </c>
       <c r="E156" s="2">
-        <v>44167</v>
+        <v>44166.95833333333</v>
       </c>
       <c r="F156" t="s">
         <v>50</v>
@@ -14329,7 +14329,7 @@
         <v>582</v>
       </c>
       <c r="E157" s="2">
-        <v>44167</v>
+        <v>44166.95833333333</v>
       </c>
       <c r="F157" t="s">
         <v>50</v>
@@ -14397,7 +14397,7 @@
         <v>582</v>
       </c>
       <c r="E158" s="2">
-        <v>44167</v>
+        <v>44166.95833333333</v>
       </c>
       <c r="F158" t="s">
         <v>50</v>
@@ -14465,7 +14465,7 @@
         <v>582</v>
       </c>
       <c r="E159" s="2">
-        <v>44167</v>
+        <v>44166.95833333333</v>
       </c>
       <c r="F159" t="s">
         <v>50</v>
@@ -14533,7 +14533,7 @@
         <v>582</v>
       </c>
       <c r="E160" s="2">
-        <v>44167</v>
+        <v>44166.95833333333</v>
       </c>
       <c r="F160" t="s">
         <v>50</v>
@@ -14601,7 +14601,7 @@
         <v>582</v>
       </c>
       <c r="E161" s="2">
-        <v>44167</v>
+        <v>44166.95833333333</v>
       </c>
       <c r="F161" t="s">
         <v>50</v>
@@ -14669,7 +14669,7 @@
         <v>582</v>
       </c>
       <c r="E162" s="2">
-        <v>44167</v>
+        <v>44166.95833333333</v>
       </c>
       <c r="F162" t="s">
         <v>50</v>
@@ -14737,7 +14737,7 @@
         <v>582</v>
       </c>
       <c r="E163" s="2">
-        <v>44167</v>
+        <v>44166.95833333333</v>
       </c>
       <c r="F163" t="s">
         <v>50</v>
@@ -14805,7 +14805,7 @@
         <v>582</v>
       </c>
       <c r="E164" s="2">
-        <v>44167</v>
+        <v>44166.95833333333</v>
       </c>
       <c r="F164" t="s">
         <v>50</v>
@@ -14873,7 +14873,7 @@
         <v>582</v>
       </c>
       <c r="E165" s="2">
-        <v>44167</v>
+        <v>44166.95833333333</v>
       </c>
       <c r="F165" t="s">
         <v>50</v>
@@ -14941,7 +14941,7 @@
         <v>582</v>
       </c>
       <c r="E166" s="2">
-        <v>44167</v>
+        <v>44166.95833333333</v>
       </c>
       <c r="F166" t="s">
         <v>50</v>
@@ -15009,7 +15009,7 @@
         <v>582</v>
       </c>
       <c r="E167" s="2">
-        <v>44167</v>
+        <v>44166.95833333333</v>
       </c>
       <c r="F167" t="s">
         <v>50</v>
@@ -15077,7 +15077,7 @@
         <v>582</v>
       </c>
       <c r="E168" s="2">
-        <v>44167</v>
+        <v>44166.95833333333</v>
       </c>
       <c r="F168" t="s">
         <v>50</v>
@@ -15145,7 +15145,7 @@
         <v>582</v>
       </c>
       <c r="E169" s="2">
-        <v>44167</v>
+        <v>44166.95833333333</v>
       </c>
       <c r="F169" t="s">
         <v>50</v>
@@ -15213,7 +15213,7 @@
         <v>582</v>
       </c>
       <c r="E170" s="2">
-        <v>44167</v>
+        <v>44166.95833333333</v>
       </c>
       <c r="F170" t="s">
         <v>50</v>
@@ -15281,7 +15281,7 @@
         <v>582</v>
       </c>
       <c r="E171" s="2">
-        <v>44167</v>
+        <v>44166.95833333333</v>
       </c>
       <c r="F171" t="s">
         <v>50</v>
@@ -15349,7 +15349,7 @@
         <v>582</v>
       </c>
       <c r="E172" s="2">
-        <v>44167</v>
+        <v>44166.95833333333</v>
       </c>
       <c r="F172" t="s">
         <v>50</v>
@@ -15417,7 +15417,7 @@
         <v>582</v>
       </c>
       <c r="E173" s="2">
-        <v>44167</v>
+        <v>44166.95833333333</v>
       </c>
       <c r="F173" t="s">
         <v>50</v>
@@ -15485,7 +15485,7 @@
         <v>582</v>
       </c>
       <c r="E174" s="2">
-        <v>44167</v>
+        <v>44166.95833333333</v>
       </c>
       <c r="F174" t="s">
         <v>50</v>
@@ -15553,7 +15553,7 @@
         <v>582</v>
       </c>
       <c r="E175" s="2">
-        <v>44167</v>
+        <v>44166.95833333333</v>
       </c>
       <c r="F175" t="s">
         <v>50</v>
@@ -15621,7 +15621,7 @@
         <v>582</v>
       </c>
       <c r="E176" s="2">
-        <v>44167</v>
+        <v>44166.95833333333</v>
       </c>
       <c r="F176" t="s">
         <v>50</v>
@@ -15689,7 +15689,7 @@
         <v>582</v>
       </c>
       <c r="E177" s="2">
-        <v>44167</v>
+        <v>44166.95833333333</v>
       </c>
       <c r="F177" t="s">
         <v>50</v>
@@ -15757,7 +15757,7 @@
         <v>582</v>
       </c>
       <c r="E178" s="2">
-        <v>44167</v>
+        <v>44166.95833333333</v>
       </c>
       <c r="F178" t="s">
         <v>50</v>
@@ -15825,7 +15825,7 @@
         <v>582</v>
       </c>
       <c r="E179" s="2">
-        <v>44167</v>
+        <v>44166.95833333333</v>
       </c>
       <c r="F179" t="s">
         <v>50</v>
@@ -15893,7 +15893,7 @@
         <v>582</v>
       </c>
       <c r="E180" s="2">
-        <v>44167</v>
+        <v>44166.95833333333</v>
       </c>
       <c r="F180" t="s">
         <v>50</v>
@@ -16100,7 +16100,7 @@
         <v>41</v>
       </c>
       <c r="E183" s="2">
-        <v>44532</v>
+        <v>44531.95833333333</v>
       </c>
       <c r="F183" t="s">
         <v>50</v>
@@ -16307,7 +16307,7 @@
         <v>41</v>
       </c>
       <c r="E186" s="2">
-        <v>44595</v>
+        <v>44594.95833333333</v>
       </c>
       <c r="F186" t="s">
         <v>50</v>
@@ -16375,7 +16375,7 @@
         <v>41</v>
       </c>
       <c r="E187" s="2">
-        <v>44896</v>
+        <v>44895.95833333333</v>
       </c>
       <c r="F187" t="s">
         <v>50</v>
@@ -16408,13 +16408,13 @@
         <v>57</v>
       </c>
       <c r="P187" s="2">
-        <v>44453</v>
+        <v>44452.91666666667</v>
       </c>
       <c r="Q187" s="2">
-        <v>44875</v>
+        <v>44874.95833333333</v>
       </c>
       <c r="R187" s="2">
-        <v>44896</v>
+        <v>44895.95833333333</v>
       </c>
       <c r="S187" t="s">
         <v>36</v>
@@ -16443,7 +16443,7 @@
         <v>41</v>
       </c>
       <c r="E188" s="2">
-        <v>44896</v>
+        <v>44895.95833333333</v>
       </c>
       <c r="F188" t="s">
         <v>50</v>
@@ -16476,13 +16476,13 @@
         <v>57</v>
       </c>
       <c r="P188" s="2">
-        <v>44453</v>
+        <v>44452.91666666667</v>
       </c>
       <c r="Q188" s="2">
-        <v>44875</v>
+        <v>44874.95833333333</v>
       </c>
       <c r="R188" s="2">
-        <v>44896</v>
+        <v>44895.95833333333</v>
       </c>
       <c r="S188" t="s">
         <v>36</v>
@@ -16511,7 +16511,7 @@
         <v>41</v>
       </c>
       <c r="E189" s="2">
-        <v>44896</v>
+        <v>44895.95833333333</v>
       </c>
       <c r="F189" t="s">
         <v>50</v>
@@ -16573,7 +16573,7 @@
         <v>41</v>
       </c>
       <c r="E190" s="2">
-        <v>44896</v>
+        <v>44895.95833333333</v>
       </c>
       <c r="F190" t="s">
         <v>50</v>
@@ -16635,7 +16635,7 @@
         <v>149</v>
       </c>
       <c r="E191" s="2">
-        <v>44641</v>
+        <v>44640.95833333333</v>
       </c>
       <c r="F191" t="s">
         <v>26</v>
@@ -16839,7 +16839,7 @@
         <v>41</v>
       </c>
       <c r="E194" s="2">
-        <v>44896</v>
+        <v>44895.95833333333</v>
       </c>
       <c r="F194" t="s">
         <v>50</v>
@@ -16875,10 +16875,10 @@
         <v>26</v>
       </c>
       <c r="R194" s="2">
-        <v>44896</v>
+        <v>44895.95833333333</v>
       </c>
       <c r="S194" s="2">
-        <v>44845</v>
+        <v>44844.91666666667</v>
       </c>
       <c r="T194" t="s">
         <v>36</v>
@@ -16904,7 +16904,7 @@
         <v>41</v>
       </c>
       <c r="E195" s="2">
-        <v>44896</v>
+        <v>44895.95833333333</v>
       </c>
       <c r="F195" t="s">
         <v>50</v>
@@ -16940,10 +16940,10 @@
         <v>26</v>
       </c>
       <c r="R195" s="2">
-        <v>44896</v>
+        <v>44895.95833333333</v>
       </c>
       <c r="S195" s="2">
-        <v>44845</v>
+        <v>44844.91666666667</v>
       </c>
       <c r="T195" t="s">
         <v>36</v>
@@ -16969,7 +16969,7 @@
         <v>41</v>
       </c>
       <c r="E196" s="2">
-        <v>44915</v>
+        <v>44914.95833333333</v>
       </c>
       <c r="F196" t="s">
         <v>50</v>
@@ -17037,7 +17037,7 @@
         <v>41</v>
       </c>
       <c r="E197" s="2">
-        <v>45239</v>
+        <v>45238.95833333333</v>
       </c>
       <c r="F197" t="s">
         <v>50</v>
@@ -17070,10 +17070,10 @@
         <v>57</v>
       </c>
       <c r="P197" s="2">
-        <v>44812</v>
+        <v>44811.91666666667</v>
       </c>
       <c r="Q197" s="2">
-        <v>45239</v>
+        <v>45238.95833333333</v>
       </c>
       <c r="R197" t="s">
         <v>26</v>
@@ -17105,7 +17105,7 @@
         <v>41</v>
       </c>
       <c r="E198" s="2">
-        <v>45239</v>
+        <v>45238.95833333333</v>
       </c>
       <c r="F198" t="s">
         <v>50</v>
@@ -17138,10 +17138,10 @@
         <v>57</v>
       </c>
       <c r="P198" s="2">
-        <v>44812</v>
+        <v>44811.91666666667</v>
       </c>
       <c r="Q198" s="2">
-        <v>45239</v>
+        <v>45238.95833333333</v>
       </c>
       <c r="R198" t="s">
         <v>26</v>
@@ -17335,7 +17335,7 @@
         <v>41</v>
       </c>
       <c r="E202" s="2">
-        <v>45131</v>
+        <v>45130.91666666667</v>
       </c>
       <c r="F202" t="s">
         <v>50</v>
@@ -17368,7 +17368,7 @@
         <v>57</v>
       </c>
       <c r="P202" s="2">
-        <v>44873</v>
+        <v>44872.95833333333</v>
       </c>
       <c r="Q202" t="s">
         <v>26</v>
@@ -17403,7 +17403,7 @@
         <v>41</v>
       </c>
       <c r="E203" s="2">
-        <v>45131</v>
+        <v>45130.91666666667</v>
       </c>
       <c r="F203" t="s">
         <v>50</v>
@@ -17436,7 +17436,7 @@
         <v>57</v>
       </c>
       <c r="P203" s="2">
-        <v>44873</v>
+        <v>44872.95833333333</v>
       </c>
       <c r="Q203" t="s">
         <v>26</v>
@@ -17471,7 +17471,7 @@
         <v>490</v>
       </c>
       <c r="E204" s="2">
-        <v>45236</v>
+        <v>45235.95833333333</v>
       </c>
       <c r="F204" t="s">
         <v>50</v>
@@ -17611,11 +17611,11 @@
       <c r="D2" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="E2" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="F2" s="3" t="b">
-        <v>1</v>
+      <c r="E2" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="F2" s="4" t="b">
+        <v>0</v>
       </c>
       <c r="G2" s="3" t="b">
         <v>1</v>
@@ -17647,11 +17647,11 @@
       <c r="P2" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="Q2" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="R2" s="3" t="b">
-        <v>1</v>
+      <c r="Q2" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="R2" s="4" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
@@ -17667,11 +17667,11 @@
       <c r="D3" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="E3" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="F3" s="3" t="b">
-        <v>1</v>
+      <c r="E3" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="F3" s="4" t="b">
+        <v>0</v>
       </c>
       <c r="G3" s="3" t="b">
         <v>1</v>
@@ -17703,11 +17703,11 @@
       <c r="P3" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="Q3" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="R3" s="3" t="b">
-        <v>1</v>
+      <c r="Q3" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="R3" s="4" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
@@ -17815,11 +17815,11 @@
       <c r="P5" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="Q5" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="R5" s="3" t="b">
-        <v>1</v>
+      <c r="Q5" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="R5" s="4" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
@@ -18171,11 +18171,11 @@
       <c r="D12" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="E12" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="F12" s="3" t="b">
-        <v>1</v>
+      <c r="E12" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="F12" s="4" t="b">
+        <v>0</v>
       </c>
       <c r="G12" s="3" t="b">
         <v>1</v>
@@ -18207,11 +18207,11 @@
       <c r="P12" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="Q12" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="R12" s="3" t="b">
-        <v>1</v>
+      <c r="Q12" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="R12" s="4" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
@@ -18227,11 +18227,11 @@
       <c r="D13" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="E13" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="F13" s="3" t="b">
-        <v>1</v>
+      <c r="E13" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="F13" s="4" t="b">
+        <v>0</v>
       </c>
       <c r="G13" s="3" t="b">
         <v>1</v>
@@ -18263,11 +18263,11 @@
       <c r="P13" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="Q13" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="R13" s="3" t="b">
-        <v>1</v>
+      <c r="Q13" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="R13" s="4" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
@@ -18283,11 +18283,11 @@
       <c r="D14" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="E14" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="F14" s="3" t="b">
-        <v>1</v>
+      <c r="E14" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="F14" s="4" t="b">
+        <v>0</v>
       </c>
       <c r="G14" s="3" t="b">
         <v>1</v>
@@ -18319,11 +18319,11 @@
       <c r="P14" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="Q14" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="R14" s="3" t="b">
-        <v>1</v>
+      <c r="Q14" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="R14" s="4" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
@@ -18339,11 +18339,11 @@
       <c r="D15" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="E15" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="F15" s="3" t="b">
-        <v>1</v>
+      <c r="E15" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="F15" s="4" t="b">
+        <v>0</v>
       </c>
       <c r="G15" s="3" t="b">
         <v>1</v>
@@ -18375,11 +18375,11 @@
       <c r="P15" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="Q15" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="R15" s="3" t="b">
-        <v>1</v>
+      <c r="Q15" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="R15" s="4" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
@@ -18395,11 +18395,11 @@
       <c r="D16" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="E16" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="F16" s="3" t="b">
-        <v>1</v>
+      <c r="E16" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="F16" s="4" t="b">
+        <v>0</v>
       </c>
       <c r="G16" s="3" t="b">
         <v>1</v>
@@ -18431,11 +18431,11 @@
       <c r="P16" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="Q16" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="R16" s="3" t="b">
-        <v>1</v>
+      <c r="Q16" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="R16" s="4" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.25">
@@ -18451,11 +18451,11 @@
       <c r="D17" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="E17" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="F17" s="3" t="b">
-        <v>1</v>
+      <c r="E17" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="F17" s="4" t="b">
+        <v>0</v>
       </c>
       <c r="G17" s="3" t="b">
         <v>1</v>
@@ -18487,11 +18487,11 @@
       <c r="P17" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="Q17" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="R17" s="3" t="b">
-        <v>1</v>
+      <c r="Q17" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="R17" s="4" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.25">
@@ -18507,11 +18507,11 @@
       <c r="D18" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="E18" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="F18" s="3" t="b">
-        <v>1</v>
+      <c r="E18" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="F18" s="4" t="b">
+        <v>0</v>
       </c>
       <c r="G18" s="3" t="b">
         <v>1</v>
@@ -18543,11 +18543,11 @@
       <c r="P18" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="Q18" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="R18" s="3" t="b">
-        <v>1</v>
+      <c r="Q18" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="R18" s="4" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.25">
@@ -18563,11 +18563,11 @@
       <c r="D19" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="E19" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="F19" s="3" t="b">
-        <v>1</v>
+      <c r="E19" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="F19" s="4" t="b">
+        <v>0</v>
       </c>
       <c r="G19" s="3" t="b">
         <v>1</v>
@@ -18599,11 +18599,11 @@
       <c r="P19" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="Q19" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="R19" s="3" t="b">
-        <v>1</v>
+      <c r="Q19" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="R19" s="4" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.25">
@@ -18619,11 +18619,11 @@
       <c r="D20" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="E20" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="F20" s="3" t="b">
-        <v>1</v>
+      <c r="E20" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="F20" s="4" t="b">
+        <v>0</v>
       </c>
       <c r="G20" s="3" t="b">
         <v>1</v>
@@ -18655,11 +18655,11 @@
       <c r="P20" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="Q20" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="R20" s="3" t="b">
-        <v>1</v>
+      <c r="Q20" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="R20" s="4" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.25">
@@ -18675,11 +18675,11 @@
       <c r="D21" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="E21" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="F21" s="3" t="b">
-        <v>1</v>
+      <c r="E21" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="F21" s="4" t="b">
+        <v>0</v>
       </c>
       <c r="G21" s="3" t="b">
         <v>1</v>
@@ -18711,11 +18711,11 @@
       <c r="P21" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="Q21" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="R21" s="3" t="b">
-        <v>1</v>
+      <c r="Q21" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="R21" s="4" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.25">
@@ -18731,11 +18731,11 @@
       <c r="D22" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="E22" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="F22" s="3" t="b">
-        <v>1</v>
+      <c r="E22" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="F22" s="4" t="b">
+        <v>0</v>
       </c>
       <c r="G22" s="3" t="b">
         <v>1</v>
@@ -18767,11 +18767,11 @@
       <c r="P22" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="Q22" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="R22" s="3" t="b">
-        <v>1</v>
+      <c r="Q22" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="R22" s="4" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.25">
@@ -18787,11 +18787,11 @@
       <c r="D23" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="E23" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="F23" s="3" t="b">
-        <v>1</v>
+      <c r="E23" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="F23" s="4" t="b">
+        <v>0</v>
       </c>
       <c r="G23" s="3" t="b">
         <v>1</v>
@@ -18823,11 +18823,11 @@
       <c r="P23" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="Q23" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="R23" s="3" t="b">
-        <v>1</v>
+      <c r="Q23" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="R23" s="4" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.25">
@@ -18843,11 +18843,11 @@
       <c r="D24" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="E24" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="F24" s="3" t="b">
-        <v>1</v>
+      <c r="E24" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="F24" s="4" t="b">
+        <v>0</v>
       </c>
       <c r="G24" s="3" t="b">
         <v>1</v>
@@ -18879,11 +18879,11 @@
       <c r="P24" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="Q24" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="R24" s="3" t="b">
-        <v>1</v>
+      <c r="Q24" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="R24" s="4" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.25">
@@ -18899,11 +18899,11 @@
       <c r="D25" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="E25" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="F25" s="3" t="b">
-        <v>1</v>
+      <c r="E25" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="F25" s="4" t="b">
+        <v>0</v>
       </c>
       <c r="G25" s="3" t="b">
         <v>1</v>
@@ -18935,11 +18935,11 @@
       <c r="P25" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="Q25" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="R25" s="3" t="b">
-        <v>1</v>
+      <c r="Q25" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="R25" s="4" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.25">
@@ -18955,11 +18955,11 @@
       <c r="D26" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="E26" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="F26" s="3" t="b">
-        <v>1</v>
+      <c r="E26" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="F26" s="4" t="b">
+        <v>0</v>
       </c>
       <c r="G26" s="3" t="b">
         <v>1</v>
@@ -18991,11 +18991,11 @@
       <c r="P26" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="Q26" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="R26" s="3" t="b">
-        <v>1</v>
+      <c r="Q26" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="R26" s="4" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.25">
@@ -19011,11 +19011,11 @@
       <c r="D27" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="E27" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="F27" s="3" t="b">
-        <v>1</v>
+      <c r="E27" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="F27" s="4" t="b">
+        <v>0</v>
       </c>
       <c r="G27" s="3" t="b">
         <v>1</v>
@@ -19047,11 +19047,11 @@
       <c r="P27" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="Q27" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="R27" s="3" t="b">
-        <v>1</v>
+      <c r="Q27" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="R27" s="4" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.25">
@@ -19067,11 +19067,11 @@
       <c r="D28" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="E28" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="F28" s="3" t="b">
-        <v>1</v>
+      <c r="E28" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="F28" s="4" t="b">
+        <v>0</v>
       </c>
       <c r="G28" s="3" t="b">
         <v>1</v>
@@ -19103,11 +19103,11 @@
       <c r="P28" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="Q28" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="R28" s="3" t="b">
-        <v>1</v>
+      <c r="Q28" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="R28" s="4" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:18" x14ac:dyDescent="0.25">
@@ -19123,11 +19123,11 @@
       <c r="D29" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="E29" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="F29" s="3" t="b">
-        <v>1</v>
+      <c r="E29" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="F29" s="4" t="b">
+        <v>0</v>
       </c>
       <c r="G29" s="3" t="b">
         <v>1</v>
@@ -19159,11 +19159,11 @@
       <c r="P29" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="Q29" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="R29" s="3" t="b">
-        <v>1</v>
+      <c r="Q29" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="R29" s="4" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.25">
@@ -19179,11 +19179,11 @@
       <c r="D30" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="E30" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="F30" s="3" t="b">
-        <v>1</v>
+      <c r="E30" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="F30" s="4" t="b">
+        <v>0</v>
       </c>
       <c r="G30" s="3" t="b">
         <v>1</v>
@@ -19215,11 +19215,11 @@
       <c r="P30" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="Q30" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="R30" s="3" t="b">
-        <v>1</v>
+      <c r="Q30" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="R30" s="4" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.25">
@@ -19235,11 +19235,11 @@
       <c r="D31" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="E31" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="F31" s="3" t="b">
-        <v>1</v>
+      <c r="E31" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="F31" s="4" t="b">
+        <v>0</v>
       </c>
       <c r="G31" s="3" t="b">
         <v>1</v>
@@ -19271,11 +19271,11 @@
       <c r="P31" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="Q31" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="R31" s="3" t="b">
-        <v>1</v>
+      <c r="Q31" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="R31" s="4" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:18" x14ac:dyDescent="0.25">
@@ -19386,8 +19386,8 @@
       <c r="Q33" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="R33" s="3" t="b">
-        <v>1</v>
+      <c r="R33" s="4" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:18" x14ac:dyDescent="0.25">
@@ -19442,8 +19442,8 @@
       <c r="Q34" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="R34" s="3" t="b">
-        <v>1</v>
+      <c r="R34" s="4" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:18" x14ac:dyDescent="0.25">
@@ -19462,8 +19462,8 @@
       <c r="E35" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="F35" s="3" t="b">
-        <v>1</v>
+      <c r="F35" s="4" t="b">
+        <v>0</v>
       </c>
       <c r="G35" s="3" t="b">
         <v>1</v>
@@ -19492,14 +19492,14 @@
       <c r="O35" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="P35" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q35" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="R35" s="3" t="b">
-        <v>1</v>
+      <c r="P35" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q35" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="R35" s="4" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:18" x14ac:dyDescent="0.25">
@@ -19518,8 +19518,8 @@
       <c r="E36" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="F36" s="3" t="b">
-        <v>1</v>
+      <c r="F36" s="4" t="b">
+        <v>0</v>
       </c>
       <c r="G36" s="3" t="b">
         <v>1</v>
@@ -19548,14 +19548,14 @@
       <c r="O36" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="P36" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q36" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="R36" s="3" t="b">
-        <v>1</v>
+      <c r="P36" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q36" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="R36" s="4" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:18" x14ac:dyDescent="0.25">
@@ -19851,11 +19851,11 @@
       <c r="D42" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="E42" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="F42" s="3" t="b">
-        <v>1</v>
+      <c r="E42" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="F42" s="4" t="b">
+        <v>0</v>
       </c>
       <c r="G42" s="3" t="b">
         <v>1</v>
@@ -19887,11 +19887,11 @@
       <c r="P42" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="Q42" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="R42" s="3" t="b">
-        <v>1</v>
+      <c r="Q42" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="R42" s="4" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="43" spans="1:18" x14ac:dyDescent="0.25">
@@ -19963,11 +19963,11 @@
       <c r="D44" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="E44" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="F44" s="3" t="b">
-        <v>1</v>
+      <c r="E44" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="F44" s="4" t="b">
+        <v>0</v>
       </c>
       <c r="G44" s="3" t="b">
         <v>1</v>
@@ -20002,8 +20002,8 @@
       <c r="Q44" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="R44" s="3" t="b">
-        <v>1</v>
+      <c r="R44" s="4" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="45" spans="1:18" x14ac:dyDescent="0.25">
@@ -20187,8 +20187,8 @@
       <c r="D48" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="E48" s="3" t="b">
-        <v>1</v>
+      <c r="E48" s="4" t="b">
+        <v>0</v>
       </c>
       <c r="F48" s="3" t="b">
         <v>1</v>
@@ -20223,11 +20223,11 @@
       <c r="P48" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="Q48" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="R48" s="3" t="b">
-        <v>1</v>
+      <c r="Q48" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="R48" s="4" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="49" spans="1:18" x14ac:dyDescent="0.25">
@@ -20355,11 +20355,11 @@
       <c r="D51" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="E51" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="F51" s="3" t="b">
-        <v>1</v>
+      <c r="E51" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="F51" s="4" t="b">
+        <v>0</v>
       </c>
       <c r="G51" s="3" t="b">
         <v>1</v>
@@ -20391,11 +20391,11 @@
       <c r="P51" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="Q51" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="R51" s="3" t="b">
-        <v>1</v>
+      <c r="Q51" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="R51" s="4" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="52" spans="1:18" x14ac:dyDescent="0.25">
@@ -20523,8 +20523,8 @@
       <c r="D54" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="E54" s="3" t="b">
-        <v>1</v>
+      <c r="E54" s="4" t="b">
+        <v>0</v>
       </c>
       <c r="F54" s="3" t="b">
         <v>1</v>
@@ -20559,11 +20559,11 @@
       <c r="P54" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="Q54" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="R54" s="3" t="b">
-        <v>1</v>
+      <c r="Q54" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="R54" s="4" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="55" spans="1:18" x14ac:dyDescent="0.25">
@@ -20674,8 +20674,8 @@
       <c r="Q56" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="R56" s="3" t="b">
-        <v>1</v>
+      <c r="R56" s="4" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="57" spans="1:18" x14ac:dyDescent="0.25">
@@ -20730,8 +20730,8 @@
       <c r="Q57" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="R57" s="3" t="b">
-        <v>1</v>
+      <c r="R57" s="4" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="58" spans="1:18" x14ac:dyDescent="0.25">
@@ -20747,11 +20747,11 @@
       <c r="D58" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="E58" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="F58" s="3" t="b">
-        <v>1</v>
+      <c r="E58" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="F58" s="4" t="b">
+        <v>0</v>
       </c>
       <c r="G58" s="3" t="b">
         <v>1</v>
@@ -20783,11 +20783,11 @@
       <c r="P58" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="Q58" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="R58" s="3" t="b">
-        <v>1</v>
+      <c r="Q58" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="R58" s="4" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="59" spans="1:18" x14ac:dyDescent="0.25">
@@ -21119,8 +21119,8 @@
       <c r="P64" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="Q64" s="3" t="b">
-        <v>1</v>
+      <c r="Q64" s="4" t="b">
+        <v>0</v>
       </c>
       <c r="R64" s="3" t="b">
         <v>1</v>
@@ -21175,8 +21175,8 @@
       <c r="P65" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="Q65" s="3" t="b">
-        <v>1</v>
+      <c r="Q65" s="4" t="b">
+        <v>0</v>
       </c>
       <c r="R65" s="3" t="b">
         <v>1</v>
@@ -21195,11 +21195,11 @@
       <c r="D66" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="E66" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="F66" s="3" t="b">
-        <v>1</v>
+      <c r="E66" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="F66" s="4" t="b">
+        <v>0</v>
       </c>
       <c r="G66" s="3" t="b">
         <v>1</v>
@@ -21231,11 +21231,11 @@
       <c r="P66" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="Q66" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="R66" s="3" t="b">
-        <v>1</v>
+      <c r="Q66" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="R66" s="4" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="67" spans="1:18" x14ac:dyDescent="0.25">
@@ -21251,11 +21251,11 @@
       <c r="D67" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="E67" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="F67" s="3" t="b">
-        <v>1</v>
+      <c r="E67" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="F67" s="4" t="b">
+        <v>0</v>
       </c>
       <c r="G67" s="3" t="b">
         <v>1</v>
@@ -21287,11 +21287,11 @@
       <c r="P67" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="Q67" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="R67" s="3" t="b">
-        <v>1</v>
+      <c r="Q67" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="R67" s="4" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="68" spans="1:18" x14ac:dyDescent="0.25">
@@ -23323,11 +23323,11 @@
       <c r="D104" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="E104" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="F104" s="3" t="b">
-        <v>1</v>
+      <c r="E104" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="F104" s="4" t="b">
+        <v>0</v>
       </c>
       <c r="G104" s="3" t="b">
         <v>1</v>
@@ -23359,11 +23359,11 @@
       <c r="P104" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="Q104" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="R104" s="3" t="b">
-        <v>1</v>
+      <c r="Q104" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="R104" s="4" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="105" spans="1:18" x14ac:dyDescent="0.25">
@@ -23659,11 +23659,11 @@
       <c r="D110" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="E110" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="F110" s="3" t="b">
-        <v>1</v>
+      <c r="E110" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="F110" s="4" t="b">
+        <v>0</v>
       </c>
       <c r="G110" s="3" t="b">
         <v>1</v>
@@ -23695,11 +23695,11 @@
       <c r="P110" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="Q110" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="R110" s="3" t="b">
-        <v>1</v>
+      <c r="Q110" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="R110" s="4" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="111" spans="1:18" x14ac:dyDescent="0.25">
@@ -23715,11 +23715,11 @@
       <c r="D111" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="E111" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="F111" s="3" t="b">
-        <v>1</v>
+      <c r="E111" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="F111" s="4" t="b">
+        <v>0</v>
       </c>
       <c r="G111" s="3" t="b">
         <v>1</v>
@@ -23751,11 +23751,11 @@
       <c r="P111" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="Q111" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="R111" s="3" t="b">
-        <v>1</v>
+      <c r="Q111" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="R111" s="4" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="112" spans="1:18" x14ac:dyDescent="0.25">
@@ -23804,14 +23804,14 @@
       <c r="O112" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="P112" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q112" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="R112" s="3" t="b">
-        <v>1</v>
+      <c r="P112" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q112" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="R112" s="4" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="113" spans="1:18" x14ac:dyDescent="0.25">
@@ -25059,11 +25059,11 @@
       <c r="D135" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="E135" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="F135" s="3" t="b">
-        <v>1</v>
+      <c r="E135" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="F135" s="4" t="b">
+        <v>0</v>
       </c>
       <c r="G135" s="3" t="b">
         <v>1</v>
@@ -25095,11 +25095,11 @@
       <c r="P135" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="Q135" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="R135" s="3" t="b">
-        <v>1</v>
+      <c r="Q135" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="R135" s="4" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="136" spans="1:18" x14ac:dyDescent="0.25">
@@ -25115,11 +25115,11 @@
       <c r="D136" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="E136" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="F136" s="3" t="b">
-        <v>1</v>
+      <c r="E136" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="F136" s="4" t="b">
+        <v>0</v>
       </c>
       <c r="G136" s="3" t="b">
         <v>1</v>
@@ -25148,14 +25148,14 @@
       <c r="O136" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="P136" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q136" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="R136" s="3" t="b">
-        <v>1</v>
+      <c r="P136" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q136" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="R136" s="4" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="137" spans="1:18" x14ac:dyDescent="0.25">
@@ -25283,11 +25283,11 @@
       <c r="D139" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="E139" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="F139" s="3" t="b">
-        <v>1</v>
+      <c r="E139" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="F139" s="4" t="b">
+        <v>0</v>
       </c>
       <c r="G139" s="3" t="b">
         <v>1</v>
@@ -25319,11 +25319,11 @@
       <c r="P139" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="Q139" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="R139" s="3" t="b">
-        <v>1</v>
+      <c r="Q139" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="R139" s="4" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="140" spans="1:18" x14ac:dyDescent="0.25">
@@ -27635,11 +27635,11 @@
       <c r="D181" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="E181" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="F181" s="3" t="b">
-        <v>1</v>
+      <c r="E181" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="F181" s="4" t="b">
+        <v>0</v>
       </c>
       <c r="G181" s="3" t="b">
         <v>1</v>
@@ -27671,11 +27671,11 @@
       <c r="P181" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="Q181" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="R181" s="3" t="b">
-        <v>1</v>
+      <c r="Q181" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="R181" s="4" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="182" spans="1:18" x14ac:dyDescent="0.25">
@@ -27691,11 +27691,11 @@
       <c r="D182" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="E182" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="F182" s="3" t="b">
-        <v>1</v>
+      <c r="E182" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="F182" s="4" t="b">
+        <v>0</v>
       </c>
       <c r="G182" s="3" t="b">
         <v>1</v>
@@ -27727,11 +27727,11 @@
       <c r="P182" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="Q182" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="R182" s="3" t="b">
-        <v>1</v>
+      <c r="Q182" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="R182" s="4" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="183" spans="1:18" x14ac:dyDescent="0.25">
@@ -27803,8 +27803,8 @@
       <c r="D184" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="E184" s="3" t="b">
-        <v>1</v>
+      <c r="E184" s="4" t="b">
+        <v>0</v>
       </c>
       <c r="F184" s="3" t="b">
         <v>1</v>
@@ -27839,11 +27839,11 @@
       <c r="P184" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="Q184" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="R184" s="3" t="b">
-        <v>1</v>
+      <c r="Q184" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="R184" s="4" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="185" spans="1:18" x14ac:dyDescent="0.25">
@@ -27895,11 +27895,11 @@
       <c r="P185" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="Q185" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="R185" s="3" t="b">
-        <v>1</v>
+      <c r="Q185" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="R185" s="4" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="186" spans="1:18" x14ac:dyDescent="0.25">
@@ -27951,11 +27951,11 @@
       <c r="P186" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="Q186" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="R186" s="3" t="b">
-        <v>1</v>
+      <c r="Q186" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="R186" s="4" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="187" spans="1:18" x14ac:dyDescent="0.25">
@@ -28119,8 +28119,8 @@
       <c r="P189" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="Q189" s="3" t="b">
-        <v>1</v>
+      <c r="Q189" s="4" t="b">
+        <v>0</v>
       </c>
       <c r="R189" s="3" t="b">
         <v>1</v>
@@ -28175,8 +28175,8 @@
       <c r="P190" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="Q190" s="3" t="b">
-        <v>1</v>
+      <c r="Q190" s="4" t="b">
+        <v>0</v>
       </c>
       <c r="R190" s="3" t="b">
         <v>1</v>
@@ -28198,8 +28198,8 @@
       <c r="E191" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="F191" s="3" t="b">
-        <v>1</v>
+      <c r="F191" s="4" t="b">
+        <v>0</v>
       </c>
       <c r="G191" s="3" t="b">
         <v>1</v>
@@ -28234,8 +28234,8 @@
       <c r="Q191" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="R191" s="3" t="b">
-        <v>1</v>
+      <c r="R191" s="4" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="192" spans="1:18" x14ac:dyDescent="0.25">
@@ -28251,11 +28251,11 @@
       <c r="D192" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="E192" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="F192" s="3" t="b">
-        <v>1</v>
+      <c r="E192" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="F192" s="4" t="b">
+        <v>0</v>
       </c>
       <c r="G192" s="3" t="b">
         <v>1</v>
@@ -28278,20 +28278,20 @@
       <c r="M192" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="N192" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="O192" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="P192" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q192" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="R192" s="3" t="b">
-        <v>1</v>
+      <c r="N192" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="O192" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="P192" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q192" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="R192" s="4" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="193" spans="1:18" x14ac:dyDescent="0.25">
@@ -28307,11 +28307,11 @@
       <c r="D193" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="E193" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="F193" s="3" t="b">
-        <v>1</v>
+      <c r="E193" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="F193" s="4" t="b">
+        <v>0</v>
       </c>
       <c r="G193" s="3" t="b">
         <v>1</v>
@@ -28334,20 +28334,20 @@
       <c r="M193" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="N193" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="O193" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="P193" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q193" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="R193" s="3" t="b">
-        <v>1</v>
+      <c r="N193" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="O193" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="P193" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q193" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="R193" s="4" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="194" spans="1:18" x14ac:dyDescent="0.25">
@@ -28399,8 +28399,8 @@
       <c r="P194" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="Q194" s="3" t="b">
-        <v>1</v>
+      <c r="Q194" s="4" t="b">
+        <v>0</v>
       </c>
       <c r="R194" s="3" t="b">
         <v>1</v>
@@ -28455,8 +28455,8 @@
       <c r="P195" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="Q195" s="3" t="b">
-        <v>1</v>
+      <c r="Q195" s="4" t="b">
+        <v>0</v>
       </c>
       <c r="R195" s="3" t="b">
         <v>1</v>
@@ -28511,11 +28511,11 @@
       <c r="P196" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="Q196" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="R196" s="3" t="b">
-        <v>1</v>
+      <c r="Q196" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="R196" s="4" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="197" spans="1:18" x14ac:dyDescent="0.25">
@@ -28570,8 +28570,8 @@
       <c r="Q197" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="R197" s="3" t="b">
-        <v>1</v>
+      <c r="R197" s="4" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="198" spans="1:18" x14ac:dyDescent="0.25">
@@ -28626,8 +28626,8 @@
       <c r="Q198" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="R198" s="3" t="b">
-        <v>1</v>
+      <c r="R198" s="4" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="199" spans="1:18" x14ac:dyDescent="0.25">
@@ -28699,8 +28699,8 @@
       <c r="D200" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="E200" s="3" t="b">
-        <v>1</v>
+      <c r="E200" s="4" t="b">
+        <v>0</v>
       </c>
       <c r="F200" s="3" t="b">
         <v>1</v>
@@ -28732,14 +28732,14 @@
       <c r="O200" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="P200" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q200" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="R200" s="3" t="b">
-        <v>1</v>
+      <c r="P200" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q200" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="R200" s="4" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="201" spans="1:18" x14ac:dyDescent="0.25">
@@ -28847,11 +28847,11 @@
       <c r="P202" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="Q202" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="R202" s="3" t="b">
-        <v>1</v>
+      <c r="Q202" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="R202" s="4" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="203" spans="1:18" x14ac:dyDescent="0.25">
@@ -28903,11 +28903,11 @@
       <c r="P203" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="Q203" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="R203" s="3" t="b">
-        <v>1</v>
+      <c r="Q203" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="R203" s="4" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="204" spans="1:18" x14ac:dyDescent="0.25">
@@ -28959,11 +28959,11 @@
       <c r="P204" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="Q204" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="R204" s="3" t="b">
-        <v>1</v>
+      <c r="Q204" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="R204" s="4" t="b">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
generated all the reports on 2023-11-23
</commit_message>
<xml_diff>
--- a/report/merged_configurations.xlsx
+++ b/report/merged_configurations.xlsx
@@ -3712,7 +3712,7 @@
         <v>41</v>
       </c>
       <c r="E4" s="2">
-        <v>45221.91666666667</v>
+        <v>45222</v>
       </c>
       <c r="G4" t="s">
         <v>42</v>
@@ -3768,7 +3768,7 @@
         <v>41</v>
       </c>
       <c r="E5" s="2">
-        <v>45117.91666666667</v>
+        <v>45118</v>
       </c>
       <c r="F5" t="s">
         <v>50</v>
@@ -3801,7 +3801,7 @@
         <v>57</v>
       </c>
       <c r="P5" s="2">
-        <v>44973.95833333333</v>
+        <v>44974</v>
       </c>
       <c r="Q5" t="s">
         <v>26</v>
@@ -5556,7 +5556,7 @@
         <v>149</v>
       </c>
       <c r="E32" s="2">
-        <v>44678.91666666667</v>
+        <v>44679</v>
       </c>
       <c r="F32" t="s">
         <v>50</v>
@@ -5627,7 +5627,7 @@
         <v>164</v>
       </c>
       <c r="E33" s="2">
-        <v>44454.91666666667</v>
+        <v>44455</v>
       </c>
       <c r="F33" t="s">
         <v>50</v>
@@ -5660,7 +5660,7 @@
         <v>171</v>
       </c>
       <c r="P33" s="2">
-        <v>44454.91666666667</v>
+        <v>44455</v>
       </c>
       <c r="Q33" t="s">
         <v>172</v>
@@ -5669,7 +5669,7 @@
         <v>26</v>
       </c>
       <c r="S33" s="2">
-        <v>44729.91666666667</v>
+        <v>44730</v>
       </c>
       <c r="T33" t="s">
         <v>36</v>
@@ -5698,7 +5698,7 @@
         <v>164</v>
       </c>
       <c r="E34" s="2">
-        <v>44454.91666666667</v>
+        <v>44455</v>
       </c>
       <c r="F34" t="s">
         <v>50</v>
@@ -5731,7 +5731,7 @@
         <v>171</v>
       </c>
       <c r="P34" s="2">
-        <v>44454.91666666667</v>
+        <v>44455</v>
       </c>
       <c r="Q34" t="s">
         <v>172</v>
@@ -5740,7 +5740,7 @@
         <v>26</v>
       </c>
       <c r="S34" s="2">
-        <v>44729.91666666667</v>
+        <v>44730</v>
       </c>
       <c r="T34" t="s">
         <v>36</v>
@@ -5766,7 +5766,7 @@
         <v>149</v>
       </c>
       <c r="E35" s="2">
-        <v>44594.95833333333</v>
+        <v>44595</v>
       </c>
       <c r="F35" t="s">
         <v>26</v>
@@ -5834,7 +5834,7 @@
         <v>149</v>
       </c>
       <c r="E36" s="2">
-        <v>44594.95833333333</v>
+        <v>44595</v>
       </c>
       <c r="F36" t="s">
         <v>26</v>
@@ -5905,7 +5905,7 @@
         <v>191</v>
       </c>
       <c r="E37" s="2">
-        <v>44671.91666666667</v>
+        <v>44672</v>
       </c>
       <c r="F37" t="s">
         <v>192</v>
@@ -5938,13 +5938,13 @@
         <v>65</v>
       </c>
       <c r="P37" s="2">
-        <v>44146.95833333333</v>
+        <v>44147</v>
       </c>
       <c r="Q37" s="2">
-        <v>44636.95833333333</v>
+        <v>44637</v>
       </c>
       <c r="R37" s="2">
-        <v>44671.91666666667</v>
+        <v>44672</v>
       </c>
       <c r="S37" t="s">
         <v>36</v>
@@ -5976,7 +5976,7 @@
         <v>191</v>
       </c>
       <c r="E38" s="2">
-        <v>44671.91666666667</v>
+        <v>44672</v>
       </c>
       <c r="F38" t="s">
         <v>192</v>
@@ -6009,13 +6009,13 @@
         <v>65</v>
       </c>
       <c r="P38" s="2">
-        <v>44146.95833333333</v>
+        <v>44147</v>
       </c>
       <c r="Q38" s="2">
-        <v>44636.95833333333</v>
+        <v>44637</v>
       </c>
       <c r="R38" s="2">
-        <v>44671.91666666667</v>
+        <v>44672</v>
       </c>
       <c r="S38" t="s">
         <v>36</v>
@@ -6047,7 +6047,7 @@
         <v>191</v>
       </c>
       <c r="E39" s="2">
-        <v>44671.91666666667</v>
+        <v>44672</v>
       </c>
       <c r="F39" t="s">
         <v>192</v>
@@ -6080,13 +6080,13 @@
         <v>65</v>
       </c>
       <c r="P39" s="2">
-        <v>44146.95833333333</v>
+        <v>44147</v>
       </c>
       <c r="Q39" s="2">
-        <v>44636.95833333333</v>
+        <v>44637</v>
       </c>
       <c r="R39" s="2">
-        <v>44671.91666666667</v>
+        <v>44672</v>
       </c>
       <c r="S39" t="s">
         <v>36</v>
@@ -6118,7 +6118,7 @@
         <v>191</v>
       </c>
       <c r="E40" s="2">
-        <v>44671.91666666667</v>
+        <v>44672</v>
       </c>
       <c r="F40" t="s">
         <v>192</v>
@@ -6151,13 +6151,13 @@
         <v>65</v>
       </c>
       <c r="P40" s="2">
-        <v>44146.95833333333</v>
+        <v>44147</v>
       </c>
       <c r="Q40" s="2">
-        <v>44636.95833333333</v>
+        <v>44637</v>
       </c>
       <c r="R40" s="2">
-        <v>44671.91666666667</v>
+        <v>44672</v>
       </c>
       <c r="S40" t="s">
         <v>36</v>
@@ -6189,7 +6189,7 @@
         <v>41</v>
       </c>
       <c r="E41" s="2">
-        <v>43283.91666666667</v>
+        <v>43284</v>
       </c>
       <c r="F41" t="s">
         <v>50</v>
@@ -6331,7 +6331,7 @@
         <v>41</v>
       </c>
       <c r="E43" s="2">
-        <v>43430.95833333333</v>
+        <v>43431</v>
       </c>
       <c r="F43" t="s">
         <v>50</v>
@@ -6473,7 +6473,7 @@
         <v>41</v>
       </c>
       <c r="E45" s="2">
-        <v>43502.95833333333</v>
+        <v>43503</v>
       </c>
       <c r="F45" t="s">
         <v>50</v>
@@ -6544,7 +6544,7 @@
         <v>41</v>
       </c>
       <c r="E46" s="2">
-        <v>43502.95833333333</v>
+        <v>43503</v>
       </c>
       <c r="F46" t="s">
         <v>50</v>
@@ -6615,7 +6615,7 @@
         <v>41</v>
       </c>
       <c r="E47" s="2">
-        <v>43283.91666666667</v>
+        <v>43284</v>
       </c>
       <c r="F47" t="s">
         <v>50</v>
@@ -6757,7 +6757,7 @@
         <v>269</v>
       </c>
       <c r="E49" s="2">
-        <v>43502.95833333333</v>
+        <v>43503</v>
       </c>
       <c r="F49" t="s">
         <v>50</v>
@@ -6828,7 +6828,7 @@
         <v>41</v>
       </c>
       <c r="E50" s="2">
-        <v>43283.91666666667</v>
+        <v>43284</v>
       </c>
       <c r="F50" t="s">
         <v>50</v>
@@ -6970,7 +6970,7 @@
         <v>296</v>
       </c>
       <c r="E52" s="2">
-        <v>43803.95833333333</v>
+        <v>43804</v>
       </c>
       <c r="F52" t="s">
         <v>50</v>
@@ -7041,7 +7041,7 @@
         <v>296</v>
       </c>
       <c r="E53" s="2">
-        <v>43803.95833333333</v>
+        <v>43804</v>
       </c>
       <c r="F53" t="s">
         <v>50</v>
@@ -7183,7 +7183,7 @@
         <v>41</v>
       </c>
       <c r="E55" s="2">
-        <v>43283.91666666667</v>
+        <v>43284</v>
       </c>
       <c r="F55" t="s">
         <v>50</v>
@@ -7254,7 +7254,7 @@
         <v>41</v>
       </c>
       <c r="E56" s="2">
-        <v>43411.95833333333</v>
+        <v>43412</v>
       </c>
       <c r="F56" t="s">
         <v>50</v>
@@ -7325,7 +7325,7 @@
         <v>41</v>
       </c>
       <c r="E57" s="2">
-        <v>43411.95833333333</v>
+        <v>43412</v>
       </c>
       <c r="F57" t="s">
         <v>50</v>
@@ -7467,7 +7467,7 @@
         <v>41</v>
       </c>
       <c r="E59" s="2">
-        <v>43502.95833333333</v>
+        <v>43503</v>
       </c>
       <c r="F59" t="s">
         <v>50</v>
@@ -7538,7 +7538,7 @@
         <v>41</v>
       </c>
       <c r="E60" s="2">
-        <v>43502.95833333333</v>
+        <v>43503</v>
       </c>
       <c r="F60" t="s">
         <v>50</v>
@@ -7609,7 +7609,7 @@
         <v>41</v>
       </c>
       <c r="E61" s="2">
-        <v>43502.95833333333</v>
+        <v>43503</v>
       </c>
       <c r="F61" t="s">
         <v>50</v>
@@ -7680,7 +7680,7 @@
         <v>41</v>
       </c>
       <c r="E62" s="2">
-        <v>43502.95833333333</v>
+        <v>43503</v>
       </c>
       <c r="F62" t="s">
         <v>50</v>
@@ -7751,7 +7751,7 @@
         <v>41</v>
       </c>
       <c r="E63" s="2">
-        <v>43502.95833333333</v>
+        <v>43503</v>
       </c>
       <c r="F63" t="s">
         <v>50</v>
@@ -7819,7 +7819,7 @@
         <v>369</v>
       </c>
       <c r="E64" s="2">
-        <v>45193.91666666667</v>
+        <v>45194</v>
       </c>
       <c r="F64" t="s">
         <v>50</v>
@@ -7887,7 +7887,7 @@
         <v>369</v>
       </c>
       <c r="E65" s="2">
-        <v>45193.91666666667</v>
+        <v>45194</v>
       </c>
       <c r="F65" t="s">
         <v>50</v>
@@ -8100,7 +8100,7 @@
         <v>400</v>
       </c>
       <c r="E68" s="2">
-        <v>43943.91666666667</v>
+        <v>43944</v>
       </c>
       <c r="F68" t="s">
         <v>50</v>
@@ -8171,7 +8171,7 @@
         <v>400</v>
       </c>
       <c r="E69" s="2">
-        <v>43943.91666666667</v>
+        <v>43944</v>
       </c>
       <c r="F69" t="s">
         <v>50</v>
@@ -8242,7 +8242,7 @@
         <v>400</v>
       </c>
       <c r="E70" s="2">
-        <v>43943.91666666667</v>
+        <v>43944</v>
       </c>
       <c r="F70" t="s">
         <v>50</v>
@@ -8313,7 +8313,7 @@
         <v>400</v>
       </c>
       <c r="E71" s="2">
-        <v>43943.91666666667</v>
+        <v>43944</v>
       </c>
       <c r="F71" t="s">
         <v>50</v>
@@ -8384,7 +8384,7 @@
         <v>41</v>
       </c>
       <c r="E72" s="2">
-        <v>44531.95833333333</v>
+        <v>44532</v>
       </c>
       <c r="F72" t="s">
         <v>50</v>
@@ -8452,7 +8452,7 @@
         <v>41</v>
       </c>
       <c r="E73" s="2">
-        <v>43502.95833333333</v>
+        <v>43503</v>
       </c>
       <c r="F73" t="s">
         <v>50</v>
@@ -8523,7 +8523,7 @@
         <v>41</v>
       </c>
       <c r="E74" s="2">
-        <v>43502.95833333333</v>
+        <v>43503</v>
       </c>
       <c r="F74" t="s">
         <v>50</v>
@@ -8594,7 +8594,7 @@
         <v>41</v>
       </c>
       <c r="E75" s="2">
-        <v>43502.95833333333</v>
+        <v>43503</v>
       </c>
       <c r="F75" t="s">
         <v>50</v>
@@ -8665,7 +8665,7 @@
         <v>463</v>
       </c>
       <c r="E76" s="2">
-        <v>43999.91666666667</v>
+        <v>44000</v>
       </c>
       <c r="F76" t="s">
         <v>50</v>
@@ -8736,7 +8736,7 @@
         <v>463</v>
       </c>
       <c r="E77" s="2">
-        <v>43999.91666666667</v>
+        <v>44000</v>
       </c>
       <c r="F77" t="s">
         <v>50</v>
@@ -8807,7 +8807,7 @@
         <v>463</v>
       </c>
       <c r="E78" s="2">
-        <v>43999.91666666667</v>
+        <v>44000</v>
       </c>
       <c r="F78" t="s">
         <v>50</v>
@@ -8878,7 +8878,7 @@
         <v>463</v>
       </c>
       <c r="E79" s="2">
-        <v>43999.91666666667</v>
+        <v>44000</v>
       </c>
       <c r="F79" t="s">
         <v>50</v>
@@ -8949,7 +8949,7 @@
         <v>490</v>
       </c>
       <c r="E80" s="2">
-        <v>43300.91666666667</v>
+        <v>43301</v>
       </c>
       <c r="F80" t="s">
         <v>50</v>
@@ -9020,7 +9020,7 @@
         <v>490</v>
       </c>
       <c r="E81" s="2">
-        <v>43300.91666666667</v>
+        <v>43301</v>
       </c>
       <c r="F81" t="s">
         <v>498</v>
@@ -9091,7 +9091,7 @@
         <v>490</v>
       </c>
       <c r="E82" s="2">
-        <v>43300.91666666667</v>
+        <v>43301</v>
       </c>
       <c r="F82" t="s">
         <v>50</v>
@@ -9162,7 +9162,7 @@
         <v>490</v>
       </c>
       <c r="E83" s="2">
-        <v>43300.91666666667</v>
+        <v>43301</v>
       </c>
       <c r="F83" t="s">
         <v>498</v>
@@ -9233,7 +9233,7 @@
         <v>490</v>
       </c>
       <c r="E84" s="2">
-        <v>43276.91666666667</v>
+        <v>43277</v>
       </c>
       <c r="F84" t="s">
         <v>498</v>
@@ -9301,7 +9301,7 @@
         <v>41</v>
       </c>
       <c r="E85" s="2">
-        <v>43241.91666666667</v>
+        <v>43242</v>
       </c>
       <c r="F85" t="s">
         <v>520</v>
@@ -9369,7 +9369,7 @@
         <v>41</v>
       </c>
       <c r="E86" s="2">
-        <v>43241.91666666667</v>
+        <v>43242</v>
       </c>
       <c r="F86" t="s">
         <v>520</v>
@@ -9437,7 +9437,7 @@
         <v>41</v>
       </c>
       <c r="E87" s="2">
-        <v>43241.91666666667</v>
+        <v>43242</v>
       </c>
       <c r="F87" t="s">
         <v>50</v>
@@ -9508,7 +9508,7 @@
         <v>41</v>
       </c>
       <c r="E88" s="2">
-        <v>43430.95833333333</v>
+        <v>43431</v>
       </c>
       <c r="F88" t="s">
         <v>50</v>
@@ -9579,7 +9579,7 @@
         <v>41</v>
       </c>
       <c r="E89" s="2">
-        <v>43430.95833333333</v>
+        <v>43431</v>
       </c>
       <c r="F89" t="s">
         <v>50</v>
@@ -9650,7 +9650,7 @@
         <v>41</v>
       </c>
       <c r="E90" s="2">
-        <v>43430.95833333333</v>
+        <v>43431</v>
       </c>
       <c r="F90" t="s">
         <v>50</v>
@@ -9721,7 +9721,7 @@
         <v>41</v>
       </c>
       <c r="E91" s="2">
-        <v>43430.95833333333</v>
+        <v>43431</v>
       </c>
       <c r="F91" t="s">
         <v>50</v>
@@ -9792,7 +9792,7 @@
         <v>41</v>
       </c>
       <c r="E92" s="2">
-        <v>43430.95833333333</v>
+        <v>43431</v>
       </c>
       <c r="F92" t="s">
         <v>50</v>
@@ -9863,7 +9863,7 @@
         <v>41</v>
       </c>
       <c r="E93" s="2">
-        <v>43430.95833333333</v>
+        <v>43431</v>
       </c>
       <c r="F93" t="s">
         <v>50</v>
@@ -9934,7 +9934,7 @@
         <v>41</v>
       </c>
       <c r="E94" s="2">
-        <v>43430.95833333333</v>
+        <v>43431</v>
       </c>
       <c r="F94" t="s">
         <v>50</v>
@@ -10005,7 +10005,7 @@
         <v>41</v>
       </c>
       <c r="E95" s="2">
-        <v>43430.95833333333</v>
+        <v>43431</v>
       </c>
       <c r="F95" t="s">
         <v>50</v>
@@ -10076,7 +10076,7 @@
         <v>41</v>
       </c>
       <c r="E96" s="2">
-        <v>43430.95833333333</v>
+        <v>43431</v>
       </c>
       <c r="F96" t="s">
         <v>50</v>
@@ -10147,7 +10147,7 @@
         <v>41</v>
       </c>
       <c r="E97" s="2">
-        <v>43430.95833333333</v>
+        <v>43431</v>
       </c>
       <c r="F97" t="s">
         <v>50</v>
@@ -10218,7 +10218,7 @@
         <v>41</v>
       </c>
       <c r="E98" s="2">
-        <v>43430.95833333333</v>
+        <v>43431</v>
       </c>
       <c r="F98" t="s">
         <v>50</v>
@@ -10289,7 +10289,7 @@
         <v>41</v>
       </c>
       <c r="E99" s="2">
-        <v>43430.95833333333</v>
+        <v>43431</v>
       </c>
       <c r="F99" t="s">
         <v>50</v>
@@ -10360,7 +10360,7 @@
         <v>41</v>
       </c>
       <c r="E100" s="2">
-        <v>43430.95833333333</v>
+        <v>43431</v>
       </c>
       <c r="F100" t="s">
         <v>50</v>
@@ -10431,7 +10431,7 @@
         <v>41</v>
       </c>
       <c r="E101" s="2">
-        <v>43430.95833333333</v>
+        <v>43431</v>
       </c>
       <c r="F101" t="s">
         <v>50</v>
@@ -10502,7 +10502,7 @@
         <v>41</v>
       </c>
       <c r="E102" s="2">
-        <v>43430.95833333333</v>
+        <v>43431</v>
       </c>
       <c r="F102" t="s">
         <v>50</v>
@@ -10573,7 +10573,7 @@
         <v>41</v>
       </c>
       <c r="E103" s="2">
-        <v>43430.95833333333</v>
+        <v>43431</v>
       </c>
       <c r="F103" t="s">
         <v>50</v>
@@ -10715,7 +10715,7 @@
         <v>269</v>
       </c>
       <c r="E105" s="2">
-        <v>44230.95833333333</v>
+        <v>44231</v>
       </c>
       <c r="F105" t="s">
         <v>50</v>
@@ -10786,7 +10786,7 @@
         <v>269</v>
       </c>
       <c r="E106" s="2">
-        <v>44230.95833333333</v>
+        <v>44231</v>
       </c>
       <c r="F106" t="s">
         <v>50</v>
@@ -10857,7 +10857,7 @@
         <v>149</v>
       </c>
       <c r="E107" s="2">
-        <v>44307.91666666667</v>
+        <v>44308</v>
       </c>
       <c r="F107" t="s">
         <v>192</v>
@@ -10893,10 +10893,10 @@
         <v>609</v>
       </c>
       <c r="Q107" s="2">
-        <v>44265.95833333333</v>
+        <v>44266</v>
       </c>
       <c r="R107" s="2">
-        <v>44307.91666666667</v>
+        <v>44308</v>
       </c>
       <c r="S107" t="s">
         <v>36</v>
@@ -10928,7 +10928,7 @@
         <v>149</v>
       </c>
       <c r="E108" s="2">
-        <v>44307.91666666667</v>
+        <v>44308</v>
       </c>
       <c r="F108" t="s">
         <v>192</v>
@@ -10964,10 +10964,10 @@
         <v>609</v>
       </c>
       <c r="Q108" s="2">
-        <v>44265.95833333333</v>
+        <v>44266</v>
       </c>
       <c r="R108" s="2">
-        <v>44307.91666666667</v>
+        <v>44308</v>
       </c>
       <c r="S108" t="s">
         <v>36</v>
@@ -10999,7 +10999,7 @@
         <v>149</v>
       </c>
       <c r="E109" s="2">
-        <v>44307.91666666667</v>
+        <v>44308</v>
       </c>
       <c r="F109" t="s">
         <v>50</v>
@@ -11032,13 +11032,13 @@
         <v>65</v>
       </c>
       <c r="P109" s="2">
-        <v>43788.95833333333</v>
+        <v>43789</v>
       </c>
       <c r="Q109" s="2">
-        <v>44265.95833333333</v>
+        <v>44266</v>
       </c>
       <c r="R109" s="2">
-        <v>44307.91666666667</v>
+        <v>44308</v>
       </c>
       <c r="S109" t="s">
         <v>36</v>
@@ -11212,7 +11212,7 @@
         <v>41</v>
       </c>
       <c r="E112" s="2">
-        <v>42816.95833333333</v>
+        <v>42817</v>
       </c>
       <c r="F112" t="s">
         <v>50</v>
@@ -11274,7 +11274,7 @@
         <v>41</v>
       </c>
       <c r="E113" s="2">
-        <v>42824.91666666667</v>
+        <v>42825</v>
       </c>
       <c r="F113" t="s">
         <v>50</v>
@@ -12966,7 +12966,7 @@
         <v>25</v>
       </c>
       <c r="E137" s="2">
-        <v>44307.91666666667</v>
+        <v>44308</v>
       </c>
       <c r="F137" t="s">
         <v>192</v>
@@ -12999,13 +12999,13 @@
         <v>34</v>
       </c>
       <c r="P137" s="2">
-        <v>44031.91666666667</v>
+        <v>44032</v>
       </c>
       <c r="Q137" s="2">
-        <v>44265.95833333333</v>
+        <v>44266</v>
       </c>
       <c r="R137" s="2">
-        <v>44307.91666666667</v>
+        <v>44308</v>
       </c>
       <c r="S137" t="s">
         <v>36</v>
@@ -13037,7 +13037,7 @@
         <v>25</v>
       </c>
       <c r="E138" s="2">
-        <v>44307.91666666667</v>
+        <v>44308</v>
       </c>
       <c r="F138" t="s">
         <v>192</v>
@@ -13070,13 +13070,13 @@
         <v>34</v>
       </c>
       <c r="P138" s="2">
-        <v>44396.91666666667</v>
+        <v>44397</v>
       </c>
       <c r="Q138" s="2">
-        <v>44265.95833333333</v>
+        <v>44266</v>
       </c>
       <c r="R138" s="2">
-        <v>44307.91666666667</v>
+        <v>44308</v>
       </c>
       <c r="S138" t="s">
         <v>36</v>
@@ -13173,7 +13173,7 @@
         <v>582</v>
       </c>
       <c r="E140" s="2">
-        <v>44166.95833333333</v>
+        <v>44167</v>
       </c>
       <c r="F140" t="s">
         <v>50</v>
@@ -13241,7 +13241,7 @@
         <v>582</v>
       </c>
       <c r="E141" s="2">
-        <v>44166.95833333333</v>
+        <v>44167</v>
       </c>
       <c r="F141" t="s">
         <v>50</v>
@@ -13309,7 +13309,7 @@
         <v>582</v>
       </c>
       <c r="E142" s="2">
-        <v>44166.95833333333</v>
+        <v>44167</v>
       </c>
       <c r="F142" t="s">
         <v>50</v>
@@ -13377,7 +13377,7 @@
         <v>582</v>
       </c>
       <c r="E143" s="2">
-        <v>44166.95833333333</v>
+        <v>44167</v>
       </c>
       <c r="F143" t="s">
         <v>50</v>
@@ -13445,7 +13445,7 @@
         <v>582</v>
       </c>
       <c r="E144" s="2">
-        <v>44166.95833333333</v>
+        <v>44167</v>
       </c>
       <c r="F144" t="s">
         <v>50</v>
@@ -13513,7 +13513,7 @@
         <v>582</v>
       </c>
       <c r="E145" s="2">
-        <v>44166.95833333333</v>
+        <v>44167</v>
       </c>
       <c r="F145" t="s">
         <v>50</v>
@@ -13581,7 +13581,7 @@
         <v>582</v>
       </c>
       <c r="E146" s="2">
-        <v>44166.95833333333</v>
+        <v>44167</v>
       </c>
       <c r="F146" t="s">
         <v>50</v>
@@ -13649,7 +13649,7 @@
         <v>582</v>
       </c>
       <c r="E147" s="2">
-        <v>44166.95833333333</v>
+        <v>44167</v>
       </c>
       <c r="F147" t="s">
         <v>50</v>
@@ -13717,7 +13717,7 @@
         <v>582</v>
       </c>
       <c r="E148" s="2">
-        <v>44166.95833333333</v>
+        <v>44167</v>
       </c>
       <c r="F148" t="s">
         <v>50</v>
@@ -13785,7 +13785,7 @@
         <v>582</v>
       </c>
       <c r="E149" s="2">
-        <v>44166.95833333333</v>
+        <v>44167</v>
       </c>
       <c r="F149" t="s">
         <v>50</v>
@@ -13853,7 +13853,7 @@
         <v>582</v>
       </c>
       <c r="E150" s="2">
-        <v>44166.95833333333</v>
+        <v>44167</v>
       </c>
       <c r="F150" t="s">
         <v>50</v>
@@ -13921,7 +13921,7 @@
         <v>582</v>
       </c>
       <c r="E151" s="2">
-        <v>44166.95833333333</v>
+        <v>44167</v>
       </c>
       <c r="F151" t="s">
         <v>50</v>
@@ -13989,7 +13989,7 @@
         <v>582</v>
       </c>
       <c r="E152" s="2">
-        <v>44166.95833333333</v>
+        <v>44167</v>
       </c>
       <c r="F152" t="s">
         <v>50</v>
@@ -14057,7 +14057,7 @@
         <v>582</v>
       </c>
       <c r="E153" s="2">
-        <v>44166.95833333333</v>
+        <v>44167</v>
       </c>
       <c r="F153" t="s">
         <v>50</v>
@@ -14125,7 +14125,7 @@
         <v>582</v>
       </c>
       <c r="E154" s="2">
-        <v>44166.95833333333</v>
+        <v>44167</v>
       </c>
       <c r="F154" t="s">
         <v>50</v>
@@ -14193,7 +14193,7 @@
         <v>582</v>
       </c>
       <c r="E155" s="2">
-        <v>44166.95833333333</v>
+        <v>44167</v>
       </c>
       <c r="F155" t="s">
         <v>50</v>
@@ -14261,7 +14261,7 @@
         <v>582</v>
       </c>
       <c r="E156" s="2">
-        <v>44166.95833333333</v>
+        <v>44167</v>
       </c>
       <c r="F156" t="s">
         <v>50</v>
@@ -14329,7 +14329,7 @@
         <v>582</v>
       </c>
       <c r="E157" s="2">
-        <v>44166.95833333333</v>
+        <v>44167</v>
       </c>
       <c r="F157" t="s">
         <v>50</v>
@@ -14397,7 +14397,7 @@
         <v>582</v>
       </c>
       <c r="E158" s="2">
-        <v>44166.95833333333</v>
+        <v>44167</v>
       </c>
       <c r="F158" t="s">
         <v>50</v>
@@ -14465,7 +14465,7 @@
         <v>582</v>
       </c>
       <c r="E159" s="2">
-        <v>44166.95833333333</v>
+        <v>44167</v>
       </c>
       <c r="F159" t="s">
         <v>50</v>
@@ -14533,7 +14533,7 @@
         <v>582</v>
       </c>
       <c r="E160" s="2">
-        <v>44166.95833333333</v>
+        <v>44167</v>
       </c>
       <c r="F160" t="s">
         <v>50</v>
@@ -14601,7 +14601,7 @@
         <v>582</v>
       </c>
       <c r="E161" s="2">
-        <v>44166.95833333333</v>
+        <v>44167</v>
       </c>
       <c r="F161" t="s">
         <v>50</v>
@@ -14669,7 +14669,7 @@
         <v>582</v>
       </c>
       <c r="E162" s="2">
-        <v>44166.95833333333</v>
+        <v>44167</v>
       </c>
       <c r="F162" t="s">
         <v>50</v>
@@ -14737,7 +14737,7 @@
         <v>582</v>
       </c>
       <c r="E163" s="2">
-        <v>44166.95833333333</v>
+        <v>44167</v>
       </c>
       <c r="F163" t="s">
         <v>50</v>
@@ -14805,7 +14805,7 @@
         <v>582</v>
       </c>
       <c r="E164" s="2">
-        <v>44166.95833333333</v>
+        <v>44167</v>
       </c>
       <c r="F164" t="s">
         <v>50</v>
@@ -14873,7 +14873,7 @@
         <v>582</v>
       </c>
       <c r="E165" s="2">
-        <v>44166.95833333333</v>
+        <v>44167</v>
       </c>
       <c r="F165" t="s">
         <v>50</v>
@@ -14941,7 +14941,7 @@
         <v>582</v>
       </c>
       <c r="E166" s="2">
-        <v>44166.95833333333</v>
+        <v>44167</v>
       </c>
       <c r="F166" t="s">
         <v>50</v>
@@ -15009,7 +15009,7 @@
         <v>582</v>
       </c>
       <c r="E167" s="2">
-        <v>44166.95833333333</v>
+        <v>44167</v>
       </c>
       <c r="F167" t="s">
         <v>50</v>
@@ -15077,7 +15077,7 @@
         <v>582</v>
       </c>
       <c r="E168" s="2">
-        <v>44166.95833333333</v>
+        <v>44167</v>
       </c>
       <c r="F168" t="s">
         <v>50</v>
@@ -15145,7 +15145,7 @@
         <v>582</v>
       </c>
       <c r="E169" s="2">
-        <v>44166.95833333333</v>
+        <v>44167</v>
       </c>
       <c r="F169" t="s">
         <v>50</v>
@@ -15213,7 +15213,7 @@
         <v>582</v>
       </c>
       <c r="E170" s="2">
-        <v>44166.95833333333</v>
+        <v>44167</v>
       </c>
       <c r="F170" t="s">
         <v>50</v>
@@ -15281,7 +15281,7 @@
         <v>582</v>
       </c>
       <c r="E171" s="2">
-        <v>44166.95833333333</v>
+        <v>44167</v>
       </c>
       <c r="F171" t="s">
         <v>50</v>
@@ -15349,7 +15349,7 @@
         <v>582</v>
       </c>
       <c r="E172" s="2">
-        <v>44166.95833333333</v>
+        <v>44167</v>
       </c>
       <c r="F172" t="s">
         <v>50</v>
@@ -15417,7 +15417,7 @@
         <v>582</v>
       </c>
       <c r="E173" s="2">
-        <v>44166.95833333333</v>
+        <v>44167</v>
       </c>
       <c r="F173" t="s">
         <v>50</v>
@@ -15485,7 +15485,7 @@
         <v>582</v>
       </c>
       <c r="E174" s="2">
-        <v>44166.95833333333</v>
+        <v>44167</v>
       </c>
       <c r="F174" t="s">
         <v>50</v>
@@ -15553,7 +15553,7 @@
         <v>582</v>
       </c>
       <c r="E175" s="2">
-        <v>44166.95833333333</v>
+        <v>44167</v>
       </c>
       <c r="F175" t="s">
         <v>50</v>
@@ -15621,7 +15621,7 @@
         <v>582</v>
       </c>
       <c r="E176" s="2">
-        <v>44166.95833333333</v>
+        <v>44167</v>
       </c>
       <c r="F176" t="s">
         <v>50</v>
@@ -15689,7 +15689,7 @@
         <v>582</v>
       </c>
       <c r="E177" s="2">
-        <v>44166.95833333333</v>
+        <v>44167</v>
       </c>
       <c r="F177" t="s">
         <v>50</v>
@@ -15757,7 +15757,7 @@
         <v>582</v>
       </c>
       <c r="E178" s="2">
-        <v>44166.95833333333</v>
+        <v>44167</v>
       </c>
       <c r="F178" t="s">
         <v>50</v>
@@ -15825,7 +15825,7 @@
         <v>582</v>
       </c>
       <c r="E179" s="2">
-        <v>44166.95833333333</v>
+        <v>44167</v>
       </c>
       <c r="F179" t="s">
         <v>50</v>
@@ -15893,7 +15893,7 @@
         <v>582</v>
       </c>
       <c r="E180" s="2">
-        <v>44166.95833333333</v>
+        <v>44167</v>
       </c>
       <c r="F180" t="s">
         <v>50</v>
@@ -16100,7 +16100,7 @@
         <v>41</v>
       </c>
       <c r="E183" s="2">
-        <v>44531.95833333333</v>
+        <v>44532</v>
       </c>
       <c r="F183" t="s">
         <v>50</v>
@@ -16307,7 +16307,7 @@
         <v>41</v>
       </c>
       <c r="E186" s="2">
-        <v>44594.95833333333</v>
+        <v>44595</v>
       </c>
       <c r="F186" t="s">
         <v>50</v>
@@ -16375,7 +16375,7 @@
         <v>41</v>
       </c>
       <c r="E187" s="2">
-        <v>44895.95833333333</v>
+        <v>44896</v>
       </c>
       <c r="F187" t="s">
         <v>50</v>
@@ -16408,13 +16408,13 @@
         <v>57</v>
       </c>
       <c r="P187" s="2">
-        <v>44452.91666666667</v>
+        <v>44453</v>
       </c>
       <c r="Q187" s="2">
-        <v>44874.95833333333</v>
+        <v>44875</v>
       </c>
       <c r="R187" s="2">
-        <v>44895.95833333333</v>
+        <v>44896</v>
       </c>
       <c r="S187" t="s">
         <v>36</v>
@@ -16443,7 +16443,7 @@
         <v>41</v>
       </c>
       <c r="E188" s="2">
-        <v>44895.95833333333</v>
+        <v>44896</v>
       </c>
       <c r="F188" t="s">
         <v>50</v>
@@ -16476,13 +16476,13 @@
         <v>57</v>
       </c>
       <c r="P188" s="2">
-        <v>44452.91666666667</v>
+        <v>44453</v>
       </c>
       <c r="Q188" s="2">
-        <v>44874.95833333333</v>
+        <v>44875</v>
       </c>
       <c r="R188" s="2">
-        <v>44895.95833333333</v>
+        <v>44896</v>
       </c>
       <c r="S188" t="s">
         <v>36</v>
@@ -16511,7 +16511,7 @@
         <v>41</v>
       </c>
       <c r="E189" s="2">
-        <v>44895.95833333333</v>
+        <v>44896</v>
       </c>
       <c r="F189" t="s">
         <v>50</v>
@@ -16573,7 +16573,7 @@
         <v>41</v>
       </c>
       <c r="E190" s="2">
-        <v>44895.95833333333</v>
+        <v>44896</v>
       </c>
       <c r="F190" t="s">
         <v>50</v>
@@ -16635,7 +16635,7 @@
         <v>149</v>
       </c>
       <c r="E191" s="2">
-        <v>44640.95833333333</v>
+        <v>44641</v>
       </c>
       <c r="F191" t="s">
         <v>26</v>
@@ -16839,7 +16839,7 @@
         <v>41</v>
       </c>
       <c r="E194" s="2">
-        <v>44895.95833333333</v>
+        <v>44896</v>
       </c>
       <c r="F194" t="s">
         <v>50</v>
@@ -16875,10 +16875,10 @@
         <v>26</v>
       </c>
       <c r="R194" s="2">
-        <v>44895.95833333333</v>
+        <v>44896</v>
       </c>
       <c r="S194" s="2">
-        <v>44844.91666666667</v>
+        <v>44845</v>
       </c>
       <c r="T194" t="s">
         <v>36</v>
@@ -16904,7 +16904,7 @@
         <v>41</v>
       </c>
       <c r="E195" s="2">
-        <v>44895.95833333333</v>
+        <v>44896</v>
       </c>
       <c r="F195" t="s">
         <v>50</v>
@@ -16940,10 +16940,10 @@
         <v>26</v>
       </c>
       <c r="R195" s="2">
-        <v>44895.95833333333</v>
+        <v>44896</v>
       </c>
       <c r="S195" s="2">
-        <v>44844.91666666667</v>
+        <v>44845</v>
       </c>
       <c r="T195" t="s">
         <v>36</v>
@@ -16969,7 +16969,7 @@
         <v>41</v>
       </c>
       <c r="E196" s="2">
-        <v>44914.95833333333</v>
+        <v>44915</v>
       </c>
       <c r="F196" t="s">
         <v>50</v>
@@ -17037,7 +17037,7 @@
         <v>41</v>
       </c>
       <c r="E197" s="2">
-        <v>45238.95833333333</v>
+        <v>45239</v>
       </c>
       <c r="F197" t="s">
         <v>50</v>
@@ -17070,10 +17070,10 @@
         <v>57</v>
       </c>
       <c r="P197" s="2">
-        <v>44811.91666666667</v>
+        <v>44812</v>
       </c>
       <c r="Q197" s="2">
-        <v>45238.95833333333</v>
+        <v>45239</v>
       </c>
       <c r="R197" t="s">
         <v>26</v>
@@ -17105,7 +17105,7 @@
         <v>41</v>
       </c>
       <c r="E198" s="2">
-        <v>45238.95833333333</v>
+        <v>45239</v>
       </c>
       <c r="F198" t="s">
         <v>50</v>
@@ -17138,10 +17138,10 @@
         <v>57</v>
       </c>
       <c r="P198" s="2">
-        <v>44811.91666666667</v>
+        <v>44812</v>
       </c>
       <c r="Q198" s="2">
-        <v>45238.95833333333</v>
+        <v>45239</v>
       </c>
       <c r="R198" t="s">
         <v>26</v>
@@ -17335,7 +17335,7 @@
         <v>41</v>
       </c>
       <c r="E202" s="2">
-        <v>45130.91666666667</v>
+        <v>45131</v>
       </c>
       <c r="F202" t="s">
         <v>50</v>
@@ -17368,7 +17368,7 @@
         <v>57</v>
       </c>
       <c r="P202" s="2">
-        <v>44872.95833333333</v>
+        <v>44873</v>
       </c>
       <c r="Q202" t="s">
         <v>26</v>
@@ -17403,7 +17403,7 @@
         <v>41</v>
       </c>
       <c r="E203" s="2">
-        <v>45130.91666666667</v>
+        <v>45131</v>
       </c>
       <c r="F203" t="s">
         <v>50</v>
@@ -17436,7 +17436,7 @@
         <v>57</v>
       </c>
       <c r="P203" s="2">
-        <v>44872.95833333333</v>
+        <v>44873</v>
       </c>
       <c r="Q203" t="s">
         <v>26</v>
@@ -17471,7 +17471,7 @@
         <v>490</v>
       </c>
       <c r="E204" s="2">
-        <v>45235.95833333333</v>
+        <v>45236</v>
       </c>
       <c r="F204" t="s">
         <v>50</v>

</xml_diff>

<commit_message>
generated all the reports on 2023-12-08
</commit_message>
<xml_diff>
--- a/report/merged_configurations.xlsx
+++ b/report/merged_configurations.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4811" uniqueCount="1039">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4811" uniqueCount="1038">
   <si>
     <t>naam</t>
   </si>
@@ -83,7 +83,7 @@
     <t>datum_van_review</t>
   </si>
   <si>
-    <t>Vocabularia en Applicatieprofiel IMKL</t>
+    <t>Vocabularium en Applicatieprofiel Nutsvoorzieningen</t>
   </si>
   <si>
     <t>Agentschap Digitaal Vlaanderen</t>
@@ -95,13 +95,13 @@
     <t>Aanbevolen</t>
   </si>
   <si>
-    <t>Vocabularia &amp; applicatieprofiel</t>
-  </si>
-  <si>
-    <t>imkl-description.md</t>
-  </si>
-  <si>
-    <t>[{"naam":"OSLO-IMKL","waarde":"https://data.vlaanderen.be/doc/applicatieprofiel/imkl"}]</t>
+    <t>Vocabularium &amp; applicatieprofiel</t>
+  </si>
+  <si>
+    <t>nutsvoorzieningen-description.md</t>
+  </si>
+  <si>
+    <t>[{"naam":"Nutsvoorzieningen Vocabularium","waarde":"https://data.vlaanderen.be/ns/nutsvoorzieningen"},{"naam":"Nutsvoorzieningen Applicatieprofiel","waarde":"https://data.vlaanderen.be/doc/applicatieprofiel/nutsvoorzieningen"}]</t>
   </si>
   <si>
     <t>[]</t>
@@ -116,7 +116,7 @@
     <t>[{"naam":"Presentatie business werkgroep - 24 april 2023","waarde":"Business Werkgroep presentatie IMKL - 24 april 2023"},{"naam":"Presentatie thematische werkgroep 1 - 25 mei 2023","waarde":"Presentatie eerste thematische werkgroep - IMKL -  25 mei 2023.pdf"},{"naam":"Presentatie thematische werkgroep 2 - 29 juni 2023","waarde":"Presentatie tweede thematische werkgroep - IMKL -  29 juni 2023.pdf"}]</t>
   </si>
   <si>
-    <t>Semantische standaard voor informatie over informatiemodel kabels en leidingen</t>
+    <t>Semantische standaard voor informatie over nutsvoorzieningen</t>
   </si>
   <si>
     <t>Alle entiteiten van de Vlaamse Overheid</t>
@@ -2970,9 +2970,6 @@
   </si>
   <si>
     <t>Vocabularium en Applicatieprofiel Leercredential</t>
-  </si>
-  <si>
-    <t>Vocabularium &amp; applicatieprofiel</t>
   </si>
   <si>
     <t>leercredential-description.md</t>
@@ -17222,34 +17219,34 @@
         <v>60</v>
       </c>
       <c r="G197" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="H197" s="3" t="s">
         <v>986</v>
       </c>
-      <c r="H197" s="3" t="s">
+      <c r="I197" s="3" t="s">
         <v>987</v>
       </c>
-      <c r="I197" s="3" t="s">
+      <c r="J197" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="K197" s="3" t="s">
         <v>988</v>
       </c>
-      <c r="J197" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="K197" s="3" t="s">
+      <c r="L197" s="3" t="s">
         <v>989</v>
       </c>
-      <c r="L197" s="3" t="s">
+      <c r="M197" s="3" t="s">
         <v>990</v>
       </c>
-      <c r="M197" s="3" t="s">
+      <c r="N197" s="3" t="s">
         <v>991</v>
       </c>
-      <c r="N197" s="3" t="s">
+      <c r="O197" s="3" t="s">
         <v>992</v>
       </c>
-      <c r="O197" s="3" t="s">
+      <c r="P197" s="3" t="s">
         <v>993</v>
-      </c>
-      <c r="P197" s="3" t="s">
-        <v>994</v>
       </c>
       <c r="Q197" s="3" t="s">
         <v>36</v>
@@ -17275,7 +17272,7 @@
     </row>
     <row r="198" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A198" s="3" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="B198" s="3"/>
       <c r="C198" s="3" t="s">
@@ -17297,22 +17294,22 @@
         <v>61</v>
       </c>
       <c r="I198" s="3" t="s">
+        <v>995</v>
+      </c>
+      <c r="J198" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="K198" s="3" t="s">
         <v>996</v>
       </c>
-      <c r="J198" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="K198" s="3" t="s">
+      <c r="L198" s="3" t="s">
         <v>997</v>
       </c>
-      <c r="L198" s="3" t="s">
+      <c r="M198" s="3" t="s">
         <v>998</v>
       </c>
-      <c r="M198" s="3" t="s">
+      <c r="N198" s="3" t="s">
         <v>999</v>
-      </c>
-      <c r="N198" s="3" t="s">
-        <v>1000</v>
       </c>
       <c r="O198" s="3" t="s">
         <v>35</v>
@@ -17344,7 +17341,7 @@
     </row>
     <row r="199" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A199" s="3" t="s">
-        <v>1001</v>
+        <v>1000</v>
       </c>
       <c r="B199" s="3"/>
       <c r="C199" s="3" t="s">
@@ -17366,22 +17363,22 @@
         <v>61</v>
       </c>
       <c r="I199" s="3" t="s">
+        <v>1001</v>
+      </c>
+      <c r="J199" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="K199" s="3" t="s">
+        <v>996</v>
+      </c>
+      <c r="L199" s="3" t="s">
         <v>1002</v>
       </c>
-      <c r="J199" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="K199" s="3" t="s">
-        <v>997</v>
-      </c>
-      <c r="L199" s="3" t="s">
-        <v>1003</v>
-      </c>
       <c r="M199" s="3" t="s">
+        <v>998</v>
+      </c>
+      <c r="N199" s="3" t="s">
         <v>999</v>
-      </c>
-      <c r="N199" s="3" t="s">
-        <v>1000</v>
       </c>
       <c r="O199" s="3" t="s">
         <v>35</v>
@@ -17413,7 +17410,7 @@
     </row>
     <row r="200" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A200" s="3" t="s">
-        <v>1004</v>
+        <v>1003</v>
       </c>
       <c r="B200" s="3"/>
       <c r="C200" s="3" t="s">
@@ -17427,11 +17424,11 @@
         <v>60</v>
       </c>
       <c r="G200" s="3" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
       <c r="H200" s="3"/>
       <c r="I200" s="3" t="s">
-        <v>1006</v>
+        <v>1005</v>
       </c>
       <c r="J200" s="3" t="s">
         <v>30</v>
@@ -17468,7 +17465,7 @@
     </row>
     <row r="201" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A201" s="3" t="s">
-        <v>1007</v>
+        <v>1006</v>
       </c>
       <c r="B201" s="3"/>
       <c r="C201" s="3" t="s">
@@ -17487,25 +17484,25 @@
         <v>162</v>
       </c>
       <c r="H201" s="3" t="s">
+        <v>1007</v>
+      </c>
+      <c r="I201" s="3" t="s">
         <v>1008</v>
       </c>
-      <c r="I201" s="3" t="s">
+      <c r="J201" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="K201" s="3" t="s">
         <v>1009</v>
       </c>
-      <c r="J201" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="K201" s="3" t="s">
+      <c r="L201" s="3" t="s">
         <v>1010</v>
       </c>
-      <c r="L201" s="3" t="s">
+      <c r="M201" s="3" t="s">
         <v>1011</v>
       </c>
-      <c r="M201" s="3" t="s">
+      <c r="N201" s="3" t="s">
         <v>1012</v>
-      </c>
-      <c r="N201" s="3" t="s">
-        <v>1013</v>
       </c>
       <c r="O201" s="3"/>
       <c r="P201" s="3" t="s">
@@ -17535,7 +17532,7 @@
     </row>
     <row r="202" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A202" s="3" t="s">
-        <v>1014</v>
+        <v>1013</v>
       </c>
       <c r="B202" s="3"/>
       <c r="C202" s="3" t="s">
@@ -17551,22 +17548,22 @@
       </c>
       <c r="H202" s="3"/>
       <c r="I202" s="3" t="s">
+        <v>1014</v>
+      </c>
+      <c r="J202" s="3" t="s">
         <v>1015</v>
       </c>
-      <c r="J202" s="3" t="s">
+      <c r="K202" s="3" t="s">
         <v>1016</v>
       </c>
-      <c r="K202" s="3" t="s">
+      <c r="L202" s="3" t="s">
         <v>1017</v>
       </c>
-      <c r="L202" s="3" t="s">
+      <c r="M202" s="3" t="s">
         <v>1018</v>
       </c>
-      <c r="M202" s="3" t="s">
+      <c r="N202" s="3" t="s">
         <v>1019</v>
-      </c>
-      <c r="N202" s="3" t="s">
-        <v>1020</v>
       </c>
       <c r="O202" s="3" t="s">
         <v>35</v>
@@ -17592,7 +17589,7 @@
     </row>
     <row r="203" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A203" s="3" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
       <c r="B203" s="3"/>
       <c r="C203" s="3" t="s">
@@ -17614,22 +17611,22 @@
         <v>61</v>
       </c>
       <c r="I203" s="3" t="s">
+        <v>1021</v>
+      </c>
+      <c r="J203" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="K203" s="3" t="s">
         <v>1022</v>
       </c>
-      <c r="J203" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="K203" s="3" t="s">
+      <c r="L203" s="3" t="s">
         <v>1023</v>
       </c>
-      <c r="L203" s="3" t="s">
+      <c r="M203" s="3" t="s">
         <v>1024</v>
       </c>
-      <c r="M203" s="3" t="s">
+      <c r="N203" s="3" t="s">
         <v>1025</v>
-      </c>
-      <c r="N203" s="3" t="s">
-        <v>1026</v>
       </c>
       <c r="O203" s="3" t="s">
         <v>35</v>
@@ -17661,7 +17658,7 @@
     </row>
     <row r="204" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A204" s="3" t="s">
-        <v>1027</v>
+        <v>1026</v>
       </c>
       <c r="B204" s="3"/>
       <c r="C204" s="3" t="s">
@@ -17683,22 +17680,22 @@
         <v>61</v>
       </c>
       <c r="I204" s="3" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
       <c r="J204" s="3" t="s">
         <v>30</v>
       </c>
       <c r="K204" s="3" t="s">
+        <v>1022</v>
+      </c>
+      <c r="L204" s="3" t="s">
         <v>1023</v>
       </c>
-      <c r="L204" s="3" t="s">
+      <c r="M204" s="3" t="s">
         <v>1024</v>
       </c>
-      <c r="M204" s="3" t="s">
+      <c r="N204" s="3" t="s">
         <v>1025</v>
-      </c>
-      <c r="N204" s="3" t="s">
-        <v>1026</v>
       </c>
       <c r="O204" s="3" t="s">
         <v>35</v>
@@ -17730,7 +17727,7 @@
     </row>
     <row r="205" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A205" s="3" t="s">
-        <v>1029</v>
+        <v>1028</v>
       </c>
       <c r="B205" s="3"/>
       <c r="C205" s="3" t="s">
@@ -17749,31 +17746,31 @@
         <v>162</v>
       </c>
       <c r="H205" s="3" t="s">
+        <v>1029</v>
+      </c>
+      <c r="I205" s="3" t="s">
         <v>1030</v>
       </c>
-      <c r="I205" s="3" t="s">
+      <c r="J205" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="K205" s="3" t="s">
         <v>1031</v>
       </c>
-      <c r="J205" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="K205" s="3" t="s">
+      <c r="L205" s="3" t="s">
         <v>1032</v>
       </c>
-      <c r="L205" s="3" t="s">
+      <c r="M205" s="3" t="s">
         <v>1033</v>
       </c>
-      <c r="M205" s="3" t="s">
+      <c r="N205" s="3" t="s">
         <v>1034</v>
       </c>
-      <c r="N205" s="3" t="s">
+      <c r="O205" s="3" t="s">
         <v>1035</v>
       </c>
-      <c r="O205" s="3" t="s">
+      <c r="P205" s="3" t="s">
         <v>1036</v>
-      </c>
-      <c r="P205" s="3" t="s">
-        <v>1037</v>
       </c>
       <c r="Q205" s="3" t="s">
         <v>36</v>
@@ -17872,7 +17869,7 @@
         <v>23</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="C2" s="5" t="b">
         <v>1</v>
@@ -17928,7 +17925,7 @@
         <v>38</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="C3" s="5" t="b">
         <v>1</v>
@@ -17984,7 +17981,7 @@
         <v>48</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="C4" s="5" t="b">
         <v>1</v>
@@ -18040,7 +18037,7 @@
         <v>51</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="C5" s="5" t="b">
         <v>1</v>
@@ -18096,7 +18093,7 @@
         <v>59</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="C6" s="5" t="b">
         <v>1</v>
@@ -18152,7 +18149,7 @@
         <v>67</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="C7" s="5" t="b">
         <v>1</v>
@@ -18208,7 +18205,7 @@
         <v>76</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="C8" s="5" t="b">
         <v>1</v>
@@ -18264,7 +18261,7 @@
         <v>78</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="C9" s="5" t="b">
         <v>1</v>
@@ -18320,7 +18317,7 @@
         <v>87</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="C10" s="5" t="b">
         <v>1</v>
@@ -18488,7 +18485,7 @@
         <v>112</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="C13" s="5" t="b">
         <v>1</v>
@@ -18544,7 +18541,7 @@
         <v>123</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="C14" s="5" t="b">
         <v>1</v>
@@ -18600,7 +18597,7 @@
         <v>125</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="C15" s="5" t="b">
         <v>1</v>
@@ -18656,7 +18653,7 @@
         <v>127</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="C16" s="5" t="b">
         <v>1</v>
@@ -18712,7 +18709,7 @@
         <v>129</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="C17" s="5" t="b">
         <v>1</v>
@@ -18768,7 +18765,7 @@
         <v>132</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="C18" s="5" t="b">
         <v>1</v>
@@ -18824,7 +18821,7 @@
         <v>134</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="C19" s="5" t="b">
         <v>1</v>
@@ -18880,7 +18877,7 @@
         <v>136</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="C20" s="5" t="b">
         <v>1</v>
@@ -18936,7 +18933,7 @@
         <v>138</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="C21" s="5" t="b">
         <v>1</v>
@@ -18992,7 +18989,7 @@
         <v>140</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="C22" s="5" t="b">
         <v>1</v>
@@ -19048,7 +19045,7 @@
         <v>142</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="C23" s="5" t="b">
         <v>1</v>
@@ -19104,7 +19101,7 @@
         <v>140</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="C24" s="5" t="b">
         <v>1</v>
@@ -19160,7 +19157,7 @@
         <v>144</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="C25" s="5" t="b">
         <v>1</v>
@@ -19216,7 +19213,7 @@
         <v>146</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="C26" s="5" t="b">
         <v>1</v>
@@ -19272,7 +19269,7 @@
         <v>148</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="C27" s="5" t="b">
         <v>1</v>
@@ -19328,7 +19325,7 @@
         <v>150</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="C28" s="5" t="b">
         <v>1</v>
@@ -19384,7 +19381,7 @@
         <v>152</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="C29" s="5" t="b">
         <v>1</v>
@@ -19440,7 +19437,7 @@
         <v>154</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="C30" s="5" t="b">
         <v>1</v>
@@ -19496,7 +19493,7 @@
         <v>156</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="C31" s="5" t="b">
         <v>1</v>
@@ -19552,7 +19549,7 @@
         <v>158</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="C32" s="5" t="b">
         <v>1</v>
@@ -19608,7 +19605,7 @@
         <v>160</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="C33" s="5" t="b">
         <v>1</v>
@@ -19776,7 +19773,7 @@
         <v>190</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="C36" s="5" t="b">
         <v>1</v>
@@ -19832,7 +19829,7 @@
         <v>197</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="C37" s="5" t="b">
         <v>1</v>
@@ -21400,7 +21397,7 @@
         <v>379</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="C65" s="5" t="b">
         <v>1</v>
@@ -21456,7 +21453,7 @@
         <v>391</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="C66" s="5" t="b">
         <v>1</v>
@@ -21904,7 +21901,7 @@
         <v>450</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="C74" s="5" t="b">
         <v>1</v>
@@ -22576,7 +22573,7 @@
         <v>531</v>
       </c>
       <c r="B86" s="3" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="C86" s="5" t="b">
         <v>1</v>
@@ -22632,7 +22629,7 @@
         <v>540</v>
       </c>
       <c r="B87" s="3" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="C87" s="5" t="b">
         <v>1</v>
@@ -22688,7 +22685,7 @@
         <v>542</v>
       </c>
       <c r="B88" s="3" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="C88" s="5" t="b">
         <v>1</v>
@@ -24816,7 +24813,7 @@
         <v>696</v>
       </c>
       <c r="B126" s="3" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="C126" s="5" t="b">
         <v>1</v>
@@ -25376,7 +25373,7 @@
         <v>728</v>
       </c>
       <c r="B136" s="3" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="C136" s="5" t="b">
         <v>1</v>
@@ -25432,7 +25429,7 @@
         <v>734</v>
       </c>
       <c r="B137" s="3" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="C137" s="5" t="b">
         <v>1</v>
@@ -25600,7 +25597,7 @@
         <v>754</v>
       </c>
       <c r="B140" s="3" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="C140" s="5" t="b">
         <v>1</v>
@@ -25656,7 +25653,7 @@
         <v>756</v>
       </c>
       <c r="B141" s="3" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="C141" s="5" t="b">
         <v>1</v>
@@ -25712,7 +25709,7 @@
         <v>765</v>
       </c>
       <c r="B142" s="3" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="C142" s="5" t="b">
         <v>1</v>
@@ -25768,7 +25765,7 @@
         <v>769</v>
       </c>
       <c r="B143" s="3" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="C143" s="5" t="b">
         <v>1</v>
@@ -25824,7 +25821,7 @@
         <v>772</v>
       </c>
       <c r="B144" s="3" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="C144" s="5" t="b">
         <v>1</v>
@@ -25880,7 +25877,7 @@
         <v>775</v>
       </c>
       <c r="B145" s="3" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="C145" s="5" t="b">
         <v>1</v>
@@ -25936,7 +25933,7 @@
         <v>778</v>
       </c>
       <c r="B146" s="3" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="C146" s="5" t="b">
         <v>1</v>
@@ -25992,7 +25989,7 @@
         <v>781</v>
       </c>
       <c r="B147" s="3" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="C147" s="5" t="b">
         <v>1</v>
@@ -26048,7 +26045,7 @@
         <v>784</v>
       </c>
       <c r="B148" s="3" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="C148" s="5" t="b">
         <v>1</v>
@@ -26104,7 +26101,7 @@
         <v>787</v>
       </c>
       <c r="B149" s="3" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="C149" s="5" t="b">
         <v>1</v>
@@ -26160,7 +26157,7 @@
         <v>790</v>
       </c>
       <c r="B150" s="3" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="C150" s="5" t="b">
         <v>1</v>
@@ -26216,7 +26213,7 @@
         <v>793</v>
       </c>
       <c r="B151" s="3" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="C151" s="5" t="b">
         <v>1</v>
@@ -26272,7 +26269,7 @@
         <v>796</v>
       </c>
       <c r="B152" s="3" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="C152" s="5" t="b">
         <v>1</v>
@@ -26328,7 +26325,7 @@
         <v>799</v>
       </c>
       <c r="B153" s="3" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="C153" s="5" t="b">
         <v>1</v>
@@ -26384,7 +26381,7 @@
         <v>802</v>
       </c>
       <c r="B154" s="3" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="C154" s="5" t="b">
         <v>1</v>
@@ -26440,7 +26437,7 @@
         <v>805</v>
       </c>
       <c r="B155" s="3" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="C155" s="5" t="b">
         <v>1</v>
@@ -26496,7 +26493,7 @@
         <v>808</v>
       </c>
       <c r="B156" s="3" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="C156" s="5" t="b">
         <v>1</v>
@@ -26552,7 +26549,7 @@
         <v>811</v>
       </c>
       <c r="B157" s="3" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="C157" s="5" t="b">
         <v>1</v>
@@ -26608,7 +26605,7 @@
         <v>814</v>
       </c>
       <c r="B158" s="3" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="C158" s="5" t="b">
         <v>1</v>
@@ -26664,7 +26661,7 @@
         <v>817</v>
       </c>
       <c r="B159" s="3" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="C159" s="5" t="b">
         <v>1</v>
@@ -26720,7 +26717,7 @@
         <v>820</v>
       </c>
       <c r="B160" s="3" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="C160" s="5" t="b">
         <v>1</v>
@@ -26776,7 +26773,7 @@
         <v>823</v>
       </c>
       <c r="B161" s="3" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="C161" s="5" t="b">
         <v>1</v>
@@ -26832,7 +26829,7 @@
         <v>826</v>
       </c>
       <c r="B162" s="3" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="C162" s="5" t="b">
         <v>1</v>
@@ -26888,7 +26885,7 @@
         <v>829</v>
       </c>
       <c r="B163" s="3" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="C163" s="5" t="b">
         <v>1</v>
@@ -26944,7 +26941,7 @@
         <v>832</v>
       </c>
       <c r="B164" s="3" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="C164" s="5" t="b">
         <v>1</v>
@@ -27000,7 +26997,7 @@
         <v>835</v>
       </c>
       <c r="B165" s="3" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="C165" s="5" t="b">
         <v>1</v>
@@ -27056,7 +27053,7 @@
         <v>838</v>
       </c>
       <c r="B166" s="3" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="C166" s="5" t="b">
         <v>1</v>
@@ -27112,7 +27109,7 @@
         <v>841</v>
       </c>
       <c r="B167" s="3" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="C167" s="5" t="b">
         <v>1</v>
@@ -27168,7 +27165,7 @@
         <v>844</v>
       </c>
       <c r="B168" s="3" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="C168" s="5" t="b">
         <v>1</v>
@@ -27224,7 +27221,7 @@
         <v>847</v>
       </c>
       <c r="B169" s="3" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="C169" s="5" t="b">
         <v>1</v>
@@ -27280,7 +27277,7 @@
         <v>850</v>
       </c>
       <c r="B170" s="3" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="C170" s="5" t="b">
         <v>1</v>
@@ -27336,7 +27333,7 @@
         <v>853</v>
       </c>
       <c r="B171" s="3" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="C171" s="5" t="b">
         <v>1</v>
@@ -27392,7 +27389,7 @@
         <v>856</v>
       </c>
       <c r="B172" s="3" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="C172" s="5" t="b">
         <v>1</v>
@@ -27448,7 +27445,7 @@
         <v>859</v>
       </c>
       <c r="B173" s="3" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="C173" s="5" t="b">
         <v>1</v>
@@ -27504,7 +27501,7 @@
         <v>862</v>
       </c>
       <c r="B174" s="3" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="C174" s="5" t="b">
         <v>1</v>
@@ -27560,7 +27557,7 @@
         <v>865</v>
       </c>
       <c r="B175" s="3" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="C175" s="5" t="b">
         <v>1</v>
@@ -27616,7 +27613,7 @@
         <v>868</v>
       </c>
       <c r="B176" s="3" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="C176" s="5" t="b">
         <v>1</v>
@@ -27672,7 +27669,7 @@
         <v>870</v>
       </c>
       <c r="B177" s="3" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="C177" s="5" t="b">
         <v>1</v>
@@ -27728,7 +27725,7 @@
         <v>873</v>
       </c>
       <c r="B178" s="3" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="C178" s="5" t="b">
         <v>1</v>
@@ -27784,7 +27781,7 @@
         <v>875</v>
       </c>
       <c r="B179" s="3" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="C179" s="5" t="b">
         <v>1</v>
@@ -27840,7 +27837,7 @@
         <v>877</v>
       </c>
       <c r="B180" s="3" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="C180" s="5" t="b">
         <v>1</v>
@@ -27896,7 +27893,7 @@
         <v>879</v>
       </c>
       <c r="B181" s="3" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="C181" s="5" t="b">
         <v>1</v>
@@ -27952,7 +27949,7 @@
         <v>882</v>
       </c>
       <c r="B182" s="3" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="C182" s="5" t="b">
         <v>1</v>
@@ -28008,7 +28005,7 @@
         <v>888</v>
       </c>
       <c r="B183" s="3" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="C183" s="5" t="b">
         <v>1</v>
@@ -28120,7 +28117,7 @@
         <v>906</v>
       </c>
       <c r="B185" s="3" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="C185" s="5" t="b">
         <v>1</v>
@@ -28176,7 +28173,7 @@
         <v>915</v>
       </c>
       <c r="B186" s="3" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="C186" s="5" t="b">
         <v>1</v>
@@ -28288,7 +28285,7 @@
         <v>935</v>
       </c>
       <c r="B188" s="3" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="C188" s="5" t="b">
         <v>1</v>
@@ -28344,7 +28341,7 @@
         <v>943</v>
       </c>
       <c r="B189" s="3" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="C189" s="5" t="b">
         <v>1</v>
@@ -28400,7 +28397,7 @@
         <v>945</v>
       </c>
       <c r="B190" s="3" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="C190" s="5" t="b">
         <v>1</v>
@@ -28456,7 +28453,7 @@
         <v>952</v>
       </c>
       <c r="B191" s="3" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="C191" s="5" t="b">
         <v>1</v>
@@ -28512,7 +28509,7 @@
         <v>954</v>
       </c>
       <c r="B192" s="3" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="C192" s="5" t="b">
         <v>1</v>
@@ -28568,7 +28565,7 @@
         <v>964</v>
       </c>
       <c r="B193" s="3" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="C193" s="5" t="b">
         <v>1</v>
@@ -28624,7 +28621,7 @@
         <v>970</v>
       </c>
       <c r="B194" s="3" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="C194" s="5" t="b">
         <v>1</v>
@@ -28680,7 +28677,7 @@
         <v>973</v>
       </c>
       <c r="B195" s="3" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="C195" s="5" t="b">
         <v>1</v>
@@ -28736,7 +28733,7 @@
         <v>981</v>
       </c>
       <c r="B196" s="3" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="C196" s="5" t="b">
         <v>1</v>
@@ -28792,7 +28789,7 @@
         <v>985</v>
       </c>
       <c r="B197" s="3" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="C197" s="5" t="b">
         <v>1</v>
@@ -28845,10 +28842,10 @@
     </row>
     <row r="198" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A198" s="3" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="B198" s="3" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="C198" s="5" t="b">
         <v>1</v>
@@ -28901,10 +28898,10 @@
     </row>
     <row r="199" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A199" s="3" t="s">
-        <v>1001</v>
+        <v>1000</v>
       </c>
       <c r="B199" s="3" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="C199" s="5" t="b">
         <v>1</v>
@@ -28957,10 +28954,10 @@
     </row>
     <row r="200" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A200" s="3" t="s">
-        <v>1004</v>
+        <v>1003</v>
       </c>
       <c r="B200" s="3" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="C200" s="5" t="b">
         <v>1</v>
@@ -29013,10 +29010,10 @@
     </row>
     <row r="201" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A201" s="3" t="s">
-        <v>1007</v>
+        <v>1006</v>
       </c>
       <c r="B201" s="3" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="C201" s="5" t="b">
         <v>1</v>
@@ -29069,10 +29066,10 @@
     </row>
     <row r="202" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A202" s="3" t="s">
-        <v>1014</v>
+        <v>1013</v>
       </c>
       <c r="B202" s="3" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="C202" s="5" t="b">
         <v>1</v>
@@ -29125,10 +29122,10 @@
     </row>
     <row r="203" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A203" s="3" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
       <c r="B203" s="3" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="C203" s="5" t="b">
         <v>1</v>
@@ -29181,10 +29178,10 @@
     </row>
     <row r="204" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A204" s="3" t="s">
-        <v>1027</v>
+        <v>1026</v>
       </c>
       <c r="B204" s="3" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="C204" s="5" t="b">
         <v>1</v>
@@ -29237,10 +29234,10 @@
     </row>
     <row r="205" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A205" s="3" t="s">
-        <v>1029</v>
+        <v>1028</v>
       </c>
       <c r="B205" s="3" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="C205" s="5" t="b">
         <v>1</v>

</xml_diff>

<commit_message>
generated all the reports on 2023-12-14
</commit_message>
<xml_diff>
--- a/report/merged_configurations.xlsx
+++ b/report/merged_configurations.xlsx
@@ -182,7 +182,7 @@
     <t>slim-ruimtelijk-plannen-description.md</t>
   </si>
   <si>
-    <t>[{"naam":"Slim Ruimtelijk Plannen vocabularium en applicatieprofiel","waarde":"https://data.test-vlaanderen.be/doc/applicatieprofiel/slim-ruimtelijk-plannen/ontwerpstandaard/2023-10-20"}]</t>
+    <t>[{"naam":"Slim Ruimtelijk Plannen vocabularium en applicatieprofiel","waarde":"https://data.test-vlaanderen.be/doc/applicatieprofiel/slim-ruimtelijk-plannen/ontwerpstandaard/2023-12-12"}]</t>
   </si>
   <si>
     <t>[{"naam":"Projectcharter","waarde":"Werkgroep-charter-OSLO_SlimRuimtelijkPlannen.docx"}]</t>
@@ -3119,10 +3119,10 @@
     <t>[{"naam":"Werkgroep Charter Slimme Raadpleegomgeving","waarde":"Werkgroep charter OSLO Slimme Raadpleegomgeving.docx"}]</t>
   </si>
   <si>
-    <t>[{"naam":"Verslag Business Werkgroep - 17 oktober 2023","waarde":"Verslag Business Workshop Slimme Raadpleegomgeving.pdf"}]</t>
-  </si>
-  <si>
-    <t>[{"naam":"Presentatie Business Werkgroep - 17 oktober 2023","waarde":"Business Werkgroep presentatie - slimme raadpleegomgeving.pdf"},{"naam":"Presentatie Thematische Werkgroep I - 7 november 2023","waarde":"20231107 Thematische Werkgroep 1 - Slimme Raadpleegomgeving V.01.pptx"}]</t>
+    <t>[{"naam":"Verslag Business Werkgroep - 17 oktober 2023","waarde":"Verslag Business Workshop Slimme Raadpleegomgeving.pdf"},{"naam":"Verslag Thematische Werkgroep I - 7 November 2023","waarde":"20231107_ThematicWorkshop1_Verslag_OSLOSlimmeRaadpleegomgeving.pdf"},{"naam":"Verslag Thematische Werkgroep II - 28 November 2023","waarde":"20231128_ThematicWorkshop2_Verslag_OSLOSlimmeRaadpleegomgeving.pdf"}]</t>
+  </si>
+  <si>
+    <t>[{"naam":"Presentatie Business Werkgroep - 17 oktober 2023","waarde":"Business Werkgroep presentatie - slimme raadpleegomgeving.pdf"},{"naam":"Presentatie Thematische Werkgroep I - 7 november 2023","waarde":"20231107 Thematische Werkgroep 1 - Slimme Raadpleegomgeving V.01.pptx"},{"naam":"Presentatie Thematische Werkgroep II - 2 november 2023","waarde":"20231128_ThematicWorkshop2_Powerpoint_OSLOSlimmeRaadpleegomgeving.pptx"}]</t>
   </si>
   <si>
     <t>Semantische standaard voor de digitale transformatie van de Vlaamse lokale besturen</t>

</xml_diff>

<commit_message>
generated all the reports on 2023-12-20
</commit_message>
<xml_diff>
--- a/report/merged_configurations.xlsx
+++ b/report/merged_configurations.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4833" uniqueCount="1041">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4853" uniqueCount="1047">
   <si>
     <t>naam</t>
   </si>
@@ -206,7 +206,7 @@
     <t>template-description.md</t>
   </si>
   <si>
-    <t>[{"naam":"Applicatieprofiel Voorwaarden Dienstverlening","waarde":"https://data.vlaanderen.be/doc/applicatieprofiel/publicatie-advertentie/kandidaatstandaard/2023-07-11"}]</t>
+    <t>[{"naam":"Applicatieprofiel Voorwaarden Dienstverlening","waarde":"https://data.vlaanderen.be/doc/applicatieprofiel/voorwaarden-dienstverlening/kandidaatstandaard/2023-07-11"}]</t>
   </si>
   <si>
     <t>[{"naam":"Charter","waarde":"Charter OSLO Voorwaarden Dienstverlening.docx.pdf"},{"naam":"Documenten desk research","waarde":"4. Desk research.zip"}]</t>
@@ -3132,6 +3132,24 @@
   </si>
   <si>
     <t>7 november 2023</t>
+  </si>
+  <si>
+    <t>Applicatieprofiel Lokale Economie</t>
+  </si>
+  <si>
+    <t>[{"naam":"Lokale Economie Applicatieprofiel","waarde":"https://data.vlaanderen.be/doc/applicatieprofiel/lokale-economie"}]</t>
+  </si>
+  <si>
+    <t>[{"naam":"OSLO Lokale Economie Charter","waarde":"Charter_OSLO_Lokale_Economie.docx"}]</t>
+  </si>
+  <si>
+    <t>[{"naam":"Verslag business werkgroep - 19-09-2023","waarde":"Verslag Business Werkgroep - Lokale Economie - 19092023.pdf"},{"naam":"Verslag thematische werkgroep 1 - 17-10-2023","waarde":"Verslag Thematische Werkgroep 1 - Lokale Economie - 17102023.pdf"},{"naam":"Verslag thematische werkgroep 2 - 16-11-2023","waarde":"Verslag Thematische Werkgroep 2 - Lokale Economie - 16112023.pdf"}]</t>
+  </si>
+  <si>
+    <t>[{"naam":"Presentatie business werkgroep - 19-09-2023","waarde":"Presentatie Business Werkgroep - Lokale Economie - 19092023.pdf"},{"naam":"Presentatie thematische werkgroep 1 - 17-10-2023","waarde":"Presentatie Thematische Werkgroep 1 - Lokale Economie - 17102023.pdf"},{"naam":"Presentatie thematische werkgroep 2 - 16-11-2023","waarde":"Presentatie Thematische Werkgroep 2 - Lokale Economie - 16112023.pdf"}]</t>
+  </si>
+  <si>
+    <t>Semantische standaard voor informatie over Lokale Economie</t>
   </si>
   <si>
     <t>Geen rapport gevonden</t>
@@ -3542,7 +3560,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W206"/>
+  <dimension ref="A1:W207"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="23" width="44" customWidth="1"/>
@@ -17867,6 +17885,69 @@
         <v>37</v>
       </c>
       <c r="W206" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="207" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A207" s="3" t="s">
+        <v>1040</v>
+      </c>
+      <c r="B207" s="3"/>
+      <c r="C207" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D207" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E207" s="4">
+        <v>45274</v>
+      </c>
+      <c r="F207" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="G207" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="H207" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="I207" s="3" t="s">
+        <v>1041</v>
+      </c>
+      <c r="J207" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="K207" s="3" t="s">
+        <v>1042</v>
+      </c>
+      <c r="L207" s="3" t="s">
+        <v>1043</v>
+      </c>
+      <c r="M207" s="3" t="s">
+        <v>1044</v>
+      </c>
+      <c r="N207" s="3" t="s">
+        <v>1045</v>
+      </c>
+      <c r="O207" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="P207" s="3"/>
+      <c r="Q207" s="3"/>
+      <c r="R207" s="3"/>
+      <c r="S207" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="T207" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="U207" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="V207" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="W207" s="3" t="s">
         <v>37</v>
       </c>
     </row>
@@ -17878,7 +17959,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R206"/>
+  <dimension ref="A1:R207"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="18" width="44" customWidth="1"/>
@@ -17945,7 +18026,7 @@
         <v>23</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>1040</v>
+        <v>1046</v>
       </c>
       <c r="C2" s="5" t="b">
         <v>1</v>
@@ -18001,7 +18082,7 @@
         <v>38</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>1040</v>
+        <v>1046</v>
       </c>
       <c r="C3" s="5" t="b">
         <v>1</v>
@@ -18057,7 +18138,7 @@
         <v>42</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>1040</v>
+        <v>1046</v>
       </c>
       <c r="C4" s="5" t="b">
         <v>1</v>
@@ -18113,7 +18194,7 @@
         <v>51</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>1040</v>
+        <v>1046</v>
       </c>
       <c r="C5" s="5" t="b">
         <v>1</v>
@@ -18169,7 +18250,7 @@
         <v>53</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>1040</v>
+        <v>1046</v>
       </c>
       <c r="C6" s="5" t="b">
         <v>1</v>
@@ -18225,7 +18306,7 @@
         <v>61</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>1040</v>
+        <v>1046</v>
       </c>
       <c r="C7" s="5" t="b">
         <v>1</v>
@@ -18281,7 +18362,7 @@
         <v>69</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>1040</v>
+        <v>1046</v>
       </c>
       <c r="C8" s="5" t="b">
         <v>1</v>
@@ -18337,7 +18418,7 @@
         <v>78</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>1040</v>
+        <v>1046</v>
       </c>
       <c r="C9" s="5" t="b">
         <v>1</v>
@@ -18393,7 +18474,7 @@
         <v>80</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>1040</v>
+        <v>1046</v>
       </c>
       <c r="C10" s="5" t="b">
         <v>1</v>
@@ -18449,7 +18530,7 @@
         <v>89</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>1040</v>
+        <v>1046</v>
       </c>
       <c r="C11" s="5" t="b">
         <v>1</v>
@@ -18617,7 +18698,7 @@
         <v>114</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>1040</v>
+        <v>1046</v>
       </c>
       <c r="C14" s="5" t="b">
         <v>1</v>
@@ -18673,7 +18754,7 @@
         <v>125</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>1040</v>
+        <v>1046</v>
       </c>
       <c r="C15" s="5" t="b">
         <v>1</v>
@@ -18729,7 +18810,7 @@
         <v>127</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>1040</v>
+        <v>1046</v>
       </c>
       <c r="C16" s="5" t="b">
         <v>1</v>
@@ -18785,7 +18866,7 @@
         <v>129</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>1040</v>
+        <v>1046</v>
       </c>
       <c r="C17" s="5" t="b">
         <v>1</v>
@@ -18841,7 +18922,7 @@
         <v>131</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>1040</v>
+        <v>1046</v>
       </c>
       <c r="C18" s="5" t="b">
         <v>1</v>
@@ -18897,7 +18978,7 @@
         <v>134</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>1040</v>
+        <v>1046</v>
       </c>
       <c r="C19" s="5" t="b">
         <v>1</v>
@@ -18953,7 +19034,7 @@
         <v>136</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>1040</v>
+        <v>1046</v>
       </c>
       <c r="C20" s="5" t="b">
         <v>1</v>
@@ -19009,7 +19090,7 @@
         <v>138</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>1040</v>
+        <v>1046</v>
       </c>
       <c r="C21" s="5" t="b">
         <v>1</v>
@@ -19065,7 +19146,7 @@
         <v>140</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>1040</v>
+        <v>1046</v>
       </c>
       <c r="C22" s="5" t="b">
         <v>1</v>
@@ -19121,7 +19202,7 @@
         <v>142</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>1040</v>
+        <v>1046</v>
       </c>
       <c r="C23" s="5" t="b">
         <v>1</v>
@@ -19177,7 +19258,7 @@
         <v>144</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>1040</v>
+        <v>1046</v>
       </c>
       <c r="C24" s="5" t="b">
         <v>1</v>
@@ -19233,7 +19314,7 @@
         <v>142</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>1040</v>
+        <v>1046</v>
       </c>
       <c r="C25" s="5" t="b">
         <v>1</v>
@@ -19289,7 +19370,7 @@
         <v>146</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>1040</v>
+        <v>1046</v>
       </c>
       <c r="C26" s="5" t="b">
         <v>1</v>
@@ -19345,7 +19426,7 @@
         <v>148</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>1040</v>
+        <v>1046</v>
       </c>
       <c r="C27" s="5" t="b">
         <v>1</v>
@@ -19401,7 +19482,7 @@
         <v>150</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>1040</v>
+        <v>1046</v>
       </c>
       <c r="C28" s="5" t="b">
         <v>1</v>
@@ -19457,7 +19538,7 @@
         <v>152</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>1040</v>
+        <v>1046</v>
       </c>
       <c r="C29" s="5" t="b">
         <v>1</v>
@@ -19513,7 +19594,7 @@
         <v>154</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>1040</v>
+        <v>1046</v>
       </c>
       <c r="C30" s="5" t="b">
         <v>1</v>
@@ -19569,7 +19650,7 @@
         <v>156</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>1040</v>
+        <v>1046</v>
       </c>
       <c r="C31" s="5" t="b">
         <v>1</v>
@@ -19625,7 +19706,7 @@
         <v>158</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>1040</v>
+        <v>1046</v>
       </c>
       <c r="C32" s="5" t="b">
         <v>1</v>
@@ -19681,7 +19762,7 @@
         <v>160</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>1040</v>
+        <v>1046</v>
       </c>
       <c r="C33" s="5" t="b">
         <v>1</v>
@@ -19737,7 +19818,7 @@
         <v>162</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>1040</v>
+        <v>1046</v>
       </c>
       <c r="C34" s="5" t="b">
         <v>1</v>
@@ -19905,7 +19986,7 @@
         <v>192</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>1040</v>
+        <v>1046</v>
       </c>
       <c r="C37" s="5" t="b">
         <v>1</v>
@@ -19961,7 +20042,7 @@
         <v>199</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>1040</v>
+        <v>1046</v>
       </c>
       <c r="C38" s="5" t="b">
         <v>1</v>
@@ -21529,7 +21610,7 @@
         <v>381</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>1040</v>
+        <v>1046</v>
       </c>
       <c r="C66" s="5" t="b">
         <v>1</v>
@@ -21585,7 +21666,7 @@
         <v>393</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>1040</v>
+        <v>1046</v>
       </c>
       <c r="C67" s="5" t="b">
         <v>1</v>
@@ -22033,7 +22114,7 @@
         <v>452</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>1040</v>
+        <v>1046</v>
       </c>
       <c r="C75" s="5" t="b">
         <v>1</v>
@@ -22705,7 +22786,7 @@
         <v>533</v>
       </c>
       <c r="B87" s="3" t="s">
-        <v>1040</v>
+        <v>1046</v>
       </c>
       <c r="C87" s="5" t="b">
         <v>1</v>
@@ -22761,7 +22842,7 @@
         <v>542</v>
       </c>
       <c r="B88" s="3" t="s">
-        <v>1040</v>
+        <v>1046</v>
       </c>
       <c r="C88" s="5" t="b">
         <v>1</v>
@@ -22817,7 +22898,7 @@
         <v>544</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>1040</v>
+        <v>1046</v>
       </c>
       <c r="C89" s="5" t="b">
         <v>1</v>
@@ -24945,7 +25026,7 @@
         <v>698</v>
       </c>
       <c r="B127" s="3" t="s">
-        <v>1040</v>
+        <v>1046</v>
       </c>
       <c r="C127" s="5" t="b">
         <v>1</v>
@@ -25505,7 +25586,7 @@
         <v>730</v>
       </c>
       <c r="B137" s="3" t="s">
-        <v>1040</v>
+        <v>1046</v>
       </c>
       <c r="C137" s="5" t="b">
         <v>1</v>
@@ -25561,7 +25642,7 @@
         <v>736</v>
       </c>
       <c r="B138" s="3" t="s">
-        <v>1040</v>
+        <v>1046</v>
       </c>
       <c r="C138" s="5" t="b">
         <v>1</v>
@@ -25729,7 +25810,7 @@
         <v>756</v>
       </c>
       <c r="B141" s="3" t="s">
-        <v>1040</v>
+        <v>1046</v>
       </c>
       <c r="C141" s="5" t="b">
         <v>1</v>
@@ -25785,7 +25866,7 @@
         <v>758</v>
       </c>
       <c r="B142" s="3" t="s">
-        <v>1040</v>
+        <v>1046</v>
       </c>
       <c r="C142" s="5" t="b">
         <v>1</v>
@@ -25841,7 +25922,7 @@
         <v>767</v>
       </c>
       <c r="B143" s="3" t="s">
-        <v>1040</v>
+        <v>1046</v>
       </c>
       <c r="C143" s="5" t="b">
         <v>1</v>
@@ -25897,7 +25978,7 @@
         <v>771</v>
       </c>
       <c r="B144" s="3" t="s">
-        <v>1040</v>
+        <v>1046</v>
       </c>
       <c r="C144" s="5" t="b">
         <v>1</v>
@@ -25953,7 +26034,7 @@
         <v>774</v>
       </c>
       <c r="B145" s="3" t="s">
-        <v>1040</v>
+        <v>1046</v>
       </c>
       <c r="C145" s="5" t="b">
         <v>1</v>
@@ -26009,7 +26090,7 @@
         <v>777</v>
       </c>
       <c r="B146" s="3" t="s">
-        <v>1040</v>
+        <v>1046</v>
       </c>
       <c r="C146" s="5" t="b">
         <v>1</v>
@@ -26065,7 +26146,7 @@
         <v>780</v>
       </c>
       <c r="B147" s="3" t="s">
-        <v>1040</v>
+        <v>1046</v>
       </c>
       <c r="C147" s="5" t="b">
         <v>1</v>
@@ -26121,7 +26202,7 @@
         <v>783</v>
       </c>
       <c r="B148" s="3" t="s">
-        <v>1040</v>
+        <v>1046</v>
       </c>
       <c r="C148" s="5" t="b">
         <v>1</v>
@@ -26177,7 +26258,7 @@
         <v>786</v>
       </c>
       <c r="B149" s="3" t="s">
-        <v>1040</v>
+        <v>1046</v>
       </c>
       <c r="C149" s="5" t="b">
         <v>1</v>
@@ -26233,7 +26314,7 @@
         <v>789</v>
       </c>
       <c r="B150" s="3" t="s">
-        <v>1040</v>
+        <v>1046</v>
       </c>
       <c r="C150" s="5" t="b">
         <v>1</v>
@@ -26289,7 +26370,7 @@
         <v>792</v>
       </c>
       <c r="B151" s="3" t="s">
-        <v>1040</v>
+        <v>1046</v>
       </c>
       <c r="C151" s="5" t="b">
         <v>1</v>
@@ -26345,7 +26426,7 @@
         <v>795</v>
       </c>
       <c r="B152" s="3" t="s">
-        <v>1040</v>
+        <v>1046</v>
       </c>
       <c r="C152" s="5" t="b">
         <v>1</v>
@@ -26401,7 +26482,7 @@
         <v>798</v>
       </c>
       <c r="B153" s="3" t="s">
-        <v>1040</v>
+        <v>1046</v>
       </c>
       <c r="C153" s="5" t="b">
         <v>1</v>
@@ -26457,7 +26538,7 @@
         <v>801</v>
       </c>
       <c r="B154" s="3" t="s">
-        <v>1040</v>
+        <v>1046</v>
       </c>
       <c r="C154" s="5" t="b">
         <v>1</v>
@@ -26513,7 +26594,7 @@
         <v>804</v>
       </c>
       <c r="B155" s="3" t="s">
-        <v>1040</v>
+        <v>1046</v>
       </c>
       <c r="C155" s="5" t="b">
         <v>1</v>
@@ -26569,7 +26650,7 @@
         <v>807</v>
       </c>
       <c r="B156" s="3" t="s">
-        <v>1040</v>
+        <v>1046</v>
       </c>
       <c r="C156" s="5" t="b">
         <v>1</v>
@@ -26625,7 +26706,7 @@
         <v>810</v>
       </c>
       <c r="B157" s="3" t="s">
-        <v>1040</v>
+        <v>1046</v>
       </c>
       <c r="C157" s="5" t="b">
         <v>1</v>
@@ -26681,7 +26762,7 @@
         <v>813</v>
       </c>
       <c r="B158" s="3" t="s">
-        <v>1040</v>
+        <v>1046</v>
       </c>
       <c r="C158" s="5" t="b">
         <v>1</v>
@@ -26737,7 +26818,7 @@
         <v>816</v>
       </c>
       <c r="B159" s="3" t="s">
-        <v>1040</v>
+        <v>1046</v>
       </c>
       <c r="C159" s="5" t="b">
         <v>1</v>
@@ -26793,7 +26874,7 @@
         <v>819</v>
       </c>
       <c r="B160" s="3" t="s">
-        <v>1040</v>
+        <v>1046</v>
       </c>
       <c r="C160" s="5" t="b">
         <v>1</v>
@@ -26849,7 +26930,7 @@
         <v>822</v>
       </c>
       <c r="B161" s="3" t="s">
-        <v>1040</v>
+        <v>1046</v>
       </c>
       <c r="C161" s="5" t="b">
         <v>1</v>
@@ -26905,7 +26986,7 @@
         <v>825</v>
       </c>
       <c r="B162" s="3" t="s">
-        <v>1040</v>
+        <v>1046</v>
       </c>
       <c r="C162" s="5" t="b">
         <v>1</v>
@@ -26961,7 +27042,7 @@
         <v>828</v>
       </c>
       <c r="B163" s="3" t="s">
-        <v>1040</v>
+        <v>1046</v>
       </c>
       <c r="C163" s="5" t="b">
         <v>1</v>
@@ -27017,7 +27098,7 @@
         <v>831</v>
       </c>
       <c r="B164" s="3" t="s">
-        <v>1040</v>
+        <v>1046</v>
       </c>
       <c r="C164" s="5" t="b">
         <v>1</v>
@@ -27073,7 +27154,7 @@
         <v>834</v>
       </c>
       <c r="B165" s="3" t="s">
-        <v>1040</v>
+        <v>1046</v>
       </c>
       <c r="C165" s="5" t="b">
         <v>1</v>
@@ -27129,7 +27210,7 @@
         <v>837</v>
       </c>
       <c r="B166" s="3" t="s">
-        <v>1040</v>
+        <v>1046</v>
       </c>
       <c r="C166" s="5" t="b">
         <v>1</v>
@@ -27185,7 +27266,7 @@
         <v>840</v>
       </c>
       <c r="B167" s="3" t="s">
-        <v>1040</v>
+        <v>1046</v>
       </c>
       <c r="C167" s="5" t="b">
         <v>1</v>
@@ -27241,7 +27322,7 @@
         <v>843</v>
       </c>
       <c r="B168" s="3" t="s">
-        <v>1040</v>
+        <v>1046</v>
       </c>
       <c r="C168" s="5" t="b">
         <v>1</v>
@@ -27297,7 +27378,7 @@
         <v>846</v>
       </c>
       <c r="B169" s="3" t="s">
-        <v>1040</v>
+        <v>1046</v>
       </c>
       <c r="C169" s="5" t="b">
         <v>1</v>
@@ -27353,7 +27434,7 @@
         <v>849</v>
       </c>
       <c r="B170" s="3" t="s">
-        <v>1040</v>
+        <v>1046</v>
       </c>
       <c r="C170" s="5" t="b">
         <v>1</v>
@@ -27409,7 +27490,7 @@
         <v>852</v>
       </c>
       <c r="B171" s="3" t="s">
-        <v>1040</v>
+        <v>1046</v>
       </c>
       <c r="C171" s="5" t="b">
         <v>1</v>
@@ -27465,7 +27546,7 @@
         <v>855</v>
       </c>
       <c r="B172" s="3" t="s">
-        <v>1040</v>
+        <v>1046</v>
       </c>
       <c r="C172" s="5" t="b">
         <v>1</v>
@@ -27521,7 +27602,7 @@
         <v>858</v>
       </c>
       <c r="B173" s="3" t="s">
-        <v>1040</v>
+        <v>1046</v>
       </c>
       <c r="C173" s="5" t="b">
         <v>1</v>
@@ -27577,7 +27658,7 @@
         <v>861</v>
       </c>
       <c r="B174" s="3" t="s">
-        <v>1040</v>
+        <v>1046</v>
       </c>
       <c r="C174" s="5" t="b">
         <v>1</v>
@@ -27633,7 +27714,7 @@
         <v>864</v>
       </c>
       <c r="B175" s="3" t="s">
-        <v>1040</v>
+        <v>1046</v>
       </c>
       <c r="C175" s="5" t="b">
         <v>1</v>
@@ -27689,7 +27770,7 @@
         <v>867</v>
       </c>
       <c r="B176" s="3" t="s">
-        <v>1040</v>
+        <v>1046</v>
       </c>
       <c r="C176" s="5" t="b">
         <v>1</v>
@@ -27745,7 +27826,7 @@
         <v>870</v>
       </c>
       <c r="B177" s="3" t="s">
-        <v>1040</v>
+        <v>1046</v>
       </c>
       <c r="C177" s="5" t="b">
         <v>1</v>
@@ -27801,7 +27882,7 @@
         <v>872</v>
       </c>
       <c r="B178" s="3" t="s">
-        <v>1040</v>
+        <v>1046</v>
       </c>
       <c r="C178" s="5" t="b">
         <v>1</v>
@@ -27857,7 +27938,7 @@
         <v>875</v>
       </c>
       <c r="B179" s="3" t="s">
-        <v>1040</v>
+        <v>1046</v>
       </c>
       <c r="C179" s="5" t="b">
         <v>1</v>
@@ -27913,7 +27994,7 @@
         <v>877</v>
       </c>
       <c r="B180" s="3" t="s">
-        <v>1040</v>
+        <v>1046</v>
       </c>
       <c r="C180" s="5" t="b">
         <v>1</v>
@@ -27969,7 +28050,7 @@
         <v>879</v>
       </c>
       <c r="B181" s="3" t="s">
-        <v>1040</v>
+        <v>1046</v>
       </c>
       <c r="C181" s="5" t="b">
         <v>1</v>
@@ -28025,7 +28106,7 @@
         <v>881</v>
       </c>
       <c r="B182" s="3" t="s">
-        <v>1040</v>
+        <v>1046</v>
       </c>
       <c r="C182" s="5" t="b">
         <v>1</v>
@@ -28081,7 +28162,7 @@
         <v>884</v>
       </c>
       <c r="B183" s="3" t="s">
-        <v>1040</v>
+        <v>1046</v>
       </c>
       <c r="C183" s="5" t="b">
         <v>1</v>
@@ -28137,7 +28218,7 @@
         <v>890</v>
       </c>
       <c r="B184" s="3" t="s">
-        <v>1040</v>
+        <v>1046</v>
       </c>
       <c r="C184" s="5" t="b">
         <v>1</v>
@@ -28249,7 +28330,7 @@
         <v>908</v>
       </c>
       <c r="B186" s="3" t="s">
-        <v>1040</v>
+        <v>1046</v>
       </c>
       <c r="C186" s="5" t="b">
         <v>1</v>
@@ -28305,7 +28386,7 @@
         <v>917</v>
       </c>
       <c r="B187" s="3" t="s">
-        <v>1040</v>
+        <v>1046</v>
       </c>
       <c r="C187" s="5" t="b">
         <v>1</v>
@@ -28417,7 +28498,7 @@
         <v>937</v>
       </c>
       <c r="B189" s="3" t="s">
-        <v>1040</v>
+        <v>1046</v>
       </c>
       <c r="C189" s="5" t="b">
         <v>1</v>
@@ -28473,7 +28554,7 @@
         <v>945</v>
       </c>
       <c r="B190" s="3" t="s">
-        <v>1040</v>
+        <v>1046</v>
       </c>
       <c r="C190" s="5" t="b">
         <v>1</v>
@@ -28529,7 +28610,7 @@
         <v>947</v>
       </c>
       <c r="B191" s="3" t="s">
-        <v>1040</v>
+        <v>1046</v>
       </c>
       <c r="C191" s="5" t="b">
         <v>1</v>
@@ -28585,7 +28666,7 @@
         <v>954</v>
       </c>
       <c r="B192" s="3" t="s">
-        <v>1040</v>
+        <v>1046</v>
       </c>
       <c r="C192" s="5" t="b">
         <v>1</v>
@@ -28641,7 +28722,7 @@
         <v>956</v>
       </c>
       <c r="B193" s="3" t="s">
-        <v>1040</v>
+        <v>1046</v>
       </c>
       <c r="C193" s="5" t="b">
         <v>1</v>
@@ -28697,7 +28778,7 @@
         <v>966</v>
       </c>
       <c r="B194" s="3" t="s">
-        <v>1040</v>
+        <v>1046</v>
       </c>
       <c r="C194" s="5" t="b">
         <v>1</v>
@@ -28753,7 +28834,7 @@
         <v>972</v>
       </c>
       <c r="B195" s="3" t="s">
-        <v>1040</v>
+        <v>1046</v>
       </c>
       <c r="C195" s="5" t="b">
         <v>1</v>
@@ -28809,7 +28890,7 @@
         <v>975</v>
       </c>
       <c r="B196" s="3" t="s">
-        <v>1040</v>
+        <v>1046</v>
       </c>
       <c r="C196" s="5" t="b">
         <v>1</v>
@@ -28865,7 +28946,7 @@
         <v>983</v>
       </c>
       <c r="B197" s="3" t="s">
-        <v>1040</v>
+        <v>1046</v>
       </c>
       <c r="C197" s="5" t="b">
         <v>1</v>
@@ -28921,7 +29002,7 @@
         <v>987</v>
       </c>
       <c r="B198" s="3" t="s">
-        <v>1040</v>
+        <v>1046</v>
       </c>
       <c r="C198" s="5" t="b">
         <v>1</v>
@@ -28977,7 +29058,7 @@
         <v>997</v>
       </c>
       <c r="B199" s="3" t="s">
-        <v>1040</v>
+        <v>1046</v>
       </c>
       <c r="C199" s="5" t="b">
         <v>1</v>
@@ -29033,7 +29114,7 @@
         <v>1003</v>
       </c>
       <c r="B200" s="3" t="s">
-        <v>1040</v>
+        <v>1046</v>
       </c>
       <c r="C200" s="5" t="b">
         <v>1</v>
@@ -29089,7 +29170,7 @@
         <v>1006</v>
       </c>
       <c r="B201" s="3" t="s">
-        <v>1040</v>
+        <v>1046</v>
       </c>
       <c r="C201" s="5" t="b">
         <v>1</v>
@@ -29145,7 +29226,7 @@
         <v>1009</v>
       </c>
       <c r="B202" s="3" t="s">
-        <v>1040</v>
+        <v>1046</v>
       </c>
       <c r="C202" s="5" t="b">
         <v>1</v>
@@ -29201,7 +29282,7 @@
         <v>1016</v>
       </c>
       <c r="B203" s="3" t="s">
-        <v>1040</v>
+        <v>1046</v>
       </c>
       <c r="C203" s="5" t="b">
         <v>1</v>
@@ -29257,7 +29338,7 @@
         <v>1023</v>
       </c>
       <c r="B204" s="3" t="s">
-        <v>1040</v>
+        <v>1046</v>
       </c>
       <c r="C204" s="5" t="b">
         <v>1</v>
@@ -29313,7 +29394,7 @@
         <v>1029</v>
       </c>
       <c r="B205" s="3" t="s">
-        <v>1040</v>
+        <v>1046</v>
       </c>
       <c r="C205" s="5" t="b">
         <v>1</v>
@@ -29369,54 +29450,110 @@
         <v>1031</v>
       </c>
       <c r="B206" s="3" t="s">
+        <v>1046</v>
+      </c>
+      <c r="C206" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="D206" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="E206" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="F206" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="G206" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="H206" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="I206" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="J206" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="K206" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="L206" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="M206" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="N206" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="O206" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="P206" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q206" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="R206" s="6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="207" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A207" s="3" t="s">
         <v>1040</v>
       </c>
-      <c r="C206" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="D206" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="E206" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="F206" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="G206" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="H206" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="I206" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="J206" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="K206" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="L206" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="M206" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="N206" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="O206" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="P206" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q206" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="R206" s="6" t="b">
+      <c r="B207" s="3" t="s">
+        <v>1046</v>
+      </c>
+      <c r="C207" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="D207" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="E207" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="F207" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="G207" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="H207" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="I207" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="J207" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="K207" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="L207" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="M207" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="N207" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="O207" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="P207" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q207" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="R207" s="6" t="b">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
generated all the reports on 2024-01-12
</commit_message>
<xml_diff>
--- a/report/merged_configurations.xlsx
+++ b/report/merged_configurations.xlsx
@@ -3143,10 +3143,10 @@
     <t>[{"naam":"OSLO Lokale Economie Charter","waarde":"Charter_OSLO_Lokale_Economie.docx"}]</t>
   </si>
   <si>
-    <t>[{"naam":"Verslag business werkgroep - 19-09-2023","waarde":"Verslag Business Werkgroep - Lokale Economie - 19092023.pdf"},{"naam":"Verslag thematische werkgroep 1 - 17-10-2023","waarde":"Verslag Thematische Werkgroep 1 - Lokale Economie - 17102023.pdf"},{"naam":"Verslag thematische werkgroep 2 - 16-11-2023","waarde":"Verslag Thematische Werkgroep 2 - Lokale Economie - 16112023.pdf"}]</t>
-  </si>
-  <si>
-    <t>[{"naam":"Presentatie business werkgroep - 19-09-2023","waarde":"Presentatie Business Werkgroep - Lokale Economie - 19092023.pdf"},{"naam":"Presentatie thematische werkgroep 1 - 17-10-2023","waarde":"Presentatie Thematische Werkgroep 1 - Lokale Economie - 17102023.pdf"},{"naam":"Presentatie thematische werkgroep 2 - 16-11-2023","waarde":"Presentatie Thematische Werkgroep 2 - Lokale Economie - 16112023.pdf"}]</t>
+    <t>[{"naam":"Verslag business werkgroep - 19-09-2023","waarde":"Verslag Business Werkgroep - Lokale Economie - 19092023.pdf"},{"naam":"Verslag thematische werkgroep 1 - 17-10-2023","waarde":"Verslag Thematische Werkgroep 1 - Lokale Economie - 17102023.pdf"},{"naam":"Verslag thematische werkgroep 2 - 16-11-2023","waarde":"Verslag Thematische Werkgroep 2 - Lokale Economie - 16112023.pdf"},{"naam":"Verslag thematische werkgroep 3 - 19-12-2023","waarde":"Verslag Thematische Werkgroep 3 - Lokale Economie - 1912023.pdf"}]</t>
+  </si>
+  <si>
+    <t>[{"naam":"Presentatie business werkgroep - 19-09-2023","waarde":"Presentatie Business Werkgroep - Lokale Economie - 19092023.pdf"},{"naam":"Presentatie thematische werkgroep 1 - 17-10-2023","waarde":"Presentatie Thematische Werkgroep 1 - Lokale Economie - 17102023.pdf"},{"naam":"Presentatie thematische werkgroep 2 - 16-11-2023","waarde":"Presentatie Thematische Werkgroep 2 - Lokale Economie - 16112023.pdf"},{"naam":"Presentatie thematische werkgroep 3 - 19-12-2023","waarde":"Presentatie Thematische Werkgroep 3 - Lokale Economie - 19122023.pdf"}]</t>
   </si>
   <si>
     <t>Semantische standaard voor informatie over Lokale Economie</t>

</xml_diff>

<commit_message>
generated all the reports on 2024-01-16
</commit_message>
<xml_diff>
--- a/report/merged_configurations.xlsx
+++ b/report/merged_configurations.xlsx
@@ -188,10 +188,10 @@
     <t>[{"naam":"Projectcharter","waarde":"Werkgroep-charter-OSLO_SlimRuimtelijkPlannen.docx"}]</t>
   </si>
   <si>
-    <t>[{"naam":"Verslag Business werkgroep - OSLO Slim Ruimtelijk Plannen 27 september 2023","waarde":"Verslag Business werkgroep SRP 2023-09-27.pdf"},{"naam":"Verslag thematische werkgroep 1 - OSLO Slim Ruimtelijk Plannen 25 oktober 2023","waarde":"Verslag 1e thematische werkgroep SRP 2023-09-25.pdf"},{"naam":"Verslag thematische werkgroep 2 - OSLO Slim Ruimtelijk Plannen 30 november 2023","waarde":"Verslag thematische werkgroep 2 - OSLO Slim Ruimtelijk Plannen 30 november 2023.docx"}]</t>
-  </si>
-  <si>
-    <t>[{"naam":"Business Werkgroep presentatie Slim Ruimtelijk Plannen 27 september 2023","waarde":"Business Werkgroep presentatie Slim Ruimtelijk Plannen.pdf"},{"naam":"Eerste Thematische Werkgroep presentatie Slim Ruimtelijk Plannen 25 oktober 2023","waarde":"Eerste Thematische Werkgroep presentatie Slim Ruimtelijk Plannen.pdf"},{"naam":"Tweede Thematische Werkgroep presentatie Slim Ruimtelijk Plannen 30 november 2023","waarde":"Presentatie thematische werkgroep 2 - 30 november 2023.pdf"}]</t>
+    <t>[{"naam":"Verslag Business werkgroep - OSLO Slim Ruimtelijk Plannen 27 september 2023","waarde":"Verslag Business werkgroep SRP 2023-09-27.pdf"},{"naam":"Verslag thematische werkgroep 1 - OSLO Slim Ruimtelijk Plannen 25 oktober 2023","waarde":"Verslag 1e thematische werkgroep SRP 2023-09-25.pdf"},{"naam":"Verslag thematische werkgroep 2 - OSLO Slim Ruimtelijk Plannen 30 november 2023","waarde":"Verslag thematische werkgroep 2 - OSLO Slim Ruimtelijk Plannen 30 november 2023.docx"},{"naam":"Verslag thematische werkgroep 3 - OSLO Slim Ruimtelijk Plannen 21 december 2023","waarde":"Verslag thematische werkgroep 3 - OSLO Slim Ruimtelijk Plannen 21 december 2023.pdf"}]</t>
+  </si>
+  <si>
+    <t>[{"naam":"Business Werkgroep presentatie Slim Ruimtelijk Plannen 27 september 2023","waarde":"Business Werkgroep presentatie Slim Ruimtelijk Plannen.pdf"},{"naam":"Eerste Thematische Werkgroep presentatie Slim Ruimtelijk Plannen 25 oktober 2023","waarde":"Eerste Thematische Werkgroep presentatie Slim Ruimtelijk Plannen.pdf"},{"naam":"Tweede Thematische Werkgroep presentatie Slim Ruimtelijk Plannen 30 november 2023","waarde":"Presentatie thematische werkgroep 2 - 30 november 2023.pdf"},{"naam":"Derde Thematische Werkgroep presentatie Slim Ruimtelijk Plannen 21 december 2023","waarde":"Derde Thematische Werkgroep presentatie Slim Ruimtelijk Plannen 21 december 2023.pptx.pdf"}]</t>
   </si>
   <si>
     <t>Semantische standaard voor informatie over Slim Ruimtelijk Plannen</t>

</xml_diff>

<commit_message>
generated all the reports on 2024-01-20
</commit_message>
<xml_diff>
--- a/report/merged_configurations.xlsx
+++ b/report/merged_configurations.xlsx
@@ -2786,10 +2786,10 @@
     <t>[{"naam":"OSLO Omgeving - codelijsten - Technische documentatie","waarde":"OSLO Omgeving - codelijsten - Technische documentatie.pdf"}]</t>
   </si>
   <si>
-    <t>[{"naam":"Verslag Business werkgroep - 9 november 2021","waarde":"Verslag Business werkgroep - 9 november 2021.docx"},{"naam":"Verslag thematische werkgroep 1 - 9 december 2021","waarde":"Verslag Thematische werkgroep 1 - 9 november 2021.docx"},{"naam":"Verslag thematische werkgroep 2 - 1 februari 2022","waarde":"Verslag thematische werkgroep 2 - 1 februari 2022.docx"},{"naam":"OSLO Omgeving_ codelijsten - Verslag thematische werkgroep 1 - 22 juni 2022","waarde":"OSLO Omgeving_ codelijsten - Verslag thematische werkgroep 1 - 22 juni 2022.docx"},{"naam":"OSLO Omgeving_ codelijsten - Verslag thematische werkgroep 2 - 14 juli 2022","waarde":"OSLO Omgeving_ codelijsten - Verslag thematische werkgroep 2 - 14 juli 2022.docx"}]</t>
-  </si>
-  <si>
-    <t>[{"naam":"Presentatie Business werkgroep  - 9 november 2021","waarde":"Presentatie Business werkgroep - 9 november 2021.pdf"},{"naam":"Presentatie Thematische werkgroep 1 - 9 december 2021","waarde":"Presentatie Thematische werkgroep 1 - 9 december 2021.pdf"},{"naam":"Presentatie thematische werkgroep 2 - 1 februari 2022","waarde":"Presentatie thematische werkgroep 2 - 1 februari 2022.pdf"},{"naam":"OSLO Omgeving_codelijsten - Presentatie thematische werkgroep 1 - 22 juni 2022","waarde":"OSLO Omgeving_codelijsten-Presentatie Thematische werkgroep 1 - 22 juni 2022.pdf"},{"naam":"OSLO Omgeving_codelijsten - Presentatie thematische werkgroep 2 - 14 juli 2022","waarde":"OSLO Omgeving_codelijsten-Presentatie Thematische werkgroep 2 - 14 juli 2022.pdf"}]</t>
+    <t>[{"naam":"Verslag Business werkgroep - 9 november 2021","waarde":"Verslag Business werkgroep - 9 november 2021.docx"},{"naam":"Verslag thematische werkgroep 1 - 9 december 2021","waarde":"Verslag Thematische werkgroep 1 - 9 november 2021.docx"},{"naam":"Verslag thematische werkgroep 2 - 1 februari 2022","waarde":"Verslag thematische werkgroep 2 - 1 februari 2022.docx"},{"naam":"OSLO Omgeving codelijsten - Verslag thematische werkgroep 1 - 22 juni 2022","waarde":"OSLO Omgeving codelijsten - Verslag thematische werkgroep 1 - 22 juni 2022.docx"},{"naam":"OSLO Omgeving codelijsten - Verslag thematische werkgroep 2 - 14 juli 2022","waarde":"OSLO Omgeving codelijsten - Verslag thematische werkgroep 2 - 14 juli 2022.docx"}]</t>
+  </si>
+  <si>
+    <t>[{"naam":"Presentatie Business werkgroep  - 9 november 2021","waarde":"Presentatie Business werkgroep - 9 november 2021.pdf"},{"naam":"Presentatie Thematische werkgroep 1 - 9 december 2021","waarde":"Presentatie Thematische werkgroep 1 - 9 december 2021.pdf"},{"naam":"Presentatie thematische werkgroep 2 - 1 februari 2022","waarde":"Presentatie thematische werkgroep 2 - 1 februari 2022.pdf"},{"naam":"OSLO Omgeving codelijsten - Presentatie thematische werkgroep 1 - 22 juni 2022","waarde":"OSLO Omgeving codelijsten-Presentatie Thematische werkgroep 1 - 22 juni 2022.pdf"},{"naam":"OSLO Omgeving codelijsten - Presentatie thematische werkgroep 2 - 14 juli 2022","waarde":"OSLO Omgeving codelijsten-Presentatie Thematische werkgroep 2 - 14 juli 2022.pdf"}]</t>
   </si>
   <si>
     <t>Semantische standaard voor waterkwaliteit</t>

</xml_diff>

<commit_message>
generated all the reports on 2024-01-27
</commit_message>
<xml_diff>
--- a/report/merged_configurations.xlsx
+++ b/report/merged_configurations.xlsx
@@ -101,7 +101,7 @@
     <t>kabels-en-leidingen-description.md</t>
   </si>
   <si>
-    <t>[{"naam":"Kabels en Leidingen Applicatieprofiel","waarde":"https://data.vlaanderen.be/doc/applicatieprofiel/kabels-en-leidingen"},{"naam":"Cables and Pipes Application profile","waarde":"https://data.vlaanderen.be/doc/applicatieprofiel/kabels-en-leidingen/index_en.html"}]</t>
+    <t>[{"naam":"Kabels en Leidingen Applicatieprofiel","waarde":"https://data.vlaanderen.be/doc/applicatieprofiel/kabels-en-leidingen"},{"naam":"Cables and Pipes Application profile","waarde":"https://data.vlaanderen.be/doc/applicatieprofiel/kabels-en-leidingen/index_en.html"},{"naam":"Câbles et Conduites Profil d'application","waarde":"https://data.vlaanderen.be/doc/applicatieprofiel/kabels-en-leidingen/index_fr.html"}]</t>
   </si>
   <si>
     <t>[]</t>
@@ -134,7 +134,7 @@
     <t>Vocabularium</t>
   </si>
   <si>
-    <t>[{"naam":"Nutsvoorzieningen Vocabularium","waarde":"https://data.vlaanderen.be/ns/nutsvoorzieningen"},{"naam":"Utility Services Vocabularium","waarde":"https://data.vlaanderen.be/ns/nutsvoorzieningen/index_en.html"}]</t>
+    <t>[{"naam":"Nutsvoorzieningen Vocabularium","waarde":"https://data.vlaanderen.be/ns/nutsvoorzieningen"},{"naam":"Utility Services Vocabularium","waarde":"https://data.vlaanderen.be/ns/nutsvoorzieningen/index_en.html"},{"naam":"Câbles et Conduites Vocabulaire","waarde":"https://data.vlaanderen.be/doc/applicatieprofiel/kabels-en-leidingen/index_fr.html"}]</t>
   </si>
   <si>
     <t>[{"naam":"Presentatie business werkgroep - 24 april 2023","waarde":"Business Werkgroep presentatie IMKL - 24 april 2023.pdf"},{"naam":"Presentatie thematische werkgroep 1 - 25 mei 2023","waarde":"Presentatie eerste thematische werkgroep - IMKL -  25 mei 2023.pdf"},{"naam":"Presentatie thematische werkgroep 2 - 29 juni 2023","waarde":"Presentatie tweede thematische werkgroep - IMKL -  29 juni 2023.pdf"},{"naam":"Presentatie thematische werkgroep 3 - 7 september 2023","waarde":"Presentatie derde thematische werkgroep - IMKL - 7 september  2023.pdf"},{"naam":"Presentatie thematische werkgroep 4 - 5 oktober 2023","waarde":"Presentatie vierde thematische werkgroep - IMKL - 5 oktober 2023.pdf"}]</t>

</xml_diff>

<commit_message>
generated all the reports on 2024-02-13
</commit_message>
<xml_diff>
--- a/report/merged_configurations.xlsx
+++ b/report/merged_configurations.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4853" uniqueCount="1047">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4922" uniqueCount="1065">
   <si>
     <t>naam</t>
   </si>
@@ -3107,22 +3107,25 @@
     <t>[{"naam":"Vocabularium Kwaliteit Wegen en Wegmarkeringen","waarde":"https://data.vlaanderen.be/doc/ns/kwaliteit-wegen-en-wegmarkeringen"}]</t>
   </si>
   <si>
-    <t>Applicatieprofiel en Vocabularium Slimme Raadpleegomgeving</t>
+    <t>Applicatieprofiel Slimme Raadpleegomgeving</t>
   </si>
   <si>
     <t>ap-slimme-raadpleegomgeving-config.md</t>
   </si>
   <si>
-    <t>[{"naam":"Applicatieprofiel Slimme Raadpleegomgeving","waarde":"https://data.vlaanderen.be/doc/applicatieprofiel/slimme-raadpleegomgeving"},{"naam":"Vocabularium Slimme Raadpleegomgeving","waarde":"https://data.vlaanderen.be/ns/slimme-raadpleegomgeving"}]</t>
+    <t>[{"naam":"Applicatieprofiel Slimme Raadpleegomgeving","waarde":"https://data.vlaanderen.be/doc/applicatieprofiel/slimmeraadpleegomgeving"}]</t>
+  </si>
+  <si>
+    <t>[{"naam":"Vocabularium Slimme Raadpleegomgeving","waarde":"https://data.vlaanderen.be/ns/slimmeraadpleegomgeving"}]</t>
   </si>
   <si>
     <t>[{"naam":"Werkgroep Charter Slimme Raadpleegomgeving","waarde":"Werkgroep charter OSLO Slimme Raadpleegomgeving.docx"}]</t>
   </si>
   <si>
-    <t>[{"naam":"Verslag Business Werkgroep - 17 oktober 2023","waarde":"Verslag Business Workshop Slimme Raadpleegomgeving.pdf"},{"naam":"Verslag Thematische Werkgroep I - 7 November 2023","waarde":"20231107_ThematicWorkshop1_Verslag_OSLOSlimmeRaadpleegomgeving.pdf"},{"naam":"Verslag Thematische Werkgroep II - 28 November 2023","waarde":"20231128_ThematicWorkshop2_Verslag_OSLOSlimmeRaadpleegomgeving.pdf"}]</t>
-  </si>
-  <si>
-    <t>[{"naam":"Presentatie Business Werkgroep - 17 oktober 2023","waarde":"Business Werkgroep presentatie - slimme raadpleegomgeving.pdf"},{"naam":"Presentatie Thematische Werkgroep I - 7 november 2023","waarde":"20231107 Thematische Werkgroep 1 - Slimme Raadpleegomgeving V.01.pptx"},{"naam":"Presentatie Thematische Werkgroep II - 2 november 2023","waarde":"20231128_ThematicWorkshop2_Powerpoint_OSLOSlimmeRaadpleegomgeving.pptx"}]</t>
+    <t>[{"naam":"Verslag Business Werkgroep - 17 oktober 2023","waarde":"20231017_BusinessWorkshop_Verslag_OSLOSlimmeRaadpleegomgeving.pdf"},{"naam":"Verslag Thematische Werkgroep I - 7 November 2023","waarde":"20231107_ThematicWorkshop1_Verslag_OSLOSlimmeRaadpleegomgeving.pdf"},{"naam":"Verslag Thematische Werkgroep II - 28 November 2023","waarde":"20231128_ThematicWorkshop2_Verslag_OSLOSlimmeRaadpleegomgeving.pdf"},{"naam":"Verslag Thematische Werkgroep III - 9 Januari 2024","waarde":"20240109_ThematicWorkshop1_Verslag_OSLOSlimmeRaadpleegomgeving.pdf"},{"naam":"Verslag Thematische Werkgroep IV - 30 Januari 2024","waarde":"20240130_ThematicWorkshop1_Verslag_OSLOSlimmeRaadpleegomgeving.pdf"}]</t>
+  </si>
+  <si>
+    <t>[{"naam":"Presentatie Business Werkgroep - 17 oktober 2023","waarde":"Business Werkgroep presentatie - slimme raadpleegomgeving.pdf"},{"naam":"Presentatie Thematische Werkgroep I - 7 november 2023","waarde":"20231107 Thematische Werkgroep 1 - Slimme Raadpleegomgeving V.01.pptx"},{"naam":"Presentatie Thematische Werkgroep II - 28 november 2023","waarde":"20231128_ThematicWorkshop2_Powerpoint_OSLOSlimmeRaadpleegomgeving.pptx"},{"naam":"Presentatie Thematische Werkgroep III - 9 Januari 2024","waarde":"20240109_ThematicWorkshop3_Powerpoint_OSLOSlimmeRaadpleegomgeving.pptx"},{"naam":"Presentatie Thematische Werkgroep IV - 30 Januari 2024","waarde":"20240130_ThematicWorkshop4_Powerpoint_OSLOSlimmeRaadpleegomgeving.pptx"}]</t>
   </si>
   <si>
     <t>Semantische standaard voor de digitale transformatie van de Vlaamse lokale besturen</t>
@@ -3134,6 +3137,15 @@
     <t>7 november 2023</t>
   </si>
   <si>
+    <t>12 februari 2024</t>
+  </si>
+  <si>
+    <t>Vocabularium Slimme Raadpleegomgeving</t>
+  </si>
+  <si>
+    <t>voc-slimme-raadpleegomgeving-config.md</t>
+  </si>
+  <si>
     <t>Applicatieprofiel Lokale Economie</t>
   </si>
   <si>
@@ -3143,13 +3155,55 @@
     <t>[{"naam":"OSLO Lokale Economie Charter","waarde":"Charter_OSLO_Lokale_Economie.docx"}]</t>
   </si>
   <si>
-    <t>[{"naam":"Verslag business werkgroep - 19-09-2023","waarde":"Verslag Business Werkgroep - Lokale Economie - 19092023.pdf"},{"naam":"Verslag thematische werkgroep 1 - 17-10-2023","waarde":"Verslag Thematische Werkgroep 1 - Lokale Economie - 17102023.pdf"},{"naam":"Verslag thematische werkgroep 2 - 16-11-2023","waarde":"Verslag Thematische Werkgroep 2 - Lokale Economie - 16112023.pdf"},{"naam":"Verslag thematische werkgroep 3 - 19-12-2023","waarde":"Verslag Thematische Werkgroep 3 - Lokale Economie - 1912023.pdf"}]</t>
-  </si>
-  <si>
-    <t>[{"naam":"Presentatie business werkgroep - 19-09-2023","waarde":"Presentatie Business Werkgroep - Lokale Economie - 19092023.pdf"},{"naam":"Presentatie thematische werkgroep 1 - 17-10-2023","waarde":"Presentatie Thematische Werkgroep 1 - Lokale Economie - 17102023.pdf"},{"naam":"Presentatie thematische werkgroep 2 - 16-11-2023","waarde":"Presentatie Thematische Werkgroep 2 - Lokale Economie - 16112023.pdf"},{"naam":"Presentatie thematische werkgroep 3 - 19-12-2023","waarde":"Presentatie Thematische Werkgroep 3 - Lokale Economie - 19122023.pdf"}]</t>
+    <t>[{"naam":"Verslag business werkgroep - 19-09-2023","waarde":"Verslag Business Werkgroep - Lokale Economie - 19092023.pdf"},{"naam":"Verslag thematische werkgroep 1 - 17-10-2023","waarde":"Verslag Thematische Werkgroep 1 - Lokale Economie - 17102023.pdf"},{"naam":"Verslag thematische werkgroep 2 - 16-11-2023","waarde":"Verslag Thematische Werkgroep 2 - Lokale Economie - 16112023.pdf"},{"naam":"Verslag thematische werkgroep 3 - 19-12-2023","waarde":"Verslag Thematische Werkgroep 3 - Lokale Economie - 1912023.pdf"},{"naam":"Verslag thematische werkgroep 4 - 23-01-2024","waarde":"Verslag Thematische Werkgroep 4 - Lokale Economie - 23012024.pdf"}]</t>
+  </si>
+  <si>
+    <t>[{"naam":"Presentatie business werkgroep - 19-09-2023","waarde":"Presentatie Business Werkgroep - Lokale Economie - 19092023.pdf"},{"naam":"Presentatie thematische werkgroep 1 - 17-10-2023","waarde":"Presentatie Thematische Werkgroep 1 - Lokale Economie - 17102023.pdf"},{"naam":"Presentatie thematische werkgroep 2 - 16-11-2023","waarde":"Presentatie Thematische Werkgroep 2 - Lokale Economie - 16112023.pdf"},{"naam":"Presentatie thematische werkgroep 3 - 19-12-2023","waarde":"Presentatie Thematische Werkgroep 3 - Lokale Economie - 19122023.pdf"},{"naam":"Presentatie thematische werkgroep 4 - 23-01-2024","waarde":"Presentatie Thematische Werkgroep 4 - Lokale Economie - 23012024.pdf"}]</t>
   </si>
   <si>
     <t>Semantische standaard voor informatie over Lokale Economie</t>
+  </si>
+  <si>
+    <t>Applicatieprofiel Overlijdensaangifte</t>
+  </si>
+  <si>
+    <t>Athumi</t>
+  </si>
+  <si>
+    <t>https://data.vlaanderen.be/id/organisatie/OVO051320</t>
+  </si>
+  <si>
+    <t>ap-overlijdensaangifte-config.md</t>
+  </si>
+  <si>
+    <t>[{"naam":"Applicatieprofiel Overlijdensaangifte","waarde":"https://data.vlaanderen.be/doc/applicatieprofiel/overlijdensaangifte"}]</t>
+  </si>
+  <si>
+    <t>[{"naam":"Vocabularium Overlijdensaangifte","waarde":"https://data.vlaanderen.be/ns/overlijdensaangifte"}]</t>
+  </si>
+  <si>
+    <t>[{"naam":"Charter Overlijdensaangifte","waarde":"Charter OSLO_Overlijdensaangifte.pdf"}]</t>
+  </si>
+  <si>
+    <t>[{"naam":"Verslag Thematische Werkgroep I - 16 januari 2024","waarde":"20240116__ThematicWorkshop1_Verslag_OSLOOverlijdensaangifte"}]</t>
+  </si>
+  <si>
+    <t>[{"naam":"Presentatie Thematische Werkgroep I - 16 januari 2024","waarde":"20240116_ThematicWorkshop1_Powerpoint_OSLOOverlijdensaangifte.pptx"}]</t>
+  </si>
+  <si>
+    <t>Semantische standaard voor de digitale transformatie van de Vlaamse Overheid en lokale besturen</t>
+  </si>
+  <si>
+    <t>Lokale besturen, alle entiteiten van de Vlaamse overheid, zorgsector, uitvaartsector</t>
+  </si>
+  <si>
+    <t>25 januari 2024</t>
+  </si>
+  <si>
+    <t>Vocabularium Overlijdensaangifte</t>
+  </si>
+  <si>
+    <t>voc-overlijdensaangifte-config.md</t>
   </si>
   <si>
     <t>Geen rapport gevonden</t>
@@ -3560,7 +3614,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W207"/>
+  <dimension ref="A1:W210"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="23" width="44" customWidth="1"/>
@@ -17831,13 +17885,13 @@
         <v>504</v>
       </c>
       <c r="E206" s="4">
-        <v>45236</v>
+        <v>45330</v>
       </c>
       <c r="F206" s="3" t="s">
         <v>62</v>
       </c>
       <c r="G206" s="3" t="s">
-        <v>164</v>
+        <v>27</v>
       </c>
       <c r="H206" s="3" t="s">
         <v>1032</v>
@@ -17846,28 +17900,28 @@
         <v>1033</v>
       </c>
       <c r="J206" s="3" t="s">
-        <v>30</v>
+        <v>1034</v>
       </c>
       <c r="K206" s="3" t="s">
-        <v>1034</v>
+        <v>1035</v>
       </c>
       <c r="L206" s="3" t="s">
-        <v>1035</v>
+        <v>1036</v>
       </c>
       <c r="M206" s="3" t="s">
-        <v>1036</v>
+        <v>1037</v>
       </c>
       <c r="N206" s="3" t="s">
-        <v>1037</v>
+        <v>1038</v>
       </c>
       <c r="O206" s="3" t="s">
-        <v>1038</v>
+        <v>1039</v>
       </c>
       <c r="P206" s="3" t="s">
-        <v>1039</v>
+        <v>1040</v>
       </c>
       <c r="Q206" s="3" t="s">
-        <v>36</v>
+        <v>1041</v>
       </c>
       <c r="R206" s="3" t="s">
         <v>36</v>
@@ -17890,64 +17944,271 @@
     </row>
     <row r="207" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A207" s="3" t="s">
-        <v>1040</v>
+        <v>1042</v>
       </c>
       <c r="B207" s="3"/>
       <c r="C207" s="3" t="s">
-        <v>24</v>
+        <v>398</v>
       </c>
       <c r="D207" s="3" t="s">
-        <v>25</v>
+        <v>504</v>
       </c>
       <c r="E207" s="4">
-        <v>45308</v>
+        <v>45330</v>
       </c>
       <c r="F207" s="3" t="s">
         <v>62</v>
       </c>
       <c r="G207" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="H207" s="3" t="s">
+        <v>1043</v>
+      </c>
+      <c r="I207" s="3" t="s">
+        <v>1034</v>
+      </c>
+      <c r="J207" s="3" t="s">
+        <v>1033</v>
+      </c>
+      <c r="K207" s="3" t="s">
+        <v>1035</v>
+      </c>
+      <c r="L207" s="3" t="s">
+        <v>1036</v>
+      </c>
+      <c r="M207" s="3" t="s">
+        <v>1037</v>
+      </c>
+      <c r="N207" s="3" t="s">
+        <v>1038</v>
+      </c>
+      <c r="O207" s="3" t="s">
+        <v>1039</v>
+      </c>
+      <c r="P207" s="3" t="s">
+        <v>1040</v>
+      </c>
+      <c r="Q207" s="3" t="s">
+        <v>1041</v>
+      </c>
+      <c r="R207" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="S207" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="T207" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="U207" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="V207" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="W207" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="208" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A208" s="3" t="s">
+        <v>1044</v>
+      </c>
+      <c r="B208" s="3"/>
+      <c r="C208" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D208" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E208" s="4">
+        <v>45308</v>
+      </c>
+      <c r="F208" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="G208" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="H207" s="3" t="s">
+      <c r="H208" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="I207" s="3" t="s">
-        <v>1041</v>
-      </c>
-      <c r="J207" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="K207" s="3" t="s">
-        <v>1042</v>
-      </c>
-      <c r="L207" s="3" t="s">
-        <v>1043</v>
-      </c>
-      <c r="M207" s="3" t="s">
-        <v>1044</v>
-      </c>
-      <c r="N207" s="3" t="s">
+      <c r="I208" s="3" t="s">
         <v>1045</v>
       </c>
-      <c r="O207" s="3" t="s">
+      <c r="J208" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="K208" s="3" t="s">
+        <v>1046</v>
+      </c>
+      <c r="L208" s="3" t="s">
+        <v>1047</v>
+      </c>
+      <c r="M208" s="3" t="s">
+        <v>1048</v>
+      </c>
+      <c r="N208" s="3" t="s">
+        <v>1049</v>
+      </c>
+      <c r="O208" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="P207" s="3"/>
-      <c r="Q207" s="3"/>
-      <c r="R207" s="3"/>
-      <c r="S207" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="T207" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="U207" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="V207" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="W207" s="3" t="s">
+      <c r="P208" s="3"/>
+      <c r="Q208" s="3"/>
+      <c r="R208" s="3"/>
+      <c r="S208" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="T208" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="U208" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="V208" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="W208" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="209" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A209" s="3" t="s">
+        <v>1050</v>
+      </c>
+      <c r="B209" s="3"/>
+      <c r="C209" s="3" t="s">
+        <v>1051</v>
+      </c>
+      <c r="D209" s="3" t="s">
+        <v>1052</v>
+      </c>
+      <c r="E209" s="4">
+        <v>45323</v>
+      </c>
+      <c r="F209" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="G209" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="H209" s="3" t="s">
+        <v>1053</v>
+      </c>
+      <c r="I209" s="3" t="s">
+        <v>1054</v>
+      </c>
+      <c r="J209" s="3" t="s">
+        <v>1055</v>
+      </c>
+      <c r="K209" s="3" t="s">
+        <v>1056</v>
+      </c>
+      <c r="L209" s="3" t="s">
+        <v>1057</v>
+      </c>
+      <c r="M209" s="3" t="s">
+        <v>1058</v>
+      </c>
+      <c r="N209" s="3" t="s">
+        <v>1059</v>
+      </c>
+      <c r="O209" s="3" t="s">
+        <v>1060</v>
+      </c>
+      <c r="P209" s="3" t="s">
+        <v>1061</v>
+      </c>
+      <c r="Q209" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="R209" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="S209" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="T209" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="U209" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="V209" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="W209" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="210" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A210" s="3" t="s">
+        <v>1062</v>
+      </c>
+      <c r="B210" s="3"/>
+      <c r="C210" s="3" t="s">
+        <v>1051</v>
+      </c>
+      <c r="D210" s="3" t="s">
+        <v>1052</v>
+      </c>
+      <c r="E210" s="4">
+        <v>45323</v>
+      </c>
+      <c r="F210" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="G210" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="H210" s="3" t="s">
+        <v>1063</v>
+      </c>
+      <c r="I210" s="3" t="s">
+        <v>1054</v>
+      </c>
+      <c r="J210" s="3" t="s">
+        <v>1055</v>
+      </c>
+      <c r="K210" s="3" t="s">
+        <v>1056</v>
+      </c>
+      <c r="L210" s="3" t="s">
+        <v>1057</v>
+      </c>
+      <c r="M210" s="3" t="s">
+        <v>1058</v>
+      </c>
+      <c r="N210" s="3" t="s">
+        <v>1059</v>
+      </c>
+      <c r="O210" s="3" t="s">
+        <v>1060</v>
+      </c>
+      <c r="P210" s="3" t="s">
+        <v>1061</v>
+      </c>
+      <c r="Q210" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="R210" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="S210" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="T210" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="U210" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="V210" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="W210" s="3" t="s">
         <v>37</v>
       </c>
     </row>
@@ -17959,7 +18220,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R207"/>
+  <dimension ref="A1:R210"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="18" width="44" customWidth="1"/>
@@ -18026,7 +18287,7 @@
         <v>23</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>1046</v>
+        <v>1064</v>
       </c>
       <c r="C2" s="5" t="b">
         <v>1</v>
@@ -18082,7 +18343,7 @@
         <v>38</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>1046</v>
+        <v>1064</v>
       </c>
       <c r="C3" s="5" t="b">
         <v>1</v>
@@ -18138,7 +18399,7 @@
         <v>42</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>1046</v>
+        <v>1064</v>
       </c>
       <c r="C4" s="5" t="b">
         <v>1</v>
@@ -18194,7 +18455,7 @@
         <v>51</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>1046</v>
+        <v>1064</v>
       </c>
       <c r="C5" s="5" t="b">
         <v>1</v>
@@ -18250,7 +18511,7 @@
         <v>53</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>1046</v>
+        <v>1064</v>
       </c>
       <c r="C6" s="5" t="b">
         <v>1</v>
@@ -18306,7 +18567,7 @@
         <v>61</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>1046</v>
+        <v>1064</v>
       </c>
       <c r="C7" s="5" t="b">
         <v>1</v>
@@ -18362,7 +18623,7 @@
         <v>69</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>1046</v>
+        <v>1064</v>
       </c>
       <c r="C8" s="5" t="b">
         <v>1</v>
@@ -18418,7 +18679,7 @@
         <v>78</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>1046</v>
+        <v>1064</v>
       </c>
       <c r="C9" s="5" t="b">
         <v>1</v>
@@ -18474,7 +18735,7 @@
         <v>80</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>1046</v>
+        <v>1064</v>
       </c>
       <c r="C10" s="5" t="b">
         <v>1</v>
@@ -18530,7 +18791,7 @@
         <v>89</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>1046</v>
+        <v>1064</v>
       </c>
       <c r="C11" s="5" t="b">
         <v>1</v>
@@ -18698,7 +18959,7 @@
         <v>114</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>1046</v>
+        <v>1064</v>
       </c>
       <c r="C14" s="5" t="b">
         <v>1</v>
@@ -18754,7 +19015,7 @@
         <v>125</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>1046</v>
+        <v>1064</v>
       </c>
       <c r="C15" s="5" t="b">
         <v>1</v>
@@ -18810,7 +19071,7 @@
         <v>127</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>1046</v>
+        <v>1064</v>
       </c>
       <c r="C16" s="5" t="b">
         <v>1</v>
@@ -18866,7 +19127,7 @@
         <v>129</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>1046</v>
+        <v>1064</v>
       </c>
       <c r="C17" s="5" t="b">
         <v>1</v>
@@ -18922,7 +19183,7 @@
         <v>131</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>1046</v>
+        <v>1064</v>
       </c>
       <c r="C18" s="5" t="b">
         <v>1</v>
@@ -18978,7 +19239,7 @@
         <v>134</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>1046</v>
+        <v>1064</v>
       </c>
       <c r="C19" s="5" t="b">
         <v>1</v>
@@ -19034,7 +19295,7 @@
         <v>136</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>1046</v>
+        <v>1064</v>
       </c>
       <c r="C20" s="5" t="b">
         <v>1</v>
@@ -19090,7 +19351,7 @@
         <v>138</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>1046</v>
+        <v>1064</v>
       </c>
       <c r="C21" s="5" t="b">
         <v>1</v>
@@ -19146,7 +19407,7 @@
         <v>140</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>1046</v>
+        <v>1064</v>
       </c>
       <c r="C22" s="5" t="b">
         <v>1</v>
@@ -19202,7 +19463,7 @@
         <v>142</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>1046</v>
+        <v>1064</v>
       </c>
       <c r="C23" s="5" t="b">
         <v>1</v>
@@ -19258,7 +19519,7 @@
         <v>144</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>1046</v>
+        <v>1064</v>
       </c>
       <c r="C24" s="5" t="b">
         <v>1</v>
@@ -19314,7 +19575,7 @@
         <v>142</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>1046</v>
+        <v>1064</v>
       </c>
       <c r="C25" s="5" t="b">
         <v>1</v>
@@ -19370,7 +19631,7 @@
         <v>146</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>1046</v>
+        <v>1064</v>
       </c>
       <c r="C26" s="5" t="b">
         <v>1</v>
@@ -19426,7 +19687,7 @@
         <v>148</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>1046</v>
+        <v>1064</v>
       </c>
       <c r="C27" s="5" t="b">
         <v>1</v>
@@ -19482,7 +19743,7 @@
         <v>150</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>1046</v>
+        <v>1064</v>
       </c>
       <c r="C28" s="5" t="b">
         <v>1</v>
@@ -19538,7 +19799,7 @@
         <v>152</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>1046</v>
+        <v>1064</v>
       </c>
       <c r="C29" s="5" t="b">
         <v>1</v>
@@ -19594,7 +19855,7 @@
         <v>154</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>1046</v>
+        <v>1064</v>
       </c>
       <c r="C30" s="5" t="b">
         <v>1</v>
@@ -19650,7 +19911,7 @@
         <v>156</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>1046</v>
+        <v>1064</v>
       </c>
       <c r="C31" s="5" t="b">
         <v>1</v>
@@ -19706,7 +19967,7 @@
         <v>158</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>1046</v>
+        <v>1064</v>
       </c>
       <c r="C32" s="5" t="b">
         <v>1</v>
@@ -19762,7 +20023,7 @@
         <v>160</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>1046</v>
+        <v>1064</v>
       </c>
       <c r="C33" s="5" t="b">
         <v>1</v>
@@ -19818,7 +20079,7 @@
         <v>162</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>1046</v>
+        <v>1064</v>
       </c>
       <c r="C34" s="5" t="b">
         <v>1</v>
@@ -19986,7 +20247,7 @@
         <v>192</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>1046</v>
+        <v>1064</v>
       </c>
       <c r="C37" s="5" t="b">
         <v>1</v>
@@ -20042,7 +20303,7 @@
         <v>199</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>1046</v>
+        <v>1064</v>
       </c>
       <c r="C38" s="5" t="b">
         <v>1</v>
@@ -21610,7 +21871,7 @@
         <v>381</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>1046</v>
+        <v>1064</v>
       </c>
       <c r="C66" s="5" t="b">
         <v>1</v>
@@ -21666,7 +21927,7 @@
         <v>393</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>1046</v>
+        <v>1064</v>
       </c>
       <c r="C67" s="5" t="b">
         <v>1</v>
@@ -22114,7 +22375,7 @@
         <v>452</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>1046</v>
+        <v>1064</v>
       </c>
       <c r="C75" s="5" t="b">
         <v>1</v>
@@ -22786,7 +23047,7 @@
         <v>533</v>
       </c>
       <c r="B87" s="3" t="s">
-        <v>1046</v>
+        <v>1064</v>
       </c>
       <c r="C87" s="5" t="b">
         <v>1</v>
@@ -22842,7 +23103,7 @@
         <v>542</v>
       </c>
       <c r="B88" s="3" t="s">
-        <v>1046</v>
+        <v>1064</v>
       </c>
       <c r="C88" s="5" t="b">
         <v>1</v>
@@ -22898,7 +23159,7 @@
         <v>544</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>1046</v>
+        <v>1064</v>
       </c>
       <c r="C89" s="5" t="b">
         <v>1</v>
@@ -25026,7 +25287,7 @@
         <v>698</v>
       </c>
       <c r="B127" s="3" t="s">
-        <v>1046</v>
+        <v>1064</v>
       </c>
       <c r="C127" s="5" t="b">
         <v>1</v>
@@ -25586,7 +25847,7 @@
         <v>730</v>
       </c>
       <c r="B137" s="3" t="s">
-        <v>1046</v>
+        <v>1064</v>
       </c>
       <c r="C137" s="5" t="b">
         <v>1</v>
@@ -25642,7 +25903,7 @@
         <v>736</v>
       </c>
       <c r="B138" s="3" t="s">
-        <v>1046</v>
+        <v>1064</v>
       </c>
       <c r="C138" s="5" t="b">
         <v>1</v>
@@ -25810,7 +26071,7 @@
         <v>756</v>
       </c>
       <c r="B141" s="3" t="s">
-        <v>1046</v>
+        <v>1064</v>
       </c>
       <c r="C141" s="5" t="b">
         <v>1</v>
@@ -25866,7 +26127,7 @@
         <v>758</v>
       </c>
       <c r="B142" s="3" t="s">
-        <v>1046</v>
+        <v>1064</v>
       </c>
       <c r="C142" s="5" t="b">
         <v>1</v>
@@ -25922,7 +26183,7 @@
         <v>767</v>
       </c>
       <c r="B143" s="3" t="s">
-        <v>1046</v>
+        <v>1064</v>
       </c>
       <c r="C143" s="5" t="b">
         <v>1</v>
@@ -25978,7 +26239,7 @@
         <v>771</v>
       </c>
       <c r="B144" s="3" t="s">
-        <v>1046</v>
+        <v>1064</v>
       </c>
       <c r="C144" s="5" t="b">
         <v>1</v>
@@ -26034,7 +26295,7 @@
         <v>774</v>
       </c>
       <c r="B145" s="3" t="s">
-        <v>1046</v>
+        <v>1064</v>
       </c>
       <c r="C145" s="5" t="b">
         <v>1</v>
@@ -26090,7 +26351,7 @@
         <v>777</v>
       </c>
       <c r="B146" s="3" t="s">
-        <v>1046</v>
+        <v>1064</v>
       </c>
       <c r="C146" s="5" t="b">
         <v>1</v>
@@ -26146,7 +26407,7 @@
         <v>780</v>
       </c>
       <c r="B147" s="3" t="s">
-        <v>1046</v>
+        <v>1064</v>
       </c>
       <c r="C147" s="5" t="b">
         <v>1</v>
@@ -26202,7 +26463,7 @@
         <v>783</v>
       </c>
       <c r="B148" s="3" t="s">
-        <v>1046</v>
+        <v>1064</v>
       </c>
       <c r="C148" s="5" t="b">
         <v>1</v>
@@ -26258,7 +26519,7 @@
         <v>786</v>
       </c>
       <c r="B149" s="3" t="s">
-        <v>1046</v>
+        <v>1064</v>
       </c>
       <c r="C149" s="5" t="b">
         <v>1</v>
@@ -26314,7 +26575,7 @@
         <v>789</v>
       </c>
       <c r="B150" s="3" t="s">
-        <v>1046</v>
+        <v>1064</v>
       </c>
       <c r="C150" s="5" t="b">
         <v>1</v>
@@ -26370,7 +26631,7 @@
         <v>792</v>
       </c>
       <c r="B151" s="3" t="s">
-        <v>1046</v>
+        <v>1064</v>
       </c>
       <c r="C151" s="5" t="b">
         <v>1</v>
@@ -26426,7 +26687,7 @@
         <v>795</v>
       </c>
       <c r="B152" s="3" t="s">
-        <v>1046</v>
+        <v>1064</v>
       </c>
       <c r="C152" s="5" t="b">
         <v>1</v>
@@ -26482,7 +26743,7 @@
         <v>798</v>
       </c>
       <c r="B153" s="3" t="s">
-        <v>1046</v>
+        <v>1064</v>
       </c>
       <c r="C153" s="5" t="b">
         <v>1</v>
@@ -26538,7 +26799,7 @@
         <v>801</v>
       </c>
       <c r="B154" s="3" t="s">
-        <v>1046</v>
+        <v>1064</v>
       </c>
       <c r="C154" s="5" t="b">
         <v>1</v>
@@ -26594,7 +26855,7 @@
         <v>804</v>
       </c>
       <c r="B155" s="3" t="s">
-        <v>1046</v>
+        <v>1064</v>
       </c>
       <c r="C155" s="5" t="b">
         <v>1</v>
@@ -26650,7 +26911,7 @@
         <v>807</v>
       </c>
       <c r="B156" s="3" t="s">
-        <v>1046</v>
+        <v>1064</v>
       </c>
       <c r="C156" s="5" t="b">
         <v>1</v>
@@ -26706,7 +26967,7 @@
         <v>810</v>
       </c>
       <c r="B157" s="3" t="s">
-        <v>1046</v>
+        <v>1064</v>
       </c>
       <c r="C157" s="5" t="b">
         <v>1</v>
@@ -26762,7 +27023,7 @@
         <v>813</v>
       </c>
       <c r="B158" s="3" t="s">
-        <v>1046</v>
+        <v>1064</v>
       </c>
       <c r="C158" s="5" t="b">
         <v>1</v>
@@ -26818,7 +27079,7 @@
         <v>816</v>
       </c>
       <c r="B159" s="3" t="s">
-        <v>1046</v>
+        <v>1064</v>
       </c>
       <c r="C159" s="5" t="b">
         <v>1</v>
@@ -26874,7 +27135,7 @@
         <v>819</v>
       </c>
       <c r="B160" s="3" t="s">
-        <v>1046</v>
+        <v>1064</v>
       </c>
       <c r="C160" s="5" t="b">
         <v>1</v>
@@ -26930,7 +27191,7 @@
         <v>822</v>
       </c>
       <c r="B161" s="3" t="s">
-        <v>1046</v>
+        <v>1064</v>
       </c>
       <c r="C161" s="5" t="b">
         <v>1</v>
@@ -26986,7 +27247,7 @@
         <v>825</v>
       </c>
       <c r="B162" s="3" t="s">
-        <v>1046</v>
+        <v>1064</v>
       </c>
       <c r="C162" s="5" t="b">
         <v>1</v>
@@ -27042,7 +27303,7 @@
         <v>828</v>
       </c>
       <c r="B163" s="3" t="s">
-        <v>1046</v>
+        <v>1064</v>
       </c>
       <c r="C163" s="5" t="b">
         <v>1</v>
@@ -27098,7 +27359,7 @@
         <v>831</v>
       </c>
       <c r="B164" s="3" t="s">
-        <v>1046</v>
+        <v>1064</v>
       </c>
       <c r="C164" s="5" t="b">
         <v>1</v>
@@ -27154,7 +27415,7 @@
         <v>834</v>
       </c>
       <c r="B165" s="3" t="s">
-        <v>1046</v>
+        <v>1064</v>
       </c>
       <c r="C165" s="5" t="b">
         <v>1</v>
@@ -27210,7 +27471,7 @@
         <v>837</v>
       </c>
       <c r="B166" s="3" t="s">
-        <v>1046</v>
+        <v>1064</v>
       </c>
       <c r="C166" s="5" t="b">
         <v>1</v>
@@ -27266,7 +27527,7 @@
         <v>840</v>
       </c>
       <c r="B167" s="3" t="s">
-        <v>1046</v>
+        <v>1064</v>
       </c>
       <c r="C167" s="5" t="b">
         <v>1</v>
@@ -27322,7 +27583,7 @@
         <v>843</v>
       </c>
       <c r="B168" s="3" t="s">
-        <v>1046</v>
+        <v>1064</v>
       </c>
       <c r="C168" s="5" t="b">
         <v>1</v>
@@ -27378,7 +27639,7 @@
         <v>846</v>
       </c>
       <c r="B169" s="3" t="s">
-        <v>1046</v>
+        <v>1064</v>
       </c>
       <c r="C169" s="5" t="b">
         <v>1</v>
@@ -27434,7 +27695,7 @@
         <v>849</v>
       </c>
       <c r="B170" s="3" t="s">
-        <v>1046</v>
+        <v>1064</v>
       </c>
       <c r="C170" s="5" t="b">
         <v>1</v>
@@ -27490,7 +27751,7 @@
         <v>852</v>
       </c>
       <c r="B171" s="3" t="s">
-        <v>1046</v>
+        <v>1064</v>
       </c>
       <c r="C171" s="5" t="b">
         <v>1</v>
@@ -27546,7 +27807,7 @@
         <v>855</v>
       </c>
       <c r="B172" s="3" t="s">
-        <v>1046</v>
+        <v>1064</v>
       </c>
       <c r="C172" s="5" t="b">
         <v>1</v>
@@ -27602,7 +27863,7 @@
         <v>858</v>
       </c>
       <c r="B173" s="3" t="s">
-        <v>1046</v>
+        <v>1064</v>
       </c>
       <c r="C173" s="5" t="b">
         <v>1</v>
@@ -27658,7 +27919,7 @@
         <v>861</v>
       </c>
       <c r="B174" s="3" t="s">
-        <v>1046</v>
+        <v>1064</v>
       </c>
       <c r="C174" s="5" t="b">
         <v>1</v>
@@ -27714,7 +27975,7 @@
         <v>864</v>
       </c>
       <c r="B175" s="3" t="s">
-        <v>1046</v>
+        <v>1064</v>
       </c>
       <c r="C175" s="5" t="b">
         <v>1</v>
@@ -27770,7 +28031,7 @@
         <v>867</v>
       </c>
       <c r="B176" s="3" t="s">
-        <v>1046</v>
+        <v>1064</v>
       </c>
       <c r="C176" s="5" t="b">
         <v>1</v>
@@ -27826,7 +28087,7 @@
         <v>870</v>
       </c>
       <c r="B177" s="3" t="s">
-        <v>1046</v>
+        <v>1064</v>
       </c>
       <c r="C177" s="5" t="b">
         <v>1</v>
@@ -27882,7 +28143,7 @@
         <v>872</v>
       </c>
       <c r="B178" s="3" t="s">
-        <v>1046</v>
+        <v>1064</v>
       </c>
       <c r="C178" s="5" t="b">
         <v>1</v>
@@ -27938,7 +28199,7 @@
         <v>875</v>
       </c>
       <c r="B179" s="3" t="s">
-        <v>1046</v>
+        <v>1064</v>
       </c>
       <c r="C179" s="5" t="b">
         <v>1</v>
@@ -27994,7 +28255,7 @@
         <v>877</v>
       </c>
       <c r="B180" s="3" t="s">
-        <v>1046</v>
+        <v>1064</v>
       </c>
       <c r="C180" s="5" t="b">
         <v>1</v>
@@ -28050,7 +28311,7 @@
         <v>879</v>
       </c>
       <c r="B181" s="3" t="s">
-        <v>1046</v>
+        <v>1064</v>
       </c>
       <c r="C181" s="5" t="b">
         <v>1</v>
@@ -28106,7 +28367,7 @@
         <v>881</v>
       </c>
       <c r="B182" s="3" t="s">
-        <v>1046</v>
+        <v>1064</v>
       </c>
       <c r="C182" s="5" t="b">
         <v>1</v>
@@ -28162,7 +28423,7 @@
         <v>884</v>
       </c>
       <c r="B183" s="3" t="s">
-        <v>1046</v>
+        <v>1064</v>
       </c>
       <c r="C183" s="5" t="b">
         <v>1</v>
@@ -28218,7 +28479,7 @@
         <v>890</v>
       </c>
       <c r="B184" s="3" t="s">
-        <v>1046</v>
+        <v>1064</v>
       </c>
       <c r="C184" s="5" t="b">
         <v>1</v>
@@ -28330,7 +28591,7 @@
         <v>908</v>
       </c>
       <c r="B186" s="3" t="s">
-        <v>1046</v>
+        <v>1064</v>
       </c>
       <c r="C186" s="5" t="b">
         <v>1</v>
@@ -28386,7 +28647,7 @@
         <v>917</v>
       </c>
       <c r="B187" s="3" t="s">
-        <v>1046</v>
+        <v>1064</v>
       </c>
       <c r="C187" s="5" t="b">
         <v>1</v>
@@ -28498,7 +28759,7 @@
         <v>937</v>
       </c>
       <c r="B189" s="3" t="s">
-        <v>1046</v>
+        <v>1064</v>
       </c>
       <c r="C189" s="5" t="b">
         <v>1</v>
@@ -28554,7 +28815,7 @@
         <v>945</v>
       </c>
       <c r="B190" s="3" t="s">
-        <v>1046</v>
+        <v>1064</v>
       </c>
       <c r="C190" s="5" t="b">
         <v>1</v>
@@ -28610,7 +28871,7 @@
         <v>947</v>
       </c>
       <c r="B191" s="3" t="s">
-        <v>1046</v>
+        <v>1064</v>
       </c>
       <c r="C191" s="5" t="b">
         <v>1</v>
@@ -28666,7 +28927,7 @@
         <v>954</v>
       </c>
       <c r="B192" s="3" t="s">
-        <v>1046</v>
+        <v>1064</v>
       </c>
       <c r="C192" s="5" t="b">
         <v>1</v>
@@ -28722,7 +28983,7 @@
         <v>956</v>
       </c>
       <c r="B193" s="3" t="s">
-        <v>1046</v>
+        <v>1064</v>
       </c>
       <c r="C193" s="5" t="b">
         <v>1</v>
@@ -28778,7 +29039,7 @@
         <v>966</v>
       </c>
       <c r="B194" s="3" t="s">
-        <v>1046</v>
+        <v>1064</v>
       </c>
       <c r="C194" s="5" t="b">
         <v>1</v>
@@ -28834,7 +29095,7 @@
         <v>972</v>
       </c>
       <c r="B195" s="3" t="s">
-        <v>1046</v>
+        <v>1064</v>
       </c>
       <c r="C195" s="5" t="b">
         <v>1</v>
@@ -28890,7 +29151,7 @@
         <v>975</v>
       </c>
       <c r="B196" s="3" t="s">
-        <v>1046</v>
+        <v>1064</v>
       </c>
       <c r="C196" s="5" t="b">
         <v>1</v>
@@ -28946,7 +29207,7 @@
         <v>983</v>
       </c>
       <c r="B197" s="3" t="s">
-        <v>1046</v>
+        <v>1064</v>
       </c>
       <c r="C197" s="5" t="b">
         <v>1</v>
@@ -29002,7 +29263,7 @@
         <v>987</v>
       </c>
       <c r="B198" s="3" t="s">
-        <v>1046</v>
+        <v>1064</v>
       </c>
       <c r="C198" s="5" t="b">
         <v>1</v>
@@ -29058,7 +29319,7 @@
         <v>997</v>
       </c>
       <c r="B199" s="3" t="s">
-        <v>1046</v>
+        <v>1064</v>
       </c>
       <c r="C199" s="5" t="b">
         <v>1</v>
@@ -29114,7 +29375,7 @@
         <v>1003</v>
       </c>
       <c r="B200" s="3" t="s">
-        <v>1046</v>
+        <v>1064</v>
       </c>
       <c r="C200" s="5" t="b">
         <v>1</v>
@@ -29170,7 +29431,7 @@
         <v>1006</v>
       </c>
       <c r="B201" s="3" t="s">
-        <v>1046</v>
+        <v>1064</v>
       </c>
       <c r="C201" s="5" t="b">
         <v>1</v>
@@ -29226,7 +29487,7 @@
         <v>1009</v>
       </c>
       <c r="B202" s="3" t="s">
-        <v>1046</v>
+        <v>1064</v>
       </c>
       <c r="C202" s="5" t="b">
         <v>1</v>
@@ -29282,7 +29543,7 @@
         <v>1016</v>
       </c>
       <c r="B203" s="3" t="s">
-        <v>1046</v>
+        <v>1064</v>
       </c>
       <c r="C203" s="5" t="b">
         <v>1</v>
@@ -29338,7 +29599,7 @@
         <v>1023</v>
       </c>
       <c r="B204" s="3" t="s">
-        <v>1046</v>
+        <v>1064</v>
       </c>
       <c r="C204" s="5" t="b">
         <v>1</v>
@@ -29394,7 +29655,7 @@
         <v>1029</v>
       </c>
       <c r="B205" s="3" t="s">
-        <v>1046</v>
+        <v>1064</v>
       </c>
       <c r="C205" s="5" t="b">
         <v>1</v>
@@ -29450,7 +29711,7 @@
         <v>1031</v>
       </c>
       <c r="B206" s="3" t="s">
-        <v>1046</v>
+        <v>1064</v>
       </c>
       <c r="C206" s="5" t="b">
         <v>1</v>
@@ -29473,8 +29734,8 @@
       <c r="I206" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="J206" s="6" t="b">
-        <v>0</v>
+      <c r="J206" s="5" t="b">
+        <v>1</v>
       </c>
       <c r="K206" s="5" t="b">
         <v>1</v>
@@ -29494,8 +29755,8 @@
       <c r="P206" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="Q206" s="6" t="b">
-        <v>0</v>
+      <c r="Q206" s="5" t="b">
+        <v>1</v>
       </c>
       <c r="R206" s="6" t="b">
         <v>0</v>
@@ -29503,10 +29764,10 @@
     </row>
     <row r="207" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A207" s="3" t="s">
-        <v>1040</v>
+        <v>1042</v>
       </c>
       <c r="B207" s="3" t="s">
-        <v>1046</v>
+        <v>1064</v>
       </c>
       <c r="C207" s="5" t="b">
         <v>1</v>
@@ -29529,8 +29790,8 @@
       <c r="I207" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="J207" s="6" t="b">
-        <v>0</v>
+      <c r="J207" s="5" t="b">
+        <v>1</v>
       </c>
       <c r="K207" s="5" t="b">
         <v>1</v>
@@ -29547,13 +29808,181 @@
       <c r="O207" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="P207" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="Q207" s="6" t="b">
-        <v>0</v>
+      <c r="P207" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q207" s="5" t="b">
+        <v>1</v>
       </c>
       <c r="R207" s="6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="208" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A208" s="3" t="s">
+        <v>1044</v>
+      </c>
+      <c r="B208" s="3" t="s">
+        <v>1064</v>
+      </c>
+      <c r="C208" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="D208" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="E208" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="F208" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="G208" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="H208" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="I208" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="J208" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="K208" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="L208" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="M208" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="N208" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="O208" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="P208" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q208" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="R208" s="6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="209" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A209" s="3" t="s">
+        <v>1050</v>
+      </c>
+      <c r="B209" s="3" t="s">
+        <v>1064</v>
+      </c>
+      <c r="C209" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="D209" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="E209" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="F209" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="G209" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="H209" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="I209" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="J209" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="K209" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="L209" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="M209" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="N209" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="O209" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="P209" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q209" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="R209" s="6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="210" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A210" s="3" t="s">
+        <v>1062</v>
+      </c>
+      <c r="B210" s="3" t="s">
+        <v>1064</v>
+      </c>
+      <c r="C210" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="D210" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="E210" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="F210" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="G210" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="H210" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="I210" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="J210" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="K210" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="L210" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="M210" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="N210" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="O210" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="P210" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q210" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="R210" s="6" t="b">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
generated all the reports on 2024-02-14
</commit_message>
<xml_diff>
--- a/report/merged_configurations.xlsx
+++ b/report/merged_configurations.xlsx
@@ -188,10 +188,10 @@
     <t>[{"naam":"Projectcharter","waarde":"Werkgroep-charter-OSLO_SlimRuimtelijkPlannen.docx"}]</t>
   </si>
   <si>
-    <t>[{"naam":"Verslag Business werkgroep - OSLO Slim Ruimtelijk Plannen 27 september 2023","waarde":"Verslag Business werkgroep SRP 2023-09-27.pdf"},{"naam":"Verslag thematische werkgroep 1 - OSLO Slim Ruimtelijk Plannen 25 oktober 2023","waarde":"Verslag 1e thematische werkgroep SRP 2023-09-25.pdf"},{"naam":"Verslag thematische werkgroep 2 - OSLO Slim Ruimtelijk Plannen 30 november 2023","waarde":"Verslag thematische werkgroep 2 - OSLO Slim Ruimtelijk Plannen 30 november 2023.docx"},{"naam":"Verslag thematische werkgroep 3 - OSLO Slim Ruimtelijk Plannen 21 december 2023","waarde":"Verslag thematische werkgroep 3 - OSLO Slim Ruimtelijk Plannen 21 december 2023.pdf"}]</t>
-  </si>
-  <si>
-    <t>[{"naam":"Business Werkgroep presentatie Slim Ruimtelijk Plannen 27 september 2023","waarde":"Business Werkgroep presentatie Slim Ruimtelijk Plannen.pdf"},{"naam":"Eerste Thematische Werkgroep presentatie Slim Ruimtelijk Plannen 25 oktober 2023","waarde":"Eerste Thematische Werkgroep presentatie Slim Ruimtelijk Plannen.pdf"},{"naam":"Tweede Thematische Werkgroep presentatie Slim Ruimtelijk Plannen 30 november 2023","waarde":"Presentatie thematische werkgroep 2 - 30 november 2023.pdf"},{"naam":"Derde Thematische Werkgroep presentatie Slim Ruimtelijk Plannen 21 december 2023","waarde":"Derde Thematische Werkgroep presentatie Slim Ruimtelijk Plannen 21 december 2023.pptx.pdf"}]</t>
+    <t>[{"naam":"Verslag Business werkgroep - OSLO Slim Ruimtelijk Plannen 27 september 2023","waarde":"Verslag Business werkgroep SRP 2023-09-27.pdf"},{"naam":"Verslag thematische werkgroep 1 - OSLO Slim Ruimtelijk Plannen 25 oktober 2023","waarde":"Verslag 1e thematische werkgroep SRP 2023-09-25.pdf"},{"naam":"Verslag thematische werkgroep 2 - OSLO Slim Ruimtelijk Plannen 30 november 2023","waarde":"Verslag thematische werkgroep 2 - OSLO Slim Ruimtelijk Plannen 30 november 2023.docx"},{"naam":"Verslag thematische werkgroep 3 - OSLO Slim Ruimtelijk Plannen 21 december 2023","waarde":"Verslag thematische werkgroep 3 - OSLO Slim Ruimtelijk Plannen 21 december 2023.pdf"},{"naam":"Verslag thematische werkgroep 4 - OSLO Slim Ruimtelijk Plannen 1 februari 2024","waarde":"Verslag 4e thematische werkgroep SRP 2024-02-01.pdf"}]</t>
+  </si>
+  <si>
+    <t>[{"naam":"Business Werkgroep presentatie Slim Ruimtelijk Plannen 27 september 2023","waarde":"Business Werkgroep presentatie Slim Ruimtelijk Plannen.pdf"},{"naam":"Eerste Thematische Werkgroep presentatie Slim Ruimtelijk Plannen 25 oktober 2023","waarde":"Eerste Thematische Werkgroep presentatie Slim Ruimtelijk Plannen.pdf"},{"naam":"Tweede Thematische Werkgroep presentatie Slim Ruimtelijk Plannen 30 november 2023","waarde":"Presentatie thematische werkgroep 2 - 30 november 2023.pdf"},{"naam":"Derde Thematische Werkgroep presentatie Slim Ruimtelijk Plannen 21 december 2023","waarde":"Derde Thematische Werkgroep presentatie Slim Ruimtelijk Plannen 21 december 2023.pptx.pdf"},{"naam":"Vierde Thematische Werkgroep presentatie Slim Ruimtelijk Plannen 1 februari 2024","waarde":"Presentatie thematische werkgroep 4 - SRP.pdf"}]</t>
   </si>
   <si>
     <t>Semantische standaard voor informatie over Slim Ruimtelijk Plannen</t>

</xml_diff>

<commit_message>
generated all the reports on 2024-02-23
</commit_message>
<xml_diff>
--- a/report/merged_configurations.xlsx
+++ b/report/merged_configurations.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4941" uniqueCount="1066">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4961" uniqueCount="1068">
   <si>
     <t>naam</t>
   </si>
@@ -3165,6 +3165,12 @@
   </si>
   <si>
     <t>Semantische standaard voor informatie over Lokale Economie</t>
+  </si>
+  <si>
+    <t>Vocabularium Lokale Economie</t>
+  </si>
+  <si>
+    <t>[{"naam":"Lokale Economie Vocabularium","waarde":"https://data.vlaanderen.be/doc/vocabularium/lokale-economie"}]</t>
   </si>
   <si>
     <t>Applicatieprofiel Overlijdensaangifte</t>
@@ -3617,7 +3623,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W211"/>
+  <dimension ref="A1:W212"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="23" width="44" customWidth="1"/>
@@ -18144,53 +18150,47 @@
       </c>
       <c r="B210" s="3"/>
       <c r="C210" s="3" t="s">
-        <v>1052</v>
+        <v>24</v>
       </c>
       <c r="D210" s="3" t="s">
-        <v>1053</v>
+        <v>25</v>
       </c>
       <c r="E210" s="4">
-        <v>45323</v>
+        <v>45308</v>
       </c>
       <c r="F210" s="3" t="s">
         <v>63</v>
       </c>
       <c r="G210" s="3" t="s">
-        <v>27</v>
+        <v>112</v>
       </c>
       <c r="H210" s="3" t="s">
-        <v>1054</v>
+        <v>64</v>
       </c>
       <c r="I210" s="3" t="s">
-        <v>1055</v>
+        <v>1052</v>
       </c>
       <c r="J210" s="3" t="s">
-        <v>1056</v>
+        <v>30</v>
       </c>
       <c r="K210" s="3" t="s">
-        <v>1057</v>
+        <v>1047</v>
       </c>
       <c r="L210" s="3" t="s">
-        <v>1058</v>
+        <v>1048</v>
       </c>
       <c r="M210" s="3" t="s">
-        <v>1059</v>
+        <v>1049</v>
       </c>
       <c r="N210" s="3" t="s">
-        <v>1060</v>
+        <v>1050</v>
       </c>
       <c r="O210" s="3" t="s">
-        <v>1061</v>
-      </c>
-      <c r="P210" s="3" t="s">
-        <v>1062</v>
-      </c>
-      <c r="Q210" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="R210" s="3" t="s">
-        <v>36</v>
-      </c>
+        <v>77</v>
+      </c>
+      <c r="P210" s="3"/>
+      <c r="Q210" s="3"/>
+      <c r="R210" s="3"/>
       <c r="S210" s="3" t="s">
         <v>37</v>
       </c>
@@ -18209,14 +18209,14 @@
     </row>
     <row r="211" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A211" s="3" t="s">
-        <v>1063</v>
+        <v>1053</v>
       </c>
       <c r="B211" s="3"/>
       <c r="C211" s="3" t="s">
-        <v>1052</v>
+        <v>1054</v>
       </c>
       <c r="D211" s="3" t="s">
-        <v>1053</v>
+        <v>1055</v>
       </c>
       <c r="E211" s="4">
         <v>45323</v>
@@ -18225,34 +18225,34 @@
         <v>63</v>
       </c>
       <c r="G211" s="3" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="H211" s="3" t="s">
+        <v>1056</v>
+      </c>
+      <c r="I211" s="3" t="s">
+        <v>1057</v>
+      </c>
+      <c r="J211" s="3" t="s">
+        <v>1058</v>
+      </c>
+      <c r="K211" s="3" t="s">
+        <v>1059</v>
+      </c>
+      <c r="L211" s="3" t="s">
+        <v>1060</v>
+      </c>
+      <c r="M211" s="3" t="s">
+        <v>1061</v>
+      </c>
+      <c r="N211" s="3" t="s">
+        <v>1062</v>
+      </c>
+      <c r="O211" s="3" t="s">
+        <v>1063</v>
+      </c>
+      <c r="P211" s="3" t="s">
         <v>1064</v>
-      </c>
-      <c r="I211" s="3" t="s">
-        <v>1055</v>
-      </c>
-      <c r="J211" s="3" t="s">
-        <v>1056</v>
-      </c>
-      <c r="K211" s="3" t="s">
-        <v>1057</v>
-      </c>
-      <c r="L211" s="3" t="s">
-        <v>1058</v>
-      </c>
-      <c r="M211" s="3" t="s">
-        <v>1059</v>
-      </c>
-      <c r="N211" s="3" t="s">
-        <v>1060</v>
-      </c>
-      <c r="O211" s="3" t="s">
-        <v>1061</v>
-      </c>
-      <c r="P211" s="3" t="s">
-        <v>1062</v>
       </c>
       <c r="Q211" s="3" t="s">
         <v>36</v>
@@ -18273,6 +18273,75 @@
         <v>37</v>
       </c>
       <c r="W211" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="212" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A212" s="3" t="s">
+        <v>1065</v>
+      </c>
+      <c r="B212" s="3"/>
+      <c r="C212" s="3" t="s">
+        <v>1054</v>
+      </c>
+      <c r="D212" s="3" t="s">
+        <v>1055</v>
+      </c>
+      <c r="E212" s="4">
+        <v>45323</v>
+      </c>
+      <c r="F212" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="G212" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="H212" s="3" t="s">
+        <v>1066</v>
+      </c>
+      <c r="I212" s="3" t="s">
+        <v>1057</v>
+      </c>
+      <c r="J212" s="3" t="s">
+        <v>1058</v>
+      </c>
+      <c r="K212" s="3" t="s">
+        <v>1059</v>
+      </c>
+      <c r="L212" s="3" t="s">
+        <v>1060</v>
+      </c>
+      <c r="M212" s="3" t="s">
+        <v>1061</v>
+      </c>
+      <c r="N212" s="3" t="s">
+        <v>1062</v>
+      </c>
+      <c r="O212" s="3" t="s">
+        <v>1063</v>
+      </c>
+      <c r="P212" s="3" t="s">
+        <v>1064</v>
+      </c>
+      <c r="Q212" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="R212" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="S212" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="T212" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="U212" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="V212" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="W212" s="3" t="s">
         <v>37</v>
       </c>
     </row>
@@ -18284,7 +18353,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R211"/>
+  <dimension ref="A1:R212"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="18" width="44" customWidth="1"/>
@@ -18351,7 +18420,7 @@
         <v>23</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>1065</v>
+        <v>1067</v>
       </c>
       <c r="C2" s="5" t="b">
         <v>1</v>
@@ -18407,7 +18476,7 @@
         <v>38</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>1065</v>
+        <v>1067</v>
       </c>
       <c r="C3" s="5" t="b">
         <v>1</v>
@@ -18463,7 +18532,7 @@
         <v>42</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>1065</v>
+        <v>1067</v>
       </c>
       <c r="C4" s="5" t="b">
         <v>1</v>
@@ -18519,7 +18588,7 @@
         <v>51</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>1065</v>
+        <v>1067</v>
       </c>
       <c r="C5" s="5" t="b">
         <v>1</v>
@@ -18575,7 +18644,7 @@
         <v>53</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>1065</v>
+        <v>1067</v>
       </c>
       <c r="C6" s="5" t="b">
         <v>1</v>
@@ -18631,7 +18700,7 @@
         <v>60</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>1065</v>
+        <v>1067</v>
       </c>
       <c r="C7" s="5" t="b">
         <v>1</v>
@@ -18687,7 +18756,7 @@
         <v>62</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>1065</v>
+        <v>1067</v>
       </c>
       <c r="C8" s="5" t="b">
         <v>1</v>
@@ -18743,7 +18812,7 @@
         <v>70</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>1065</v>
+        <v>1067</v>
       </c>
       <c r="C9" s="5" t="b">
         <v>1</v>
@@ -18799,7 +18868,7 @@
         <v>79</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>1065</v>
+        <v>1067</v>
       </c>
       <c r="C10" s="5" t="b">
         <v>1</v>
@@ -18855,7 +18924,7 @@
         <v>81</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>1065</v>
+        <v>1067</v>
       </c>
       <c r="C11" s="5" t="b">
         <v>1</v>
@@ -18911,7 +18980,7 @@
         <v>90</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>1065</v>
+        <v>1067</v>
       </c>
       <c r="C12" s="5" t="b">
         <v>1</v>
@@ -19079,7 +19148,7 @@
         <v>115</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>1065</v>
+        <v>1067</v>
       </c>
       <c r="C15" s="5" t="b">
         <v>1</v>
@@ -19135,7 +19204,7 @@
         <v>126</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>1065</v>
+        <v>1067</v>
       </c>
       <c r="C16" s="5" t="b">
         <v>1</v>
@@ -19191,7 +19260,7 @@
         <v>128</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>1065</v>
+        <v>1067</v>
       </c>
       <c r="C17" s="5" t="b">
         <v>1</v>
@@ -19247,7 +19316,7 @@
         <v>130</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>1065</v>
+        <v>1067</v>
       </c>
       <c r="C18" s="5" t="b">
         <v>1</v>
@@ -19303,7 +19372,7 @@
         <v>132</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>1065</v>
+        <v>1067</v>
       </c>
       <c r="C19" s="5" t="b">
         <v>1</v>
@@ -19359,7 +19428,7 @@
         <v>135</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>1065</v>
+        <v>1067</v>
       </c>
       <c r="C20" s="5" t="b">
         <v>1</v>
@@ -19415,7 +19484,7 @@
         <v>137</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>1065</v>
+        <v>1067</v>
       </c>
       <c r="C21" s="5" t="b">
         <v>1</v>
@@ -19471,7 +19540,7 @@
         <v>139</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>1065</v>
+        <v>1067</v>
       </c>
       <c r="C22" s="5" t="b">
         <v>1</v>
@@ -19527,7 +19596,7 @@
         <v>141</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>1065</v>
+        <v>1067</v>
       </c>
       <c r="C23" s="5" t="b">
         <v>1</v>
@@ -19583,7 +19652,7 @@
         <v>143</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>1065</v>
+        <v>1067</v>
       </c>
       <c r="C24" s="5" t="b">
         <v>1</v>
@@ -19639,7 +19708,7 @@
         <v>145</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>1065</v>
+        <v>1067</v>
       </c>
       <c r="C25" s="5" t="b">
         <v>1</v>
@@ -19695,7 +19764,7 @@
         <v>143</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>1065</v>
+        <v>1067</v>
       </c>
       <c r="C26" s="5" t="b">
         <v>1</v>
@@ -19751,7 +19820,7 @@
         <v>147</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>1065</v>
+        <v>1067</v>
       </c>
       <c r="C27" s="5" t="b">
         <v>1</v>
@@ -19807,7 +19876,7 @@
         <v>149</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>1065</v>
+        <v>1067</v>
       </c>
       <c r="C28" s="5" t="b">
         <v>1</v>
@@ -19863,7 +19932,7 @@
         <v>151</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>1065</v>
+        <v>1067</v>
       </c>
       <c r="C29" s="5" t="b">
         <v>1</v>
@@ -19919,7 +19988,7 @@
         <v>153</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>1065</v>
+        <v>1067</v>
       </c>
       <c r="C30" s="5" t="b">
         <v>1</v>
@@ -19975,7 +20044,7 @@
         <v>155</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>1065</v>
+        <v>1067</v>
       </c>
       <c r="C31" s="5" t="b">
         <v>1</v>
@@ -20031,7 +20100,7 @@
         <v>157</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>1065</v>
+        <v>1067</v>
       </c>
       <c r="C32" s="5" t="b">
         <v>1</v>
@@ -20087,7 +20156,7 @@
         <v>159</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>1065</v>
+        <v>1067</v>
       </c>
       <c r="C33" s="5" t="b">
         <v>1</v>
@@ -20143,7 +20212,7 @@
         <v>161</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>1065</v>
+        <v>1067</v>
       </c>
       <c r="C34" s="5" t="b">
         <v>1</v>
@@ -20199,7 +20268,7 @@
         <v>163</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>1065</v>
+        <v>1067</v>
       </c>
       <c r="C35" s="5" t="b">
         <v>1</v>
@@ -20367,7 +20436,7 @@
         <v>193</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>1065</v>
+        <v>1067</v>
       </c>
       <c r="C38" s="5" t="b">
         <v>1</v>
@@ -20423,7 +20492,7 @@
         <v>200</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>1065</v>
+        <v>1067</v>
       </c>
       <c r="C39" s="5" t="b">
         <v>1</v>
@@ -21991,7 +22060,7 @@
         <v>382</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>1065</v>
+        <v>1067</v>
       </c>
       <c r="C67" s="5" t="b">
         <v>1</v>
@@ -22047,7 +22116,7 @@
         <v>394</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>1065</v>
+        <v>1067</v>
       </c>
       <c r="C68" s="5" t="b">
         <v>1</v>
@@ -22495,7 +22564,7 @@
         <v>453</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>1065</v>
+        <v>1067</v>
       </c>
       <c r="C76" s="5" t="b">
         <v>1</v>
@@ -23167,7 +23236,7 @@
         <v>534</v>
       </c>
       <c r="B88" s="3" t="s">
-        <v>1065</v>
+        <v>1067</v>
       </c>
       <c r="C88" s="5" t="b">
         <v>1</v>
@@ -23223,7 +23292,7 @@
         <v>543</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>1065</v>
+        <v>1067</v>
       </c>
       <c r="C89" s="5" t="b">
         <v>1</v>
@@ -23279,7 +23348,7 @@
         <v>545</v>
       </c>
       <c r="B90" s="3" t="s">
-        <v>1065</v>
+        <v>1067</v>
       </c>
       <c r="C90" s="5" t="b">
         <v>1</v>
@@ -25407,7 +25476,7 @@
         <v>699</v>
       </c>
       <c r="B128" s="3" t="s">
-        <v>1065</v>
+        <v>1067</v>
       </c>
       <c r="C128" s="5" t="b">
         <v>1</v>
@@ -25967,7 +26036,7 @@
         <v>731</v>
       </c>
       <c r="B138" s="3" t="s">
-        <v>1065</v>
+        <v>1067</v>
       </c>
       <c r="C138" s="5" t="b">
         <v>1</v>
@@ -26023,7 +26092,7 @@
         <v>737</v>
       </c>
       <c r="B139" s="3" t="s">
-        <v>1065</v>
+        <v>1067</v>
       </c>
       <c r="C139" s="5" t="b">
         <v>1</v>
@@ -26191,7 +26260,7 @@
         <v>757</v>
       </c>
       <c r="B142" s="3" t="s">
-        <v>1065</v>
+        <v>1067</v>
       </c>
       <c r="C142" s="5" t="b">
         <v>1</v>
@@ -26247,7 +26316,7 @@
         <v>759</v>
       </c>
       <c r="B143" s="3" t="s">
-        <v>1065</v>
+        <v>1067</v>
       </c>
       <c r="C143" s="5" t="b">
         <v>1</v>
@@ -26303,7 +26372,7 @@
         <v>768</v>
       </c>
       <c r="B144" s="3" t="s">
-        <v>1065</v>
+        <v>1067</v>
       </c>
       <c r="C144" s="5" t="b">
         <v>1</v>
@@ -26359,7 +26428,7 @@
         <v>772</v>
       </c>
       <c r="B145" s="3" t="s">
-        <v>1065</v>
+        <v>1067</v>
       </c>
       <c r="C145" s="5" t="b">
         <v>1</v>
@@ -26415,7 +26484,7 @@
         <v>775</v>
       </c>
       <c r="B146" s="3" t="s">
-        <v>1065</v>
+        <v>1067</v>
       </c>
       <c r="C146" s="5" t="b">
         <v>1</v>
@@ -26471,7 +26540,7 @@
         <v>778</v>
       </c>
       <c r="B147" s="3" t="s">
-        <v>1065</v>
+        <v>1067</v>
       </c>
       <c r="C147" s="5" t="b">
         <v>1</v>
@@ -26527,7 +26596,7 @@
         <v>781</v>
       </c>
       <c r="B148" s="3" t="s">
-        <v>1065</v>
+        <v>1067</v>
       </c>
       <c r="C148" s="5" t="b">
         <v>1</v>
@@ -26583,7 +26652,7 @@
         <v>784</v>
       </c>
       <c r="B149" s="3" t="s">
-        <v>1065</v>
+        <v>1067</v>
       </c>
       <c r="C149" s="5" t="b">
         <v>1</v>
@@ -26639,7 +26708,7 @@
         <v>787</v>
       </c>
       <c r="B150" s="3" t="s">
-        <v>1065</v>
+        <v>1067</v>
       </c>
       <c r="C150" s="5" t="b">
         <v>1</v>
@@ -26695,7 +26764,7 @@
         <v>790</v>
       </c>
       <c r="B151" s="3" t="s">
-        <v>1065</v>
+        <v>1067</v>
       </c>
       <c r="C151" s="5" t="b">
         <v>1</v>
@@ -26751,7 +26820,7 @@
         <v>793</v>
       </c>
       <c r="B152" s="3" t="s">
-        <v>1065</v>
+        <v>1067</v>
       </c>
       <c r="C152" s="5" t="b">
         <v>1</v>
@@ -26807,7 +26876,7 @@
         <v>796</v>
       </c>
       <c r="B153" s="3" t="s">
-        <v>1065</v>
+        <v>1067</v>
       </c>
       <c r="C153" s="5" t="b">
         <v>1</v>
@@ -26863,7 +26932,7 @@
         <v>799</v>
       </c>
       <c r="B154" s="3" t="s">
-        <v>1065</v>
+        <v>1067</v>
       </c>
       <c r="C154" s="5" t="b">
         <v>1</v>
@@ -26919,7 +26988,7 @@
         <v>802</v>
       </c>
       <c r="B155" s="3" t="s">
-        <v>1065</v>
+        <v>1067</v>
       </c>
       <c r="C155" s="5" t="b">
         <v>1</v>
@@ -26975,7 +27044,7 @@
         <v>805</v>
       </c>
       <c r="B156" s="3" t="s">
-        <v>1065</v>
+        <v>1067</v>
       </c>
       <c r="C156" s="5" t="b">
         <v>1</v>
@@ -27031,7 +27100,7 @@
         <v>808</v>
       </c>
       <c r="B157" s="3" t="s">
-        <v>1065</v>
+        <v>1067</v>
       </c>
       <c r="C157" s="5" t="b">
         <v>1</v>
@@ -27087,7 +27156,7 @@
         <v>811</v>
       </c>
       <c r="B158" s="3" t="s">
-        <v>1065</v>
+        <v>1067</v>
       </c>
       <c r="C158" s="5" t="b">
         <v>1</v>
@@ -27143,7 +27212,7 @@
         <v>814</v>
       </c>
       <c r="B159" s="3" t="s">
-        <v>1065</v>
+        <v>1067</v>
       </c>
       <c r="C159" s="5" t="b">
         <v>1</v>
@@ -27199,7 +27268,7 @@
         <v>817</v>
       </c>
       <c r="B160" s="3" t="s">
-        <v>1065</v>
+        <v>1067</v>
       </c>
       <c r="C160" s="5" t="b">
         <v>1</v>
@@ -27255,7 +27324,7 @@
         <v>820</v>
       </c>
       <c r="B161" s="3" t="s">
-        <v>1065</v>
+        <v>1067</v>
       </c>
       <c r="C161" s="5" t="b">
         <v>1</v>
@@ -27311,7 +27380,7 @@
         <v>823</v>
       </c>
       <c r="B162" s="3" t="s">
-        <v>1065</v>
+        <v>1067</v>
       </c>
       <c r="C162" s="5" t="b">
         <v>1</v>
@@ -27367,7 +27436,7 @@
         <v>826</v>
       </c>
       <c r="B163" s="3" t="s">
-        <v>1065</v>
+        <v>1067</v>
       </c>
       <c r="C163" s="5" t="b">
         <v>1</v>
@@ -27423,7 +27492,7 @@
         <v>829</v>
       </c>
       <c r="B164" s="3" t="s">
-        <v>1065</v>
+        <v>1067</v>
       </c>
       <c r="C164" s="5" t="b">
         <v>1</v>
@@ -27479,7 +27548,7 @@
         <v>832</v>
       </c>
       <c r="B165" s="3" t="s">
-        <v>1065</v>
+        <v>1067</v>
       </c>
       <c r="C165" s="5" t="b">
         <v>1</v>
@@ -27535,7 +27604,7 @@
         <v>835</v>
       </c>
       <c r="B166" s="3" t="s">
-        <v>1065</v>
+        <v>1067</v>
       </c>
       <c r="C166" s="5" t="b">
         <v>1</v>
@@ -27591,7 +27660,7 @@
         <v>838</v>
       </c>
       <c r="B167" s="3" t="s">
-        <v>1065</v>
+        <v>1067</v>
       </c>
       <c r="C167" s="5" t="b">
         <v>1</v>
@@ -27647,7 +27716,7 @@
         <v>841</v>
       </c>
       <c r="B168" s="3" t="s">
-        <v>1065</v>
+        <v>1067</v>
       </c>
       <c r="C168" s="5" t="b">
         <v>1</v>
@@ -27703,7 +27772,7 @@
         <v>844</v>
       </c>
       <c r="B169" s="3" t="s">
-        <v>1065</v>
+        <v>1067</v>
       </c>
       <c r="C169" s="5" t="b">
         <v>1</v>
@@ -27759,7 +27828,7 @@
         <v>847</v>
       </c>
       <c r="B170" s="3" t="s">
-        <v>1065</v>
+        <v>1067</v>
       </c>
       <c r="C170" s="5" t="b">
         <v>1</v>
@@ -27815,7 +27884,7 @@
         <v>850</v>
       </c>
       <c r="B171" s="3" t="s">
-        <v>1065</v>
+        <v>1067</v>
       </c>
       <c r="C171" s="5" t="b">
         <v>1</v>
@@ -27871,7 +27940,7 @@
         <v>853</v>
       </c>
       <c r="B172" s="3" t="s">
-        <v>1065</v>
+        <v>1067</v>
       </c>
       <c r="C172" s="5" t="b">
         <v>1</v>
@@ -27927,7 +27996,7 @@
         <v>856</v>
       </c>
       <c r="B173" s="3" t="s">
-        <v>1065</v>
+        <v>1067</v>
       </c>
       <c r="C173" s="5" t="b">
         <v>1</v>
@@ -27983,7 +28052,7 @@
         <v>859</v>
       </c>
       <c r="B174" s="3" t="s">
-        <v>1065</v>
+        <v>1067</v>
       </c>
       <c r="C174" s="5" t="b">
         <v>1</v>
@@ -28039,7 +28108,7 @@
         <v>862</v>
       </c>
       <c r="B175" s="3" t="s">
-        <v>1065</v>
+        <v>1067</v>
       </c>
       <c r="C175" s="5" t="b">
         <v>1</v>
@@ -28095,7 +28164,7 @@
         <v>865</v>
       </c>
       <c r="B176" s="3" t="s">
-        <v>1065</v>
+        <v>1067</v>
       </c>
       <c r="C176" s="5" t="b">
         <v>1</v>
@@ -28151,7 +28220,7 @@
         <v>868</v>
       </c>
       <c r="B177" s="3" t="s">
-        <v>1065</v>
+        <v>1067</v>
       </c>
       <c r="C177" s="5" t="b">
         <v>1</v>
@@ -28207,7 +28276,7 @@
         <v>871</v>
       </c>
       <c r="B178" s="3" t="s">
-        <v>1065</v>
+        <v>1067</v>
       </c>
       <c r="C178" s="5" t="b">
         <v>1</v>
@@ -28263,7 +28332,7 @@
         <v>873</v>
       </c>
       <c r="B179" s="3" t="s">
-        <v>1065</v>
+        <v>1067</v>
       </c>
       <c r="C179" s="5" t="b">
         <v>1</v>
@@ -28319,7 +28388,7 @@
         <v>876</v>
       </c>
       <c r="B180" s="3" t="s">
-        <v>1065</v>
+        <v>1067</v>
       </c>
       <c r="C180" s="5" t="b">
         <v>1</v>
@@ -28375,7 +28444,7 @@
         <v>878</v>
       </c>
       <c r="B181" s="3" t="s">
-        <v>1065</v>
+        <v>1067</v>
       </c>
       <c r="C181" s="5" t="b">
         <v>1</v>
@@ -28431,7 +28500,7 @@
         <v>880</v>
       </c>
       <c r="B182" s="3" t="s">
-        <v>1065</v>
+        <v>1067</v>
       </c>
       <c r="C182" s="5" t="b">
         <v>1</v>
@@ -28487,7 +28556,7 @@
         <v>882</v>
       </c>
       <c r="B183" s="3" t="s">
-        <v>1065</v>
+        <v>1067</v>
       </c>
       <c r="C183" s="5" t="b">
         <v>1</v>
@@ -28543,7 +28612,7 @@
         <v>885</v>
       </c>
       <c r="B184" s="3" t="s">
-        <v>1065</v>
+        <v>1067</v>
       </c>
       <c r="C184" s="5" t="b">
         <v>1</v>
@@ -28599,7 +28668,7 @@
         <v>891</v>
       </c>
       <c r="B185" s="3" t="s">
-        <v>1065</v>
+        <v>1067</v>
       </c>
       <c r="C185" s="5" t="b">
         <v>1</v>
@@ -28711,7 +28780,7 @@
         <v>909</v>
       </c>
       <c r="B187" s="3" t="s">
-        <v>1065</v>
+        <v>1067</v>
       </c>
       <c r="C187" s="5" t="b">
         <v>1</v>
@@ -28767,7 +28836,7 @@
         <v>918</v>
       </c>
       <c r="B188" s="3" t="s">
-        <v>1065</v>
+        <v>1067</v>
       </c>
       <c r="C188" s="5" t="b">
         <v>1</v>
@@ -28879,7 +28948,7 @@
         <v>938</v>
       </c>
       <c r="B190" s="3" t="s">
-        <v>1065</v>
+        <v>1067</v>
       </c>
       <c r="C190" s="5" t="b">
         <v>1</v>
@@ -28935,7 +29004,7 @@
         <v>946</v>
       </c>
       <c r="B191" s="3" t="s">
-        <v>1065</v>
+        <v>1067</v>
       </c>
       <c r="C191" s="5" t="b">
         <v>1</v>
@@ -28991,7 +29060,7 @@
         <v>948</v>
       </c>
       <c r="B192" s="3" t="s">
-        <v>1065</v>
+        <v>1067</v>
       </c>
       <c r="C192" s="5" t="b">
         <v>1</v>
@@ -29047,7 +29116,7 @@
         <v>955</v>
       </c>
       <c r="B193" s="3" t="s">
-        <v>1065</v>
+        <v>1067</v>
       </c>
       <c r="C193" s="5" t="b">
         <v>1</v>
@@ -29103,7 +29172,7 @@
         <v>957</v>
       </c>
       <c r="B194" s="3" t="s">
-        <v>1065</v>
+        <v>1067</v>
       </c>
       <c r="C194" s="5" t="b">
         <v>1</v>
@@ -29159,7 +29228,7 @@
         <v>967</v>
       </c>
       <c r="B195" s="3" t="s">
-        <v>1065</v>
+        <v>1067</v>
       </c>
       <c r="C195" s="5" t="b">
         <v>1</v>
@@ -29215,7 +29284,7 @@
         <v>973</v>
       </c>
       <c r="B196" s="3" t="s">
-        <v>1065</v>
+        <v>1067</v>
       </c>
       <c r="C196" s="5" t="b">
         <v>1</v>
@@ -29271,7 +29340,7 @@
         <v>976</v>
       </c>
       <c r="B197" s="3" t="s">
-        <v>1065</v>
+        <v>1067</v>
       </c>
       <c r="C197" s="5" t="b">
         <v>1</v>
@@ -29327,7 +29396,7 @@
         <v>984</v>
       </c>
       <c r="B198" s="3" t="s">
-        <v>1065</v>
+        <v>1067</v>
       </c>
       <c r="C198" s="5" t="b">
         <v>1</v>
@@ -29383,7 +29452,7 @@
         <v>988</v>
       </c>
       <c r="B199" s="3" t="s">
-        <v>1065</v>
+        <v>1067</v>
       </c>
       <c r="C199" s="5" t="b">
         <v>1</v>
@@ -29439,7 +29508,7 @@
         <v>998</v>
       </c>
       <c r="B200" s="3" t="s">
-        <v>1065</v>
+        <v>1067</v>
       </c>
       <c r="C200" s="5" t="b">
         <v>1</v>
@@ -29495,7 +29564,7 @@
         <v>1004</v>
       </c>
       <c r="B201" s="3" t="s">
-        <v>1065</v>
+        <v>1067</v>
       </c>
       <c r="C201" s="5" t="b">
         <v>1</v>
@@ -29551,7 +29620,7 @@
         <v>1007</v>
       </c>
       <c r="B202" s="3" t="s">
-        <v>1065</v>
+        <v>1067</v>
       </c>
       <c r="C202" s="5" t="b">
         <v>1</v>
@@ -29607,7 +29676,7 @@
         <v>1010</v>
       </c>
       <c r="B203" s="3" t="s">
-        <v>1065</v>
+        <v>1067</v>
       </c>
       <c r="C203" s="5" t="b">
         <v>1</v>
@@ -29663,7 +29732,7 @@
         <v>1017</v>
       </c>
       <c r="B204" s="3" t="s">
-        <v>1065</v>
+        <v>1067</v>
       </c>
       <c r="C204" s="5" t="b">
         <v>1</v>
@@ -29719,7 +29788,7 @@
         <v>1024</v>
       </c>
       <c r="B205" s="3" t="s">
-        <v>1065</v>
+        <v>1067</v>
       </c>
       <c r="C205" s="5" t="b">
         <v>1</v>
@@ -29775,7 +29844,7 @@
         <v>1030</v>
       </c>
       <c r="B206" s="3" t="s">
-        <v>1065</v>
+        <v>1067</v>
       </c>
       <c r="C206" s="5" t="b">
         <v>1</v>
@@ -29831,7 +29900,7 @@
         <v>1032</v>
       </c>
       <c r="B207" s="3" t="s">
-        <v>1065</v>
+        <v>1067</v>
       </c>
       <c r="C207" s="5" t="b">
         <v>1</v>
@@ -29887,7 +29956,7 @@
         <v>1043</v>
       </c>
       <c r="B208" s="3" t="s">
-        <v>1065</v>
+        <v>1067</v>
       </c>
       <c r="C208" s="5" t="b">
         <v>1</v>
@@ -29943,7 +30012,7 @@
         <v>1045</v>
       </c>
       <c r="B209" s="3" t="s">
-        <v>1065</v>
+        <v>1067</v>
       </c>
       <c r="C209" s="5" t="b">
         <v>1</v>
@@ -29999,7 +30068,7 @@
         <v>1051</v>
       </c>
       <c r="B210" s="3" t="s">
-        <v>1065</v>
+        <v>1067</v>
       </c>
       <c r="C210" s="5" t="b">
         <v>1</v>
@@ -30022,8 +30091,8 @@
       <c r="I210" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="J210" s="5" t="b">
-        <v>1</v>
+      <c r="J210" s="6" t="b">
+        <v>0</v>
       </c>
       <c r="K210" s="5" t="b">
         <v>1</v>
@@ -30040,8 +30109,8 @@
       <c r="O210" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="P210" s="5" t="b">
-        <v>1</v>
+      <c r="P210" s="6" t="b">
+        <v>0</v>
       </c>
       <c r="Q210" s="6" t="b">
         <v>0</v>
@@ -30052,57 +30121,113 @@
     </row>
     <row r="211" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A211" s="3" t="s">
-        <v>1063</v>
+        <v>1053</v>
       </c>
       <c r="B211" s="3" t="s">
+        <v>1067</v>
+      </c>
+      <c r="C211" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="D211" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="E211" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="F211" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="G211" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="H211" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="I211" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="J211" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="K211" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="L211" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="M211" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="N211" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="O211" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="P211" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q211" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="R211" s="6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="212" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A212" s="3" t="s">
         <v>1065</v>
       </c>
-      <c r="C211" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="D211" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="E211" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="F211" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="G211" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="H211" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="I211" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="J211" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="K211" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="L211" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="M211" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="N211" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="O211" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="P211" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q211" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="R211" s="6" t="b">
+      <c r="B212" s="3" t="s">
+        <v>1067</v>
+      </c>
+      <c r="C212" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="D212" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="E212" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="F212" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="G212" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="H212" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="I212" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="J212" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="K212" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="L212" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="M212" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="N212" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="O212" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="P212" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q212" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="R212" s="6" t="b">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
generated all the reports on 2024-02-24
</commit_message>
<xml_diff>
--- a/report/merged_configurations.xlsx
+++ b/report/merged_configurations.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4961" uniqueCount="1068">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4985" uniqueCount="1075">
   <si>
     <t>naam</t>
   </si>
@@ -179,7 +179,7 @@
     <t>slim-ruimtelijk-plannen-description.md</t>
   </si>
   <si>
-    <t>[{"naam":"Slim Ruimtelijk Plannen applicatieprofiel","waarde":"https://data.test-vlaanderen.be/doc/applicatieprofiel/slim-ruimtelijk-plannen/ontwerpstandaard/2023-12-12"}]</t>
+    <t>[{"naam":"Slim Ruimtelijk Plannen applicatieprofiel","waarde":"https://data.test-vlaanderen.be/doc/applicatieprofiel/slim-ruimtelijk-plannen/ontwerpstandaard/2024-01-22/"}]</t>
   </si>
   <si>
     <t>[{"naam":"Projectcharter","waarde":"Werkgroep-charter-OSLO_SlimRuimtelijkPlannen.docx"}]</t>
@@ -2687,10 +2687,25 @@
     <t>Semantische standaard voor informatie over lucht en water</t>
   </si>
   <si>
-    <t>Vocabularium en applicatieprofiel Fietsinfrastructuur</t>
-  </si>
-  <si>
-    <t>fietsinfrastructuur.md</t>
+    <t>Applicatieprofiel Fietsinfrastructuur</t>
+  </si>
+  <si>
+    <t>17 december 2021</t>
+  </si>
+  <si>
+    <t>Aanbevolgen (vrijwillig)</t>
+  </si>
+  <si>
+    <t>ap-fietsinfrastructuur-config.md</t>
+  </si>
+  <si>
+    <t>[{"naam":"Applicatieprofiel Fietsinfrastructuur","waarde":"https://data.vlaanderen.be/doc/applicatieprofiel/fietsinfrastructuur"}]</t>
+  </si>
+  <si>
+    <t>[{"naam":"Vocabularium Fietsinfrastructuur","waarde":"https://data.vlaanderen.be/ns/fiets"}]</t>
+  </si>
+  <si>
+    <t>[{"naam":"Werkgroep Charter OSLO Fietsinfrastructuur","waarde":"Werkgroep charter OSLO Fietsinfrastructuur.docx"}]</t>
   </si>
   <si>
     <t>[{"naam":"Verslag Business werkgroep - 25 maart 2021","waarde":"Verslag Business werkgroep - 25 maart 2021.docx"},{"naam":"Verslag Thematische werkgroep 1 - 20 april 2021","waarde":"Verslag Thematische werkgroep 1 - 20 april 2021.docx"},{"naam":"Verslag Thematische werkgroep 2 - 18 mei 2021","waarde":"Verslag Thematische werkgroep 2 - 18 mei 2021.docx"},{"naam":"Verslag thematische werkgroep 3 - 15 juni 2021","waarde":"Verslag thematische werkgroep 3 - 15 juni 2021.docx"},{"naam":"Verslag thematische werkgroep 4 - 16 september 2021","waarde":"Verslag thematische werkgroep 4 - 16 september 2021.docx"}]</t>
@@ -2703,6 +2718,12 @@
   </si>
   <si>
     <t>25 Maart 2021</t>
+  </si>
+  <si>
+    <t>Vocabularium Fietsinfrastructuur</t>
+  </si>
+  <si>
+    <t>voc-fietsinfrastructuur-config.md</t>
   </si>
   <si>
     <t>Applicatieprofiel DCAT-AP VL 2.0</t>
@@ -3623,7 +3644,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W212"/>
+  <dimension ref="A1:W213"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="23" width="44" customWidth="1"/>
@@ -16473,40 +16494,40 @@
         <v>43</v>
       </c>
       <c r="E185" s="3" t="s">
-        <v>36</v>
+        <v>892</v>
       </c>
       <c r="F185" s="3" t="s">
-        <v>36</v>
+        <v>893</v>
       </c>
       <c r="G185" s="3" t="s">
-        <v>165</v>
+        <v>27</v>
       </c>
       <c r="H185" s="3" t="s">
-        <v>892</v>
+        <v>894</v>
       </c>
       <c r="I185" s="3" t="s">
-        <v>30</v>
+        <v>895</v>
       </c>
       <c r="J185" s="3" t="s">
-        <v>30</v>
+        <v>896</v>
       </c>
       <c r="K185" s="3" t="s">
-        <v>30</v>
+        <v>897</v>
       </c>
       <c r="L185" s="3" t="s">
-        <v>893</v>
+        <v>898</v>
       </c>
       <c r="M185" s="3" t="s">
-        <v>894</v>
+        <v>899</v>
       </c>
       <c r="N185" s="3" t="s">
-        <v>895</v>
+        <v>900</v>
       </c>
       <c r="O185" s="3" t="s">
         <v>49</v>
       </c>
       <c r="P185" s="3" t="s">
-        <v>896</v>
+        <v>901</v>
       </c>
       <c r="Q185" s="3" t="s">
         <v>36</v>
@@ -16532,61 +16553,59 @@
     </row>
     <row r="186" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A186" s="3" t="s">
-        <v>897</v>
-      </c>
-      <c r="B186" s="3" t="s">
-        <v>898</v>
-      </c>
+        <v>902</v>
+      </c>
+      <c r="B186" s="3"/>
       <c r="C186" s="3" t="s">
-        <v>899</v>
+        <v>24</v>
       </c>
       <c r="D186" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="E186" s="4">
-        <v>44532</v>
+        <v>43</v>
+      </c>
+      <c r="E186" s="3" t="s">
+        <v>892</v>
       </c>
       <c r="F186" s="3" t="s">
         <v>63</v>
       </c>
       <c r="G186" s="3" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="H186" s="3" t="s">
-        <v>442</v>
+        <v>903</v>
       </c>
       <c r="I186" s="3" t="s">
+        <v>896</v>
+      </c>
+      <c r="J186" s="3" t="s">
+        <v>895</v>
+      </c>
+      <c r="K186" s="3" t="s">
+        <v>897</v>
+      </c>
+      <c r="L186" s="3" t="s">
+        <v>898</v>
+      </c>
+      <c r="M186" s="3" t="s">
+        <v>899</v>
+      </c>
+      <c r="N186" s="3" t="s">
         <v>900</v>
       </c>
-      <c r="J186" s="3" t="s">
+      <c r="O186" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="P186" s="3" t="s">
         <v>901</v>
       </c>
-      <c r="K186" s="3" t="s">
-        <v>902</v>
-      </c>
-      <c r="L186" s="3" t="s">
-        <v>903</v>
-      </c>
-      <c r="M186" s="3" t="s">
-        <v>904</v>
-      </c>
-      <c r="N186" s="3" t="s">
-        <v>448</v>
-      </c>
-      <c r="O186" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="P186" s="3" t="s">
-        <v>905</v>
-      </c>
       <c r="Q186" s="3" t="s">
-        <v>906</v>
+        <v>36</v>
       </c>
       <c r="R186" s="3" t="s">
-        <v>907</v>
+        <v>36</v>
       </c>
       <c r="S186" s="3" t="s">
-        <v>908</v>
+        <v>37</v>
       </c>
       <c r="T186" s="3" t="s">
         <v>37</v>
@@ -16603,59 +16622,61 @@
     </row>
     <row r="187" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A187" s="3" t="s">
-        <v>909</v>
-      </c>
-      <c r="B187" s="3"/>
+        <v>904</v>
+      </c>
+      <c r="B187" s="3" t="s">
+        <v>905</v>
+      </c>
       <c r="C187" s="3" t="s">
-        <v>24</v>
+        <v>906</v>
       </c>
       <c r="D187" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="E187" s="3" t="s">
-        <v>36</v>
+      <c r="E187" s="4">
+        <v>44532</v>
       </c>
       <c r="F187" s="3" t="s">
         <v>63</v>
       </c>
       <c r="G187" s="3" t="s">
-        <v>165</v>
+        <v>27</v>
       </c>
       <c r="H187" s="3" t="s">
+        <v>442</v>
+      </c>
+      <c r="I187" s="3" t="s">
+        <v>907</v>
+      </c>
+      <c r="J187" s="3" t="s">
+        <v>908</v>
+      </c>
+      <c r="K187" s="3" t="s">
+        <v>909</v>
+      </c>
+      <c r="L187" s="3" t="s">
         <v>910</v>
       </c>
-      <c r="I187" s="3" t="s">
+      <c r="M187" s="3" t="s">
         <v>911</v>
       </c>
-      <c r="J187" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="K187" s="3" t="s">
+      <c r="N187" s="3" t="s">
+        <v>448</v>
+      </c>
+      <c r="O187" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="P187" s="3" t="s">
         <v>912</v>
       </c>
-      <c r="L187" s="3" t="s">
+      <c r="Q187" s="3" t="s">
         <v>913</v>
       </c>
-      <c r="M187" s="3" t="s">
+      <c r="R187" s="3" t="s">
         <v>914</v>
       </c>
-      <c r="N187" s="3" t="s">
+      <c r="S187" s="3" t="s">
         <v>915</v>
-      </c>
-      <c r="O187" s="3" t="s">
-        <v>916</v>
-      </c>
-      <c r="P187" s="3" t="s">
-        <v>917</v>
-      </c>
-      <c r="Q187" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="R187" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="S187" s="3" t="s">
-        <v>37</v>
       </c>
       <c r="T187" s="3" t="s">
         <v>37</v>
@@ -16672,17 +16693,17 @@
     </row>
     <row r="188" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A188" s="3" t="s">
-        <v>918</v>
+        <v>916</v>
       </c>
       <c r="B188" s="3"/>
       <c r="C188" s="3" t="s">
-        <v>919</v>
+        <v>24</v>
       </c>
       <c r="D188" s="3" t="s">
-        <v>920</v>
+        <v>25</v>
       </c>
       <c r="E188" s="3" t="s">
-        <v>921</v>
+        <v>36</v>
       </c>
       <c r="F188" s="3" t="s">
         <v>63</v>
@@ -16691,31 +16712,31 @@
         <v>165</v>
       </c>
       <c r="H188" s="3" t="s">
+        <v>917</v>
+      </c>
+      <c r="I188" s="3" t="s">
+        <v>918</v>
+      </c>
+      <c r="J188" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="K188" s="3" t="s">
+        <v>919</v>
+      </c>
+      <c r="L188" s="3" t="s">
+        <v>920</v>
+      </c>
+      <c r="M188" s="3" t="s">
+        <v>921</v>
+      </c>
+      <c r="N188" s="3" t="s">
         <v>922</v>
       </c>
-      <c r="I188" s="3" t="s">
+      <c r="O188" s="3" t="s">
         <v>923</v>
       </c>
-      <c r="J188" s="3" t="s">
+      <c r="P188" s="3" t="s">
         <v>924</v>
-      </c>
-      <c r="K188" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="L188" s="3" t="s">
-        <v>925</v>
-      </c>
-      <c r="M188" s="3" t="s">
-        <v>926</v>
-      </c>
-      <c r="N188" s="3" t="s">
-        <v>927</v>
-      </c>
-      <c r="O188" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="P188" s="3" t="s">
-        <v>921</v>
       </c>
       <c r="Q188" s="3" t="s">
         <v>36</v>
@@ -16741,52 +16762,50 @@
     </row>
     <row r="189" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A189" s="3" t="s">
+        <v>925</v>
+      </c>
+      <c r="B189" s="3"/>
+      <c r="C189" s="3" t="s">
+        <v>926</v>
+      </c>
+      <c r="D189" s="3" t="s">
+        <v>927</v>
+      </c>
+      <c r="E189" s="3" t="s">
         <v>928</v>
-      </c>
-      <c r="B189" s="3" t="s">
-        <v>929</v>
-      </c>
-      <c r="C189" s="3" t="s">
-        <v>899</v>
-      </c>
-      <c r="D189" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="E189" s="4">
-        <v>44595</v>
       </c>
       <c r="F189" s="3" t="s">
         <v>63</v>
       </c>
       <c r="G189" s="3" t="s">
-        <v>27</v>
+        <v>165</v>
       </c>
       <c r="H189" s="3" t="s">
+        <v>929</v>
+      </c>
+      <c r="I189" s="3" t="s">
         <v>930</v>
       </c>
-      <c r="I189" s="3" t="s">
+      <c r="J189" s="3" t="s">
         <v>931</v>
       </c>
-      <c r="J189" s="3" t="s">
+      <c r="K189" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="L189" s="3" t="s">
         <v>932</v>
       </c>
-      <c r="K189" s="3" t="s">
+      <c r="M189" s="3" t="s">
         <v>933</v>
       </c>
-      <c r="L189" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="M189" s="3" t="s">
+      <c r="N189" s="3" t="s">
         <v>934</v>
-      </c>
-      <c r="N189" s="3" t="s">
-        <v>935</v>
       </c>
       <c r="O189" s="3" t="s">
         <v>77</v>
       </c>
       <c r="P189" s="3" t="s">
-        <v>936</v>
+        <v>928</v>
       </c>
       <c r="Q189" s="3" t="s">
         <v>36</v>
@@ -16795,7 +16814,7 @@
         <v>36</v>
       </c>
       <c r="S189" s="3" t="s">
-        <v>937</v>
+        <v>37</v>
       </c>
       <c r="T189" s="3" t="s">
         <v>37</v>
@@ -16812,17 +16831,19 @@
     </row>
     <row r="190" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A190" s="3" t="s">
-        <v>938</v>
-      </c>
-      <c r="B190" s="3"/>
+        <v>935</v>
+      </c>
+      <c r="B190" s="3" t="s">
+        <v>936</v>
+      </c>
       <c r="C190" s="3" t="s">
-        <v>24</v>
+        <v>906</v>
       </c>
       <c r="D190" s="3" t="s">
         <v>25</v>
       </c>
       <c r="E190" s="4">
-        <v>44896</v>
+        <v>44595</v>
       </c>
       <c r="F190" s="3" t="s">
         <v>63</v>
@@ -16831,40 +16852,40 @@
         <v>27</v>
       </c>
       <c r="H190" s="3" t="s">
+        <v>937</v>
+      </c>
+      <c r="I190" s="3" t="s">
+        <v>938</v>
+      </c>
+      <c r="J190" s="3" t="s">
         <v>939</v>
       </c>
-      <c r="I190" s="3" t="s">
+      <c r="K190" s="3" t="s">
         <v>940</v>
       </c>
-      <c r="J190" s="3" t="s">
+      <c r="L190" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="M190" s="3" t="s">
         <v>941</v>
       </c>
-      <c r="K190" s="3" t="s">
+      <c r="N190" s="3" t="s">
         <v>942</v>
       </c>
-      <c r="L190" s="3" t="s">
+      <c r="O190" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="P190" s="3" t="s">
         <v>943</v>
       </c>
-      <c r="M190" s="3" t="s">
+      <c r="Q190" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="R190" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="S190" s="3" t="s">
         <v>944</v>
-      </c>
-      <c r="N190" s="3" t="s">
-        <v>945</v>
-      </c>
-      <c r="O190" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="P190" s="4">
-        <v>44453</v>
-      </c>
-      <c r="Q190" s="4">
-        <v>44875</v>
-      </c>
-      <c r="R190" s="4">
-        <v>44896</v>
-      </c>
-      <c r="S190" s="3" t="s">
-        <v>37</v>
       </c>
       <c r="T190" s="3" t="s">
         <v>37</v>
@@ -16881,7 +16902,7 @@
     </row>
     <row r="191" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A191" s="3" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="B191" s="3"/>
       <c r="C191" s="3" t="s">
@@ -16897,28 +16918,28 @@
         <v>63</v>
       </c>
       <c r="G191" s="3" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="H191" s="3" t="s">
-        <v>939</v>
+        <v>946</v>
       </c>
       <c r="I191" s="3" t="s">
         <v>947</v>
       </c>
       <c r="J191" s="3" t="s">
-        <v>941</v>
+        <v>948</v>
       </c>
       <c r="K191" s="3" t="s">
-        <v>942</v>
+        <v>949</v>
       </c>
       <c r="L191" s="3" t="s">
-        <v>943</v>
+        <v>950</v>
       </c>
       <c r="M191" s="3" t="s">
-        <v>944</v>
+        <v>951</v>
       </c>
       <c r="N191" s="3" t="s">
-        <v>945</v>
+        <v>952</v>
       </c>
       <c r="O191" s="3" t="s">
         <v>35</v>
@@ -16950,7 +16971,7 @@
     </row>
     <row r="192" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A192" s="3" t="s">
-        <v>948</v>
+        <v>953</v>
       </c>
       <c r="B192" s="3"/>
       <c r="C192" s="3" t="s">
@@ -16966,36 +16987,40 @@
         <v>63</v>
       </c>
       <c r="G192" s="3" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="H192" s="3" t="s">
+        <v>946</v>
+      </c>
+      <c r="I192" s="3" t="s">
+        <v>954</v>
+      </c>
+      <c r="J192" s="3" t="s">
+        <v>948</v>
+      </c>
+      <c r="K192" s="3" t="s">
         <v>949</v>
       </c>
-      <c r="I192" s="3" t="s">
+      <c r="L192" s="3" t="s">
         <v>950</v>
       </c>
-      <c r="J192" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="K192" s="3" t="s">
+      <c r="M192" s="3" t="s">
         <v>951</v>
       </c>
-      <c r="L192" s="3" t="s">
+      <c r="N192" s="3" t="s">
         <v>952</v>
       </c>
-      <c r="M192" s="3" t="s">
-        <v>953</v>
-      </c>
-      <c r="N192" s="3"/>
-      <c r="O192" s="3"/>
-      <c r="P192" s="3" t="s">
-        <v>906</v>
-      </c>
-      <c r="Q192" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="R192" s="3" t="s">
-        <v>954</v>
+      <c r="O192" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="P192" s="4">
+        <v>44453</v>
+      </c>
+      <c r="Q192" s="4">
+        <v>44875</v>
+      </c>
+      <c r="R192" s="4">
+        <v>44896</v>
       </c>
       <c r="S192" s="3" t="s">
         <v>37</v>
@@ -17031,36 +17056,36 @@
         <v>63</v>
       </c>
       <c r="G193" s="3" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="H193" s="3" t="s">
-        <v>949</v>
+        <v>956</v>
       </c>
       <c r="I193" s="3" t="s">
-        <v>956</v>
+        <v>957</v>
       </c>
       <c r="J193" s="3" t="s">
         <v>30</v>
       </c>
       <c r="K193" s="3" t="s">
-        <v>951</v>
+        <v>958</v>
       </c>
       <c r="L193" s="3" t="s">
-        <v>952</v>
+        <v>959</v>
       </c>
       <c r="M193" s="3" t="s">
-        <v>953</v>
+        <v>960</v>
       </c>
       <c r="N193" s="3"/>
       <c r="O193" s="3"/>
       <c r="P193" s="3" t="s">
-        <v>906</v>
+        <v>913</v>
       </c>
       <c r="Q193" s="3" t="s">
         <v>36</v>
       </c>
       <c r="R193" s="3" t="s">
-        <v>954</v>
+        <v>961</v>
       </c>
       <c r="S193" s="3" t="s">
         <v>37</v>
@@ -17080,56 +17105,52 @@
     </row>
     <row r="194" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A194" s="3" t="s">
-        <v>957</v>
+        <v>962</v>
       </c>
       <c r="B194" s="3"/>
       <c r="C194" s="3" t="s">
-        <v>99</v>
+        <v>24</v>
       </c>
       <c r="D194" s="3" t="s">
-        <v>164</v>
+        <v>25</v>
       </c>
       <c r="E194" s="4">
-        <v>44641</v>
+        <v>44896</v>
       </c>
       <c r="F194" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="G194" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="H194" s="3" t="s">
+        <v>956</v>
+      </c>
+      <c r="I194" s="3" t="s">
+        <v>963</v>
+      </c>
+      <c r="J194" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="K194" s="3" t="s">
+        <v>958</v>
+      </c>
+      <c r="L194" s="3" t="s">
+        <v>959</v>
+      </c>
+      <c r="M194" s="3" t="s">
+        <v>960</v>
+      </c>
+      <c r="N194" s="3"/>
+      <c r="O194" s="3"/>
+      <c r="P194" s="3" t="s">
+        <v>913</v>
+      </c>
+      <c r="Q194" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="G194" s="3" t="s">
-        <v>165</v>
-      </c>
-      <c r="H194" s="3" t="s">
-        <v>958</v>
-      </c>
-      <c r="I194" s="3" t="s">
-        <v>959</v>
-      </c>
-      <c r="J194" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="K194" s="3" t="s">
-        <v>960</v>
-      </c>
-      <c r="L194" s="3" t="s">
+      <c r="R194" s="3" t="s">
         <v>961</v>
-      </c>
-      <c r="M194" s="3" t="s">
-        <v>962</v>
-      </c>
-      <c r="N194" s="3" t="s">
-        <v>963</v>
-      </c>
-      <c r="O194" s="3" t="s">
-        <v>964</v>
-      </c>
-      <c r="P194" s="3" t="s">
-        <v>965</v>
-      </c>
-      <c r="Q194" s="3" t="s">
-        <v>966</v>
-      </c>
-      <c r="R194" s="3" t="s">
-        <v>36</v>
       </c>
       <c r="S194" s="3" t="s">
         <v>37</v>
@@ -17149,53 +17170,53 @@
     </row>
     <row r="195" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A195" s="3" t="s">
-        <v>967</v>
+        <v>964</v>
       </c>
       <c r="B195" s="3"/>
       <c r="C195" s="3" t="s">
-        <v>24</v>
+        <v>99</v>
       </c>
       <c r="D195" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="E195" s="3" t="s">
-        <v>36</v>
+        <v>164</v>
+      </c>
+      <c r="E195" s="4">
+        <v>44641</v>
       </c>
       <c r="F195" s="3" t="s">
         <v>36</v>
       </c>
       <c r="G195" s="3" t="s">
-        <v>27</v>
+        <v>165</v>
       </c>
       <c r="H195" s="3" t="s">
+        <v>965</v>
+      </c>
+      <c r="I195" s="3" t="s">
+        <v>966</v>
+      </c>
+      <c r="J195" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="K195" s="3" t="s">
+        <v>967</v>
+      </c>
+      <c r="L195" s="3" t="s">
         <v>968</v>
       </c>
-      <c r="I195" s="3" t="s">
+      <c r="M195" s="3" t="s">
         <v>969</v>
       </c>
-      <c r="J195" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="K195" s="3" t="s">
+      <c r="N195" s="3" t="s">
         <v>970</v>
       </c>
-      <c r="L195" s="3" t="s">
+      <c r="O195" s="3" t="s">
         <v>971</v>
       </c>
-      <c r="M195" s="3" t="s">
+      <c r="P195" s="3" t="s">
         <v>972</v>
       </c>
-      <c r="N195" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="O195" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="P195" s="3" t="s">
-        <v>36</v>
-      </c>
       <c r="Q195" s="3" t="s">
-        <v>36</v>
+        <v>973</v>
       </c>
       <c r="R195" s="3" t="s">
         <v>36</v>
@@ -17218,7 +17239,7 @@
     </row>
     <row r="196" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A196" s="3" t="s">
-        <v>973</v>
+        <v>974</v>
       </c>
       <c r="B196" s="3"/>
       <c r="C196" s="3" t="s">
@@ -17234,25 +17255,25 @@
         <v>36</v>
       </c>
       <c r="G196" s="3" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="H196" s="3" t="s">
-        <v>974</v>
+        <v>975</v>
       </c>
       <c r="I196" s="3" t="s">
-        <v>975</v>
+        <v>976</v>
       </c>
       <c r="J196" s="3" t="s">
         <v>30</v>
       </c>
       <c r="K196" s="3" t="s">
-        <v>970</v>
+        <v>977</v>
       </c>
       <c r="L196" s="3" t="s">
-        <v>971</v>
+        <v>978</v>
       </c>
       <c r="M196" s="3" t="s">
-        <v>972</v>
+        <v>979</v>
       </c>
       <c r="N196" s="3" t="s">
         <v>36</v>
@@ -17287,57 +17308,59 @@
     </row>
     <row r="197" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A197" s="3" t="s">
-        <v>976</v>
+        <v>980</v>
       </c>
       <c r="B197" s="3"/>
       <c r="C197" s="3" t="s">
         <v>24</v>
       </c>
       <c r="D197" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="E197" s="4">
-        <v>44896</v>
+        <v>43</v>
+      </c>
+      <c r="E197" s="3" t="s">
+        <v>36</v>
       </c>
       <c r="F197" s="3" t="s">
-        <v>63</v>
+        <v>36</v>
       </c>
       <c r="G197" s="3" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="H197" s="3" t="s">
+        <v>981</v>
+      </c>
+      <c r="I197" s="3" t="s">
+        <v>982</v>
+      </c>
+      <c r="J197" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="K197" s="3" t="s">
         <v>977</v>
       </c>
-      <c r="I197" s="3" t="s">
+      <c r="L197" s="3" t="s">
         <v>978</v>
       </c>
-      <c r="J197" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="K197" s="3" t="s">
+      <c r="M197" s="3" t="s">
         <v>979</v>
       </c>
-      <c r="L197" s="3" t="s">
-        <v>980</v>
-      </c>
-      <c r="M197" s="3" t="s">
-        <v>981</v>
-      </c>
       <c r="N197" s="3" t="s">
-        <v>982</v>
+        <v>36</v>
       </c>
       <c r="O197" s="3" t="s">
-        <v>983</v>
-      </c>
-      <c r="P197" s="3"/>
+        <v>36</v>
+      </c>
+      <c r="P197" s="3" t="s">
+        <v>36</v>
+      </c>
       <c r="Q197" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="R197" s="4">
-        <v>44896</v>
-      </c>
-      <c r="S197" s="4">
-        <v>44845</v>
+      <c r="R197" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="S197" s="3" t="s">
+        <v>37</v>
       </c>
       <c r="T197" s="3" t="s">
         <v>37</v>
@@ -17354,7 +17377,7 @@
     </row>
     <row r="198" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A198" s="3" t="s">
-        <v>984</v>
+        <v>983</v>
       </c>
       <c r="B198" s="3"/>
       <c r="C198" s="3" t="s">
@@ -17370,31 +17393,31 @@
         <v>63</v>
       </c>
       <c r="G198" s="3" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="H198" s="3" t="s">
+        <v>984</v>
+      </c>
+      <c r="I198" s="3" t="s">
         <v>985</v>
       </c>
-      <c r="I198" s="3" t="s">
+      <c r="J198" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="K198" s="3" t="s">
         <v>986</v>
-      </c>
-      <c r="J198" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="K198" s="3" t="s">
-        <v>979</v>
       </c>
       <c r="L198" s="3" t="s">
         <v>987</v>
       </c>
       <c r="M198" s="3" t="s">
-        <v>981</v>
+        <v>988</v>
       </c>
       <c r="N198" s="3" t="s">
-        <v>982</v>
+        <v>989</v>
       </c>
       <c r="O198" s="3" t="s">
-        <v>983</v>
+        <v>990</v>
       </c>
       <c r="P198" s="3"/>
       <c r="Q198" s="3" t="s">
@@ -17421,7 +17444,7 @@
     </row>
     <row r="199" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A199" s="3" t="s">
-        <v>988</v>
+        <v>991</v>
       </c>
       <c r="B199" s="3"/>
       <c r="C199" s="3" t="s">
@@ -17431,49 +17454,47 @@
         <v>25</v>
       </c>
       <c r="E199" s="4">
-        <v>44915</v>
+        <v>44896</v>
       </c>
       <c r="F199" s="3" t="s">
         <v>63</v>
       </c>
       <c r="G199" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="H199" s="3" t="s">
+        <v>992</v>
+      </c>
+      <c r="I199" s="3" t="s">
+        <v>993</v>
+      </c>
+      <c r="J199" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="K199" s="3" t="s">
+        <v>986</v>
+      </c>
+      <c r="L199" s="3" t="s">
+        <v>994</v>
+      </c>
+      <c r="M199" s="3" t="s">
+        <v>988</v>
+      </c>
+      <c r="N199" s="3" t="s">
         <v>989</v>
       </c>
-      <c r="H199" s="3" t="s">
+      <c r="O199" s="3" t="s">
         <v>990</v>
       </c>
-      <c r="I199" s="3" t="s">
-        <v>991</v>
-      </c>
-      <c r="J199" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="K199" s="3" t="s">
-        <v>992</v>
-      </c>
-      <c r="L199" s="3" t="s">
-        <v>993</v>
-      </c>
-      <c r="M199" s="3" t="s">
-        <v>994</v>
-      </c>
-      <c r="N199" s="3" t="s">
-        <v>995</v>
-      </c>
-      <c r="O199" s="3" t="s">
-        <v>996</v>
-      </c>
-      <c r="P199" s="3" t="s">
-        <v>997</v>
-      </c>
+      <c r="P199" s="3"/>
       <c r="Q199" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="R199" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="S199" s="3" t="s">
-        <v>37</v>
+      <c r="R199" s="4">
+        <v>44896</v>
+      </c>
+      <c r="S199" s="4">
+        <v>44845</v>
       </c>
       <c r="T199" s="3" t="s">
         <v>37</v>
@@ -17490,7 +17511,7 @@
     </row>
     <row r="200" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A200" s="3" t="s">
-        <v>998</v>
+        <v>995</v>
       </c>
       <c r="B200" s="3"/>
       <c r="C200" s="3" t="s">
@@ -17500,43 +17521,43 @@
         <v>25</v>
       </c>
       <c r="E200" s="4">
-        <v>45239</v>
+        <v>44915</v>
       </c>
       <c r="F200" s="3" t="s">
         <v>63</v>
       </c>
       <c r="G200" s="3" t="s">
-        <v>27</v>
+        <v>996</v>
       </c>
       <c r="H200" s="3" t="s">
-        <v>64</v>
+        <v>997</v>
       </c>
       <c r="I200" s="3" t="s">
+        <v>998</v>
+      </c>
+      <c r="J200" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="K200" s="3" t="s">
         <v>999</v>
       </c>
-      <c r="J200" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="K200" s="3" t="s">
+      <c r="L200" s="3" t="s">
         <v>1000</v>
       </c>
-      <c r="L200" s="3" t="s">
+      <c r="M200" s="3" t="s">
         <v>1001</v>
       </c>
-      <c r="M200" s="3" t="s">
+      <c r="N200" s="3" t="s">
         <v>1002</v>
       </c>
-      <c r="N200" s="3" t="s">
+      <c r="O200" s="3" t="s">
         <v>1003</v>
       </c>
-      <c r="O200" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="P200" s="4">
-        <v>44812</v>
-      </c>
-      <c r="Q200" s="4">
-        <v>45239</v>
+      <c r="P200" s="3" t="s">
+        <v>1004</v>
+      </c>
+      <c r="Q200" s="3" t="s">
+        <v>36</v>
       </c>
       <c r="R200" s="3" t="s">
         <v>36</v>
@@ -17559,7 +17580,7 @@
     </row>
     <row r="201" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A201" s="3" t="s">
-        <v>1004</v>
+        <v>1005</v>
       </c>
       <c r="B201" s="3"/>
       <c r="C201" s="3" t="s">
@@ -17575,28 +17596,28 @@
         <v>63</v>
       </c>
       <c r="G201" s="3" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="H201" s="3" t="s">
         <v>64</v>
       </c>
       <c r="I201" s="3" t="s">
-        <v>1005</v>
+        <v>1006</v>
       </c>
       <c r="J201" s="3" t="s">
         <v>30</v>
       </c>
       <c r="K201" s="3" t="s">
-        <v>1000</v>
+        <v>1007</v>
       </c>
       <c r="L201" s="3" t="s">
-        <v>1006</v>
+        <v>1008</v>
       </c>
       <c r="M201" s="3" t="s">
-        <v>1002</v>
+        <v>1009</v>
       </c>
       <c r="N201" s="3" t="s">
-        <v>1003</v>
+        <v>1010</v>
       </c>
       <c r="O201" s="3" t="s">
         <v>35</v>
@@ -17628,7 +17649,7 @@
     </row>
     <row r="202" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A202" s="3" t="s">
-        <v>1007</v>
+        <v>1011</v>
       </c>
       <c r="B202" s="3"/>
       <c r="C202" s="3" t="s">
@@ -17637,34 +17658,48 @@
       <c r="D202" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="E202" s="3"/>
+      <c r="E202" s="4">
+        <v>45239</v>
+      </c>
       <c r="F202" s="3" t="s">
         <v>63</v>
       </c>
       <c r="G202" s="3" t="s">
-        <v>1008</v>
-      </c>
-      <c r="H202" s="3"/>
+        <v>39</v>
+      </c>
+      <c r="H202" s="3" t="s">
+        <v>64</v>
+      </c>
       <c r="I202" s="3" t="s">
+        <v>1012</v>
+      </c>
+      <c r="J202" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="K202" s="3" t="s">
+        <v>1007</v>
+      </c>
+      <c r="L202" s="3" t="s">
+        <v>1013</v>
+      </c>
+      <c r="M202" s="3" t="s">
         <v>1009</v>
       </c>
-      <c r="J202" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="K202" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="L202" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="M202" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="N202" s="3"/>
-      <c r="O202" s="3"/>
-      <c r="P202" s="3"/>
-      <c r="Q202" s="3"/>
-      <c r="R202" s="3"/>
+      <c r="N202" s="3" t="s">
+        <v>1010</v>
+      </c>
+      <c r="O202" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="P202" s="4">
+        <v>44812</v>
+      </c>
+      <c r="Q202" s="4">
+        <v>45239</v>
+      </c>
+      <c r="R202" s="3" t="s">
+        <v>36</v>
+      </c>
       <c r="S202" s="3" t="s">
         <v>37</v>
       </c>
@@ -17683,7 +17718,7 @@
     </row>
     <row r="203" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A203" s="3" t="s">
-        <v>1010</v>
+        <v>1014</v>
       </c>
       <c r="B203" s="3"/>
       <c r="C203" s="3" t="s">
@@ -17692,46 +17727,34 @@
       <c r="D203" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="E203" s="3" t="s">
-        <v>36</v>
-      </c>
+      <c r="E203" s="3"/>
       <c r="F203" s="3" t="s">
         <v>63</v>
       </c>
       <c r="G203" s="3" t="s">
-        <v>165</v>
-      </c>
-      <c r="H203" s="3" t="s">
-        <v>1011</v>
-      </c>
+        <v>1015</v>
+      </c>
+      <c r="H203" s="3"/>
       <c r="I203" s="3" t="s">
-        <v>1012</v>
+        <v>1016</v>
       </c>
       <c r="J203" s="3" t="s">
         <v>30</v>
       </c>
       <c r="K203" s="3" t="s">
-        <v>1013</v>
+        <v>30</v>
       </c>
       <c r="L203" s="3" t="s">
-        <v>1014</v>
+        <v>30</v>
       </c>
       <c r="M203" s="3" t="s">
-        <v>1015</v>
-      </c>
-      <c r="N203" s="3" t="s">
-        <v>1016</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="N203" s="3"/>
       <c r="O203" s="3"/>
-      <c r="P203" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q203" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="R203" s="3" t="s">
-        <v>36</v>
-      </c>
+      <c r="P203" s="3"/>
+      <c r="Q203" s="3"/>
+      <c r="R203" s="3"/>
       <c r="S203" s="3" t="s">
         <v>37</v>
       </c>
@@ -17759,17 +17782,23 @@
       <c r="D204" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="E204" s="3"/>
-      <c r="F204" s="3"/>
+      <c r="E204" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F204" s="3" t="s">
+        <v>63</v>
+      </c>
       <c r="G204" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="H204" s="3"/>
+        <v>165</v>
+      </c>
+      <c r="H204" s="3" t="s">
+        <v>1018</v>
+      </c>
       <c r="I204" s="3" t="s">
-        <v>1018</v>
+        <v>1019</v>
       </c>
       <c r="J204" s="3" t="s">
-        <v>1019</v>
+        <v>30</v>
       </c>
       <c r="K204" s="3" t="s">
         <v>1020</v>
@@ -17783,12 +17812,16 @@
       <c r="N204" s="3" t="s">
         <v>1023</v>
       </c>
-      <c r="O204" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="P204" s="3"/>
-      <c r="Q204" s="3"/>
-      <c r="R204" s="3"/>
+      <c r="O204" s="3"/>
+      <c r="P204" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q204" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="R204" s="3" t="s">
+        <v>36</v>
+      </c>
       <c r="S204" s="3" t="s">
         <v>37</v>
       </c>
@@ -17816,48 +17849,36 @@
       <c r="D205" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="E205" s="4">
-        <v>45131</v>
-      </c>
-      <c r="F205" s="3" t="s">
-        <v>63</v>
-      </c>
+      <c r="E205" s="3"/>
+      <c r="F205" s="3"/>
       <c r="G205" s="3" t="s">
-        <v>760</v>
-      </c>
-      <c r="H205" s="3" t="s">
-        <v>64</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="H205" s="3"/>
       <c r="I205" s="3" t="s">
         <v>1025</v>
       </c>
       <c r="J205" s="3" t="s">
-        <v>30</v>
+        <v>1026</v>
       </c>
       <c r="K205" s="3" t="s">
-        <v>1026</v>
+        <v>1027</v>
       </c>
       <c r="L205" s="3" t="s">
-        <v>1027</v>
+        <v>1028</v>
       </c>
       <c r="M205" s="3" t="s">
-        <v>1028</v>
+        <v>1029</v>
       </c>
       <c r="N205" s="3" t="s">
-        <v>1029</v>
+        <v>1030</v>
       </c>
       <c r="O205" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="P205" s="4">
-        <v>44873</v>
-      </c>
-      <c r="Q205" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="R205" s="3" t="s">
-        <v>36</v>
-      </c>
+      <c r="P205" s="3"/>
+      <c r="Q205" s="3"/>
+      <c r="R205" s="3"/>
       <c r="S205" s="3" t="s">
         <v>37</v>
       </c>
@@ -17876,7 +17897,7 @@
     </row>
     <row r="206" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A206" s="3" t="s">
-        <v>1030</v>
+        <v>1031</v>
       </c>
       <c r="B206" s="3"/>
       <c r="C206" s="3" t="s">
@@ -17892,28 +17913,28 @@
         <v>63</v>
       </c>
       <c r="G206" s="3" t="s">
-        <v>39</v>
+        <v>760</v>
       </c>
       <c r="H206" s="3" t="s">
         <v>64</v>
       </c>
       <c r="I206" s="3" t="s">
-        <v>1031</v>
+        <v>1032</v>
       </c>
       <c r="J206" s="3" t="s">
         <v>30</v>
       </c>
       <c r="K206" s="3" t="s">
-        <v>1026</v>
+        <v>1033</v>
       </c>
       <c r="L206" s="3" t="s">
-        <v>1027</v>
+        <v>1034</v>
       </c>
       <c r="M206" s="3" t="s">
-        <v>1028</v>
+        <v>1035</v>
       </c>
       <c r="N206" s="3" t="s">
-        <v>1029</v>
+        <v>1036</v>
       </c>
       <c r="O206" s="3" t="s">
         <v>35</v>
@@ -17945,53 +17966,53 @@
     </row>
     <row r="207" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A207" s="3" t="s">
-        <v>1032</v>
+        <v>1037</v>
       </c>
       <c r="B207" s="3"/>
       <c r="C207" s="3" t="s">
-        <v>399</v>
+        <v>24</v>
       </c>
       <c r="D207" s="3" t="s">
-        <v>505</v>
+        <v>25</v>
       </c>
       <c r="E207" s="4">
-        <v>45330</v>
+        <v>45131</v>
       </c>
       <c r="F207" s="3" t="s">
         <v>63</v>
       </c>
       <c r="G207" s="3" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="H207" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="I207" s="3" t="s">
+        <v>1038</v>
+      </c>
+      <c r="J207" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="K207" s="3" t="s">
         <v>1033</v>
       </c>
-      <c r="I207" s="3" t="s">
+      <c r="L207" s="3" t="s">
         <v>1034</v>
       </c>
-      <c r="J207" s="3" t="s">
+      <c r="M207" s="3" t="s">
         <v>1035</v>
       </c>
-      <c r="K207" s="3" t="s">
+      <c r="N207" s="3" t="s">
         <v>1036</v>
       </c>
-      <c r="L207" s="3" t="s">
-        <v>1037</v>
-      </c>
-      <c r="M207" s="3" t="s">
-        <v>1038</v>
-      </c>
-      <c r="N207" s="3" t="s">
-        <v>1039</v>
-      </c>
       <c r="O207" s="3" t="s">
-        <v>1040</v>
-      </c>
-      <c r="P207" s="3" t="s">
-        <v>1041</v>
+        <v>35</v>
+      </c>
+      <c r="P207" s="4">
+        <v>44873</v>
       </c>
       <c r="Q207" s="3" t="s">
-        <v>1042</v>
+        <v>36</v>
       </c>
       <c r="R207" s="3" t="s">
         <v>36</v>
@@ -18014,7 +18035,7 @@
     </row>
     <row r="208" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A208" s="3" t="s">
-        <v>1043</v>
+        <v>1039</v>
       </c>
       <c r="B208" s="3"/>
       <c r="C208" s="3" t="s">
@@ -18030,37 +18051,37 @@
         <v>63</v>
       </c>
       <c r="G208" s="3" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="H208" s="3" t="s">
+        <v>1040</v>
+      </c>
+      <c r="I208" s="3" t="s">
+        <v>1041</v>
+      </c>
+      <c r="J208" s="3" t="s">
+        <v>1042</v>
+      </c>
+      <c r="K208" s="3" t="s">
+        <v>1043</v>
+      </c>
+      <c r="L208" s="3" t="s">
         <v>1044</v>
       </c>
-      <c r="I208" s="3" t="s">
-        <v>1035</v>
-      </c>
-      <c r="J208" s="3" t="s">
-        <v>1034</v>
-      </c>
-      <c r="K208" s="3" t="s">
-        <v>1036</v>
-      </c>
-      <c r="L208" s="3" t="s">
-        <v>1037</v>
-      </c>
       <c r="M208" s="3" t="s">
-        <v>1038</v>
+        <v>1045</v>
       </c>
       <c r="N208" s="3" t="s">
-        <v>1039</v>
+        <v>1046</v>
       </c>
       <c r="O208" s="3" t="s">
-        <v>1040</v>
+        <v>1047</v>
       </c>
       <c r="P208" s="3" t="s">
-        <v>1041</v>
+        <v>1048</v>
       </c>
       <c r="Q208" s="3" t="s">
-        <v>1042</v>
+        <v>1049</v>
       </c>
       <c r="R208" s="3" t="s">
         <v>36</v>
@@ -18083,51 +18104,57 @@
     </row>
     <row r="209" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A209" s="3" t="s">
-        <v>1045</v>
+        <v>1050</v>
       </c>
       <c r="B209" s="3"/>
       <c r="C209" s="3" t="s">
-        <v>24</v>
+        <v>399</v>
       </c>
       <c r="D209" s="3" t="s">
-        <v>25</v>
+        <v>505</v>
       </c>
       <c r="E209" s="4">
-        <v>45308</v>
+        <v>45330</v>
       </c>
       <c r="F209" s="3" t="s">
         <v>63</v>
       </c>
       <c r="G209" s="3" t="s">
-        <v>102</v>
+        <v>39</v>
       </c>
       <c r="H209" s="3" t="s">
-        <v>64</v>
+        <v>1051</v>
       </c>
       <c r="I209" s="3" t="s">
+        <v>1042</v>
+      </c>
+      <c r="J209" s="3" t="s">
+        <v>1041</v>
+      </c>
+      <c r="K209" s="3" t="s">
+        <v>1043</v>
+      </c>
+      <c r="L209" s="3" t="s">
+        <v>1044</v>
+      </c>
+      <c r="M209" s="3" t="s">
+        <v>1045</v>
+      </c>
+      <c r="N209" s="3" t="s">
         <v>1046</v>
       </c>
-      <c r="J209" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="K209" s="3" t="s">
+      <c r="O209" s="3" t="s">
         <v>1047</v>
       </c>
-      <c r="L209" s="3" t="s">
+      <c r="P209" s="3" t="s">
         <v>1048</v>
       </c>
-      <c r="M209" s="3" t="s">
+      <c r="Q209" s="3" t="s">
         <v>1049</v>
       </c>
-      <c r="N209" s="3" t="s">
-        <v>1050</v>
-      </c>
-      <c r="O209" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="P209" s="3"/>
-      <c r="Q209" s="3"/>
-      <c r="R209" s="3"/>
+      <c r="R209" s="3" t="s">
+        <v>36</v>
+      </c>
       <c r="S209" s="3" t="s">
         <v>37</v>
       </c>
@@ -18146,7 +18173,7 @@
     </row>
     <row r="210" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A210" s="3" t="s">
-        <v>1051</v>
+        <v>1052</v>
       </c>
       <c r="B210" s="3"/>
       <c r="C210" s="3" t="s">
@@ -18162,28 +18189,28 @@
         <v>63</v>
       </c>
       <c r="G210" s="3" t="s">
-        <v>112</v>
+        <v>102</v>
       </c>
       <c r="H210" s="3" t="s">
         <v>64</v>
       </c>
       <c r="I210" s="3" t="s">
-        <v>1052</v>
+        <v>1053</v>
       </c>
       <c r="J210" s="3" t="s">
         <v>30</v>
       </c>
       <c r="K210" s="3" t="s">
-        <v>1047</v>
+        <v>1054</v>
       </c>
       <c r="L210" s="3" t="s">
-        <v>1048</v>
+        <v>1055</v>
       </c>
       <c r="M210" s="3" t="s">
-        <v>1049</v>
+        <v>1056</v>
       </c>
       <c r="N210" s="3" t="s">
-        <v>1050</v>
+        <v>1057</v>
       </c>
       <c r="O210" s="3" t="s">
         <v>77</v>
@@ -18209,57 +18236,51 @@
     </row>
     <row r="211" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A211" s="3" t="s">
-        <v>1053</v>
+        <v>1058</v>
       </c>
       <c r="B211" s="3"/>
       <c r="C211" s="3" t="s">
-        <v>1054</v>
+        <v>24</v>
       </c>
       <c r="D211" s="3" t="s">
-        <v>1055</v>
+        <v>25</v>
       </c>
       <c r="E211" s="4">
-        <v>45323</v>
+        <v>45308</v>
       </c>
       <c r="F211" s="3" t="s">
         <v>63</v>
       </c>
       <c r="G211" s="3" t="s">
-        <v>27</v>
+        <v>112</v>
       </c>
       <c r="H211" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="I211" s="3" t="s">
+        <v>1059</v>
+      </c>
+      <c r="J211" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="K211" s="3" t="s">
+        <v>1054</v>
+      </c>
+      <c r="L211" s="3" t="s">
+        <v>1055</v>
+      </c>
+      <c r="M211" s="3" t="s">
         <v>1056</v>
       </c>
-      <c r="I211" s="3" t="s">
+      <c r="N211" s="3" t="s">
         <v>1057</v>
       </c>
-      <c r="J211" s="3" t="s">
-        <v>1058</v>
-      </c>
-      <c r="K211" s="3" t="s">
-        <v>1059</v>
-      </c>
-      <c r="L211" s="3" t="s">
-        <v>1060</v>
-      </c>
-      <c r="M211" s="3" t="s">
-        <v>1061</v>
-      </c>
-      <c r="N211" s="3" t="s">
-        <v>1062</v>
-      </c>
       <c r="O211" s="3" t="s">
-        <v>1063</v>
-      </c>
-      <c r="P211" s="3" t="s">
-        <v>1064</v>
-      </c>
-      <c r="Q211" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="R211" s="3" t="s">
-        <v>36</v>
-      </c>
+        <v>77</v>
+      </c>
+      <c r="P211" s="3"/>
+      <c r="Q211" s="3"/>
+      <c r="R211" s="3"/>
       <c r="S211" s="3" t="s">
         <v>37</v>
       </c>
@@ -18278,14 +18299,14 @@
     </row>
     <row r="212" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A212" s="3" t="s">
-        <v>1065</v>
+        <v>1060</v>
       </c>
       <c r="B212" s="3"/>
       <c r="C212" s="3" t="s">
-        <v>1054</v>
+        <v>1061</v>
       </c>
       <c r="D212" s="3" t="s">
-        <v>1055</v>
+        <v>1062</v>
       </c>
       <c r="E212" s="4">
         <v>45323</v>
@@ -18294,34 +18315,34 @@
         <v>63</v>
       </c>
       <c r="G212" s="3" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="H212" s="3" t="s">
+        <v>1063</v>
+      </c>
+      <c r="I212" s="3" t="s">
+        <v>1064</v>
+      </c>
+      <c r="J212" s="3" t="s">
+        <v>1065</v>
+      </c>
+      <c r="K212" s="3" t="s">
         <v>1066</v>
       </c>
-      <c r="I212" s="3" t="s">
-        <v>1057</v>
-      </c>
-      <c r="J212" s="3" t="s">
-        <v>1058</v>
-      </c>
-      <c r="K212" s="3" t="s">
-        <v>1059</v>
-      </c>
       <c r="L212" s="3" t="s">
-        <v>1060</v>
+        <v>1067</v>
       </c>
       <c r="M212" s="3" t="s">
-        <v>1061</v>
+        <v>1068</v>
       </c>
       <c r="N212" s="3" t="s">
-        <v>1062</v>
+        <v>1069</v>
       </c>
       <c r="O212" s="3" t="s">
-        <v>1063</v>
+        <v>1070</v>
       </c>
       <c r="P212" s="3" t="s">
-        <v>1064</v>
+        <v>1071</v>
       </c>
       <c r="Q212" s="3" t="s">
         <v>36</v>
@@ -18342,6 +18363,75 @@
         <v>37</v>
       </c>
       <c r="W212" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="213" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A213" s="3" t="s">
+        <v>1072</v>
+      </c>
+      <c r="B213" s="3"/>
+      <c r="C213" s="3" t="s">
+        <v>1061</v>
+      </c>
+      <c r="D213" s="3" t="s">
+        <v>1062</v>
+      </c>
+      <c r="E213" s="4">
+        <v>45323</v>
+      </c>
+      <c r="F213" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="G213" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="H213" s="3" t="s">
+        <v>1073</v>
+      </c>
+      <c r="I213" s="3" t="s">
+        <v>1064</v>
+      </c>
+      <c r="J213" s="3" t="s">
+        <v>1065</v>
+      </c>
+      <c r="K213" s="3" t="s">
+        <v>1066</v>
+      </c>
+      <c r="L213" s="3" t="s">
+        <v>1067</v>
+      </c>
+      <c r="M213" s="3" t="s">
+        <v>1068</v>
+      </c>
+      <c r="N213" s="3" t="s">
+        <v>1069</v>
+      </c>
+      <c r="O213" s="3" t="s">
+        <v>1070</v>
+      </c>
+      <c r="P213" s="3" t="s">
+        <v>1071</v>
+      </c>
+      <c r="Q213" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="R213" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="S213" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="T213" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="U213" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="V213" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="W213" s="3" t="s">
         <v>37</v>
       </c>
     </row>
@@ -18353,7 +18443,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R212"/>
+  <dimension ref="A1:R213"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="18" width="44" customWidth="1"/>
@@ -18420,7 +18510,7 @@
         <v>23</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>1067</v>
+        <v>1074</v>
       </c>
       <c r="C2" s="5" t="b">
         <v>1</v>
@@ -18476,7 +18566,7 @@
         <v>38</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>1067</v>
+        <v>1074</v>
       </c>
       <c r="C3" s="5" t="b">
         <v>1</v>
@@ -18532,7 +18622,7 @@
         <v>42</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>1067</v>
+        <v>1074</v>
       </c>
       <c r="C4" s="5" t="b">
         <v>1</v>
@@ -18588,7 +18678,7 @@
         <v>51</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>1067</v>
+        <v>1074</v>
       </c>
       <c r="C5" s="5" t="b">
         <v>1</v>
@@ -18644,7 +18734,7 @@
         <v>53</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>1067</v>
+        <v>1074</v>
       </c>
       <c r="C6" s="5" t="b">
         <v>1</v>
@@ -18700,7 +18790,7 @@
         <v>60</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>1067</v>
+        <v>1074</v>
       </c>
       <c r="C7" s="5" t="b">
         <v>1</v>
@@ -18756,7 +18846,7 @@
         <v>62</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>1067</v>
+        <v>1074</v>
       </c>
       <c r="C8" s="5" t="b">
         <v>1</v>
@@ -18812,7 +18902,7 @@
         <v>70</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>1067</v>
+        <v>1074</v>
       </c>
       <c r="C9" s="5" t="b">
         <v>1</v>
@@ -18868,7 +18958,7 @@
         <v>79</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>1067</v>
+        <v>1074</v>
       </c>
       <c r="C10" s="5" t="b">
         <v>1</v>
@@ -18924,7 +19014,7 @@
         <v>81</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>1067</v>
+        <v>1074</v>
       </c>
       <c r="C11" s="5" t="b">
         <v>1</v>
@@ -18980,7 +19070,7 @@
         <v>90</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>1067</v>
+        <v>1074</v>
       </c>
       <c r="C12" s="5" t="b">
         <v>1</v>
@@ -19148,7 +19238,7 @@
         <v>115</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>1067</v>
+        <v>1074</v>
       </c>
       <c r="C15" s="5" t="b">
         <v>1</v>
@@ -19204,7 +19294,7 @@
         <v>126</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>1067</v>
+        <v>1074</v>
       </c>
       <c r="C16" s="5" t="b">
         <v>1</v>
@@ -19260,7 +19350,7 @@
         <v>128</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>1067</v>
+        <v>1074</v>
       </c>
       <c r="C17" s="5" t="b">
         <v>1</v>
@@ -19316,7 +19406,7 @@
         <v>130</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>1067</v>
+        <v>1074</v>
       </c>
       <c r="C18" s="5" t="b">
         <v>1</v>
@@ -19372,7 +19462,7 @@
         <v>132</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>1067</v>
+        <v>1074</v>
       </c>
       <c r="C19" s="5" t="b">
         <v>1</v>
@@ -19428,7 +19518,7 @@
         <v>135</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>1067</v>
+        <v>1074</v>
       </c>
       <c r="C20" s="5" t="b">
         <v>1</v>
@@ -19484,7 +19574,7 @@
         <v>137</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>1067</v>
+        <v>1074</v>
       </c>
       <c r="C21" s="5" t="b">
         <v>1</v>
@@ -19540,7 +19630,7 @@
         <v>139</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>1067</v>
+        <v>1074</v>
       </c>
       <c r="C22" s="5" t="b">
         <v>1</v>
@@ -19596,7 +19686,7 @@
         <v>141</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>1067</v>
+        <v>1074</v>
       </c>
       <c r="C23" s="5" t="b">
         <v>1</v>
@@ -19652,7 +19742,7 @@
         <v>143</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>1067</v>
+        <v>1074</v>
       </c>
       <c r="C24" s="5" t="b">
         <v>1</v>
@@ -19708,7 +19798,7 @@
         <v>145</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>1067</v>
+        <v>1074</v>
       </c>
       <c r="C25" s="5" t="b">
         <v>1</v>
@@ -19764,7 +19854,7 @@
         <v>143</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>1067</v>
+        <v>1074</v>
       </c>
       <c r="C26" s="5" t="b">
         <v>1</v>
@@ -19820,7 +19910,7 @@
         <v>147</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>1067</v>
+        <v>1074</v>
       </c>
       <c r="C27" s="5" t="b">
         <v>1</v>
@@ -19876,7 +19966,7 @@
         <v>149</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>1067</v>
+        <v>1074</v>
       </c>
       <c r="C28" s="5" t="b">
         <v>1</v>
@@ -19932,7 +20022,7 @@
         <v>151</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>1067</v>
+        <v>1074</v>
       </c>
       <c r="C29" s="5" t="b">
         <v>1</v>
@@ -19988,7 +20078,7 @@
         <v>153</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>1067</v>
+        <v>1074</v>
       </c>
       <c r="C30" s="5" t="b">
         <v>1</v>
@@ -20044,7 +20134,7 @@
         <v>155</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>1067</v>
+        <v>1074</v>
       </c>
       <c r="C31" s="5" t="b">
         <v>1</v>
@@ -20100,7 +20190,7 @@
         <v>157</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>1067</v>
+        <v>1074</v>
       </c>
       <c r="C32" s="5" t="b">
         <v>1</v>
@@ -20156,7 +20246,7 @@
         <v>159</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>1067</v>
+        <v>1074</v>
       </c>
       <c r="C33" s="5" t="b">
         <v>1</v>
@@ -20212,7 +20302,7 @@
         <v>161</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>1067</v>
+        <v>1074</v>
       </c>
       <c r="C34" s="5" t="b">
         <v>1</v>
@@ -20268,7 +20358,7 @@
         <v>163</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>1067</v>
+        <v>1074</v>
       </c>
       <c r="C35" s="5" t="b">
         <v>1</v>
@@ -20436,7 +20526,7 @@
         <v>193</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>1067</v>
+        <v>1074</v>
       </c>
       <c r="C38" s="5" t="b">
         <v>1</v>
@@ -20492,7 +20582,7 @@
         <v>200</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>1067</v>
+        <v>1074</v>
       </c>
       <c r="C39" s="5" t="b">
         <v>1</v>
@@ -22060,7 +22150,7 @@
         <v>382</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>1067</v>
+        <v>1074</v>
       </c>
       <c r="C67" s="5" t="b">
         <v>1</v>
@@ -22116,7 +22206,7 @@
         <v>394</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>1067</v>
+        <v>1074</v>
       </c>
       <c r="C68" s="5" t="b">
         <v>1</v>
@@ -22564,7 +22654,7 @@
         <v>453</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>1067</v>
+        <v>1074</v>
       </c>
       <c r="C76" s="5" t="b">
         <v>1</v>
@@ -23236,7 +23326,7 @@
         <v>534</v>
       </c>
       <c r="B88" s="3" t="s">
-        <v>1067</v>
+        <v>1074</v>
       </c>
       <c r="C88" s="5" t="b">
         <v>1</v>
@@ -23292,7 +23382,7 @@
         <v>543</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>1067</v>
+        <v>1074</v>
       </c>
       <c r="C89" s="5" t="b">
         <v>1</v>
@@ -23348,7 +23438,7 @@
         <v>545</v>
       </c>
       <c r="B90" s="3" t="s">
-        <v>1067</v>
+        <v>1074</v>
       </c>
       <c r="C90" s="5" t="b">
         <v>1</v>
@@ -25476,7 +25566,7 @@
         <v>699</v>
       </c>
       <c r="B128" s="3" t="s">
-        <v>1067</v>
+        <v>1074</v>
       </c>
       <c r="C128" s="5" t="b">
         <v>1</v>
@@ -26036,7 +26126,7 @@
         <v>731</v>
       </c>
       <c r="B138" s="3" t="s">
-        <v>1067</v>
+        <v>1074</v>
       </c>
       <c r="C138" s="5" t="b">
         <v>1</v>
@@ -26092,7 +26182,7 @@
         <v>737</v>
       </c>
       <c r="B139" s="3" t="s">
-        <v>1067</v>
+        <v>1074</v>
       </c>
       <c r="C139" s="5" t="b">
         <v>1</v>
@@ -26260,7 +26350,7 @@
         <v>757</v>
       </c>
       <c r="B142" s="3" t="s">
-        <v>1067</v>
+        <v>1074</v>
       </c>
       <c r="C142" s="5" t="b">
         <v>1</v>
@@ -26316,7 +26406,7 @@
         <v>759</v>
       </c>
       <c r="B143" s="3" t="s">
-        <v>1067</v>
+        <v>1074</v>
       </c>
       <c r="C143" s="5" t="b">
         <v>1</v>
@@ -26372,7 +26462,7 @@
         <v>768</v>
       </c>
       <c r="B144" s="3" t="s">
-        <v>1067</v>
+        <v>1074</v>
       </c>
       <c r="C144" s="5" t="b">
         <v>1</v>
@@ -26428,7 +26518,7 @@
         <v>772</v>
       </c>
       <c r="B145" s="3" t="s">
-        <v>1067</v>
+        <v>1074</v>
       </c>
       <c r="C145" s="5" t="b">
         <v>1</v>
@@ -26484,7 +26574,7 @@
         <v>775</v>
       </c>
       <c r="B146" s="3" t="s">
-        <v>1067</v>
+        <v>1074</v>
       </c>
       <c r="C146" s="5" t="b">
         <v>1</v>
@@ -26540,7 +26630,7 @@
         <v>778</v>
       </c>
       <c r="B147" s="3" t="s">
-        <v>1067</v>
+        <v>1074</v>
       </c>
       <c r="C147" s="5" t="b">
         <v>1</v>
@@ -26596,7 +26686,7 @@
         <v>781</v>
       </c>
       <c r="B148" s="3" t="s">
-        <v>1067</v>
+        <v>1074</v>
       </c>
       <c r="C148" s="5" t="b">
         <v>1</v>
@@ -26652,7 +26742,7 @@
         <v>784</v>
       </c>
       <c r="B149" s="3" t="s">
-        <v>1067</v>
+        <v>1074</v>
       </c>
       <c r="C149" s="5" t="b">
         <v>1</v>
@@ -26708,7 +26798,7 @@
         <v>787</v>
       </c>
       <c r="B150" s="3" t="s">
-        <v>1067</v>
+        <v>1074</v>
       </c>
       <c r="C150" s="5" t="b">
         <v>1</v>
@@ -26764,7 +26854,7 @@
         <v>790</v>
       </c>
       <c r="B151" s="3" t="s">
-        <v>1067</v>
+        <v>1074</v>
       </c>
       <c r="C151" s="5" t="b">
         <v>1</v>
@@ -26820,7 +26910,7 @@
         <v>793</v>
       </c>
       <c r="B152" s="3" t="s">
-        <v>1067</v>
+        <v>1074</v>
       </c>
       <c r="C152" s="5" t="b">
         <v>1</v>
@@ -26876,7 +26966,7 @@
         <v>796</v>
       </c>
       <c r="B153" s="3" t="s">
-        <v>1067</v>
+        <v>1074</v>
       </c>
       <c r="C153" s="5" t="b">
         <v>1</v>
@@ -26932,7 +27022,7 @@
         <v>799</v>
       </c>
       <c r="B154" s="3" t="s">
-        <v>1067</v>
+        <v>1074</v>
       </c>
       <c r="C154" s="5" t="b">
         <v>1</v>
@@ -26988,7 +27078,7 @@
         <v>802</v>
       </c>
       <c r="B155" s="3" t="s">
-        <v>1067</v>
+        <v>1074</v>
       </c>
       <c r="C155" s="5" t="b">
         <v>1</v>
@@ -27044,7 +27134,7 @@
         <v>805</v>
       </c>
       <c r="B156" s="3" t="s">
-        <v>1067</v>
+        <v>1074</v>
       </c>
       <c r="C156" s="5" t="b">
         <v>1</v>
@@ -27100,7 +27190,7 @@
         <v>808</v>
       </c>
       <c r="B157" s="3" t="s">
-        <v>1067</v>
+        <v>1074</v>
       </c>
       <c r="C157" s="5" t="b">
         <v>1</v>
@@ -27156,7 +27246,7 @@
         <v>811</v>
       </c>
       <c r="B158" s="3" t="s">
-        <v>1067</v>
+        <v>1074</v>
       </c>
       <c r="C158" s="5" t="b">
         <v>1</v>
@@ -27212,7 +27302,7 @@
         <v>814</v>
       </c>
       <c r="B159" s="3" t="s">
-        <v>1067</v>
+        <v>1074</v>
       </c>
       <c r="C159" s="5" t="b">
         <v>1</v>
@@ -27268,7 +27358,7 @@
         <v>817</v>
       </c>
       <c r="B160" s="3" t="s">
-        <v>1067</v>
+        <v>1074</v>
       </c>
       <c r="C160" s="5" t="b">
         <v>1</v>
@@ -27324,7 +27414,7 @@
         <v>820</v>
       </c>
       <c r="B161" s="3" t="s">
-        <v>1067</v>
+        <v>1074</v>
       </c>
       <c r="C161" s="5" t="b">
         <v>1</v>
@@ -27380,7 +27470,7 @@
         <v>823</v>
       </c>
       <c r="B162" s="3" t="s">
-        <v>1067</v>
+        <v>1074</v>
       </c>
       <c r="C162" s="5" t="b">
         <v>1</v>
@@ -27436,7 +27526,7 @@
         <v>826</v>
       </c>
       <c r="B163" s="3" t="s">
-        <v>1067</v>
+        <v>1074</v>
       </c>
       <c r="C163" s="5" t="b">
         <v>1</v>
@@ -27492,7 +27582,7 @@
         <v>829</v>
       </c>
       <c r="B164" s="3" t="s">
-        <v>1067</v>
+        <v>1074</v>
       </c>
       <c r="C164" s="5" t="b">
         <v>1</v>
@@ -27548,7 +27638,7 @@
         <v>832</v>
       </c>
       <c r="B165" s="3" t="s">
-        <v>1067</v>
+        <v>1074</v>
       </c>
       <c r="C165" s="5" t="b">
         <v>1</v>
@@ -27604,7 +27694,7 @@
         <v>835</v>
       </c>
       <c r="B166" s="3" t="s">
-        <v>1067</v>
+        <v>1074</v>
       </c>
       <c r="C166" s="5" t="b">
         <v>1</v>
@@ -27660,7 +27750,7 @@
         <v>838</v>
       </c>
       <c r="B167" s="3" t="s">
-        <v>1067</v>
+        <v>1074</v>
       </c>
       <c r="C167" s="5" t="b">
         <v>1</v>
@@ -27716,7 +27806,7 @@
         <v>841</v>
       </c>
       <c r="B168" s="3" t="s">
-        <v>1067</v>
+        <v>1074</v>
       </c>
       <c r="C168" s="5" t="b">
         <v>1</v>
@@ -27772,7 +27862,7 @@
         <v>844</v>
       </c>
       <c r="B169" s="3" t="s">
-        <v>1067</v>
+        <v>1074</v>
       </c>
       <c r="C169" s="5" t="b">
         <v>1</v>
@@ -27828,7 +27918,7 @@
         <v>847</v>
       </c>
       <c r="B170" s="3" t="s">
-        <v>1067</v>
+        <v>1074</v>
       </c>
       <c r="C170" s="5" t="b">
         <v>1</v>
@@ -27884,7 +27974,7 @@
         <v>850</v>
       </c>
       <c r="B171" s="3" t="s">
-        <v>1067</v>
+        <v>1074</v>
       </c>
       <c r="C171" s="5" t="b">
         <v>1</v>
@@ -27940,7 +28030,7 @@
         <v>853</v>
       </c>
       <c r="B172" s="3" t="s">
-        <v>1067</v>
+        <v>1074</v>
       </c>
       <c r="C172" s="5" t="b">
         <v>1</v>
@@ -27996,7 +28086,7 @@
         <v>856</v>
       </c>
       <c r="B173" s="3" t="s">
-        <v>1067</v>
+        <v>1074</v>
       </c>
       <c r="C173" s="5" t="b">
         <v>1</v>
@@ -28052,7 +28142,7 @@
         <v>859</v>
       </c>
       <c r="B174" s="3" t="s">
-        <v>1067</v>
+        <v>1074</v>
       </c>
       <c r="C174" s="5" t="b">
         <v>1</v>
@@ -28108,7 +28198,7 @@
         <v>862</v>
       </c>
       <c r="B175" s="3" t="s">
-        <v>1067</v>
+        <v>1074</v>
       </c>
       <c r="C175" s="5" t="b">
         <v>1</v>
@@ -28164,7 +28254,7 @@
         <v>865</v>
       </c>
       <c r="B176" s="3" t="s">
-        <v>1067</v>
+        <v>1074</v>
       </c>
       <c r="C176" s="5" t="b">
         <v>1</v>
@@ -28220,7 +28310,7 @@
         <v>868</v>
       </c>
       <c r="B177" s="3" t="s">
-        <v>1067</v>
+        <v>1074</v>
       </c>
       <c r="C177" s="5" t="b">
         <v>1</v>
@@ -28276,7 +28366,7 @@
         <v>871</v>
       </c>
       <c r="B178" s="3" t="s">
-        <v>1067</v>
+        <v>1074</v>
       </c>
       <c r="C178" s="5" t="b">
         <v>1</v>
@@ -28332,7 +28422,7 @@
         <v>873</v>
       </c>
       <c r="B179" s="3" t="s">
-        <v>1067</v>
+        <v>1074</v>
       </c>
       <c r="C179" s="5" t="b">
         <v>1</v>
@@ -28388,7 +28478,7 @@
         <v>876</v>
       </c>
       <c r="B180" s="3" t="s">
-        <v>1067</v>
+        <v>1074</v>
       </c>
       <c r="C180" s="5" t="b">
         <v>1</v>
@@ -28444,7 +28534,7 @@
         <v>878</v>
       </c>
       <c r="B181" s="3" t="s">
-        <v>1067</v>
+        <v>1074</v>
       </c>
       <c r="C181" s="5" t="b">
         <v>1</v>
@@ -28500,7 +28590,7 @@
         <v>880</v>
       </c>
       <c r="B182" s="3" t="s">
-        <v>1067</v>
+        <v>1074</v>
       </c>
       <c r="C182" s="5" t="b">
         <v>1</v>
@@ -28556,7 +28646,7 @@
         <v>882</v>
       </c>
       <c r="B183" s="3" t="s">
-        <v>1067</v>
+        <v>1074</v>
       </c>
       <c r="C183" s="5" t="b">
         <v>1</v>
@@ -28612,7 +28702,7 @@
         <v>885</v>
       </c>
       <c r="B184" s="3" t="s">
-        <v>1067</v>
+        <v>1074</v>
       </c>
       <c r="C184" s="5" t="b">
         <v>1</v>
@@ -28668,7 +28758,7 @@
         <v>891</v>
       </c>
       <c r="B185" s="3" t="s">
-        <v>1067</v>
+        <v>1074</v>
       </c>
       <c r="C185" s="5" t="b">
         <v>1</v>
@@ -28676,11 +28766,11 @@
       <c r="D185" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="E185" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="F185" s="6" t="b">
-        <v>0</v>
+      <c r="E185" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="F185" s="5" t="b">
+        <v>1</v>
       </c>
       <c r="G185" s="5" t="b">
         <v>1</v>
@@ -28688,14 +28778,14 @@
       <c r="H185" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="I185" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="J185" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="K185" s="6" t="b">
-        <v>0</v>
+      <c r="I185" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="J185" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="K185" s="5" t="b">
+        <v>1</v>
       </c>
       <c r="L185" s="5" t="b">
         <v>1</v>
@@ -28721,10 +28811,10 @@
     </row>
     <row r="186" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A186" s="3" t="s">
-        <v>897</v>
+        <v>902</v>
       </c>
       <c r="B186" s="3" t="s">
-        <v>898</v>
+        <v>1074</v>
       </c>
       <c r="C186" s="5" t="b">
         <v>1</v>
@@ -28768,19 +28858,19 @@
       <c r="P186" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="Q186" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="R186" s="5" t="b">
-        <v>1</v>
+      <c r="Q186" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="R186" s="6" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="187" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A187" s="3" t="s">
-        <v>909</v>
+        <v>904</v>
       </c>
       <c r="B187" s="3" t="s">
-        <v>1067</v>
+        <v>905</v>
       </c>
       <c r="C187" s="5" t="b">
         <v>1</v>
@@ -28788,8 +28878,8 @@
       <c r="D187" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="E187" s="6" t="b">
-        <v>0</v>
+      <c r="E187" s="5" t="b">
+        <v>1</v>
       </c>
       <c r="F187" s="5" t="b">
         <v>1</v>
@@ -28803,8 +28893,8 @@
       <c r="I187" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="J187" s="6" t="b">
-        <v>0</v>
+      <c r="J187" s="5" t="b">
+        <v>1</v>
       </c>
       <c r="K187" s="5" t="b">
         <v>1</v>
@@ -28824,19 +28914,19 @@
       <c r="P187" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="Q187" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="R187" s="6" t="b">
-        <v>0</v>
+      <c r="Q187" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="R187" s="5" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="188" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A188" s="3" t="s">
-        <v>918</v>
+        <v>916</v>
       </c>
       <c r="B188" s="3" t="s">
-        <v>1067</v>
+        <v>1074</v>
       </c>
       <c r="C188" s="5" t="b">
         <v>1</v>
@@ -28844,8 +28934,8 @@
       <c r="D188" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="E188" s="5" t="b">
-        <v>1</v>
+      <c r="E188" s="6" t="b">
+        <v>0</v>
       </c>
       <c r="F188" s="5" t="b">
         <v>1</v>
@@ -28859,11 +28949,11 @@
       <c r="I188" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="J188" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="K188" s="6" t="b">
-        <v>0</v>
+      <c r="J188" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="K188" s="5" t="b">
+        <v>1</v>
       </c>
       <c r="L188" s="5" t="b">
         <v>1</v>
@@ -28889,10 +28979,10 @@
     </row>
     <row r="189" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A189" s="3" t="s">
-        <v>928</v>
+        <v>925</v>
       </c>
       <c r="B189" s="3" t="s">
-        <v>929</v>
+        <v>1074</v>
       </c>
       <c r="C189" s="5" t="b">
         <v>1</v>
@@ -28918,11 +29008,11 @@
       <c r="J189" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="K189" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="L189" s="6" t="b">
-        <v>0</v>
+      <c r="K189" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="L189" s="5" t="b">
+        <v>1</v>
       </c>
       <c r="M189" s="5" t="b">
         <v>1</v>
@@ -28945,10 +29035,10 @@
     </row>
     <row r="190" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A190" s="3" t="s">
-        <v>938</v>
+        <v>935</v>
       </c>
       <c r="B190" s="3" t="s">
-        <v>1067</v>
+        <v>936</v>
       </c>
       <c r="C190" s="5" t="b">
         <v>1</v>
@@ -28977,8 +29067,8 @@
       <c r="K190" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="L190" s="5" t="b">
-        <v>1</v>
+      <c r="L190" s="6" t="b">
+        <v>0</v>
       </c>
       <c r="M190" s="5" t="b">
         <v>1</v>
@@ -28992,19 +29082,19 @@
       <c r="P190" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="Q190" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="R190" s="5" t="b">
-        <v>1</v>
+      <c r="Q190" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="R190" s="6" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="191" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A191" s="3" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="B191" s="3" t="s">
-        <v>1067</v>
+        <v>1074</v>
       </c>
       <c r="C191" s="5" t="b">
         <v>1</v>
@@ -29057,10 +29147,10 @@
     </row>
     <row r="192" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A192" s="3" t="s">
-        <v>948</v>
+        <v>953</v>
       </c>
       <c r="B192" s="3" t="s">
-        <v>1067</v>
+        <v>1074</v>
       </c>
       <c r="C192" s="5" t="b">
         <v>1</v>
@@ -29083,8 +29173,8 @@
       <c r="I192" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="J192" s="6" t="b">
-        <v>0</v>
+      <c r="J192" s="5" t="b">
+        <v>1</v>
       </c>
       <c r="K192" s="5" t="b">
         <v>1</v>
@@ -29095,17 +29185,17 @@
       <c r="M192" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="N192" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="O192" s="6" t="b">
-        <v>0</v>
+      <c r="N192" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="O192" s="5" t="b">
+        <v>1</v>
       </c>
       <c r="P192" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="Q192" s="6" t="b">
-        <v>0</v>
+      <c r="Q192" s="5" t="b">
+        <v>1</v>
       </c>
       <c r="R192" s="5" t="b">
         <v>1</v>
@@ -29116,7 +29206,7 @@
         <v>955</v>
       </c>
       <c r="B193" s="3" t="s">
-        <v>1067</v>
+        <v>1074</v>
       </c>
       <c r="C193" s="5" t="b">
         <v>1</v>
@@ -29169,10 +29259,10 @@
     </row>
     <row r="194" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A194" s="3" t="s">
-        <v>957</v>
+        <v>962</v>
       </c>
       <c r="B194" s="3" t="s">
-        <v>1067</v>
+        <v>1074</v>
       </c>
       <c r="C194" s="5" t="b">
         <v>1</v>
@@ -29183,8 +29273,8 @@
       <c r="E194" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="F194" s="6" t="b">
-        <v>0</v>
+      <c r="F194" s="5" t="b">
+        <v>1</v>
       </c>
       <c r="G194" s="5" t="b">
         <v>1</v>
@@ -29207,28 +29297,28 @@
       <c r="M194" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="N194" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="O194" s="5" t="b">
-        <v>1</v>
+      <c r="N194" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="O194" s="6" t="b">
+        <v>0</v>
       </c>
       <c r="P194" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="Q194" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="R194" s="6" t="b">
-        <v>0</v>
+      <c r="Q194" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="R194" s="5" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="195" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A195" s="3" t="s">
-        <v>967</v>
+        <v>964</v>
       </c>
       <c r="B195" s="3" t="s">
-        <v>1067</v>
+        <v>1074</v>
       </c>
       <c r="C195" s="5" t="b">
         <v>1</v>
@@ -29236,8 +29326,8 @@
       <c r="D195" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="E195" s="6" t="b">
-        <v>0</v>
+      <c r="E195" s="5" t="b">
+        <v>1</v>
       </c>
       <c r="F195" s="6" t="b">
         <v>0</v>
@@ -29263,17 +29353,17 @@
       <c r="M195" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="N195" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="O195" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="P195" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="Q195" s="6" t="b">
-        <v>0</v>
+      <c r="N195" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="O195" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="P195" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q195" s="5" t="b">
+        <v>1</v>
       </c>
       <c r="R195" s="6" t="b">
         <v>0</v>
@@ -29281,10 +29371,10 @@
     </row>
     <row r="196" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A196" s="3" t="s">
-        <v>973</v>
+        <v>974</v>
       </c>
       <c r="B196" s="3" t="s">
-        <v>1067</v>
+        <v>1074</v>
       </c>
       <c r="C196" s="5" t="b">
         <v>1</v>
@@ -29337,10 +29427,10 @@
     </row>
     <row r="197" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A197" s="3" t="s">
-        <v>976</v>
+        <v>980</v>
       </c>
       <c r="B197" s="3" t="s">
-        <v>1067</v>
+        <v>1074</v>
       </c>
       <c r="C197" s="5" t="b">
         <v>1</v>
@@ -29348,11 +29438,11 @@
       <c r="D197" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="E197" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="F197" s="5" t="b">
-        <v>1</v>
+      <c r="E197" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="F197" s="6" t="b">
+        <v>0</v>
       </c>
       <c r="G197" s="5" t="b">
         <v>1</v>
@@ -29375,11 +29465,11 @@
       <c r="M197" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="N197" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="O197" s="5" t="b">
-        <v>1</v>
+      <c r="N197" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="O197" s="6" t="b">
+        <v>0</v>
       </c>
       <c r="P197" s="6" t="b">
         <v>0</v>
@@ -29387,16 +29477,16 @@
       <c r="Q197" s="6" t="b">
         <v>0</v>
       </c>
-      <c r="R197" s="5" t="b">
-        <v>1</v>
+      <c r="R197" s="6" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="198" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A198" s="3" t="s">
-        <v>984</v>
+        <v>983</v>
       </c>
       <c r="B198" s="3" t="s">
-        <v>1067</v>
+        <v>1074</v>
       </c>
       <c r="C198" s="5" t="b">
         <v>1</v>
@@ -29449,10 +29539,10 @@
     </row>
     <row r="199" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A199" s="3" t="s">
-        <v>988</v>
+        <v>991</v>
       </c>
       <c r="B199" s="3" t="s">
-        <v>1067</v>
+        <v>1074</v>
       </c>
       <c r="C199" s="5" t="b">
         <v>1</v>
@@ -29493,22 +29583,22 @@
       <c r="O199" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="P199" s="5" t="b">
-        <v>1</v>
+      <c r="P199" s="6" t="b">
+        <v>0</v>
       </c>
       <c r="Q199" s="6" t="b">
         <v>0</v>
       </c>
-      <c r="R199" s="6" t="b">
-        <v>0</v>
+      <c r="R199" s="5" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="200" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A200" s="3" t="s">
-        <v>998</v>
+        <v>995</v>
       </c>
       <c r="B200" s="3" t="s">
-        <v>1067</v>
+        <v>1074</v>
       </c>
       <c r="C200" s="5" t="b">
         <v>1</v>
@@ -29552,8 +29642,8 @@
       <c r="P200" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="Q200" s="5" t="b">
-        <v>1</v>
+      <c r="Q200" s="6" t="b">
+        <v>0</v>
       </c>
       <c r="R200" s="6" t="b">
         <v>0</v>
@@ -29561,10 +29651,10 @@
     </row>
     <row r="201" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A201" s="3" t="s">
-        <v>1004</v>
+        <v>1005</v>
       </c>
       <c r="B201" s="3" t="s">
-        <v>1067</v>
+        <v>1074</v>
       </c>
       <c r="C201" s="5" t="b">
         <v>1</v>
@@ -29617,10 +29707,10 @@
     </row>
     <row r="202" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A202" s="3" t="s">
-        <v>1007</v>
+        <v>1011</v>
       </c>
       <c r="B202" s="3" t="s">
-        <v>1067</v>
+        <v>1074</v>
       </c>
       <c r="C202" s="5" t="b">
         <v>1</v>
@@ -29628,8 +29718,8 @@
       <c r="D202" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="E202" s="6" t="b">
-        <v>0</v>
+      <c r="E202" s="5" t="b">
+        <v>1</v>
       </c>
       <c r="F202" s="5" t="b">
         <v>1</v>
@@ -29637,8 +29727,8 @@
       <c r="G202" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="H202" s="6" t="b">
-        <v>0</v>
+      <c r="H202" s="5" t="b">
+        <v>1</v>
       </c>
       <c r="I202" s="5" t="b">
         <v>1</v>
@@ -29646,26 +29736,26 @@
       <c r="J202" s="6" t="b">
         <v>0</v>
       </c>
-      <c r="K202" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="L202" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="M202" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="N202" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="O202" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="P202" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="Q202" s="6" t="b">
-        <v>0</v>
+      <c r="K202" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="L202" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="M202" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="N202" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="O202" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="P202" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q202" s="5" t="b">
+        <v>1</v>
       </c>
       <c r="R202" s="6" t="b">
         <v>0</v>
@@ -29673,10 +29763,10 @@
     </row>
     <row r="203" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A203" s="3" t="s">
-        <v>1010</v>
+        <v>1014</v>
       </c>
       <c r="B203" s="3" t="s">
-        <v>1067</v>
+        <v>1074</v>
       </c>
       <c r="C203" s="5" t="b">
         <v>1</v>
@@ -29693,8 +29783,8 @@
       <c r="G203" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="H203" s="5" t="b">
-        <v>1</v>
+      <c r="H203" s="6" t="b">
+        <v>0</v>
       </c>
       <c r="I203" s="5" t="b">
         <v>1</v>
@@ -29702,17 +29792,17 @@
       <c r="J203" s="6" t="b">
         <v>0</v>
       </c>
-      <c r="K203" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="L203" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="M203" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="N203" s="5" t="b">
-        <v>1</v>
+      <c r="K203" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="L203" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="M203" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="N203" s="6" t="b">
+        <v>0</v>
       </c>
       <c r="O203" s="6" t="b">
         <v>0</v>
@@ -29732,7 +29822,7 @@
         <v>1017</v>
       </c>
       <c r="B204" s="3" t="s">
-        <v>1067</v>
+        <v>1074</v>
       </c>
       <c r="C204" s="5" t="b">
         <v>1</v>
@@ -29743,20 +29833,20 @@
       <c r="E204" s="6" t="b">
         <v>0</v>
       </c>
-      <c r="F204" s="6" t="b">
-        <v>0</v>
+      <c r="F204" s="5" t="b">
+        <v>1</v>
       </c>
       <c r="G204" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="H204" s="6" t="b">
-        <v>0</v>
+      <c r="H204" s="5" t="b">
+        <v>1</v>
       </c>
       <c r="I204" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="J204" s="5" t="b">
-        <v>1</v>
+      <c r="J204" s="6" t="b">
+        <v>0</v>
       </c>
       <c r="K204" s="5" t="b">
         <v>1</v>
@@ -29770,8 +29860,8 @@
       <c r="N204" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="O204" s="5" t="b">
-        <v>1</v>
+      <c r="O204" s="6" t="b">
+        <v>0</v>
       </c>
       <c r="P204" s="6" t="b">
         <v>0</v>
@@ -29788,7 +29878,7 @@
         <v>1024</v>
       </c>
       <c r="B205" s="3" t="s">
-        <v>1067</v>
+        <v>1074</v>
       </c>
       <c r="C205" s="5" t="b">
         <v>1</v>
@@ -29796,23 +29886,23 @@
       <c r="D205" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="E205" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="F205" s="5" t="b">
-        <v>1</v>
+      <c r="E205" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="F205" s="6" t="b">
+        <v>0</v>
       </c>
       <c r="G205" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="H205" s="5" t="b">
-        <v>1</v>
+      <c r="H205" s="6" t="b">
+        <v>0</v>
       </c>
       <c r="I205" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="J205" s="6" t="b">
-        <v>0</v>
+      <c r="J205" s="5" t="b">
+        <v>1</v>
       </c>
       <c r="K205" s="5" t="b">
         <v>1</v>
@@ -29829,8 +29919,8 @@
       <c r="O205" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="P205" s="5" t="b">
-        <v>1</v>
+      <c r="P205" s="6" t="b">
+        <v>0</v>
       </c>
       <c r="Q205" s="6" t="b">
         <v>0</v>
@@ -29841,10 +29931,10 @@
     </row>
     <row r="206" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A206" s="3" t="s">
-        <v>1030</v>
+        <v>1031</v>
       </c>
       <c r="B206" s="3" t="s">
-        <v>1067</v>
+        <v>1074</v>
       </c>
       <c r="C206" s="5" t="b">
         <v>1</v>
@@ -29897,10 +29987,10 @@
     </row>
     <row r="207" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A207" s="3" t="s">
-        <v>1032</v>
+        <v>1037</v>
       </c>
       <c r="B207" s="3" t="s">
-        <v>1067</v>
+        <v>1074</v>
       </c>
       <c r="C207" s="5" t="b">
         <v>1</v>
@@ -29923,8 +30013,8 @@
       <c r="I207" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="J207" s="5" t="b">
-        <v>1</v>
+      <c r="J207" s="6" t="b">
+        <v>0</v>
       </c>
       <c r="K207" s="5" t="b">
         <v>1</v>
@@ -29944,8 +30034,8 @@
       <c r="P207" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="Q207" s="5" t="b">
-        <v>1</v>
+      <c r="Q207" s="6" t="b">
+        <v>0</v>
       </c>
       <c r="R207" s="6" t="b">
         <v>0</v>
@@ -29953,10 +30043,10 @@
     </row>
     <row r="208" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A208" s="3" t="s">
-        <v>1043</v>
+        <v>1039</v>
       </c>
       <c r="B208" s="3" t="s">
-        <v>1067</v>
+        <v>1074</v>
       </c>
       <c r="C208" s="5" t="b">
         <v>1</v>
@@ -30009,10 +30099,10 @@
     </row>
     <row r="209" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A209" s="3" t="s">
-        <v>1045</v>
+        <v>1050</v>
       </c>
       <c r="B209" s="3" t="s">
-        <v>1067</v>
+        <v>1074</v>
       </c>
       <c r="C209" s="5" t="b">
         <v>1</v>
@@ -30035,8 +30125,8 @@
       <c r="I209" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="J209" s="6" t="b">
-        <v>0</v>
+      <c r="J209" s="5" t="b">
+        <v>1</v>
       </c>
       <c r="K209" s="5" t="b">
         <v>1</v>
@@ -30053,11 +30143,11 @@
       <c r="O209" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="P209" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="Q209" s="6" t="b">
-        <v>0</v>
+      <c r="P209" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q209" s="5" t="b">
+        <v>1</v>
       </c>
       <c r="R209" s="6" t="b">
         <v>0</v>
@@ -30065,10 +30155,10 @@
     </row>
     <row r="210" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A210" s="3" t="s">
-        <v>1051</v>
+        <v>1052</v>
       </c>
       <c r="B210" s="3" t="s">
-        <v>1067</v>
+        <v>1074</v>
       </c>
       <c r="C210" s="5" t="b">
         <v>1</v>
@@ -30121,10 +30211,10 @@
     </row>
     <row r="211" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A211" s="3" t="s">
-        <v>1053</v>
+        <v>1058</v>
       </c>
       <c r="B211" s="3" t="s">
-        <v>1067</v>
+        <v>1074</v>
       </c>
       <c r="C211" s="5" t="b">
         <v>1</v>
@@ -30147,8 +30237,8 @@
       <c r="I211" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="J211" s="5" t="b">
-        <v>1</v>
+      <c r="J211" s="6" t="b">
+        <v>0</v>
       </c>
       <c r="K211" s="5" t="b">
         <v>1</v>
@@ -30165,8 +30255,8 @@
       <c r="O211" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="P211" s="5" t="b">
-        <v>1</v>
+      <c r="P211" s="6" t="b">
+        <v>0</v>
       </c>
       <c r="Q211" s="6" t="b">
         <v>0</v>
@@ -30177,10 +30267,10 @@
     </row>
     <row r="212" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A212" s="3" t="s">
-        <v>1065</v>
+        <v>1060</v>
       </c>
       <c r="B212" s="3" t="s">
-        <v>1067</v>
+        <v>1074</v>
       </c>
       <c r="C212" s="5" t="b">
         <v>1</v>
@@ -30228,6 +30318,62 @@
         <v>0</v>
       </c>
       <c r="R212" s="6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="213" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A213" s="3" t="s">
+        <v>1072</v>
+      </c>
+      <c r="B213" s="3" t="s">
+        <v>1074</v>
+      </c>
+      <c r="C213" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="D213" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="E213" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="F213" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="G213" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="H213" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="I213" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="J213" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="K213" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="L213" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="M213" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="N213" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="O213" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="P213" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q213" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="R213" s="6" t="b">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
generated all the reports on 2024-02-28
</commit_message>
<xml_diff>
--- a/report/merged_configurations.xlsx
+++ b/report/merged_configurations.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4985" uniqueCount="1075">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4987" uniqueCount="1075">
   <si>
     <t>naam</t>
   </si>
@@ -176,10 +176,13 @@
     <t>Applicatieprofiel Slim Ruimtelijk Plannen</t>
   </si>
   <si>
+    <t>Aanbevolen (vrijwillig)</t>
+  </si>
+  <si>
     <t>slim-ruimtelijk-plannen-description.md</t>
   </si>
   <si>
-    <t>[{"naam":"Slim Ruimtelijk Plannen applicatieprofiel","waarde":"https://data.test-vlaanderen.be/doc/applicatieprofiel/slim-ruimtelijk-plannen/ontwerpstandaard/2024-01-22/"}]</t>
+    <t>[{"naam":"Slim Ruimtelijk Plannen applicatieprofiel","waarde":"https://data.vlaanderen.be/doc/applicatieprofiel/slim-ruimtelijk-plannen/ontwerpstandaard/2024-01-22/"}]</t>
   </si>
   <si>
     <t>[{"naam":"Projectcharter","waarde":"Werkgroep-charter-OSLO_SlimRuimtelijkPlannen.docx"}]</t>
@@ -197,13 +200,10 @@
     <t>Vocabularium Slim Ruimtelijk Plannen</t>
   </si>
   <si>
-    <t>[{"naam":"Slim Ruimtelijk Plannen vocabularium","waarde":"https://data.test-vlaanderen.be/doc/vocabularium/slim-ruimtelijk-plannen/ontwerpstandaard/2024-01-22"}]</t>
+    <t>[{"naam":"Slim Ruimtelijk Plannen vocabularium","waarde":"https://data.vlaanderen.be/doc/vocabularium/slim-ruimtelijk-plannen/ontwerpstandaard/2024-01-22"}]</t>
   </si>
   <si>
     <t>OSLO Voorwaarden Dienstverlening</t>
-  </si>
-  <si>
-    <t>Aanbevolen (vrijwillig)</t>
   </si>
   <si>
     <t>template-description.md</t>
@@ -4007,30 +4007,32 @@
       <c r="E6" s="4">
         <v>45222</v>
       </c>
-      <c r="F6" s="3"/>
+      <c r="F6" s="3" t="s">
+        <v>54</v>
+      </c>
       <c r="G6" s="3" t="s">
         <v>27</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="J6" s="3" t="s">
         <v>30</v>
       </c>
       <c r="K6" s="3" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="L6" s="3" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="M6" s="3" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="N6" s="3" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="O6" s="3" t="s">
         <v>49</v>
@@ -4056,7 +4058,7 @@
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B7" s="3"/>
       <c r="C7" s="3" t="s">
@@ -4068,30 +4070,32 @@
       <c r="E7" s="4">
         <v>45222</v>
       </c>
-      <c r="F7" s="3"/>
+      <c r="F7" s="3" t="s">
+        <v>54</v>
+      </c>
       <c r="G7" s="3" t="s">
         <v>39</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="J7" s="3" t="s">
         <v>30</v>
       </c>
       <c r="K7" s="3" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="L7" s="3" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="M7" s="3" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="N7" s="3" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="O7" s="3" t="s">
         <v>49</v>
@@ -4117,7 +4121,7 @@
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B8" s="3"/>
       <c r="C8" s="3" t="s">
@@ -4130,7 +4134,7 @@
         <v>45118</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="G8" s="3" t="s">
         <v>27</v>
@@ -4197,7 +4201,7 @@
       </c>
       <c r="E9" s="3"/>
       <c r="F9" s="3" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="G9" s="3" t="s">
         <v>27</v>
@@ -4260,7 +4264,7 @@
       </c>
       <c r="E10" s="3"/>
       <c r="F10" s="3" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="G10" s="3" t="s">
         <v>39</v>
@@ -4325,7 +4329,7 @@
         <v>82</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="G11" s="3" t="s">
         <v>27</v>
@@ -4390,7 +4394,7 @@
         <v>82</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="G12" s="3" t="s">
         <v>91</v>
@@ -4457,7 +4461,7 @@
         <v>101</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="G13" s="3" t="s">
         <v>102</v>
@@ -4522,7 +4526,7 @@
         <v>101</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="G14" s="3" t="s">
         <v>112</v>
@@ -5965,7 +5969,7 @@
         <v>44679</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="G35" s="3" t="s">
         <v>165</v>
@@ -6036,7 +6040,7 @@
         <v>44455</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="G36" s="3" t="s">
         <v>39</v>
@@ -6107,7 +6111,7 @@
         <v>44455</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="G37" s="3" t="s">
         <v>27</v>
@@ -6600,7 +6604,7 @@
         <v>43284</v>
       </c>
       <c r="F44" s="3" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="G44" s="3" t="s">
         <v>39</v>
@@ -6742,7 +6746,7 @@
         <v>43431</v>
       </c>
       <c r="F46" s="3" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="G46" s="3" t="s">
         <v>39</v>
@@ -6884,7 +6888,7 @@
         <v>43503</v>
       </c>
       <c r="F48" s="3" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="G48" s="3" t="s">
         <v>27</v>
@@ -6955,7 +6959,7 @@
         <v>43503</v>
       </c>
       <c r="F49" s="3" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="G49" s="3" t="s">
         <v>39</v>
@@ -7026,7 +7030,7 @@
         <v>43284</v>
       </c>
       <c r="F50" s="3" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="G50" s="3" t="s">
         <v>39</v>
@@ -7097,7 +7101,7 @@
         <v>36</v>
       </c>
       <c r="F51" s="3" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="G51" s="3" t="s">
         <v>27</v>
@@ -7168,7 +7172,7 @@
         <v>43503</v>
       </c>
       <c r="F52" s="3" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="G52" s="3" t="s">
         <v>27</v>
@@ -7239,7 +7243,7 @@
         <v>43284</v>
       </c>
       <c r="F53" s="3" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="G53" s="3" t="s">
         <v>39</v>
@@ -7381,7 +7385,7 @@
         <v>43804</v>
       </c>
       <c r="F55" s="3" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="G55" s="3" t="s">
         <v>27</v>
@@ -7452,7 +7456,7 @@
         <v>43804</v>
       </c>
       <c r="F56" s="3" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="G56" s="3" t="s">
         <v>39</v>
@@ -7523,7 +7527,7 @@
         <v>36</v>
       </c>
       <c r="F57" s="3" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="G57" s="3" t="s">
         <v>27</v>
@@ -7594,7 +7598,7 @@
         <v>43284</v>
       </c>
       <c r="F58" s="3" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="G58" s="3" t="s">
         <v>39</v>
@@ -7665,7 +7669,7 @@
         <v>43412</v>
       </c>
       <c r="F59" s="3" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="G59" s="3" t="s">
         <v>27</v>
@@ -7736,7 +7740,7 @@
         <v>43412</v>
       </c>
       <c r="F60" s="3" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="G60" s="3" t="s">
         <v>39</v>
@@ -7878,7 +7882,7 @@
         <v>43503</v>
       </c>
       <c r="F62" s="3" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="G62" s="3" t="s">
         <v>27</v>
@@ -7949,7 +7953,7 @@
         <v>43503</v>
       </c>
       <c r="F63" s="3" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="G63" s="3" t="s">
         <v>39</v>
@@ -8020,7 +8024,7 @@
         <v>43503</v>
       </c>
       <c r="F64" s="3" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="G64" s="3" t="s">
         <v>39</v>
@@ -8091,7 +8095,7 @@
         <v>43503</v>
       </c>
       <c r="F65" s="3" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="G65" s="3" t="s">
         <v>27</v>
@@ -8162,7 +8166,7 @@
         <v>43503</v>
       </c>
       <c r="F66" s="3" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="G66" s="3" t="s">
         <v>27</v>
@@ -8231,7 +8235,7 @@
         <v>45194</v>
       </c>
       <c r="F67" s="3" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="G67" s="3" t="s">
         <v>27</v>
@@ -8300,7 +8304,7 @@
         <v>45194</v>
       </c>
       <c r="F68" s="3" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="G68" s="3" t="s">
         <v>39</v>
@@ -8513,7 +8517,7 @@
         <v>43944</v>
       </c>
       <c r="F71" s="3" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="G71" s="3" t="s">
         <v>27</v>
@@ -8584,7 +8588,7 @@
         <v>43944</v>
       </c>
       <c r="F72" s="3" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="G72" s="3" t="s">
         <v>39</v>
@@ -8655,7 +8659,7 @@
         <v>43944</v>
       </c>
       <c r="F73" s="3" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="G73" s="3" t="s">
         <v>39</v>
@@ -8726,7 +8730,7 @@
         <v>43944</v>
       </c>
       <c r="F74" s="3" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="G74" s="3" t="s">
         <v>39</v>
@@ -8797,7 +8801,7 @@
         <v>44532</v>
       </c>
       <c r="F75" s="3" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="G75" s="3" t="s">
         <v>27</v>
@@ -8866,7 +8870,7 @@
         <v>43503</v>
       </c>
       <c r="F76" s="3" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="G76" s="3" t="s">
         <v>454</v>
@@ -8937,7 +8941,7 @@
         <v>43503</v>
       </c>
       <c r="F77" s="3" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="G77" s="3" t="s">
         <v>39</v>
@@ -9008,7 +9012,7 @@
         <v>43503</v>
       </c>
       <c r="F78" s="3" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="G78" s="3" t="s">
         <v>27</v>
@@ -9079,7 +9083,7 @@
         <v>44000</v>
       </c>
       <c r="F79" s="3" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="G79" s="3" t="s">
         <v>39</v>
@@ -9150,7 +9154,7 @@
         <v>44000</v>
       </c>
       <c r="F80" s="3" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="G80" s="3" t="s">
         <v>27</v>
@@ -9221,7 +9225,7 @@
         <v>44000</v>
       </c>
       <c r="F81" s="3" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="G81" s="3" t="s">
         <v>39</v>
@@ -9292,7 +9296,7 @@
         <v>44000</v>
       </c>
       <c r="F82" s="3" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="G82" s="3" t="s">
         <v>27</v>
@@ -9363,7 +9367,7 @@
         <v>43301</v>
       </c>
       <c r="F83" s="3" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="G83" s="3" t="s">
         <v>39</v>
@@ -9505,7 +9509,7 @@
         <v>43301</v>
       </c>
       <c r="F85" s="3" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="G85" s="3" t="s">
         <v>39</v>
@@ -9854,7 +9858,7 @@
         <v>43242</v>
       </c>
       <c r="F90" s="3" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="G90" s="3" t="s">
         <v>454</v>
@@ -9925,7 +9929,7 @@
         <v>43431</v>
       </c>
       <c r="F91" s="3" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="G91" s="3" t="s">
         <v>39</v>
@@ -9996,7 +10000,7 @@
         <v>43431</v>
       </c>
       <c r="F92" s="3" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="G92" s="3" t="s">
         <v>39</v>
@@ -10067,7 +10071,7 @@
         <v>43431</v>
       </c>
       <c r="F93" s="3" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="G93" s="3" t="s">
         <v>39</v>
@@ -10138,7 +10142,7 @@
         <v>43431</v>
       </c>
       <c r="F94" s="3" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="G94" s="3" t="s">
         <v>39</v>
@@ -10209,7 +10213,7 @@
         <v>43431</v>
       </c>
       <c r="F95" s="3" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="G95" s="3" t="s">
         <v>39</v>
@@ -10280,7 +10284,7 @@
         <v>43431</v>
       </c>
       <c r="F96" s="3" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="G96" s="3" t="s">
         <v>39</v>
@@ -10351,7 +10355,7 @@
         <v>43431</v>
       </c>
       <c r="F97" s="3" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="G97" s="3" t="s">
         <v>39</v>
@@ -10422,7 +10426,7 @@
         <v>43431</v>
       </c>
       <c r="F98" s="3" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="G98" s="3" t="s">
         <v>27</v>
@@ -10493,7 +10497,7 @@
         <v>43431</v>
       </c>
       <c r="F99" s="3" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="G99" s="3" t="s">
         <v>27</v>
@@ -10564,7 +10568,7 @@
         <v>43431</v>
       </c>
       <c r="F100" s="3" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="G100" s="3" t="s">
         <v>27</v>
@@ -10635,7 +10639,7 @@
         <v>43431</v>
       </c>
       <c r="F101" s="3" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="G101" s="3" t="s">
         <v>27</v>
@@ -10706,7 +10710,7 @@
         <v>43431</v>
       </c>
       <c r="F102" s="3" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="G102" s="3" t="s">
         <v>27</v>
@@ -10777,7 +10781,7 @@
         <v>43431</v>
       </c>
       <c r="F103" s="3" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="G103" s="3" t="s">
         <v>27</v>
@@ -10848,7 +10852,7 @@
         <v>43431</v>
       </c>
       <c r="F104" s="3" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="G104" s="3" t="s">
         <v>27</v>
@@ -10919,7 +10923,7 @@
         <v>43431</v>
       </c>
       <c r="F105" s="3" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="G105" s="3" t="s">
         <v>27</v>
@@ -10990,7 +10994,7 @@
         <v>43431</v>
       </c>
       <c r="F106" s="3" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="G106" s="3" t="s">
         <v>27</v>
@@ -11132,7 +11136,7 @@
         <v>44231</v>
       </c>
       <c r="F108" s="3" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="G108" s="3" t="s">
         <v>27</v>
@@ -11203,7 +11207,7 @@
         <v>44231</v>
       </c>
       <c r="F109" s="3" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="G109" s="3" t="s">
         <v>39</v>
@@ -11416,7 +11420,7 @@
         <v>44308</v>
       </c>
       <c r="F112" s="3" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="G112" s="3" t="s">
         <v>39</v>
@@ -11629,7 +11633,7 @@
         <v>42817</v>
       </c>
       <c r="F115" s="3" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="G115" s="3" t="s">
         <v>27</v>
@@ -11694,7 +11698,7 @@
         <v>42825</v>
       </c>
       <c r="F116" s="3" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="G116" s="3" t="s">
         <v>39</v>
@@ -11763,7 +11767,7 @@
         <v>659</v>
       </c>
       <c r="F117" s="3" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="G117" s="3" t="s">
         <v>27</v>
@@ -11834,7 +11838,7 @@
         <v>659</v>
       </c>
       <c r="F118" s="3" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="G118" s="3" t="s">
         <v>27</v>
@@ -11905,7 +11909,7 @@
         <v>659</v>
       </c>
       <c r="F119" s="3" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="G119" s="3" t="s">
         <v>27</v>
@@ -11976,7 +11980,7 @@
         <v>659</v>
       </c>
       <c r="F120" s="3" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="G120" s="3" t="s">
         <v>27</v>
@@ -12047,7 +12051,7 @@
         <v>659</v>
       </c>
       <c r="F121" s="3" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="G121" s="3" t="s">
         <v>27</v>
@@ -12118,7 +12122,7 @@
         <v>659</v>
       </c>
       <c r="F122" s="3" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="G122" s="3" t="s">
         <v>27</v>
@@ -12189,7 +12193,7 @@
         <v>659</v>
       </c>
       <c r="F123" s="3" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="G123" s="3" t="s">
         <v>27</v>
@@ -12260,7 +12264,7 @@
         <v>659</v>
       </c>
       <c r="F124" s="3" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="G124" s="3" t="s">
         <v>27</v>
@@ -12331,7 +12335,7 @@
         <v>659</v>
       </c>
       <c r="F125" s="3" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="G125" s="3" t="s">
         <v>27</v>
@@ -12402,7 +12406,7 @@
         <v>659</v>
       </c>
       <c r="F126" s="3" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="G126" s="3" t="s">
         <v>27</v>
@@ -12473,7 +12477,7 @@
         <v>659</v>
       </c>
       <c r="F127" s="3" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="G127" s="3" t="s">
         <v>27</v>
@@ -12542,7 +12546,7 @@
         <v>659</v>
       </c>
       <c r="F128" s="3" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="G128" s="3" t="s">
         <v>700</v>
@@ -12613,7 +12617,7 @@
         <v>659</v>
       </c>
       <c r="F129" s="3" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="G129" s="3" t="s">
         <v>39</v>
@@ -12684,7 +12688,7 @@
         <v>659</v>
       </c>
       <c r="F130" s="3" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="G130" s="3" t="s">
         <v>39</v>
@@ -12755,7 +12759,7 @@
         <v>659</v>
       </c>
       <c r="F131" s="3" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="G131" s="3" t="s">
         <v>39</v>
@@ -12826,7 +12830,7 @@
         <v>659</v>
       </c>
       <c r="F132" s="3" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="G132" s="3" t="s">
         <v>39</v>
@@ -12897,7 +12901,7 @@
         <v>659</v>
       </c>
       <c r="F133" s="3" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="G133" s="3" t="s">
         <v>39</v>
@@ -12968,7 +12972,7 @@
         <v>659</v>
       </c>
       <c r="F134" s="3" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="G134" s="3" t="s">
         <v>39</v>
@@ -13039,7 +13043,7 @@
         <v>659</v>
       </c>
       <c r="F135" s="3" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="G135" s="3" t="s">
         <v>39</v>
@@ -13110,7 +13114,7 @@
         <v>659</v>
       </c>
       <c r="F136" s="3" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="G136" s="3" t="s">
         <v>39</v>
@@ -13181,7 +13185,7 @@
         <v>659</v>
       </c>
       <c r="F137" s="3" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="G137" s="3" t="s">
         <v>39</v>
@@ -13599,7 +13603,7 @@
         <v>44167</v>
       </c>
       <c r="F143" s="3" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="G143" s="3" t="s">
         <v>760</v>
@@ -13668,7 +13672,7 @@
         <v>44167</v>
       </c>
       <c r="F144" s="3" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="G144" s="3" t="s">
         <v>769</v>
@@ -13737,7 +13741,7 @@
         <v>44167</v>
       </c>
       <c r="F145" s="3" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="G145" s="3" t="s">
         <v>769</v>
@@ -13806,7 +13810,7 @@
         <v>44167</v>
       </c>
       <c r="F146" s="3" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="G146" s="3" t="s">
         <v>769</v>
@@ -13875,7 +13879,7 @@
         <v>44167</v>
       </c>
       <c r="F147" s="3" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="G147" s="3" t="s">
         <v>760</v>
@@ -13944,7 +13948,7 @@
         <v>44167</v>
       </c>
       <c r="F148" s="3" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="G148" s="3" t="s">
         <v>769</v>
@@ -14013,7 +14017,7 @@
         <v>44167</v>
       </c>
       <c r="F149" s="3" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="G149" s="3" t="s">
         <v>769</v>
@@ -14082,7 +14086,7 @@
         <v>44167</v>
       </c>
       <c r="F150" s="3" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="G150" s="3" t="s">
         <v>769</v>
@@ -14151,7 +14155,7 @@
         <v>44167</v>
       </c>
       <c r="F151" s="3" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="G151" s="3" t="s">
         <v>760</v>
@@ -14220,7 +14224,7 @@
         <v>44167</v>
       </c>
       <c r="F152" s="3" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="G152" s="3" t="s">
         <v>769</v>
@@ -14289,7 +14293,7 @@
         <v>44167</v>
       </c>
       <c r="F153" s="3" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="G153" s="3" t="s">
         <v>769</v>
@@ -14358,7 +14362,7 @@
         <v>44167</v>
       </c>
       <c r="F154" s="3" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="G154" s="3" t="s">
         <v>769</v>
@@ -14427,7 +14431,7 @@
         <v>44167</v>
       </c>
       <c r="F155" s="3" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="G155" s="3" t="s">
         <v>769</v>
@@ -14496,7 +14500,7 @@
         <v>44167</v>
       </c>
       <c r="F156" s="3" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="G156" s="3" t="s">
         <v>769</v>
@@ -14565,7 +14569,7 @@
         <v>44167</v>
       </c>
       <c r="F157" s="3" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="G157" s="3" t="s">
         <v>769</v>
@@ -14634,7 +14638,7 @@
         <v>44167</v>
       </c>
       <c r="F158" s="3" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="G158" s="3" t="s">
         <v>769</v>
@@ -14703,7 +14707,7 @@
         <v>44167</v>
       </c>
       <c r="F159" s="3" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="G159" s="3" t="s">
         <v>769</v>
@@ -14772,7 +14776,7 @@
         <v>44167</v>
       </c>
       <c r="F160" s="3" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="G160" s="3" t="s">
         <v>760</v>
@@ -14841,7 +14845,7 @@
         <v>44167</v>
       </c>
       <c r="F161" s="3" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="G161" s="3" t="s">
         <v>769</v>
@@ -14910,7 +14914,7 @@
         <v>44167</v>
       </c>
       <c r="F162" s="3" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="G162" s="3" t="s">
         <v>769</v>
@@ -14979,7 +14983,7 @@
         <v>44167</v>
       </c>
       <c r="F163" s="3" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="G163" s="3" t="s">
         <v>769</v>
@@ -15048,7 +15052,7 @@
         <v>44167</v>
       </c>
       <c r="F164" s="3" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="G164" s="3" t="s">
         <v>760</v>
@@ -15117,7 +15121,7 @@
         <v>44167</v>
       </c>
       <c r="F165" s="3" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="G165" s="3" t="s">
         <v>769</v>
@@ -15186,7 +15190,7 @@
         <v>44167</v>
       </c>
       <c r="F166" s="3" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="G166" s="3" t="s">
         <v>769</v>
@@ -15255,7 +15259,7 @@
         <v>44167</v>
       </c>
       <c r="F167" s="3" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="G167" s="3" t="s">
         <v>769</v>
@@ -15324,7 +15328,7 @@
         <v>44167</v>
       </c>
       <c r="F168" s="3" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="G168" s="3" t="s">
         <v>769</v>
@@ -15393,7 +15397,7 @@
         <v>44167</v>
       </c>
       <c r="F169" s="3" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="G169" s="3" t="s">
         <v>769</v>
@@ -15462,7 +15466,7 @@
         <v>44167</v>
       </c>
       <c r="F170" s="3" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="G170" s="3" t="s">
         <v>760</v>
@@ -15531,7 +15535,7 @@
         <v>44167</v>
       </c>
       <c r="F171" s="3" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="G171" s="3" t="s">
         <v>769</v>
@@ -15600,7 +15604,7 @@
         <v>44167</v>
       </c>
       <c r="F172" s="3" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="G172" s="3" t="s">
         <v>769</v>
@@ -15669,7 +15673,7 @@
         <v>44167</v>
       </c>
       <c r="F173" s="3" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="G173" s="3" t="s">
         <v>769</v>
@@ -15738,7 +15742,7 @@
         <v>44167</v>
       </c>
       <c r="F174" s="3" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="G174" s="3" t="s">
         <v>769</v>
@@ -15807,7 +15811,7 @@
         <v>44167</v>
       </c>
       <c r="F175" s="3" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="G175" s="3" t="s">
         <v>769</v>
@@ -15876,7 +15880,7 @@
         <v>44167</v>
       </c>
       <c r="F176" s="3" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="G176" s="3" t="s">
         <v>769</v>
@@ -15945,7 +15949,7 @@
         <v>44167</v>
       </c>
       <c r="F177" s="3" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="G177" s="3" t="s">
         <v>39</v>
@@ -16014,7 +16018,7 @@
         <v>44167</v>
       </c>
       <c r="F178" s="3" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="G178" s="3" t="s">
         <v>39</v>
@@ -16083,7 +16087,7 @@
         <v>44167</v>
       </c>
       <c r="F179" s="3" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="G179" s="3" t="s">
         <v>39</v>
@@ -16152,7 +16156,7 @@
         <v>44167</v>
       </c>
       <c r="F180" s="3" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="G180" s="3" t="s">
         <v>39</v>
@@ -16221,7 +16225,7 @@
         <v>44167</v>
       </c>
       <c r="F181" s="3" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="G181" s="3" t="s">
         <v>39</v>
@@ -16290,7 +16294,7 @@
         <v>44167</v>
       </c>
       <c r="F182" s="3" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="G182" s="3" t="s">
         <v>39</v>
@@ -16359,7 +16363,7 @@
         <v>44167</v>
       </c>
       <c r="F183" s="3" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="G183" s="3" t="s">
         <v>883</v>
@@ -16566,7 +16570,7 @@
         <v>892</v>
       </c>
       <c r="F186" s="3" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="G186" s="3" t="s">
         <v>39</v>
@@ -16637,7 +16641,7 @@
         <v>44532</v>
       </c>
       <c r="F187" s="3" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="G187" s="3" t="s">
         <v>27</v>
@@ -16706,7 +16710,7 @@
         <v>36</v>
       </c>
       <c r="F188" s="3" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="G188" s="3" t="s">
         <v>165</v>
@@ -16775,7 +16779,7 @@
         <v>928</v>
       </c>
       <c r="F189" s="3" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="G189" s="3" t="s">
         <v>165</v>
@@ -16846,7 +16850,7 @@
         <v>44595</v>
       </c>
       <c r="F190" s="3" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="G190" s="3" t="s">
         <v>27</v>
@@ -16915,7 +16919,7 @@
         <v>44896</v>
       </c>
       <c r="F191" s="3" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="G191" s="3" t="s">
         <v>27</v>
@@ -16984,7 +16988,7 @@
         <v>44896</v>
       </c>
       <c r="F192" s="3" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="G192" s="3" t="s">
         <v>39</v>
@@ -17053,7 +17057,7 @@
         <v>44896</v>
       </c>
       <c r="F193" s="3" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="G193" s="3" t="s">
         <v>27</v>
@@ -17118,7 +17122,7 @@
         <v>44896</v>
       </c>
       <c r="F194" s="3" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="G194" s="3" t="s">
         <v>39</v>
@@ -17390,7 +17394,7 @@
         <v>44896</v>
       </c>
       <c r="F198" s="3" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="G198" s="3" t="s">
         <v>27</v>
@@ -17457,7 +17461,7 @@
         <v>44896</v>
       </c>
       <c r="F199" s="3" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="G199" s="3" t="s">
         <v>39</v>
@@ -17524,7 +17528,7 @@
         <v>44915</v>
       </c>
       <c r="F200" s="3" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="G200" s="3" t="s">
         <v>996</v>
@@ -17593,7 +17597,7 @@
         <v>45239</v>
       </c>
       <c r="F201" s="3" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="G201" s="3" t="s">
         <v>27</v>
@@ -17662,7 +17666,7 @@
         <v>45239</v>
       </c>
       <c r="F202" s="3" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="G202" s="3" t="s">
         <v>39</v>
@@ -17729,7 +17733,7 @@
       </c>
       <c r="E203" s="3"/>
       <c r="F203" s="3" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="G203" s="3" t="s">
         <v>1015</v>
@@ -17786,7 +17790,7 @@
         <v>36</v>
       </c>
       <c r="F204" s="3" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="G204" s="3" t="s">
         <v>165</v>
@@ -17910,7 +17914,7 @@
         <v>45131</v>
       </c>
       <c r="F206" s="3" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="G206" s="3" t="s">
         <v>760</v>
@@ -17979,7 +17983,7 @@
         <v>45131</v>
       </c>
       <c r="F207" s="3" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="G207" s="3" t="s">
         <v>39</v>
@@ -18048,7 +18052,7 @@
         <v>45330</v>
       </c>
       <c r="F208" s="3" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="G208" s="3" t="s">
         <v>27</v>
@@ -18117,7 +18121,7 @@
         <v>45330</v>
       </c>
       <c r="F209" s="3" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="G209" s="3" t="s">
         <v>39</v>
@@ -18186,7 +18190,7 @@
         <v>45308</v>
       </c>
       <c r="F210" s="3" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="G210" s="3" t="s">
         <v>102</v>
@@ -18249,7 +18253,7 @@
         <v>45308</v>
       </c>
       <c r="F211" s="3" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="G211" s="3" t="s">
         <v>112</v>
@@ -18312,7 +18316,7 @@
         <v>45323</v>
       </c>
       <c r="F212" s="3" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="G212" s="3" t="s">
         <v>27</v>
@@ -18381,7 +18385,7 @@
         <v>45323</v>
       </c>
       <c r="F213" s="3" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="G213" s="3" t="s">
         <v>39</v>
@@ -18745,8 +18749,8 @@
       <c r="E6" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="F6" s="6" t="b">
-        <v>0</v>
+      <c r="F6" s="5" t="b">
+        <v>1</v>
       </c>
       <c r="G6" s="5" t="b">
         <v>1</v>
@@ -18787,7 +18791,7 @@
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>1074</v>
@@ -18801,8 +18805,8 @@
       <c r="E7" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="F7" s="6" t="b">
-        <v>0</v>
+      <c r="F7" s="5" t="b">
+        <v>1</v>
       </c>
       <c r="G7" s="5" t="b">
         <v>1</v>
@@ -18843,7 +18847,7 @@
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>1074</v>

</xml_diff>

<commit_message>
generated all the reports on 2024-03-05
</commit_message>
<xml_diff>
--- a/report/merged_configurations.xlsx
+++ b/report/merged_configurations.xlsx
@@ -3215,10 +3215,10 @@
     <t>[{"naam":"Charter Overlijdensaangifte","waarde":"Charter OSLO_Overlijdensaangifte.pdf"}]</t>
   </si>
   <si>
-    <t>[{"naam":"Verslag Thematische Werkgroep I - 16 januari 2024","waarde":"20240116__ThematicWorkshop1_Verslag_OSLOOverlijdensaangifte"}]</t>
-  </si>
-  <si>
-    <t>[{"naam":"Presentatie Thematische Werkgroep I - 16 januari 2024","waarde":"20240116_ThematicWorkshop1_Powerpoint_OSLOOverlijdensaangifte.pptx"}]</t>
+    <t>[{"naam":"Verslag Thematische Werkgroep I - 16 januari 2024","waarde":"20240116__ThematicWorkshop1_Verslag_OSLOOverlijdensaangifte.pdf"},{"naam":"Verslag Thematische Werkgroep II - 20 februari 2024","waarde":"20240220__ThematicWorkshop2_Verslag_OSLOOverlijdensaangifte.pdf"}]</t>
+  </si>
+  <si>
+    <t>[{"naam":"Presentatie Thematische Werkgroep I - 16 januari 2024","waarde":"20240116_ThematicWorkshop1_Powerpoint_OSLOOverlijdensaangifte.pptx"},{"naam":"Presentatie Thematische Werkgroep II - 20 februari 2024","waarde":"20240220_ThematicWorkshop2_Powerpoint_OSLOOverlijdensaangifte.pptx"}]</t>
   </si>
   <si>
     <t>Semantische standaard voor de digitale transformatie van de Vlaamse Overheid en lokale besturen</t>

</xml_diff>

<commit_message>
generated all the reports on 2024-03-20
</commit_message>
<xml_diff>
--- a/report/merged_configurations.xlsx
+++ b/report/merged_configurations.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5033" uniqueCount="1084">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5051" uniqueCount="1087">
   <si>
     <t>naam</t>
   </si>
@@ -3261,6 +3261,15 @@
   </si>
   <si>
     <t>voc-overlijdensaangifte-config.md</t>
+  </si>
+  <si>
+    <t>Applicatieprofiel Kind fiche</t>
+  </si>
+  <si>
+    <t>kind-fiche-description.md</t>
+  </si>
+  <si>
+    <t>[{"naam":"Kind fiche applicatieprofiel","waarde":"https://data.test-vlaanderen.be/doc/applicatieprofiel/kind-fiche/ontwerpstandaard/2024-03-19/"}]</t>
   </si>
   <si>
     <t>Geen rapport gevonden</t>
@@ -3671,7 +3680,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W215"/>
+  <dimension ref="A1:W216"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="23" width="44" customWidth="1"/>
@@ -18597,6 +18606,65 @@
         <v>37</v>
       </c>
       <c r="W215" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="216" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A216" s="3" t="s">
+        <v>1083</v>
+      </c>
+      <c r="B216" s="3"/>
+      <c r="C216" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D216" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E216" s="4">
+        <v>45370</v>
+      </c>
+      <c r="F216" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="G216" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="H216" s="3" t="s">
+        <v>1084</v>
+      </c>
+      <c r="I216" s="3" t="s">
+        <v>1085</v>
+      </c>
+      <c r="J216" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="K216" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="L216" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="M216" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="N216" s="3"/>
+      <c r="O216" s="3"/>
+      <c r="P216" s="3"/>
+      <c r="Q216" s="3"/>
+      <c r="R216" s="3"/>
+      <c r="S216" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="T216" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="U216" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="V216" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="W216" s="3" t="s">
         <v>37</v>
       </c>
     </row>
@@ -18608,7 +18676,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R215"/>
+  <dimension ref="A1:R216"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="18" width="44" customWidth="1"/>
@@ -18675,7 +18743,7 @@
         <v>23</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>1083</v>
+        <v>1086</v>
       </c>
       <c r="C2" s="5" t="b">
         <v>1</v>
@@ -18731,7 +18799,7 @@
         <v>38</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>1083</v>
+        <v>1086</v>
       </c>
       <c r="C3" s="5" t="b">
         <v>1</v>
@@ -18787,7 +18855,7 @@
         <v>41</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>1083</v>
+        <v>1086</v>
       </c>
       <c r="C4" s="5" t="b">
         <v>1</v>
@@ -18843,7 +18911,7 @@
         <v>48</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>1083</v>
+        <v>1086</v>
       </c>
       <c r="C5" s="5" t="b">
         <v>1</v>
@@ -18899,7 +18967,7 @@
         <v>51</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>1083</v>
+        <v>1086</v>
       </c>
       <c r="C6" s="5" t="b">
         <v>1</v>
@@ -18955,7 +19023,7 @@
         <v>60</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>1083</v>
+        <v>1086</v>
       </c>
       <c r="C7" s="5" t="b">
         <v>1</v>
@@ -19011,7 +19079,7 @@
         <v>62</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>1083</v>
+        <v>1086</v>
       </c>
       <c r="C8" s="5" t="b">
         <v>1</v>
@@ -19067,7 +19135,7 @@
         <v>70</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>1083</v>
+        <v>1086</v>
       </c>
       <c r="C9" s="5" t="b">
         <v>1</v>
@@ -19123,7 +19191,7 @@
         <v>72</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>1083</v>
+        <v>1086</v>
       </c>
       <c r="C10" s="5" t="b">
         <v>1</v>
@@ -19179,7 +19247,7 @@
         <v>79</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>1083</v>
+        <v>1086</v>
       </c>
       <c r="C11" s="5" t="b">
         <v>1</v>
@@ -19235,7 +19303,7 @@
         <v>88</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>1083</v>
+        <v>1086</v>
       </c>
       <c r="C12" s="5" t="b">
         <v>1</v>
@@ -19291,7 +19359,7 @@
         <v>90</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>1083</v>
+        <v>1086</v>
       </c>
       <c r="C13" s="5" t="b">
         <v>1</v>
@@ -19347,7 +19415,7 @@
         <v>99</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>1083</v>
+        <v>1086</v>
       </c>
       <c r="C14" s="5" t="b">
         <v>1</v>
@@ -19515,7 +19583,7 @@
         <v>124</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>1083</v>
+        <v>1086</v>
       </c>
       <c r="C17" s="5" t="b">
         <v>1</v>
@@ -19571,7 +19639,7 @@
         <v>135</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>1083</v>
+        <v>1086</v>
       </c>
       <c r="C18" s="5" t="b">
         <v>1</v>
@@ -19627,7 +19695,7 @@
         <v>137</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>1083</v>
+        <v>1086</v>
       </c>
       <c r="C19" s="5" t="b">
         <v>1</v>
@@ -19683,7 +19751,7 @@
         <v>139</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>1083</v>
+        <v>1086</v>
       </c>
       <c r="C20" s="5" t="b">
         <v>1</v>
@@ -19739,7 +19807,7 @@
         <v>141</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>1083</v>
+        <v>1086</v>
       </c>
       <c r="C21" s="5" t="b">
         <v>1</v>
@@ -19795,7 +19863,7 @@
         <v>144</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>1083</v>
+        <v>1086</v>
       </c>
       <c r="C22" s="5" t="b">
         <v>1</v>
@@ -19851,7 +19919,7 @@
         <v>146</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>1083</v>
+        <v>1086</v>
       </c>
       <c r="C23" s="5" t="b">
         <v>1</v>
@@ -19907,7 +19975,7 @@
         <v>148</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>1083</v>
+        <v>1086</v>
       </c>
       <c r="C24" s="5" t="b">
         <v>1</v>
@@ -19963,7 +20031,7 @@
         <v>150</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>1083</v>
+        <v>1086</v>
       </c>
       <c r="C25" s="5" t="b">
         <v>1</v>
@@ -20019,7 +20087,7 @@
         <v>152</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>1083</v>
+        <v>1086</v>
       </c>
       <c r="C26" s="5" t="b">
         <v>1</v>
@@ -20075,7 +20143,7 @@
         <v>154</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>1083</v>
+        <v>1086</v>
       </c>
       <c r="C27" s="5" t="b">
         <v>1</v>
@@ -20131,7 +20199,7 @@
         <v>152</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>1083</v>
+        <v>1086</v>
       </c>
       <c r="C28" s="5" t="b">
         <v>1</v>
@@ -20187,7 +20255,7 @@
         <v>156</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>1083</v>
+        <v>1086</v>
       </c>
       <c r="C29" s="5" t="b">
         <v>1</v>
@@ -20243,7 +20311,7 @@
         <v>158</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>1083</v>
+        <v>1086</v>
       </c>
       <c r="C30" s="5" t="b">
         <v>1</v>
@@ -20299,7 +20367,7 @@
         <v>160</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>1083</v>
+        <v>1086</v>
       </c>
       <c r="C31" s="5" t="b">
         <v>1</v>
@@ -20355,7 +20423,7 @@
         <v>162</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>1083</v>
+        <v>1086</v>
       </c>
       <c r="C32" s="5" t="b">
         <v>1</v>
@@ -20411,7 +20479,7 @@
         <v>164</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>1083</v>
+        <v>1086</v>
       </c>
       <c r="C33" s="5" t="b">
         <v>1</v>
@@ -20467,7 +20535,7 @@
         <v>166</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>1083</v>
+        <v>1086</v>
       </c>
       <c r="C34" s="5" t="b">
         <v>1</v>
@@ -20523,7 +20591,7 @@
         <v>168</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>1083</v>
+        <v>1086</v>
       </c>
       <c r="C35" s="5" t="b">
         <v>1</v>
@@ -20579,7 +20647,7 @@
         <v>170</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>1083</v>
+        <v>1086</v>
       </c>
       <c r="C36" s="5" t="b">
         <v>1</v>
@@ -20635,7 +20703,7 @@
         <v>172</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>1083</v>
+        <v>1086</v>
       </c>
       <c r="C37" s="5" t="b">
         <v>1</v>
@@ -20803,7 +20871,7 @@
         <v>202</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>1083</v>
+        <v>1086</v>
       </c>
       <c r="C40" s="5" t="b">
         <v>1</v>
@@ -20859,7 +20927,7 @@
         <v>209</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>1083</v>
+        <v>1086</v>
       </c>
       <c r="C41" s="5" t="b">
         <v>1</v>
@@ -22427,7 +22495,7 @@
         <v>391</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>1083</v>
+        <v>1086</v>
       </c>
       <c r="C69" s="5" t="b">
         <v>1</v>
@@ -22483,7 +22551,7 @@
         <v>403</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>1083</v>
+        <v>1086</v>
       </c>
       <c r="C70" s="5" t="b">
         <v>1</v>
@@ -22931,7 +22999,7 @@
         <v>462</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>1083</v>
+        <v>1086</v>
       </c>
       <c r="C78" s="5" t="b">
         <v>1</v>
@@ -23603,7 +23671,7 @@
         <v>543</v>
       </c>
       <c r="B90" s="3" t="s">
-        <v>1083</v>
+        <v>1086</v>
       </c>
       <c r="C90" s="5" t="b">
         <v>1</v>
@@ -23659,7 +23727,7 @@
         <v>552</v>
       </c>
       <c r="B91" s="3" t="s">
-        <v>1083</v>
+        <v>1086</v>
       </c>
       <c r="C91" s="5" t="b">
         <v>1</v>
@@ -23715,7 +23783,7 @@
         <v>554</v>
       </c>
       <c r="B92" s="3" t="s">
-        <v>1083</v>
+        <v>1086</v>
       </c>
       <c r="C92" s="5" t="b">
         <v>1</v>
@@ -25843,7 +25911,7 @@
         <v>708</v>
       </c>
       <c r="B130" s="3" t="s">
-        <v>1083</v>
+        <v>1086</v>
       </c>
       <c r="C130" s="5" t="b">
         <v>1</v>
@@ -26403,7 +26471,7 @@
         <v>740</v>
       </c>
       <c r="B140" s="3" t="s">
-        <v>1083</v>
+        <v>1086</v>
       </c>
       <c r="C140" s="5" t="b">
         <v>1</v>
@@ -26459,7 +26527,7 @@
         <v>746</v>
       </c>
       <c r="B141" s="3" t="s">
-        <v>1083</v>
+        <v>1086</v>
       </c>
       <c r="C141" s="5" t="b">
         <v>1</v>
@@ -26627,7 +26695,7 @@
         <v>766</v>
       </c>
       <c r="B144" s="3" t="s">
-        <v>1083</v>
+        <v>1086</v>
       </c>
       <c r="C144" s="5" t="b">
         <v>1</v>
@@ -26683,7 +26751,7 @@
         <v>768</v>
       </c>
       <c r="B145" s="3" t="s">
-        <v>1083</v>
+        <v>1086</v>
       </c>
       <c r="C145" s="5" t="b">
         <v>1</v>
@@ -26739,7 +26807,7 @@
         <v>777</v>
       </c>
       <c r="B146" s="3" t="s">
-        <v>1083</v>
+        <v>1086</v>
       </c>
       <c r="C146" s="5" t="b">
         <v>1</v>
@@ -26795,7 +26863,7 @@
         <v>781</v>
       </c>
       <c r="B147" s="3" t="s">
-        <v>1083</v>
+        <v>1086</v>
       </c>
       <c r="C147" s="5" t="b">
         <v>1</v>
@@ -26851,7 +26919,7 @@
         <v>784</v>
       </c>
       <c r="B148" s="3" t="s">
-        <v>1083</v>
+        <v>1086</v>
       </c>
       <c r="C148" s="5" t="b">
         <v>1</v>
@@ -26907,7 +26975,7 @@
         <v>787</v>
       </c>
       <c r="B149" s="3" t="s">
-        <v>1083</v>
+        <v>1086</v>
       </c>
       <c r="C149" s="5" t="b">
         <v>1</v>
@@ -26963,7 +27031,7 @@
         <v>790</v>
       </c>
       <c r="B150" s="3" t="s">
-        <v>1083</v>
+        <v>1086</v>
       </c>
       <c r="C150" s="5" t="b">
         <v>1</v>
@@ -27019,7 +27087,7 @@
         <v>793</v>
       </c>
       <c r="B151" s="3" t="s">
-        <v>1083</v>
+        <v>1086</v>
       </c>
       <c r="C151" s="5" t="b">
         <v>1</v>
@@ -27075,7 +27143,7 @@
         <v>796</v>
       </c>
       <c r="B152" s="3" t="s">
-        <v>1083</v>
+        <v>1086</v>
       </c>
       <c r="C152" s="5" t="b">
         <v>1</v>
@@ -27131,7 +27199,7 @@
         <v>799</v>
       </c>
       <c r="B153" s="3" t="s">
-        <v>1083</v>
+        <v>1086</v>
       </c>
       <c r="C153" s="5" t="b">
         <v>1</v>
@@ -27187,7 +27255,7 @@
         <v>802</v>
       </c>
       <c r="B154" s="3" t="s">
-        <v>1083</v>
+        <v>1086</v>
       </c>
       <c r="C154" s="5" t="b">
         <v>1</v>
@@ -27243,7 +27311,7 @@
         <v>805</v>
       </c>
       <c r="B155" s="3" t="s">
-        <v>1083</v>
+        <v>1086</v>
       </c>
       <c r="C155" s="5" t="b">
         <v>1</v>
@@ -27299,7 +27367,7 @@
         <v>808</v>
       </c>
       <c r="B156" s="3" t="s">
-        <v>1083</v>
+        <v>1086</v>
       </c>
       <c r="C156" s="5" t="b">
         <v>1</v>
@@ -27355,7 +27423,7 @@
         <v>811</v>
       </c>
       <c r="B157" s="3" t="s">
-        <v>1083</v>
+        <v>1086</v>
       </c>
       <c r="C157" s="5" t="b">
         <v>1</v>
@@ -27411,7 +27479,7 @@
         <v>814</v>
       </c>
       <c r="B158" s="3" t="s">
-        <v>1083</v>
+        <v>1086</v>
       </c>
       <c r="C158" s="5" t="b">
         <v>1</v>
@@ -27467,7 +27535,7 @@
         <v>817</v>
       </c>
       <c r="B159" s="3" t="s">
-        <v>1083</v>
+        <v>1086</v>
       </c>
       <c r="C159" s="5" t="b">
         <v>1</v>
@@ -27523,7 +27591,7 @@
         <v>820</v>
       </c>
       <c r="B160" s="3" t="s">
-        <v>1083</v>
+        <v>1086</v>
       </c>
       <c r="C160" s="5" t="b">
         <v>1</v>
@@ -27579,7 +27647,7 @@
         <v>823</v>
       </c>
       <c r="B161" s="3" t="s">
-        <v>1083</v>
+        <v>1086</v>
       </c>
       <c r="C161" s="5" t="b">
         <v>1</v>
@@ -27635,7 +27703,7 @@
         <v>826</v>
       </c>
       <c r="B162" s="3" t="s">
-        <v>1083</v>
+        <v>1086</v>
       </c>
       <c r="C162" s="5" t="b">
         <v>1</v>
@@ -27691,7 +27759,7 @@
         <v>829</v>
       </c>
       <c r="B163" s="3" t="s">
-        <v>1083</v>
+        <v>1086</v>
       </c>
       <c r="C163" s="5" t="b">
         <v>1</v>
@@ -27747,7 +27815,7 @@
         <v>832</v>
       </c>
       <c r="B164" s="3" t="s">
-        <v>1083</v>
+        <v>1086</v>
       </c>
       <c r="C164" s="5" t="b">
         <v>1</v>
@@ -27803,7 +27871,7 @@
         <v>835</v>
       </c>
       <c r="B165" s="3" t="s">
-        <v>1083</v>
+        <v>1086</v>
       </c>
       <c r="C165" s="5" t="b">
         <v>1</v>
@@ -27859,7 +27927,7 @@
         <v>838</v>
       </c>
       <c r="B166" s="3" t="s">
-        <v>1083</v>
+        <v>1086</v>
       </c>
       <c r="C166" s="5" t="b">
         <v>1</v>
@@ -27915,7 +27983,7 @@
         <v>841</v>
       </c>
       <c r="B167" s="3" t="s">
-        <v>1083</v>
+        <v>1086</v>
       </c>
       <c r="C167" s="5" t="b">
         <v>1</v>
@@ -27971,7 +28039,7 @@
         <v>844</v>
       </c>
       <c r="B168" s="3" t="s">
-        <v>1083</v>
+        <v>1086</v>
       </c>
       <c r="C168" s="5" t="b">
         <v>1</v>
@@ -28027,7 +28095,7 @@
         <v>847</v>
       </c>
       <c r="B169" s="3" t="s">
-        <v>1083</v>
+        <v>1086</v>
       </c>
       <c r="C169" s="5" t="b">
         <v>1</v>
@@ -28083,7 +28151,7 @@
         <v>850</v>
       </c>
       <c r="B170" s="3" t="s">
-        <v>1083</v>
+        <v>1086</v>
       </c>
       <c r="C170" s="5" t="b">
         <v>1</v>
@@ -28139,7 +28207,7 @@
         <v>853</v>
       </c>
       <c r="B171" s="3" t="s">
-        <v>1083</v>
+        <v>1086</v>
       </c>
       <c r="C171" s="5" t="b">
         <v>1</v>
@@ -28195,7 +28263,7 @@
         <v>856</v>
       </c>
       <c r="B172" s="3" t="s">
-        <v>1083</v>
+        <v>1086</v>
       </c>
       <c r="C172" s="5" t="b">
         <v>1</v>
@@ -28251,7 +28319,7 @@
         <v>859</v>
       </c>
       <c r="B173" s="3" t="s">
-        <v>1083</v>
+        <v>1086</v>
       </c>
       <c r="C173" s="5" t="b">
         <v>1</v>
@@ -28307,7 +28375,7 @@
         <v>862</v>
       </c>
       <c r="B174" s="3" t="s">
-        <v>1083</v>
+        <v>1086</v>
       </c>
       <c r="C174" s="5" t="b">
         <v>1</v>
@@ -28363,7 +28431,7 @@
         <v>865</v>
       </c>
       <c r="B175" s="3" t="s">
-        <v>1083</v>
+        <v>1086</v>
       </c>
       <c r="C175" s="5" t="b">
         <v>1</v>
@@ -28419,7 +28487,7 @@
         <v>868</v>
       </c>
       <c r="B176" s="3" t="s">
-        <v>1083</v>
+        <v>1086</v>
       </c>
       <c r="C176" s="5" t="b">
         <v>1</v>
@@ -28475,7 +28543,7 @@
         <v>871</v>
       </c>
       <c r="B177" s="3" t="s">
-        <v>1083</v>
+        <v>1086</v>
       </c>
       <c r="C177" s="5" t="b">
         <v>1</v>
@@ -28531,7 +28599,7 @@
         <v>874</v>
       </c>
       <c r="B178" s="3" t="s">
-        <v>1083</v>
+        <v>1086</v>
       </c>
       <c r="C178" s="5" t="b">
         <v>1</v>
@@ -28587,7 +28655,7 @@
         <v>877</v>
       </c>
       <c r="B179" s="3" t="s">
-        <v>1083</v>
+        <v>1086</v>
       </c>
       <c r="C179" s="5" t="b">
         <v>1</v>
@@ -28643,7 +28711,7 @@
         <v>880</v>
       </c>
       <c r="B180" s="3" t="s">
-        <v>1083</v>
+        <v>1086</v>
       </c>
       <c r="C180" s="5" t="b">
         <v>1</v>
@@ -28699,7 +28767,7 @@
         <v>882</v>
       </c>
       <c r="B181" s="3" t="s">
-        <v>1083</v>
+        <v>1086</v>
       </c>
       <c r="C181" s="5" t="b">
         <v>1</v>
@@ -28755,7 +28823,7 @@
         <v>885</v>
       </c>
       <c r="B182" s="3" t="s">
-        <v>1083</v>
+        <v>1086</v>
       </c>
       <c r="C182" s="5" t="b">
         <v>1</v>
@@ -28811,7 +28879,7 @@
         <v>887</v>
       </c>
       <c r="B183" s="3" t="s">
-        <v>1083</v>
+        <v>1086</v>
       </c>
       <c r="C183" s="5" t="b">
         <v>1</v>
@@ -28867,7 +28935,7 @@
         <v>889</v>
       </c>
       <c r="B184" s="3" t="s">
-        <v>1083</v>
+        <v>1086</v>
       </c>
       <c r="C184" s="5" t="b">
         <v>1</v>
@@ -28923,7 +28991,7 @@
         <v>891</v>
       </c>
       <c r="B185" s="3" t="s">
-        <v>1083</v>
+        <v>1086</v>
       </c>
       <c r="C185" s="5" t="b">
         <v>1</v>
@@ -28979,7 +29047,7 @@
         <v>894</v>
       </c>
       <c r="B186" s="3" t="s">
-        <v>1083</v>
+        <v>1086</v>
       </c>
       <c r="C186" s="5" t="b">
         <v>1</v>
@@ -29035,7 +29103,7 @@
         <v>900</v>
       </c>
       <c r="B187" s="3" t="s">
-        <v>1083</v>
+        <v>1086</v>
       </c>
       <c r="C187" s="5" t="b">
         <v>1</v>
@@ -29091,7 +29159,7 @@
         <v>911</v>
       </c>
       <c r="B188" s="3" t="s">
-        <v>1083</v>
+        <v>1086</v>
       </c>
       <c r="C188" s="5" t="b">
         <v>1</v>
@@ -29203,7 +29271,7 @@
         <v>925</v>
       </c>
       <c r="B190" s="3" t="s">
-        <v>1083</v>
+        <v>1086</v>
       </c>
       <c r="C190" s="5" t="b">
         <v>1</v>
@@ -29259,7 +29327,7 @@
         <v>934</v>
       </c>
       <c r="B191" s="3" t="s">
-        <v>1083</v>
+        <v>1086</v>
       </c>
       <c r="C191" s="5" t="b">
         <v>1</v>
@@ -29371,7 +29439,7 @@
         <v>954</v>
       </c>
       <c r="B193" s="3" t="s">
-        <v>1083</v>
+        <v>1086</v>
       </c>
       <c r="C193" s="5" t="b">
         <v>1</v>
@@ -29427,7 +29495,7 @@
         <v>962</v>
       </c>
       <c r="B194" s="3" t="s">
-        <v>1083</v>
+        <v>1086</v>
       </c>
       <c r="C194" s="5" t="b">
         <v>1</v>
@@ -29483,7 +29551,7 @@
         <v>964</v>
       </c>
       <c r="B195" s="3" t="s">
-        <v>1083</v>
+        <v>1086</v>
       </c>
       <c r="C195" s="5" t="b">
         <v>1</v>
@@ -29539,7 +29607,7 @@
         <v>971</v>
       </c>
       <c r="B196" s="3" t="s">
-        <v>1083</v>
+        <v>1086</v>
       </c>
       <c r="C196" s="5" t="b">
         <v>1</v>
@@ -29595,7 +29663,7 @@
         <v>973</v>
       </c>
       <c r="B197" s="3" t="s">
-        <v>1083</v>
+        <v>1086</v>
       </c>
       <c r="C197" s="5" t="b">
         <v>1</v>
@@ -29651,7 +29719,7 @@
         <v>983</v>
       </c>
       <c r="B198" s="3" t="s">
-        <v>1083</v>
+        <v>1086</v>
       </c>
       <c r="C198" s="5" t="b">
         <v>1</v>
@@ -29707,7 +29775,7 @@
         <v>989</v>
       </c>
       <c r="B199" s="3" t="s">
-        <v>1083</v>
+        <v>1086</v>
       </c>
       <c r="C199" s="5" t="b">
         <v>1</v>
@@ -29763,7 +29831,7 @@
         <v>992</v>
       </c>
       <c r="B200" s="3" t="s">
-        <v>1083</v>
+        <v>1086</v>
       </c>
       <c r="C200" s="5" t="b">
         <v>1</v>
@@ -29819,7 +29887,7 @@
         <v>1000</v>
       </c>
       <c r="B201" s="3" t="s">
-        <v>1083</v>
+        <v>1086</v>
       </c>
       <c r="C201" s="5" t="b">
         <v>1</v>
@@ -29875,7 +29943,7 @@
         <v>1004</v>
       </c>
       <c r="B202" s="3" t="s">
-        <v>1083</v>
+        <v>1086</v>
       </c>
       <c r="C202" s="5" t="b">
         <v>1</v>
@@ -29931,7 +29999,7 @@
         <v>1014</v>
       </c>
       <c r="B203" s="3" t="s">
-        <v>1083</v>
+        <v>1086</v>
       </c>
       <c r="C203" s="5" t="b">
         <v>1</v>
@@ -29987,7 +30055,7 @@
         <v>1020</v>
       </c>
       <c r="B204" s="3" t="s">
-        <v>1083</v>
+        <v>1086</v>
       </c>
       <c r="C204" s="5" t="b">
         <v>1</v>
@@ -30043,7 +30111,7 @@
         <v>1023</v>
       </c>
       <c r="B205" s="3" t="s">
-        <v>1083</v>
+        <v>1086</v>
       </c>
       <c r="C205" s="5" t="b">
         <v>1</v>
@@ -30099,7 +30167,7 @@
         <v>1026</v>
       </c>
       <c r="B206" s="3" t="s">
-        <v>1083</v>
+        <v>1086</v>
       </c>
       <c r="C206" s="5" t="b">
         <v>1</v>
@@ -30155,7 +30223,7 @@
         <v>1033</v>
       </c>
       <c r="B207" s="3" t="s">
-        <v>1083</v>
+        <v>1086</v>
       </c>
       <c r="C207" s="5" t="b">
         <v>1</v>
@@ -30211,7 +30279,7 @@
         <v>1040</v>
       </c>
       <c r="B208" s="3" t="s">
-        <v>1083</v>
+        <v>1086</v>
       </c>
       <c r="C208" s="5" t="b">
         <v>1</v>
@@ -30267,7 +30335,7 @@
         <v>1046</v>
       </c>
       <c r="B209" s="3" t="s">
-        <v>1083</v>
+        <v>1086</v>
       </c>
       <c r="C209" s="5" t="b">
         <v>1</v>
@@ -30323,7 +30391,7 @@
         <v>1048</v>
       </c>
       <c r="B210" s="3" t="s">
-        <v>1083</v>
+        <v>1086</v>
       </c>
       <c r="C210" s="5" t="b">
         <v>1</v>
@@ -30379,7 +30447,7 @@
         <v>1059</v>
       </c>
       <c r="B211" s="3" t="s">
-        <v>1083</v>
+        <v>1086</v>
       </c>
       <c r="C211" s="5" t="b">
         <v>1</v>
@@ -30435,7 +30503,7 @@
         <v>1061</v>
       </c>
       <c r="B212" s="3" t="s">
-        <v>1083</v>
+        <v>1086</v>
       </c>
       <c r="C212" s="5" t="b">
         <v>1</v>
@@ -30491,7 +30559,7 @@
         <v>1067</v>
       </c>
       <c r="B213" s="3" t="s">
-        <v>1083</v>
+        <v>1086</v>
       </c>
       <c r="C213" s="5" t="b">
         <v>1</v>
@@ -30547,7 +30615,7 @@
         <v>1069</v>
       </c>
       <c r="B214" s="3" t="s">
-        <v>1083</v>
+        <v>1086</v>
       </c>
       <c r="C214" s="5" t="b">
         <v>1</v>
@@ -30603,54 +30671,110 @@
         <v>1081</v>
       </c>
       <c r="B215" s="3" t="s">
+        <v>1086</v>
+      </c>
+      <c r="C215" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="D215" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="E215" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="F215" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="G215" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="H215" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="I215" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="J215" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="K215" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="L215" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="M215" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="N215" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="O215" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="P215" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q215" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="R215" s="6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="216" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A216" s="3" t="s">
         <v>1083</v>
       </c>
-      <c r="C215" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="D215" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="E215" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="F215" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="G215" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="H215" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="I215" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="J215" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="K215" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="L215" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="M215" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="N215" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="O215" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="P215" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q215" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="R215" s="6" t="b">
+      <c r="B216" s="3" t="s">
+        <v>1086</v>
+      </c>
+      <c r="C216" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="D216" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="E216" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="F216" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="G216" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="H216" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="I216" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="J216" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="K216" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="L216" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="M216" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="N216" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="O216" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="P216" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q216" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="R216" s="6" t="b">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
generated all the reports on 2024-03-22
</commit_message>
<xml_diff>
--- a/report/merged_configurations.xlsx
+++ b/report/merged_configurations.xlsx
@@ -356,10 +356,10 @@
     <t>ap-FinanciëleData.md</t>
   </si>
   <si>
-    <t>[{"naam":"Financiële Rapportering Applicatieprofiel","waarde":"https://data.vlaanderen.be/doc/applicatieprofiel/financiele-data"}]</t>
-  </si>
-  <si>
-    <t>[{"naam":"Financiële Rapportering taxonomie-dcjm vocabularium","waarde":"https://data.vlaanderen.be/ns/financiele-data/taxonomie-dcjm"}]</t>
+    <t>[{"naam":"Financiële Rapportering Applicatieprofiel","waarde":"https://data.vlaanderen.be/doc/applicatieprofiel/financiele-rapportering"}]</t>
+  </si>
+  <si>
+    <t>[{"naam":"Financiële Rapportering taxonomie-dcjm vocabularium","waarde":"https://data.vlaanderen.be/ns/financiele-rapportering/taxonomie-dcjm"}]</t>
   </si>
   <si>
     <t>[{"naam":"OSLO Financiële Rapportering Charter","waarde":"Template-Werkgroep-Charter-OSLO.docx"}]</t>
@@ -389,7 +389,7 @@
     <t>voc-FinanciëleData.md</t>
   </si>
   <si>
-    <t>[{"naam":"Financiële Rapportering vocabularium","waarde":"https://data.vlaanderen.be/ns/financiele-data/"}]</t>
+    <t>[{"naam":"Financiële Rapportering vocabularium","waarde":"https://data.vlaanderen.be/ns/financiele-rapportering/"}]</t>
   </si>
   <si>
     <t>Applicatieprofiel Bodem</t>

</xml_diff>

<commit_message>
generated all the reports on 2024-04-04
</commit_message>
<xml_diff>
--- a/report/merged_configurations.xlsx
+++ b/report/merged_configurations.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5179" uniqueCount="1106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5177" uniqueCount="1106">
   <si>
     <t>naam</t>
   </si>
@@ -239,7 +239,7 @@
     <t>[{"naam":"Applicatieprofiel Voorwaarden Dienstverlening","waarde":"https://data.vlaanderen.be/doc/applicatieprofiel/voorwaarden-dienstverlening/kandidaatstandaard/2023-07-11"}]</t>
   </si>
   <si>
-    <t>[{"naam":"Charter","waarde":"Charter OSLO Voorwaarden Dienstverlening.docx.pdf"},{"naam":"Documenten desk research","waarde":"4. Desk research (1).zip"}]</t>
+    <t>[{"naam":"Charter","waarde":"Charter OSLO Voorwaarden Dienstverlening.docx.pdf"},{"naam":"Documenten desk research","waarde":"Desk research.zip"}]</t>
   </si>
   <si>
     <t>[{"naam":"Verslag business werkgroep - 6 april 2023","waarde":"Verslag Business Workshop Voorwaarden Dienstverlening.pdf"},{"naam":"Verslag thematische werkgroep 1 - 4 mei 2023","waarde":"Verslag OSLO voorwaarden dienstverlening - thematische werkgroep 1.pdf"},{"naam":"Verslag thematische werkgroep 2 - 15 juni 2023","waarde":"Verslag OSLO voorwaarden dienstverlening - thematische werkgroep 2.pdf"},{"naam":"Verslag thematische werkgroep 3 - 27 juli 2023","waarde":"Verslag OSLO voorwaarden dienstverlening - thematische werkgroep 3.pdf"},{"naam":"Verslag thematische werkgroep 4 - 13 oktober 2023","waarde":"Verslag OSLO voorwaarden dienstverlening - thematische werkgroep 4.pdf"}]</t>
@@ -18128,8 +18128,8 @@
       <c r="P207" s="4">
         <v>44873</v>
       </c>
-      <c r="Q207" s="3" t="s">
-        <v>26</v>
+      <c r="Q207" s="4">
+        <v>45239</v>
       </c>
       <c r="R207" s="3" t="s">
         <v>26</v>
@@ -18197,8 +18197,8 @@
       <c r="P208" s="4">
         <v>44873</v>
       </c>
-      <c r="Q208" s="3" t="s">
-        <v>26</v>
+      <c r="Q208" s="4">
+        <v>45239</v>
       </c>
       <c r="R208" s="3" t="s">
         <v>26</v>
@@ -30693,8 +30693,8 @@
       <c r="P207" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="Q207" s="6" t="b">
-        <v>0</v>
+      <c r="Q207" s="5" t="b">
+        <v>1</v>
       </c>
       <c r="R207" s="6" t="b">
         <v>0</v>
@@ -30749,8 +30749,8 @@
       <c r="P208" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="Q208" s="6" t="b">
-        <v>0</v>
+      <c r="Q208" s="5" t="b">
+        <v>1</v>
       </c>
       <c r="R208" s="6" t="b">
         <v>0</v>

</xml_diff>

<commit_message>
generated all the reports on 2024-04-05
</commit_message>
<xml_diff>
--- a/report/merged_configurations.xlsx
+++ b/report/merged_configurations.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5177" uniqueCount="1106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5177" uniqueCount="1109">
   <si>
     <t>naam</t>
   </si>
@@ -3119,7 +3119,7 @@
     <t>Implementatiemodel Kwaliteit Wegen en Wegmarkeringen</t>
   </si>
   <si>
-    <t>[{"naam":"Implementatiemodel Kwaliteit Wegen en Wegmarkeringen","waarde":"https://data.vlaanderen.be/doc/applicatieprofiel/kwaliteit-wegen-en-wegmarkeringen"}]</t>
+    <t>[{"naam":"Implementatiemodel Kwaliteit Wegen en Wegmarkeringen","waarde":"https://implementatie.data.vlaanderen.be/doc/implementatiemodel/kwaliteit-wegen-en-wegmarkeringen/"}]</t>
   </si>
   <si>
     <t>[{"naam":"Charter","waarde":"Charter Machine Learning as a Service.pdf"}]</t>
@@ -3137,7 +3137,7 @@
     <t>Vocabularium Kwaliteit Wegen en Wegmarkeringen</t>
   </si>
   <si>
-    <t>[{"naam":"Vocabularium Kwaliteit Wegen en Wegmarkeringen","waarde":"https://data.vlaanderen.be/doc/ns/kwaliteit-wegen-en-wegmarkeringen"}]</t>
+    <t>[{"naam":"Vocabularium Kwaliteit Wegen en Wegmarkeringen","waarde":"https://implementatie.data.vlaanderen.be/doc/ns/kwaliteit-wegen-en-wegmarkeringen"}]</t>
   </si>
   <si>
     <t>Applicatieprofiel Slimme Raadpleegomgeving</t>
@@ -3263,13 +3263,22 @@
     <t>https://data.vlaanderen.be/id/organisatie/OVO000092</t>
   </si>
   <si>
+    <t>1 juni 2023</t>
+  </si>
+  <si>
+    <t>voc-statistiek.md</t>
+  </si>
+  <si>
+    <t>[{"naam":"Vocabularium Statistiek","waarde":"https://data.vlaanderen.be/ns/statistiek"}]</t>
+  </si>
+  <si>
+    <t>[{"naam":"Zie OSLO Waterkwaliteit","waarde":"https://data.vlaanderen.be/standaarden/kandidaat-standaard/applicatieprofiel-oslo-waterkwaliteit.html"}]</t>
+  </si>
+  <si>
+    <t>Semantische standaard voor datakwaliteit</t>
+  </si>
+  <si>
     <t>17 oktober 2022</t>
-  </si>
-  <si>
-    <t>voc-statistiek.md</t>
-  </si>
-  <si>
-    <t>[{"naam":"Vocabularium Statistiek","waarde":"https://data.vlaanderen.be/ns/statistiek"}]</t>
   </si>
   <si>
     <t>Applicatieprofiel OSLO Statistiek</t>
@@ -18707,25 +18716,25 @@
         <v>1085</v>
       </c>
       <c r="J216" s="3" t="s">
-        <v>31</v>
+        <v>1086</v>
       </c>
       <c r="K216" s="3" t="s">
-        <v>31</v>
+        <v>1086</v>
       </c>
       <c r="L216" s="3" t="s">
-        <v>31</v>
+        <v>1086</v>
       </c>
       <c r="M216" s="3" t="s">
-        <v>31</v>
+        <v>1086</v>
       </c>
       <c r="N216" s="3" t="s">
-        <v>26</v>
+        <v>1087</v>
       </c>
       <c r="O216" s="3" t="s">
-        <v>26</v>
+        <v>58</v>
       </c>
       <c r="P216" s="3" t="s">
-        <v>26</v>
+        <v>1088</v>
       </c>
       <c r="Q216" s="3" t="s">
         <v>26</v>
@@ -18751,7 +18760,7 @@
     </row>
     <row r="217" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A217" s="3" t="s">
-        <v>1086</v>
+        <v>1089</v>
       </c>
       <c r="B217" s="3"/>
       <c r="C217" s="3" t="s">
@@ -18770,31 +18779,31 @@
         <v>28</v>
       </c>
       <c r="H217" s="3" t="s">
+        <v>1090</v>
+      </c>
+      <c r="I217" s="3" t="s">
+        <v>1091</v>
+      </c>
+      <c r="J217" s="3" t="s">
+        <v>1086</v>
+      </c>
+      <c r="K217" s="3" t="s">
+        <v>1086</v>
+      </c>
+      <c r="L217" s="3" t="s">
+        <v>1086</v>
+      </c>
+      <c r="M217" s="3" t="s">
+        <v>1086</v>
+      </c>
+      <c r="N217" s="3" t="s">
         <v>1087</v>
       </c>
-      <c r="I217" s="3" t="s">
+      <c r="O217" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="P217" s="3" t="s">
         <v>1088</v>
-      </c>
-      <c r="J217" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="K217" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="L217" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="M217" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="N217" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="O217" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="P217" s="3" t="s">
-        <v>26</v>
       </c>
       <c r="Q217" s="3" t="s">
         <v>26</v>
@@ -18820,7 +18829,7 @@
     </row>
     <row r="218" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A218" s="3" t="s">
-        <v>1089</v>
+        <v>1092</v>
       </c>
       <c r="B218" s="3"/>
       <c r="C218" s="3" t="s">
@@ -18839,31 +18848,31 @@
         <v>39</v>
       </c>
       <c r="H218" s="3" t="s">
-        <v>1090</v>
+        <v>1093</v>
       </c>
       <c r="I218" s="3" t="s">
-        <v>1091</v>
+        <v>1094</v>
       </c>
       <c r="J218" s="3" t="s">
-        <v>31</v>
+        <v>1086</v>
       </c>
       <c r="K218" s="3" t="s">
-        <v>31</v>
+        <v>1086</v>
       </c>
       <c r="L218" s="3" t="s">
-        <v>31</v>
+        <v>1086</v>
       </c>
       <c r="M218" s="3" t="s">
-        <v>31</v>
+        <v>1086</v>
       </c>
       <c r="N218" s="3" t="s">
-        <v>26</v>
+        <v>1087</v>
       </c>
       <c r="O218" s="3" t="s">
-        <v>26</v>
+        <v>58</v>
       </c>
       <c r="P218" s="3" t="s">
-        <v>26</v>
+        <v>1088</v>
       </c>
       <c r="Q218" s="3" t="s">
         <v>26</v>
@@ -18889,7 +18898,7 @@
     </row>
     <row r="219" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A219" s="3" t="s">
-        <v>1092</v>
+        <v>1095</v>
       </c>
       <c r="B219" s="3"/>
       <c r="C219" s="3" t="s">
@@ -18908,31 +18917,31 @@
         <v>28</v>
       </c>
       <c r="H219" s="3" t="s">
-        <v>1093</v>
+        <v>1096</v>
       </c>
       <c r="I219" s="3" t="s">
-        <v>1094</v>
+        <v>1097</v>
       </c>
       <c r="J219" s="3" t="s">
-        <v>31</v>
+        <v>1086</v>
       </c>
       <c r="K219" s="3" t="s">
-        <v>31</v>
+        <v>1086</v>
       </c>
       <c r="L219" s="3" t="s">
-        <v>31</v>
+        <v>1086</v>
       </c>
       <c r="M219" s="3" t="s">
-        <v>31</v>
+        <v>1086</v>
       </c>
       <c r="N219" s="3" t="s">
-        <v>26</v>
+        <v>1087</v>
       </c>
       <c r="O219" s="3" t="s">
-        <v>26</v>
+        <v>58</v>
       </c>
       <c r="P219" s="3" t="s">
-        <v>26</v>
+        <v>1088</v>
       </c>
       <c r="Q219" s="3" t="s">
         <v>26</v>
@@ -18958,7 +18967,7 @@
     </row>
     <row r="220" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A220" s="3" t="s">
-        <v>1095</v>
+        <v>1098</v>
       </c>
       <c r="B220" s="3"/>
       <c r="C220" s="3" t="s">
@@ -18977,31 +18986,31 @@
         <v>28</v>
       </c>
       <c r="H220" s="3" t="s">
-        <v>1096</v>
+        <v>1099</v>
       </c>
       <c r="I220" s="3" t="s">
-        <v>1097</v>
+        <v>1100</v>
       </c>
       <c r="J220" s="3" t="s">
-        <v>1098</v>
+        <v>1101</v>
       </c>
       <c r="K220" s="3" t="s">
         <v>31</v>
       </c>
       <c r="L220" s="3" t="s">
-        <v>1099</v>
+        <v>1102</v>
       </c>
       <c r="M220" s="3" t="s">
-        <v>1100</v>
+        <v>1103</v>
       </c>
       <c r="N220" s="3" t="s">
-        <v>1101</v>
+        <v>1104</v>
       </c>
       <c r="O220" s="3" t="s">
         <v>86</v>
       </c>
       <c r="P220" s="3" t="s">
-        <v>1083</v>
+        <v>1088</v>
       </c>
       <c r="Q220" s="3" t="s">
         <v>26</v>
@@ -19027,7 +19036,7 @@
     </row>
     <row r="221" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A221" s="3" t="s">
-        <v>1102</v>
+        <v>1105</v>
       </c>
       <c r="B221" s="3"/>
       <c r="C221" s="3" t="s">
@@ -19046,31 +19055,31 @@
         <v>39</v>
       </c>
       <c r="H221" s="3" t="s">
+        <v>1106</v>
+      </c>
+      <c r="I221" s="3" t="s">
+        <v>1107</v>
+      </c>
+      <c r="J221" s="3" t="s">
+        <v>1101</v>
+      </c>
+      <c r="K221" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="L221" s="3" t="s">
+        <v>1102</v>
+      </c>
+      <c r="M221" s="3" t="s">
         <v>1103</v>
       </c>
-      <c r="I221" s="3" t="s">
+      <c r="N221" s="3" t="s">
         <v>1104</v>
-      </c>
-      <c r="J221" s="3" t="s">
-        <v>1098</v>
-      </c>
-      <c r="K221" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="L221" s="3" t="s">
-        <v>1099</v>
-      </c>
-      <c r="M221" s="3" t="s">
-        <v>1100</v>
-      </c>
-      <c r="N221" s="3" t="s">
-        <v>1101</v>
       </c>
       <c r="O221" s="3" t="s">
         <v>86</v>
       </c>
       <c r="P221" s="3" t="s">
-        <v>1083</v>
+        <v>1088</v>
       </c>
       <c r="Q221" s="3" t="s">
         <v>26</v>
@@ -19169,7 +19178,7 @@
         <v>23</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>1105</v>
+        <v>1108</v>
       </c>
       <c r="C2" s="5" t="b">
         <v>1</v>
@@ -19225,7 +19234,7 @@
         <v>38</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>1105</v>
+        <v>1108</v>
       </c>
       <c r="C3" s="5" t="b">
         <v>1</v>
@@ -19281,7 +19290,7 @@
         <v>41</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>1105</v>
+        <v>1108</v>
       </c>
       <c r="C4" s="5" t="b">
         <v>1</v>
@@ -19337,7 +19346,7 @@
         <v>48</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>1105</v>
+        <v>1108</v>
       </c>
       <c r="C5" s="5" t="b">
         <v>1</v>
@@ -19393,7 +19402,7 @@
         <v>51</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>1105</v>
+        <v>1108</v>
       </c>
       <c r="C6" s="5" t="b">
         <v>1</v>
@@ -19449,7 +19458,7 @@
         <v>60</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>1105</v>
+        <v>1108</v>
       </c>
       <c r="C7" s="5" t="b">
         <v>1</v>
@@ -19505,7 +19514,7 @@
         <v>62</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>1105</v>
+        <v>1108</v>
       </c>
       <c r="C8" s="5" t="b">
         <v>1</v>
@@ -19561,7 +19570,7 @@
         <v>70</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>1105</v>
+        <v>1108</v>
       </c>
       <c r="C9" s="5" t="b">
         <v>1</v>
@@ -19617,7 +19626,7 @@
         <v>72</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>1105</v>
+        <v>1108</v>
       </c>
       <c r="C10" s="5" t="b">
         <v>1</v>
@@ -19673,7 +19682,7 @@
         <v>79</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>1105</v>
+        <v>1108</v>
       </c>
       <c r="C11" s="5" t="b">
         <v>1</v>
@@ -19729,7 +19738,7 @@
         <v>89</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>1105</v>
+        <v>1108</v>
       </c>
       <c r="C12" s="5" t="b">
         <v>1</v>
@@ -19785,7 +19794,7 @@
         <v>92</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>1105</v>
+        <v>1108</v>
       </c>
       <c r="C13" s="5" t="b">
         <v>1</v>
@@ -19841,7 +19850,7 @@
         <v>102</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>1105</v>
+        <v>1108</v>
       </c>
       <c r="C14" s="5" t="b">
         <v>1</v>
@@ -20009,7 +20018,7 @@
         <v>128</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>1105</v>
+        <v>1108</v>
       </c>
       <c r="C17" s="5" t="b">
         <v>1</v>
@@ -20065,7 +20074,7 @@
         <v>139</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>1105</v>
+        <v>1108</v>
       </c>
       <c r="C18" s="5" t="b">
         <v>1</v>
@@ -20121,7 +20130,7 @@
         <v>141</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>1105</v>
+        <v>1108</v>
       </c>
       <c r="C19" s="5" t="b">
         <v>1</v>
@@ -20177,7 +20186,7 @@
         <v>143</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>1105</v>
+        <v>1108</v>
       </c>
       <c r="C20" s="5" t="b">
         <v>1</v>
@@ -20233,7 +20242,7 @@
         <v>145</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>1105</v>
+        <v>1108</v>
       </c>
       <c r="C21" s="5" t="b">
         <v>1</v>
@@ -20289,7 +20298,7 @@
         <v>148</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>1105</v>
+        <v>1108</v>
       </c>
       <c r="C22" s="5" t="b">
         <v>1</v>
@@ -20345,7 +20354,7 @@
         <v>150</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>1105</v>
+        <v>1108</v>
       </c>
       <c r="C23" s="5" t="b">
         <v>1</v>
@@ -20401,7 +20410,7 @@
         <v>152</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>1105</v>
+        <v>1108</v>
       </c>
       <c r="C24" s="5" t="b">
         <v>1</v>
@@ -20457,7 +20466,7 @@
         <v>154</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>1105</v>
+        <v>1108</v>
       </c>
       <c r="C25" s="5" t="b">
         <v>1</v>
@@ -20513,7 +20522,7 @@
         <v>156</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>1105</v>
+        <v>1108</v>
       </c>
       <c r="C26" s="5" t="b">
         <v>1</v>
@@ -20569,7 +20578,7 @@
         <v>158</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>1105</v>
+        <v>1108</v>
       </c>
       <c r="C27" s="5" t="b">
         <v>1</v>
@@ -20625,7 +20634,7 @@
         <v>156</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>1105</v>
+        <v>1108</v>
       </c>
       <c r="C28" s="5" t="b">
         <v>1</v>
@@ -20681,7 +20690,7 @@
         <v>160</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>1105</v>
+        <v>1108</v>
       </c>
       <c r="C29" s="5" t="b">
         <v>1</v>
@@ -20737,7 +20746,7 @@
         <v>162</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>1105</v>
+        <v>1108</v>
       </c>
       <c r="C30" s="5" t="b">
         <v>1</v>
@@ -20793,7 +20802,7 @@
         <v>164</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>1105</v>
+        <v>1108</v>
       </c>
       <c r="C31" s="5" t="b">
         <v>1</v>
@@ -20849,7 +20858,7 @@
         <v>166</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>1105</v>
+        <v>1108</v>
       </c>
       <c r="C32" s="5" t="b">
         <v>1</v>
@@ -20905,7 +20914,7 @@
         <v>168</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>1105</v>
+        <v>1108</v>
       </c>
       <c r="C33" s="5" t="b">
         <v>1</v>
@@ -20961,7 +20970,7 @@
         <v>170</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>1105</v>
+        <v>1108</v>
       </c>
       <c r="C34" s="5" t="b">
         <v>1</v>
@@ -21017,7 +21026,7 @@
         <v>172</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>1105</v>
+        <v>1108</v>
       </c>
       <c r="C35" s="5" t="b">
         <v>1</v>
@@ -21073,7 +21082,7 @@
         <v>174</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>1105</v>
+        <v>1108</v>
       </c>
       <c r="C36" s="5" t="b">
         <v>1</v>
@@ -21129,7 +21138,7 @@
         <v>176</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>1105</v>
+        <v>1108</v>
       </c>
       <c r="C37" s="5" t="b">
         <v>1</v>
@@ -21297,7 +21306,7 @@
         <v>206</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>1105</v>
+        <v>1108</v>
       </c>
       <c r="C40" s="5" t="b">
         <v>1</v>
@@ -21353,7 +21362,7 @@
         <v>213</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>1105</v>
+        <v>1108</v>
       </c>
       <c r="C41" s="5" t="b">
         <v>1</v>
@@ -22921,7 +22930,7 @@
         <v>395</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>1105</v>
+        <v>1108</v>
       </c>
       <c r="C69" s="5" t="b">
         <v>1</v>
@@ -22977,7 +22986,7 @@
         <v>407</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>1105</v>
+        <v>1108</v>
       </c>
       <c r="C70" s="5" t="b">
         <v>1</v>
@@ -23425,7 +23434,7 @@
         <v>466</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>1105</v>
+        <v>1108</v>
       </c>
       <c r="C78" s="5" t="b">
         <v>1</v>
@@ -24097,7 +24106,7 @@
         <v>547</v>
       </c>
       <c r="B90" s="3" t="s">
-        <v>1105</v>
+        <v>1108</v>
       </c>
       <c r="C90" s="5" t="b">
         <v>1</v>
@@ -24153,7 +24162,7 @@
         <v>556</v>
       </c>
       <c r="B91" s="3" t="s">
-        <v>1105</v>
+        <v>1108</v>
       </c>
       <c r="C91" s="5" t="b">
         <v>1</v>
@@ -24209,7 +24218,7 @@
         <v>558</v>
       </c>
       <c r="B92" s="3" t="s">
-        <v>1105</v>
+        <v>1108</v>
       </c>
       <c r="C92" s="5" t="b">
         <v>1</v>
@@ -26337,7 +26346,7 @@
         <v>712</v>
       </c>
       <c r="B130" s="3" t="s">
-        <v>1105</v>
+        <v>1108</v>
       </c>
       <c r="C130" s="5" t="b">
         <v>1</v>
@@ -26897,7 +26906,7 @@
         <v>744</v>
       </c>
       <c r="B140" s="3" t="s">
-        <v>1105</v>
+        <v>1108</v>
       </c>
       <c r="C140" s="5" t="b">
         <v>1</v>
@@ -26953,7 +26962,7 @@
         <v>750</v>
       </c>
       <c r="B141" s="3" t="s">
-        <v>1105</v>
+        <v>1108</v>
       </c>
       <c r="C141" s="5" t="b">
         <v>1</v>
@@ -27121,7 +27130,7 @@
         <v>770</v>
       </c>
       <c r="B144" s="3" t="s">
-        <v>1105</v>
+        <v>1108</v>
       </c>
       <c r="C144" s="5" t="b">
         <v>1</v>
@@ -27177,7 +27186,7 @@
         <v>772</v>
       </c>
       <c r="B145" s="3" t="s">
-        <v>1105</v>
+        <v>1108</v>
       </c>
       <c r="C145" s="5" t="b">
         <v>1</v>
@@ -27233,7 +27242,7 @@
         <v>781</v>
       </c>
       <c r="B146" s="3" t="s">
-        <v>1105</v>
+        <v>1108</v>
       </c>
       <c r="C146" s="5" t="b">
         <v>1</v>
@@ -27289,7 +27298,7 @@
         <v>785</v>
       </c>
       <c r="B147" s="3" t="s">
-        <v>1105</v>
+        <v>1108</v>
       </c>
       <c r="C147" s="5" t="b">
         <v>1</v>
@@ -27345,7 +27354,7 @@
         <v>788</v>
       </c>
       <c r="B148" s="3" t="s">
-        <v>1105</v>
+        <v>1108</v>
       </c>
       <c r="C148" s="5" t="b">
         <v>1</v>
@@ -27401,7 +27410,7 @@
         <v>791</v>
       </c>
       <c r="B149" s="3" t="s">
-        <v>1105</v>
+        <v>1108</v>
       </c>
       <c r="C149" s="5" t="b">
         <v>1</v>
@@ -27457,7 +27466,7 @@
         <v>794</v>
       </c>
       <c r="B150" s="3" t="s">
-        <v>1105</v>
+        <v>1108</v>
       </c>
       <c r="C150" s="5" t="b">
         <v>1</v>
@@ -27513,7 +27522,7 @@
         <v>797</v>
       </c>
       <c r="B151" s="3" t="s">
-        <v>1105</v>
+        <v>1108</v>
       </c>
       <c r="C151" s="5" t="b">
         <v>1</v>
@@ -27569,7 +27578,7 @@
         <v>800</v>
       </c>
       <c r="B152" s="3" t="s">
-        <v>1105</v>
+        <v>1108</v>
       </c>
       <c r="C152" s="5" t="b">
         <v>1</v>
@@ -27625,7 +27634,7 @@
         <v>803</v>
       </c>
       <c r="B153" s="3" t="s">
-        <v>1105</v>
+        <v>1108</v>
       </c>
       <c r="C153" s="5" t="b">
         <v>1</v>
@@ -27681,7 +27690,7 @@
         <v>806</v>
       </c>
       <c r="B154" s="3" t="s">
-        <v>1105</v>
+        <v>1108</v>
       </c>
       <c r="C154" s="5" t="b">
         <v>1</v>
@@ -27737,7 +27746,7 @@
         <v>809</v>
       </c>
       <c r="B155" s="3" t="s">
-        <v>1105</v>
+        <v>1108</v>
       </c>
       <c r="C155" s="5" t="b">
         <v>1</v>
@@ -27793,7 +27802,7 @@
         <v>812</v>
       </c>
       <c r="B156" s="3" t="s">
-        <v>1105</v>
+        <v>1108</v>
       </c>
       <c r="C156" s="5" t="b">
         <v>1</v>
@@ -27849,7 +27858,7 @@
         <v>815</v>
       </c>
       <c r="B157" s="3" t="s">
-        <v>1105</v>
+        <v>1108</v>
       </c>
       <c r="C157" s="5" t="b">
         <v>1</v>
@@ -27905,7 +27914,7 @@
         <v>818</v>
       </c>
       <c r="B158" s="3" t="s">
-        <v>1105</v>
+        <v>1108</v>
       </c>
       <c r="C158" s="5" t="b">
         <v>1</v>
@@ -27961,7 +27970,7 @@
         <v>821</v>
       </c>
       <c r="B159" s="3" t="s">
-        <v>1105</v>
+        <v>1108</v>
       </c>
       <c r="C159" s="5" t="b">
         <v>1</v>
@@ -28017,7 +28026,7 @@
         <v>824</v>
       </c>
       <c r="B160" s="3" t="s">
-        <v>1105</v>
+        <v>1108</v>
       </c>
       <c r="C160" s="5" t="b">
         <v>1</v>
@@ -28073,7 +28082,7 @@
         <v>827</v>
       </c>
       <c r="B161" s="3" t="s">
-        <v>1105</v>
+        <v>1108</v>
       </c>
       <c r="C161" s="5" t="b">
         <v>1</v>
@@ -28129,7 +28138,7 @@
         <v>830</v>
       </c>
       <c r="B162" s="3" t="s">
-        <v>1105</v>
+        <v>1108</v>
       </c>
       <c r="C162" s="5" t="b">
         <v>1</v>
@@ -28185,7 +28194,7 @@
         <v>833</v>
       </c>
       <c r="B163" s="3" t="s">
-        <v>1105</v>
+        <v>1108</v>
       </c>
       <c r="C163" s="5" t="b">
         <v>1</v>
@@ -28241,7 +28250,7 @@
         <v>836</v>
       </c>
       <c r="B164" s="3" t="s">
-        <v>1105</v>
+        <v>1108</v>
       </c>
       <c r="C164" s="5" t="b">
         <v>1</v>
@@ -28297,7 +28306,7 @@
         <v>839</v>
       </c>
       <c r="B165" s="3" t="s">
-        <v>1105</v>
+        <v>1108</v>
       </c>
       <c r="C165" s="5" t="b">
         <v>1</v>
@@ -28353,7 +28362,7 @@
         <v>842</v>
       </c>
       <c r="B166" s="3" t="s">
-        <v>1105</v>
+        <v>1108</v>
       </c>
       <c r="C166" s="5" t="b">
         <v>1</v>
@@ -28409,7 +28418,7 @@
         <v>845</v>
       </c>
       <c r="B167" s="3" t="s">
-        <v>1105</v>
+        <v>1108</v>
       </c>
       <c r="C167" s="5" t="b">
         <v>1</v>
@@ -28465,7 +28474,7 @@
         <v>848</v>
       </c>
       <c r="B168" s="3" t="s">
-        <v>1105</v>
+        <v>1108</v>
       </c>
       <c r="C168" s="5" t="b">
         <v>1</v>
@@ -28521,7 +28530,7 @@
         <v>851</v>
       </c>
       <c r="B169" s="3" t="s">
-        <v>1105</v>
+        <v>1108</v>
       </c>
       <c r="C169" s="5" t="b">
         <v>1</v>
@@ -28577,7 +28586,7 @@
         <v>854</v>
       </c>
       <c r="B170" s="3" t="s">
-        <v>1105</v>
+        <v>1108</v>
       </c>
       <c r="C170" s="5" t="b">
         <v>1</v>
@@ -28633,7 +28642,7 @@
         <v>857</v>
       </c>
       <c r="B171" s="3" t="s">
-        <v>1105</v>
+        <v>1108</v>
       </c>
       <c r="C171" s="5" t="b">
         <v>1</v>
@@ -28689,7 +28698,7 @@
         <v>860</v>
       </c>
       <c r="B172" s="3" t="s">
-        <v>1105</v>
+        <v>1108</v>
       </c>
       <c r="C172" s="5" t="b">
         <v>1</v>
@@ -28745,7 +28754,7 @@
         <v>863</v>
       </c>
       <c r="B173" s="3" t="s">
-        <v>1105</v>
+        <v>1108</v>
       </c>
       <c r="C173" s="5" t="b">
         <v>1</v>
@@ -28801,7 +28810,7 @@
         <v>866</v>
       </c>
       <c r="B174" s="3" t="s">
-        <v>1105</v>
+        <v>1108</v>
       </c>
       <c r="C174" s="5" t="b">
         <v>1</v>
@@ -28857,7 +28866,7 @@
         <v>869</v>
       </c>
       <c r="B175" s="3" t="s">
-        <v>1105</v>
+        <v>1108</v>
       </c>
       <c r="C175" s="5" t="b">
         <v>1</v>
@@ -28913,7 +28922,7 @@
         <v>872</v>
       </c>
       <c r="B176" s="3" t="s">
-        <v>1105</v>
+        <v>1108</v>
       </c>
       <c r="C176" s="5" t="b">
         <v>1</v>
@@ -28969,7 +28978,7 @@
         <v>875</v>
       </c>
       <c r="B177" s="3" t="s">
-        <v>1105</v>
+        <v>1108</v>
       </c>
       <c r="C177" s="5" t="b">
         <v>1</v>
@@ -29025,7 +29034,7 @@
         <v>878</v>
       </c>
       <c r="B178" s="3" t="s">
-        <v>1105</v>
+        <v>1108</v>
       </c>
       <c r="C178" s="5" t="b">
         <v>1</v>
@@ -29081,7 +29090,7 @@
         <v>881</v>
       </c>
       <c r="B179" s="3" t="s">
-        <v>1105</v>
+        <v>1108</v>
       </c>
       <c r="C179" s="5" t="b">
         <v>1</v>
@@ -29137,7 +29146,7 @@
         <v>884</v>
       </c>
       <c r="B180" s="3" t="s">
-        <v>1105</v>
+        <v>1108</v>
       </c>
       <c r="C180" s="5" t="b">
         <v>1</v>
@@ -29193,7 +29202,7 @@
         <v>886</v>
       </c>
       <c r="B181" s="3" t="s">
-        <v>1105</v>
+        <v>1108</v>
       </c>
       <c r="C181" s="5" t="b">
         <v>1</v>
@@ -29249,7 +29258,7 @@
         <v>889</v>
       </c>
       <c r="B182" s="3" t="s">
-        <v>1105</v>
+        <v>1108</v>
       </c>
       <c r="C182" s="5" t="b">
         <v>1</v>
@@ -29305,7 +29314,7 @@
         <v>891</v>
       </c>
       <c r="B183" s="3" t="s">
-        <v>1105</v>
+        <v>1108</v>
       </c>
       <c r="C183" s="5" t="b">
         <v>1</v>
@@ -29361,7 +29370,7 @@
         <v>893</v>
       </c>
       <c r="B184" s="3" t="s">
-        <v>1105</v>
+        <v>1108</v>
       </c>
       <c r="C184" s="5" t="b">
         <v>1</v>
@@ -29417,7 +29426,7 @@
         <v>895</v>
       </c>
       <c r="B185" s="3" t="s">
-        <v>1105</v>
+        <v>1108</v>
       </c>
       <c r="C185" s="5" t="b">
         <v>1</v>
@@ -29473,7 +29482,7 @@
         <v>898</v>
       </c>
       <c r="B186" s="3" t="s">
-        <v>1105</v>
+        <v>1108</v>
       </c>
       <c r="C186" s="5" t="b">
         <v>1</v>
@@ -29529,7 +29538,7 @@
         <v>904</v>
       </c>
       <c r="B187" s="3" t="s">
-        <v>1105</v>
+        <v>1108</v>
       </c>
       <c r="C187" s="5" t="b">
         <v>1</v>
@@ -29585,7 +29594,7 @@
         <v>915</v>
       </c>
       <c r="B188" s="3" t="s">
-        <v>1105</v>
+        <v>1108</v>
       </c>
       <c r="C188" s="5" t="b">
         <v>1</v>
@@ -29697,7 +29706,7 @@
         <v>929</v>
       </c>
       <c r="B190" s="3" t="s">
-        <v>1105</v>
+        <v>1108</v>
       </c>
       <c r="C190" s="5" t="b">
         <v>1</v>
@@ -29809,7 +29818,7 @@
         <v>948</v>
       </c>
       <c r="B192" s="3" t="s">
-        <v>1105</v>
+        <v>1108</v>
       </c>
       <c r="C192" s="5" t="b">
         <v>1</v>
@@ -29865,7 +29874,7 @@
         <v>956</v>
       </c>
       <c r="B193" s="3" t="s">
-        <v>1105</v>
+        <v>1108</v>
       </c>
       <c r="C193" s="5" t="b">
         <v>1</v>
@@ -29921,7 +29930,7 @@
         <v>958</v>
       </c>
       <c r="B194" s="3" t="s">
-        <v>1105</v>
+        <v>1108</v>
       </c>
       <c r="C194" s="5" t="b">
         <v>1</v>
@@ -29977,7 +29986,7 @@
         <v>965</v>
       </c>
       <c r="B195" s="3" t="s">
-        <v>1105</v>
+        <v>1108</v>
       </c>
       <c r="C195" s="5" t="b">
         <v>1</v>
@@ -30033,7 +30042,7 @@
         <v>967</v>
       </c>
       <c r="B196" s="3" t="s">
-        <v>1105</v>
+        <v>1108</v>
       </c>
       <c r="C196" s="5" t="b">
         <v>1</v>
@@ -30089,7 +30098,7 @@
         <v>977</v>
       </c>
       <c r="B197" s="3" t="s">
-        <v>1105</v>
+        <v>1108</v>
       </c>
       <c r="C197" s="5" t="b">
         <v>1</v>
@@ -30145,7 +30154,7 @@
         <v>983</v>
       </c>
       <c r="B198" s="3" t="s">
-        <v>1105</v>
+        <v>1108</v>
       </c>
       <c r="C198" s="5" t="b">
         <v>1</v>
@@ -30201,7 +30210,7 @@
         <v>986</v>
       </c>
       <c r="B199" s="3" t="s">
-        <v>1105</v>
+        <v>1108</v>
       </c>
       <c r="C199" s="5" t="b">
         <v>1</v>
@@ -30257,7 +30266,7 @@
         <v>994</v>
       </c>
       <c r="B200" s="3" t="s">
-        <v>1105</v>
+        <v>1108</v>
       </c>
       <c r="C200" s="5" t="b">
         <v>1</v>
@@ -30313,7 +30322,7 @@
         <v>998</v>
       </c>
       <c r="B201" s="3" t="s">
-        <v>1105</v>
+        <v>1108</v>
       </c>
       <c r="C201" s="5" t="b">
         <v>1</v>
@@ -30369,7 +30378,7 @@
         <v>1008</v>
       </c>
       <c r="B202" s="3" t="s">
-        <v>1105</v>
+        <v>1108</v>
       </c>
       <c r="C202" s="5" t="b">
         <v>1</v>
@@ -30425,7 +30434,7 @@
         <v>1014</v>
       </c>
       <c r="B203" s="3" t="s">
-        <v>1105</v>
+        <v>1108</v>
       </c>
       <c r="C203" s="5" t="b">
         <v>1</v>
@@ -30481,7 +30490,7 @@
         <v>1017</v>
       </c>
       <c r="B204" s="3" t="s">
-        <v>1105</v>
+        <v>1108</v>
       </c>
       <c r="C204" s="5" t="b">
         <v>1</v>
@@ -30537,7 +30546,7 @@
         <v>1020</v>
       </c>
       <c r="B205" s="3" t="s">
-        <v>1105</v>
+        <v>1108</v>
       </c>
       <c r="C205" s="5" t="b">
         <v>1</v>
@@ -30593,7 +30602,7 @@
         <v>1027</v>
       </c>
       <c r="B206" s="3" t="s">
-        <v>1105</v>
+        <v>1108</v>
       </c>
       <c r="C206" s="5" t="b">
         <v>1</v>
@@ -30649,7 +30658,7 @@
         <v>1034</v>
       </c>
       <c r="B207" s="3" t="s">
-        <v>1105</v>
+        <v>1108</v>
       </c>
       <c r="C207" s="5" t="b">
         <v>1</v>
@@ -30705,7 +30714,7 @@
         <v>1040</v>
       </c>
       <c r="B208" s="3" t="s">
-        <v>1105</v>
+        <v>1108</v>
       </c>
       <c r="C208" s="5" t="b">
         <v>1</v>
@@ -30761,7 +30770,7 @@
         <v>1042</v>
       </c>
       <c r="B209" s="3" t="s">
-        <v>1105</v>
+        <v>1108</v>
       </c>
       <c r="C209" s="5" t="b">
         <v>1</v>
@@ -30817,7 +30826,7 @@
         <v>1053</v>
       </c>
       <c r="B210" s="3" t="s">
-        <v>1105</v>
+        <v>1108</v>
       </c>
       <c r="C210" s="5" t="b">
         <v>1</v>
@@ -30873,7 +30882,7 @@
         <v>1055</v>
       </c>
       <c r="B211" s="3" t="s">
-        <v>1105</v>
+        <v>1108</v>
       </c>
       <c r="C211" s="5" t="b">
         <v>1</v>
@@ -30929,7 +30938,7 @@
         <v>1061</v>
       </c>
       <c r="B212" s="3" t="s">
-        <v>1105</v>
+        <v>1108</v>
       </c>
       <c r="C212" s="5" t="b">
         <v>1</v>
@@ -30985,7 +30994,7 @@
         <v>1063</v>
       </c>
       <c r="B213" s="3" t="s">
-        <v>1105</v>
+        <v>1108</v>
       </c>
       <c r="C213" s="5" t="b">
         <v>1</v>
@@ -31041,7 +31050,7 @@
         <v>1075</v>
       </c>
       <c r="B214" s="3" t="s">
-        <v>1105</v>
+        <v>1108</v>
       </c>
       <c r="C214" s="5" t="b">
         <v>1</v>
@@ -31097,7 +31106,7 @@
         <v>1077</v>
       </c>
       <c r="B215" s="3" t="s">
-        <v>1105</v>
+        <v>1108</v>
       </c>
       <c r="C215" s="5" t="b">
         <v>1</v>
@@ -31153,7 +31162,7 @@
         <v>1080</v>
       </c>
       <c r="B216" s="3" t="s">
-        <v>1105</v>
+        <v>1108</v>
       </c>
       <c r="C216" s="5" t="b">
         <v>1</v>
@@ -31176,26 +31185,26 @@
       <c r="I216" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="J216" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="K216" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="L216" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="M216" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="N216" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="O216" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="P216" s="6" t="b">
-        <v>0</v>
+      <c r="J216" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="K216" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="L216" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="M216" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="N216" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="O216" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="P216" s="5" t="b">
+        <v>1</v>
       </c>
       <c r="Q216" s="6" t="b">
         <v>0</v>
@@ -31206,10 +31215,10 @@
     </row>
     <row r="217" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A217" s="3" t="s">
-        <v>1086</v>
+        <v>1089</v>
       </c>
       <c r="B217" s="3" t="s">
-        <v>1105</v>
+        <v>1108</v>
       </c>
       <c r="C217" s="5" t="b">
         <v>1</v>
@@ -31232,26 +31241,26 @@
       <c r="I217" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="J217" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="K217" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="L217" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="M217" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="N217" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="O217" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="P217" s="6" t="b">
-        <v>0</v>
+      <c r="J217" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="K217" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="L217" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="M217" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="N217" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="O217" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="P217" s="5" t="b">
+        <v>1</v>
       </c>
       <c r="Q217" s="6" t="b">
         <v>0</v>
@@ -31262,10 +31271,10 @@
     </row>
     <row r="218" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A218" s="3" t="s">
-        <v>1089</v>
+        <v>1092</v>
       </c>
       <c r="B218" s="3" t="s">
-        <v>1105</v>
+        <v>1108</v>
       </c>
       <c r="C218" s="5" t="b">
         <v>1</v>
@@ -31288,26 +31297,26 @@
       <c r="I218" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="J218" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="K218" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="L218" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="M218" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="N218" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="O218" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="P218" s="6" t="b">
-        <v>0</v>
+      <c r="J218" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="K218" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="L218" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="M218" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="N218" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="O218" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="P218" s="5" t="b">
+        <v>1</v>
       </c>
       <c r="Q218" s="6" t="b">
         <v>0</v>
@@ -31318,10 +31327,10 @@
     </row>
     <row r="219" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A219" s="3" t="s">
-        <v>1092</v>
+        <v>1095</v>
       </c>
       <c r="B219" s="3" t="s">
-        <v>1105</v>
+        <v>1108</v>
       </c>
       <c r="C219" s="5" t="b">
         <v>1</v>
@@ -31344,26 +31353,26 @@
       <c r="I219" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="J219" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="K219" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="L219" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="M219" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="N219" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="O219" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="P219" s="6" t="b">
-        <v>0</v>
+      <c r="J219" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="K219" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="L219" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="M219" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="N219" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="O219" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="P219" s="5" t="b">
+        <v>1</v>
       </c>
       <c r="Q219" s="6" t="b">
         <v>0</v>
@@ -31374,10 +31383,10 @@
     </row>
     <row r="220" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A220" s="3" t="s">
-        <v>1095</v>
+        <v>1098</v>
       </c>
       <c r="B220" s="3" t="s">
-        <v>1105</v>
+        <v>1108</v>
       </c>
       <c r="C220" s="5" t="b">
         <v>1</v>
@@ -31430,10 +31439,10 @@
     </row>
     <row r="221" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A221" s="3" t="s">
-        <v>1102</v>
+        <v>1105</v>
       </c>
       <c r="B221" s="3" t="s">
-        <v>1105</v>
+        <v>1108</v>
       </c>
       <c r="C221" s="5" t="b">
         <v>1</v>

</xml_diff>

<commit_message>
generated all the reports on 2024-04-06
</commit_message>
<xml_diff>
--- a/report/merged_configurations.xlsx
+++ b/report/merged_configurations.xlsx
@@ -18719,7 +18719,7 @@
         <v>1086</v>
       </c>
       <c r="K216" s="3" t="s">
-        <v>1086</v>
+        <v>31</v>
       </c>
       <c r="L216" s="3" t="s">
         <v>1086</v>
@@ -18788,7 +18788,7 @@
         <v>1086</v>
       </c>
       <c r="K217" s="3" t="s">
-        <v>1086</v>
+        <v>31</v>
       </c>
       <c r="L217" s="3" t="s">
         <v>1086</v>
@@ -18857,7 +18857,7 @@
         <v>1086</v>
       </c>
       <c r="K218" s="3" t="s">
-        <v>1086</v>
+        <v>31</v>
       </c>
       <c r="L218" s="3" t="s">
         <v>1086</v>
@@ -18926,7 +18926,7 @@
         <v>1086</v>
       </c>
       <c r="K219" s="3" t="s">
-        <v>1086</v>
+        <v>31</v>
       </c>
       <c r="L219" s="3" t="s">
         <v>1086</v>
@@ -31188,8 +31188,8 @@
       <c r="J216" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="K216" s="5" t="b">
-        <v>1</v>
+      <c r="K216" s="6" t="b">
+        <v>0</v>
       </c>
       <c r="L216" s="5" t="b">
         <v>1</v>
@@ -31244,8 +31244,8 @@
       <c r="J217" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="K217" s="5" t="b">
-        <v>1</v>
+      <c r="K217" s="6" t="b">
+        <v>0</v>
       </c>
       <c r="L217" s="5" t="b">
         <v>1</v>
@@ -31300,8 +31300,8 @@
       <c r="J218" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="K218" s="5" t="b">
-        <v>1</v>
+      <c r="K218" s="6" t="b">
+        <v>0</v>
       </c>
       <c r="L218" s="5" t="b">
         <v>1</v>
@@ -31356,8 +31356,8 @@
       <c r="J219" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="K219" s="5" t="b">
-        <v>1</v>
+      <c r="K219" s="6" t="b">
+        <v>0</v>
       </c>
       <c r="L219" s="5" t="b">
         <v>1</v>

</xml_diff>

<commit_message>
generated all the reports on 2024-04-09
</commit_message>
<xml_diff>
--- a/report/merged_configurations.xlsx
+++ b/report/merged_configurations.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5177" uniqueCount="1109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5200" uniqueCount="1113">
   <si>
     <t>naam</t>
   </si>
@@ -3336,6 +3336,18 @@
   </si>
   <si>
     <t>[{"naam":"Vocabularium Waterkwaliteit","waarde":"https://data.vlaanderen.be/ns/waterkwaliteit"}]</t>
+  </si>
+  <si>
+    <t>Applicatieprofiel Studentenattesten</t>
+  </si>
+  <si>
+    <t>studentenattesten-description.md</t>
+  </si>
+  <si>
+    <t>[{"naam":"Applicatieprofiel Studentenattesten","waarde":"https://data.vlaanderen.be/doc/applicatieprofiel/studentenattesten/ontwerpstandaard/2024-04-08"}]</t>
+  </si>
+  <si>
+    <t>Semantische standaard voor informatie over Studentenattesten</t>
   </si>
   <si>
     <t>Geen rapport gevonden</t>
@@ -3746,7 +3758,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W221"/>
+  <dimension ref="A1:W222"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="23" width="44" customWidth="1"/>
@@ -19100,6 +19112,75 @@
         <v>37</v>
       </c>
       <c r="W221" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="222" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A222" s="3" t="s">
+        <v>1108</v>
+      </c>
+      <c r="B222" s="3"/>
+      <c r="C222" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D222" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E222" s="4">
+        <v>45390</v>
+      </c>
+      <c r="F222" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="G222" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="H222" s="3" t="s">
+        <v>1109</v>
+      </c>
+      <c r="I222" s="3" t="s">
+        <v>1110</v>
+      </c>
+      <c r="J222" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="K222" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="L222" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="M222" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="N222" s="3" t="s">
+        <v>1111</v>
+      </c>
+      <c r="O222" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="P222" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q222" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="R222" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="S222" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="T222" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="U222" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="V222" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="W222" s="3" t="s">
         <v>37</v>
       </c>
     </row>
@@ -19111,7 +19192,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R221"/>
+  <dimension ref="A1:R222"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="18" width="44" customWidth="1"/>
@@ -19178,7 +19259,7 @@
         <v>23</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>1108</v>
+        <v>1112</v>
       </c>
       <c r="C2" s="5" t="b">
         <v>1</v>
@@ -19234,7 +19315,7 @@
         <v>38</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>1108</v>
+        <v>1112</v>
       </c>
       <c r="C3" s="5" t="b">
         <v>1</v>
@@ -19290,7 +19371,7 @@
         <v>41</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>1108</v>
+        <v>1112</v>
       </c>
       <c r="C4" s="5" t="b">
         <v>1</v>
@@ -19346,7 +19427,7 @@
         <v>48</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>1108</v>
+        <v>1112</v>
       </c>
       <c r="C5" s="5" t="b">
         <v>1</v>
@@ -19402,7 +19483,7 @@
         <v>51</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>1108</v>
+        <v>1112</v>
       </c>
       <c r="C6" s="5" t="b">
         <v>1</v>
@@ -19458,7 +19539,7 @@
         <v>60</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>1108</v>
+        <v>1112</v>
       </c>
       <c r="C7" s="5" t="b">
         <v>1</v>
@@ -19514,7 +19595,7 @@
         <v>62</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>1108</v>
+        <v>1112</v>
       </c>
       <c r="C8" s="5" t="b">
         <v>1</v>
@@ -19570,7 +19651,7 @@
         <v>70</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>1108</v>
+        <v>1112</v>
       </c>
       <c r="C9" s="5" t="b">
         <v>1</v>
@@ -19626,7 +19707,7 @@
         <v>72</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>1108</v>
+        <v>1112</v>
       </c>
       <c r="C10" s="5" t="b">
         <v>1</v>
@@ -19682,7 +19763,7 @@
         <v>79</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>1108</v>
+        <v>1112</v>
       </c>
       <c r="C11" s="5" t="b">
         <v>1</v>
@@ -19738,7 +19819,7 @@
         <v>89</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>1108</v>
+        <v>1112</v>
       </c>
       <c r="C12" s="5" t="b">
         <v>1</v>
@@ -19794,7 +19875,7 @@
         <v>92</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>1108</v>
+        <v>1112</v>
       </c>
       <c r="C13" s="5" t="b">
         <v>1</v>
@@ -19850,7 +19931,7 @@
         <v>102</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>1108</v>
+        <v>1112</v>
       </c>
       <c r="C14" s="5" t="b">
         <v>1</v>
@@ -20018,7 +20099,7 @@
         <v>128</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>1108</v>
+        <v>1112</v>
       </c>
       <c r="C17" s="5" t="b">
         <v>1</v>
@@ -20074,7 +20155,7 @@
         <v>139</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>1108</v>
+        <v>1112</v>
       </c>
       <c r="C18" s="5" t="b">
         <v>1</v>
@@ -20130,7 +20211,7 @@
         <v>141</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>1108</v>
+        <v>1112</v>
       </c>
       <c r="C19" s="5" t="b">
         <v>1</v>
@@ -20186,7 +20267,7 @@
         <v>143</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>1108</v>
+        <v>1112</v>
       </c>
       <c r="C20" s="5" t="b">
         <v>1</v>
@@ -20242,7 +20323,7 @@
         <v>145</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>1108</v>
+        <v>1112</v>
       </c>
       <c r="C21" s="5" t="b">
         <v>1</v>
@@ -20298,7 +20379,7 @@
         <v>148</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>1108</v>
+        <v>1112</v>
       </c>
       <c r="C22" s="5" t="b">
         <v>1</v>
@@ -20354,7 +20435,7 @@
         <v>150</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>1108</v>
+        <v>1112</v>
       </c>
       <c r="C23" s="5" t="b">
         <v>1</v>
@@ -20410,7 +20491,7 @@
         <v>152</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>1108</v>
+        <v>1112</v>
       </c>
       <c r="C24" s="5" t="b">
         <v>1</v>
@@ -20466,7 +20547,7 @@
         <v>154</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>1108</v>
+        <v>1112</v>
       </c>
       <c r="C25" s="5" t="b">
         <v>1</v>
@@ -20522,7 +20603,7 @@
         <v>156</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>1108</v>
+        <v>1112</v>
       </c>
       <c r="C26" s="5" t="b">
         <v>1</v>
@@ -20578,7 +20659,7 @@
         <v>158</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>1108</v>
+        <v>1112</v>
       </c>
       <c r="C27" s="5" t="b">
         <v>1</v>
@@ -20634,7 +20715,7 @@
         <v>156</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>1108</v>
+        <v>1112</v>
       </c>
       <c r="C28" s="5" t="b">
         <v>1</v>
@@ -20690,7 +20771,7 @@
         <v>160</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>1108</v>
+        <v>1112</v>
       </c>
       <c r="C29" s="5" t="b">
         <v>1</v>
@@ -20746,7 +20827,7 @@
         <v>162</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>1108</v>
+        <v>1112</v>
       </c>
       <c r="C30" s="5" t="b">
         <v>1</v>
@@ -20802,7 +20883,7 @@
         <v>164</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>1108</v>
+        <v>1112</v>
       </c>
       <c r="C31" s="5" t="b">
         <v>1</v>
@@ -20858,7 +20939,7 @@
         <v>166</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>1108</v>
+        <v>1112</v>
       </c>
       <c r="C32" s="5" t="b">
         <v>1</v>
@@ -20914,7 +20995,7 @@
         <v>168</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>1108</v>
+        <v>1112</v>
       </c>
       <c r="C33" s="5" t="b">
         <v>1</v>
@@ -20970,7 +21051,7 @@
         <v>170</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>1108</v>
+        <v>1112</v>
       </c>
       <c r="C34" s="5" t="b">
         <v>1</v>
@@ -21026,7 +21107,7 @@
         <v>172</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>1108</v>
+        <v>1112</v>
       </c>
       <c r="C35" s="5" t="b">
         <v>1</v>
@@ -21082,7 +21163,7 @@
         <v>174</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>1108</v>
+        <v>1112</v>
       </c>
       <c r="C36" s="5" t="b">
         <v>1</v>
@@ -21138,7 +21219,7 @@
         <v>176</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>1108</v>
+        <v>1112</v>
       </c>
       <c r="C37" s="5" t="b">
         <v>1</v>
@@ -21306,7 +21387,7 @@
         <v>206</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>1108</v>
+        <v>1112</v>
       </c>
       <c r="C40" s="5" t="b">
         <v>1</v>
@@ -21362,7 +21443,7 @@
         <v>213</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>1108</v>
+        <v>1112</v>
       </c>
       <c r="C41" s="5" t="b">
         <v>1</v>
@@ -22930,7 +23011,7 @@
         <v>395</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>1108</v>
+        <v>1112</v>
       </c>
       <c r="C69" s="5" t="b">
         <v>1</v>
@@ -22986,7 +23067,7 @@
         <v>407</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>1108</v>
+        <v>1112</v>
       </c>
       <c r="C70" s="5" t="b">
         <v>1</v>
@@ -23434,7 +23515,7 @@
         <v>466</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>1108</v>
+        <v>1112</v>
       </c>
       <c r="C78" s="5" t="b">
         <v>1</v>
@@ -24106,7 +24187,7 @@
         <v>547</v>
       </c>
       <c r="B90" s="3" t="s">
-        <v>1108</v>
+        <v>1112</v>
       </c>
       <c r="C90" s="5" t="b">
         <v>1</v>
@@ -24162,7 +24243,7 @@
         <v>556</v>
       </c>
       <c r="B91" s="3" t="s">
-        <v>1108</v>
+        <v>1112</v>
       </c>
       <c r="C91" s="5" t="b">
         <v>1</v>
@@ -24218,7 +24299,7 @@
         <v>558</v>
       </c>
       <c r="B92" s="3" t="s">
-        <v>1108</v>
+        <v>1112</v>
       </c>
       <c r="C92" s="5" t="b">
         <v>1</v>
@@ -26346,7 +26427,7 @@
         <v>712</v>
       </c>
       <c r="B130" s="3" t="s">
-        <v>1108</v>
+        <v>1112</v>
       </c>
       <c r="C130" s="5" t="b">
         <v>1</v>
@@ -26906,7 +26987,7 @@
         <v>744</v>
       </c>
       <c r="B140" s="3" t="s">
-        <v>1108</v>
+        <v>1112</v>
       </c>
       <c r="C140" s="5" t="b">
         <v>1</v>
@@ -26962,7 +27043,7 @@
         <v>750</v>
       </c>
       <c r="B141" s="3" t="s">
-        <v>1108</v>
+        <v>1112</v>
       </c>
       <c r="C141" s="5" t="b">
         <v>1</v>
@@ -27130,7 +27211,7 @@
         <v>770</v>
       </c>
       <c r="B144" s="3" t="s">
-        <v>1108</v>
+        <v>1112</v>
       </c>
       <c r="C144" s="5" t="b">
         <v>1</v>
@@ -27186,7 +27267,7 @@
         <v>772</v>
       </c>
       <c r="B145" s="3" t="s">
-        <v>1108</v>
+        <v>1112</v>
       </c>
       <c r="C145" s="5" t="b">
         <v>1</v>
@@ -27242,7 +27323,7 @@
         <v>781</v>
       </c>
       <c r="B146" s="3" t="s">
-        <v>1108</v>
+        <v>1112</v>
       </c>
       <c r="C146" s="5" t="b">
         <v>1</v>
@@ -27298,7 +27379,7 @@
         <v>785</v>
       </c>
       <c r="B147" s="3" t="s">
-        <v>1108</v>
+        <v>1112</v>
       </c>
       <c r="C147" s="5" t="b">
         <v>1</v>
@@ -27354,7 +27435,7 @@
         <v>788</v>
       </c>
       <c r="B148" s="3" t="s">
-        <v>1108</v>
+        <v>1112</v>
       </c>
       <c r="C148" s="5" t="b">
         <v>1</v>
@@ -27410,7 +27491,7 @@
         <v>791</v>
       </c>
       <c r="B149" s="3" t="s">
-        <v>1108</v>
+        <v>1112</v>
       </c>
       <c r="C149" s="5" t="b">
         <v>1</v>
@@ -27466,7 +27547,7 @@
         <v>794</v>
       </c>
       <c r="B150" s="3" t="s">
-        <v>1108</v>
+        <v>1112</v>
       </c>
       <c r="C150" s="5" t="b">
         <v>1</v>
@@ -27522,7 +27603,7 @@
         <v>797</v>
       </c>
       <c r="B151" s="3" t="s">
-        <v>1108</v>
+        <v>1112</v>
       </c>
       <c r="C151" s="5" t="b">
         <v>1</v>
@@ -27578,7 +27659,7 @@
         <v>800</v>
       </c>
       <c r="B152" s="3" t="s">
-        <v>1108</v>
+        <v>1112</v>
       </c>
       <c r="C152" s="5" t="b">
         <v>1</v>
@@ -27634,7 +27715,7 @@
         <v>803</v>
       </c>
       <c r="B153" s="3" t="s">
-        <v>1108</v>
+        <v>1112</v>
       </c>
       <c r="C153" s="5" t="b">
         <v>1</v>
@@ -27690,7 +27771,7 @@
         <v>806</v>
       </c>
       <c r="B154" s="3" t="s">
-        <v>1108</v>
+        <v>1112</v>
       </c>
       <c r="C154" s="5" t="b">
         <v>1</v>
@@ -27746,7 +27827,7 @@
         <v>809</v>
       </c>
       <c r="B155" s="3" t="s">
-        <v>1108</v>
+        <v>1112</v>
       </c>
       <c r="C155" s="5" t="b">
         <v>1</v>
@@ -27802,7 +27883,7 @@
         <v>812</v>
       </c>
       <c r="B156" s="3" t="s">
-        <v>1108</v>
+        <v>1112</v>
       </c>
       <c r="C156" s="5" t="b">
         <v>1</v>
@@ -27858,7 +27939,7 @@
         <v>815</v>
       </c>
       <c r="B157" s="3" t="s">
-        <v>1108</v>
+        <v>1112</v>
       </c>
       <c r="C157" s="5" t="b">
         <v>1</v>
@@ -27914,7 +27995,7 @@
         <v>818</v>
       </c>
       <c r="B158" s="3" t="s">
-        <v>1108</v>
+        <v>1112</v>
       </c>
       <c r="C158" s="5" t="b">
         <v>1</v>
@@ -27970,7 +28051,7 @@
         <v>821</v>
       </c>
       <c r="B159" s="3" t="s">
-        <v>1108</v>
+        <v>1112</v>
       </c>
       <c r="C159" s="5" t="b">
         <v>1</v>
@@ -28026,7 +28107,7 @@
         <v>824</v>
       </c>
       <c r="B160" s="3" t="s">
-        <v>1108</v>
+        <v>1112</v>
       </c>
       <c r="C160" s="5" t="b">
         <v>1</v>
@@ -28082,7 +28163,7 @@
         <v>827</v>
       </c>
       <c r="B161" s="3" t="s">
-        <v>1108</v>
+        <v>1112</v>
       </c>
       <c r="C161" s="5" t="b">
         <v>1</v>
@@ -28138,7 +28219,7 @@
         <v>830</v>
       </c>
       <c r="B162" s="3" t="s">
-        <v>1108</v>
+        <v>1112</v>
       </c>
       <c r="C162" s="5" t="b">
         <v>1</v>
@@ -28194,7 +28275,7 @@
         <v>833</v>
       </c>
       <c r="B163" s="3" t="s">
-        <v>1108</v>
+        <v>1112</v>
       </c>
       <c r="C163" s="5" t="b">
         <v>1</v>
@@ -28250,7 +28331,7 @@
         <v>836</v>
       </c>
       <c r="B164" s="3" t="s">
-        <v>1108</v>
+        <v>1112</v>
       </c>
       <c r="C164" s="5" t="b">
         <v>1</v>
@@ -28306,7 +28387,7 @@
         <v>839</v>
       </c>
       <c r="B165" s="3" t="s">
-        <v>1108</v>
+        <v>1112</v>
       </c>
       <c r="C165" s="5" t="b">
         <v>1</v>
@@ -28362,7 +28443,7 @@
         <v>842</v>
       </c>
       <c r="B166" s="3" t="s">
-        <v>1108</v>
+        <v>1112</v>
       </c>
       <c r="C166" s="5" t="b">
         <v>1</v>
@@ -28418,7 +28499,7 @@
         <v>845</v>
       </c>
       <c r="B167" s="3" t="s">
-        <v>1108</v>
+        <v>1112</v>
       </c>
       <c r="C167" s="5" t="b">
         <v>1</v>
@@ -28474,7 +28555,7 @@
         <v>848</v>
       </c>
       <c r="B168" s="3" t="s">
-        <v>1108</v>
+        <v>1112</v>
       </c>
       <c r="C168" s="5" t="b">
         <v>1</v>
@@ -28530,7 +28611,7 @@
         <v>851</v>
       </c>
       <c r="B169" s="3" t="s">
-        <v>1108</v>
+        <v>1112</v>
       </c>
       <c r="C169" s="5" t="b">
         <v>1</v>
@@ -28586,7 +28667,7 @@
         <v>854</v>
       </c>
       <c r="B170" s="3" t="s">
-        <v>1108</v>
+        <v>1112</v>
       </c>
       <c r="C170" s="5" t="b">
         <v>1</v>
@@ -28642,7 +28723,7 @@
         <v>857</v>
       </c>
       <c r="B171" s="3" t="s">
-        <v>1108</v>
+        <v>1112</v>
       </c>
       <c r="C171" s="5" t="b">
         <v>1</v>
@@ -28698,7 +28779,7 @@
         <v>860</v>
       </c>
       <c r="B172" s="3" t="s">
-        <v>1108</v>
+        <v>1112</v>
       </c>
       <c r="C172" s="5" t="b">
         <v>1</v>
@@ -28754,7 +28835,7 @@
         <v>863</v>
       </c>
       <c r="B173" s="3" t="s">
-        <v>1108</v>
+        <v>1112</v>
       </c>
       <c r="C173" s="5" t="b">
         <v>1</v>
@@ -28810,7 +28891,7 @@
         <v>866</v>
       </c>
       <c r="B174" s="3" t="s">
-        <v>1108</v>
+        <v>1112</v>
       </c>
       <c r="C174" s="5" t="b">
         <v>1</v>
@@ -28866,7 +28947,7 @@
         <v>869</v>
       </c>
       <c r="B175" s="3" t="s">
-        <v>1108</v>
+        <v>1112</v>
       </c>
       <c r="C175" s="5" t="b">
         <v>1</v>
@@ -28922,7 +29003,7 @@
         <v>872</v>
       </c>
       <c r="B176" s="3" t="s">
-        <v>1108</v>
+        <v>1112</v>
       </c>
       <c r="C176" s="5" t="b">
         <v>1</v>
@@ -28978,7 +29059,7 @@
         <v>875</v>
       </c>
       <c r="B177" s="3" t="s">
-        <v>1108</v>
+        <v>1112</v>
       </c>
       <c r="C177" s="5" t="b">
         <v>1</v>
@@ -29034,7 +29115,7 @@
         <v>878</v>
       </c>
       <c r="B178" s="3" t="s">
-        <v>1108</v>
+        <v>1112</v>
       </c>
       <c r="C178" s="5" t="b">
         <v>1</v>
@@ -29090,7 +29171,7 @@
         <v>881</v>
       </c>
       <c r="B179" s="3" t="s">
-        <v>1108</v>
+        <v>1112</v>
       </c>
       <c r="C179" s="5" t="b">
         <v>1</v>
@@ -29146,7 +29227,7 @@
         <v>884</v>
       </c>
       <c r="B180" s="3" t="s">
-        <v>1108</v>
+        <v>1112</v>
       </c>
       <c r="C180" s="5" t="b">
         <v>1</v>
@@ -29202,7 +29283,7 @@
         <v>886</v>
       </c>
       <c r="B181" s="3" t="s">
-        <v>1108</v>
+        <v>1112</v>
       </c>
       <c r="C181" s="5" t="b">
         <v>1</v>
@@ -29258,7 +29339,7 @@
         <v>889</v>
       </c>
       <c r="B182" s="3" t="s">
-        <v>1108</v>
+        <v>1112</v>
       </c>
       <c r="C182" s="5" t="b">
         <v>1</v>
@@ -29314,7 +29395,7 @@
         <v>891</v>
       </c>
       <c r="B183" s="3" t="s">
-        <v>1108</v>
+        <v>1112</v>
       </c>
       <c r="C183" s="5" t="b">
         <v>1</v>
@@ -29370,7 +29451,7 @@
         <v>893</v>
       </c>
       <c r="B184" s="3" t="s">
-        <v>1108</v>
+        <v>1112</v>
       </c>
       <c r="C184" s="5" t="b">
         <v>1</v>
@@ -29426,7 +29507,7 @@
         <v>895</v>
       </c>
       <c r="B185" s="3" t="s">
-        <v>1108</v>
+        <v>1112</v>
       </c>
       <c r="C185" s="5" t="b">
         <v>1</v>
@@ -29482,7 +29563,7 @@
         <v>898</v>
       </c>
       <c r="B186" s="3" t="s">
-        <v>1108</v>
+        <v>1112</v>
       </c>
       <c r="C186" s="5" t="b">
         <v>1</v>
@@ -29538,7 +29619,7 @@
         <v>904</v>
       </c>
       <c r="B187" s="3" t="s">
-        <v>1108</v>
+        <v>1112</v>
       </c>
       <c r="C187" s="5" t="b">
         <v>1</v>
@@ -29594,7 +29675,7 @@
         <v>915</v>
       </c>
       <c r="B188" s="3" t="s">
-        <v>1108</v>
+        <v>1112</v>
       </c>
       <c r="C188" s="5" t="b">
         <v>1</v>
@@ -29706,7 +29787,7 @@
         <v>929</v>
       </c>
       <c r="B190" s="3" t="s">
-        <v>1108</v>
+        <v>1112</v>
       </c>
       <c r="C190" s="5" t="b">
         <v>1</v>
@@ -29818,7 +29899,7 @@
         <v>948</v>
       </c>
       <c r="B192" s="3" t="s">
-        <v>1108</v>
+        <v>1112</v>
       </c>
       <c r="C192" s="5" t="b">
         <v>1</v>
@@ -29874,7 +29955,7 @@
         <v>956</v>
       </c>
       <c r="B193" s="3" t="s">
-        <v>1108</v>
+        <v>1112</v>
       </c>
       <c r="C193" s="5" t="b">
         <v>1</v>
@@ -29930,7 +30011,7 @@
         <v>958</v>
       </c>
       <c r="B194" s="3" t="s">
-        <v>1108</v>
+        <v>1112</v>
       </c>
       <c r="C194" s="5" t="b">
         <v>1</v>
@@ -29986,7 +30067,7 @@
         <v>965</v>
       </c>
       <c r="B195" s="3" t="s">
-        <v>1108</v>
+        <v>1112</v>
       </c>
       <c r="C195" s="5" t="b">
         <v>1</v>
@@ -30042,7 +30123,7 @@
         <v>967</v>
       </c>
       <c r="B196" s="3" t="s">
-        <v>1108</v>
+        <v>1112</v>
       </c>
       <c r="C196" s="5" t="b">
         <v>1</v>
@@ -30098,7 +30179,7 @@
         <v>977</v>
       </c>
       <c r="B197" s="3" t="s">
-        <v>1108</v>
+        <v>1112</v>
       </c>
       <c r="C197" s="5" t="b">
         <v>1</v>
@@ -30154,7 +30235,7 @@
         <v>983</v>
       </c>
       <c r="B198" s="3" t="s">
-        <v>1108</v>
+        <v>1112</v>
       </c>
       <c r="C198" s="5" t="b">
         <v>1</v>
@@ -30210,7 +30291,7 @@
         <v>986</v>
       </c>
       <c r="B199" s="3" t="s">
-        <v>1108</v>
+        <v>1112</v>
       </c>
       <c r="C199" s="5" t="b">
         <v>1</v>
@@ -30266,7 +30347,7 @@
         <v>994</v>
       </c>
       <c r="B200" s="3" t="s">
-        <v>1108</v>
+        <v>1112</v>
       </c>
       <c r="C200" s="5" t="b">
         <v>1</v>
@@ -30322,7 +30403,7 @@
         <v>998</v>
       </c>
       <c r="B201" s="3" t="s">
-        <v>1108</v>
+        <v>1112</v>
       </c>
       <c r="C201" s="5" t="b">
         <v>1</v>
@@ -30378,7 +30459,7 @@
         <v>1008</v>
       </c>
       <c r="B202" s="3" t="s">
-        <v>1108</v>
+        <v>1112</v>
       </c>
       <c r="C202" s="5" t="b">
         <v>1</v>
@@ -30434,7 +30515,7 @@
         <v>1014</v>
       </c>
       <c r="B203" s="3" t="s">
-        <v>1108</v>
+        <v>1112</v>
       </c>
       <c r="C203" s="5" t="b">
         <v>1</v>
@@ -30490,7 +30571,7 @@
         <v>1017</v>
       </c>
       <c r="B204" s="3" t="s">
-        <v>1108</v>
+        <v>1112</v>
       </c>
       <c r="C204" s="5" t="b">
         <v>1</v>
@@ -30546,7 +30627,7 @@
         <v>1020</v>
       </c>
       <c r="B205" s="3" t="s">
-        <v>1108</v>
+        <v>1112</v>
       </c>
       <c r="C205" s="5" t="b">
         <v>1</v>
@@ -30602,7 +30683,7 @@
         <v>1027</v>
       </c>
       <c r="B206" s="3" t="s">
-        <v>1108</v>
+        <v>1112</v>
       </c>
       <c r="C206" s="5" t="b">
         <v>1</v>
@@ -30658,7 +30739,7 @@
         <v>1034</v>
       </c>
       <c r="B207" s="3" t="s">
-        <v>1108</v>
+        <v>1112</v>
       </c>
       <c r="C207" s="5" t="b">
         <v>1</v>
@@ -30714,7 +30795,7 @@
         <v>1040</v>
       </c>
       <c r="B208" s="3" t="s">
-        <v>1108</v>
+        <v>1112</v>
       </c>
       <c r="C208" s="5" t="b">
         <v>1</v>
@@ -30770,7 +30851,7 @@
         <v>1042</v>
       </c>
       <c r="B209" s="3" t="s">
-        <v>1108</v>
+        <v>1112</v>
       </c>
       <c r="C209" s="5" t="b">
         <v>1</v>
@@ -30826,7 +30907,7 @@
         <v>1053</v>
       </c>
       <c r="B210" s="3" t="s">
-        <v>1108</v>
+        <v>1112</v>
       </c>
       <c r="C210" s="5" t="b">
         <v>1</v>
@@ -30882,7 +30963,7 @@
         <v>1055</v>
       </c>
       <c r="B211" s="3" t="s">
-        <v>1108</v>
+        <v>1112</v>
       </c>
       <c r="C211" s="5" t="b">
         <v>1</v>
@@ -30938,7 +31019,7 @@
         <v>1061</v>
       </c>
       <c r="B212" s="3" t="s">
-        <v>1108</v>
+        <v>1112</v>
       </c>
       <c r="C212" s="5" t="b">
         <v>1</v>
@@ -30994,7 +31075,7 @@
         <v>1063</v>
       </c>
       <c r="B213" s="3" t="s">
-        <v>1108</v>
+        <v>1112</v>
       </c>
       <c r="C213" s="5" t="b">
         <v>1</v>
@@ -31050,7 +31131,7 @@
         <v>1075</v>
       </c>
       <c r="B214" s="3" t="s">
-        <v>1108</v>
+        <v>1112</v>
       </c>
       <c r="C214" s="5" t="b">
         <v>1</v>
@@ -31106,7 +31187,7 @@
         <v>1077</v>
       </c>
       <c r="B215" s="3" t="s">
-        <v>1108</v>
+        <v>1112</v>
       </c>
       <c r="C215" s="5" t="b">
         <v>1</v>
@@ -31162,7 +31243,7 @@
         <v>1080</v>
       </c>
       <c r="B216" s="3" t="s">
-        <v>1108</v>
+        <v>1112</v>
       </c>
       <c r="C216" s="5" t="b">
         <v>1</v>
@@ -31218,7 +31299,7 @@
         <v>1089</v>
       </c>
       <c r="B217" s="3" t="s">
-        <v>1108</v>
+        <v>1112</v>
       </c>
       <c r="C217" s="5" t="b">
         <v>1</v>
@@ -31274,7 +31355,7 @@
         <v>1092</v>
       </c>
       <c r="B218" s="3" t="s">
-        <v>1108</v>
+        <v>1112</v>
       </c>
       <c r="C218" s="5" t="b">
         <v>1</v>
@@ -31330,7 +31411,7 @@
         <v>1095</v>
       </c>
       <c r="B219" s="3" t="s">
-        <v>1108</v>
+        <v>1112</v>
       </c>
       <c r="C219" s="5" t="b">
         <v>1</v>
@@ -31386,7 +31467,7 @@
         <v>1098</v>
       </c>
       <c r="B220" s="3" t="s">
-        <v>1108</v>
+        <v>1112</v>
       </c>
       <c r="C220" s="5" t="b">
         <v>1</v>
@@ -31442,54 +31523,110 @@
         <v>1105</v>
       </c>
       <c r="B221" s="3" t="s">
+        <v>1112</v>
+      </c>
+      <c r="C221" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="D221" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="E221" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="F221" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="G221" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="H221" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="I221" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="J221" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="K221" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="L221" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="M221" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="N221" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="O221" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="P221" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q221" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="R221" s="6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="222" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A222" s="3" t="s">
         <v>1108</v>
       </c>
-      <c r="C221" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="D221" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="E221" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="F221" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="G221" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="H221" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="I221" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="J221" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="K221" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="L221" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="M221" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="N221" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="O221" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="P221" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q221" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="R221" s="6" t="b">
+      <c r="B222" s="3" t="s">
+        <v>1112</v>
+      </c>
+      <c r="C222" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="D222" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="E222" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="F222" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="G222" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="H222" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="I222" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="J222" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="K222" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="L222" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="M222" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="N222" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="O222" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="P222" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q222" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="R222" s="6" t="b">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
generated all the reports on 2024-04-16
</commit_message>
<xml_diff>
--- a/report/merged_configurations.xlsx
+++ b/report/merged_configurations.xlsx
@@ -437,7 +437,7 @@
     <t>Databank Ondergrond Vlaanderen en OVAM</t>
   </si>
   <si>
-    <t>http://data.vlaanderen.be/id/organisatie/OVO037637</t>
+    <t>https://data.vlaanderen.be/id/organisatie/OVO027735</t>
   </si>
   <si>
     <t>bodemenondergrond.md</t>
@@ -461,7 +461,7 @@
     <t>18 juni 2020</t>
   </si>
   <si>
-    <t>[{"verantwoordelijke":"Databank Ondergrond Vlaanderen","identificator":"http://data.vlaanderen.be/id/organisatie/OVO037637"},{"verantwoordelijke":"OVAM","identificator":"http://data.vlaanderen.be/id/organisatie/OVO000091"}]</t>
+    <t>[{"verantwoordelijke":"Databank Ondergrond Vlaanderen","identificator":"https://data.vlaanderen.be/id/organisatie/OVO027735"},{"verantwoordelijke":"OVAM","identificator":"https://data.vlaanderen.be/id/organisatie/OVO000091"}]</t>
   </si>
   <si>
     <t>Vocabularium Bodem</t>
@@ -3128,7 +3128,7 @@
     <t xml:space="preserve">Applicatieprofiel Mobiliteitsbudget </t>
   </si>
   <si>
-    <t>[{"naam":"Applicatieprofiel Mobiliteitsbudget","waarde":"https://test.data.vlaanderen.be/doc/applicatieprofiel/mobiliteitsbudget/"},{"naam":"Vocabularium Mobiliteitsbudget","waarde":"https://test.data.vlaanderen.be/ns/mobiliteitsbudget/"}]</t>
+    <t>[{"naam":"Applicatieprofiel Mobiliteitsbudget","waarde":"https://data.vlaanderen.be/doc/applicatieprofiel/mobiliteitsbudget/"},{"naam":"Vocabularium Mobiliteitsbudget","waarde":"https://data.vlaanderen.be/ns/mobiliteitsbudget/"}]</t>
   </si>
   <si>
     <t>[{"naam":"Modificatie Mobiliteitsbudget - datum","waarde":"link"}]</t>

</xml_diff>

<commit_message>
generated all the reports on 2024-04-18
</commit_message>
<xml_diff>
--- a/report/merged_configurations.xlsx
+++ b/report/merged_configurations.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5241" uniqueCount="1136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5245" uniqueCount="1136">
   <si>
     <t>naam</t>
   </si>
@@ -3143,13 +3143,13 @@
     <t>[{"naam":"Vocabularium Mobiliteitsbudget","waarde":"https://data.vlaanderen.be/ns/mobiliteitsbudget/"}]</t>
   </si>
   <si>
-    <t>[{"naam":"Charter","waarde":"charter-OSLO-Mobiliteitsbudget.pdf"}]</t>
+    <t>[{"naam":"Charter Mobiliteitsbudget","waarde":"charter-OSLO-Mobiliteitsbudget.pdf"}]</t>
   </si>
   <si>
     <t>[{"naam":"Verslag business werkgroep - 7 december 2022 ","waarde":"Verslag Business Workshop Mobiliteitsbudget.docx.pdf"},{"naam":"Verslag Thematische Werkgroep 1 - 11 januari 2023","waarde":"11012023_OSLO Mobiliteitsbudget_Thematische Werkgroep 1_Verslag.pdf"},{"naam":"Verslag Thematische Werkgroep 2 - 8 februari 2023","waarde":"08022023-Verslag-Thematische-Werkgroep-2-OSLO-Mobiliteitsbudget.pdf"}]</t>
   </si>
   <si>
-    <t>[{"naam":"Presentatie business werkgroep - 7 december 2022","waarde":"07122022-Business Werkgroep presentatie - MOBURGER.pptx.pdf"},{"naam":"Presentatie thematische werkgroep - 11 januari 2023 ","waarde":"11012023_OSLO Mobiliteitsbudget_Thematische Werkgroep 1_Verslag.pdf"}]</t>
+    <t>[{"naam":"Presentatie business werkgroep - 7 december 2022","waarde":"07122022-Business Werkgroep presentatie - MOBURGER.pptx.pdf"},{"naam":"Presentatie thematische werkgroep 1 - 11 januari 2023 ","waarde":"11012023_OSLO Mobiliteitsbudget_Thematische Werkgroep 1_Verslag.pdf"}]</t>
   </si>
   <si>
     <t>Semantische standaard voor informatie over Mobiliteitsbudget</t>
@@ -18230,8 +18230,12 @@
       <c r="P207" s="3" t="s">
         <v>1047</v>
       </c>
-      <c r="Q207" s="3"/>
-      <c r="R207" s="3"/>
+      <c r="Q207" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="R207" s="3" t="s">
+        <v>26</v>
+      </c>
       <c r="S207" s="3" t="s">
         <v>37</v>
       </c>
@@ -18295,8 +18299,12 @@
       <c r="P208" s="3" t="s">
         <v>1047</v>
       </c>
-      <c r="Q208" s="3"/>
-      <c r="R208" s="3"/>
+      <c r="Q208" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="R208" s="3" t="s">
+        <v>26</v>
+      </c>
       <c r="S208" s="3" t="s">
         <v>37</v>
       </c>

</xml_diff>

<commit_message>
generated all the reports on 2024-04-24
</commit_message>
<xml_diff>
--- a/report/merged_configurations.xlsx
+++ b/report/merged_configurations.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5245" uniqueCount="1136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5250" uniqueCount="1141">
   <si>
     <t>naam</t>
   </si>
@@ -3308,13 +3308,28 @@
     <t>[{"naam":"Vocabularium Overlijdensaangifte","waarde":"https://data.vlaanderen.be/ns/overlijdensaangifte"},{"naam":"Applicatieprofiel Overlijdensaangifte","waarde":"https://data.vlaanderen.be/doc/applicatieprofiel/overlijdensaangifte"}]</t>
   </si>
   <si>
-    <t>Applicatieprofiel Kind fiche</t>
+    <t>Applicatieprofiel Kindfiche</t>
   </si>
   <si>
     <t>kind-fiche-description.md</t>
   </si>
   <si>
-    <t>[{"naam":"Kind fiche applicatieprofiel","waarde":"https://data.test-vlaanderen.be/doc/applicatieprofiel/kind-fiche/ontwerpstandaard/2024-03-19/"}]</t>
+    <t>[{"naam":"Applicatieprofiel Kindfiche","waarde":"https://data.test-vlaanderen.be/doc/applicatieprofiel/kind-fiche/ontwerpstandaard/2024-03-19/"}]</t>
+  </si>
+  <si>
+    <t>[{"naam":"Charter Kindfiche","waarde":"Werkgroep charter OSLO_Kindfiche.pdf"}]</t>
+  </si>
+  <si>
+    <t>[{"naam":"Verslag Business Werkgroep - 13 februari 2024","waarde":"2.0 Business Werkgroep presentatie Kindfiche (1).pdf"},{"naam":"Verslag Thematische Werkgroep I - 12 maart 2024","waarde":"Thematische werkgroep 1 presentatie Kindfiche (1).pdf"},{"naam":"Verslag Thematische Werkgroep II - 9 april 2024","waarde":"Thematische werkgroep 2 presentatie Kindfiche.pdf"}]</t>
+  </si>
+  <si>
+    <t>[{"naam":"Presentatie Business Werkgroep -  13 februari 2024","waarde":"20240116_ThematicWorkshop1_Powerpoint_OSLOOverlijdensaangifte.pptx"},{"naam":"Presentatie Thematische Werkgroep I - 12 maart 2024","waarde":"20240116_ThematicWorkshop1_Powerpoint_OSLOOverlijdensaangifte.pptx"},{"naam":"Presentatie Thematische Werkgroep II - 9 april 2024","waarde":"20240220_ThematicWorkshop2_Powerpoint_OSLOOverlijdensaangifte.pptx"}]</t>
+  </si>
+  <si>
+    <t>Lokale besturen, alle entiteiten van de Vlaamse overheid, zorgsector</t>
+  </si>
+  <si>
+    <t>19 december 2024</t>
   </si>
   <si>
     <t>Vocabularium OSLO Statistiek</t>
@@ -18960,19 +18975,29 @@
         <v>31</v>
       </c>
       <c r="K218" s="3" t="s">
-        <v>31</v>
+        <v>1101</v>
       </c>
       <c r="L218" s="3" t="s">
-        <v>31</v>
+        <v>1102</v>
       </c>
       <c r="M218" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="N218" s="3"/>
-      <c r="O218" s="3"/>
-      <c r="P218" s="3"/>
-      <c r="Q218" s="3"/>
-      <c r="R218" s="3"/>
+        <v>1103</v>
+      </c>
+      <c r="N218" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="O218" s="3" t="s">
+        <v>1104</v>
+      </c>
+      <c r="P218" s="3" t="s">
+        <v>1105</v>
+      </c>
+      <c r="Q218" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="R218" s="3" t="s">
+        <v>26</v>
+      </c>
       <c r="S218" s="3" t="s">
         <v>37</v>
       </c>
@@ -18991,17 +19016,17 @@
     </row>
     <row r="219" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A219" s="3" t="s">
-        <v>1101</v>
+        <v>1106</v>
       </c>
       <c r="B219" s="3"/>
       <c r="C219" s="3" t="s">
-        <v>1102</v>
+        <v>1107</v>
       </c>
       <c r="D219" s="3" t="s">
-        <v>1103</v>
+        <v>1108</v>
       </c>
       <c r="E219" s="3" t="s">
-        <v>1104</v>
+        <v>1109</v>
       </c>
       <c r="F219" s="3" t="s">
         <v>43</v>
@@ -19010,31 +19035,31 @@
         <v>39</v>
       </c>
       <c r="H219" s="3" t="s">
-        <v>1105</v>
+        <v>1110</v>
       </c>
       <c r="I219" s="3" t="s">
-        <v>1106</v>
+        <v>1111</v>
       </c>
       <c r="J219" s="3" t="s">
-        <v>1107</v>
+        <v>1112</v>
       </c>
       <c r="K219" s="3" t="s">
         <v>31</v>
       </c>
       <c r="L219" s="3" t="s">
-        <v>1107</v>
+        <v>1112</v>
       </c>
       <c r="M219" s="3" t="s">
-        <v>1107</v>
+        <v>1112</v>
       </c>
       <c r="N219" s="3" t="s">
-        <v>1108</v>
+        <v>1113</v>
       </c>
       <c r="O219" s="3" t="s">
         <v>70</v>
       </c>
       <c r="P219" s="3" t="s">
-        <v>1109</v>
+        <v>1114</v>
       </c>
       <c r="Q219" s="3" t="s">
         <v>26</v>
@@ -19060,17 +19085,17 @@
     </row>
     <row r="220" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A220" s="3" t="s">
-        <v>1110</v>
+        <v>1115</v>
       </c>
       <c r="B220" s="3"/>
       <c r="C220" s="3" t="s">
-        <v>1102</v>
+        <v>1107</v>
       </c>
       <c r="D220" s="3" t="s">
-        <v>1103</v>
+        <v>1108</v>
       </c>
       <c r="E220" s="3" t="s">
-        <v>1104</v>
+        <v>1109</v>
       </c>
       <c r="F220" s="3" t="s">
         <v>43</v>
@@ -19079,31 +19104,31 @@
         <v>28</v>
       </c>
       <c r="H220" s="3" t="s">
-        <v>1111</v>
+        <v>1116</v>
       </c>
       <c r="I220" s="3" t="s">
+        <v>1117</v>
+      </c>
+      <c r="J220" s="3" t="s">
         <v>1112</v>
       </c>
-      <c r="J220" s="3" t="s">
-        <v>1107</v>
-      </c>
       <c r="K220" s="3" t="s">
         <v>31</v>
       </c>
       <c r="L220" s="3" t="s">
-        <v>1107</v>
+        <v>1112</v>
       </c>
       <c r="M220" s="3" t="s">
-        <v>1107</v>
+        <v>1112</v>
       </c>
       <c r="N220" s="3" t="s">
-        <v>1108</v>
+        <v>1113</v>
       </c>
       <c r="O220" s="3" t="s">
         <v>70</v>
       </c>
       <c r="P220" s="3" t="s">
-        <v>1109</v>
+        <v>1114</v>
       </c>
       <c r="Q220" s="3" t="s">
         <v>26</v>
@@ -19129,17 +19154,17 @@
     </row>
     <row r="221" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A221" s="3" t="s">
-        <v>1113</v>
+        <v>1118</v>
       </c>
       <c r="B221" s="3"/>
       <c r="C221" s="3" t="s">
-        <v>1102</v>
+        <v>1107</v>
       </c>
       <c r="D221" s="3" t="s">
-        <v>1103</v>
+        <v>1108</v>
       </c>
       <c r="E221" s="3" t="s">
-        <v>1104</v>
+        <v>1109</v>
       </c>
       <c r="F221" s="3" t="s">
         <v>43</v>
@@ -19148,31 +19173,31 @@
         <v>39</v>
       </c>
       <c r="H221" s="3" t="s">
-        <v>1114</v>
+        <v>1119</v>
       </c>
       <c r="I221" s="3" t="s">
-        <v>1115</v>
+        <v>1120</v>
       </c>
       <c r="J221" s="3" t="s">
-        <v>1107</v>
+        <v>1112</v>
       </c>
       <c r="K221" s="3" t="s">
         <v>31</v>
       </c>
       <c r="L221" s="3" t="s">
-        <v>1107</v>
+        <v>1112</v>
       </c>
       <c r="M221" s="3" t="s">
-        <v>1107</v>
+        <v>1112</v>
       </c>
       <c r="N221" s="3" t="s">
-        <v>1108</v>
+        <v>1113</v>
       </c>
       <c r="O221" s="3" t="s">
         <v>70</v>
       </c>
       <c r="P221" s="3" t="s">
-        <v>1109</v>
+        <v>1114</v>
       </c>
       <c r="Q221" s="3" t="s">
         <v>26</v>
@@ -19198,17 +19223,17 @@
     </row>
     <row r="222" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A222" s="3" t="s">
-        <v>1116</v>
+        <v>1121</v>
       </c>
       <c r="B222" s="3"/>
       <c r="C222" s="3" t="s">
-        <v>1102</v>
+        <v>1107</v>
       </c>
       <c r="D222" s="3" t="s">
-        <v>1103</v>
+        <v>1108</v>
       </c>
       <c r="E222" s="3" t="s">
-        <v>1104</v>
+        <v>1109</v>
       </c>
       <c r="F222" s="3" t="s">
         <v>43</v>
@@ -19217,31 +19242,31 @@
         <v>28</v>
       </c>
       <c r="H222" s="3" t="s">
-        <v>1117</v>
+        <v>1122</v>
       </c>
       <c r="I222" s="3" t="s">
-        <v>1118</v>
+        <v>1123</v>
       </c>
       <c r="J222" s="3" t="s">
-        <v>1107</v>
+        <v>1112</v>
       </c>
       <c r="K222" s="3" t="s">
         <v>31</v>
       </c>
       <c r="L222" s="3" t="s">
-        <v>1107</v>
+        <v>1112</v>
       </c>
       <c r="M222" s="3" t="s">
-        <v>1107</v>
+        <v>1112</v>
       </c>
       <c r="N222" s="3" t="s">
-        <v>1108</v>
+        <v>1113</v>
       </c>
       <c r="O222" s="3" t="s">
         <v>70</v>
       </c>
       <c r="P222" s="3" t="s">
-        <v>1109</v>
+        <v>1114</v>
       </c>
       <c r="Q222" s="3" t="s">
         <v>26</v>
@@ -19267,17 +19292,17 @@
     </row>
     <row r="223" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A223" s="3" t="s">
-        <v>1119</v>
+        <v>1124</v>
       </c>
       <c r="B223" s="3"/>
       <c r="C223" s="3" t="s">
-        <v>1102</v>
+        <v>1107</v>
       </c>
       <c r="D223" s="3" t="s">
-        <v>1103</v>
+        <v>1108</v>
       </c>
       <c r="E223" s="3" t="s">
-        <v>1104</v>
+        <v>1109</v>
       </c>
       <c r="F223" s="3" t="s">
         <v>43</v>
@@ -19286,31 +19311,31 @@
         <v>28</v>
       </c>
       <c r="H223" s="3" t="s">
-        <v>1120</v>
+        <v>1125</v>
       </c>
       <c r="I223" s="3" t="s">
-        <v>1121</v>
+        <v>1126</v>
       </c>
       <c r="J223" s="3" t="s">
-        <v>1122</v>
+        <v>1127</v>
       </c>
       <c r="K223" s="3" t="s">
         <v>31</v>
       </c>
       <c r="L223" s="3" t="s">
-        <v>1123</v>
+        <v>1128</v>
       </c>
       <c r="M223" s="3" t="s">
-        <v>1124</v>
+        <v>1129</v>
       </c>
       <c r="N223" s="3" t="s">
-        <v>1125</v>
+        <v>1130</v>
       </c>
       <c r="O223" s="3" t="s">
         <v>97</v>
       </c>
       <c r="P223" s="3" t="s">
-        <v>1109</v>
+        <v>1114</v>
       </c>
       <c r="Q223" s="3" t="s">
         <v>26</v>
@@ -19336,17 +19361,17 @@
     </row>
     <row r="224" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A224" s="3" t="s">
-        <v>1126</v>
+        <v>1131</v>
       </c>
       <c r="B224" s="3"/>
       <c r="C224" s="3" t="s">
-        <v>1102</v>
+        <v>1107</v>
       </c>
       <c r="D224" s="3" t="s">
-        <v>1103</v>
+        <v>1108</v>
       </c>
       <c r="E224" s="3" t="s">
-        <v>1104</v>
+        <v>1109</v>
       </c>
       <c r="F224" s="3" t="s">
         <v>43</v>
@@ -19355,31 +19380,31 @@
         <v>39</v>
       </c>
       <c r="H224" s="3" t="s">
+        <v>1132</v>
+      </c>
+      <c r="I224" s="3" t="s">
+        <v>1133</v>
+      </c>
+      <c r="J224" s="3" t="s">
         <v>1127</v>
       </c>
-      <c r="I224" s="3" t="s">
+      <c r="K224" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="L224" s="3" t="s">
         <v>1128</v>
       </c>
-      <c r="J224" s="3" t="s">
-        <v>1122</v>
-      </c>
-      <c r="K224" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="L224" s="3" t="s">
-        <v>1123</v>
-      </c>
       <c r="M224" s="3" t="s">
-        <v>1124</v>
+        <v>1129</v>
       </c>
       <c r="N224" s="3" t="s">
-        <v>1125</v>
+        <v>1130</v>
       </c>
       <c r="O224" s="3" t="s">
         <v>97</v>
       </c>
       <c r="P224" s="3" t="s">
-        <v>1109</v>
+        <v>1114</v>
       </c>
       <c r="Q224" s="3" t="s">
         <v>26</v>
@@ -19405,7 +19430,7 @@
     </row>
     <row r="225" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A225" s="3" t="s">
-        <v>1129</v>
+        <v>1134</v>
       </c>
       <c r="B225" s="3"/>
       <c r="C225" s="3" t="s">
@@ -19424,10 +19449,10 @@
         <v>28</v>
       </c>
       <c r="H225" s="3" t="s">
-        <v>1130</v>
+        <v>1135</v>
       </c>
       <c r="I225" s="3" t="s">
-        <v>1131</v>
+        <v>1136</v>
       </c>
       <c r="J225" s="3" t="s">
         <v>31</v>
@@ -19436,13 +19461,13 @@
         <v>31</v>
       </c>
       <c r="L225" s="3" t="s">
-        <v>1132</v>
+        <v>1137</v>
       </c>
       <c r="M225" s="3" t="s">
-        <v>1133</v>
+        <v>1138</v>
       </c>
       <c r="N225" s="3" t="s">
-        <v>1134</v>
+        <v>1139</v>
       </c>
       <c r="O225" s="3" t="s">
         <v>70</v>
@@ -19547,7 +19572,7 @@
         <v>23</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>1135</v>
+        <v>1140</v>
       </c>
       <c r="C2" s="5" t="b">
         <v>1</v>
@@ -19603,7 +19628,7 @@
         <v>38</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>1135</v>
+        <v>1140</v>
       </c>
       <c r="C3" s="5" t="b">
         <v>1</v>
@@ -19659,7 +19684,7 @@
         <v>41</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>1135</v>
+        <v>1140</v>
       </c>
       <c r="C4" s="5" t="b">
         <v>1</v>
@@ -19715,7 +19740,7 @@
         <v>53</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>1135</v>
+        <v>1140</v>
       </c>
       <c r="C5" s="5" t="b">
         <v>1</v>
@@ -19771,7 +19796,7 @@
         <v>60</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>1135</v>
+        <v>1140</v>
       </c>
       <c r="C6" s="5" t="b">
         <v>1</v>
@@ -19827,7 +19852,7 @@
         <v>63</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>1135</v>
+        <v>1140</v>
       </c>
       <c r="C7" s="5" t="b">
         <v>1</v>
@@ -19883,7 +19908,7 @@
         <v>72</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>1135</v>
+        <v>1140</v>
       </c>
       <c r="C8" s="5" t="b">
         <v>1</v>
@@ -19939,7 +19964,7 @@
         <v>74</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>1135</v>
+        <v>1140</v>
       </c>
       <c r="C9" s="5" t="b">
         <v>1</v>
@@ -19995,7 +20020,7 @@
         <v>81</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>1135</v>
+        <v>1140</v>
       </c>
       <c r="C10" s="5" t="b">
         <v>1</v>
@@ -20051,7 +20076,7 @@
         <v>83</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>1135</v>
+        <v>1140</v>
       </c>
       <c r="C11" s="5" t="b">
         <v>1</v>
@@ -20107,7 +20132,7 @@
         <v>90</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>1135</v>
+        <v>1140</v>
       </c>
       <c r="C12" s="5" t="b">
         <v>1</v>
@@ -20163,7 +20188,7 @@
         <v>100</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>1135</v>
+        <v>1140</v>
       </c>
       <c r="C13" s="5" t="b">
         <v>1</v>
@@ -20219,7 +20244,7 @@
         <v>103</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>1135</v>
+        <v>1140</v>
       </c>
       <c r="C14" s="5" t="b">
         <v>1</v>
@@ -20275,7 +20300,7 @@
         <v>113</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>1135</v>
+        <v>1140</v>
       </c>
       <c r="C15" s="5" t="b">
         <v>1</v>
@@ -20443,7 +20468,7 @@
         <v>139</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>1135</v>
+        <v>1140</v>
       </c>
       <c r="C18" s="5" t="b">
         <v>1</v>
@@ -20499,7 +20524,7 @@
         <v>150</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>1135</v>
+        <v>1140</v>
       </c>
       <c r="C19" s="5" t="b">
         <v>1</v>
@@ -20555,7 +20580,7 @@
         <v>152</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>1135</v>
+        <v>1140</v>
       </c>
       <c r="C20" s="5" t="b">
         <v>1</v>
@@ -20611,7 +20636,7 @@
         <v>154</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>1135</v>
+        <v>1140</v>
       </c>
       <c r="C21" s="5" t="b">
         <v>1</v>
@@ -20667,7 +20692,7 @@
         <v>156</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>1135</v>
+        <v>1140</v>
       </c>
       <c r="C22" s="5" t="b">
         <v>1</v>
@@ -20723,7 +20748,7 @@
         <v>159</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>1135</v>
+        <v>1140</v>
       </c>
       <c r="C23" s="5" t="b">
         <v>1</v>
@@ -20779,7 +20804,7 @@
         <v>161</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>1135</v>
+        <v>1140</v>
       </c>
       <c r="C24" s="5" t="b">
         <v>1</v>
@@ -20835,7 +20860,7 @@
         <v>163</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>1135</v>
+        <v>1140</v>
       </c>
       <c r="C25" s="5" t="b">
         <v>1</v>
@@ -20891,7 +20916,7 @@
         <v>165</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>1135</v>
+        <v>1140</v>
       </c>
       <c r="C26" s="5" t="b">
         <v>1</v>
@@ -20947,7 +20972,7 @@
         <v>167</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>1135</v>
+        <v>1140</v>
       </c>
       <c r="C27" s="5" t="b">
         <v>1</v>
@@ -21003,7 +21028,7 @@
         <v>169</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>1135</v>
+        <v>1140</v>
       </c>
       <c r="C28" s="5" t="b">
         <v>1</v>
@@ -21059,7 +21084,7 @@
         <v>167</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>1135</v>
+        <v>1140</v>
       </c>
       <c r="C29" s="5" t="b">
         <v>1</v>
@@ -21115,7 +21140,7 @@
         <v>171</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>1135</v>
+        <v>1140</v>
       </c>
       <c r="C30" s="5" t="b">
         <v>1</v>
@@ -21171,7 +21196,7 @@
         <v>173</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>1135</v>
+        <v>1140</v>
       </c>
       <c r="C31" s="5" t="b">
         <v>1</v>
@@ -21227,7 +21252,7 @@
         <v>175</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>1135</v>
+        <v>1140</v>
       </c>
       <c r="C32" s="5" t="b">
         <v>1</v>
@@ -21283,7 +21308,7 @@
         <v>177</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>1135</v>
+        <v>1140</v>
       </c>
       <c r="C33" s="5" t="b">
         <v>1</v>
@@ -21339,7 +21364,7 @@
         <v>179</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>1135</v>
+        <v>1140</v>
       </c>
       <c r="C34" s="5" t="b">
         <v>1</v>
@@ -21395,7 +21420,7 @@
         <v>181</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>1135</v>
+        <v>1140</v>
       </c>
       <c r="C35" s="5" t="b">
         <v>1</v>
@@ -21451,7 +21476,7 @@
         <v>183</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>1135</v>
+        <v>1140</v>
       </c>
       <c r="C36" s="5" t="b">
         <v>1</v>
@@ -21507,7 +21532,7 @@
         <v>185</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>1135</v>
+        <v>1140</v>
       </c>
       <c r="C37" s="5" t="b">
         <v>1</v>
@@ -21563,7 +21588,7 @@
         <v>187</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>1135</v>
+        <v>1140</v>
       </c>
       <c r="C38" s="5" t="b">
         <v>1</v>
@@ -21731,7 +21756,7 @@
         <v>217</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>1135</v>
+        <v>1140</v>
       </c>
       <c r="C41" s="5" t="b">
         <v>1</v>
@@ -21787,7 +21812,7 @@
         <v>225</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>1135</v>
+        <v>1140</v>
       </c>
       <c r="C42" s="5" t="b">
         <v>1</v>
@@ -23355,7 +23380,7 @@
         <v>407</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>1135</v>
+        <v>1140</v>
       </c>
       <c r="C70" s="5" t="b">
         <v>1</v>
@@ -23411,7 +23436,7 @@
         <v>419</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>1135</v>
+        <v>1140</v>
       </c>
       <c r="C71" s="5" t="b">
         <v>1</v>
@@ -23859,7 +23884,7 @@
         <v>478</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>1135</v>
+        <v>1140</v>
       </c>
       <c r="C79" s="5" t="b">
         <v>1</v>
@@ -24531,7 +24556,7 @@
         <v>559</v>
       </c>
       <c r="B91" s="3" t="s">
-        <v>1135</v>
+        <v>1140</v>
       </c>
       <c r="C91" s="5" t="b">
         <v>1</v>
@@ -24587,7 +24612,7 @@
         <v>568</v>
       </c>
       <c r="B92" s="3" t="s">
-        <v>1135</v>
+        <v>1140</v>
       </c>
       <c r="C92" s="5" t="b">
         <v>1</v>
@@ -24643,7 +24668,7 @@
         <v>570</v>
       </c>
       <c r="B93" s="3" t="s">
-        <v>1135</v>
+        <v>1140</v>
       </c>
       <c r="C93" s="5" t="b">
         <v>1</v>
@@ -26771,7 +26796,7 @@
         <v>723</v>
       </c>
       <c r="B131" s="3" t="s">
-        <v>1135</v>
+        <v>1140</v>
       </c>
       <c r="C131" s="5" t="b">
         <v>1</v>
@@ -27331,7 +27356,7 @@
         <v>755</v>
       </c>
       <c r="B141" s="3" t="s">
-        <v>1135</v>
+        <v>1140</v>
       </c>
       <c r="C141" s="5" t="b">
         <v>1</v>
@@ -27387,7 +27412,7 @@
         <v>761</v>
       </c>
       <c r="B142" s="3" t="s">
-        <v>1135</v>
+        <v>1140</v>
       </c>
       <c r="C142" s="5" t="b">
         <v>1</v>
@@ -27555,7 +27580,7 @@
         <v>781</v>
       </c>
       <c r="B145" s="3" t="s">
-        <v>1135</v>
+        <v>1140</v>
       </c>
       <c r="C145" s="5" t="b">
         <v>1</v>
@@ -27611,7 +27636,7 @@
         <v>783</v>
       </c>
       <c r="B146" s="3" t="s">
-        <v>1135</v>
+        <v>1140</v>
       </c>
       <c r="C146" s="5" t="b">
         <v>1</v>
@@ -27667,7 +27692,7 @@
         <v>792</v>
       </c>
       <c r="B147" s="3" t="s">
-        <v>1135</v>
+        <v>1140</v>
       </c>
       <c r="C147" s="5" t="b">
         <v>1</v>
@@ -27723,7 +27748,7 @@
         <v>796</v>
       </c>
       <c r="B148" s="3" t="s">
-        <v>1135</v>
+        <v>1140</v>
       </c>
       <c r="C148" s="5" t="b">
         <v>1</v>
@@ -27779,7 +27804,7 @@
         <v>799</v>
       </c>
       <c r="B149" s="3" t="s">
-        <v>1135</v>
+        <v>1140</v>
       </c>
       <c r="C149" s="5" t="b">
         <v>1</v>
@@ -27835,7 +27860,7 @@
         <v>802</v>
       </c>
       <c r="B150" s="3" t="s">
-        <v>1135</v>
+        <v>1140</v>
       </c>
       <c r="C150" s="5" t="b">
         <v>1</v>
@@ -27891,7 +27916,7 @@
         <v>805</v>
       </c>
       <c r="B151" s="3" t="s">
-        <v>1135</v>
+        <v>1140</v>
       </c>
       <c r="C151" s="5" t="b">
         <v>1</v>
@@ -27947,7 +27972,7 @@
         <v>808</v>
       </c>
       <c r="B152" s="3" t="s">
-        <v>1135</v>
+        <v>1140</v>
       </c>
       <c r="C152" s="5" t="b">
         <v>1</v>
@@ -28003,7 +28028,7 @@
         <v>811</v>
       </c>
       <c r="B153" s="3" t="s">
-        <v>1135</v>
+        <v>1140</v>
       </c>
       <c r="C153" s="5" t="b">
         <v>1</v>
@@ -28059,7 +28084,7 @@
         <v>814</v>
       </c>
       <c r="B154" s="3" t="s">
-        <v>1135</v>
+        <v>1140</v>
       </c>
       <c r="C154" s="5" t="b">
         <v>1</v>
@@ -28115,7 +28140,7 @@
         <v>817</v>
       </c>
       <c r="B155" s="3" t="s">
-        <v>1135</v>
+        <v>1140</v>
       </c>
       <c r="C155" s="5" t="b">
         <v>1</v>
@@ -28171,7 +28196,7 @@
         <v>820</v>
       </c>
       <c r="B156" s="3" t="s">
-        <v>1135</v>
+        <v>1140</v>
       </c>
       <c r="C156" s="5" t="b">
         <v>1</v>
@@ -28227,7 +28252,7 @@
         <v>823</v>
       </c>
       <c r="B157" s="3" t="s">
-        <v>1135</v>
+        <v>1140</v>
       </c>
       <c r="C157" s="5" t="b">
         <v>1</v>
@@ -28283,7 +28308,7 @@
         <v>826</v>
       </c>
       <c r="B158" s="3" t="s">
-        <v>1135</v>
+        <v>1140</v>
       </c>
       <c r="C158" s="5" t="b">
         <v>1</v>
@@ -28339,7 +28364,7 @@
         <v>829</v>
       </c>
       <c r="B159" s="3" t="s">
-        <v>1135</v>
+        <v>1140</v>
       </c>
       <c r="C159" s="5" t="b">
         <v>1</v>
@@ -28395,7 +28420,7 @@
         <v>832</v>
       </c>
       <c r="B160" s="3" t="s">
-        <v>1135</v>
+        <v>1140</v>
       </c>
       <c r="C160" s="5" t="b">
         <v>1</v>
@@ -28451,7 +28476,7 @@
         <v>835</v>
       </c>
       <c r="B161" s="3" t="s">
-        <v>1135</v>
+        <v>1140</v>
       </c>
       <c r="C161" s="5" t="b">
         <v>1</v>
@@ -28507,7 +28532,7 @@
         <v>838</v>
       </c>
       <c r="B162" s="3" t="s">
-        <v>1135</v>
+        <v>1140</v>
       </c>
       <c r="C162" s="5" t="b">
         <v>1</v>
@@ -28563,7 +28588,7 @@
         <v>841</v>
       </c>
       <c r="B163" s="3" t="s">
-        <v>1135</v>
+        <v>1140</v>
       </c>
       <c r="C163" s="5" t="b">
         <v>1</v>
@@ -28619,7 +28644,7 @@
         <v>844</v>
       </c>
       <c r="B164" s="3" t="s">
-        <v>1135</v>
+        <v>1140</v>
       </c>
       <c r="C164" s="5" t="b">
         <v>1</v>
@@ -28675,7 +28700,7 @@
         <v>847</v>
       </c>
       <c r="B165" s="3" t="s">
-        <v>1135</v>
+        <v>1140</v>
       </c>
       <c r="C165" s="5" t="b">
         <v>1</v>
@@ -28731,7 +28756,7 @@
         <v>850</v>
       </c>
       <c r="B166" s="3" t="s">
-        <v>1135</v>
+        <v>1140</v>
       </c>
       <c r="C166" s="5" t="b">
         <v>1</v>
@@ -28787,7 +28812,7 @@
         <v>853</v>
       </c>
       <c r="B167" s="3" t="s">
-        <v>1135</v>
+        <v>1140</v>
       </c>
       <c r="C167" s="5" t="b">
         <v>1</v>
@@ -28843,7 +28868,7 @@
         <v>856</v>
       </c>
       <c r="B168" s="3" t="s">
-        <v>1135</v>
+        <v>1140</v>
       </c>
       <c r="C168" s="5" t="b">
         <v>1</v>
@@ -28899,7 +28924,7 @@
         <v>859</v>
       </c>
       <c r="B169" s="3" t="s">
-        <v>1135</v>
+        <v>1140</v>
       </c>
       <c r="C169" s="5" t="b">
         <v>1</v>
@@ -28955,7 +28980,7 @@
         <v>862</v>
       </c>
       <c r="B170" s="3" t="s">
-        <v>1135</v>
+        <v>1140</v>
       </c>
       <c r="C170" s="5" t="b">
         <v>1</v>
@@ -29011,7 +29036,7 @@
         <v>865</v>
       </c>
       <c r="B171" s="3" t="s">
-        <v>1135</v>
+        <v>1140</v>
       </c>
       <c r="C171" s="5" t="b">
         <v>1</v>
@@ -29067,7 +29092,7 @@
         <v>868</v>
       </c>
       <c r="B172" s="3" t="s">
-        <v>1135</v>
+        <v>1140</v>
       </c>
       <c r="C172" s="5" t="b">
         <v>1</v>
@@ -29123,7 +29148,7 @@
         <v>871</v>
       </c>
       <c r="B173" s="3" t="s">
-        <v>1135</v>
+        <v>1140</v>
       </c>
       <c r="C173" s="5" t="b">
         <v>1</v>
@@ -29179,7 +29204,7 @@
         <v>874</v>
       </c>
       <c r="B174" s="3" t="s">
-        <v>1135</v>
+        <v>1140</v>
       </c>
       <c r="C174" s="5" t="b">
         <v>1</v>
@@ -29235,7 +29260,7 @@
         <v>877</v>
       </c>
       <c r="B175" s="3" t="s">
-        <v>1135</v>
+        <v>1140</v>
       </c>
       <c r="C175" s="5" t="b">
         <v>1</v>
@@ -29291,7 +29316,7 @@
         <v>880</v>
       </c>
       <c r="B176" s="3" t="s">
-        <v>1135</v>
+        <v>1140</v>
       </c>
       <c r="C176" s="5" t="b">
         <v>1</v>
@@ -29347,7 +29372,7 @@
         <v>883</v>
       </c>
       <c r="B177" s="3" t="s">
-        <v>1135</v>
+        <v>1140</v>
       </c>
       <c r="C177" s="5" t="b">
         <v>1</v>
@@ -29403,7 +29428,7 @@
         <v>886</v>
       </c>
       <c r="B178" s="3" t="s">
-        <v>1135</v>
+        <v>1140</v>
       </c>
       <c r="C178" s="5" t="b">
         <v>1</v>
@@ -29459,7 +29484,7 @@
         <v>889</v>
       </c>
       <c r="B179" s="3" t="s">
-        <v>1135</v>
+        <v>1140</v>
       </c>
       <c r="C179" s="5" t="b">
         <v>1</v>
@@ -29515,7 +29540,7 @@
         <v>892</v>
       </c>
       <c r="B180" s="3" t="s">
-        <v>1135</v>
+        <v>1140</v>
       </c>
       <c r="C180" s="5" t="b">
         <v>1</v>
@@ -29571,7 +29596,7 @@
         <v>895</v>
       </c>
       <c r="B181" s="3" t="s">
-        <v>1135</v>
+        <v>1140</v>
       </c>
       <c r="C181" s="5" t="b">
         <v>1</v>
@@ -29627,7 +29652,7 @@
         <v>897</v>
       </c>
       <c r="B182" s="3" t="s">
-        <v>1135</v>
+        <v>1140</v>
       </c>
       <c r="C182" s="5" t="b">
         <v>1</v>
@@ -29683,7 +29708,7 @@
         <v>900</v>
       </c>
       <c r="B183" s="3" t="s">
-        <v>1135</v>
+        <v>1140</v>
       </c>
       <c r="C183" s="5" t="b">
         <v>1</v>
@@ -29739,7 +29764,7 @@
         <v>902</v>
       </c>
       <c r="B184" s="3" t="s">
-        <v>1135</v>
+        <v>1140</v>
       </c>
       <c r="C184" s="5" t="b">
         <v>1</v>
@@ -29795,7 +29820,7 @@
         <v>904</v>
       </c>
       <c r="B185" s="3" t="s">
-        <v>1135</v>
+        <v>1140</v>
       </c>
       <c r="C185" s="5" t="b">
         <v>1</v>
@@ -29851,7 +29876,7 @@
         <v>906</v>
       </c>
       <c r="B186" s="3" t="s">
-        <v>1135</v>
+        <v>1140</v>
       </c>
       <c r="C186" s="5" t="b">
         <v>1</v>
@@ -29907,7 +29932,7 @@
         <v>909</v>
       </c>
       <c r="B187" s="3" t="s">
-        <v>1135</v>
+        <v>1140</v>
       </c>
       <c r="C187" s="5" t="b">
         <v>1</v>
@@ -29963,7 +29988,7 @@
         <v>915</v>
       </c>
       <c r="B188" s="3" t="s">
-        <v>1135</v>
+        <v>1140</v>
       </c>
       <c r="C188" s="5" t="b">
         <v>1</v>
@@ -30019,7 +30044,7 @@
         <v>926</v>
       </c>
       <c r="B189" s="3" t="s">
-        <v>1135</v>
+        <v>1140</v>
       </c>
       <c r="C189" s="5" t="b">
         <v>1</v>
@@ -30131,7 +30156,7 @@
         <v>939</v>
       </c>
       <c r="B191" s="3" t="s">
-        <v>1135</v>
+        <v>1140</v>
       </c>
       <c r="C191" s="5" t="b">
         <v>1</v>
@@ -30243,7 +30268,7 @@
         <v>958</v>
       </c>
       <c r="B193" s="3" t="s">
-        <v>1135</v>
+        <v>1140</v>
       </c>
       <c r="C193" s="5" t="b">
         <v>1</v>
@@ -30299,7 +30324,7 @@
         <v>966</v>
       </c>
       <c r="B194" s="3" t="s">
-        <v>1135</v>
+        <v>1140</v>
       </c>
       <c r="C194" s="5" t="b">
         <v>1</v>
@@ -30355,7 +30380,7 @@
         <v>968</v>
       </c>
       <c r="B195" s="3" t="s">
-        <v>1135</v>
+        <v>1140</v>
       </c>
       <c r="C195" s="5" t="b">
         <v>1</v>
@@ -30411,7 +30436,7 @@
         <v>975</v>
       </c>
       <c r="B196" s="3" t="s">
-        <v>1135</v>
+        <v>1140</v>
       </c>
       <c r="C196" s="5" t="b">
         <v>1</v>
@@ -30467,7 +30492,7 @@
         <v>977</v>
       </c>
       <c r="B197" s="3" t="s">
-        <v>1135</v>
+        <v>1140</v>
       </c>
       <c r="C197" s="5" t="b">
         <v>1</v>
@@ -30523,7 +30548,7 @@
         <v>987</v>
       </c>
       <c r="B198" s="3" t="s">
-        <v>1135</v>
+        <v>1140</v>
       </c>
       <c r="C198" s="5" t="b">
         <v>1</v>
@@ -30579,7 +30604,7 @@
         <v>995</v>
       </c>
       <c r="B199" s="3" t="s">
-        <v>1135</v>
+        <v>1140</v>
       </c>
       <c r="C199" s="5" t="b">
         <v>1</v>
@@ -30635,7 +30660,7 @@
         <v>998</v>
       </c>
       <c r="B200" s="3" t="s">
-        <v>1135</v>
+        <v>1140</v>
       </c>
       <c r="C200" s="5" t="b">
         <v>1</v>
@@ -30691,7 +30716,7 @@
         <v>1006</v>
       </c>
       <c r="B201" s="3" t="s">
-        <v>1135</v>
+        <v>1140</v>
       </c>
       <c r="C201" s="5" t="b">
         <v>1</v>
@@ -30747,7 +30772,7 @@
         <v>1010</v>
       </c>
       <c r="B202" s="3" t="s">
-        <v>1135</v>
+        <v>1140</v>
       </c>
       <c r="C202" s="5" t="b">
         <v>1</v>
@@ -30803,7 +30828,7 @@
         <v>1020</v>
       </c>
       <c r="B203" s="3" t="s">
-        <v>1135</v>
+        <v>1140</v>
       </c>
       <c r="C203" s="5" t="b">
         <v>1</v>
@@ -30859,7 +30884,7 @@
         <v>1026</v>
       </c>
       <c r="B204" s="3" t="s">
-        <v>1135</v>
+        <v>1140</v>
       </c>
       <c r="C204" s="5" t="b">
         <v>1</v>
@@ -30915,7 +30940,7 @@
         <v>1029</v>
       </c>
       <c r="B205" s="3" t="s">
-        <v>1135</v>
+        <v>1140</v>
       </c>
       <c r="C205" s="5" t="b">
         <v>1</v>
@@ -30971,7 +30996,7 @@
         <v>1032</v>
       </c>
       <c r="B206" s="3" t="s">
-        <v>1135</v>
+        <v>1140</v>
       </c>
       <c r="C206" s="5" t="b">
         <v>1</v>
@@ -31027,7 +31052,7 @@
         <v>1039</v>
       </c>
       <c r="B207" s="3" t="s">
-        <v>1135</v>
+        <v>1140</v>
       </c>
       <c r="C207" s="5" t="b">
         <v>1</v>
@@ -31083,7 +31108,7 @@
         <v>1048</v>
       </c>
       <c r="B208" s="3" t="s">
-        <v>1135</v>
+        <v>1140</v>
       </c>
       <c r="C208" s="5" t="b">
         <v>1</v>
@@ -31139,7 +31164,7 @@
         <v>1050</v>
       </c>
       <c r="B209" s="3" t="s">
-        <v>1135</v>
+        <v>1140</v>
       </c>
       <c r="C209" s="5" t="b">
         <v>1</v>
@@ -31195,7 +31220,7 @@
         <v>1056</v>
       </c>
       <c r="B210" s="3" t="s">
-        <v>1135</v>
+        <v>1140</v>
       </c>
       <c r="C210" s="5" t="b">
         <v>1</v>
@@ -31251,7 +31276,7 @@
         <v>1058</v>
       </c>
       <c r="B211" s="3" t="s">
-        <v>1135</v>
+        <v>1140</v>
       </c>
       <c r="C211" s="5" t="b">
         <v>1</v>
@@ -31307,7 +31332,7 @@
         <v>1069</v>
       </c>
       <c r="B212" s="3" t="s">
-        <v>1135</v>
+        <v>1140</v>
       </c>
       <c r="C212" s="5" t="b">
         <v>1</v>
@@ -31363,7 +31388,7 @@
         <v>1071</v>
       </c>
       <c r="B213" s="3" t="s">
-        <v>1135</v>
+        <v>1140</v>
       </c>
       <c r="C213" s="5" t="b">
         <v>1</v>
@@ -31419,7 +31444,7 @@
         <v>1077</v>
       </c>
       <c r="B214" s="3" t="s">
-        <v>1135</v>
+        <v>1140</v>
       </c>
       <c r="C214" s="5" t="b">
         <v>1</v>
@@ -31475,7 +31500,7 @@
         <v>1079</v>
       </c>
       <c r="B215" s="3" t="s">
-        <v>1135</v>
+        <v>1140</v>
       </c>
       <c r="C215" s="5" t="b">
         <v>1</v>
@@ -31531,7 +31556,7 @@
         <v>1090</v>
       </c>
       <c r="B216" s="3" t="s">
-        <v>1135</v>
+        <v>1140</v>
       </c>
       <c r="C216" s="5" t="b">
         <v>1</v>
@@ -31587,7 +31612,7 @@
         <v>1094</v>
       </c>
       <c r="B217" s="3" t="s">
-        <v>1135</v>
+        <v>1140</v>
       </c>
       <c r="C217" s="5" t="b">
         <v>1</v>
@@ -31643,7 +31668,7 @@
         <v>1098</v>
       </c>
       <c r="B218" s="3" t="s">
-        <v>1135</v>
+        <v>1140</v>
       </c>
       <c r="C218" s="5" t="b">
         <v>1</v>
@@ -31669,23 +31694,23 @@
       <c r="J218" s="6" t="b">
         <v>0</v>
       </c>
-      <c r="K218" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="L218" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="M218" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="N218" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="O218" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="P218" s="6" t="b">
-        <v>0</v>
+      <c r="K218" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="L218" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="M218" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="N218" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="O218" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="P218" s="5" t="b">
+        <v>1</v>
       </c>
       <c r="Q218" s="6" t="b">
         <v>0</v>
@@ -31696,10 +31721,10 @@
     </row>
     <row r="219" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A219" s="3" t="s">
-        <v>1101</v>
+        <v>1106</v>
       </c>
       <c r="B219" s="3" t="s">
-        <v>1135</v>
+        <v>1140</v>
       </c>
       <c r="C219" s="5" t="b">
         <v>1</v>
@@ -31752,10 +31777,10 @@
     </row>
     <row r="220" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A220" s="3" t="s">
-        <v>1110</v>
+        <v>1115</v>
       </c>
       <c r="B220" s="3" t="s">
-        <v>1135</v>
+        <v>1140</v>
       </c>
       <c r="C220" s="5" t="b">
         <v>1</v>
@@ -31808,10 +31833,10 @@
     </row>
     <row r="221" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A221" s="3" t="s">
-        <v>1113</v>
+        <v>1118</v>
       </c>
       <c r="B221" s="3" t="s">
-        <v>1135</v>
+        <v>1140</v>
       </c>
       <c r="C221" s="5" t="b">
         <v>1</v>
@@ -31864,10 +31889,10 @@
     </row>
     <row r="222" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A222" s="3" t="s">
-        <v>1116</v>
+        <v>1121</v>
       </c>
       <c r="B222" s="3" t="s">
-        <v>1135</v>
+        <v>1140</v>
       </c>
       <c r="C222" s="5" t="b">
         <v>1</v>
@@ -31920,10 +31945,10 @@
     </row>
     <row r="223" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A223" s="3" t="s">
-        <v>1119</v>
+        <v>1124</v>
       </c>
       <c r="B223" s="3" t="s">
-        <v>1135</v>
+        <v>1140</v>
       </c>
       <c r="C223" s="5" t="b">
         <v>1</v>
@@ -31976,10 +32001,10 @@
     </row>
     <row r="224" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A224" s="3" t="s">
-        <v>1126</v>
+        <v>1131</v>
       </c>
       <c r="B224" s="3" t="s">
-        <v>1135</v>
+        <v>1140</v>
       </c>
       <c r="C224" s="5" t="b">
         <v>1</v>
@@ -32032,10 +32057,10 @@
     </row>
     <row r="225" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A225" s="3" t="s">
-        <v>1129</v>
+        <v>1134</v>
       </c>
       <c r="B225" s="3" t="s">
-        <v>1135</v>
+        <v>1140</v>
       </c>
       <c r="C225" s="5" t="b">
         <v>1</v>

</xml_diff>

<commit_message>
generated all the reports on 2024-05-07
</commit_message>
<xml_diff>
--- a/report/merged_configurations.xlsx
+++ b/report/merged_configurations.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5252" uniqueCount="1142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5252" uniqueCount="1143">
   <si>
     <t>naam</t>
   </si>
@@ -3309,6 +3309,9 @@
   </si>
   <si>
     <t>[{"naam":"Vocabularium Overlijdensaangifte","waarde":"https://data.vlaanderen.be/ns/overlijdensaangifte"},{"naam":"Applicatieprofiel Overlijdensaangifte","waarde":"https://data.vlaanderen.be/doc/applicatieprofiel/overlijdensaangifte"}]</t>
+  </si>
+  <si>
+    <t>[{"naam":"Verslag Thematische Werkgroep I - 16 januari 2024","waarde":"20240116__ThematicWorkshop1_Verslag_OSLOOverlijdensaangifte.pdf"},{"naam":"Verslag Thematische Werkgroep II - 20 februari 2024","waarde":"20240220_ThematicWorkshop2_Verslag_OSLOOverlijdensaangifte.pdf"},{"naam":"Verslag Thematische Werkgroep III - 12 maart 2024","waarde":"20240312_ThematicWorkshop3_Verslag_OSLOOverlijdensaangifte.pdf"}]</t>
   </si>
   <si>
     <t>Applicatieprofiel Kindfiche</t>
@@ -18916,7 +18919,7 @@
         <v>1086</v>
       </c>
       <c r="L217" s="3" t="s">
-        <v>1087</v>
+        <v>1099</v>
       </c>
       <c r="M217" s="3" t="s">
         <v>1088</v>
@@ -18954,7 +18957,7 @@
     </row>
     <row r="218" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A218" s="3" t="s">
-        <v>1099</v>
+        <v>1100</v>
       </c>
       <c r="B218" s="3"/>
       <c r="C218" s="3" t="s">
@@ -18973,31 +18976,31 @@
         <v>28</v>
       </c>
       <c r="H218" s="3" t="s">
-        <v>1100</v>
+        <v>1101</v>
       </c>
       <c r="I218" s="3" t="s">
-        <v>1101</v>
+        <v>1102</v>
       </c>
       <c r="J218" s="3" t="s">
         <v>31</v>
       </c>
       <c r="K218" s="3" t="s">
-        <v>1102</v>
+        <v>1103</v>
       </c>
       <c r="L218" s="3" t="s">
-        <v>1103</v>
+        <v>1104</v>
       </c>
       <c r="M218" s="3" t="s">
-        <v>1104</v>
+        <v>1105</v>
       </c>
       <c r="N218" s="3" t="s">
         <v>50</v>
       </c>
       <c r="O218" s="3" t="s">
-        <v>1105</v>
+        <v>1106</v>
       </c>
       <c r="P218" s="3" t="s">
-        <v>1106</v>
+        <v>1107</v>
       </c>
       <c r="Q218" s="3" t="s">
         <v>26</v>
@@ -19023,17 +19026,17 @@
     </row>
     <row r="219" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A219" s="3" t="s">
-        <v>1107</v>
+        <v>1108</v>
       </c>
       <c r="B219" s="3"/>
       <c r="C219" s="3" t="s">
-        <v>1108</v>
+        <v>1109</v>
       </c>
       <c r="D219" s="3" t="s">
-        <v>1109</v>
+        <v>1110</v>
       </c>
       <c r="E219" s="3" t="s">
-        <v>1110</v>
+        <v>1111</v>
       </c>
       <c r="F219" s="3" t="s">
         <v>43</v>
@@ -19042,31 +19045,31 @@
         <v>39</v>
       </c>
       <c r="H219" s="3" t="s">
-        <v>1111</v>
+        <v>1112</v>
       </c>
       <c r="I219" s="3" t="s">
-        <v>1112</v>
+        <v>1113</v>
       </c>
       <c r="J219" s="3" t="s">
-        <v>1113</v>
+        <v>1114</v>
       </c>
       <c r="K219" s="3" t="s">
         <v>31</v>
       </c>
       <c r="L219" s="3" t="s">
-        <v>1113</v>
+        <v>1114</v>
       </c>
       <c r="M219" s="3" t="s">
-        <v>1113</v>
+        <v>1114</v>
       </c>
       <c r="N219" s="3" t="s">
-        <v>1114</v>
+        <v>1115</v>
       </c>
       <c r="O219" s="3" t="s">
         <v>70</v>
       </c>
       <c r="P219" s="3" t="s">
-        <v>1115</v>
+        <v>1116</v>
       </c>
       <c r="Q219" s="3" t="s">
         <v>26</v>
@@ -19092,17 +19095,17 @@
     </row>
     <row r="220" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A220" s="3" t="s">
-        <v>1116</v>
+        <v>1117</v>
       </c>
       <c r="B220" s="3"/>
       <c r="C220" s="3" t="s">
-        <v>1108</v>
+        <v>1109</v>
       </c>
       <c r="D220" s="3" t="s">
-        <v>1109</v>
+        <v>1110</v>
       </c>
       <c r="E220" s="3" t="s">
-        <v>1110</v>
+        <v>1111</v>
       </c>
       <c r="F220" s="3" t="s">
         <v>43</v>
@@ -19111,31 +19114,31 @@
         <v>28</v>
       </c>
       <c r="H220" s="3" t="s">
-        <v>1117</v>
+        <v>1118</v>
       </c>
       <c r="I220" s="3" t="s">
-        <v>1118</v>
+        <v>1119</v>
       </c>
       <c r="J220" s="3" t="s">
-        <v>1113</v>
+        <v>1114</v>
       </c>
       <c r="K220" s="3" t="s">
         <v>31</v>
       </c>
       <c r="L220" s="3" t="s">
-        <v>1113</v>
+        <v>1114</v>
       </c>
       <c r="M220" s="3" t="s">
-        <v>1113</v>
+        <v>1114</v>
       </c>
       <c r="N220" s="3" t="s">
-        <v>1114</v>
+        <v>1115</v>
       </c>
       <c r="O220" s="3" t="s">
         <v>70</v>
       </c>
       <c r="P220" s="3" t="s">
-        <v>1115</v>
+        <v>1116</v>
       </c>
       <c r="Q220" s="3" t="s">
         <v>26</v>
@@ -19161,17 +19164,17 @@
     </row>
     <row r="221" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A221" s="3" t="s">
-        <v>1119</v>
+        <v>1120</v>
       </c>
       <c r="B221" s="3"/>
       <c r="C221" s="3" t="s">
-        <v>1108</v>
+        <v>1109</v>
       </c>
       <c r="D221" s="3" t="s">
-        <v>1109</v>
+        <v>1110</v>
       </c>
       <c r="E221" s="3" t="s">
-        <v>1110</v>
+        <v>1111</v>
       </c>
       <c r="F221" s="3" t="s">
         <v>43</v>
@@ -19180,31 +19183,31 @@
         <v>39</v>
       </c>
       <c r="H221" s="3" t="s">
-        <v>1120</v>
+        <v>1121</v>
       </c>
       <c r="I221" s="3" t="s">
-        <v>1121</v>
+        <v>1122</v>
       </c>
       <c r="J221" s="3" t="s">
-        <v>1113</v>
+        <v>1114</v>
       </c>
       <c r="K221" s="3" t="s">
         <v>31</v>
       </c>
       <c r="L221" s="3" t="s">
-        <v>1113</v>
+        <v>1114</v>
       </c>
       <c r="M221" s="3" t="s">
-        <v>1113</v>
+        <v>1114</v>
       </c>
       <c r="N221" s="3" t="s">
-        <v>1114</v>
+        <v>1115</v>
       </c>
       <c r="O221" s="3" t="s">
         <v>70</v>
       </c>
       <c r="P221" s="3" t="s">
-        <v>1115</v>
+        <v>1116</v>
       </c>
       <c r="Q221" s="3" t="s">
         <v>26</v>
@@ -19230,17 +19233,17 @@
     </row>
     <row r="222" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A222" s="3" t="s">
-        <v>1122</v>
+        <v>1123</v>
       </c>
       <c r="B222" s="3"/>
       <c r="C222" s="3" t="s">
-        <v>1108</v>
+        <v>1109</v>
       </c>
       <c r="D222" s="3" t="s">
-        <v>1109</v>
+        <v>1110</v>
       </c>
       <c r="E222" s="3" t="s">
-        <v>1110</v>
+        <v>1111</v>
       </c>
       <c r="F222" s="3" t="s">
         <v>43</v>
@@ -19249,31 +19252,31 @@
         <v>28</v>
       </c>
       <c r="H222" s="3" t="s">
-        <v>1123</v>
+        <v>1124</v>
       </c>
       <c r="I222" s="3" t="s">
-        <v>1124</v>
+        <v>1125</v>
       </c>
       <c r="J222" s="3" t="s">
-        <v>1113</v>
+        <v>1114</v>
       </c>
       <c r="K222" s="3" t="s">
         <v>31</v>
       </c>
       <c r="L222" s="3" t="s">
-        <v>1113</v>
+        <v>1114</v>
       </c>
       <c r="M222" s="3" t="s">
-        <v>1113</v>
+        <v>1114</v>
       </c>
       <c r="N222" s="3" t="s">
-        <v>1114</v>
+        <v>1115</v>
       </c>
       <c r="O222" s="3" t="s">
         <v>70</v>
       </c>
       <c r="P222" s="3" t="s">
-        <v>1115</v>
+        <v>1116</v>
       </c>
       <c r="Q222" s="3" t="s">
         <v>26</v>
@@ -19299,17 +19302,17 @@
     </row>
     <row r="223" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A223" s="3" t="s">
-        <v>1125</v>
+        <v>1126</v>
       </c>
       <c r="B223" s="3"/>
       <c r="C223" s="3" t="s">
-        <v>1108</v>
+        <v>1109</v>
       </c>
       <c r="D223" s="3" t="s">
-        <v>1109</v>
+        <v>1110</v>
       </c>
       <c r="E223" s="3" t="s">
-        <v>1110</v>
+        <v>1111</v>
       </c>
       <c r="F223" s="3" t="s">
         <v>43</v>
@@ -19318,31 +19321,31 @@
         <v>28</v>
       </c>
       <c r="H223" s="3" t="s">
-        <v>1126</v>
+        <v>1127</v>
       </c>
       <c r="I223" s="3" t="s">
-        <v>1127</v>
+        <v>1128</v>
       </c>
       <c r="J223" s="3" t="s">
-        <v>1128</v>
+        <v>1129</v>
       </c>
       <c r="K223" s="3" t="s">
         <v>31</v>
       </c>
       <c r="L223" s="3" t="s">
-        <v>1129</v>
+        <v>1130</v>
       </c>
       <c r="M223" s="3" t="s">
-        <v>1130</v>
+        <v>1131</v>
       </c>
       <c r="N223" s="3" t="s">
-        <v>1131</v>
+        <v>1132</v>
       </c>
       <c r="O223" s="3" t="s">
         <v>97</v>
       </c>
       <c r="P223" s="3" t="s">
-        <v>1115</v>
+        <v>1116</v>
       </c>
       <c r="Q223" s="3" t="s">
         <v>26</v>
@@ -19368,17 +19371,17 @@
     </row>
     <row r="224" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A224" s="3" t="s">
-        <v>1132</v>
+        <v>1133</v>
       </c>
       <c r="B224" s="3"/>
       <c r="C224" s="3" t="s">
-        <v>1108</v>
+        <v>1109</v>
       </c>
       <c r="D224" s="3" t="s">
-        <v>1109</v>
+        <v>1110</v>
       </c>
       <c r="E224" s="3" t="s">
-        <v>1110</v>
+        <v>1111</v>
       </c>
       <c r="F224" s="3" t="s">
         <v>43</v>
@@ -19387,31 +19390,31 @@
         <v>39</v>
       </c>
       <c r="H224" s="3" t="s">
-        <v>1133</v>
+        <v>1134</v>
       </c>
       <c r="I224" s="3" t="s">
-        <v>1134</v>
+        <v>1135</v>
       </c>
       <c r="J224" s="3" t="s">
-        <v>1128</v>
+        <v>1129</v>
       </c>
       <c r="K224" s="3" t="s">
         <v>31</v>
       </c>
       <c r="L224" s="3" t="s">
-        <v>1129</v>
+        <v>1130</v>
       </c>
       <c r="M224" s="3" t="s">
-        <v>1130</v>
+        <v>1131</v>
       </c>
       <c r="N224" s="3" t="s">
-        <v>1131</v>
+        <v>1132</v>
       </c>
       <c r="O224" s="3" t="s">
         <v>97</v>
       </c>
       <c r="P224" s="3" t="s">
-        <v>1115</v>
+        <v>1116</v>
       </c>
       <c r="Q224" s="3" t="s">
         <v>26</v>
@@ -19437,7 +19440,7 @@
     </row>
     <row r="225" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A225" s="3" t="s">
-        <v>1135</v>
+        <v>1136</v>
       </c>
       <c r="B225" s="3"/>
       <c r="C225" s="3" t="s">
@@ -19456,10 +19459,10 @@
         <v>28</v>
       </c>
       <c r="H225" s="3" t="s">
-        <v>1136</v>
+        <v>1137</v>
       </c>
       <c r="I225" s="3" t="s">
-        <v>1137</v>
+        <v>1138</v>
       </c>
       <c r="J225" s="3" t="s">
         <v>31</v>
@@ -19468,13 +19471,13 @@
         <v>31</v>
       </c>
       <c r="L225" s="3" t="s">
-        <v>1138</v>
+        <v>1139</v>
       </c>
       <c r="M225" s="3" t="s">
-        <v>1139</v>
+        <v>1140</v>
       </c>
       <c r="N225" s="3" t="s">
-        <v>1140</v>
+        <v>1141</v>
       </c>
       <c r="O225" s="3" t="s">
         <v>70</v>
@@ -19579,7 +19582,7 @@
         <v>23</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>1141</v>
+        <v>1142</v>
       </c>
       <c r="C2" s="5" t="b">
         <v>1</v>
@@ -19635,7 +19638,7 @@
         <v>38</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>1141</v>
+        <v>1142</v>
       </c>
       <c r="C3" s="5" t="b">
         <v>1</v>
@@ -19691,7 +19694,7 @@
         <v>41</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>1141</v>
+        <v>1142</v>
       </c>
       <c r="C4" s="5" t="b">
         <v>1</v>
@@ -19747,7 +19750,7 @@
         <v>53</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>1141</v>
+        <v>1142</v>
       </c>
       <c r="C5" s="5" t="b">
         <v>1</v>
@@ -19803,7 +19806,7 @@
         <v>60</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>1141</v>
+        <v>1142</v>
       </c>
       <c r="C6" s="5" t="b">
         <v>1</v>
@@ -19859,7 +19862,7 @@
         <v>63</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>1141</v>
+        <v>1142</v>
       </c>
       <c r="C7" s="5" t="b">
         <v>1</v>
@@ -19915,7 +19918,7 @@
         <v>72</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>1141</v>
+        <v>1142</v>
       </c>
       <c r="C8" s="5" t="b">
         <v>1</v>
@@ -19971,7 +19974,7 @@
         <v>74</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>1141</v>
+        <v>1142</v>
       </c>
       <c r="C9" s="5" t="b">
         <v>1</v>
@@ -20027,7 +20030,7 @@
         <v>81</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>1141</v>
+        <v>1142</v>
       </c>
       <c r="C10" s="5" t="b">
         <v>1</v>
@@ -20083,7 +20086,7 @@
         <v>83</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>1141</v>
+        <v>1142</v>
       </c>
       <c r="C11" s="5" t="b">
         <v>1</v>
@@ -20139,7 +20142,7 @@
         <v>90</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>1141</v>
+        <v>1142</v>
       </c>
       <c r="C12" s="5" t="b">
         <v>1</v>
@@ -20195,7 +20198,7 @@
         <v>100</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>1141</v>
+        <v>1142</v>
       </c>
       <c r="C13" s="5" t="b">
         <v>1</v>
@@ -20251,7 +20254,7 @@
         <v>103</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>1141</v>
+        <v>1142</v>
       </c>
       <c r="C14" s="5" t="b">
         <v>1</v>
@@ -20307,7 +20310,7 @@
         <v>114</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>1141</v>
+        <v>1142</v>
       </c>
       <c r="C15" s="5" t="b">
         <v>1</v>
@@ -20475,7 +20478,7 @@
         <v>140</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>1141</v>
+        <v>1142</v>
       </c>
       <c r="C18" s="5" t="b">
         <v>1</v>
@@ -20531,7 +20534,7 @@
         <v>151</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>1141</v>
+        <v>1142</v>
       </c>
       <c r="C19" s="5" t="b">
         <v>1</v>
@@ -20587,7 +20590,7 @@
         <v>153</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>1141</v>
+        <v>1142</v>
       </c>
       <c r="C20" s="5" t="b">
         <v>1</v>
@@ -20643,7 +20646,7 @@
         <v>155</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>1141</v>
+        <v>1142</v>
       </c>
       <c r="C21" s="5" t="b">
         <v>1</v>
@@ -20699,7 +20702,7 @@
         <v>157</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>1141</v>
+        <v>1142</v>
       </c>
       <c r="C22" s="5" t="b">
         <v>1</v>
@@ -20755,7 +20758,7 @@
         <v>160</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>1141</v>
+        <v>1142</v>
       </c>
       <c r="C23" s="5" t="b">
         <v>1</v>
@@ -20811,7 +20814,7 @@
         <v>162</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>1141</v>
+        <v>1142</v>
       </c>
       <c r="C24" s="5" t="b">
         <v>1</v>
@@ -20867,7 +20870,7 @@
         <v>164</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>1141</v>
+        <v>1142</v>
       </c>
       <c r="C25" s="5" t="b">
         <v>1</v>
@@ -20923,7 +20926,7 @@
         <v>166</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>1141</v>
+        <v>1142</v>
       </c>
       <c r="C26" s="5" t="b">
         <v>1</v>
@@ -20979,7 +20982,7 @@
         <v>168</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>1141</v>
+        <v>1142</v>
       </c>
       <c r="C27" s="5" t="b">
         <v>1</v>
@@ -21035,7 +21038,7 @@
         <v>170</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>1141</v>
+        <v>1142</v>
       </c>
       <c r="C28" s="5" t="b">
         <v>1</v>
@@ -21091,7 +21094,7 @@
         <v>168</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>1141</v>
+        <v>1142</v>
       </c>
       <c r="C29" s="5" t="b">
         <v>1</v>
@@ -21147,7 +21150,7 @@
         <v>172</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>1141</v>
+        <v>1142</v>
       </c>
       <c r="C30" s="5" t="b">
         <v>1</v>
@@ -21203,7 +21206,7 @@
         <v>174</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>1141</v>
+        <v>1142</v>
       </c>
       <c r="C31" s="5" t="b">
         <v>1</v>
@@ -21259,7 +21262,7 @@
         <v>176</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>1141</v>
+        <v>1142</v>
       </c>
       <c r="C32" s="5" t="b">
         <v>1</v>
@@ -21315,7 +21318,7 @@
         <v>178</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>1141</v>
+        <v>1142</v>
       </c>
       <c r="C33" s="5" t="b">
         <v>1</v>
@@ -21371,7 +21374,7 @@
         <v>180</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>1141</v>
+        <v>1142</v>
       </c>
       <c r="C34" s="5" t="b">
         <v>1</v>
@@ -21427,7 +21430,7 @@
         <v>182</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>1141</v>
+        <v>1142</v>
       </c>
       <c r="C35" s="5" t="b">
         <v>1</v>
@@ -21483,7 +21486,7 @@
         <v>184</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>1141</v>
+        <v>1142</v>
       </c>
       <c r="C36" s="5" t="b">
         <v>1</v>
@@ -21539,7 +21542,7 @@
         <v>186</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>1141</v>
+        <v>1142</v>
       </c>
       <c r="C37" s="5" t="b">
         <v>1</v>
@@ -21595,7 +21598,7 @@
         <v>188</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>1141</v>
+        <v>1142</v>
       </c>
       <c r="C38" s="5" t="b">
         <v>1</v>
@@ -21763,7 +21766,7 @@
         <v>218</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>1141</v>
+        <v>1142</v>
       </c>
       <c r="C41" s="5" t="b">
         <v>1</v>
@@ -21819,7 +21822,7 @@
         <v>226</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>1141</v>
+        <v>1142</v>
       </c>
       <c r="C42" s="5" t="b">
         <v>1</v>
@@ -23387,7 +23390,7 @@
         <v>408</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>1141</v>
+        <v>1142</v>
       </c>
       <c r="C70" s="5" t="b">
         <v>1</v>
@@ -23443,7 +23446,7 @@
         <v>420</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>1141</v>
+        <v>1142</v>
       </c>
       <c r="C71" s="5" t="b">
         <v>1</v>
@@ -23891,7 +23894,7 @@
         <v>479</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>1141</v>
+        <v>1142</v>
       </c>
       <c r="C79" s="5" t="b">
         <v>1</v>
@@ -24563,7 +24566,7 @@
         <v>560</v>
       </c>
       <c r="B91" s="3" t="s">
-        <v>1141</v>
+        <v>1142</v>
       </c>
       <c r="C91" s="5" t="b">
         <v>1</v>
@@ -24619,7 +24622,7 @@
         <v>569</v>
       </c>
       <c r="B92" s="3" t="s">
-        <v>1141</v>
+        <v>1142</v>
       </c>
       <c r="C92" s="5" t="b">
         <v>1</v>
@@ -24675,7 +24678,7 @@
         <v>571</v>
       </c>
       <c r="B93" s="3" t="s">
-        <v>1141</v>
+        <v>1142</v>
       </c>
       <c r="C93" s="5" t="b">
         <v>1</v>
@@ -26803,7 +26806,7 @@
         <v>724</v>
       </c>
       <c r="B131" s="3" t="s">
-        <v>1141</v>
+        <v>1142</v>
       </c>
       <c r="C131" s="5" t="b">
         <v>1</v>
@@ -27363,7 +27366,7 @@
         <v>756</v>
       </c>
       <c r="B141" s="3" t="s">
-        <v>1141</v>
+        <v>1142</v>
       </c>
       <c r="C141" s="5" t="b">
         <v>1</v>
@@ -27419,7 +27422,7 @@
         <v>762</v>
       </c>
       <c r="B142" s="3" t="s">
-        <v>1141</v>
+        <v>1142</v>
       </c>
       <c r="C142" s="5" t="b">
         <v>1</v>
@@ -27587,7 +27590,7 @@
         <v>782</v>
       </c>
       <c r="B145" s="3" t="s">
-        <v>1141</v>
+        <v>1142</v>
       </c>
       <c r="C145" s="5" t="b">
         <v>1</v>
@@ -27643,7 +27646,7 @@
         <v>784</v>
       </c>
       <c r="B146" s="3" t="s">
-        <v>1141</v>
+        <v>1142</v>
       </c>
       <c r="C146" s="5" t="b">
         <v>1</v>
@@ -27699,7 +27702,7 @@
         <v>793</v>
       </c>
       <c r="B147" s="3" t="s">
-        <v>1141</v>
+        <v>1142</v>
       </c>
       <c r="C147" s="5" t="b">
         <v>1</v>
@@ -27755,7 +27758,7 @@
         <v>797</v>
       </c>
       <c r="B148" s="3" t="s">
-        <v>1141</v>
+        <v>1142</v>
       </c>
       <c r="C148" s="5" t="b">
         <v>1</v>
@@ -27811,7 +27814,7 @@
         <v>800</v>
       </c>
       <c r="B149" s="3" t="s">
-        <v>1141</v>
+        <v>1142</v>
       </c>
       <c r="C149" s="5" t="b">
         <v>1</v>
@@ -27867,7 +27870,7 @@
         <v>803</v>
       </c>
       <c r="B150" s="3" t="s">
-        <v>1141</v>
+        <v>1142</v>
       </c>
       <c r="C150" s="5" t="b">
         <v>1</v>
@@ -27923,7 +27926,7 @@
         <v>806</v>
       </c>
       <c r="B151" s="3" t="s">
-        <v>1141</v>
+        <v>1142</v>
       </c>
       <c r="C151" s="5" t="b">
         <v>1</v>
@@ -27979,7 +27982,7 @@
         <v>809</v>
       </c>
       <c r="B152" s="3" t="s">
-        <v>1141</v>
+        <v>1142</v>
       </c>
       <c r="C152" s="5" t="b">
         <v>1</v>
@@ -28035,7 +28038,7 @@
         <v>812</v>
       </c>
       <c r="B153" s="3" t="s">
-        <v>1141</v>
+        <v>1142</v>
       </c>
       <c r="C153" s="5" t="b">
         <v>1</v>
@@ -28091,7 +28094,7 @@
         <v>815</v>
       </c>
       <c r="B154" s="3" t="s">
-        <v>1141</v>
+        <v>1142</v>
       </c>
       <c r="C154" s="5" t="b">
         <v>1</v>
@@ -28147,7 +28150,7 @@
         <v>818</v>
       </c>
       <c r="B155" s="3" t="s">
-        <v>1141</v>
+        <v>1142</v>
       </c>
       <c r="C155" s="5" t="b">
         <v>1</v>
@@ -28203,7 +28206,7 @@
         <v>821</v>
       </c>
       <c r="B156" s="3" t="s">
-        <v>1141</v>
+        <v>1142</v>
       </c>
       <c r="C156" s="5" t="b">
         <v>1</v>
@@ -28259,7 +28262,7 @@
         <v>824</v>
       </c>
       <c r="B157" s="3" t="s">
-        <v>1141</v>
+        <v>1142</v>
       </c>
       <c r="C157" s="5" t="b">
         <v>1</v>
@@ -28315,7 +28318,7 @@
         <v>827</v>
       </c>
       <c r="B158" s="3" t="s">
-        <v>1141</v>
+        <v>1142</v>
       </c>
       <c r="C158" s="5" t="b">
         <v>1</v>
@@ -28371,7 +28374,7 @@
         <v>830</v>
       </c>
       <c r="B159" s="3" t="s">
-        <v>1141</v>
+        <v>1142</v>
       </c>
       <c r="C159" s="5" t="b">
         <v>1</v>
@@ -28427,7 +28430,7 @@
         <v>833</v>
       </c>
       <c r="B160" s="3" t="s">
-        <v>1141</v>
+        <v>1142</v>
       </c>
       <c r="C160" s="5" t="b">
         <v>1</v>
@@ -28483,7 +28486,7 @@
         <v>836</v>
       </c>
       <c r="B161" s="3" t="s">
-        <v>1141</v>
+        <v>1142</v>
       </c>
       <c r="C161" s="5" t="b">
         <v>1</v>
@@ -28539,7 +28542,7 @@
         <v>839</v>
       </c>
       <c r="B162" s="3" t="s">
-        <v>1141</v>
+        <v>1142</v>
       </c>
       <c r="C162" s="5" t="b">
         <v>1</v>
@@ -28595,7 +28598,7 @@
         <v>842</v>
       </c>
       <c r="B163" s="3" t="s">
-        <v>1141</v>
+        <v>1142</v>
       </c>
       <c r="C163" s="5" t="b">
         <v>1</v>
@@ -28651,7 +28654,7 @@
         <v>845</v>
       </c>
       <c r="B164" s="3" t="s">
-        <v>1141</v>
+        <v>1142</v>
       </c>
       <c r="C164" s="5" t="b">
         <v>1</v>
@@ -28707,7 +28710,7 @@
         <v>848</v>
       </c>
       <c r="B165" s="3" t="s">
-        <v>1141</v>
+        <v>1142</v>
       </c>
       <c r="C165" s="5" t="b">
         <v>1</v>
@@ -28763,7 +28766,7 @@
         <v>851</v>
       </c>
       <c r="B166" s="3" t="s">
-        <v>1141</v>
+        <v>1142</v>
       </c>
       <c r="C166" s="5" t="b">
         <v>1</v>
@@ -28819,7 +28822,7 @@
         <v>854</v>
       </c>
       <c r="B167" s="3" t="s">
-        <v>1141</v>
+        <v>1142</v>
       </c>
       <c r="C167" s="5" t="b">
         <v>1</v>
@@ -28875,7 +28878,7 @@
         <v>857</v>
       </c>
       <c r="B168" s="3" t="s">
-        <v>1141</v>
+        <v>1142</v>
       </c>
       <c r="C168" s="5" t="b">
         <v>1</v>
@@ -28931,7 +28934,7 @@
         <v>860</v>
       </c>
       <c r="B169" s="3" t="s">
-        <v>1141</v>
+        <v>1142</v>
       </c>
       <c r="C169" s="5" t="b">
         <v>1</v>
@@ -28987,7 +28990,7 @@
         <v>863</v>
       </c>
       <c r="B170" s="3" t="s">
-        <v>1141</v>
+        <v>1142</v>
       </c>
       <c r="C170" s="5" t="b">
         <v>1</v>
@@ -29043,7 +29046,7 @@
         <v>866</v>
       </c>
       <c r="B171" s="3" t="s">
-        <v>1141</v>
+        <v>1142</v>
       </c>
       <c r="C171" s="5" t="b">
         <v>1</v>
@@ -29099,7 +29102,7 @@
         <v>869</v>
       </c>
       <c r="B172" s="3" t="s">
-        <v>1141</v>
+        <v>1142</v>
       </c>
       <c r="C172" s="5" t="b">
         <v>1</v>
@@ -29155,7 +29158,7 @@
         <v>872</v>
       </c>
       <c r="B173" s="3" t="s">
-        <v>1141</v>
+        <v>1142</v>
       </c>
       <c r="C173" s="5" t="b">
         <v>1</v>
@@ -29211,7 +29214,7 @@
         <v>875</v>
       </c>
       <c r="B174" s="3" t="s">
-        <v>1141</v>
+        <v>1142</v>
       </c>
       <c r="C174" s="5" t="b">
         <v>1</v>
@@ -29267,7 +29270,7 @@
         <v>878</v>
       </c>
       <c r="B175" s="3" t="s">
-        <v>1141</v>
+        <v>1142</v>
       </c>
       <c r="C175" s="5" t="b">
         <v>1</v>
@@ -29323,7 +29326,7 @@
         <v>881</v>
       </c>
       <c r="B176" s="3" t="s">
-        <v>1141</v>
+        <v>1142</v>
       </c>
       <c r="C176" s="5" t="b">
         <v>1</v>
@@ -29379,7 +29382,7 @@
         <v>884</v>
       </c>
       <c r="B177" s="3" t="s">
-        <v>1141</v>
+        <v>1142</v>
       </c>
       <c r="C177" s="5" t="b">
         <v>1</v>
@@ -29435,7 +29438,7 @@
         <v>887</v>
       </c>
       <c r="B178" s="3" t="s">
-        <v>1141</v>
+        <v>1142</v>
       </c>
       <c r="C178" s="5" t="b">
         <v>1</v>
@@ -29491,7 +29494,7 @@
         <v>890</v>
       </c>
       <c r="B179" s="3" t="s">
-        <v>1141</v>
+        <v>1142</v>
       </c>
       <c r="C179" s="5" t="b">
         <v>1</v>
@@ -29547,7 +29550,7 @@
         <v>893</v>
       </c>
       <c r="B180" s="3" t="s">
-        <v>1141</v>
+        <v>1142</v>
       </c>
       <c r="C180" s="5" t="b">
         <v>1</v>
@@ -29603,7 +29606,7 @@
         <v>896</v>
       </c>
       <c r="B181" s="3" t="s">
-        <v>1141</v>
+        <v>1142</v>
       </c>
       <c r="C181" s="5" t="b">
         <v>1</v>
@@ -29659,7 +29662,7 @@
         <v>898</v>
       </c>
       <c r="B182" s="3" t="s">
-        <v>1141</v>
+        <v>1142</v>
       </c>
       <c r="C182" s="5" t="b">
         <v>1</v>
@@ -29715,7 +29718,7 @@
         <v>901</v>
       </c>
       <c r="B183" s="3" t="s">
-        <v>1141</v>
+        <v>1142</v>
       </c>
       <c r="C183" s="5" t="b">
         <v>1</v>
@@ -29771,7 +29774,7 @@
         <v>903</v>
       </c>
       <c r="B184" s="3" t="s">
-        <v>1141</v>
+        <v>1142</v>
       </c>
       <c r="C184" s="5" t="b">
         <v>1</v>
@@ -29827,7 +29830,7 @@
         <v>905</v>
       </c>
       <c r="B185" s="3" t="s">
-        <v>1141</v>
+        <v>1142</v>
       </c>
       <c r="C185" s="5" t="b">
         <v>1</v>
@@ -29883,7 +29886,7 @@
         <v>907</v>
       </c>
       <c r="B186" s="3" t="s">
-        <v>1141</v>
+        <v>1142</v>
       </c>
       <c r="C186" s="5" t="b">
         <v>1</v>
@@ -29939,7 +29942,7 @@
         <v>910</v>
       </c>
       <c r="B187" s="3" t="s">
-        <v>1141</v>
+        <v>1142</v>
       </c>
       <c r="C187" s="5" t="b">
         <v>1</v>
@@ -29995,7 +29998,7 @@
         <v>916</v>
       </c>
       <c r="B188" s="3" t="s">
-        <v>1141</v>
+        <v>1142</v>
       </c>
       <c r="C188" s="5" t="b">
         <v>1</v>
@@ -30051,7 +30054,7 @@
         <v>927</v>
       </c>
       <c r="B189" s="3" t="s">
-        <v>1141</v>
+        <v>1142</v>
       </c>
       <c r="C189" s="5" t="b">
         <v>1</v>
@@ -30163,7 +30166,7 @@
         <v>940</v>
       </c>
       <c r="B191" s="3" t="s">
-        <v>1141</v>
+        <v>1142</v>
       </c>
       <c r="C191" s="5" t="b">
         <v>1</v>
@@ -30275,7 +30278,7 @@
         <v>959</v>
       </c>
       <c r="B193" s="3" t="s">
-        <v>1141</v>
+        <v>1142</v>
       </c>
       <c r="C193" s="5" t="b">
         <v>1</v>
@@ -30331,7 +30334,7 @@
         <v>967</v>
       </c>
       <c r="B194" s="3" t="s">
-        <v>1141</v>
+        <v>1142</v>
       </c>
       <c r="C194" s="5" t="b">
         <v>1</v>
@@ -30387,7 +30390,7 @@
         <v>969</v>
       </c>
       <c r="B195" s="3" t="s">
-        <v>1141</v>
+        <v>1142</v>
       </c>
       <c r="C195" s="5" t="b">
         <v>1</v>
@@ -30443,7 +30446,7 @@
         <v>976</v>
       </c>
       <c r="B196" s="3" t="s">
-        <v>1141</v>
+        <v>1142</v>
       </c>
       <c r="C196" s="5" t="b">
         <v>1</v>
@@ -30499,7 +30502,7 @@
         <v>978</v>
       </c>
       <c r="B197" s="3" t="s">
-        <v>1141</v>
+        <v>1142</v>
       </c>
       <c r="C197" s="5" t="b">
         <v>1</v>
@@ -30555,7 +30558,7 @@
         <v>988</v>
       </c>
       <c r="B198" s="3" t="s">
-        <v>1141</v>
+        <v>1142</v>
       </c>
       <c r="C198" s="5" t="b">
         <v>1</v>
@@ -30611,7 +30614,7 @@
         <v>996</v>
       </c>
       <c r="B199" s="3" t="s">
-        <v>1141</v>
+        <v>1142</v>
       </c>
       <c r="C199" s="5" t="b">
         <v>1</v>
@@ -30667,7 +30670,7 @@
         <v>999</v>
       </c>
       <c r="B200" s="3" t="s">
-        <v>1141</v>
+        <v>1142</v>
       </c>
       <c r="C200" s="5" t="b">
         <v>1</v>
@@ -30723,7 +30726,7 @@
         <v>1007</v>
       </c>
       <c r="B201" s="3" t="s">
-        <v>1141</v>
+        <v>1142</v>
       </c>
       <c r="C201" s="5" t="b">
         <v>1</v>
@@ -30779,7 +30782,7 @@
         <v>1011</v>
       </c>
       <c r="B202" s="3" t="s">
-        <v>1141</v>
+        <v>1142</v>
       </c>
       <c r="C202" s="5" t="b">
         <v>1</v>
@@ -30835,7 +30838,7 @@
         <v>1021</v>
       </c>
       <c r="B203" s="3" t="s">
-        <v>1141</v>
+        <v>1142</v>
       </c>
       <c r="C203" s="5" t="b">
         <v>1</v>
@@ -30891,7 +30894,7 @@
         <v>1027</v>
       </c>
       <c r="B204" s="3" t="s">
-        <v>1141</v>
+        <v>1142</v>
       </c>
       <c r="C204" s="5" t="b">
         <v>1</v>
@@ -30947,7 +30950,7 @@
         <v>1030</v>
       </c>
       <c r="B205" s="3" t="s">
-        <v>1141</v>
+        <v>1142</v>
       </c>
       <c r="C205" s="5" t="b">
         <v>1</v>
@@ -31003,7 +31006,7 @@
         <v>1033</v>
       </c>
       <c r="B206" s="3" t="s">
-        <v>1141</v>
+        <v>1142</v>
       </c>
       <c r="C206" s="5" t="b">
         <v>1</v>
@@ -31059,7 +31062,7 @@
         <v>1040</v>
       </c>
       <c r="B207" s="3" t="s">
-        <v>1141</v>
+        <v>1142</v>
       </c>
       <c r="C207" s="5" t="b">
         <v>1</v>
@@ -31115,7 +31118,7 @@
         <v>1049</v>
       </c>
       <c r="B208" s="3" t="s">
-        <v>1141</v>
+        <v>1142</v>
       </c>
       <c r="C208" s="5" t="b">
         <v>1</v>
@@ -31171,7 +31174,7 @@
         <v>1051</v>
       </c>
       <c r="B209" s="3" t="s">
-        <v>1141</v>
+        <v>1142</v>
       </c>
       <c r="C209" s="5" t="b">
         <v>1</v>
@@ -31227,7 +31230,7 @@
         <v>1057</v>
       </c>
       <c r="B210" s="3" t="s">
-        <v>1141</v>
+        <v>1142</v>
       </c>
       <c r="C210" s="5" t="b">
         <v>1</v>
@@ -31283,7 +31286,7 @@
         <v>1059</v>
       </c>
       <c r="B211" s="3" t="s">
-        <v>1141</v>
+        <v>1142</v>
       </c>
       <c r="C211" s="5" t="b">
         <v>1</v>
@@ -31339,7 +31342,7 @@
         <v>1070</v>
       </c>
       <c r="B212" s="3" t="s">
-        <v>1141</v>
+        <v>1142</v>
       </c>
       <c r="C212" s="5" t="b">
         <v>1</v>
@@ -31395,7 +31398,7 @@
         <v>1072</v>
       </c>
       <c r="B213" s="3" t="s">
-        <v>1141</v>
+        <v>1142</v>
       </c>
       <c r="C213" s="5" t="b">
         <v>1</v>
@@ -31451,7 +31454,7 @@
         <v>1078</v>
       </c>
       <c r="B214" s="3" t="s">
-        <v>1141</v>
+        <v>1142</v>
       </c>
       <c r="C214" s="5" t="b">
         <v>1</v>
@@ -31507,7 +31510,7 @@
         <v>1080</v>
       </c>
       <c r="B215" s="3" t="s">
-        <v>1141</v>
+        <v>1142</v>
       </c>
       <c r="C215" s="5" t="b">
         <v>1</v>
@@ -31563,7 +31566,7 @@
         <v>1091</v>
       </c>
       <c r="B216" s="3" t="s">
-        <v>1141</v>
+        <v>1142</v>
       </c>
       <c r="C216" s="5" t="b">
         <v>1</v>
@@ -31619,7 +31622,7 @@
         <v>1095</v>
       </c>
       <c r="B217" s="3" t="s">
-        <v>1141</v>
+        <v>1142</v>
       </c>
       <c r="C217" s="5" t="b">
         <v>1</v>
@@ -31672,10 +31675,10 @@
     </row>
     <row r="218" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A218" s="3" t="s">
-        <v>1099</v>
+        <v>1100</v>
       </c>
       <c r="B218" s="3" t="s">
-        <v>1141</v>
+        <v>1142</v>
       </c>
       <c r="C218" s="5" t="b">
         <v>1</v>
@@ -31728,10 +31731,10 @@
     </row>
     <row r="219" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A219" s="3" t="s">
-        <v>1107</v>
+        <v>1108</v>
       </c>
       <c r="B219" s="3" t="s">
-        <v>1141</v>
+        <v>1142</v>
       </c>
       <c r="C219" s="5" t="b">
         <v>1</v>
@@ -31784,10 +31787,10 @@
     </row>
     <row r="220" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A220" s="3" t="s">
-        <v>1116</v>
+        <v>1117</v>
       </c>
       <c r="B220" s="3" t="s">
-        <v>1141</v>
+        <v>1142</v>
       </c>
       <c r="C220" s="5" t="b">
         <v>1</v>
@@ -31840,10 +31843,10 @@
     </row>
     <row r="221" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A221" s="3" t="s">
-        <v>1119</v>
+        <v>1120</v>
       </c>
       <c r="B221" s="3" t="s">
-        <v>1141</v>
+        <v>1142</v>
       </c>
       <c r="C221" s="5" t="b">
         <v>1</v>
@@ -31896,10 +31899,10 @@
     </row>
     <row r="222" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A222" s="3" t="s">
-        <v>1122</v>
+        <v>1123</v>
       </c>
       <c r="B222" s="3" t="s">
-        <v>1141</v>
+        <v>1142</v>
       </c>
       <c r="C222" s="5" t="b">
         <v>1</v>
@@ -31952,10 +31955,10 @@
     </row>
     <row r="223" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A223" s="3" t="s">
-        <v>1125</v>
+        <v>1126</v>
       </c>
       <c r="B223" s="3" t="s">
-        <v>1141</v>
+        <v>1142</v>
       </c>
       <c r="C223" s="5" t="b">
         <v>1</v>
@@ -32008,10 +32011,10 @@
     </row>
     <row r="224" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A224" s="3" t="s">
-        <v>1132</v>
+        <v>1133</v>
       </c>
       <c r="B224" s="3" t="s">
-        <v>1141</v>
+        <v>1142</v>
       </c>
       <c r="C224" s="5" t="b">
         <v>1</v>
@@ -32064,10 +32067,10 @@
     </row>
     <row r="225" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A225" s="3" t="s">
-        <v>1135</v>
+        <v>1136</v>
       </c>
       <c r="B225" s="3" t="s">
-        <v>1141</v>
+        <v>1142</v>
       </c>
       <c r="C225" s="5" t="b">
         <v>1</v>

</xml_diff>

<commit_message>
generated all the reports on 2024-05-08
</commit_message>
<xml_diff>
--- a/report/merged_configurations.xlsx
+++ b/report/merged_configurations.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5252" uniqueCount="1143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5252" uniqueCount="1144">
   <si>
     <t>naam</t>
   </si>
@@ -3275,10 +3275,10 @@
     <t>[{"naam":"Charter Overlijdensaangifte","waarde":"Charter OSLO_Overlijdensaangifte.pdf"}]</t>
   </si>
   <si>
-    <t>[{"naam":"Verslag Thematische Werkgroep I - 16 januari 2024","waarde":"20240116__ThematicWorkshop1_Verslag_OSLOOverlijdensaangifte.pdf"},{"naam":"Verslag Thematische Werkgroep II - 20 februari 2024","waarde":"20240220__ThematicWorkshop2_Verslag_OSLOOverlijdensaangifte.pdf"},{"naam":"Verslag Thematische Werkgroep III - 12 maart 2024","waarde":"20240312_ThematicWorkshop3_Verslag_OSLOOverlijdensaangifte.pdf"}]</t>
-  </si>
-  <si>
-    <t>[{"naam":"Presentatie Thematische Werkgroep I - 16 januari 2024","waarde":"20240116_ThematicWorkshop1_Powerpoint_OSLOOverlijdensaangifte.pptx"},{"naam":"Presentatie Thematische Werkgroep II - 20 februari 2024","waarde":"20240220_ThematicWorkshop2_Powerpoint_OSLOOverlijdensaangifte.pptx"},{"naam":"Presentatie Thematische Werkgroep III - 12 maart 2024","waarde":"20240312_ThematicWorkshop3_Powerpoint_OSLOOverlijdensaangifte.pptx"}]</t>
+    <t>[{"naam":"Verslag Thematische Werkgroep I - 16 januari 2024","waarde":"20240116_ThematicWorkshop1_Verslag_OSLOOverlijdensaangifte.pdf"},{"naam":"Verslag Thematische Werkgroep II - 20 februari 2024","waarde":"20240220__ThematicWorkshop2_Verslag_OSLOOverlijdensaangifte.pdf"},{"naam":"Verslag Thematische Werkgroep III - 12 maart 2024","waarde":"20240312_ThematicWorkshop3_Verslag_OSLOOverlijdensaangifte.pdf"},{"naam":"Verslag Thematische Werkgroep IV - 23 april 2024","waarde":"20240423_ThematicWorkshop4_Verslag_OSLOOverlijdensaangifte.pdf"}]</t>
+  </si>
+  <si>
+    <t>[{"naam":"Presentatie Thematische Werkgroep I - 16 januari 2024","waarde":"20240116_ThematicWorkshop1_Powerpoint_OSLOOverlijdensaangifte.pptx"},{"naam":"Presentatie Thematische Werkgroep II - 20 februari 2024","waarde":"20240220_ThematicWorkshop2_Powerpoint_OSLOOverlijdensaangifte.pptx"},{"naam":"Presentatie Thematische Werkgroep III - 12 maart 2024","waarde":"20240312_ThematicWorkshop3_Powerpoint_OSLOOverlijdensaangifte.pptx"},{"naam":"Presentatie Thematische Werkgroep IV - 23 april 2024","waarde":"20240423_ThematicWorkshop4_Powerpoint_OSLOOverlijdensaangifte.pptx"}]</t>
   </si>
   <si>
     <t>Lokale besturen, alle entiteiten van de Vlaamse overheid, zorgsector, uitvaartsector</t>
@@ -3299,6 +3299,9 @@
     <t>[{"naam":"Applicatieprofiel Overlijdensaangifte","waarde":"https://data.vlaanderen.be/doc/applicatieprofiel/overlijdensaangifte"},{"naam":"Vocabularium Gezondsheidstoestand Persoon","waarde":"https://data.vlaanderen.be/ns/gezondheidstoestand"}]</t>
   </si>
   <si>
+    <t>[{"naam":"Verslag Thematische Werkgroep I - 16 januari 2024","waarde":"20240116__ThematicWorkshop1_Verslag_OSLOOverlijdensaangifte.pdf"},{"naam":"Verslag Thematische Werkgroep II - 20 februari 2024","waarde":"20240220__ThematicWorkshop2_Verslag_OSLOOverlijdensaangifte.pdf"},{"naam":"Verslag Thematische Werkgroep III - 12 maart 2024","waarde":"20240312_ThematicWorkshop3_Verslag_OSLOOverlijdensaangifte.pdf"},{"naam":"Verslag Thematische Werkgroep IV - 23 april 2024","waarde":"20240423_ThematicWorkshop4_Verslag_OSLOOverlijdensaangifte.pdf"}]</t>
+  </si>
+  <si>
     <t>Vocabularium Gezondheidstoestand Persoon</t>
   </si>
   <si>
@@ -3311,7 +3314,7 @@
     <t>[{"naam":"Vocabularium Overlijdensaangifte","waarde":"https://data.vlaanderen.be/ns/overlijdensaangifte"},{"naam":"Applicatieprofiel Overlijdensaangifte","waarde":"https://data.vlaanderen.be/doc/applicatieprofiel/overlijdensaangifte"}]</t>
   </si>
   <si>
-    <t>[{"naam":"Verslag Thematische Werkgroep I - 16 januari 2024","waarde":"20240116__ThematicWorkshop1_Verslag_OSLOOverlijdensaangifte.pdf"},{"naam":"Verslag Thematische Werkgroep II - 20 februari 2024","waarde":"20240220_ThematicWorkshop2_Verslag_OSLOOverlijdensaangifte.pdf"},{"naam":"Verslag Thematische Werkgroep III - 12 maart 2024","waarde":"20240312_ThematicWorkshop3_Verslag_OSLOOverlijdensaangifte.pdf"}]</t>
+    <t>[{"naam":"Verslag Thematische Werkgroep I - 16 januari 2024","waarde":"20240116__ThematicWorkshop1_Verslag_OSLOOverlijdensaangifte.pdf"},{"naam":"Verslag Thematische Werkgroep II - 20 februari 2024","waarde":"20240220_ThematicWorkshop2_Verslag_OSLOOverlijdensaangifte.pdf"},{"naam":"Verslag Thematische Werkgroep III - 12 maart 2024","waarde":"20240312_ThematicWorkshop3_Verslag_OSLOOverlijdensaangifte.pdf"},{"naam":"Verslag Thematische Werkgroep IV - 23 april 2024","waarde":"20240423_ThematicWorkshop4_Verslag_OSLOOverlijdensaangifte.pdf"}]</t>
   </si>
   <si>
     <t>Applicatieprofiel Kindfiche</t>
@@ -18850,7 +18853,7 @@
         <v>1086</v>
       </c>
       <c r="L216" s="3" t="s">
-        <v>1087</v>
+        <v>1095</v>
       </c>
       <c r="M216" s="3" t="s">
         <v>1088</v>
@@ -18888,7 +18891,7 @@
     </row>
     <row r="217" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A217" s="3" t="s">
-        <v>1095</v>
+        <v>1096</v>
       </c>
       <c r="B217" s="3"/>
       <c r="C217" s="3" t="s">
@@ -18907,19 +18910,19 @@
         <v>39</v>
       </c>
       <c r="H217" s="3" t="s">
-        <v>1096</v>
+        <v>1097</v>
       </c>
       <c r="I217" s="3" t="s">
-        <v>1097</v>
+        <v>1098</v>
       </c>
       <c r="J217" s="3" t="s">
-        <v>1098</v>
+        <v>1099</v>
       </c>
       <c r="K217" s="3" t="s">
         <v>1086</v>
       </c>
       <c r="L217" s="3" t="s">
-        <v>1099</v>
+        <v>1100</v>
       </c>
       <c r="M217" s="3" t="s">
         <v>1088</v>
@@ -18957,7 +18960,7 @@
     </row>
     <row r="218" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A218" s="3" t="s">
-        <v>1100</v>
+        <v>1101</v>
       </c>
       <c r="B218" s="3"/>
       <c r="C218" s="3" t="s">
@@ -18976,31 +18979,31 @@
         <v>28</v>
       </c>
       <c r="H218" s="3" t="s">
-        <v>1101</v>
+        <v>1102</v>
       </c>
       <c r="I218" s="3" t="s">
-        <v>1102</v>
+        <v>1103</v>
       </c>
       <c r="J218" s="3" t="s">
         <v>31</v>
       </c>
       <c r="K218" s="3" t="s">
-        <v>1103</v>
+        <v>1104</v>
       </c>
       <c r="L218" s="3" t="s">
-        <v>1104</v>
+        <v>1105</v>
       </c>
       <c r="M218" s="3" t="s">
-        <v>1105</v>
+        <v>1106</v>
       </c>
       <c r="N218" s="3" t="s">
         <v>50</v>
       </c>
       <c r="O218" s="3" t="s">
-        <v>1106</v>
+        <v>1107</v>
       </c>
       <c r="P218" s="3" t="s">
-        <v>1107</v>
+        <v>1108</v>
       </c>
       <c r="Q218" s="3" t="s">
         <v>26</v>
@@ -19026,17 +19029,17 @@
     </row>
     <row r="219" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A219" s="3" t="s">
-        <v>1108</v>
+        <v>1109</v>
       </c>
       <c r="B219" s="3"/>
       <c r="C219" s="3" t="s">
-        <v>1109</v>
+        <v>1110</v>
       </c>
       <c r="D219" s="3" t="s">
-        <v>1110</v>
+        <v>1111</v>
       </c>
       <c r="E219" s="3" t="s">
-        <v>1111</v>
+        <v>1112</v>
       </c>
       <c r="F219" s="3" t="s">
         <v>43</v>
@@ -19045,31 +19048,31 @@
         <v>39</v>
       </c>
       <c r="H219" s="3" t="s">
-        <v>1112</v>
+        <v>1113</v>
       </c>
       <c r="I219" s="3" t="s">
-        <v>1113</v>
+        <v>1114</v>
       </c>
       <c r="J219" s="3" t="s">
-        <v>1114</v>
+        <v>1115</v>
       </c>
       <c r="K219" s="3" t="s">
         <v>31</v>
       </c>
       <c r="L219" s="3" t="s">
-        <v>1114</v>
+        <v>1115</v>
       </c>
       <c r="M219" s="3" t="s">
-        <v>1114</v>
+        <v>1115</v>
       </c>
       <c r="N219" s="3" t="s">
-        <v>1115</v>
+        <v>1116</v>
       </c>
       <c r="O219" s="3" t="s">
         <v>70</v>
       </c>
       <c r="P219" s="3" t="s">
-        <v>1116</v>
+        <v>1117</v>
       </c>
       <c r="Q219" s="3" t="s">
         <v>26</v>
@@ -19095,17 +19098,17 @@
     </row>
     <row r="220" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A220" s="3" t="s">
-        <v>1117</v>
+        <v>1118</v>
       </c>
       <c r="B220" s="3"/>
       <c r="C220" s="3" t="s">
-        <v>1109</v>
+        <v>1110</v>
       </c>
       <c r="D220" s="3" t="s">
-        <v>1110</v>
+        <v>1111</v>
       </c>
       <c r="E220" s="3" t="s">
-        <v>1111</v>
+        <v>1112</v>
       </c>
       <c r="F220" s="3" t="s">
         <v>43</v>
@@ -19114,31 +19117,31 @@
         <v>28</v>
       </c>
       <c r="H220" s="3" t="s">
-        <v>1118</v>
+        <v>1119</v>
       </c>
       <c r="I220" s="3" t="s">
-        <v>1119</v>
+        <v>1120</v>
       </c>
       <c r="J220" s="3" t="s">
-        <v>1114</v>
+        <v>1115</v>
       </c>
       <c r="K220" s="3" t="s">
         <v>31</v>
       </c>
       <c r="L220" s="3" t="s">
-        <v>1114</v>
+        <v>1115</v>
       </c>
       <c r="M220" s="3" t="s">
-        <v>1114</v>
+        <v>1115</v>
       </c>
       <c r="N220" s="3" t="s">
-        <v>1115</v>
+        <v>1116</v>
       </c>
       <c r="O220" s="3" t="s">
         <v>70</v>
       </c>
       <c r="P220" s="3" t="s">
-        <v>1116</v>
+        <v>1117</v>
       </c>
       <c r="Q220" s="3" t="s">
         <v>26</v>
@@ -19164,17 +19167,17 @@
     </row>
     <row r="221" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A221" s="3" t="s">
-        <v>1120</v>
+        <v>1121</v>
       </c>
       <c r="B221" s="3"/>
       <c r="C221" s="3" t="s">
-        <v>1109</v>
+        <v>1110</v>
       </c>
       <c r="D221" s="3" t="s">
-        <v>1110</v>
+        <v>1111</v>
       </c>
       <c r="E221" s="3" t="s">
-        <v>1111</v>
+        <v>1112</v>
       </c>
       <c r="F221" s="3" t="s">
         <v>43</v>
@@ -19183,31 +19186,31 @@
         <v>39</v>
       </c>
       <c r="H221" s="3" t="s">
-        <v>1121</v>
+        <v>1122</v>
       </c>
       <c r="I221" s="3" t="s">
-        <v>1122</v>
+        <v>1123</v>
       </c>
       <c r="J221" s="3" t="s">
-        <v>1114</v>
+        <v>1115</v>
       </c>
       <c r="K221" s="3" t="s">
         <v>31</v>
       </c>
       <c r="L221" s="3" t="s">
-        <v>1114</v>
+        <v>1115</v>
       </c>
       <c r="M221" s="3" t="s">
-        <v>1114</v>
+        <v>1115</v>
       </c>
       <c r="N221" s="3" t="s">
-        <v>1115</v>
+        <v>1116</v>
       </c>
       <c r="O221" s="3" t="s">
         <v>70</v>
       </c>
       <c r="P221" s="3" t="s">
-        <v>1116</v>
+        <v>1117</v>
       </c>
       <c r="Q221" s="3" t="s">
         <v>26</v>
@@ -19233,17 +19236,17 @@
     </row>
     <row r="222" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A222" s="3" t="s">
-        <v>1123</v>
+        <v>1124</v>
       </c>
       <c r="B222" s="3"/>
       <c r="C222" s="3" t="s">
-        <v>1109</v>
+        <v>1110</v>
       </c>
       <c r="D222" s="3" t="s">
-        <v>1110</v>
+        <v>1111</v>
       </c>
       <c r="E222" s="3" t="s">
-        <v>1111</v>
+        <v>1112</v>
       </c>
       <c r="F222" s="3" t="s">
         <v>43</v>
@@ -19252,31 +19255,31 @@
         <v>28</v>
       </c>
       <c r="H222" s="3" t="s">
-        <v>1124</v>
+        <v>1125</v>
       </c>
       <c r="I222" s="3" t="s">
-        <v>1125</v>
+        <v>1126</v>
       </c>
       <c r="J222" s="3" t="s">
-        <v>1114</v>
+        <v>1115</v>
       </c>
       <c r="K222" s="3" t="s">
         <v>31</v>
       </c>
       <c r="L222" s="3" t="s">
-        <v>1114</v>
+        <v>1115</v>
       </c>
       <c r="M222" s="3" t="s">
-        <v>1114</v>
+        <v>1115</v>
       </c>
       <c r="N222" s="3" t="s">
-        <v>1115</v>
+        <v>1116</v>
       </c>
       <c r="O222" s="3" t="s">
         <v>70</v>
       </c>
       <c r="P222" s="3" t="s">
-        <v>1116</v>
+        <v>1117</v>
       </c>
       <c r="Q222" s="3" t="s">
         <v>26</v>
@@ -19302,17 +19305,17 @@
     </row>
     <row r="223" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A223" s="3" t="s">
-        <v>1126</v>
+        <v>1127</v>
       </c>
       <c r="B223" s="3"/>
       <c r="C223" s="3" t="s">
-        <v>1109</v>
+        <v>1110</v>
       </c>
       <c r="D223" s="3" t="s">
-        <v>1110</v>
+        <v>1111</v>
       </c>
       <c r="E223" s="3" t="s">
-        <v>1111</v>
+        <v>1112</v>
       </c>
       <c r="F223" s="3" t="s">
         <v>43</v>
@@ -19321,31 +19324,31 @@
         <v>28</v>
       </c>
       <c r="H223" s="3" t="s">
-        <v>1127</v>
+        <v>1128</v>
       </c>
       <c r="I223" s="3" t="s">
-        <v>1128</v>
+        <v>1129</v>
       </c>
       <c r="J223" s="3" t="s">
-        <v>1129</v>
+        <v>1130</v>
       </c>
       <c r="K223" s="3" t="s">
         <v>31</v>
       </c>
       <c r="L223" s="3" t="s">
-        <v>1130</v>
+        <v>1131</v>
       </c>
       <c r="M223" s="3" t="s">
-        <v>1131</v>
+        <v>1132</v>
       </c>
       <c r="N223" s="3" t="s">
-        <v>1132</v>
+        <v>1133</v>
       </c>
       <c r="O223" s="3" t="s">
         <v>97</v>
       </c>
       <c r="P223" s="3" t="s">
-        <v>1116</v>
+        <v>1117</v>
       </c>
       <c r="Q223" s="3" t="s">
         <v>26</v>
@@ -19371,17 +19374,17 @@
     </row>
     <row r="224" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A224" s="3" t="s">
-        <v>1133</v>
+        <v>1134</v>
       </c>
       <c r="B224" s="3"/>
       <c r="C224" s="3" t="s">
-        <v>1109</v>
+        <v>1110</v>
       </c>
       <c r="D224" s="3" t="s">
-        <v>1110</v>
+        <v>1111</v>
       </c>
       <c r="E224" s="3" t="s">
-        <v>1111</v>
+        <v>1112</v>
       </c>
       <c r="F224" s="3" t="s">
         <v>43</v>
@@ -19390,31 +19393,31 @@
         <v>39</v>
       </c>
       <c r="H224" s="3" t="s">
-        <v>1134</v>
+        <v>1135</v>
       </c>
       <c r="I224" s="3" t="s">
-        <v>1135</v>
+        <v>1136</v>
       </c>
       <c r="J224" s="3" t="s">
-        <v>1129</v>
+        <v>1130</v>
       </c>
       <c r="K224" s="3" t="s">
         <v>31</v>
       </c>
       <c r="L224" s="3" t="s">
-        <v>1130</v>
+        <v>1131</v>
       </c>
       <c r="M224" s="3" t="s">
-        <v>1131</v>
+        <v>1132</v>
       </c>
       <c r="N224" s="3" t="s">
-        <v>1132</v>
+        <v>1133</v>
       </c>
       <c r="O224" s="3" t="s">
         <v>97</v>
       </c>
       <c r="P224" s="3" t="s">
-        <v>1116</v>
+        <v>1117</v>
       </c>
       <c r="Q224" s="3" t="s">
         <v>26</v>
@@ -19440,7 +19443,7 @@
     </row>
     <row r="225" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A225" s="3" t="s">
-        <v>1136</v>
+        <v>1137</v>
       </c>
       <c r="B225" s="3"/>
       <c r="C225" s="3" t="s">
@@ -19459,10 +19462,10 @@
         <v>28</v>
       </c>
       <c r="H225" s="3" t="s">
-        <v>1137</v>
+        <v>1138</v>
       </c>
       <c r="I225" s="3" t="s">
-        <v>1138</v>
+        <v>1139</v>
       </c>
       <c r="J225" s="3" t="s">
         <v>31</v>
@@ -19471,13 +19474,13 @@
         <v>31</v>
       </c>
       <c r="L225" s="3" t="s">
-        <v>1139</v>
+        <v>1140</v>
       </c>
       <c r="M225" s="3" t="s">
-        <v>1140</v>
+        <v>1141</v>
       </c>
       <c r="N225" s="3" t="s">
-        <v>1141</v>
+        <v>1142</v>
       </c>
       <c r="O225" s="3" t="s">
         <v>70</v>
@@ -19582,7 +19585,7 @@
         <v>23</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>1142</v>
+        <v>1143</v>
       </c>
       <c r="C2" s="5" t="b">
         <v>1</v>
@@ -19638,7 +19641,7 @@
         <v>38</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>1142</v>
+        <v>1143</v>
       </c>
       <c r="C3" s="5" t="b">
         <v>1</v>
@@ -19694,7 +19697,7 @@
         <v>41</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>1142</v>
+        <v>1143</v>
       </c>
       <c r="C4" s="5" t="b">
         <v>1</v>
@@ -19750,7 +19753,7 @@
         <v>53</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>1142</v>
+        <v>1143</v>
       </c>
       <c r="C5" s="5" t="b">
         <v>1</v>
@@ -19806,7 +19809,7 @@
         <v>60</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>1142</v>
+        <v>1143</v>
       </c>
       <c r="C6" s="5" t="b">
         <v>1</v>
@@ -19862,7 +19865,7 @@
         <v>63</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>1142</v>
+        <v>1143</v>
       </c>
       <c r="C7" s="5" t="b">
         <v>1</v>
@@ -19918,7 +19921,7 @@
         <v>72</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>1142</v>
+        <v>1143</v>
       </c>
       <c r="C8" s="5" t="b">
         <v>1</v>
@@ -19974,7 +19977,7 @@
         <v>74</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>1142</v>
+        <v>1143</v>
       </c>
       <c r="C9" s="5" t="b">
         <v>1</v>
@@ -20030,7 +20033,7 @@
         <v>81</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>1142</v>
+        <v>1143</v>
       </c>
       <c r="C10" s="5" t="b">
         <v>1</v>
@@ -20086,7 +20089,7 @@
         <v>83</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>1142</v>
+        <v>1143</v>
       </c>
       <c r="C11" s="5" t="b">
         <v>1</v>
@@ -20142,7 +20145,7 @@
         <v>90</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>1142</v>
+        <v>1143</v>
       </c>
       <c r="C12" s="5" t="b">
         <v>1</v>
@@ -20198,7 +20201,7 @@
         <v>100</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>1142</v>
+        <v>1143</v>
       </c>
       <c r="C13" s="5" t="b">
         <v>1</v>
@@ -20254,7 +20257,7 @@
         <v>103</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>1142</v>
+        <v>1143</v>
       </c>
       <c r="C14" s="5" t="b">
         <v>1</v>
@@ -20310,7 +20313,7 @@
         <v>114</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>1142</v>
+        <v>1143</v>
       </c>
       <c r="C15" s="5" t="b">
         <v>1</v>
@@ -20478,7 +20481,7 @@
         <v>140</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>1142</v>
+        <v>1143</v>
       </c>
       <c r="C18" s="5" t="b">
         <v>1</v>
@@ -20534,7 +20537,7 @@
         <v>151</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>1142</v>
+        <v>1143</v>
       </c>
       <c r="C19" s="5" t="b">
         <v>1</v>
@@ -20590,7 +20593,7 @@
         <v>153</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>1142</v>
+        <v>1143</v>
       </c>
       <c r="C20" s="5" t="b">
         <v>1</v>
@@ -20646,7 +20649,7 @@
         <v>155</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>1142</v>
+        <v>1143</v>
       </c>
       <c r="C21" s="5" t="b">
         <v>1</v>
@@ -20702,7 +20705,7 @@
         <v>157</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>1142</v>
+        <v>1143</v>
       </c>
       <c r="C22" s="5" t="b">
         <v>1</v>
@@ -20758,7 +20761,7 @@
         <v>160</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>1142</v>
+        <v>1143</v>
       </c>
       <c r="C23" s="5" t="b">
         <v>1</v>
@@ -20814,7 +20817,7 @@
         <v>162</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>1142</v>
+        <v>1143</v>
       </c>
       <c r="C24" s="5" t="b">
         <v>1</v>
@@ -20870,7 +20873,7 @@
         <v>164</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>1142</v>
+        <v>1143</v>
       </c>
       <c r="C25" s="5" t="b">
         <v>1</v>
@@ -20926,7 +20929,7 @@
         <v>166</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>1142</v>
+        <v>1143</v>
       </c>
       <c r="C26" s="5" t="b">
         <v>1</v>
@@ -20982,7 +20985,7 @@
         <v>168</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>1142</v>
+        <v>1143</v>
       </c>
       <c r="C27" s="5" t="b">
         <v>1</v>
@@ -21038,7 +21041,7 @@
         <v>170</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>1142</v>
+        <v>1143</v>
       </c>
       <c r="C28" s="5" t="b">
         <v>1</v>
@@ -21094,7 +21097,7 @@
         <v>168</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>1142</v>
+        <v>1143</v>
       </c>
       <c r="C29" s="5" t="b">
         <v>1</v>
@@ -21150,7 +21153,7 @@
         <v>172</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>1142</v>
+        <v>1143</v>
       </c>
       <c r="C30" s="5" t="b">
         <v>1</v>
@@ -21206,7 +21209,7 @@
         <v>174</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>1142</v>
+        <v>1143</v>
       </c>
       <c r="C31" s="5" t="b">
         <v>1</v>
@@ -21262,7 +21265,7 @@
         <v>176</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>1142</v>
+        <v>1143</v>
       </c>
       <c r="C32" s="5" t="b">
         <v>1</v>
@@ -21318,7 +21321,7 @@
         <v>178</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>1142</v>
+        <v>1143</v>
       </c>
       <c r="C33" s="5" t="b">
         <v>1</v>
@@ -21374,7 +21377,7 @@
         <v>180</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>1142</v>
+        <v>1143</v>
       </c>
       <c r="C34" s="5" t="b">
         <v>1</v>
@@ -21430,7 +21433,7 @@
         <v>182</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>1142</v>
+        <v>1143</v>
       </c>
       <c r="C35" s="5" t="b">
         <v>1</v>
@@ -21486,7 +21489,7 @@
         <v>184</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>1142</v>
+        <v>1143</v>
       </c>
       <c r="C36" s="5" t="b">
         <v>1</v>
@@ -21542,7 +21545,7 @@
         <v>186</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>1142</v>
+        <v>1143</v>
       </c>
       <c r="C37" s="5" t="b">
         <v>1</v>
@@ -21598,7 +21601,7 @@
         <v>188</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>1142</v>
+        <v>1143</v>
       </c>
       <c r="C38" s="5" t="b">
         <v>1</v>
@@ -21766,7 +21769,7 @@
         <v>218</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>1142</v>
+        <v>1143</v>
       </c>
       <c r="C41" s="5" t="b">
         <v>1</v>
@@ -21822,7 +21825,7 @@
         <v>226</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>1142</v>
+        <v>1143</v>
       </c>
       <c r="C42" s="5" t="b">
         <v>1</v>
@@ -23390,7 +23393,7 @@
         <v>408</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>1142</v>
+        <v>1143</v>
       </c>
       <c r="C70" s="5" t="b">
         <v>1</v>
@@ -23446,7 +23449,7 @@
         <v>420</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>1142</v>
+        <v>1143</v>
       </c>
       <c r="C71" s="5" t="b">
         <v>1</v>
@@ -23894,7 +23897,7 @@
         <v>479</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>1142</v>
+        <v>1143</v>
       </c>
       <c r="C79" s="5" t="b">
         <v>1</v>
@@ -24566,7 +24569,7 @@
         <v>560</v>
       </c>
       <c r="B91" s="3" t="s">
-        <v>1142</v>
+        <v>1143</v>
       </c>
       <c r="C91" s="5" t="b">
         <v>1</v>
@@ -24622,7 +24625,7 @@
         <v>569</v>
       </c>
       <c r="B92" s="3" t="s">
-        <v>1142</v>
+        <v>1143</v>
       </c>
       <c r="C92" s="5" t="b">
         <v>1</v>
@@ -24678,7 +24681,7 @@
         <v>571</v>
       </c>
       <c r="B93" s="3" t="s">
-        <v>1142</v>
+        <v>1143</v>
       </c>
       <c r="C93" s="5" t="b">
         <v>1</v>
@@ -26806,7 +26809,7 @@
         <v>724</v>
       </c>
       <c r="B131" s="3" t="s">
-        <v>1142</v>
+        <v>1143</v>
       </c>
       <c r="C131" s="5" t="b">
         <v>1</v>
@@ -27366,7 +27369,7 @@
         <v>756</v>
       </c>
       <c r="B141" s="3" t="s">
-        <v>1142</v>
+        <v>1143</v>
       </c>
       <c r="C141" s="5" t="b">
         <v>1</v>
@@ -27422,7 +27425,7 @@
         <v>762</v>
       </c>
       <c r="B142" s="3" t="s">
-        <v>1142</v>
+        <v>1143</v>
       </c>
       <c r="C142" s="5" t="b">
         <v>1</v>
@@ -27590,7 +27593,7 @@
         <v>782</v>
       </c>
       <c r="B145" s="3" t="s">
-        <v>1142</v>
+        <v>1143</v>
       </c>
       <c r="C145" s="5" t="b">
         <v>1</v>
@@ -27646,7 +27649,7 @@
         <v>784</v>
       </c>
       <c r="B146" s="3" t="s">
-        <v>1142</v>
+        <v>1143</v>
       </c>
       <c r="C146" s="5" t="b">
         <v>1</v>
@@ -27702,7 +27705,7 @@
         <v>793</v>
       </c>
       <c r="B147" s="3" t="s">
-        <v>1142</v>
+        <v>1143</v>
       </c>
       <c r="C147" s="5" t="b">
         <v>1</v>
@@ -27758,7 +27761,7 @@
         <v>797</v>
       </c>
       <c r="B148" s="3" t="s">
-        <v>1142</v>
+        <v>1143</v>
       </c>
       <c r="C148" s="5" t="b">
         <v>1</v>
@@ -27814,7 +27817,7 @@
         <v>800</v>
       </c>
       <c r="B149" s="3" t="s">
-        <v>1142</v>
+        <v>1143</v>
       </c>
       <c r="C149" s="5" t="b">
         <v>1</v>
@@ -27870,7 +27873,7 @@
         <v>803</v>
       </c>
       <c r="B150" s="3" t="s">
-        <v>1142</v>
+        <v>1143</v>
       </c>
       <c r="C150" s="5" t="b">
         <v>1</v>
@@ -27926,7 +27929,7 @@
         <v>806</v>
       </c>
       <c r="B151" s="3" t="s">
-        <v>1142</v>
+        <v>1143</v>
       </c>
       <c r="C151" s="5" t="b">
         <v>1</v>
@@ -27982,7 +27985,7 @@
         <v>809</v>
       </c>
       <c r="B152" s="3" t="s">
-        <v>1142</v>
+        <v>1143</v>
       </c>
       <c r="C152" s="5" t="b">
         <v>1</v>
@@ -28038,7 +28041,7 @@
         <v>812</v>
       </c>
       <c r="B153" s="3" t="s">
-        <v>1142</v>
+        <v>1143</v>
       </c>
       <c r="C153" s="5" t="b">
         <v>1</v>
@@ -28094,7 +28097,7 @@
         <v>815</v>
       </c>
       <c r="B154" s="3" t="s">
-        <v>1142</v>
+        <v>1143</v>
       </c>
       <c r="C154" s="5" t="b">
         <v>1</v>
@@ -28150,7 +28153,7 @@
         <v>818</v>
       </c>
       <c r="B155" s="3" t="s">
-        <v>1142</v>
+        <v>1143</v>
       </c>
       <c r="C155" s="5" t="b">
         <v>1</v>
@@ -28206,7 +28209,7 @@
         <v>821</v>
       </c>
       <c r="B156" s="3" t="s">
-        <v>1142</v>
+        <v>1143</v>
       </c>
       <c r="C156" s="5" t="b">
         <v>1</v>
@@ -28262,7 +28265,7 @@
         <v>824</v>
       </c>
       <c r="B157" s="3" t="s">
-        <v>1142</v>
+        <v>1143</v>
       </c>
       <c r="C157" s="5" t="b">
         <v>1</v>
@@ -28318,7 +28321,7 @@
         <v>827</v>
       </c>
       <c r="B158" s="3" t="s">
-        <v>1142</v>
+        <v>1143</v>
       </c>
       <c r="C158" s="5" t="b">
         <v>1</v>
@@ -28374,7 +28377,7 @@
         <v>830</v>
       </c>
       <c r="B159" s="3" t="s">
-        <v>1142</v>
+        <v>1143</v>
       </c>
       <c r="C159" s="5" t="b">
         <v>1</v>
@@ -28430,7 +28433,7 @@
         <v>833</v>
       </c>
       <c r="B160" s="3" t="s">
-        <v>1142</v>
+        <v>1143</v>
       </c>
       <c r="C160" s="5" t="b">
         <v>1</v>
@@ -28486,7 +28489,7 @@
         <v>836</v>
       </c>
       <c r="B161" s="3" t="s">
-        <v>1142</v>
+        <v>1143</v>
       </c>
       <c r="C161" s="5" t="b">
         <v>1</v>
@@ -28542,7 +28545,7 @@
         <v>839</v>
       </c>
       <c r="B162" s="3" t="s">
-        <v>1142</v>
+        <v>1143</v>
       </c>
       <c r="C162" s="5" t="b">
         <v>1</v>
@@ -28598,7 +28601,7 @@
         <v>842</v>
       </c>
       <c r="B163" s="3" t="s">
-        <v>1142</v>
+        <v>1143</v>
       </c>
       <c r="C163" s="5" t="b">
         <v>1</v>
@@ -28654,7 +28657,7 @@
         <v>845</v>
       </c>
       <c r="B164" s="3" t="s">
-        <v>1142</v>
+        <v>1143</v>
       </c>
       <c r="C164" s="5" t="b">
         <v>1</v>
@@ -28710,7 +28713,7 @@
         <v>848</v>
       </c>
       <c r="B165" s="3" t="s">
-        <v>1142</v>
+        <v>1143</v>
       </c>
       <c r="C165" s="5" t="b">
         <v>1</v>
@@ -28766,7 +28769,7 @@
         <v>851</v>
       </c>
       <c r="B166" s="3" t="s">
-        <v>1142</v>
+        <v>1143</v>
       </c>
       <c r="C166" s="5" t="b">
         <v>1</v>
@@ -28822,7 +28825,7 @@
         <v>854</v>
       </c>
       <c r="B167" s="3" t="s">
-        <v>1142</v>
+        <v>1143</v>
       </c>
       <c r="C167" s="5" t="b">
         <v>1</v>
@@ -28878,7 +28881,7 @@
         <v>857</v>
       </c>
       <c r="B168" s="3" t="s">
-        <v>1142</v>
+        <v>1143</v>
       </c>
       <c r="C168" s="5" t="b">
         <v>1</v>
@@ -28934,7 +28937,7 @@
         <v>860</v>
       </c>
       <c r="B169" s="3" t="s">
-        <v>1142</v>
+        <v>1143</v>
       </c>
       <c r="C169" s="5" t="b">
         <v>1</v>
@@ -28990,7 +28993,7 @@
         <v>863</v>
       </c>
       <c r="B170" s="3" t="s">
-        <v>1142</v>
+        <v>1143</v>
       </c>
       <c r="C170" s="5" t="b">
         <v>1</v>
@@ -29046,7 +29049,7 @@
         <v>866</v>
       </c>
       <c r="B171" s="3" t="s">
-        <v>1142</v>
+        <v>1143</v>
       </c>
       <c r="C171" s="5" t="b">
         <v>1</v>
@@ -29102,7 +29105,7 @@
         <v>869</v>
       </c>
       <c r="B172" s="3" t="s">
-        <v>1142</v>
+        <v>1143</v>
       </c>
       <c r="C172" s="5" t="b">
         <v>1</v>
@@ -29158,7 +29161,7 @@
         <v>872</v>
       </c>
       <c r="B173" s="3" t="s">
-        <v>1142</v>
+        <v>1143</v>
       </c>
       <c r="C173" s="5" t="b">
         <v>1</v>
@@ -29214,7 +29217,7 @@
         <v>875</v>
       </c>
       <c r="B174" s="3" t="s">
-        <v>1142</v>
+        <v>1143</v>
       </c>
       <c r="C174" s="5" t="b">
         <v>1</v>
@@ -29270,7 +29273,7 @@
         <v>878</v>
       </c>
       <c r="B175" s="3" t="s">
-        <v>1142</v>
+        <v>1143</v>
       </c>
       <c r="C175" s="5" t="b">
         <v>1</v>
@@ -29326,7 +29329,7 @@
         <v>881</v>
       </c>
       <c r="B176" s="3" t="s">
-        <v>1142</v>
+        <v>1143</v>
       </c>
       <c r="C176" s="5" t="b">
         <v>1</v>
@@ -29382,7 +29385,7 @@
         <v>884</v>
       </c>
       <c r="B177" s="3" t="s">
-        <v>1142</v>
+        <v>1143</v>
       </c>
       <c r="C177" s="5" t="b">
         <v>1</v>
@@ -29438,7 +29441,7 @@
         <v>887</v>
       </c>
       <c r="B178" s="3" t="s">
-        <v>1142</v>
+        <v>1143</v>
       </c>
       <c r="C178" s="5" t="b">
         <v>1</v>
@@ -29494,7 +29497,7 @@
         <v>890</v>
       </c>
       <c r="B179" s="3" t="s">
-        <v>1142</v>
+        <v>1143</v>
       </c>
       <c r="C179" s="5" t="b">
         <v>1</v>
@@ -29550,7 +29553,7 @@
         <v>893</v>
       </c>
       <c r="B180" s="3" t="s">
-        <v>1142</v>
+        <v>1143</v>
       </c>
       <c r="C180" s="5" t="b">
         <v>1</v>
@@ -29606,7 +29609,7 @@
         <v>896</v>
       </c>
       <c r="B181" s="3" t="s">
-        <v>1142</v>
+        <v>1143</v>
       </c>
       <c r="C181" s="5" t="b">
         <v>1</v>
@@ -29662,7 +29665,7 @@
         <v>898</v>
       </c>
       <c r="B182" s="3" t="s">
-        <v>1142</v>
+        <v>1143</v>
       </c>
       <c r="C182" s="5" t="b">
         <v>1</v>
@@ -29718,7 +29721,7 @@
         <v>901</v>
       </c>
       <c r="B183" s="3" t="s">
-        <v>1142</v>
+        <v>1143</v>
       </c>
       <c r="C183" s="5" t="b">
         <v>1</v>
@@ -29774,7 +29777,7 @@
         <v>903</v>
       </c>
       <c r="B184" s="3" t="s">
-        <v>1142</v>
+        <v>1143</v>
       </c>
       <c r="C184" s="5" t="b">
         <v>1</v>
@@ -29830,7 +29833,7 @@
         <v>905</v>
       </c>
       <c r="B185" s="3" t="s">
-        <v>1142</v>
+        <v>1143</v>
       </c>
       <c r="C185" s="5" t="b">
         <v>1</v>
@@ -29886,7 +29889,7 @@
         <v>907</v>
       </c>
       <c r="B186" s="3" t="s">
-        <v>1142</v>
+        <v>1143</v>
       </c>
       <c r="C186" s="5" t="b">
         <v>1</v>
@@ -29942,7 +29945,7 @@
         <v>910</v>
       </c>
       <c r="B187" s="3" t="s">
-        <v>1142</v>
+        <v>1143</v>
       </c>
       <c r="C187" s="5" t="b">
         <v>1</v>
@@ -29998,7 +30001,7 @@
         <v>916</v>
       </c>
       <c r="B188" s="3" t="s">
-        <v>1142</v>
+        <v>1143</v>
       </c>
       <c r="C188" s="5" t="b">
         <v>1</v>
@@ -30054,7 +30057,7 @@
         <v>927</v>
       </c>
       <c r="B189" s="3" t="s">
-        <v>1142</v>
+        <v>1143</v>
       </c>
       <c r="C189" s="5" t="b">
         <v>1</v>
@@ -30166,7 +30169,7 @@
         <v>940</v>
       </c>
       <c r="B191" s="3" t="s">
-        <v>1142</v>
+        <v>1143</v>
       </c>
       <c r="C191" s="5" t="b">
         <v>1</v>
@@ -30278,7 +30281,7 @@
         <v>959</v>
       </c>
       <c r="B193" s="3" t="s">
-        <v>1142</v>
+        <v>1143</v>
       </c>
       <c r="C193" s="5" t="b">
         <v>1</v>
@@ -30334,7 +30337,7 @@
         <v>967</v>
       </c>
       <c r="B194" s="3" t="s">
-        <v>1142</v>
+        <v>1143</v>
       </c>
       <c r="C194" s="5" t="b">
         <v>1</v>
@@ -30390,7 +30393,7 @@
         <v>969</v>
       </c>
       <c r="B195" s="3" t="s">
-        <v>1142</v>
+        <v>1143</v>
       </c>
       <c r="C195" s="5" t="b">
         <v>1</v>
@@ -30446,7 +30449,7 @@
         <v>976</v>
       </c>
       <c r="B196" s="3" t="s">
-        <v>1142</v>
+        <v>1143</v>
       </c>
       <c r="C196" s="5" t="b">
         <v>1</v>
@@ -30502,7 +30505,7 @@
         <v>978</v>
       </c>
       <c r="B197" s="3" t="s">
-        <v>1142</v>
+        <v>1143</v>
       </c>
       <c r="C197" s="5" t="b">
         <v>1</v>
@@ -30558,7 +30561,7 @@
         <v>988</v>
       </c>
       <c r="B198" s="3" t="s">
-        <v>1142</v>
+        <v>1143</v>
       </c>
       <c r="C198" s="5" t="b">
         <v>1</v>
@@ -30614,7 +30617,7 @@
         <v>996</v>
       </c>
       <c r="B199" s="3" t="s">
-        <v>1142</v>
+        <v>1143</v>
       </c>
       <c r="C199" s="5" t="b">
         <v>1</v>
@@ -30670,7 +30673,7 @@
         <v>999</v>
       </c>
       <c r="B200" s="3" t="s">
-        <v>1142</v>
+        <v>1143</v>
       </c>
       <c r="C200" s="5" t="b">
         <v>1</v>
@@ -30726,7 +30729,7 @@
         <v>1007</v>
       </c>
       <c r="B201" s="3" t="s">
-        <v>1142</v>
+        <v>1143</v>
       </c>
       <c r="C201" s="5" t="b">
         <v>1</v>
@@ -30782,7 +30785,7 @@
         <v>1011</v>
       </c>
       <c r="B202" s="3" t="s">
-        <v>1142</v>
+        <v>1143</v>
       </c>
       <c r="C202" s="5" t="b">
         <v>1</v>
@@ -30838,7 +30841,7 @@
         <v>1021</v>
       </c>
       <c r="B203" s="3" t="s">
-        <v>1142</v>
+        <v>1143</v>
       </c>
       <c r="C203" s="5" t="b">
         <v>1</v>
@@ -30894,7 +30897,7 @@
         <v>1027</v>
       </c>
       <c r="B204" s="3" t="s">
-        <v>1142</v>
+        <v>1143</v>
       </c>
       <c r="C204" s="5" t="b">
         <v>1</v>
@@ -30950,7 +30953,7 @@
         <v>1030</v>
       </c>
       <c r="B205" s="3" t="s">
-        <v>1142</v>
+        <v>1143</v>
       </c>
       <c r="C205" s="5" t="b">
         <v>1</v>
@@ -31006,7 +31009,7 @@
         <v>1033</v>
       </c>
       <c r="B206" s="3" t="s">
-        <v>1142</v>
+        <v>1143</v>
       </c>
       <c r="C206" s="5" t="b">
         <v>1</v>
@@ -31062,7 +31065,7 @@
         <v>1040</v>
       </c>
       <c r="B207" s="3" t="s">
-        <v>1142</v>
+        <v>1143</v>
       </c>
       <c r="C207" s="5" t="b">
         <v>1</v>
@@ -31118,7 +31121,7 @@
         <v>1049</v>
       </c>
       <c r="B208" s="3" t="s">
-        <v>1142</v>
+        <v>1143</v>
       </c>
       <c r="C208" s="5" t="b">
         <v>1</v>
@@ -31174,7 +31177,7 @@
         <v>1051</v>
       </c>
       <c r="B209" s="3" t="s">
-        <v>1142</v>
+        <v>1143</v>
       </c>
       <c r="C209" s="5" t="b">
         <v>1</v>
@@ -31230,7 +31233,7 @@
         <v>1057</v>
       </c>
       <c r="B210" s="3" t="s">
-        <v>1142</v>
+        <v>1143</v>
       </c>
       <c r="C210" s="5" t="b">
         <v>1</v>
@@ -31286,7 +31289,7 @@
         <v>1059</v>
       </c>
       <c r="B211" s="3" t="s">
-        <v>1142</v>
+        <v>1143</v>
       </c>
       <c r="C211" s="5" t="b">
         <v>1</v>
@@ -31342,7 +31345,7 @@
         <v>1070</v>
       </c>
       <c r="B212" s="3" t="s">
-        <v>1142</v>
+        <v>1143</v>
       </c>
       <c r="C212" s="5" t="b">
         <v>1</v>
@@ -31398,7 +31401,7 @@
         <v>1072</v>
       </c>
       <c r="B213" s="3" t="s">
-        <v>1142</v>
+        <v>1143</v>
       </c>
       <c r="C213" s="5" t="b">
         <v>1</v>
@@ -31454,7 +31457,7 @@
         <v>1078</v>
       </c>
       <c r="B214" s="3" t="s">
-        <v>1142</v>
+        <v>1143</v>
       </c>
       <c r="C214" s="5" t="b">
         <v>1</v>
@@ -31510,7 +31513,7 @@
         <v>1080</v>
       </c>
       <c r="B215" s="3" t="s">
-        <v>1142</v>
+        <v>1143</v>
       </c>
       <c r="C215" s="5" t="b">
         <v>1</v>
@@ -31566,7 +31569,7 @@
         <v>1091</v>
       </c>
       <c r="B216" s="3" t="s">
-        <v>1142</v>
+        <v>1143</v>
       </c>
       <c r="C216" s="5" t="b">
         <v>1</v>
@@ -31619,10 +31622,10 @@
     </row>
     <row r="217" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A217" s="3" t="s">
-        <v>1095</v>
+        <v>1096</v>
       </c>
       <c r="B217" s="3" t="s">
-        <v>1142</v>
+        <v>1143</v>
       </c>
       <c r="C217" s="5" t="b">
         <v>1</v>
@@ -31675,10 +31678,10 @@
     </row>
     <row r="218" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A218" s="3" t="s">
-        <v>1100</v>
+        <v>1101</v>
       </c>
       <c r="B218" s="3" t="s">
-        <v>1142</v>
+        <v>1143</v>
       </c>
       <c r="C218" s="5" t="b">
         <v>1</v>
@@ -31731,10 +31734,10 @@
     </row>
     <row r="219" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A219" s="3" t="s">
-        <v>1108</v>
+        <v>1109</v>
       </c>
       <c r="B219" s="3" t="s">
-        <v>1142</v>
+        <v>1143</v>
       </c>
       <c r="C219" s="5" t="b">
         <v>1</v>
@@ -31787,10 +31790,10 @@
     </row>
     <row r="220" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A220" s="3" t="s">
-        <v>1117</v>
+        <v>1118</v>
       </c>
       <c r="B220" s="3" t="s">
-        <v>1142</v>
+        <v>1143</v>
       </c>
       <c r="C220" s="5" t="b">
         <v>1</v>
@@ -31843,10 +31846,10 @@
     </row>
     <row r="221" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A221" s="3" t="s">
-        <v>1120</v>
+        <v>1121</v>
       </c>
       <c r="B221" s="3" t="s">
-        <v>1142</v>
+        <v>1143</v>
       </c>
       <c r="C221" s="5" t="b">
         <v>1</v>
@@ -31899,10 +31902,10 @@
     </row>
     <row r="222" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A222" s="3" t="s">
-        <v>1123</v>
+        <v>1124</v>
       </c>
       <c r="B222" s="3" t="s">
-        <v>1142</v>
+        <v>1143</v>
       </c>
       <c r="C222" s="5" t="b">
         <v>1</v>
@@ -31955,10 +31958,10 @@
     </row>
     <row r="223" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A223" s="3" t="s">
-        <v>1126</v>
+        <v>1127</v>
       </c>
       <c r="B223" s="3" t="s">
-        <v>1142</v>
+        <v>1143</v>
       </c>
       <c r="C223" s="5" t="b">
         <v>1</v>
@@ -32011,10 +32014,10 @@
     </row>
     <row r="224" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A224" s="3" t="s">
-        <v>1133</v>
+        <v>1134</v>
       </c>
       <c r="B224" s="3" t="s">
-        <v>1142</v>
+        <v>1143</v>
       </c>
       <c r="C224" s="5" t="b">
         <v>1</v>
@@ -32067,10 +32070,10 @@
     </row>
     <row r="225" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A225" s="3" t="s">
-        <v>1136</v>
+        <v>1137</v>
       </c>
       <c r="B225" s="3" t="s">
-        <v>1142</v>
+        <v>1143</v>
       </c>
       <c r="C225" s="5" t="b">
         <v>1</v>

</xml_diff>

<commit_message>
generated all the reports on 2024-05-09
</commit_message>
<xml_diff>
--- a/report/merged_configurations.xlsx
+++ b/report/merged_configurations.xlsx
@@ -3206,10 +3206,10 @@
     <t>[{"naam":"Werkgroep Charter Slimme Raadpleegomgeving","waarde":"Werkgroep charter OSLO Slimme Raadpleegomgeving.docx"}]</t>
   </si>
   <si>
-    <t>[{"naam":"Verslag Business Werkgroep - 17 oktober 2023","waarde":"20231017_BusinessWorkshop_Verslag_OSLOSlimmeRaadpleegomgeving.pdf"},{"naam":"Verslag Thematische Werkgroep I - 7 November 2023","waarde":"20231107_ThematicWorkshop1_Verslag_OSLOSlimmeRaadpleegomgeving.pdf"},{"naam":"Verslag Thematische Werkgroep II - 28 November 2023","waarde":"20231128_ThematicWorkshop2_Verslag_OSLOSlimmeRaadpleegomgeving.pdf"},{"naam":"Verslag Thematische Werkgroep III - 9 Januari 2024","waarde":"20240109_ThematicWorkshop1_Verslag_OSLOSlimmeRaadpleegomgeving.pdf"},{"naam":"Verslag Thematische Werkgroep IV - 30 Januari 2024","waarde":"20240130_ThematicWorkshop1_Verslag_OSLOSlimmeRaadpleegomgeving.pdf"}]</t>
-  </si>
-  <si>
-    <t>[{"naam":"Presentatie Business Werkgroep - 17 oktober 2023","waarde":"Business Werkgroep presentatie - slimme raadpleegomgeving.pdf"},{"naam":"Presentatie Thematische Werkgroep I - 7 november 2023","waarde":"20231107 Thematische Werkgroep 1 - Slimme Raadpleegomgeving V.01.pptx"},{"naam":"Presentatie Thematische Werkgroep II - 28 november 2023","waarde":"20231128_ThematicWorkshop2_Powerpoint_OSLOSlimmeRaadpleegomgeving.pptx"},{"naam":"Presentatie Thematische Werkgroep III - 9 Januari 2024","waarde":"20240109_ThematicWorkshop3_Powerpoint_OSLOSlimmeRaadpleegomgeving.pptx"},{"naam":"Presentatie Thematische Werkgroep IV - 30 Januari 2024","waarde":"20240130_ThematicWorkshop4_Powerpoint_OSLOSlimmeRaadpleegomgeving.pptx"}]</t>
+    <t>[{"naam":"Verslag Business Werkgroep - 17 oktober 2023","waarde":"20231017_BusinessWorkshop_Verslag_OSLOSlimmeRaadpleegomgeving.pdf"},{"naam":"Verslag Thematische Werkgroep I - 7 November 2023","waarde":"20231107_ThematicWorkshop1_Verslag_OSLOSlimmeRaadpleegomgeving.pdf"},{"naam":"Verslag Thematische Werkgroep II - 28 November 2023","waarde":"20231128_ThematicWorkshop2_Verslag_OSLOSlimmeRaadpleegomgeving.pdf"},{"naam":"Verslag Thematische Werkgroep III - 9 Januari 2024","waarde":"20240109_ThematicWorkshop3_Verslag_OSLOSlimmeRaadpleegomgeving.pdf"},{"naam":"Verslag Thematische Werkgroep IV - 30 Januari 2024","waarde":"20240130_ThematicWorkshop4_Verslag_OSLOSlimmeRaadpleegomgeving.pdf"}]</t>
+  </si>
+  <si>
+    <t>[{"naam":"Presentatie Business Werkgroep - 17 oktober 2023","waarde":"20231017_BusinessWorkshop_Powerpoint_OSLOSlimmeRaadpleegomgeving.pptx"},{"naam":"Presentatie Thematische Werkgroep I - 7 november 2023","waarde":"20231107_ThematicWorkshop1_Powerpoint_OSLOSlimmeRaadpleegomgeving.pptx"},{"naam":"Presentatie Thematische Werkgroep II - 28 november 2023","waarde":"20231128_ThematicWorkshop2_Powerpoint_OSLOSlimmeRaadpleegomgeving.pptx"},{"naam":"Presentatie Thematische Werkgroep III - 9 Januari 2024","waarde":"20240109_ThematicWorkshop3_Powerpoint_OSLOSlimmeRaadpleegomgeving.pptx"},{"naam":"Presentatie Thematische Werkgroep IV - 30 Januari 2024","waarde":"20240130_ThematicWorkshop4_Powerpoint_OSLOSlimmeRaadpleegomgeving.pptx"}]</t>
   </si>
   <si>
     <t>Semantische standaard voor de digitale transformatie van de Vlaamse lokale besturen</t>
@@ -3239,7 +3239,7 @@
     <t>[{"naam":"OSLO Lokale Economie Charter","waarde":"Charter_OSLO_Lokale_Economie.docx"}]</t>
   </si>
   <si>
-    <t>[{"naam":"Verslag business werkgroep - 19-09-2023","waarde":"Verslag Business Werkgroep - Lokale Economie - 19092023.pdf"},{"naam":"Verslag thematische werkgroep 1 - 17-10-2023","waarde":"Verslag Thematische Werkgroep 1 - Lokale Economie - 17102023.pdf"},{"naam":"Verslag thematische werkgroep 2 - 16-11-2023","waarde":"Verslag Thematische Werkgroep 2 - Lokale Economie - 16112023.pdf"},{"naam":"Verslag thematische werkgroep 3 - 19-12-2023","waarde":"Verslag Thematische Werkgroep 3 - Lokale Economie - 1912023.pdf"},{"naam":"Verslag thematische werkgroep 4 - 23-01-2024","waarde":"Verslag Thematische Werkgroep 4 - Lokale Economie - 23012024.pdf"}]</t>
+    <t>[{"naam":"Verslag business werkgroep - 19-09-2023","waarde":"Verslag Business Werkgroep - Lokale Economie - 19092023.pdf"},{"naam":"Verslag thematische werkgroep 1 - 17-10-2023","waarde":"Verslag Thematische Werkgroep 1 - Lokale Economie - 17102023.pdf"},{"naam":"Verslag thematische werkgroep 2 - 16-11-2023","waarde":"Verslag Thematische Werkgroep 2 - Lokale Economie - 16112023.pdf"},{"naam":"Verslag thematische werkgroep 3 - 19-12-2023","waarde":"Verslag Thematische Werkgroep 3 - Lokale Economie - 19122023.pdf"},{"naam":"Verslag thematische werkgroep 4 - 23-01-2024","waarde":"Verslag Thematische Werkgroep 4 - Lokale Economie - 23012024.pdf"}]</t>
   </si>
   <si>
     <t>[{"naam":"Presentatie business werkgroep - 19-09-2023","waarde":"Presentatie Business Werkgroep - Lokale Economie - 19092023.pdf"},{"naam":"Presentatie thematische werkgroep 1 - 17-10-2023","waarde":"Presentatie Thematische Werkgroep 1 - Lokale Economie - 17102023.pdf"},{"naam":"Presentatie thematische werkgroep 2 - 16-11-2023","waarde":"Presentatie Thematische Werkgroep 2 - Lokale Economie - 16112023.pdf"},{"naam":"Presentatie thematische werkgroep 3 - 19-12-2023","waarde":"Presentatie Thematische Werkgroep 3 - Lokale Economie - 19122023.pdf"},{"naam":"Presentatie thematische werkgroep 4 - 23-01-2024","waarde":"Presentatie Thematische Werkgroep 4 - Lokale Economie - 23012024.pdf"}]</t>

</xml_diff>

<commit_message>
generated all the reports on 2024-05-31
</commit_message>
<xml_diff>
--- a/report/merged_configurations.xlsx
+++ b/report/merged_configurations.xlsx
@@ -14717,7 +14717,7 @@
         <v>22</v>
       </c>
       <c r="D189" s="3" t="s">
-        <v>39</v>
+        <v>23</v>
       </c>
       <c r="E189" s="3" t="s">
         <v>868</v>
@@ -14758,7 +14758,9 @@
       <c r="Q189" s="3" t="s">
         <v>876</v>
       </c>
-      <c r="R189" s="3"/>
+      <c r="R189" s="4">
+        <v>45239</v>
+      </c>
       <c r="S189" s="3"/>
       <c r="T189" s="3" t="s">
         <v>34</v>
@@ -14775,7 +14777,7 @@
         <v>22</v>
       </c>
       <c r="D190" s="3" t="s">
-        <v>39</v>
+        <v>23</v>
       </c>
       <c r="E190" s="3" t="s">
         <v>878</v>
@@ -14816,7 +14818,9 @@
       <c r="Q190" s="3" t="s">
         <v>876</v>
       </c>
-      <c r="R190" s="3"/>
+      <c r="R190" s="4">
+        <v>45239</v>
+      </c>
       <c r="S190" s="3"/>
       <c r="T190" s="3" t="s">
         <v>34</v>

</xml_diff>

<commit_message>
generated all the reports on 2024-06-13
</commit_message>
<xml_diff>
--- a/report/merged_configurations.xlsx
+++ b/report/merged_configurations.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4337" uniqueCount="1136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4335" uniqueCount="1139">
   <si>
     <t>title</t>
   </si>
@@ -3281,16 +3281,25 @@
     <t>leerinschrijfcredential-description.md</t>
   </si>
   <si>
-    <t>[{"name":"Applicatieprofiel Leerinschrijfcredential","resourceReference":"https://data.vlaanderen.be/doc/applicatieprofiel/leerinschrijfcredential"}]</t>
-  </si>
-  <si>
-    <t>[{"name":"Verslag Business Werkgroep - 26/02/2024","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-Leercredential/standaardenregister/reports/260224 SA Verslag Business werkgroep.pdf"},{"name":"Verslag Thematische Werkgroep 1 - 18/03/2024","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-Leercredential/standaardenregister/reports/180324 SA Verslag Eerste thematische werkgroep.pdf"}]</t>
-  </si>
-  <si>
-    <t>https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-Leercredential/standaardenregister/charter/</t>
-  </si>
-  <si>
-    <t>[{"name":"Presentatie Business Werkgroep - 26/02/2024","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-Leercredential/standaardenregister/presentations/260224 SA Business werkgroep.pdf"},{"name":"Presentatie Thematische Werkgroep 1 - 18/03/2024","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-Leercredential/standaardenregister/presentations/180324 SA Thematische werkgroep 1.pdf"}]</t>
+    <t>[{"name":"Athumi","resourceReference":"https://data.vlaanderen.be/id/organisatie/OVO052661"}]</t>
+  </si>
+  <si>
+    <t>[{"name":"Vocabularium Leerinschrijfcredential","resourceReference":"https://data.vlaanderen.be/doc/vocabularium/leerinschrijfcredential/"},{"name":"Applicatieprofiel Leerinschrijfcredential","resourceReference":"https://data.vlaanderen.be/doc/applicatieprofiel/leerinschrijfcredential/"}]</t>
+  </si>
+  <si>
+    <t>[{"name":"Verslag Business Werkgroep - 26/02/2024","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-Leerinschrijfcredential/standaardenregister/reports/260224 SA Verslag Business werkgroep.pdf"},{"name":"Verslag Thematische Werkgroep 1 - 18/03/2024","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-Leerinschrijfcredential/standaardenregister/reports/180324 SA Verslag Eerste thematische werkgroep.pdf"},{"name":"Verslag Thematische Werkgroep 2 - 16/04/2024","resourceReference":"160424 SA Verslag thematische werkgroep 2.docx"}]</t>
+  </si>
+  <si>
+    <t>Werkgroep Charter Document</t>
+  </si>
+  <si>
+    <t>Charter_OSLO_Athumi.docx</t>
+  </si>
+  <si>
+    <t>[{"name":"Presentatie Business Werkgroep - 26/02/2024","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-Leerinschrijfcredential/standaardenregister/presentations/260224 SA Business werkgroep.pdf"},{"name":"Presentatie Thematische Werkgroep 1 - 18/03/2024","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-Leerinschrijfcredential/standaardenregister/presentations/180324 SA Thematische werkgroep 1.pdf"},{"name":"Presentatie Thematische Werkgroep 2 - 16/04/2024","resourceReference":"Thematische werkgroep 2 presentatie Studentenattesten.pptx"}]</t>
+  </si>
+  <si>
+    <t>OSLOthema-Leerinschrijfcredential</t>
   </si>
   <si>
     <t>Applicatieprofiel OSLO Datakwaliteit</t>
@@ -16844,46 +16853,46 @@
         <v>22</v>
       </c>
       <c r="D226" s="3" t="s">
-        <v>39</v>
+        <v>23</v>
       </c>
       <c r="E226" s="3" t="s">
         <v>1088</v>
       </c>
       <c r="F226" s="3" t="s">
-        <v>41</v>
+        <v>1089</v>
       </c>
       <c r="G226" s="4">
         <v>45390</v>
       </c>
       <c r="H226" s="3" t="s">
-        <v>1089</v>
+        <v>1090</v>
       </c>
       <c r="I226" s="3" t="s">
         <v>27</v>
       </c>
       <c r="J226" s="3" t="s">
-        <v>1090</v>
+        <v>1091</v>
       </c>
       <c r="K226" s="3" t="s">
-        <v>34</v>
+        <v>1092</v>
       </c>
       <c r="L226" s="3" t="s">
-        <v>1091</v>
+        <v>1093</v>
       </c>
       <c r="M226" s="3" t="s">
-        <v>1092</v>
-      </c>
-      <c r="N226" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="O226" s="3" t="s">
-        <v>32</v>
+        <v>1094</v>
+      </c>
+      <c r="N226" s="4">
+        <v>45372</v>
+      </c>
+      <c r="O226" s="4">
+        <v>45428</v>
       </c>
       <c r="P226" s="3" t="s">
         <v>32</v>
       </c>
       <c r="Q226" s="3" t="s">
-        <v>972</v>
+        <v>1095</v>
       </c>
       <c r="R226" s="3"/>
       <c r="S226" s="3"/>
@@ -16893,7 +16902,7 @@
     </row>
     <row r="227" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A227" s="3" t="s">
-        <v>1093</v>
+        <v>1096</v>
       </c>
       <c r="B227" s="3" t="s">
         <v>21</v>
@@ -16905,7 +16914,7 @@
         <v>23</v>
       </c>
       <c r="E227" s="3" t="s">
-        <v>1094</v>
+        <v>1097</v>
       </c>
       <c r="F227" s="3" t="s">
         <v>1075</v>
@@ -16914,7 +16923,7 @@
         <v>45078</v>
       </c>
       <c r="H227" s="3" t="s">
-        <v>1095</v>
+        <v>1098</v>
       </c>
       <c r="I227" s="3" t="s">
         <v>1077</v>
@@ -16951,7 +16960,7 @@
     </row>
     <row r="228" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A228" s="3" t="s">
-        <v>1096</v>
+        <v>1099</v>
       </c>
       <c r="B228" s="3" t="s">
         <v>21</v>
@@ -16963,7 +16972,7 @@
         <v>23</v>
       </c>
       <c r="E228" s="3" t="s">
-        <v>1097</v>
+        <v>1100</v>
       </c>
       <c r="F228" s="3" t="s">
         <v>1075</v>
@@ -16972,13 +16981,13 @@
         <v>45078</v>
       </c>
       <c r="H228" s="3" t="s">
-        <v>1098</v>
+        <v>1101</v>
       </c>
       <c r="I228" s="3" t="s">
-        <v>1099</v>
+        <v>1102</v>
       </c>
       <c r="J228" s="3" t="s">
-        <v>1100</v>
+        <v>1103</v>
       </c>
       <c r="K228" s="3" t="s">
         <v>34</v>
@@ -16987,7 +16996,7 @@
         <v>1078</v>
       </c>
       <c r="M228" s="3" t="s">
-        <v>1101</v>
+        <v>1104</v>
       </c>
       <c r="N228" s="3" t="s">
         <v>1079</v>
@@ -17009,7 +17018,7 @@
     </row>
     <row r="229" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A229" s="3" t="s">
-        <v>1102</v>
+        <v>1105</v>
       </c>
       <c r="B229" s="3" t="s">
         <v>36</v>
@@ -17021,7 +17030,7 @@
         <v>23</v>
       </c>
       <c r="E229" s="3" t="s">
-        <v>1103</v>
+        <v>1106</v>
       </c>
       <c r="F229" s="3" t="s">
         <v>1075</v>
@@ -17030,13 +17039,13 @@
         <v>45078</v>
       </c>
       <c r="H229" s="3" t="s">
-        <v>1104</v>
+        <v>1107</v>
       </c>
       <c r="I229" s="3" t="s">
-        <v>1099</v>
+        <v>1102</v>
       </c>
       <c r="J229" s="3" t="s">
-        <v>1100</v>
+        <v>1103</v>
       </c>
       <c r="K229" s="3" t="s">
         <v>34</v>
@@ -17045,7 +17054,7 @@
         <v>1078</v>
       </c>
       <c r="M229" s="3" t="s">
-        <v>1101</v>
+        <v>1104</v>
       </c>
       <c r="N229" s="3" t="s">
         <v>1079</v>
@@ -17067,7 +17076,7 @@
     </row>
     <row r="230" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A230" s="3" t="s">
-        <v>1105</v>
+        <v>1108</v>
       </c>
       <c r="B230" s="3" t="s">
         <v>21</v>
@@ -17079,7 +17088,7 @@
         <v>39</v>
       </c>
       <c r="E230" s="3" t="s">
-        <v>1106</v>
+        <v>1109</v>
       </c>
       <c r="F230" s="3" t="s">
         <v>41</v>
@@ -17088,22 +17097,22 @@
         <v>45412</v>
       </c>
       <c r="H230" s="3" t="s">
-        <v>1107</v>
+        <v>1110</v>
       </c>
       <c r="I230" s="3" t="s">
-        <v>1108</v>
+        <v>1111</v>
       </c>
       <c r="J230" s="3" t="s">
-        <v>1109</v>
+        <v>1112</v>
       </c>
       <c r="K230" s="3" t="s">
-        <v>1110</v>
+        <v>1113</v>
       </c>
       <c r="L230" s="3" t="s">
-        <v>1111</v>
+        <v>1114</v>
       </c>
       <c r="M230" s="3" t="s">
-        <v>1112</v>
+        <v>1115</v>
       </c>
       <c r="N230" s="3" t="s">
         <v>48</v>
@@ -17115,7 +17124,7 @@
         <v>32</v>
       </c>
       <c r="Q230" s="3" t="s">
-        <v>1113</v>
+        <v>1116</v>
       </c>
       <c r="R230" s="3"/>
       <c r="S230" s="3"/>
@@ -17125,7 +17134,7 @@
     </row>
     <row r="231" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A231" s="3" t="s">
-        <v>1114</v>
+        <v>1117</v>
       </c>
       <c r="B231" s="3" t="s">
         <v>36</v>
@@ -17137,7 +17146,7 @@
         <v>39</v>
       </c>
       <c r="E231" s="3" t="s">
-        <v>1115</v>
+        <v>1118</v>
       </c>
       <c r="F231" s="3" t="s">
         <v>41</v>
@@ -17146,22 +17155,22 @@
         <v>45412</v>
       </c>
       <c r="H231" s="3" t="s">
-        <v>1108</v>
+        <v>1111</v>
       </c>
       <c r="I231" s="3" t="s">
-        <v>1107</v>
+        <v>1110</v>
       </c>
       <c r="J231" s="3" t="s">
-        <v>1109</v>
+        <v>1112</v>
       </c>
       <c r="K231" s="3" t="s">
-        <v>1110</v>
+        <v>1113</v>
       </c>
       <c r="L231" s="3" t="s">
-        <v>1111</v>
+        <v>1114</v>
       </c>
       <c r="M231" s="3" t="s">
-        <v>1112</v>
+        <v>1115</v>
       </c>
       <c r="N231" s="3" t="s">
         <v>48</v>
@@ -17173,7 +17182,7 @@
         <v>32</v>
       </c>
       <c r="Q231" s="3" t="s">
-        <v>1113</v>
+        <v>1116</v>
       </c>
       <c r="R231" s="3"/>
       <c r="S231" s="3"/>
@@ -17197,66 +17206,66 @@
   <sheetData>
     <row r="1" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>1116</v>
+        <v>1119</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>1117</v>
+        <v>1120</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>1118</v>
+        <v>1121</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>1119</v>
+        <v>1122</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>1120</v>
+        <v>1123</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>1121</v>
+        <v>1124</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>1122</v>
+        <v>1125</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>1123</v>
+        <v>1126</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>1124</v>
+        <v>1127</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>1125</v>
+        <v>1128</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>1126</v>
+        <v>1129</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>1127</v>
+        <v>1130</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>1128</v>
+        <v>1131</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>1129</v>
+        <v>1132</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>1130</v>
+        <v>1133</v>
       </c>
       <c r="P1" s="2" t="s">
-        <v>1131</v>
+        <v>1134</v>
       </c>
       <c r="Q1" s="2" t="s">
-        <v>1132</v>
+        <v>1135</v>
       </c>
       <c r="R1" s="2" t="s">
-        <v>1133</v>
+        <v>1136</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C2" s="5" t="b">
         <v>0</v>
@@ -17309,10 +17318,10 @@
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C3" s="5" t="b">
         <v>0</v>
@@ -17365,10 +17374,10 @@
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C4" s="5" t="b">
         <v>0</v>
@@ -17421,10 +17430,10 @@
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C5" s="5" t="b">
         <v>0</v>
@@ -17477,10 +17486,10 @@
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C6" s="5" t="b">
         <v>0</v>
@@ -17533,10 +17542,10 @@
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C7" s="5" t="b">
         <v>0</v>
@@ -17589,10 +17598,10 @@
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C8" s="5" t="b">
         <v>0</v>
@@ -17645,10 +17654,10 @@
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C9" s="5" t="b">
         <v>0</v>
@@ -17701,10 +17710,10 @@
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C10" s="5" t="b">
         <v>0</v>
@@ -17757,10 +17766,10 @@
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C11" s="5" t="b">
         <v>0</v>
@@ -17813,10 +17822,10 @@
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C12" s="5" t="b">
         <v>0</v>
@@ -17869,10 +17878,10 @@
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C13" s="5" t="b">
         <v>0</v>
@@ -17925,10 +17934,10 @@
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C14" s="5" t="b">
         <v>0</v>
@@ -17981,10 +17990,10 @@
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C15" s="5" t="b">
         <v>0</v>
@@ -18037,10 +18046,10 @@
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C16" s="5" t="b">
         <v>0</v>
@@ -18093,10 +18102,10 @@
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C17" s="5" t="b">
         <v>0</v>
@@ -18149,10 +18158,10 @@
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C18" s="5" t="b">
         <v>0</v>
@@ -18205,10 +18214,10 @@
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C19" s="5" t="b">
         <v>0</v>
@@ -18261,10 +18270,10 @@
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C20" s="5" t="b">
         <v>0</v>
@@ -18317,10 +18326,10 @@
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C21" s="5" t="b">
         <v>0</v>
@@ -18373,10 +18382,10 @@
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C22" s="5" t="b">
         <v>0</v>
@@ -18429,10 +18438,10 @@
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C23" s="5" t="b">
         <v>0</v>
@@ -18485,10 +18494,10 @@
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C24" s="5" t="b">
         <v>0</v>
@@ -18541,10 +18550,10 @@
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C25" s="5" t="b">
         <v>0</v>
@@ -18597,10 +18606,10 @@
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C26" s="5" t="b">
         <v>0</v>
@@ -18653,10 +18662,10 @@
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C27" s="5" t="b">
         <v>0</v>
@@ -18709,10 +18718,10 @@
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C28" s="5" t="b">
         <v>0</v>
@@ -18765,10 +18774,10 @@
     </row>
     <row r="29" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C29" s="5" t="b">
         <v>0</v>
@@ -18821,10 +18830,10 @@
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C30" s="5" t="b">
         <v>0</v>
@@ -18877,10 +18886,10 @@
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C31" s="5" t="b">
         <v>0</v>
@@ -18933,10 +18942,10 @@
     </row>
     <row r="32" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C32" s="5" t="b">
         <v>0</v>
@@ -18989,10 +18998,10 @@
     </row>
     <row r="33" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C33" s="5" t="b">
         <v>0</v>
@@ -19045,10 +19054,10 @@
     </row>
     <row r="34" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C34" s="5" t="b">
         <v>0</v>
@@ -19101,10 +19110,10 @@
     </row>
     <row r="35" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C35" s="5" t="b">
         <v>0</v>
@@ -19157,10 +19166,10 @@
     </row>
     <row r="36" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C36" s="5" t="b">
         <v>0</v>
@@ -19213,10 +19222,10 @@
     </row>
     <row r="37" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C37" s="5" t="b">
         <v>0</v>
@@ -19269,10 +19278,10 @@
     </row>
     <row r="38" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C38" s="5" t="b">
         <v>0</v>
@@ -19325,10 +19334,10 @@
     </row>
     <row r="39" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C39" s="5" t="b">
         <v>0</v>
@@ -19381,10 +19390,10 @@
     </row>
     <row r="40" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C40" s="5" t="b">
         <v>0</v>
@@ -19437,10 +19446,10 @@
     </row>
     <row r="41" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C41" s="5" t="b">
         <v>0</v>
@@ -19493,10 +19502,10 @@
     </row>
     <row r="42" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C42" s="5" t="b">
         <v>0</v>
@@ -19549,10 +19558,10 @@
     </row>
     <row r="43" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C43" s="5" t="b">
         <v>0</v>
@@ -19605,10 +19614,10 @@
     </row>
     <row r="44" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C44" s="5" t="b">
         <v>0</v>
@@ -19661,10 +19670,10 @@
     </row>
     <row r="45" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C45" s="5" t="b">
         <v>0</v>
@@ -19717,10 +19726,10 @@
     </row>
     <row r="46" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C46" s="5" t="b">
         <v>0</v>
@@ -19773,10 +19782,10 @@
     </row>
     <row r="47" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C47" s="5" t="b">
         <v>0</v>
@@ -19829,10 +19838,10 @@
     </row>
     <row r="48" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C48" s="5" t="b">
         <v>0</v>
@@ -19885,10 +19894,10 @@
     </row>
     <row r="49" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C49" s="5" t="b">
         <v>0</v>
@@ -19941,10 +19950,10 @@
     </row>
     <row r="50" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C50" s="5" t="b">
         <v>0</v>
@@ -19997,10 +20006,10 @@
     </row>
     <row r="51" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C51" s="5" t="b">
         <v>0</v>
@@ -20053,10 +20062,10 @@
     </row>
     <row r="52" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C52" s="5" t="b">
         <v>0</v>
@@ -20109,10 +20118,10 @@
     </row>
     <row r="53" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C53" s="5" t="b">
         <v>0</v>
@@ -20165,10 +20174,10 @@
     </row>
     <row r="54" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C54" s="5" t="b">
         <v>0</v>
@@ -20221,10 +20230,10 @@
     </row>
     <row r="55" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C55" s="5" t="b">
         <v>0</v>
@@ -20277,10 +20286,10 @@
     </row>
     <row r="56" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C56" s="5" t="b">
         <v>0</v>
@@ -20333,10 +20342,10 @@
     </row>
     <row r="57" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C57" s="5" t="b">
         <v>0</v>
@@ -20389,10 +20398,10 @@
     </row>
     <row r="58" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C58" s="5" t="b">
         <v>0</v>
@@ -20445,10 +20454,10 @@
     </row>
     <row r="59" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C59" s="5" t="b">
         <v>0</v>
@@ -20501,10 +20510,10 @@
     </row>
     <row r="60" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C60" s="5" t="b">
         <v>0</v>
@@ -20557,10 +20566,10 @@
     </row>
     <row r="61" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C61" s="5" t="b">
         <v>0</v>
@@ -20613,10 +20622,10 @@
     </row>
     <row r="62" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C62" s="5" t="b">
         <v>0</v>
@@ -20669,10 +20678,10 @@
     </row>
     <row r="63" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C63" s="5" t="b">
         <v>0</v>
@@ -20725,10 +20734,10 @@
     </row>
     <row r="64" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C64" s="5" t="b">
         <v>0</v>
@@ -20781,10 +20790,10 @@
     </row>
     <row r="65" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A65" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C65" s="5" t="b">
         <v>0</v>
@@ -20837,10 +20846,10 @@
     </row>
     <row r="66" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A66" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C66" s="5" t="b">
         <v>0</v>
@@ -20893,10 +20902,10 @@
     </row>
     <row r="67" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A67" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C67" s="5" t="b">
         <v>0</v>
@@ -20949,10 +20958,10 @@
     </row>
     <row r="68" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A68" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C68" s="5" t="b">
         <v>0</v>
@@ -21005,10 +21014,10 @@
     </row>
     <row r="69" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A69" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C69" s="5" t="b">
         <v>0</v>
@@ -21061,10 +21070,10 @@
     </row>
     <row r="70" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A70" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C70" s="5" t="b">
         <v>0</v>
@@ -21117,10 +21126,10 @@
     </row>
     <row r="71" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A71" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C71" s="5" t="b">
         <v>0</v>
@@ -21173,10 +21182,10 @@
     </row>
     <row r="72" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A72" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C72" s="5" t="b">
         <v>0</v>
@@ -21229,10 +21238,10 @@
     </row>
     <row r="73" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A73" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C73" s="5" t="b">
         <v>0</v>
@@ -21285,10 +21294,10 @@
     </row>
     <row r="74" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A74" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C74" s="5" t="b">
         <v>0</v>
@@ -21341,10 +21350,10 @@
     </row>
     <row r="75" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A75" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C75" s="5" t="b">
         <v>0</v>
@@ -21397,10 +21406,10 @@
     </row>
     <row r="76" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A76" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C76" s="5" t="b">
         <v>0</v>
@@ -21453,10 +21462,10 @@
     </row>
     <row r="77" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A77" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C77" s="5" t="b">
         <v>0</v>
@@ -21509,10 +21518,10 @@
     </row>
     <row r="78" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A78" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C78" s="5" t="b">
         <v>0</v>
@@ -21565,10 +21574,10 @@
     </row>
     <row r="79" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A79" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C79" s="5" t="b">
         <v>0</v>
@@ -21621,10 +21630,10 @@
     </row>
     <row r="80" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A80" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C80" s="5" t="b">
         <v>0</v>
@@ -21677,10 +21686,10 @@
     </row>
     <row r="81" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A81" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B81" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C81" s="5" t="b">
         <v>0</v>
@@ -21733,10 +21742,10 @@
     </row>
     <row r="82" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A82" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B82" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C82" s="5" t="b">
         <v>0</v>
@@ -21789,10 +21798,10 @@
     </row>
     <row r="83" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A83" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C83" s="5" t="b">
         <v>0</v>
@@ -21845,10 +21854,10 @@
     </row>
     <row r="84" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A84" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B84" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C84" s="5" t="b">
         <v>0</v>
@@ -21901,10 +21910,10 @@
     </row>
     <row r="85" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A85" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C85" s="5" t="b">
         <v>0</v>
@@ -21957,10 +21966,10 @@
     </row>
     <row r="86" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A86" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B86" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C86" s="5" t="b">
         <v>0</v>
@@ -22013,10 +22022,10 @@
     </row>
     <row r="87" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A87" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B87" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C87" s="5" t="b">
         <v>0</v>
@@ -22069,10 +22078,10 @@
     </row>
     <row r="88" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A88" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B88" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C88" s="5" t="b">
         <v>0</v>
@@ -22125,10 +22134,10 @@
     </row>
     <row r="89" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A89" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C89" s="5" t="b">
         <v>0</v>
@@ -22181,10 +22190,10 @@
     </row>
     <row r="90" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A90" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B90" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C90" s="5" t="b">
         <v>0</v>
@@ -22237,10 +22246,10 @@
     </row>
     <row r="91" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A91" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B91" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C91" s="5" t="b">
         <v>0</v>
@@ -22293,10 +22302,10 @@
     </row>
     <row r="92" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A92" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B92" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C92" s="5" t="b">
         <v>0</v>
@@ -22349,10 +22358,10 @@
     </row>
     <row r="93" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A93" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B93" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C93" s="5" t="b">
         <v>0</v>
@@ -22405,10 +22414,10 @@
     </row>
     <row r="94" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A94" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B94" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C94" s="5" t="b">
         <v>0</v>
@@ -22461,10 +22470,10 @@
     </row>
     <row r="95" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A95" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B95" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C95" s="5" t="b">
         <v>0</v>
@@ -22517,10 +22526,10 @@
     </row>
     <row r="96" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A96" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B96" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C96" s="5" t="b">
         <v>0</v>
@@ -22573,10 +22582,10 @@
     </row>
     <row r="97" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A97" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B97" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C97" s="5" t="b">
         <v>0</v>
@@ -22629,10 +22638,10 @@
     </row>
     <row r="98" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A98" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B98" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C98" s="5" t="b">
         <v>0</v>
@@ -22685,10 +22694,10 @@
     </row>
     <row r="99" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A99" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B99" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C99" s="5" t="b">
         <v>0</v>
@@ -22741,10 +22750,10 @@
     </row>
     <row r="100" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A100" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B100" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C100" s="5" t="b">
         <v>0</v>
@@ -22797,10 +22806,10 @@
     </row>
     <row r="101" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A101" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B101" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C101" s="5" t="b">
         <v>0</v>
@@ -22853,10 +22862,10 @@
     </row>
     <row r="102" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A102" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B102" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C102" s="5" t="b">
         <v>0</v>
@@ -22909,10 +22918,10 @@
     </row>
     <row r="103" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A103" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B103" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C103" s="5" t="b">
         <v>0</v>
@@ -22965,10 +22974,10 @@
     </row>
     <row r="104" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A104" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B104" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C104" s="5" t="b">
         <v>0</v>
@@ -23021,10 +23030,10 @@
     </row>
     <row r="105" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A105" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B105" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C105" s="5" t="b">
         <v>0</v>
@@ -23077,10 +23086,10 @@
     </row>
     <row r="106" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A106" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B106" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C106" s="5" t="b">
         <v>0</v>
@@ -23133,10 +23142,10 @@
     </row>
     <row r="107" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A107" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B107" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C107" s="5" t="b">
         <v>0</v>
@@ -23189,10 +23198,10 @@
     </row>
     <row r="108" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A108" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B108" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C108" s="5" t="b">
         <v>0</v>
@@ -23245,10 +23254,10 @@
     </row>
     <row r="109" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A109" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B109" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C109" s="5" t="b">
         <v>0</v>
@@ -23301,10 +23310,10 @@
     </row>
     <row r="110" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A110" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B110" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C110" s="5" t="b">
         <v>0</v>
@@ -23357,10 +23366,10 @@
     </row>
     <row r="111" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A111" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B111" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C111" s="5" t="b">
         <v>0</v>
@@ -23413,10 +23422,10 @@
     </row>
     <row r="112" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A112" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B112" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C112" s="5" t="b">
         <v>0</v>
@@ -23469,10 +23478,10 @@
     </row>
     <row r="113" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A113" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B113" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C113" s="5" t="b">
         <v>0</v>
@@ -23525,10 +23534,10 @@
     </row>
     <row r="114" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A114" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B114" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C114" s="5" t="b">
         <v>0</v>
@@ -23581,10 +23590,10 @@
     </row>
     <row r="115" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A115" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B115" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C115" s="5" t="b">
         <v>0</v>
@@ -23637,10 +23646,10 @@
     </row>
     <row r="116" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A116" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B116" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C116" s="5" t="b">
         <v>0</v>
@@ -23693,10 +23702,10 @@
     </row>
     <row r="117" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A117" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B117" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C117" s="5" t="b">
         <v>0</v>
@@ -23749,10 +23758,10 @@
     </row>
     <row r="118" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A118" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B118" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C118" s="5" t="b">
         <v>0</v>
@@ -23805,10 +23814,10 @@
     </row>
     <row r="119" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A119" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B119" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C119" s="5" t="b">
         <v>0</v>
@@ -23861,10 +23870,10 @@
     </row>
     <row r="120" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A120" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B120" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C120" s="5" t="b">
         <v>0</v>
@@ -23917,10 +23926,10 @@
     </row>
     <row r="121" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A121" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B121" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C121" s="5" t="b">
         <v>0</v>
@@ -23973,10 +23982,10 @@
     </row>
     <row r="122" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A122" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B122" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C122" s="5" t="b">
         <v>0</v>
@@ -24029,10 +24038,10 @@
     </row>
     <row r="123" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A123" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B123" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C123" s="5" t="b">
         <v>0</v>
@@ -24085,10 +24094,10 @@
     </row>
     <row r="124" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A124" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B124" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C124" s="5" t="b">
         <v>0</v>
@@ -24141,10 +24150,10 @@
     </row>
     <row r="125" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A125" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B125" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C125" s="5" t="b">
         <v>0</v>
@@ -24197,10 +24206,10 @@
     </row>
     <row r="126" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A126" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B126" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C126" s="5" t="b">
         <v>0</v>
@@ -24253,10 +24262,10 @@
     </row>
     <row r="127" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A127" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B127" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C127" s="5" t="b">
         <v>0</v>
@@ -24309,10 +24318,10 @@
     </row>
     <row r="128" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A128" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B128" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C128" s="5" t="b">
         <v>0</v>
@@ -24365,10 +24374,10 @@
     </row>
     <row r="129" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A129" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B129" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C129" s="5" t="b">
         <v>0</v>
@@ -24421,10 +24430,10 @@
     </row>
     <row r="130" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A130" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B130" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C130" s="5" t="b">
         <v>0</v>
@@ -24477,10 +24486,10 @@
     </row>
     <row r="131" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A131" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B131" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C131" s="5" t="b">
         <v>0</v>
@@ -24533,10 +24542,10 @@
     </row>
     <row r="132" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A132" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B132" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C132" s="5" t="b">
         <v>0</v>
@@ -24589,10 +24598,10 @@
     </row>
     <row r="133" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A133" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B133" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C133" s="5" t="b">
         <v>0</v>
@@ -24645,10 +24654,10 @@
     </row>
     <row r="134" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A134" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B134" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C134" s="5" t="b">
         <v>0</v>
@@ -24701,10 +24710,10 @@
     </row>
     <row r="135" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A135" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B135" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C135" s="5" t="b">
         <v>0</v>
@@ -24757,10 +24766,10 @@
     </row>
     <row r="136" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A136" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B136" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C136" s="5" t="b">
         <v>0</v>
@@ -24813,10 +24822,10 @@
     </row>
     <row r="137" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A137" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B137" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C137" s="5" t="b">
         <v>0</v>
@@ -24869,10 +24878,10 @@
     </row>
     <row r="138" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A138" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B138" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C138" s="5" t="b">
         <v>0</v>
@@ -24925,10 +24934,10 @@
     </row>
     <row r="139" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A139" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B139" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C139" s="5" t="b">
         <v>0</v>
@@ -24981,10 +24990,10 @@
     </row>
     <row r="140" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A140" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B140" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C140" s="5" t="b">
         <v>0</v>
@@ -25037,10 +25046,10 @@
     </row>
     <row r="141" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A141" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B141" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C141" s="5" t="b">
         <v>0</v>
@@ -25093,10 +25102,10 @@
     </row>
     <row r="142" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A142" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B142" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C142" s="5" t="b">
         <v>0</v>
@@ -25149,10 +25158,10 @@
     </row>
     <row r="143" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A143" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B143" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C143" s="5" t="b">
         <v>0</v>
@@ -25205,10 +25214,10 @@
     </row>
     <row r="144" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A144" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B144" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C144" s="5" t="b">
         <v>0</v>
@@ -25261,10 +25270,10 @@
     </row>
     <row r="145" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A145" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B145" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C145" s="5" t="b">
         <v>0</v>
@@ -25317,10 +25326,10 @@
     </row>
     <row r="146" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A146" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B146" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C146" s="5" t="b">
         <v>0</v>
@@ -25373,10 +25382,10 @@
     </row>
     <row r="147" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A147" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B147" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C147" s="5" t="b">
         <v>0</v>
@@ -25429,10 +25438,10 @@
     </row>
     <row r="148" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A148" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B148" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C148" s="5" t="b">
         <v>0</v>
@@ -25485,10 +25494,10 @@
     </row>
     <row r="149" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A149" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B149" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C149" s="5" t="b">
         <v>0</v>
@@ -25541,10 +25550,10 @@
     </row>
     <row r="150" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A150" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B150" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C150" s="5" t="b">
         <v>0</v>
@@ -25597,10 +25606,10 @@
     </row>
     <row r="151" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A151" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B151" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C151" s="5" t="b">
         <v>0</v>
@@ -25653,10 +25662,10 @@
     </row>
     <row r="152" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A152" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B152" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C152" s="5" t="b">
         <v>0</v>
@@ -25709,10 +25718,10 @@
     </row>
     <row r="153" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A153" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B153" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C153" s="5" t="b">
         <v>0</v>
@@ -25765,10 +25774,10 @@
     </row>
     <row r="154" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A154" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B154" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C154" s="5" t="b">
         <v>0</v>
@@ -25821,10 +25830,10 @@
     </row>
     <row r="155" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A155" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B155" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C155" s="5" t="b">
         <v>0</v>
@@ -25877,10 +25886,10 @@
     </row>
     <row r="156" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A156" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B156" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C156" s="5" t="b">
         <v>0</v>
@@ -25933,10 +25942,10 @@
     </row>
     <row r="157" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A157" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B157" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C157" s="5" t="b">
         <v>0</v>
@@ -25989,10 +25998,10 @@
     </row>
     <row r="158" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A158" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B158" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C158" s="5" t="b">
         <v>0</v>
@@ -26045,10 +26054,10 @@
     </row>
     <row r="159" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A159" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B159" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C159" s="5" t="b">
         <v>0</v>
@@ -26101,10 +26110,10 @@
     </row>
     <row r="160" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A160" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B160" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C160" s="5" t="b">
         <v>0</v>
@@ -26157,10 +26166,10 @@
     </row>
     <row r="161" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A161" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B161" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C161" s="5" t="b">
         <v>0</v>
@@ -26213,10 +26222,10 @@
     </row>
     <row r="162" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A162" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B162" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C162" s="5" t="b">
         <v>0</v>
@@ -26269,10 +26278,10 @@
     </row>
     <row r="163" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A163" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B163" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C163" s="5" t="b">
         <v>0</v>
@@ -26325,10 +26334,10 @@
     </row>
     <row r="164" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A164" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B164" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C164" s="5" t="b">
         <v>0</v>
@@ -26381,10 +26390,10 @@
     </row>
     <row r="165" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A165" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B165" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C165" s="5" t="b">
         <v>0</v>
@@ -26437,10 +26446,10 @@
     </row>
     <row r="166" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A166" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B166" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C166" s="5" t="b">
         <v>0</v>
@@ -26493,10 +26502,10 @@
     </row>
     <row r="167" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A167" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B167" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C167" s="5" t="b">
         <v>0</v>
@@ -26549,10 +26558,10 @@
     </row>
     <row r="168" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A168" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B168" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C168" s="5" t="b">
         <v>0</v>
@@ -26605,10 +26614,10 @@
     </row>
     <row r="169" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A169" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B169" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C169" s="5" t="b">
         <v>0</v>
@@ -26661,10 +26670,10 @@
     </row>
     <row r="170" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A170" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B170" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C170" s="5" t="b">
         <v>0</v>
@@ -26717,10 +26726,10 @@
     </row>
     <row r="171" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A171" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B171" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C171" s="5" t="b">
         <v>0</v>
@@ -26773,10 +26782,10 @@
     </row>
     <row r="172" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A172" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B172" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C172" s="5" t="b">
         <v>0</v>
@@ -26829,10 +26838,10 @@
     </row>
     <row r="173" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A173" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B173" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C173" s="5" t="b">
         <v>0</v>
@@ -26885,10 +26894,10 @@
     </row>
     <row r="174" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A174" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B174" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C174" s="5" t="b">
         <v>0</v>
@@ -26941,10 +26950,10 @@
     </row>
     <row r="175" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A175" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B175" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C175" s="5" t="b">
         <v>0</v>
@@ -26997,10 +27006,10 @@
     </row>
     <row r="176" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A176" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B176" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C176" s="5" t="b">
         <v>0</v>
@@ -27053,10 +27062,10 @@
     </row>
     <row r="177" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A177" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B177" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C177" s="5" t="b">
         <v>0</v>
@@ -27109,10 +27118,10 @@
     </row>
     <row r="178" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A178" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B178" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C178" s="5" t="b">
         <v>0</v>
@@ -27165,10 +27174,10 @@
     </row>
     <row r="179" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A179" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B179" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C179" s="5" t="b">
         <v>0</v>
@@ -27221,10 +27230,10 @@
     </row>
     <row r="180" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A180" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B180" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C180" s="5" t="b">
         <v>0</v>
@@ -27277,10 +27286,10 @@
     </row>
     <row r="181" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A181" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B181" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C181" s="5" t="b">
         <v>0</v>
@@ -27333,10 +27342,10 @@
     </row>
     <row r="182" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A182" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B182" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C182" s="5" t="b">
         <v>0</v>
@@ -27389,10 +27398,10 @@
     </row>
     <row r="183" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A183" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B183" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C183" s="5" t="b">
         <v>0</v>
@@ -27445,10 +27454,10 @@
     </row>
     <row r="184" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A184" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B184" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C184" s="5" t="b">
         <v>0</v>
@@ -27501,10 +27510,10 @@
     </row>
     <row r="185" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A185" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B185" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C185" s="5" t="b">
         <v>0</v>
@@ -27557,10 +27566,10 @@
     </row>
     <row r="186" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A186" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B186" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C186" s="5" t="b">
         <v>0</v>
@@ -27613,10 +27622,10 @@
     </row>
     <row r="187" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A187" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B187" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C187" s="5" t="b">
         <v>0</v>
@@ -27669,10 +27678,10 @@
     </row>
     <row r="188" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A188" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B188" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C188" s="5" t="b">
         <v>0</v>
@@ -27725,10 +27734,10 @@
     </row>
     <row r="189" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A189" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B189" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C189" s="5" t="b">
         <v>0</v>
@@ -27781,10 +27790,10 @@
     </row>
     <row r="190" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A190" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B190" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C190" s="5" t="b">
         <v>0</v>
@@ -27837,10 +27846,10 @@
     </row>
     <row r="191" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A191" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B191" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C191" s="5" t="b">
         <v>0</v>
@@ -27893,10 +27902,10 @@
     </row>
     <row r="192" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A192" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B192" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C192" s="5" t="b">
         <v>0</v>
@@ -27949,10 +27958,10 @@
     </row>
     <row r="193" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A193" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B193" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C193" s="5" t="b">
         <v>0</v>
@@ -28005,10 +28014,10 @@
     </row>
     <row r="194" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A194" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B194" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C194" s="5" t="b">
         <v>0</v>
@@ -28061,10 +28070,10 @@
     </row>
     <row r="195" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A195" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B195" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C195" s="5" t="b">
         <v>0</v>
@@ -28117,10 +28126,10 @@
     </row>
     <row r="196" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A196" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B196" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C196" s="5" t="b">
         <v>0</v>
@@ -28173,10 +28182,10 @@
     </row>
     <row r="197" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A197" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B197" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C197" s="5" t="b">
         <v>0</v>
@@ -28229,10 +28238,10 @@
     </row>
     <row r="198" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A198" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B198" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C198" s="5" t="b">
         <v>0</v>
@@ -28285,10 +28294,10 @@
     </row>
     <row r="199" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A199" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B199" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C199" s="5" t="b">
         <v>0</v>
@@ -28341,10 +28350,10 @@
     </row>
     <row r="200" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A200" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B200" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C200" s="5" t="b">
         <v>0</v>
@@ -28397,10 +28406,10 @@
     </row>
     <row r="201" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A201" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B201" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C201" s="5" t="b">
         <v>0</v>
@@ -28453,10 +28462,10 @@
     </row>
     <row r="202" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A202" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B202" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C202" s="5" t="b">
         <v>0</v>
@@ -28509,10 +28518,10 @@
     </row>
     <row r="203" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A203" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B203" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C203" s="5" t="b">
         <v>0</v>
@@ -28565,10 +28574,10 @@
     </row>
     <row r="204" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A204" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B204" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C204" s="5" t="b">
         <v>0</v>
@@ -28621,10 +28630,10 @@
     </row>
     <row r="205" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A205" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B205" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C205" s="5" t="b">
         <v>0</v>
@@ -28677,10 +28686,10 @@
     </row>
     <row r="206" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A206" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B206" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C206" s="5" t="b">
         <v>0</v>
@@ -28733,10 +28742,10 @@
     </row>
     <row r="207" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A207" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B207" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C207" s="5" t="b">
         <v>0</v>
@@ -28789,10 +28798,10 @@
     </row>
     <row r="208" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A208" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B208" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C208" s="5" t="b">
         <v>0</v>
@@ -28845,10 +28854,10 @@
     </row>
     <row r="209" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A209" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B209" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C209" s="5" t="b">
         <v>0</v>
@@ -28901,10 +28910,10 @@
     </row>
     <row r="210" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A210" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B210" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C210" s="5" t="b">
         <v>0</v>
@@ -28957,10 +28966,10 @@
     </row>
     <row r="211" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A211" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B211" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C211" s="5" t="b">
         <v>0</v>
@@ -29013,10 +29022,10 @@
     </row>
     <row r="212" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A212" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B212" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C212" s="5" t="b">
         <v>0</v>
@@ -29069,10 +29078,10 @@
     </row>
     <row r="213" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A213" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B213" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C213" s="5" t="b">
         <v>0</v>
@@ -29125,10 +29134,10 @@
     </row>
     <row r="214" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A214" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B214" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C214" s="5" t="b">
         <v>0</v>
@@ -29181,10 +29190,10 @@
     </row>
     <row r="215" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A215" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B215" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C215" s="5" t="b">
         <v>0</v>
@@ -29237,10 +29246,10 @@
     </row>
     <row r="216" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A216" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B216" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C216" s="5" t="b">
         <v>0</v>
@@ -29293,10 +29302,10 @@
     </row>
     <row r="217" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A217" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B217" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C217" s="5" t="b">
         <v>0</v>
@@ -29349,10 +29358,10 @@
     </row>
     <row r="218" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A218" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B218" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C218" s="5" t="b">
         <v>0</v>
@@ -29405,10 +29414,10 @@
     </row>
     <row r="219" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A219" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B219" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C219" s="5" t="b">
         <v>0</v>
@@ -29461,10 +29470,10 @@
     </row>
     <row r="220" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A220" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B220" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C220" s="5" t="b">
         <v>0</v>
@@ -29517,10 +29526,10 @@
     </row>
     <row r="221" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A221" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B221" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C221" s="5" t="b">
         <v>0</v>
@@ -29573,10 +29582,10 @@
     </row>
     <row r="222" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A222" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B222" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C222" s="5" t="b">
         <v>0</v>
@@ -29629,10 +29638,10 @@
     </row>
     <row r="223" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A223" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B223" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C223" s="5" t="b">
         <v>0</v>
@@ -29685,10 +29694,10 @@
     </row>
     <row r="224" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A224" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B224" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C224" s="5" t="b">
         <v>0</v>
@@ -29741,10 +29750,10 @@
     </row>
     <row r="225" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A225" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B225" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C225" s="5" t="b">
         <v>0</v>
@@ -29797,10 +29806,10 @@
     </row>
     <row r="226" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A226" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B226" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C226" s="5" t="b">
         <v>0</v>
@@ -29853,10 +29862,10 @@
     </row>
     <row r="227" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A227" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B227" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C227" s="5" t="b">
         <v>0</v>
@@ -29909,10 +29918,10 @@
     </row>
     <row r="228" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A228" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B228" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C228" s="5" t="b">
         <v>0</v>
@@ -29965,10 +29974,10 @@
     </row>
     <row r="229" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A229" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B229" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C229" s="5" t="b">
         <v>0</v>
@@ -30021,10 +30030,10 @@
     </row>
     <row r="230" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A230" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B230" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C230" s="5" t="b">
         <v>0</v>
@@ -30077,10 +30086,10 @@
     </row>
     <row r="231" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A231" s="3" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="B231" s="3" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="C231" s="5" t="b">
         <v>0</v>

</xml_diff>

<commit_message>
generated all the reports on 2024-06-19
</commit_message>
<xml_diff>
--- a/report/merged_configurations.xlsx
+++ b/report/merged_configurations.xlsx
@@ -16793,7 +16793,7 @@
         <v>23</v>
       </c>
       <c r="D210" s="3" t="s">
-        <v>41</v>
+        <v>24</v>
       </c>
       <c r="E210" s="3" t="s">
         <v>1068</v>
@@ -16834,7 +16834,9 @@
       <c r="Q210" s="3" t="s">
         <v>1076</v>
       </c>
-      <c r="R210" s="3"/>
+      <c r="R210" s="4">
+        <v>45461</v>
+      </c>
       <c r="S210" s="3"/>
       <c r="T210" s="3" t="s">
         <v>35</v>
@@ -16854,7 +16856,7 @@
         <v>23</v>
       </c>
       <c r="D211" s="3" t="s">
-        <v>41</v>
+        <v>24</v>
       </c>
       <c r="E211" s="3" t="s">
         <v>1079</v>
@@ -16895,7 +16897,9 @@
       <c r="Q211" s="3" t="s">
         <v>1076</v>
       </c>
-      <c r="R211" s="3"/>
+      <c r="R211" s="4">
+        <v>45461</v>
+      </c>
       <c r="S211" s="3"/>
       <c r="T211" s="3" t="s">
         <v>35</v>

</xml_diff>

<commit_message>
generated all the reports on 2024-06-21
</commit_message>
<xml_diff>
--- a/report/merged_configurations.xlsx
+++ b/report/merged_configurations.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4569" uniqueCount="1210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4573" uniqueCount="1210">
   <si>
     <t>title</t>
   </si>
@@ -2963,10 +2963,10 @@
     <t>ap-doelgericht-cultuur-en-jeugd-config.md</t>
   </si>
   <si>
-    <t>[{"name":"Applicatieprofiel Cultuur- &amp; Jeugdinfrastructuur","resourceReference":"https://data.vlaanderen.be/doc/applicatieprofiel/cultuur-en-jeugdinfrastructuur"}]</t>
-  </si>
-  <si>
-    <t>[{"name":"Vocabularium Cultuur- &amp; Jeugdinfrastructuur","resourceReference":"https://data.vlaanderen.be/ns/cultuur-en-jeugdinfrastructuur"}]</t>
+    <t>[{"name":"Applicatieprofiel Cultuur- &amp; Jeugdinfrastructuur","resourceReference":"https://data.vlaanderen.be/doc/applicatieprofiel/cultuur-en-jeugd/infrastructuur"}]</t>
+  </si>
+  <si>
+    <t>[{"name":"Vocabularium Cultuur- &amp; Jeugdinfrastructuur","resourceReference":"https://data.vlaanderen.be/ns/cultuur-en-jeugd/infrastructuur"}]</t>
   </si>
   <si>
     <t>[{"name":"Verslag Business Werkgroep - 7 december 2021","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-cultuurandjeugdinfrastructuur/standaardenregister/reports/20211207_BusinessWorkshop_MeetingMinutes_OSLOCultuurenJeugdinfrastructuur.docx"},{"name":"Verslag Thematische Werkgroep I - 26 januari 2022","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-cultuurandjeugdinfrastructuur/standaardenregister/reports/20220126_ThematicWorkshop1_MeetingMinutes_OSLOCultuurenJeugdinfrastructuur.docx"},{"name":"Verslag Thematische Werkgroep II - 22 februari 2022","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-cultuurandjeugdinfrastructuur/standaardenregister/reports/20220222_ThematicWorkshop2_MeetingMinutes_OSLOCultuurenJeugdinfrastructuur.docx"},{"name":"Verslag Thematische Werkgroep III - 22 maart 2022","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-cultuurandjeugdinfrastructuur/standaardenregister/reports/20220322_MeetingMinutes_ThematicWorkshop3_OSLOCultuurenJeugdInfrastructuur.docx"},{"name":"Verslag Thematische Werkgroep IV - 10 mei 2022","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-cultuurandjeugdinfrastructuur/standaardenregister/reports/20220510_MeetingMinutes_ThematicWorkshop4_OSLOCultuur-enJeugdinfrastructuur.docx"}]</t>
@@ -2984,10 +2984,10 @@
     <t>1 december 2021</t>
   </si>
   <si>
+    <t>OSLOthema-cultuurandjeugdinfrastructuur</t>
+  </si>
+  <si>
     <t>23 juni 2022</t>
-  </si>
-  <si>
-    <t>OSLOthema-cultuurandjeugdinfrastructuur</t>
   </si>
   <si>
     <t>{"name":"Werkgroep Charter Cultuur- &amp; Jeugdinfrastructuur","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-cultuurandjeugdinfrastructuur/standaardenregister/charter/20211018_Werkgroep charter OSLO Basisinventaris cultuur- en jeugdinfrastructuur.docx"}</t>
@@ -16100,16 +16100,20 @@
         <v>989</v>
       </c>
       <c r="O198" s="3" t="s">
-        <v>990</v>
+        <v>33</v>
       </c>
       <c r="P198" s="3" t="s">
         <v>33</v>
       </c>
       <c r="Q198" s="3" t="s">
+        <v>990</v>
+      </c>
+      <c r="R198" s="3" t="s">
         <v>991</v>
       </c>
-      <c r="R198" s="3"/>
-      <c r="S198" s="3"/>
+      <c r="S198" s="3" t="s">
+        <v>33</v>
+      </c>
       <c r="T198" s="3" t="s">
         <v>35</v>
       </c>
@@ -16161,16 +16165,20 @@
         <v>989</v>
       </c>
       <c r="O199" s="3" t="s">
-        <v>990</v>
+        <v>33</v>
       </c>
       <c r="P199" s="3" t="s">
         <v>33</v>
       </c>
       <c r="Q199" s="3" t="s">
+        <v>990</v>
+      </c>
+      <c r="R199" s="3" t="s">
         <v>991</v>
       </c>
-      <c r="R199" s="3"/>
-      <c r="S199" s="3"/>
+      <c r="S199" s="3" t="s">
+        <v>33</v>
+      </c>
       <c r="T199" s="3" t="s">
         <v>35</v>
       </c>

</xml_diff>

<commit_message>
generated all the reports on 2024-06-25
</commit_message>
<xml_diff>
--- a/report/merged_configurations.xlsx
+++ b/report/merged_configurations.xlsx
@@ -17464,7 +17464,7 @@
         <v>23</v>
       </c>
       <c r="D221" s="3" t="s">
-        <v>41</v>
+        <v>24</v>
       </c>
       <c r="E221" s="3" t="s">
         <v>1137</v>
@@ -17505,7 +17505,9 @@
       <c r="Q221" s="3" t="s">
         <v>1145</v>
       </c>
-      <c r="R221" s="3"/>
+      <c r="R221" s="4">
+        <v>45467</v>
+      </c>
       <c r="S221" s="3"/>
       <c r="T221" s="3" t="s">
         <v>35</v>
@@ -17525,7 +17527,7 @@
         <v>23</v>
       </c>
       <c r="D222" s="3" t="s">
-        <v>41</v>
+        <v>24</v>
       </c>
       <c r="E222" s="3" t="s">
         <v>1137</v>
@@ -17566,7 +17568,9 @@
       <c r="Q222" s="3" t="s">
         <v>1145</v>
       </c>
-      <c r="R222" s="3"/>
+      <c r="R222" s="4">
+        <v>45461</v>
+      </c>
       <c r="S222" s="3"/>
       <c r="T222" s="3" t="s">
         <v>35</v>

</xml_diff>

<commit_message>
generated all the reports on 2024-07-17
</commit_message>
<xml_diff>
--- a/report/merged_configurations.xlsx
+++ b/report/merged_configurations.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4573" uniqueCount="1209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4572" uniqueCount="1210">
   <si>
     <t>title</t>
   </si>
@@ -3191,7 +3191,7 @@
     <t>ap-or-voc-slimmestadsdistributie.md</t>
   </si>
   <si>
-    <t>[{"name":"Slimme Stadsdistributie - ApplicatieProfiel","resourceReference":"https://test.data.vlaanderen.be/doc/applicatieprofiel/slimme-stadsdistributie"},{"name":"Slimme Stadsdistributie - Vocabularium","resourceReference":"https://test.data.vlaanderen.be/ns/slimme-stadsdistributie"}]</t>
+    <t>[{"name":"Slimme Stadsdistributie - ApplicatieProfiel","resourceReference":"https://data.vlaanderen.be/doc/applicatieprofiel/slimme-stadsdistributie"},{"name":"Slimme Stadsdistributie - Vocabularium","resourceReference":"https://data.vlaanderen.be/ns/slimme-stadsdistributie"}]</t>
   </si>
   <si>
     <t>[{"name":"Verslag Business werkgroep - 11 januari 2023","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-slimmeStadsdistributie/standaardenregister/reports/Verslag_Business_werkgroep_-_11_januari_2023.pdf"},{"name":"Verslag Eerste Thematische werkgroep - 8 februari 2023","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-slimmeStadsdistributie/standaardenregister/reports/Verslag_Thematische_Werkgroep_1_-_8_februari_2023.pdf"}]</t>
@@ -3204,6 +3204,9 @@
   </si>
   <si>
     <t>[{"name":"Presentatie Business werkgroep  - 11 januari 2023","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-slimmeStadsdistributie/standaardenregister/presentations/Presentatie_Business_werkgroep_-_11_januari_2023.pdf"},{"name":"Presentatie Eerste Thematische werkgroep - 8 februari 2023","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-slimmeStadsdistributie/standaardenregister/presentations/Presentatie_Thematische_werkgroep_1_-_8_februari_2023.pdf"}]</t>
+  </si>
+  <si>
+    <t>25 januari 2023</t>
   </si>
   <si>
     <t>OSLOthema-slimmeStadsdistributie</t>
@@ -16745,8 +16748,8 @@
       <c r="F209" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="G209" s="3" t="s">
-        <v>33</v>
+      <c r="G209" s="4">
+        <v>45489</v>
       </c>
       <c r="H209" s="3" t="s">
         <v>1059</v>
@@ -16767,7 +16770,7 @@
         <v>1063</v>
       </c>
       <c r="N209" s="3" t="s">
-        <v>33</v>
+        <v>1064</v>
       </c>
       <c r="O209" s="3" t="s">
         <v>33</v>
@@ -16776,7 +16779,7 @@
         <v>33</v>
       </c>
       <c r="Q209" s="3" t="s">
-        <v>1064</v>
+        <v>1065</v>
       </c>
       <c r="R209" s="3"/>
       <c r="S209" s="3"/>
@@ -16784,12 +16787,12 @@
         <v>35</v>
       </c>
       <c r="U209" s="3" t="s">
-        <v>1065</v>
+        <v>1066</v>
       </c>
     </row>
     <row r="210" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A210" s="3" t="s">
-        <v>1066</v>
+        <v>1067</v>
       </c>
       <c r="B210" s="3" t="s">
         <v>22</v>
@@ -16801,7 +16804,7 @@
         <v>24</v>
       </c>
       <c r="E210" s="3" t="s">
-        <v>1067</v>
+        <v>1068</v>
       </c>
       <c r="F210" s="3" t="s">
         <v>43</v>
@@ -16810,25 +16813,25 @@
         <v>44875</v>
       </c>
       <c r="H210" s="3" t="s">
-        <v>1068</v>
+        <v>1069</v>
       </c>
       <c r="I210" s="3" t="s">
-        <v>1069</v>
+        <v>1070</v>
       </c>
       <c r="J210" s="3" t="s">
-        <v>1070</v>
+        <v>1071</v>
       </c>
       <c r="K210" s="3" t="s">
-        <v>1071</v>
+        <v>1072</v>
       </c>
       <c r="L210" s="3" t="s">
-        <v>1072</v>
+        <v>1073</v>
       </c>
       <c r="M210" s="3" t="s">
-        <v>1073</v>
+        <v>1074</v>
       </c>
       <c r="N210" s="3" t="s">
-        <v>1074</v>
+        <v>1075</v>
       </c>
       <c r="O210" s="3" t="s">
         <v>33</v>
@@ -16837,7 +16840,7 @@
         <v>33</v>
       </c>
       <c r="Q210" s="3" t="s">
-        <v>1075</v>
+        <v>1076</v>
       </c>
       <c r="R210" s="4">
         <v>45461</v>
@@ -16847,12 +16850,12 @@
         <v>35</v>
       </c>
       <c r="U210" s="3" t="s">
-        <v>1076</v>
+        <v>1077</v>
       </c>
     </row>
     <row r="211" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A211" s="3" t="s">
-        <v>1077</v>
+        <v>1078</v>
       </c>
       <c r="B211" s="3" t="s">
         <v>38</v>
@@ -16864,7 +16867,7 @@
         <v>24</v>
       </c>
       <c r="E211" s="3" t="s">
-        <v>1078</v>
+        <v>1079</v>
       </c>
       <c r="F211" s="3" t="s">
         <v>43</v>
@@ -16873,25 +16876,25 @@
         <v>44875</v>
       </c>
       <c r="H211" s="3" t="s">
+        <v>1070</v>
+      </c>
+      <c r="I211" s="3" t="s">
         <v>1069</v>
       </c>
-      <c r="I211" s="3" t="s">
-        <v>1068</v>
-      </c>
       <c r="J211" s="3" t="s">
-        <v>1070</v>
+        <v>1071</v>
       </c>
       <c r="K211" s="3" t="s">
-        <v>1071</v>
+        <v>1072</v>
       </c>
       <c r="L211" s="3" t="s">
-        <v>1072</v>
+        <v>1073</v>
       </c>
       <c r="M211" s="3" t="s">
-        <v>1073</v>
+        <v>1074</v>
       </c>
       <c r="N211" s="3" t="s">
-        <v>1074</v>
+        <v>1075</v>
       </c>
       <c r="O211" s="3" t="s">
         <v>33</v>
@@ -16900,7 +16903,7 @@
         <v>33</v>
       </c>
       <c r="Q211" s="3" t="s">
-        <v>1075</v>
+        <v>1076</v>
       </c>
       <c r="R211" s="4">
         <v>45461</v>
@@ -16910,12 +16913,12 @@
         <v>35</v>
       </c>
       <c r="U211" s="3" t="s">
-        <v>1076</v>
+        <v>1077</v>
       </c>
     </row>
     <row r="212" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A212" s="3" t="s">
-        <v>1079</v>
+        <v>1080</v>
       </c>
       <c r="B212" s="3" t="s">
         <v>778</v>
@@ -16936,22 +16939,22 @@
         <v>45131</v>
       </c>
       <c r="H212" s="3" t="s">
-        <v>1080</v>
+        <v>1081</v>
       </c>
       <c r="I212" s="3" t="s">
         <v>28</v>
       </c>
       <c r="J212" s="3" t="s">
-        <v>1081</v>
+        <v>1082</v>
       </c>
       <c r="K212" s="3" t="s">
         <v>30</v>
       </c>
       <c r="L212" s="3" t="s">
-        <v>1082</v>
+        <v>1083</v>
       </c>
       <c r="M212" s="3" t="s">
-        <v>1083</v>
+        <v>1084</v>
       </c>
       <c r="N212" s="4">
         <v>44873</v>
@@ -16963,7 +16966,7 @@
         <v>33</v>
       </c>
       <c r="Q212" s="3" t="s">
-        <v>1084</v>
+        <v>1085</v>
       </c>
       <c r="R212" s="3"/>
       <c r="S212" s="3"/>
@@ -16971,12 +16974,12 @@
         <v>35</v>
       </c>
       <c r="U212" s="3" t="s">
-        <v>1085</v>
+        <v>1086</v>
       </c>
     </row>
     <row r="213" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A213" s="3" t="s">
-        <v>1086</v>
+        <v>1087</v>
       </c>
       <c r="B213" s="3" t="s">
         <v>38</v>
@@ -16997,22 +17000,22 @@
         <v>45131</v>
       </c>
       <c r="H213" s="3" t="s">
-        <v>1087</v>
+        <v>1088</v>
       </c>
       <c r="I213" s="3" t="s">
         <v>28</v>
       </c>
       <c r="J213" s="3" t="s">
-        <v>1081</v>
+        <v>1082</v>
       </c>
       <c r="K213" s="3" t="s">
         <v>30</v>
       </c>
       <c r="L213" s="3" t="s">
-        <v>1082</v>
+        <v>1083</v>
       </c>
       <c r="M213" s="3" t="s">
-        <v>1083</v>
+        <v>1084</v>
       </c>
       <c r="N213" s="4">
         <v>44873</v>
@@ -17024,7 +17027,7 @@
         <v>33</v>
       </c>
       <c r="Q213" s="3" t="s">
-        <v>1084</v>
+        <v>1085</v>
       </c>
       <c r="R213" s="3"/>
       <c r="S213" s="3"/>
@@ -17032,12 +17035,12 @@
         <v>35</v>
       </c>
       <c r="U213" s="3" t="s">
-        <v>1085</v>
+        <v>1086</v>
       </c>
     </row>
     <row r="214" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A214" s="3" t="s">
-        <v>1088</v>
+        <v>1089</v>
       </c>
       <c r="B214" s="3" t="s">
         <v>22</v>
@@ -17049,7 +17052,7 @@
         <v>24</v>
       </c>
       <c r="E214" s="3" t="s">
-        <v>1089</v>
+        <v>1090</v>
       </c>
       <c r="F214" s="3" t="s">
         <v>545</v>
@@ -17058,34 +17061,34 @@
         <v>45330</v>
       </c>
       <c r="H214" s="3" t="s">
-        <v>1090</v>
+        <v>1091</v>
       </c>
       <c r="I214" s="3" t="s">
-        <v>1091</v>
+        <v>1092</v>
       </c>
       <c r="J214" s="3" t="s">
-        <v>1092</v>
+        <v>1093</v>
       </c>
       <c r="K214" s="3" t="s">
-        <v>1093</v>
+        <v>1094</v>
       </c>
       <c r="L214" s="3" t="s">
-        <v>1094</v>
+        <v>1095</v>
       </c>
       <c r="M214" s="3" t="s">
-        <v>1095</v>
+        <v>1096</v>
       </c>
       <c r="N214" s="3" t="s">
-        <v>1096</v>
+        <v>1097</v>
       </c>
       <c r="O214" s="3" t="s">
-        <v>1097</v>
+        <v>1098</v>
       </c>
       <c r="P214" s="3" t="s">
         <v>33</v>
       </c>
       <c r="Q214" s="3" t="s">
-        <v>1098</v>
+        <v>1099</v>
       </c>
       <c r="R214" s="3"/>
       <c r="S214" s="3"/>
@@ -17093,12 +17096,12 @@
         <v>35</v>
       </c>
       <c r="U214" s="3" t="s">
-        <v>1099</v>
+        <v>1100</v>
       </c>
     </row>
     <row r="215" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A215" s="3" t="s">
-        <v>1100</v>
+        <v>1101</v>
       </c>
       <c r="B215" s="3" t="s">
         <v>38</v>
@@ -17110,7 +17113,7 @@
         <v>24</v>
       </c>
       <c r="E215" s="3" t="s">
-        <v>1101</v>
+        <v>1102</v>
       </c>
       <c r="F215" s="3" t="s">
         <v>545</v>
@@ -17119,34 +17122,34 @@
         <v>45330</v>
       </c>
       <c r="H215" s="3" t="s">
+        <v>1092</v>
+      </c>
+      <c r="I215" s="3" t="s">
         <v>1091</v>
       </c>
-      <c r="I215" s="3" t="s">
-        <v>1090</v>
-      </c>
       <c r="J215" s="3" t="s">
-        <v>1092</v>
+        <v>1093</v>
       </c>
       <c r="K215" s="3" t="s">
-        <v>1093</v>
+        <v>1094</v>
       </c>
       <c r="L215" s="3" t="s">
-        <v>1094</v>
+        <v>1095</v>
       </c>
       <c r="M215" s="3" t="s">
-        <v>1095</v>
+        <v>1096</v>
       </c>
       <c r="N215" s="3" t="s">
-        <v>1096</v>
+        <v>1097</v>
       </c>
       <c r="O215" s="3" t="s">
-        <v>1097</v>
+        <v>1098</v>
       </c>
       <c r="P215" s="3" t="s">
         <v>33</v>
       </c>
       <c r="Q215" s="3" t="s">
-        <v>1098</v>
+        <v>1099</v>
       </c>
       <c r="R215" s="3"/>
       <c r="S215" s="3"/>
@@ -17154,15 +17157,15 @@
         <v>35</v>
       </c>
       <c r="U215" s="3" t="s">
-        <v>1099</v>
+        <v>1100</v>
       </c>
     </row>
     <row r="216" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A216" s="3" t="s">
-        <v>1102</v>
+        <v>1103</v>
       </c>
       <c r="B216" s="3" t="s">
-        <v>1103</v>
+        <v>1104</v>
       </c>
       <c r="C216" s="3" t="s">
         <v>23</v>
@@ -17180,28 +17183,28 @@
         <v>45308</v>
       </c>
       <c r="H216" s="3" t="s">
-        <v>1104</v>
+        <v>1105</v>
       </c>
       <c r="I216" s="3" t="s">
         <v>28</v>
       </c>
       <c r="J216" s="3" t="s">
-        <v>1105</v>
+        <v>1106</v>
       </c>
       <c r="K216" s="3" t="s">
-        <v>1106</v>
+        <v>1107</v>
       </c>
       <c r="L216" s="3" t="s">
-        <v>1107</v>
+        <v>1108</v>
       </c>
       <c r="M216" s="3" t="s">
-        <v>1108</v>
+        <v>1109</v>
       </c>
       <c r="N216" s="3"/>
       <c r="O216" s="3"/>
       <c r="P216" s="3"/>
       <c r="Q216" s="3" t="s">
-        <v>1109</v>
+        <v>1110</v>
       </c>
       <c r="R216" s="3"/>
       <c r="S216" s="3"/>
@@ -17209,15 +17212,15 @@
         <v>35</v>
       </c>
       <c r="U216" s="3" t="s">
-        <v>1110</v>
+        <v>1111</v>
       </c>
     </row>
     <row r="217" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A217" s="3" t="s">
-        <v>1111</v>
+        <v>1112</v>
       </c>
       <c r="B217" s="3" t="s">
-        <v>1112</v>
+        <v>1113</v>
       </c>
       <c r="C217" s="3" t="s">
         <v>23</v>
@@ -17235,28 +17238,28 @@
         <v>45308</v>
       </c>
       <c r="H217" s="3" t="s">
-        <v>1113</v>
+        <v>1114</v>
       </c>
       <c r="I217" s="3" t="s">
         <v>28</v>
       </c>
       <c r="J217" s="3" t="s">
-        <v>1105</v>
+        <v>1106</v>
       </c>
       <c r="K217" s="3" t="s">
-        <v>1106</v>
+        <v>1107</v>
       </c>
       <c r="L217" s="3" t="s">
-        <v>1107</v>
+        <v>1108</v>
       </c>
       <c r="M217" s="3" t="s">
-        <v>1108</v>
+        <v>1109</v>
       </c>
       <c r="N217" s="3"/>
       <c r="O217" s="3"/>
       <c r="P217" s="3"/>
       <c r="Q217" s="3" t="s">
-        <v>1109</v>
+        <v>1110</v>
       </c>
       <c r="R217" s="3"/>
       <c r="S217" s="3"/>
@@ -17264,12 +17267,12 @@
         <v>35</v>
       </c>
       <c r="U217" s="3" t="s">
-        <v>1110</v>
+        <v>1111</v>
       </c>
     </row>
     <row r="218" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A218" s="3" t="s">
-        <v>1114</v>
+        <v>1115</v>
       </c>
       <c r="B218" s="3" t="s">
         <v>22</v>
@@ -17281,7 +17284,7 @@
         <v>24</v>
       </c>
       <c r="E218" s="3" t="s">
-        <v>1115</v>
+        <v>1116</v>
       </c>
       <c r="F218" s="3" t="s">
         <v>1033</v>
@@ -17290,25 +17293,25 @@
         <v>45323</v>
       </c>
       <c r="H218" s="3" t="s">
-        <v>1116</v>
+        <v>1117</v>
       </c>
       <c r="I218" s="3" t="s">
-        <v>1117</v>
+        <v>1118</v>
       </c>
       <c r="J218" s="3" t="s">
-        <v>1118</v>
+        <v>1119</v>
       </c>
       <c r="K218" s="3" t="s">
-        <v>1119</v>
+        <v>1120</v>
       </c>
       <c r="L218" s="3" t="s">
-        <v>1120</v>
+        <v>1121</v>
       </c>
       <c r="M218" s="3" t="s">
-        <v>1121</v>
+        <v>1122</v>
       </c>
       <c r="N218" s="3" t="s">
-        <v>1122</v>
+        <v>1123</v>
       </c>
       <c r="O218" s="3" t="s">
         <v>33</v>
@@ -17317,7 +17320,7 @@
         <v>33</v>
       </c>
       <c r="Q218" s="3" t="s">
-        <v>1123</v>
+        <v>1124</v>
       </c>
       <c r="R218" s="3"/>
       <c r="S218" s="3"/>
@@ -17325,12 +17328,12 @@
         <v>35</v>
       </c>
       <c r="U218" s="3" t="s">
-        <v>1124</v>
+        <v>1125</v>
       </c>
     </row>
     <row r="219" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A219" s="3" t="s">
-        <v>1125</v>
+        <v>1126</v>
       </c>
       <c r="B219" s="3" t="s">
         <v>38</v>
@@ -17342,7 +17345,7 @@
         <v>24</v>
       </c>
       <c r="E219" s="3" t="s">
-        <v>1126</v>
+        <v>1127</v>
       </c>
       <c r="F219" s="3" t="s">
         <v>1033</v>
@@ -17351,25 +17354,25 @@
         <v>45323</v>
       </c>
       <c r="H219" s="3" t="s">
-        <v>1127</v>
+        <v>1128</v>
       </c>
       <c r="I219" s="3" t="s">
-        <v>1128</v>
+        <v>1129</v>
       </c>
       <c r="J219" s="3" t="s">
-        <v>1129</v>
+        <v>1130</v>
       </c>
       <c r="K219" s="3" t="s">
-        <v>1119</v>
+        <v>1120</v>
       </c>
       <c r="L219" s="3" t="s">
-        <v>1120</v>
+        <v>1121</v>
       </c>
       <c r="M219" s="3" t="s">
-        <v>1121</v>
+        <v>1122</v>
       </c>
       <c r="N219" s="3" t="s">
-        <v>1122</v>
+        <v>1123</v>
       </c>
       <c r="O219" s="3" t="s">
         <v>33</v>
@@ -17378,7 +17381,7 @@
         <v>33</v>
       </c>
       <c r="Q219" s="3" t="s">
-        <v>1123</v>
+        <v>1124</v>
       </c>
       <c r="R219" s="3"/>
       <c r="S219" s="3"/>
@@ -17386,12 +17389,12 @@
         <v>35</v>
       </c>
       <c r="U219" s="3" t="s">
-        <v>1124</v>
+        <v>1125</v>
       </c>
     </row>
     <row r="220" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A220" s="3" t="s">
-        <v>1130</v>
+        <v>1131</v>
       </c>
       <c r="B220" s="3" t="s">
         <v>38</v>
@@ -17403,7 +17406,7 @@
         <v>24</v>
       </c>
       <c r="E220" s="3" t="s">
-        <v>1131</v>
+        <v>1132</v>
       </c>
       <c r="F220" s="3" t="s">
         <v>1033</v>
@@ -17412,25 +17415,25 @@
         <v>45393</v>
       </c>
       <c r="H220" s="3" t="s">
-        <v>1132</v>
+        <v>1133</v>
       </c>
       <c r="I220" s="3" t="s">
-        <v>1133</v>
+        <v>1134</v>
       </c>
       <c r="J220" s="3" t="s">
-        <v>1134</v>
+        <v>1135</v>
       </c>
       <c r="K220" s="3" t="s">
-        <v>1119</v>
+        <v>1120</v>
       </c>
       <c r="L220" s="3" t="s">
-        <v>1120</v>
+        <v>1121</v>
       </c>
       <c r="M220" s="3" t="s">
-        <v>1121</v>
+        <v>1122</v>
       </c>
       <c r="N220" s="3" t="s">
-        <v>1122</v>
+        <v>1123</v>
       </c>
       <c r="O220" s="3" t="s">
         <v>33</v>
@@ -17439,7 +17442,7 @@
         <v>33</v>
       </c>
       <c r="Q220" s="3" t="s">
-        <v>1123</v>
+        <v>1124</v>
       </c>
       <c r="R220" s="3"/>
       <c r="S220" s="3"/>
@@ -17447,12 +17450,12 @@
         <v>35</v>
       </c>
       <c r="U220" s="3" t="s">
-        <v>1124</v>
+        <v>1125</v>
       </c>
     </row>
     <row r="221" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A221" s="3" t="s">
-        <v>1135</v>
+        <v>1136</v>
       </c>
       <c r="B221" s="3" t="s">
         <v>22</v>
@@ -17464,7 +17467,7 @@
         <v>24</v>
       </c>
       <c r="E221" s="3" t="s">
-        <v>1136</v>
+        <v>1137</v>
       </c>
       <c r="F221" s="3" t="s">
         <v>43</v>
@@ -17473,25 +17476,25 @@
         <v>45370</v>
       </c>
       <c r="H221" s="3" t="s">
-        <v>1137</v>
+        <v>1138</v>
       </c>
       <c r="I221" s="3" t="s">
-        <v>1138</v>
+        <v>1139</v>
       </c>
       <c r="J221" s="3" t="s">
-        <v>1139</v>
+        <v>1140</v>
       </c>
       <c r="K221" s="3" t="s">
-        <v>1140</v>
+        <v>1141</v>
       </c>
       <c r="L221" s="3" t="s">
-        <v>1141</v>
+        <v>1142</v>
       </c>
       <c r="M221" s="3" t="s">
-        <v>1142</v>
+        <v>1143</v>
       </c>
       <c r="N221" s="3" t="s">
-        <v>1143</v>
+        <v>1144</v>
       </c>
       <c r="O221" s="3" t="s">
         <v>33</v>
@@ -17500,7 +17503,7 @@
         <v>33</v>
       </c>
       <c r="Q221" s="3" t="s">
-        <v>1144</v>
+        <v>1145</v>
       </c>
       <c r="R221" s="4">
         <v>45467</v>
@@ -17510,12 +17513,12 @@
         <v>35</v>
       </c>
       <c r="U221" s="3" t="s">
-        <v>1145</v>
+        <v>1146</v>
       </c>
     </row>
     <row r="222" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A222" s="3" t="s">
-        <v>1146</v>
+        <v>1147</v>
       </c>
       <c r="B222" s="3" t="s">
         <v>38</v>
@@ -17527,7 +17530,7 @@
         <v>24</v>
       </c>
       <c r="E222" s="3" t="s">
-        <v>1136</v>
+        <v>1137</v>
       </c>
       <c r="F222" s="3" t="s">
         <v>43</v>
@@ -17536,25 +17539,25 @@
         <v>45370</v>
       </c>
       <c r="H222" s="3" t="s">
+        <v>1139</v>
+      </c>
+      <c r="I222" s="3" t="s">
         <v>1138</v>
       </c>
-      <c r="I222" s="3" t="s">
-        <v>1137</v>
-      </c>
       <c r="J222" s="3" t="s">
-        <v>1139</v>
+        <v>1140</v>
       </c>
       <c r="K222" s="3" t="s">
-        <v>1140</v>
+        <v>1141</v>
       </c>
       <c r="L222" s="3" t="s">
-        <v>1141</v>
+        <v>1142</v>
       </c>
       <c r="M222" s="3" t="s">
-        <v>1142</v>
+        <v>1143</v>
       </c>
       <c r="N222" s="3" t="s">
-        <v>1143</v>
+        <v>1144</v>
       </c>
       <c r="O222" s="3" t="s">
         <v>33</v>
@@ -17563,7 +17566,7 @@
         <v>33</v>
       </c>
       <c r="Q222" s="3" t="s">
-        <v>1144</v>
+        <v>1145</v>
       </c>
       <c r="R222" s="4">
         <v>45461</v>
@@ -17573,12 +17576,12 @@
         <v>35</v>
       </c>
       <c r="U222" s="3" t="s">
-        <v>1145</v>
+        <v>1146</v>
       </c>
     </row>
     <row r="223" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A223" s="3" t="s">
-        <v>1147</v>
+        <v>1148</v>
       </c>
       <c r="B223" s="3" t="s">
         <v>38</v>
@@ -17590,34 +17593,34 @@
         <v>24</v>
       </c>
       <c r="E223" s="3" t="s">
-        <v>1148</v>
+        <v>1149</v>
       </c>
       <c r="F223" s="3" t="s">
-        <v>1149</v>
+        <v>1150</v>
       </c>
       <c r="G223" s="4">
         <v>45078</v>
       </c>
       <c r="H223" s="3" t="s">
-        <v>1150</v>
+        <v>1151</v>
       </c>
       <c r="I223" s="3" t="s">
-        <v>1151</v>
+        <v>1152</v>
       </c>
       <c r="J223" s="3" t="s">
-        <v>1151</v>
+        <v>1152</v>
       </c>
       <c r="K223" s="3" t="s">
         <v>35</v>
       </c>
       <c r="L223" s="3" t="s">
+        <v>1153</v>
+      </c>
+      <c r="M223" s="3" t="s">
         <v>1152</v>
       </c>
-      <c r="M223" s="3" t="s">
-        <v>1151</v>
-      </c>
       <c r="N223" s="3" t="s">
-        <v>1153</v>
+        <v>1154</v>
       </c>
       <c r="O223" s="3" t="s">
         <v>33</v>
@@ -17626,7 +17629,7 @@
         <v>33</v>
       </c>
       <c r="Q223" s="3" t="s">
-        <v>1154</v>
+        <v>1155</v>
       </c>
       <c r="R223" s="3"/>
       <c r="S223" s="3"/>
@@ -17634,12 +17637,12 @@
         <v>35</v>
       </c>
       <c r="U223" s="3" t="s">
-        <v>1155</v>
+        <v>1156</v>
       </c>
     </row>
     <row r="224" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A224" s="3" t="s">
-        <v>1156</v>
+        <v>1157</v>
       </c>
       <c r="B224" s="3" t="s">
         <v>22</v>
@@ -17651,34 +17654,34 @@
         <v>24</v>
       </c>
       <c r="E224" s="3" t="s">
-        <v>1157</v>
+        <v>1158</v>
       </c>
       <c r="F224" s="3" t="s">
-        <v>1149</v>
+        <v>1150</v>
       </c>
       <c r="G224" s="4">
         <v>45078</v>
       </c>
       <c r="H224" s="3" t="s">
-        <v>1158</v>
+        <v>1159</v>
       </c>
       <c r="I224" s="3" t="s">
-        <v>1151</v>
+        <v>1152</v>
       </c>
       <c r="J224" s="3" t="s">
-        <v>1151</v>
+        <v>1152</v>
       </c>
       <c r="K224" s="3" t="s">
         <v>35</v>
       </c>
       <c r="L224" s="3" t="s">
+        <v>1153</v>
+      </c>
+      <c r="M224" s="3" t="s">
         <v>1152</v>
       </c>
-      <c r="M224" s="3" t="s">
-        <v>1151</v>
-      </c>
       <c r="N224" s="3" t="s">
-        <v>1153</v>
+        <v>1154</v>
       </c>
       <c r="O224" s="3" t="s">
         <v>33</v>
@@ -17687,7 +17690,7 @@
         <v>33</v>
       </c>
       <c r="Q224" s="3" t="s">
-        <v>1154</v>
+        <v>1155</v>
       </c>
       <c r="R224" s="3"/>
       <c r="S224" s="3"/>
@@ -17695,12 +17698,12 @@
         <v>35</v>
       </c>
       <c r="U224" s="3" t="s">
-        <v>1155</v>
+        <v>1156</v>
       </c>
     </row>
     <row r="225" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A225" s="3" t="s">
-        <v>1159</v>
+        <v>1160</v>
       </c>
       <c r="B225" s="3" t="s">
         <v>38</v>
@@ -17712,34 +17715,34 @@
         <v>24</v>
       </c>
       <c r="E225" s="3" t="s">
-        <v>1160</v>
+        <v>1161</v>
       </c>
       <c r="F225" s="3" t="s">
-        <v>1149</v>
+        <v>1150</v>
       </c>
       <c r="G225" s="4">
         <v>45078</v>
       </c>
       <c r="H225" s="3" t="s">
-        <v>1161</v>
+        <v>1162</v>
       </c>
       <c r="I225" s="3" t="s">
-        <v>1151</v>
+        <v>1152</v>
       </c>
       <c r="J225" s="3" t="s">
-        <v>1151</v>
+        <v>1152</v>
       </c>
       <c r="K225" s="3" t="s">
         <v>35</v>
       </c>
       <c r="L225" s="3" t="s">
+        <v>1153</v>
+      </c>
+      <c r="M225" s="3" t="s">
         <v>1152</v>
       </c>
-      <c r="M225" s="3" t="s">
-        <v>1151</v>
-      </c>
       <c r="N225" s="3" t="s">
-        <v>1153</v>
+        <v>1154</v>
       </c>
       <c r="O225" s="3" t="s">
         <v>33</v>
@@ -17748,7 +17751,7 @@
         <v>33</v>
       </c>
       <c r="Q225" s="3" t="s">
-        <v>1154</v>
+        <v>1155</v>
       </c>
       <c r="R225" s="3"/>
       <c r="S225" s="3"/>
@@ -17756,12 +17759,12 @@
         <v>35</v>
       </c>
       <c r="U225" s="3" t="s">
-        <v>1155</v>
+        <v>1156</v>
       </c>
     </row>
     <row r="226" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A226" s="3" t="s">
-        <v>1162</v>
+        <v>1163</v>
       </c>
       <c r="B226" s="3" t="s">
         <v>22</v>
@@ -17773,7 +17776,7 @@
         <v>24</v>
       </c>
       <c r="E226" s="3" t="s">
-        <v>1163</v>
+        <v>1164</v>
       </c>
       <c r="F226" s="3" t="s">
         <v>1033</v>
@@ -17782,10 +17785,10 @@
         <v>45390</v>
       </c>
       <c r="H226" s="3" t="s">
-        <v>1164</v>
+        <v>1165</v>
       </c>
       <c r="I226" s="3" t="s">
-        <v>1165</v>
+        <v>1166</v>
       </c>
       <c r="J226" s="3" t="s">
         <v>1036</v>
@@ -17826,7 +17829,7 @@
     </row>
     <row r="227" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A227" s="3" t="s">
-        <v>1166</v>
+        <v>1167</v>
       </c>
       <c r="B227" s="3" t="s">
         <v>22</v>
@@ -17838,34 +17841,34 @@
         <v>24</v>
       </c>
       <c r="E227" s="3" t="s">
-        <v>1167</v>
+        <v>1168</v>
       </c>
       <c r="F227" s="3" t="s">
-        <v>1149</v>
+        <v>1150</v>
       </c>
       <c r="G227" s="4">
         <v>45078</v>
       </c>
       <c r="H227" s="3" t="s">
-        <v>1168</v>
+        <v>1169</v>
       </c>
       <c r="I227" s="3" t="s">
-        <v>1151</v>
+        <v>1152</v>
       </c>
       <c r="J227" s="3" t="s">
-        <v>1151</v>
+        <v>1152</v>
       </c>
       <c r="K227" s="3" t="s">
         <v>35</v>
       </c>
       <c r="L227" s="3" t="s">
+        <v>1153</v>
+      </c>
+      <c r="M227" s="3" t="s">
         <v>1152</v>
       </c>
-      <c r="M227" s="3" t="s">
-        <v>1151</v>
-      </c>
       <c r="N227" s="3" t="s">
-        <v>1153</v>
+        <v>1154</v>
       </c>
       <c r="O227" s="3" t="s">
         <v>33</v>
@@ -17874,7 +17877,7 @@
         <v>33</v>
       </c>
       <c r="Q227" s="3" t="s">
-        <v>1154</v>
+        <v>1155</v>
       </c>
       <c r="R227" s="3"/>
       <c r="S227" s="3"/>
@@ -17882,12 +17885,12 @@
         <v>35</v>
       </c>
       <c r="U227" s="3" t="s">
-        <v>1155</v>
+        <v>1156</v>
       </c>
     </row>
     <row r="228" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A228" s="3" t="s">
-        <v>1169</v>
+        <v>1170</v>
       </c>
       <c r="B228" s="3" t="s">
         <v>22</v>
@@ -17899,34 +17902,34 @@
         <v>24</v>
       </c>
       <c r="E228" s="3" t="s">
-        <v>1170</v>
+        <v>1171</v>
       </c>
       <c r="F228" s="3" t="s">
-        <v>1149</v>
+        <v>1150</v>
       </c>
       <c r="G228" s="4">
         <v>45078</v>
       </c>
       <c r="H228" s="3" t="s">
-        <v>1171</v>
+        <v>1172</v>
       </c>
       <c r="I228" s="3" t="s">
-        <v>1172</v>
+        <v>1173</v>
       </c>
       <c r="J228" s="3" t="s">
-        <v>1173</v>
+        <v>1174</v>
       </c>
       <c r="K228" s="3" t="s">
         <v>35</v>
       </c>
       <c r="L228" s="3" t="s">
-        <v>1152</v>
+        <v>1153</v>
       </c>
       <c r="M228" s="3" t="s">
-        <v>1174</v>
+        <v>1175</v>
       </c>
       <c r="N228" s="3" t="s">
-        <v>1153</v>
+        <v>1154</v>
       </c>
       <c r="O228" s="3" t="s">
         <v>33</v>
@@ -17935,7 +17938,7 @@
         <v>33</v>
       </c>
       <c r="Q228" s="3" t="s">
-        <v>1154</v>
+        <v>1155</v>
       </c>
       <c r="R228" s="3"/>
       <c r="S228" s="3"/>
@@ -17943,12 +17946,12 @@
         <v>35</v>
       </c>
       <c r="U228" s="3" t="s">
-        <v>1155</v>
+        <v>1156</v>
       </c>
     </row>
     <row r="229" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A229" s="3" t="s">
-        <v>1175</v>
+        <v>1176</v>
       </c>
       <c r="B229" s="3" t="s">
         <v>38</v>
@@ -17960,34 +17963,34 @@
         <v>24</v>
       </c>
       <c r="E229" s="3" t="s">
-        <v>1176</v>
+        <v>1177</v>
       </c>
       <c r="F229" s="3" t="s">
-        <v>1149</v>
+        <v>1150</v>
       </c>
       <c r="G229" s="4">
         <v>45078</v>
       </c>
       <c r="H229" s="3" t="s">
-        <v>1177</v>
+        <v>1178</v>
       </c>
       <c r="I229" s="3" t="s">
-        <v>1172</v>
+        <v>1173</v>
       </c>
       <c r="J229" s="3" t="s">
-        <v>1173</v>
+        <v>1174</v>
       </c>
       <c r="K229" s="3" t="s">
         <v>35</v>
       </c>
       <c r="L229" s="3" t="s">
-        <v>1152</v>
+        <v>1153</v>
       </c>
       <c r="M229" s="3" t="s">
-        <v>1174</v>
+        <v>1175</v>
       </c>
       <c r="N229" s="3" t="s">
-        <v>1153</v>
+        <v>1154</v>
       </c>
       <c r="O229" s="3" t="s">
         <v>33</v>
@@ -17996,7 +17999,7 @@
         <v>33</v>
       </c>
       <c r="Q229" s="3" t="s">
-        <v>1154</v>
+        <v>1155</v>
       </c>
       <c r="R229" s="3"/>
       <c r="S229" s="3"/>
@@ -18004,12 +18007,12 @@
         <v>35</v>
       </c>
       <c r="U229" s="3" t="s">
-        <v>1155</v>
+        <v>1156</v>
       </c>
     </row>
     <row r="230" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A230" s="3" t="s">
-        <v>1178</v>
+        <v>1179</v>
       </c>
       <c r="B230" s="3" t="s">
         <v>22</v>
@@ -18021,7 +18024,7 @@
         <v>41</v>
       </c>
       <c r="E230" s="3" t="s">
-        <v>1179</v>
+        <v>1180</v>
       </c>
       <c r="F230" s="3" t="s">
         <v>43</v>
@@ -18030,22 +18033,22 @@
         <v>45412</v>
       </c>
       <c r="H230" s="3" t="s">
-        <v>1180</v>
+        <v>1181</v>
       </c>
       <c r="I230" s="3" t="s">
-        <v>1181</v>
+        <v>1182</v>
       </c>
       <c r="J230" s="3" t="s">
-        <v>1182</v>
+        <v>1183</v>
       </c>
       <c r="K230" s="3" t="s">
-        <v>1183</v>
+        <v>1184</v>
       </c>
       <c r="L230" s="3" t="s">
-        <v>1184</v>
+        <v>1185</v>
       </c>
       <c r="M230" s="3" t="s">
-        <v>1185</v>
+        <v>1186</v>
       </c>
       <c r="N230" s="3" t="s">
         <v>50</v>
@@ -18057,7 +18060,7 @@
         <v>33</v>
       </c>
       <c r="Q230" s="3" t="s">
-        <v>1186</v>
+        <v>1187</v>
       </c>
       <c r="R230" s="3"/>
       <c r="S230" s="3"/>
@@ -18065,12 +18068,12 @@
         <v>35</v>
       </c>
       <c r="U230" s="3" t="s">
-        <v>1187</v>
+        <v>1188</v>
       </c>
     </row>
     <row r="231" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A231" s="3" t="s">
-        <v>1188</v>
+        <v>1189</v>
       </c>
       <c r="B231" s="3" t="s">
         <v>38</v>
@@ -18082,7 +18085,7 @@
         <v>41</v>
       </c>
       <c r="E231" s="3" t="s">
-        <v>1189</v>
+        <v>1190</v>
       </c>
       <c r="F231" s="3" t="s">
         <v>43</v>
@@ -18091,22 +18094,22 @@
         <v>45412</v>
       </c>
       <c r="H231" s="3" t="s">
+        <v>1182</v>
+      </c>
+      <c r="I231" s="3" t="s">
         <v>1181</v>
       </c>
-      <c r="I231" s="3" t="s">
-        <v>1180</v>
-      </c>
       <c r="J231" s="3" t="s">
-        <v>1182</v>
+        <v>1183</v>
       </c>
       <c r="K231" s="3" t="s">
-        <v>1183</v>
+        <v>1184</v>
       </c>
       <c r="L231" s="3" t="s">
-        <v>1184</v>
+        <v>1185</v>
       </c>
       <c r="M231" s="3" t="s">
-        <v>1185</v>
+        <v>1186</v>
       </c>
       <c r="N231" s="3" t="s">
         <v>50</v>
@@ -18118,7 +18121,7 @@
         <v>33</v>
       </c>
       <c r="Q231" s="3" t="s">
-        <v>1186</v>
+        <v>1187</v>
       </c>
       <c r="R231" s="3"/>
       <c r="S231" s="3"/>
@@ -18126,7 +18129,7 @@
         <v>35</v>
       </c>
       <c r="U231" s="3" t="s">
-        <v>1187</v>
+        <v>1188</v>
       </c>
     </row>
   </sheetData>
@@ -18145,66 +18148,66 @@
   <sheetData>
     <row r="1" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>1190</v>
+        <v>1191</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>1191</v>
+        <v>1192</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>1192</v>
+        <v>1193</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>1193</v>
+        <v>1194</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>1194</v>
+        <v>1195</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>1195</v>
+        <v>1196</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>1196</v>
+        <v>1197</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>1197</v>
+        <v>1198</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>1198</v>
+        <v>1199</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>1199</v>
+        <v>1200</v>
       </c>
       <c r="K1" s="2" t="s">
         <v>20</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>1200</v>
+        <v>1201</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>1201</v>
+        <v>1202</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>1202</v>
+        <v>1203</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>1203</v>
+        <v>1204</v>
       </c>
       <c r="P1" s="2" t="s">
-        <v>1204</v>
+        <v>1205</v>
       </c>
       <c r="Q1" s="2" t="s">
-        <v>1205</v>
+        <v>1206</v>
       </c>
       <c r="R1" s="2" t="s">
-        <v>1206</v>
+        <v>1207</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C2" s="5" t="b">
         <v>0</v>
@@ -18257,10 +18260,10 @@
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C3" s="5" t="b">
         <v>0</v>
@@ -18313,10 +18316,10 @@
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C4" s="5" t="b">
         <v>0</v>
@@ -18369,10 +18372,10 @@
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C5" s="5" t="b">
         <v>0</v>
@@ -18425,10 +18428,10 @@
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C6" s="5" t="b">
         <v>0</v>
@@ -18481,10 +18484,10 @@
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C7" s="5" t="b">
         <v>0</v>
@@ -18537,10 +18540,10 @@
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C8" s="5" t="b">
         <v>0</v>
@@ -18593,10 +18596,10 @@
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C9" s="5" t="b">
         <v>0</v>
@@ -18649,10 +18652,10 @@
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C10" s="5" t="b">
         <v>0</v>
@@ -18705,10 +18708,10 @@
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C11" s="5" t="b">
         <v>0</v>
@@ -18761,10 +18764,10 @@
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C12" s="5" t="b">
         <v>0</v>
@@ -18817,10 +18820,10 @@
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C13" s="5" t="b">
         <v>0</v>
@@ -18873,10 +18876,10 @@
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C14" s="5" t="b">
         <v>0</v>
@@ -18929,10 +18932,10 @@
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C15" s="5" t="b">
         <v>0</v>
@@ -18985,10 +18988,10 @@
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C16" s="5" t="b">
         <v>0</v>
@@ -19041,10 +19044,10 @@
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C17" s="5" t="b">
         <v>0</v>
@@ -19097,10 +19100,10 @@
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C18" s="5" t="b">
         <v>0</v>
@@ -19153,10 +19156,10 @@
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C19" s="5" t="b">
         <v>0</v>
@@ -19209,10 +19212,10 @@
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C20" s="5" t="b">
         <v>0</v>
@@ -19265,10 +19268,10 @@
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C21" s="5" t="b">
         <v>0</v>
@@ -19321,10 +19324,10 @@
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C22" s="5" t="b">
         <v>0</v>
@@ -19377,10 +19380,10 @@
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C23" s="5" t="b">
         <v>0</v>
@@ -19433,10 +19436,10 @@
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C24" s="5" t="b">
         <v>0</v>
@@ -19489,10 +19492,10 @@
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C25" s="5" t="b">
         <v>0</v>
@@ -19545,10 +19548,10 @@
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C26" s="5" t="b">
         <v>0</v>
@@ -19601,10 +19604,10 @@
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C27" s="5" t="b">
         <v>0</v>
@@ -19657,10 +19660,10 @@
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C28" s="5" t="b">
         <v>0</v>
@@ -19713,10 +19716,10 @@
     </row>
     <row r="29" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C29" s="5" t="b">
         <v>0</v>
@@ -19769,10 +19772,10 @@
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C30" s="5" t="b">
         <v>0</v>
@@ -19825,10 +19828,10 @@
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C31" s="5" t="b">
         <v>0</v>
@@ -19881,10 +19884,10 @@
     </row>
     <row r="32" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C32" s="5" t="b">
         <v>0</v>
@@ -19937,10 +19940,10 @@
     </row>
     <row r="33" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C33" s="5" t="b">
         <v>0</v>
@@ -19993,10 +19996,10 @@
     </row>
     <row r="34" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C34" s="5" t="b">
         <v>0</v>
@@ -20049,10 +20052,10 @@
     </row>
     <row r="35" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C35" s="5" t="b">
         <v>0</v>
@@ -20105,10 +20108,10 @@
     </row>
     <row r="36" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C36" s="5" t="b">
         <v>0</v>
@@ -20161,10 +20164,10 @@
     </row>
     <row r="37" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C37" s="5" t="b">
         <v>0</v>
@@ -20217,10 +20220,10 @@
     </row>
     <row r="38" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C38" s="5" t="b">
         <v>0</v>
@@ -20273,10 +20276,10 @@
     </row>
     <row r="39" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C39" s="5" t="b">
         <v>0</v>
@@ -20329,10 +20332,10 @@
     </row>
     <row r="40" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C40" s="5" t="b">
         <v>0</v>
@@ -20385,10 +20388,10 @@
     </row>
     <row r="41" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C41" s="5" t="b">
         <v>0</v>
@@ -20441,10 +20444,10 @@
     </row>
     <row r="42" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C42" s="5" t="b">
         <v>0</v>
@@ -20497,10 +20500,10 @@
     </row>
     <row r="43" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C43" s="5" t="b">
         <v>0</v>
@@ -20553,10 +20556,10 @@
     </row>
     <row r="44" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C44" s="5" t="b">
         <v>0</v>
@@ -20609,10 +20612,10 @@
     </row>
     <row r="45" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C45" s="5" t="b">
         <v>0</v>
@@ -20665,10 +20668,10 @@
     </row>
     <row r="46" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C46" s="5" t="b">
         <v>0</v>
@@ -20721,10 +20724,10 @@
     </row>
     <row r="47" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C47" s="5" t="b">
         <v>0</v>
@@ -20777,10 +20780,10 @@
     </row>
     <row r="48" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C48" s="5" t="b">
         <v>0</v>
@@ -20833,10 +20836,10 @@
     </row>
     <row r="49" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C49" s="5" t="b">
         <v>0</v>
@@ -20889,10 +20892,10 @@
     </row>
     <row r="50" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C50" s="5" t="b">
         <v>0</v>
@@ -20945,10 +20948,10 @@
     </row>
     <row r="51" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C51" s="5" t="b">
         <v>0</v>
@@ -21001,10 +21004,10 @@
     </row>
     <row r="52" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C52" s="5" t="b">
         <v>0</v>
@@ -21057,10 +21060,10 @@
     </row>
     <row r="53" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C53" s="5" t="b">
         <v>0</v>
@@ -21113,10 +21116,10 @@
     </row>
     <row r="54" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C54" s="5" t="b">
         <v>0</v>
@@ -21169,10 +21172,10 @@
     </row>
     <row r="55" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C55" s="5" t="b">
         <v>0</v>
@@ -21225,10 +21228,10 @@
     </row>
     <row r="56" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C56" s="5" t="b">
         <v>0</v>
@@ -21281,10 +21284,10 @@
     </row>
     <row r="57" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C57" s="5" t="b">
         <v>0</v>
@@ -21337,10 +21340,10 @@
     </row>
     <row r="58" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C58" s="5" t="b">
         <v>0</v>
@@ -21393,10 +21396,10 @@
     </row>
     <row r="59" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C59" s="5" t="b">
         <v>0</v>
@@ -21449,10 +21452,10 @@
     </row>
     <row r="60" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C60" s="5" t="b">
         <v>0</v>
@@ -21505,10 +21508,10 @@
     </row>
     <row r="61" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C61" s="5" t="b">
         <v>0</v>
@@ -21561,10 +21564,10 @@
     </row>
     <row r="62" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C62" s="5" t="b">
         <v>0</v>
@@ -21617,10 +21620,10 @@
     </row>
     <row r="63" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C63" s="5" t="b">
         <v>0</v>
@@ -21673,10 +21676,10 @@
     </row>
     <row r="64" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C64" s="5" t="b">
         <v>0</v>
@@ -21729,10 +21732,10 @@
     </row>
     <row r="65" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A65" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C65" s="5" t="b">
         <v>0</v>
@@ -21785,10 +21788,10 @@
     </row>
     <row r="66" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A66" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C66" s="5" t="b">
         <v>0</v>
@@ -21841,10 +21844,10 @@
     </row>
     <row r="67" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A67" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C67" s="5" t="b">
         <v>0</v>
@@ -21897,10 +21900,10 @@
     </row>
     <row r="68" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A68" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C68" s="5" t="b">
         <v>0</v>
@@ -21953,10 +21956,10 @@
     </row>
     <row r="69" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A69" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C69" s="5" t="b">
         <v>0</v>
@@ -22009,10 +22012,10 @@
     </row>
     <row r="70" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A70" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C70" s="5" t="b">
         <v>0</v>
@@ -22065,10 +22068,10 @@
     </row>
     <row r="71" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A71" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C71" s="5" t="b">
         <v>0</v>
@@ -22121,10 +22124,10 @@
     </row>
     <row r="72" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A72" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C72" s="5" t="b">
         <v>0</v>
@@ -22177,10 +22180,10 @@
     </row>
     <row r="73" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A73" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C73" s="5" t="b">
         <v>0</v>
@@ -22233,10 +22236,10 @@
     </row>
     <row r="74" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A74" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C74" s="5" t="b">
         <v>0</v>
@@ -22289,10 +22292,10 @@
     </row>
     <row r="75" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A75" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C75" s="5" t="b">
         <v>0</v>
@@ -22345,10 +22348,10 @@
     </row>
     <row r="76" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A76" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C76" s="5" t="b">
         <v>0</v>
@@ -22401,10 +22404,10 @@
     </row>
     <row r="77" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A77" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C77" s="5" t="b">
         <v>0</v>
@@ -22457,10 +22460,10 @@
     </row>
     <row r="78" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A78" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C78" s="5" t="b">
         <v>0</v>
@@ -22513,10 +22516,10 @@
     </row>
     <row r="79" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A79" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C79" s="5" t="b">
         <v>0</v>
@@ -22569,10 +22572,10 @@
     </row>
     <row r="80" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A80" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C80" s="5" t="b">
         <v>0</v>
@@ -22625,10 +22628,10 @@
     </row>
     <row r="81" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A81" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B81" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C81" s="5" t="b">
         <v>0</v>
@@ -22681,10 +22684,10 @@
     </row>
     <row r="82" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A82" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B82" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C82" s="5" t="b">
         <v>0</v>
@@ -22737,10 +22740,10 @@
     </row>
     <row r="83" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A83" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C83" s="5" t="b">
         <v>0</v>
@@ -22793,10 +22796,10 @@
     </row>
     <row r="84" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A84" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B84" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C84" s="5" t="b">
         <v>0</v>
@@ -22849,10 +22852,10 @@
     </row>
     <row r="85" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A85" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C85" s="5" t="b">
         <v>0</v>
@@ -22905,10 +22908,10 @@
     </row>
     <row r="86" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A86" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B86" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C86" s="5" t="b">
         <v>0</v>
@@ -22961,10 +22964,10 @@
     </row>
     <row r="87" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A87" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B87" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C87" s="5" t="b">
         <v>0</v>
@@ -23017,10 +23020,10 @@
     </row>
     <row r="88" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A88" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B88" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C88" s="5" t="b">
         <v>0</v>
@@ -23073,10 +23076,10 @@
     </row>
     <row r="89" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A89" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C89" s="5" t="b">
         <v>0</v>
@@ -23129,10 +23132,10 @@
     </row>
     <row r="90" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A90" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B90" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C90" s="5" t="b">
         <v>0</v>
@@ -23185,10 +23188,10 @@
     </row>
     <row r="91" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A91" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B91" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C91" s="5" t="b">
         <v>0</v>
@@ -23241,10 +23244,10 @@
     </row>
     <row r="92" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A92" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B92" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C92" s="5" t="b">
         <v>0</v>
@@ -23297,10 +23300,10 @@
     </row>
     <row r="93" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A93" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B93" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C93" s="5" t="b">
         <v>0</v>
@@ -23353,10 +23356,10 @@
     </row>
     <row r="94" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A94" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B94" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C94" s="5" t="b">
         <v>0</v>
@@ -23409,10 +23412,10 @@
     </row>
     <row r="95" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A95" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B95" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C95" s="5" t="b">
         <v>0</v>
@@ -23465,10 +23468,10 @@
     </row>
     <row r="96" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A96" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B96" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C96" s="5" t="b">
         <v>0</v>
@@ -23521,10 +23524,10 @@
     </row>
     <row r="97" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A97" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B97" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C97" s="5" t="b">
         <v>0</v>
@@ -23577,10 +23580,10 @@
     </row>
     <row r="98" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A98" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B98" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C98" s="5" t="b">
         <v>0</v>
@@ -23633,10 +23636,10 @@
     </row>
     <row r="99" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A99" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B99" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C99" s="5" t="b">
         <v>0</v>
@@ -23689,10 +23692,10 @@
     </row>
     <row r="100" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A100" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B100" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C100" s="5" t="b">
         <v>0</v>
@@ -23745,10 +23748,10 @@
     </row>
     <row r="101" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A101" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B101" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C101" s="5" t="b">
         <v>0</v>
@@ -23801,10 +23804,10 @@
     </row>
     <row r="102" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A102" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B102" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C102" s="5" t="b">
         <v>0</v>
@@ -23857,10 +23860,10 @@
     </row>
     <row r="103" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A103" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B103" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C103" s="5" t="b">
         <v>0</v>
@@ -23913,10 +23916,10 @@
     </row>
     <row r="104" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A104" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B104" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C104" s="5" t="b">
         <v>0</v>
@@ -23969,10 +23972,10 @@
     </row>
     <row r="105" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A105" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B105" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C105" s="5" t="b">
         <v>0</v>
@@ -24025,10 +24028,10 @@
     </row>
     <row r="106" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A106" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B106" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C106" s="5" t="b">
         <v>0</v>
@@ -24081,10 +24084,10 @@
     </row>
     <row r="107" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A107" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B107" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C107" s="5" t="b">
         <v>0</v>
@@ -24137,10 +24140,10 @@
     </row>
     <row r="108" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A108" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B108" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C108" s="5" t="b">
         <v>0</v>
@@ -24193,10 +24196,10 @@
     </row>
     <row r="109" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A109" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B109" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C109" s="5" t="b">
         <v>0</v>
@@ -24249,10 +24252,10 @@
     </row>
     <row r="110" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A110" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B110" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C110" s="5" t="b">
         <v>0</v>
@@ -24305,10 +24308,10 @@
     </row>
     <row r="111" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A111" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B111" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C111" s="5" t="b">
         <v>0</v>
@@ -24361,10 +24364,10 @@
     </row>
     <row r="112" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A112" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B112" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C112" s="5" t="b">
         <v>0</v>
@@ -24417,10 +24420,10 @@
     </row>
     <row r="113" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A113" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B113" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C113" s="5" t="b">
         <v>0</v>
@@ -24473,10 +24476,10 @@
     </row>
     <row r="114" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A114" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B114" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C114" s="5" t="b">
         <v>0</v>
@@ -24529,10 +24532,10 @@
     </row>
     <row r="115" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A115" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B115" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C115" s="5" t="b">
         <v>0</v>
@@ -24585,10 +24588,10 @@
     </row>
     <row r="116" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A116" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B116" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C116" s="5" t="b">
         <v>0</v>
@@ -24641,10 +24644,10 @@
     </row>
     <row r="117" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A117" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B117" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C117" s="5" t="b">
         <v>0</v>
@@ -24697,10 +24700,10 @@
     </row>
     <row r="118" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A118" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B118" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C118" s="5" t="b">
         <v>0</v>
@@ -24753,10 +24756,10 @@
     </row>
     <row r="119" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A119" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B119" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C119" s="5" t="b">
         <v>0</v>
@@ -24809,10 +24812,10 @@
     </row>
     <row r="120" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A120" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B120" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C120" s="5" t="b">
         <v>0</v>
@@ -24865,10 +24868,10 @@
     </row>
     <row r="121" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A121" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B121" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C121" s="5" t="b">
         <v>0</v>
@@ -24921,10 +24924,10 @@
     </row>
     <row r="122" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A122" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B122" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C122" s="5" t="b">
         <v>0</v>
@@ -24977,10 +24980,10 @@
     </row>
     <row r="123" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A123" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B123" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C123" s="5" t="b">
         <v>0</v>
@@ -25033,10 +25036,10 @@
     </row>
     <row r="124" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A124" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B124" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C124" s="5" t="b">
         <v>0</v>
@@ -25089,10 +25092,10 @@
     </row>
     <row r="125" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A125" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B125" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C125" s="5" t="b">
         <v>0</v>
@@ -25145,10 +25148,10 @@
     </row>
     <row r="126" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A126" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B126" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C126" s="5" t="b">
         <v>0</v>
@@ -25201,10 +25204,10 @@
     </row>
     <row r="127" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A127" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B127" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C127" s="5" t="b">
         <v>0</v>
@@ -25257,10 +25260,10 @@
     </row>
     <row r="128" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A128" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B128" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C128" s="5" t="b">
         <v>0</v>
@@ -25313,10 +25316,10 @@
     </row>
     <row r="129" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A129" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B129" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C129" s="5" t="b">
         <v>0</v>
@@ -25369,10 +25372,10 @@
     </row>
     <row r="130" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A130" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B130" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C130" s="5" t="b">
         <v>0</v>
@@ -25425,10 +25428,10 @@
     </row>
     <row r="131" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A131" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B131" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C131" s="5" t="b">
         <v>0</v>
@@ -25481,10 +25484,10 @@
     </row>
     <row r="132" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A132" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B132" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C132" s="5" t="b">
         <v>0</v>
@@ -25537,10 +25540,10 @@
     </row>
     <row r="133" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A133" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B133" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C133" s="5" t="b">
         <v>0</v>
@@ -25593,10 +25596,10 @@
     </row>
     <row r="134" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A134" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B134" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C134" s="5" t="b">
         <v>0</v>
@@ -25649,10 +25652,10 @@
     </row>
     <row r="135" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A135" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B135" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C135" s="5" t="b">
         <v>0</v>
@@ -25705,10 +25708,10 @@
     </row>
     <row r="136" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A136" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B136" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C136" s="5" t="b">
         <v>0</v>
@@ -25761,10 +25764,10 @@
     </row>
     <row r="137" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A137" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B137" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C137" s="5" t="b">
         <v>0</v>
@@ -25817,10 +25820,10 @@
     </row>
     <row r="138" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A138" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B138" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C138" s="5" t="b">
         <v>0</v>
@@ -25873,10 +25876,10 @@
     </row>
     <row r="139" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A139" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B139" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C139" s="5" t="b">
         <v>0</v>
@@ -25929,10 +25932,10 @@
     </row>
     <row r="140" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A140" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B140" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C140" s="5" t="b">
         <v>0</v>
@@ -25985,10 +25988,10 @@
     </row>
     <row r="141" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A141" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B141" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C141" s="5" t="b">
         <v>0</v>
@@ -26041,10 +26044,10 @@
     </row>
     <row r="142" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A142" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B142" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C142" s="5" t="b">
         <v>0</v>
@@ -26097,10 +26100,10 @@
     </row>
     <row r="143" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A143" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B143" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C143" s="5" t="b">
         <v>0</v>
@@ -26153,10 +26156,10 @@
     </row>
     <row r="144" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A144" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B144" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C144" s="5" t="b">
         <v>0</v>
@@ -26209,10 +26212,10 @@
     </row>
     <row r="145" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A145" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B145" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C145" s="5" t="b">
         <v>0</v>
@@ -26265,10 +26268,10 @@
     </row>
     <row r="146" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A146" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B146" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C146" s="5" t="b">
         <v>0</v>
@@ -26321,10 +26324,10 @@
     </row>
     <row r="147" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A147" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B147" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C147" s="5" t="b">
         <v>0</v>
@@ -26377,10 +26380,10 @@
     </row>
     <row r="148" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A148" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B148" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C148" s="5" t="b">
         <v>0</v>
@@ -26433,10 +26436,10 @@
     </row>
     <row r="149" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A149" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B149" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C149" s="5" t="b">
         <v>0</v>
@@ -26489,10 +26492,10 @@
     </row>
     <row r="150" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A150" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B150" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C150" s="5" t="b">
         <v>0</v>
@@ -26545,10 +26548,10 @@
     </row>
     <row r="151" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A151" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B151" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C151" s="5" t="b">
         <v>0</v>
@@ -26601,10 +26604,10 @@
     </row>
     <row r="152" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A152" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B152" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C152" s="5" t="b">
         <v>0</v>
@@ -26657,10 +26660,10 @@
     </row>
     <row r="153" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A153" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B153" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C153" s="5" t="b">
         <v>0</v>
@@ -26713,10 +26716,10 @@
     </row>
     <row r="154" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A154" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B154" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C154" s="5" t="b">
         <v>0</v>
@@ -26769,10 +26772,10 @@
     </row>
     <row r="155" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A155" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B155" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C155" s="5" t="b">
         <v>0</v>
@@ -26825,10 +26828,10 @@
     </row>
     <row r="156" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A156" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B156" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C156" s="5" t="b">
         <v>0</v>
@@ -26881,10 +26884,10 @@
     </row>
     <row r="157" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A157" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B157" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C157" s="5" t="b">
         <v>0</v>
@@ -26937,10 +26940,10 @@
     </row>
     <row r="158" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A158" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B158" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C158" s="5" t="b">
         <v>0</v>
@@ -26993,10 +26996,10 @@
     </row>
     <row r="159" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A159" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B159" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C159" s="5" t="b">
         <v>0</v>
@@ -27049,10 +27052,10 @@
     </row>
     <row r="160" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A160" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B160" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C160" s="5" t="b">
         <v>0</v>
@@ -27105,10 +27108,10 @@
     </row>
     <row r="161" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A161" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B161" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C161" s="5" t="b">
         <v>0</v>
@@ -27161,10 +27164,10 @@
     </row>
     <row r="162" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A162" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B162" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C162" s="5" t="b">
         <v>0</v>
@@ -27217,10 +27220,10 @@
     </row>
     <row r="163" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A163" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B163" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C163" s="5" t="b">
         <v>0</v>
@@ -27273,10 +27276,10 @@
     </row>
     <row r="164" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A164" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B164" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C164" s="5" t="b">
         <v>0</v>
@@ -27329,10 +27332,10 @@
     </row>
     <row r="165" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A165" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B165" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C165" s="5" t="b">
         <v>0</v>
@@ -27385,10 +27388,10 @@
     </row>
     <row r="166" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A166" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B166" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C166" s="5" t="b">
         <v>0</v>
@@ -27441,10 +27444,10 @@
     </row>
     <row r="167" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A167" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B167" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C167" s="5" t="b">
         <v>0</v>
@@ -27497,10 +27500,10 @@
     </row>
     <row r="168" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A168" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B168" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C168" s="5" t="b">
         <v>0</v>
@@ -27553,10 +27556,10 @@
     </row>
     <row r="169" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A169" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B169" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C169" s="5" t="b">
         <v>0</v>
@@ -27609,10 +27612,10 @@
     </row>
     <row r="170" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A170" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B170" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C170" s="5" t="b">
         <v>0</v>
@@ -27665,10 +27668,10 @@
     </row>
     <row r="171" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A171" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B171" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C171" s="5" t="b">
         <v>0</v>
@@ -27721,10 +27724,10 @@
     </row>
     <row r="172" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A172" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B172" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C172" s="5" t="b">
         <v>0</v>
@@ -27777,10 +27780,10 @@
     </row>
     <row r="173" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A173" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B173" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C173" s="5" t="b">
         <v>0</v>
@@ -27833,10 +27836,10 @@
     </row>
     <row r="174" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A174" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B174" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C174" s="5" t="b">
         <v>0</v>
@@ -27889,10 +27892,10 @@
     </row>
     <row r="175" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A175" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B175" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C175" s="5" t="b">
         <v>0</v>
@@ -27945,10 +27948,10 @@
     </row>
     <row r="176" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A176" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B176" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C176" s="5" t="b">
         <v>0</v>
@@ -28001,10 +28004,10 @@
     </row>
     <row r="177" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A177" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B177" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C177" s="5" t="b">
         <v>0</v>
@@ -28057,10 +28060,10 @@
     </row>
     <row r="178" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A178" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B178" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C178" s="5" t="b">
         <v>0</v>
@@ -28113,10 +28116,10 @@
     </row>
     <row r="179" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A179" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B179" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C179" s="5" t="b">
         <v>0</v>
@@ -28169,10 +28172,10 @@
     </row>
     <row r="180" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A180" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B180" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C180" s="5" t="b">
         <v>0</v>
@@ -28225,10 +28228,10 @@
     </row>
     <row r="181" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A181" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B181" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C181" s="5" t="b">
         <v>0</v>
@@ -28281,10 +28284,10 @@
     </row>
     <row r="182" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A182" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B182" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C182" s="5" t="b">
         <v>0</v>
@@ -28337,10 +28340,10 @@
     </row>
     <row r="183" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A183" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B183" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C183" s="5" t="b">
         <v>0</v>
@@ -28393,10 +28396,10 @@
     </row>
     <row r="184" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A184" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B184" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C184" s="5" t="b">
         <v>0</v>
@@ -28449,10 +28452,10 @@
     </row>
     <row r="185" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A185" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B185" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C185" s="5" t="b">
         <v>0</v>
@@ -28505,10 +28508,10 @@
     </row>
     <row r="186" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A186" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B186" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C186" s="5" t="b">
         <v>0</v>
@@ -28561,10 +28564,10 @@
     </row>
     <row r="187" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A187" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B187" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C187" s="5" t="b">
         <v>0</v>
@@ -28617,10 +28620,10 @@
     </row>
     <row r="188" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A188" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B188" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C188" s="5" t="b">
         <v>0</v>
@@ -28673,10 +28676,10 @@
     </row>
     <row r="189" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A189" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B189" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C189" s="5" t="b">
         <v>0</v>
@@ -28729,10 +28732,10 @@
     </row>
     <row r="190" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A190" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B190" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C190" s="5" t="b">
         <v>0</v>
@@ -28785,10 +28788,10 @@
     </row>
     <row r="191" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A191" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B191" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C191" s="5" t="b">
         <v>0</v>
@@ -28841,10 +28844,10 @@
     </row>
     <row r="192" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A192" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B192" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C192" s="5" t="b">
         <v>0</v>
@@ -28897,10 +28900,10 @@
     </row>
     <row r="193" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A193" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B193" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C193" s="5" t="b">
         <v>0</v>
@@ -28953,10 +28956,10 @@
     </row>
     <row r="194" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A194" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B194" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C194" s="5" t="b">
         <v>0</v>
@@ -29009,10 +29012,10 @@
     </row>
     <row r="195" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A195" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B195" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C195" s="5" t="b">
         <v>0</v>
@@ -29065,10 +29068,10 @@
     </row>
     <row r="196" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A196" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B196" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C196" s="5" t="b">
         <v>0</v>
@@ -29121,10 +29124,10 @@
     </row>
     <row r="197" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A197" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B197" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C197" s="5" t="b">
         <v>0</v>
@@ -29177,10 +29180,10 @@
     </row>
     <row r="198" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A198" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B198" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C198" s="5" t="b">
         <v>0</v>
@@ -29233,10 +29236,10 @@
     </row>
     <row r="199" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A199" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B199" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C199" s="5" t="b">
         <v>0</v>
@@ -29289,10 +29292,10 @@
     </row>
     <row r="200" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A200" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B200" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C200" s="5" t="b">
         <v>0</v>
@@ -29345,10 +29348,10 @@
     </row>
     <row r="201" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A201" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B201" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C201" s="5" t="b">
         <v>0</v>
@@ -29401,10 +29404,10 @@
     </row>
     <row r="202" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A202" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B202" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C202" s="5" t="b">
         <v>0</v>
@@ -29457,10 +29460,10 @@
     </row>
     <row r="203" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A203" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B203" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C203" s="5" t="b">
         <v>0</v>
@@ -29513,10 +29516,10 @@
     </row>
     <row r="204" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A204" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B204" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C204" s="5" t="b">
         <v>0</v>
@@ -29569,10 +29572,10 @@
     </row>
     <row r="205" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A205" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B205" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C205" s="5" t="b">
         <v>0</v>
@@ -29625,10 +29628,10 @@
     </row>
     <row r="206" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A206" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B206" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C206" s="5" t="b">
         <v>0</v>
@@ -29681,10 +29684,10 @@
     </row>
     <row r="207" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A207" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B207" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C207" s="5" t="b">
         <v>0</v>
@@ -29737,10 +29740,10 @@
     </row>
     <row r="208" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A208" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B208" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C208" s="5" t="b">
         <v>0</v>
@@ -29793,10 +29796,10 @@
     </row>
     <row r="209" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A209" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B209" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C209" s="5" t="b">
         <v>0</v>
@@ -29849,10 +29852,10 @@
     </row>
     <row r="210" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A210" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B210" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C210" s="5" t="b">
         <v>0</v>
@@ -29905,10 +29908,10 @@
     </row>
     <row r="211" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A211" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B211" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C211" s="5" t="b">
         <v>0</v>
@@ -29961,10 +29964,10 @@
     </row>
     <row r="212" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A212" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B212" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C212" s="5" t="b">
         <v>0</v>
@@ -30017,10 +30020,10 @@
     </row>
     <row r="213" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A213" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B213" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C213" s="5" t="b">
         <v>0</v>
@@ -30073,10 +30076,10 @@
     </row>
     <row r="214" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A214" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B214" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C214" s="5" t="b">
         <v>0</v>
@@ -30129,10 +30132,10 @@
     </row>
     <row r="215" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A215" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B215" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C215" s="5" t="b">
         <v>0</v>
@@ -30185,10 +30188,10 @@
     </row>
     <row r="216" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A216" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B216" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C216" s="5" t="b">
         <v>0</v>
@@ -30241,10 +30244,10 @@
     </row>
     <row r="217" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A217" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B217" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C217" s="5" t="b">
         <v>0</v>
@@ -30297,10 +30300,10 @@
     </row>
     <row r="218" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A218" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B218" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C218" s="5" t="b">
         <v>0</v>
@@ -30353,10 +30356,10 @@
     </row>
     <row r="219" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A219" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B219" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C219" s="5" t="b">
         <v>0</v>
@@ -30409,10 +30412,10 @@
     </row>
     <row r="220" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A220" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B220" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C220" s="5" t="b">
         <v>0</v>
@@ -30465,10 +30468,10 @@
     </row>
     <row r="221" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A221" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B221" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C221" s="5" t="b">
         <v>0</v>
@@ -30521,10 +30524,10 @@
     </row>
     <row r="222" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A222" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B222" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C222" s="5" t="b">
         <v>0</v>
@@ -30577,10 +30580,10 @@
     </row>
     <row r="223" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A223" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B223" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C223" s="5" t="b">
         <v>0</v>
@@ -30633,10 +30636,10 @@
     </row>
     <row r="224" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A224" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B224" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C224" s="5" t="b">
         <v>0</v>
@@ -30689,10 +30692,10 @@
     </row>
     <row r="225" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A225" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B225" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C225" s="5" t="b">
         <v>0</v>
@@ -30745,10 +30748,10 @@
     </row>
     <row r="226" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A226" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B226" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C226" s="5" t="b">
         <v>0</v>
@@ -30801,10 +30804,10 @@
     </row>
     <row r="227" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A227" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B227" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C227" s="5" t="b">
         <v>0</v>
@@ -30857,10 +30860,10 @@
     </row>
     <row r="228" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A228" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B228" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C228" s="5" t="b">
         <v>0</v>
@@ -30913,10 +30916,10 @@
     </row>
     <row r="229" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A229" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B229" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C229" s="5" t="b">
         <v>0</v>
@@ -30969,10 +30972,10 @@
     </row>
     <row r="230" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A230" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B230" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C230" s="5" t="b">
         <v>0</v>
@@ -31025,10 +31028,10 @@
     </row>
     <row r="231" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A231" s="3" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B231" s="3" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C231" s="5" t="b">
         <v>0</v>

</xml_diff>

<commit_message>
generated all the reports on 2024-07-30
</commit_message>
<xml_diff>
--- a/report/merged_configurations.xlsx
+++ b/report/merged_configurations.xlsx
@@ -158,7 +158,7 @@
     <t>Charter Schuldbeheer</t>
   </si>
   <si>
-    <t>https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-schuldbeheer/standaardenregister/charter/Charter OSLO_Schuldbeheer.pdf</t>
+    <t>https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-schuldbeheer/standaardenregister/charter/Projectcharter_OSLOSchuldbeheer.pdf</t>
   </si>
   <si>
     <t>[{"name":"Presentatie Business Werkgroep - 4 maart 2024","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-schuldbeheer/standaardenregister/presentations/20240304_BusinessWorkshop_Presentatie_OSLOSchuldbeheer.pptx"},{"name":"Presentatie Werksessie Lokale Besturen - 16 april 2024","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-schuldbeheer/standaardenregister/presentations/20240416_PresentatieWerksessieLokaleBesturen.pptx"},{"name":"Presentatie Eerste Thematische Werkgroep - 16 mei 2024","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-schuldbeheer/standaardenregister/presentations/20240516_ThematicWorkshop1_Powerpoint_OSLOSchuldbeheer.pptx"},{"name":"Presentatie Tweede Thematische Werkgroep - 11 juni 2024","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-schuldbeheer/standaardenregister/presentations/20240611_ThematicWorkshop2_Powerpoint_OSLOSchuldbeheer.pptx"},{"name":"Presentatie Derde Thematische Werkgroep - 2 juli 2024","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-schuldbeheer/standaardenregister/presentations/20240702_ThematicWorkshop3_Powerpoint_OSLOSchuldbeheer.pptx"}]</t>
@@ -170,7 +170,7 @@
     <t>OSLOthema-schuldbeheer</t>
   </si>
   <si>
-    <t>{"name":"Charter Schuldbeheer","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-schuldbeheer/standaardenregister/charter/Charter OSLO_Schuldbeheer.pdf"}</t>
+    <t>{"name":"Charter Schuldbeheer","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-schuldbeheer/standaardenregister/charter/Projectcharter_OSLOSchuldbeheer.pdf"}</t>
   </si>
   <si>
     <t>Vocabularium Schuldbeheer</t>

</xml_diff>

<commit_message>
generated all the reports on 2024-08-01
</commit_message>
<xml_diff>
--- a/report/merged_configurations.xlsx
+++ b/report/merged_configurations.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4652" uniqueCount="1225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4652" uniqueCount="1226">
   <si>
     <t>title</t>
   </si>
@@ -3197,7 +3197,7 @@
     <t>ap-or-voc-slimmestadsdistributie.md</t>
   </si>
   <si>
-    <t>[{"name":"Slimme Stadsdistributie - ApplicatieProfiel","resourceReference":"https://data.vlaanderen.be/doc/applicatieprofiel/slimme-stadsdistributie"},{"name":"Slimme Stadsdistributie - Vocabularium","resourceReference":"https://data.vlaanderen.be/ns/slimme-stadsdistributie"}]</t>
+    <t>[{"name":"Slimme Stadsdistributie - ApplicatieProfiel","resourceReference":"https://data.vlaanderen.be/doc/applicatieprofiel/slimme-stadsdistributie"}]</t>
   </si>
   <si>
     <t>[{"name":"Verslag Business werkgroep - 11 januari 2023","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-slimmeStadsdistributie/standaardenregister/reports/Verslag_Business_werkgroep_-_11_januari_2023.pdf"},{"name":"Verslag Eerste Thematische werkgroep - 8 februari 2023","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-slimmeStadsdistributie/standaardenregister/reports/Verslag_Thematische_Werkgroep_1_-_8_februari_2023.pdf"}]</t>
@@ -3222,6 +3222,9 @@
   </si>
   <si>
     <t>Vocabularium OSLO Slimme Stadsdistributie</t>
+  </si>
+  <si>
+    <t>[{"name":"Slimme Stadsdistributie - Vocabularium","resourceReference":"https://data.vlaanderen.be/ns/slimme-stadsdistributie"}]</t>
   </si>
   <si>
     <t>Applicatieprofiel Mobiliteitsbudget</t>
@@ -16919,7 +16922,7 @@
         <v>45489</v>
       </c>
       <c r="H211" s="3" t="s">
-        <v>1061</v>
+        <v>1070</v>
       </c>
       <c r="I211" s="3" t="s">
         <v>28</v>
@@ -16959,7 +16962,7 @@
     </row>
     <row r="212" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A212" s="3" t="s">
-        <v>1070</v>
+        <v>1071</v>
       </c>
       <c r="B212" s="3" t="s">
         <v>22</v>
@@ -16971,7 +16974,7 @@
         <v>24</v>
       </c>
       <c r="E212" s="3" t="s">
-        <v>1071</v>
+        <v>1072</v>
       </c>
       <c r="F212" s="3" t="s">
         <v>43</v>
@@ -16980,25 +16983,25 @@
         <v>44875</v>
       </c>
       <c r="H212" s="3" t="s">
-        <v>1072</v>
+        <v>1073</v>
       </c>
       <c r="I212" s="3" t="s">
-        <v>1073</v>
+        <v>1074</v>
       </c>
       <c r="J212" s="3" t="s">
-        <v>1074</v>
+        <v>1075</v>
       </c>
       <c r="K212" s="3" t="s">
-        <v>1075</v>
+        <v>1076</v>
       </c>
       <c r="L212" s="3" t="s">
-        <v>1076</v>
+        <v>1077</v>
       </c>
       <c r="M212" s="3" t="s">
-        <v>1077</v>
+        <v>1078</v>
       </c>
       <c r="N212" s="3" t="s">
-        <v>1078</v>
+        <v>1079</v>
       </c>
       <c r="O212" s="3" t="s">
         <v>33</v>
@@ -17007,7 +17010,7 @@
         <v>33</v>
       </c>
       <c r="Q212" s="3" t="s">
-        <v>1079</v>
+        <v>1080</v>
       </c>
       <c r="R212" s="4">
         <v>45461</v>
@@ -17017,12 +17020,12 @@
         <v>35</v>
       </c>
       <c r="U212" s="3" t="s">
-        <v>1080</v>
+        <v>1081</v>
       </c>
     </row>
     <row r="213" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A213" s="3" t="s">
-        <v>1081</v>
+        <v>1082</v>
       </c>
       <c r="B213" s="3" t="s">
         <v>38</v>
@@ -17034,7 +17037,7 @@
         <v>24</v>
       </c>
       <c r="E213" s="3" t="s">
-        <v>1082</v>
+        <v>1083</v>
       </c>
       <c r="F213" s="3" t="s">
         <v>43</v>
@@ -17043,25 +17046,25 @@
         <v>44875</v>
       </c>
       <c r="H213" s="3" t="s">
+        <v>1074</v>
+      </c>
+      <c r="I213" s="3" t="s">
         <v>1073</v>
       </c>
-      <c r="I213" s="3" t="s">
-        <v>1072</v>
-      </c>
       <c r="J213" s="3" t="s">
-        <v>1074</v>
+        <v>1075</v>
       </c>
       <c r="K213" s="3" t="s">
-        <v>1075</v>
+        <v>1076</v>
       </c>
       <c r="L213" s="3" t="s">
-        <v>1076</v>
+        <v>1077</v>
       </c>
       <c r="M213" s="3" t="s">
-        <v>1077</v>
+        <v>1078</v>
       </c>
       <c r="N213" s="3" t="s">
-        <v>1078</v>
+        <v>1079</v>
       </c>
       <c r="O213" s="3" t="s">
         <v>33</v>
@@ -17070,7 +17073,7 @@
         <v>33</v>
       </c>
       <c r="Q213" s="3" t="s">
-        <v>1079</v>
+        <v>1080</v>
       </c>
       <c r="R213" s="4">
         <v>45461</v>
@@ -17080,12 +17083,12 @@
         <v>35</v>
       </c>
       <c r="U213" s="3" t="s">
-        <v>1080</v>
+        <v>1081</v>
       </c>
     </row>
     <row r="214" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A214" s="3" t="s">
-        <v>1083</v>
+        <v>1084</v>
       </c>
       <c r="B214" s="3" t="s">
         <v>780</v>
@@ -17106,22 +17109,22 @@
         <v>45131</v>
       </c>
       <c r="H214" s="3" t="s">
-        <v>1084</v>
+        <v>1085</v>
       </c>
       <c r="I214" s="3" t="s">
         <v>28</v>
       </c>
       <c r="J214" s="3" t="s">
-        <v>1085</v>
+        <v>1086</v>
       </c>
       <c r="K214" s="3" t="s">
         <v>30</v>
       </c>
       <c r="L214" s="3" t="s">
-        <v>1086</v>
+        <v>1087</v>
       </c>
       <c r="M214" s="3" t="s">
-        <v>1087</v>
+        <v>1088</v>
       </c>
       <c r="N214" s="4">
         <v>44873</v>
@@ -17133,7 +17136,7 @@
         <v>33</v>
       </c>
       <c r="Q214" s="3" t="s">
-        <v>1088</v>
+        <v>1089</v>
       </c>
       <c r="R214" s="3"/>
       <c r="S214" s="3"/>
@@ -17141,12 +17144,12 @@
         <v>35</v>
       </c>
       <c r="U214" s="3" t="s">
-        <v>1089</v>
+        <v>1090</v>
       </c>
     </row>
     <row r="215" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A215" s="3" t="s">
-        <v>1090</v>
+        <v>1091</v>
       </c>
       <c r="B215" s="3" t="s">
         <v>38</v>
@@ -17167,22 +17170,22 @@
         <v>45131</v>
       </c>
       <c r="H215" s="3" t="s">
-        <v>1091</v>
+        <v>1092</v>
       </c>
       <c r="I215" s="3" t="s">
         <v>28</v>
       </c>
       <c r="J215" s="3" t="s">
-        <v>1085</v>
+        <v>1086</v>
       </c>
       <c r="K215" s="3" t="s">
         <v>30</v>
       </c>
       <c r="L215" s="3" t="s">
-        <v>1086</v>
+        <v>1087</v>
       </c>
       <c r="M215" s="3" t="s">
-        <v>1087</v>
+        <v>1088</v>
       </c>
       <c r="N215" s="4">
         <v>44873</v>
@@ -17194,7 +17197,7 @@
         <v>33</v>
       </c>
       <c r="Q215" s="3" t="s">
-        <v>1088</v>
+        <v>1089</v>
       </c>
       <c r="R215" s="3"/>
       <c r="S215" s="3"/>
@@ -17202,12 +17205,12 @@
         <v>35</v>
       </c>
       <c r="U215" s="3" t="s">
-        <v>1089</v>
+        <v>1090</v>
       </c>
     </row>
     <row r="216" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A216" s="3" t="s">
-        <v>1092</v>
+        <v>1093</v>
       </c>
       <c r="B216" s="3" t="s">
         <v>22</v>
@@ -17219,7 +17222,7 @@
         <v>24</v>
       </c>
       <c r="E216" s="3" t="s">
-        <v>1093</v>
+        <v>1094</v>
       </c>
       <c r="F216" s="3" t="s">
         <v>547</v>
@@ -17228,34 +17231,34 @@
         <v>45330</v>
       </c>
       <c r="H216" s="3" t="s">
-        <v>1094</v>
+        <v>1095</v>
       </c>
       <c r="I216" s="3" t="s">
-        <v>1095</v>
+        <v>1096</v>
       </c>
       <c r="J216" s="3" t="s">
-        <v>1096</v>
+        <v>1097</v>
       </c>
       <c r="K216" s="3" t="s">
-        <v>1097</v>
+        <v>1098</v>
       </c>
       <c r="L216" s="3" t="s">
-        <v>1098</v>
+        <v>1099</v>
       </c>
       <c r="M216" s="3" t="s">
-        <v>1099</v>
+        <v>1100</v>
       </c>
       <c r="N216" s="3" t="s">
-        <v>1100</v>
+        <v>1101</v>
       </c>
       <c r="O216" s="3" t="s">
-        <v>1101</v>
+        <v>1102</v>
       </c>
       <c r="P216" s="3" t="s">
         <v>33</v>
       </c>
       <c r="Q216" s="3" t="s">
-        <v>1102</v>
+        <v>1103</v>
       </c>
       <c r="R216" s="3"/>
       <c r="S216" s="3"/>
@@ -17263,12 +17266,12 @@
         <v>35</v>
       </c>
       <c r="U216" s="3" t="s">
-        <v>1103</v>
+        <v>1104</v>
       </c>
     </row>
     <row r="217" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A217" s="3" t="s">
-        <v>1104</v>
+        <v>1105</v>
       </c>
       <c r="B217" s="3" t="s">
         <v>38</v>
@@ -17280,7 +17283,7 @@
         <v>24</v>
       </c>
       <c r="E217" s="3" t="s">
-        <v>1105</v>
+        <v>1106</v>
       </c>
       <c r="F217" s="3" t="s">
         <v>547</v>
@@ -17289,34 +17292,34 @@
         <v>45330</v>
       </c>
       <c r="H217" s="3" t="s">
+        <v>1096</v>
+      </c>
+      <c r="I217" s="3" t="s">
         <v>1095</v>
       </c>
-      <c r="I217" s="3" t="s">
-        <v>1094</v>
-      </c>
       <c r="J217" s="3" t="s">
-        <v>1096</v>
+        <v>1097</v>
       </c>
       <c r="K217" s="3" t="s">
-        <v>1097</v>
+        <v>1098</v>
       </c>
       <c r="L217" s="3" t="s">
-        <v>1098</v>
+        <v>1099</v>
       </c>
       <c r="M217" s="3" t="s">
-        <v>1099</v>
+        <v>1100</v>
       </c>
       <c r="N217" s="3" t="s">
-        <v>1100</v>
+        <v>1101</v>
       </c>
       <c r="O217" s="3" t="s">
-        <v>1101</v>
+        <v>1102</v>
       </c>
       <c r="P217" s="3" t="s">
         <v>33</v>
       </c>
       <c r="Q217" s="3" t="s">
-        <v>1102</v>
+        <v>1103</v>
       </c>
       <c r="R217" s="3"/>
       <c r="S217" s="3"/>
@@ -17324,15 +17327,15 @@
         <v>35</v>
       </c>
       <c r="U217" s="3" t="s">
-        <v>1103</v>
+        <v>1104</v>
       </c>
     </row>
     <row r="218" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A218" s="3" t="s">
-        <v>1106</v>
+        <v>1107</v>
       </c>
       <c r="B218" s="3" t="s">
-        <v>1107</v>
+        <v>1108</v>
       </c>
       <c r="C218" s="3" t="s">
         <v>23</v>
@@ -17350,28 +17353,28 @@
         <v>45308</v>
       </c>
       <c r="H218" s="3" t="s">
-        <v>1108</v>
+        <v>1109</v>
       </c>
       <c r="I218" s="3" t="s">
         <v>28</v>
       </c>
       <c r="J218" s="3" t="s">
-        <v>1109</v>
+        <v>1110</v>
       </c>
       <c r="K218" s="3" t="s">
-        <v>1110</v>
+        <v>1111</v>
       </c>
       <c r="L218" s="3" t="s">
-        <v>1111</v>
+        <v>1112</v>
       </c>
       <c r="M218" s="3" t="s">
-        <v>1112</v>
+        <v>1113</v>
       </c>
       <c r="N218" s="3"/>
       <c r="O218" s="3"/>
       <c r="P218" s="3"/>
       <c r="Q218" s="3" t="s">
-        <v>1113</v>
+        <v>1114</v>
       </c>
       <c r="R218" s="3"/>
       <c r="S218" s="3"/>
@@ -17379,15 +17382,15 @@
         <v>35</v>
       </c>
       <c r="U218" s="3" t="s">
-        <v>1114</v>
+        <v>1115</v>
       </c>
     </row>
     <row r="219" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A219" s="3" t="s">
-        <v>1115</v>
+        <v>1116</v>
       </c>
       <c r="B219" s="3" t="s">
-        <v>1116</v>
+        <v>1117</v>
       </c>
       <c r="C219" s="3" t="s">
         <v>23</v>
@@ -17405,28 +17408,28 @@
         <v>45308</v>
       </c>
       <c r="H219" s="3" t="s">
-        <v>1117</v>
+        <v>1118</v>
       </c>
       <c r="I219" s="3" t="s">
         <v>28</v>
       </c>
       <c r="J219" s="3" t="s">
-        <v>1109</v>
+        <v>1110</v>
       </c>
       <c r="K219" s="3" t="s">
-        <v>1110</v>
+        <v>1111</v>
       </c>
       <c r="L219" s="3" t="s">
-        <v>1111</v>
+        <v>1112</v>
       </c>
       <c r="M219" s="3" t="s">
-        <v>1112</v>
+        <v>1113</v>
       </c>
       <c r="N219" s="3"/>
       <c r="O219" s="3"/>
       <c r="P219" s="3"/>
       <c r="Q219" s="3" t="s">
-        <v>1113</v>
+        <v>1114</v>
       </c>
       <c r="R219" s="3"/>
       <c r="S219" s="3"/>
@@ -17434,12 +17437,12 @@
         <v>35</v>
       </c>
       <c r="U219" s="3" t="s">
-        <v>1114</v>
+        <v>1115</v>
       </c>
     </row>
     <row r="220" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A220" s="3" t="s">
-        <v>1118</v>
+        <v>1119</v>
       </c>
       <c r="B220" s="3" t="s">
         <v>22</v>
@@ -17451,7 +17454,7 @@
         <v>24</v>
       </c>
       <c r="E220" s="3" t="s">
-        <v>1119</v>
+        <v>1120</v>
       </c>
       <c r="F220" s="3" t="s">
         <v>1035</v>
@@ -17460,25 +17463,25 @@
         <v>45323</v>
       </c>
       <c r="H220" s="3" t="s">
-        <v>1120</v>
+        <v>1121</v>
       </c>
       <c r="I220" s="3" t="s">
-        <v>1121</v>
+        <v>1122</v>
       </c>
       <c r="J220" s="3" t="s">
-        <v>1122</v>
+        <v>1123</v>
       </c>
       <c r="K220" s="3" t="s">
-        <v>1123</v>
+        <v>1124</v>
       </c>
       <c r="L220" s="3" t="s">
-        <v>1124</v>
+        <v>1125</v>
       </c>
       <c r="M220" s="3" t="s">
-        <v>1125</v>
+        <v>1126</v>
       </c>
       <c r="N220" s="3" t="s">
-        <v>1126</v>
+        <v>1127</v>
       </c>
       <c r="O220" s="3" t="s">
         <v>33</v>
@@ -17487,7 +17490,7 @@
         <v>33</v>
       </c>
       <c r="Q220" s="3" t="s">
-        <v>1127</v>
+        <v>1128</v>
       </c>
       <c r="R220" s="3"/>
       <c r="S220" s="3"/>
@@ -17495,12 +17498,12 @@
         <v>35</v>
       </c>
       <c r="U220" s="3" t="s">
-        <v>1128</v>
+        <v>1129</v>
       </c>
     </row>
     <row r="221" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A221" s="3" t="s">
-        <v>1129</v>
+        <v>1130</v>
       </c>
       <c r="B221" s="3" t="s">
         <v>38</v>
@@ -17512,7 +17515,7 @@
         <v>24</v>
       </c>
       <c r="E221" s="3" t="s">
-        <v>1130</v>
+        <v>1131</v>
       </c>
       <c r="F221" s="3" t="s">
         <v>1035</v>
@@ -17521,25 +17524,25 @@
         <v>45323</v>
       </c>
       <c r="H221" s="3" t="s">
-        <v>1131</v>
+        <v>1132</v>
       </c>
       <c r="I221" s="3" t="s">
-        <v>1132</v>
+        <v>1133</v>
       </c>
       <c r="J221" s="3" t="s">
-        <v>1133</v>
+        <v>1134</v>
       </c>
       <c r="K221" s="3" t="s">
-        <v>1123</v>
+        <v>1124</v>
       </c>
       <c r="L221" s="3" t="s">
-        <v>1124</v>
+        <v>1125</v>
       </c>
       <c r="M221" s="3" t="s">
-        <v>1125</v>
+        <v>1126</v>
       </c>
       <c r="N221" s="3" t="s">
-        <v>1126</v>
+        <v>1127</v>
       </c>
       <c r="O221" s="3" t="s">
         <v>33</v>
@@ -17548,7 +17551,7 @@
         <v>33</v>
       </c>
       <c r="Q221" s="3" t="s">
-        <v>1127</v>
+        <v>1128</v>
       </c>
       <c r="R221" s="3"/>
       <c r="S221" s="3"/>
@@ -17556,12 +17559,12 @@
         <v>35</v>
       </c>
       <c r="U221" s="3" t="s">
-        <v>1128</v>
+        <v>1129</v>
       </c>
     </row>
     <row r="222" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A222" s="3" t="s">
-        <v>1134</v>
+        <v>1135</v>
       </c>
       <c r="B222" s="3" t="s">
         <v>38</v>
@@ -17573,7 +17576,7 @@
         <v>24</v>
       </c>
       <c r="E222" s="3" t="s">
-        <v>1135</v>
+        <v>1136</v>
       </c>
       <c r="F222" s="3" t="s">
         <v>1035</v>
@@ -17582,25 +17585,25 @@
         <v>45393</v>
       </c>
       <c r="H222" s="3" t="s">
-        <v>1136</v>
+        <v>1137</v>
       </c>
       <c r="I222" s="3" t="s">
-        <v>1137</v>
+        <v>1138</v>
       </c>
       <c r="J222" s="3" t="s">
-        <v>1138</v>
+        <v>1139</v>
       </c>
       <c r="K222" s="3" t="s">
-        <v>1123</v>
+        <v>1124</v>
       </c>
       <c r="L222" s="3" t="s">
-        <v>1124</v>
+        <v>1125</v>
       </c>
       <c r="M222" s="3" t="s">
-        <v>1125</v>
+        <v>1126</v>
       </c>
       <c r="N222" s="3" t="s">
-        <v>1126</v>
+        <v>1127</v>
       </c>
       <c r="O222" s="3" t="s">
         <v>33</v>
@@ -17609,7 +17612,7 @@
         <v>33</v>
       </c>
       <c r="Q222" s="3" t="s">
-        <v>1127</v>
+        <v>1128</v>
       </c>
       <c r="R222" s="3"/>
       <c r="S222" s="3"/>
@@ -17617,12 +17620,12 @@
         <v>35</v>
       </c>
       <c r="U222" s="3" t="s">
-        <v>1128</v>
+        <v>1129</v>
       </c>
     </row>
     <row r="223" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A223" s="3" t="s">
-        <v>1139</v>
+        <v>1140</v>
       </c>
       <c r="B223" s="3" t="s">
         <v>22</v>
@@ -17634,7 +17637,7 @@
         <v>24</v>
       </c>
       <c r="E223" s="3" t="s">
-        <v>1140</v>
+        <v>1141</v>
       </c>
       <c r="F223" s="3" t="s">
         <v>43</v>
@@ -17643,25 +17646,25 @@
         <v>45370</v>
       </c>
       <c r="H223" s="3" t="s">
-        <v>1141</v>
+        <v>1142</v>
       </c>
       <c r="I223" s="3" t="s">
-        <v>1142</v>
+        <v>1143</v>
       </c>
       <c r="J223" s="3" t="s">
-        <v>1143</v>
+        <v>1144</v>
       </c>
       <c r="K223" s="3" t="s">
-        <v>1144</v>
+        <v>1145</v>
       </c>
       <c r="L223" s="3" t="s">
-        <v>1145</v>
+        <v>1146</v>
       </c>
       <c r="M223" s="3" t="s">
-        <v>1146</v>
+        <v>1147</v>
       </c>
       <c r="N223" s="3" t="s">
-        <v>1147</v>
+        <v>1148</v>
       </c>
       <c r="O223" s="3" t="s">
         <v>33</v>
@@ -17670,7 +17673,7 @@
         <v>33</v>
       </c>
       <c r="Q223" s="3" t="s">
-        <v>1148</v>
+        <v>1149</v>
       </c>
       <c r="R223" s="4">
         <v>45467</v>
@@ -17680,12 +17683,12 @@
         <v>35</v>
       </c>
       <c r="U223" s="3" t="s">
-        <v>1149</v>
+        <v>1150</v>
       </c>
     </row>
     <row r="224" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A224" s="3" t="s">
-        <v>1150</v>
+        <v>1151</v>
       </c>
       <c r="B224" s="3" t="s">
         <v>38</v>
@@ -17697,7 +17700,7 @@
         <v>24</v>
       </c>
       <c r="E224" s="3" t="s">
-        <v>1140</v>
+        <v>1141</v>
       </c>
       <c r="F224" s="3" t="s">
         <v>43</v>
@@ -17706,25 +17709,25 @@
         <v>45370</v>
       </c>
       <c r="H224" s="3" t="s">
+        <v>1143</v>
+      </c>
+      <c r="I224" s="3" t="s">
         <v>1142</v>
       </c>
-      <c r="I224" s="3" t="s">
-        <v>1141</v>
-      </c>
       <c r="J224" s="3" t="s">
-        <v>1143</v>
+        <v>1144</v>
       </c>
       <c r="K224" s="3" t="s">
-        <v>1144</v>
+        <v>1145</v>
       </c>
       <c r="L224" s="3" t="s">
-        <v>1145</v>
+        <v>1146</v>
       </c>
       <c r="M224" s="3" t="s">
-        <v>1146</v>
+        <v>1147</v>
       </c>
       <c r="N224" s="3" t="s">
-        <v>1147</v>
+        <v>1148</v>
       </c>
       <c r="O224" s="3" t="s">
         <v>33</v>
@@ -17733,7 +17736,7 @@
         <v>33</v>
       </c>
       <c r="Q224" s="3" t="s">
-        <v>1148</v>
+        <v>1149</v>
       </c>
       <c r="R224" s="4">
         <v>45461</v>
@@ -17743,12 +17746,12 @@
         <v>35</v>
       </c>
       <c r="U224" s="3" t="s">
-        <v>1149</v>
+        <v>1150</v>
       </c>
     </row>
     <row r="225" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A225" s="3" t="s">
-        <v>1151</v>
+        <v>1152</v>
       </c>
       <c r="B225" s="3" t="s">
         <v>38</v>
@@ -17760,34 +17763,34 @@
         <v>24</v>
       </c>
       <c r="E225" s="3" t="s">
-        <v>1152</v>
+        <v>1153</v>
       </c>
       <c r="F225" s="3" t="s">
-        <v>1153</v>
+        <v>1154</v>
       </c>
       <c r="G225" s="4">
         <v>45078</v>
       </c>
       <c r="H225" s="3" t="s">
-        <v>1154</v>
+        <v>1155</v>
       </c>
       <c r="I225" s="3" t="s">
-        <v>1155</v>
+        <v>1156</v>
       </c>
       <c r="J225" s="3" t="s">
-        <v>1155</v>
+        <v>1156</v>
       </c>
       <c r="K225" s="3" t="s">
         <v>35</v>
       </c>
       <c r="L225" s="3" t="s">
+        <v>1157</v>
+      </c>
+      <c r="M225" s="3" t="s">
         <v>1156</v>
       </c>
-      <c r="M225" s="3" t="s">
-        <v>1155</v>
-      </c>
       <c r="N225" s="3" t="s">
-        <v>1157</v>
+        <v>1158</v>
       </c>
       <c r="O225" s="3" t="s">
         <v>33</v>
@@ -17796,7 +17799,7 @@
         <v>33</v>
       </c>
       <c r="Q225" s="3" t="s">
-        <v>1158</v>
+        <v>1159</v>
       </c>
       <c r="R225" s="3"/>
       <c r="S225" s="3"/>
@@ -17804,12 +17807,12 @@
         <v>35</v>
       </c>
       <c r="U225" s="3" t="s">
-        <v>1159</v>
+        <v>1160</v>
       </c>
     </row>
     <row r="226" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A226" s="3" t="s">
-        <v>1160</v>
+        <v>1161</v>
       </c>
       <c r="B226" s="3" t="s">
         <v>22</v>
@@ -17821,34 +17824,34 @@
         <v>24</v>
       </c>
       <c r="E226" s="3" t="s">
-        <v>1161</v>
+        <v>1162</v>
       </c>
       <c r="F226" s="3" t="s">
-        <v>1153</v>
+        <v>1154</v>
       </c>
       <c r="G226" s="4">
         <v>45078</v>
       </c>
       <c r="H226" s="3" t="s">
-        <v>1162</v>
+        <v>1163</v>
       </c>
       <c r="I226" s="3" t="s">
-        <v>1155</v>
+        <v>1156</v>
       </c>
       <c r="J226" s="3" t="s">
-        <v>1155</v>
+        <v>1156</v>
       </c>
       <c r="K226" s="3" t="s">
         <v>35</v>
       </c>
       <c r="L226" s="3" t="s">
+        <v>1157</v>
+      </c>
+      <c r="M226" s="3" t="s">
         <v>1156</v>
       </c>
-      <c r="M226" s="3" t="s">
-        <v>1155</v>
-      </c>
       <c r="N226" s="3" t="s">
-        <v>1157</v>
+        <v>1158</v>
       </c>
       <c r="O226" s="3" t="s">
         <v>33</v>
@@ -17857,7 +17860,7 @@
         <v>33</v>
       </c>
       <c r="Q226" s="3" t="s">
-        <v>1158</v>
+        <v>1159</v>
       </c>
       <c r="R226" s="3"/>
       <c r="S226" s="3"/>
@@ -17865,12 +17868,12 @@
         <v>35</v>
       </c>
       <c r="U226" s="3" t="s">
-        <v>1159</v>
+        <v>1160</v>
       </c>
     </row>
     <row r="227" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A227" s="3" t="s">
-        <v>1163</v>
+        <v>1164</v>
       </c>
       <c r="B227" s="3" t="s">
         <v>38</v>
@@ -17882,34 +17885,34 @@
         <v>24</v>
       </c>
       <c r="E227" s="3" t="s">
-        <v>1164</v>
+        <v>1165</v>
       </c>
       <c r="F227" s="3" t="s">
-        <v>1153</v>
+        <v>1154</v>
       </c>
       <c r="G227" s="4">
         <v>45078</v>
       </c>
       <c r="H227" s="3" t="s">
-        <v>1165</v>
+        <v>1166</v>
       </c>
       <c r="I227" s="3" t="s">
-        <v>1155</v>
+        <v>1156</v>
       </c>
       <c r="J227" s="3" t="s">
-        <v>1155</v>
+        <v>1156</v>
       </c>
       <c r="K227" s="3" t="s">
         <v>35</v>
       </c>
       <c r="L227" s="3" t="s">
+        <v>1157</v>
+      </c>
+      <c r="M227" s="3" t="s">
         <v>1156</v>
       </c>
-      <c r="M227" s="3" t="s">
-        <v>1155</v>
-      </c>
       <c r="N227" s="3" t="s">
-        <v>1157</v>
+        <v>1158</v>
       </c>
       <c r="O227" s="3" t="s">
         <v>33</v>
@@ -17918,7 +17921,7 @@
         <v>33</v>
       </c>
       <c r="Q227" s="3" t="s">
-        <v>1158</v>
+        <v>1159</v>
       </c>
       <c r="R227" s="3"/>
       <c r="S227" s="3"/>
@@ -17926,12 +17929,12 @@
         <v>35</v>
       </c>
       <c r="U227" s="3" t="s">
-        <v>1159</v>
+        <v>1160</v>
       </c>
     </row>
     <row r="228" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A228" s="3" t="s">
-        <v>1166</v>
+        <v>1167</v>
       </c>
       <c r="B228" s="3" t="s">
         <v>22</v>
@@ -17943,7 +17946,7 @@
         <v>24</v>
       </c>
       <c r="E228" s="3" t="s">
-        <v>1167</v>
+        <v>1168</v>
       </c>
       <c r="F228" s="3" t="s">
         <v>1035</v>
@@ -17952,10 +17955,10 @@
         <v>45390</v>
       </c>
       <c r="H228" s="3" t="s">
-        <v>1168</v>
+        <v>1169</v>
       </c>
       <c r="I228" s="3" t="s">
-        <v>1169</v>
+        <v>1170</v>
       </c>
       <c r="J228" s="3" t="s">
         <v>1038</v>
@@ -17996,7 +17999,7 @@
     </row>
     <row r="229" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A229" s="3" t="s">
-        <v>1170</v>
+        <v>1171</v>
       </c>
       <c r="B229" s="3" t="s">
         <v>22</v>
@@ -18008,34 +18011,34 @@
         <v>24</v>
       </c>
       <c r="E229" s="3" t="s">
-        <v>1171</v>
+        <v>1172</v>
       </c>
       <c r="F229" s="3" t="s">
-        <v>1153</v>
+        <v>1154</v>
       </c>
       <c r="G229" s="4">
         <v>45078</v>
       </c>
       <c r="H229" s="3" t="s">
-        <v>1172</v>
+        <v>1173</v>
       </c>
       <c r="I229" s="3" t="s">
-        <v>1155</v>
+        <v>1156</v>
       </c>
       <c r="J229" s="3" t="s">
-        <v>1155</v>
+        <v>1156</v>
       </c>
       <c r="K229" s="3" t="s">
         <v>35</v>
       </c>
       <c r="L229" s="3" t="s">
+        <v>1157</v>
+      </c>
+      <c r="M229" s="3" t="s">
         <v>1156</v>
       </c>
-      <c r="M229" s="3" t="s">
-        <v>1155</v>
-      </c>
       <c r="N229" s="3" t="s">
-        <v>1157</v>
+        <v>1158</v>
       </c>
       <c r="O229" s="3" t="s">
         <v>33</v>
@@ -18044,7 +18047,7 @@
         <v>33</v>
       </c>
       <c r="Q229" s="3" t="s">
-        <v>1158</v>
+        <v>1159</v>
       </c>
       <c r="R229" s="3"/>
       <c r="S229" s="3"/>
@@ -18052,12 +18055,12 @@
         <v>35</v>
       </c>
       <c r="U229" s="3" t="s">
-        <v>1159</v>
+        <v>1160</v>
       </c>
     </row>
     <row r="230" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A230" s="3" t="s">
-        <v>1173</v>
+        <v>1174</v>
       </c>
       <c r="B230" s="3" t="s">
         <v>22</v>
@@ -18069,34 +18072,34 @@
         <v>24</v>
       </c>
       <c r="E230" s="3" t="s">
-        <v>1174</v>
+        <v>1175</v>
       </c>
       <c r="F230" s="3" t="s">
-        <v>1153</v>
+        <v>1154</v>
       </c>
       <c r="G230" s="4">
         <v>45078</v>
       </c>
       <c r="H230" s="3" t="s">
-        <v>1175</v>
+        <v>1176</v>
       </c>
       <c r="I230" s="3" t="s">
-        <v>1176</v>
+        <v>1177</v>
       </c>
       <c r="J230" s="3" t="s">
-        <v>1177</v>
+        <v>1178</v>
       </c>
       <c r="K230" s="3" t="s">
         <v>35</v>
       </c>
       <c r="L230" s="3" t="s">
-        <v>1156</v>
+        <v>1157</v>
       </c>
       <c r="M230" s="3" t="s">
-        <v>1178</v>
+        <v>1179</v>
       </c>
       <c r="N230" s="3" t="s">
-        <v>1157</v>
+        <v>1158</v>
       </c>
       <c r="O230" s="3" t="s">
         <v>33</v>
@@ -18105,7 +18108,7 @@
         <v>33</v>
       </c>
       <c r="Q230" s="3" t="s">
-        <v>1158</v>
+        <v>1159</v>
       </c>
       <c r="R230" s="3"/>
       <c r="S230" s="3"/>
@@ -18113,12 +18116,12 @@
         <v>35</v>
       </c>
       <c r="U230" s="3" t="s">
-        <v>1159</v>
+        <v>1160</v>
       </c>
     </row>
     <row r="231" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A231" s="3" t="s">
-        <v>1179</v>
+        <v>1180</v>
       </c>
       <c r="B231" s="3" t="s">
         <v>38</v>
@@ -18130,34 +18133,34 @@
         <v>24</v>
       </c>
       <c r="E231" s="3" t="s">
-        <v>1180</v>
+        <v>1181</v>
       </c>
       <c r="F231" s="3" t="s">
-        <v>1153</v>
+        <v>1154</v>
       </c>
       <c r="G231" s="4">
         <v>45078</v>
       </c>
       <c r="H231" s="3" t="s">
-        <v>1181</v>
+        <v>1182</v>
       </c>
       <c r="I231" s="3" t="s">
-        <v>1176</v>
+        <v>1177</v>
       </c>
       <c r="J231" s="3" t="s">
-        <v>1177</v>
+        <v>1178</v>
       </c>
       <c r="K231" s="3" t="s">
         <v>35</v>
       </c>
       <c r="L231" s="3" t="s">
-        <v>1156</v>
+        <v>1157</v>
       </c>
       <c r="M231" s="3" t="s">
-        <v>1178</v>
+        <v>1179</v>
       </c>
       <c r="N231" s="3" t="s">
-        <v>1157</v>
+        <v>1158</v>
       </c>
       <c r="O231" s="3" t="s">
         <v>33</v>
@@ -18166,7 +18169,7 @@
         <v>33</v>
       </c>
       <c r="Q231" s="3" t="s">
-        <v>1158</v>
+        <v>1159</v>
       </c>
       <c r="R231" s="3"/>
       <c r="S231" s="3"/>
@@ -18174,12 +18177,12 @@
         <v>35</v>
       </c>
       <c r="U231" s="3" t="s">
-        <v>1159</v>
+        <v>1160</v>
       </c>
     </row>
     <row r="232" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A232" s="3" t="s">
-        <v>1182</v>
+        <v>1183</v>
       </c>
       <c r="B232" s="3" t="s">
         <v>22</v>
@@ -18191,7 +18194,7 @@
         <v>41</v>
       </c>
       <c r="E232" s="3" t="s">
-        <v>1183</v>
+        <v>1184</v>
       </c>
       <c r="F232" s="3" t="s">
         <v>43</v>
@@ -18200,22 +18203,22 @@
         <v>45412</v>
       </c>
       <c r="H232" s="3" t="s">
-        <v>1184</v>
+        <v>1185</v>
       </c>
       <c r="I232" s="3" t="s">
-        <v>1185</v>
+        <v>1186</v>
       </c>
       <c r="J232" s="3" t="s">
-        <v>1186</v>
+        <v>1187</v>
       </c>
       <c r="K232" s="3" t="s">
-        <v>1187</v>
+        <v>1188</v>
       </c>
       <c r="L232" s="3" t="s">
-        <v>1188</v>
+        <v>1189</v>
       </c>
       <c r="M232" s="3" t="s">
-        <v>1189</v>
+        <v>1190</v>
       </c>
       <c r="N232" s="3" t="s">
         <v>50</v>
@@ -18227,7 +18230,7 @@
         <v>33</v>
       </c>
       <c r="Q232" s="3" t="s">
-        <v>1190</v>
+        <v>1191</v>
       </c>
       <c r="R232" s="3"/>
       <c r="S232" s="3"/>
@@ -18235,12 +18238,12 @@
         <v>35</v>
       </c>
       <c r="U232" s="3" t="s">
-        <v>1191</v>
+        <v>1192</v>
       </c>
     </row>
     <row r="233" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A233" s="3" t="s">
-        <v>1192</v>
+        <v>1193</v>
       </c>
       <c r="B233" s="3" t="s">
         <v>38</v>
@@ -18252,7 +18255,7 @@
         <v>41</v>
       </c>
       <c r="E233" s="3" t="s">
-        <v>1193</v>
+        <v>1194</v>
       </c>
       <c r="F233" s="3" t="s">
         <v>43</v>
@@ -18261,22 +18264,22 @@
         <v>45412</v>
       </c>
       <c r="H233" s="3" t="s">
+        <v>1186</v>
+      </c>
+      <c r="I233" s="3" t="s">
         <v>1185</v>
       </c>
-      <c r="I233" s="3" t="s">
-        <v>1184</v>
-      </c>
       <c r="J233" s="3" t="s">
-        <v>1186</v>
+        <v>1187</v>
       </c>
       <c r="K233" s="3" t="s">
-        <v>1187</v>
+        <v>1188</v>
       </c>
       <c r="L233" s="3" t="s">
-        <v>1188</v>
+        <v>1189</v>
       </c>
       <c r="M233" s="3" t="s">
-        <v>1189</v>
+        <v>1190</v>
       </c>
       <c r="N233" s="3" t="s">
         <v>50</v>
@@ -18288,7 +18291,7 @@
         <v>33</v>
       </c>
       <c r="Q233" s="3" t="s">
-        <v>1190</v>
+        <v>1191</v>
       </c>
       <c r="R233" s="3"/>
       <c r="S233" s="3"/>
@@ -18296,24 +18299,24 @@
         <v>35</v>
       </c>
       <c r="U233" s="3" t="s">
-        <v>1191</v>
+        <v>1192</v>
       </c>
     </row>
     <row r="234" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A234" s="3" t="s">
-        <v>1194</v>
+        <v>1195</v>
       </c>
       <c r="B234" s="3" t="s">
         <v>22</v>
       </c>
       <c r="C234" s="3" t="s">
-        <v>1195</v>
+        <v>1196</v>
       </c>
       <c r="D234" s="3" t="s">
         <v>41</v>
       </c>
       <c r="E234" s="3" t="s">
-        <v>1196</v>
+        <v>1197</v>
       </c>
       <c r="F234" s="3" t="s">
         <v>43</v>
@@ -18322,25 +18325,25 @@
         <v>45503</v>
       </c>
       <c r="H234" s="3" t="s">
-        <v>1197</v>
+        <v>1198</v>
       </c>
       <c r="I234" s="3" t="s">
-        <v>1198</v>
+        <v>1199</v>
       </c>
       <c r="J234" s="3" t="s">
-        <v>1199</v>
+        <v>1200</v>
       </c>
       <c r="K234" s="3" t="s">
-        <v>1200</v>
+        <v>1201</v>
       </c>
       <c r="L234" s="3" t="s">
-        <v>1201</v>
+        <v>1202</v>
       </c>
       <c r="M234" s="3" t="s">
-        <v>1202</v>
+        <v>1203</v>
       </c>
       <c r="N234" s="3" t="s">
-        <v>1203</v>
+        <v>1204</v>
       </c>
       <c r="O234" s="3" t="s">
         <v>33</v>
@@ -18357,24 +18360,24 @@
         <v>35</v>
       </c>
       <c r="U234" s="3" t="s">
-        <v>1204</v>
+        <v>1205</v>
       </c>
     </row>
     <row r="235" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A235" s="3" t="s">
-        <v>1205</v>
+        <v>1206</v>
       </c>
       <c r="B235" s="3" t="s">
         <v>38</v>
       </c>
       <c r="C235" s="3" t="s">
-        <v>1195</v>
+        <v>1196</v>
       </c>
       <c r="D235" s="3" t="s">
         <v>41</v>
       </c>
       <c r="E235" s="3" t="s">
-        <v>1196</v>
+        <v>1197</v>
       </c>
       <c r="F235" s="3" t="s">
         <v>43</v>
@@ -18383,25 +18386,25 @@
         <v>45503</v>
       </c>
       <c r="H235" s="3" t="s">
-        <v>1198</v>
+        <v>1199</v>
       </c>
       <c r="I235" s="3" t="s">
-        <v>1198</v>
+        <v>1199</v>
       </c>
       <c r="J235" s="3" t="s">
-        <v>1199</v>
+        <v>1200</v>
       </c>
       <c r="K235" s="3" t="s">
-        <v>1200</v>
+        <v>1201</v>
       </c>
       <c r="L235" s="3" t="s">
-        <v>1201</v>
+        <v>1202</v>
       </c>
       <c r="M235" s="3" t="s">
-        <v>1202</v>
+        <v>1203</v>
       </c>
       <c r="N235" s="3" t="s">
-        <v>1203</v>
+        <v>1204</v>
       </c>
       <c r="O235" s="3" t="s">
         <v>33</v>
@@ -18418,7 +18421,7 @@
         <v>35</v>
       </c>
       <c r="U235" s="3" t="s">
-        <v>1204</v>
+        <v>1205</v>
       </c>
     </row>
   </sheetData>
@@ -18437,66 +18440,66 @@
   <sheetData>
     <row r="1" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>1206</v>
+        <v>1207</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>1209</v>
+        <v>1210</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>1210</v>
+        <v>1211</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>1211</v>
+        <v>1212</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>1212</v>
+        <v>1213</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>1213</v>
+        <v>1214</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>1214</v>
+        <v>1215</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>1215</v>
+        <v>1216</v>
       </c>
       <c r="K1" s="2" t="s">
         <v>20</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>1216</v>
+        <v>1217</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>1217</v>
+        <v>1218</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>1218</v>
+        <v>1219</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>1219</v>
+        <v>1220</v>
       </c>
       <c r="P1" s="2" t="s">
-        <v>1220</v>
+        <v>1221</v>
       </c>
       <c r="Q1" s="2" t="s">
-        <v>1221</v>
+        <v>1222</v>
       </c>
       <c r="R1" s="2" t="s">
-        <v>1222</v>
+        <v>1223</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C2" s="5" t="b">
         <v>0</v>
@@ -18549,10 +18552,10 @@
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C3" s="5" t="b">
         <v>0</v>
@@ -18605,10 +18608,10 @@
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C4" s="5" t="b">
         <v>0</v>
@@ -18661,10 +18664,10 @@
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C5" s="5" t="b">
         <v>0</v>
@@ -18717,10 +18720,10 @@
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C6" s="5" t="b">
         <v>0</v>
@@ -18773,10 +18776,10 @@
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C7" s="5" t="b">
         <v>0</v>
@@ -18829,10 +18832,10 @@
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C8" s="5" t="b">
         <v>0</v>
@@ -18885,10 +18888,10 @@
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C9" s="5" t="b">
         <v>0</v>
@@ -18941,10 +18944,10 @@
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C10" s="5" t="b">
         <v>0</v>
@@ -18997,10 +19000,10 @@
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C11" s="5" t="b">
         <v>0</v>
@@ -19053,10 +19056,10 @@
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C12" s="5" t="b">
         <v>0</v>
@@ -19109,10 +19112,10 @@
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C13" s="5" t="b">
         <v>0</v>
@@ -19165,10 +19168,10 @@
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C14" s="5" t="b">
         <v>0</v>
@@ -19221,10 +19224,10 @@
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C15" s="5" t="b">
         <v>0</v>
@@ -19277,10 +19280,10 @@
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C16" s="5" t="b">
         <v>0</v>
@@ -19333,10 +19336,10 @@
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C17" s="5" t="b">
         <v>0</v>
@@ -19389,10 +19392,10 @@
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C18" s="5" t="b">
         <v>0</v>
@@ -19445,10 +19448,10 @@
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C19" s="5" t="b">
         <v>0</v>
@@ -19501,10 +19504,10 @@
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C20" s="5" t="b">
         <v>0</v>
@@ -19557,10 +19560,10 @@
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C21" s="5" t="b">
         <v>0</v>
@@ -19613,10 +19616,10 @@
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C22" s="5" t="b">
         <v>0</v>
@@ -19669,10 +19672,10 @@
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C23" s="5" t="b">
         <v>0</v>
@@ -19725,10 +19728,10 @@
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C24" s="5" t="b">
         <v>0</v>
@@ -19781,10 +19784,10 @@
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C25" s="5" t="b">
         <v>0</v>
@@ -19837,10 +19840,10 @@
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C26" s="5" t="b">
         <v>0</v>
@@ -19893,10 +19896,10 @@
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C27" s="5" t="b">
         <v>0</v>
@@ -19949,10 +19952,10 @@
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C28" s="5" t="b">
         <v>0</v>
@@ -20005,10 +20008,10 @@
     </row>
     <row r="29" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C29" s="5" t="b">
         <v>0</v>
@@ -20061,10 +20064,10 @@
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C30" s="5" t="b">
         <v>0</v>
@@ -20117,10 +20120,10 @@
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C31" s="5" t="b">
         <v>0</v>
@@ -20173,10 +20176,10 @@
     </row>
     <row r="32" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C32" s="5" t="b">
         <v>0</v>
@@ -20229,10 +20232,10 @@
     </row>
     <row r="33" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C33" s="5" t="b">
         <v>0</v>
@@ -20285,10 +20288,10 @@
     </row>
     <row r="34" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C34" s="5" t="b">
         <v>0</v>
@@ -20341,10 +20344,10 @@
     </row>
     <row r="35" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C35" s="5" t="b">
         <v>0</v>
@@ -20397,10 +20400,10 @@
     </row>
     <row r="36" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C36" s="5" t="b">
         <v>0</v>
@@ -20453,10 +20456,10 @@
     </row>
     <row r="37" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C37" s="5" t="b">
         <v>0</v>
@@ -20509,10 +20512,10 @@
     </row>
     <row r="38" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C38" s="5" t="b">
         <v>0</v>
@@ -20565,10 +20568,10 @@
     </row>
     <row r="39" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C39" s="5" t="b">
         <v>0</v>
@@ -20621,10 +20624,10 @@
     </row>
     <row r="40" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C40" s="5" t="b">
         <v>0</v>
@@ -20677,10 +20680,10 @@
     </row>
     <row r="41" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C41" s="5" t="b">
         <v>0</v>
@@ -20733,10 +20736,10 @@
     </row>
     <row r="42" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C42" s="5" t="b">
         <v>0</v>
@@ -20789,10 +20792,10 @@
     </row>
     <row r="43" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C43" s="5" t="b">
         <v>0</v>
@@ -20845,10 +20848,10 @@
     </row>
     <row r="44" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C44" s="5" t="b">
         <v>0</v>
@@ -20901,10 +20904,10 @@
     </row>
     <row r="45" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C45" s="5" t="b">
         <v>0</v>
@@ -20957,10 +20960,10 @@
     </row>
     <row r="46" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C46" s="5" t="b">
         <v>0</v>
@@ -21013,10 +21016,10 @@
     </row>
     <row r="47" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C47" s="5" t="b">
         <v>0</v>
@@ -21069,10 +21072,10 @@
     </row>
     <row r="48" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C48" s="5" t="b">
         <v>0</v>
@@ -21125,10 +21128,10 @@
     </row>
     <row r="49" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C49" s="5" t="b">
         <v>0</v>
@@ -21181,10 +21184,10 @@
     </row>
     <row r="50" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C50" s="5" t="b">
         <v>0</v>
@@ -21237,10 +21240,10 @@
     </row>
     <row r="51" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C51" s="5" t="b">
         <v>0</v>
@@ -21293,10 +21296,10 @@
     </row>
     <row r="52" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C52" s="5" t="b">
         <v>0</v>
@@ -21349,10 +21352,10 @@
     </row>
     <row r="53" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C53" s="5" t="b">
         <v>0</v>
@@ -21405,10 +21408,10 @@
     </row>
     <row r="54" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C54" s="5" t="b">
         <v>0</v>
@@ -21461,10 +21464,10 @@
     </row>
     <row r="55" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C55" s="5" t="b">
         <v>0</v>
@@ -21517,10 +21520,10 @@
     </row>
     <row r="56" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C56" s="5" t="b">
         <v>0</v>
@@ -21573,10 +21576,10 @@
     </row>
     <row r="57" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C57" s="5" t="b">
         <v>0</v>
@@ -21629,10 +21632,10 @@
     </row>
     <row r="58" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C58" s="5" t="b">
         <v>0</v>
@@ -21685,10 +21688,10 @@
     </row>
     <row r="59" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C59" s="5" t="b">
         <v>0</v>
@@ -21741,10 +21744,10 @@
     </row>
     <row r="60" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C60" s="5" t="b">
         <v>0</v>
@@ -21797,10 +21800,10 @@
     </row>
     <row r="61" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C61" s="5" t="b">
         <v>0</v>
@@ -21853,10 +21856,10 @@
     </row>
     <row r="62" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C62" s="5" t="b">
         <v>0</v>
@@ -21909,10 +21912,10 @@
     </row>
     <row r="63" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C63" s="5" t="b">
         <v>0</v>
@@ -21965,10 +21968,10 @@
     </row>
     <row r="64" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C64" s="5" t="b">
         <v>0</v>
@@ -22021,10 +22024,10 @@
     </row>
     <row r="65" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A65" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C65" s="5" t="b">
         <v>0</v>
@@ -22077,10 +22080,10 @@
     </row>
     <row r="66" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A66" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C66" s="5" t="b">
         <v>0</v>
@@ -22133,10 +22136,10 @@
     </row>
     <row r="67" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A67" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C67" s="5" t="b">
         <v>0</v>
@@ -22189,10 +22192,10 @@
     </row>
     <row r="68" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A68" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C68" s="5" t="b">
         <v>0</v>
@@ -22245,10 +22248,10 @@
     </row>
     <row r="69" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A69" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C69" s="5" t="b">
         <v>0</v>
@@ -22301,10 +22304,10 @@
     </row>
     <row r="70" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A70" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C70" s="5" t="b">
         <v>0</v>
@@ -22357,10 +22360,10 @@
     </row>
     <row r="71" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A71" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C71" s="5" t="b">
         <v>0</v>
@@ -22413,10 +22416,10 @@
     </row>
     <row r="72" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A72" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C72" s="5" t="b">
         <v>0</v>
@@ -22469,10 +22472,10 @@
     </row>
     <row r="73" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A73" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C73" s="5" t="b">
         <v>0</v>
@@ -22525,10 +22528,10 @@
     </row>
     <row r="74" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A74" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C74" s="5" t="b">
         <v>0</v>
@@ -22581,10 +22584,10 @@
     </row>
     <row r="75" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A75" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C75" s="5" t="b">
         <v>0</v>
@@ -22637,10 +22640,10 @@
     </row>
     <row r="76" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A76" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C76" s="5" t="b">
         <v>0</v>
@@ -22693,10 +22696,10 @@
     </row>
     <row r="77" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A77" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C77" s="5" t="b">
         <v>0</v>
@@ -22749,10 +22752,10 @@
     </row>
     <row r="78" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A78" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C78" s="5" t="b">
         <v>0</v>
@@ -22805,10 +22808,10 @@
     </row>
     <row r="79" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A79" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C79" s="5" t="b">
         <v>0</v>
@@ -22861,10 +22864,10 @@
     </row>
     <row r="80" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A80" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C80" s="5" t="b">
         <v>0</v>
@@ -22917,10 +22920,10 @@
     </row>
     <row r="81" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A81" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B81" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C81" s="5" t="b">
         <v>0</v>
@@ -22973,10 +22976,10 @@
     </row>
     <row r="82" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A82" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B82" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C82" s="5" t="b">
         <v>0</v>
@@ -23029,10 +23032,10 @@
     </row>
     <row r="83" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A83" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C83" s="5" t="b">
         <v>0</v>
@@ -23085,10 +23088,10 @@
     </row>
     <row r="84" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A84" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B84" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C84" s="5" t="b">
         <v>0</v>
@@ -23141,10 +23144,10 @@
     </row>
     <row r="85" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A85" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C85" s="5" t="b">
         <v>0</v>
@@ -23197,10 +23200,10 @@
     </row>
     <row r="86" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A86" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B86" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C86" s="5" t="b">
         <v>0</v>
@@ -23253,10 +23256,10 @@
     </row>
     <row r="87" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A87" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B87" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C87" s="5" t="b">
         <v>0</v>
@@ -23309,10 +23312,10 @@
     </row>
     <row r="88" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A88" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B88" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C88" s="5" t="b">
         <v>0</v>
@@ -23365,10 +23368,10 @@
     </row>
     <row r="89" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A89" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C89" s="5" t="b">
         <v>0</v>
@@ -23421,10 +23424,10 @@
     </row>
     <row r="90" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A90" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B90" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C90" s="5" t="b">
         <v>0</v>
@@ -23477,10 +23480,10 @@
     </row>
     <row r="91" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A91" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B91" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C91" s="5" t="b">
         <v>0</v>
@@ -23533,10 +23536,10 @@
     </row>
     <row r="92" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A92" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B92" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C92" s="5" t="b">
         <v>0</v>
@@ -23589,10 +23592,10 @@
     </row>
     <row r="93" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A93" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B93" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C93" s="5" t="b">
         <v>0</v>
@@ -23645,10 +23648,10 @@
     </row>
     <row r="94" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A94" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B94" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C94" s="5" t="b">
         <v>0</v>
@@ -23701,10 +23704,10 @@
     </row>
     <row r="95" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A95" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B95" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C95" s="5" t="b">
         <v>0</v>
@@ -23757,10 +23760,10 @@
     </row>
     <row r="96" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A96" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B96" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C96" s="5" t="b">
         <v>0</v>
@@ -23813,10 +23816,10 @@
     </row>
     <row r="97" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A97" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B97" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C97" s="5" t="b">
         <v>0</v>
@@ -23869,10 +23872,10 @@
     </row>
     <row r="98" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A98" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B98" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C98" s="5" t="b">
         <v>0</v>
@@ -23925,10 +23928,10 @@
     </row>
     <row r="99" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A99" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B99" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C99" s="5" t="b">
         <v>0</v>
@@ -23981,10 +23984,10 @@
     </row>
     <row r="100" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A100" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B100" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C100" s="5" t="b">
         <v>0</v>
@@ -24037,10 +24040,10 @@
     </row>
     <row r="101" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A101" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B101" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C101" s="5" t="b">
         <v>0</v>
@@ -24093,10 +24096,10 @@
     </row>
     <row r="102" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A102" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B102" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C102" s="5" t="b">
         <v>0</v>
@@ -24149,10 +24152,10 @@
     </row>
     <row r="103" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A103" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B103" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C103" s="5" t="b">
         <v>0</v>
@@ -24205,10 +24208,10 @@
     </row>
     <row r="104" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A104" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B104" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C104" s="5" t="b">
         <v>0</v>
@@ -24261,10 +24264,10 @@
     </row>
     <row r="105" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A105" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B105" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C105" s="5" t="b">
         <v>0</v>
@@ -24317,10 +24320,10 @@
     </row>
     <row r="106" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A106" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B106" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C106" s="5" t="b">
         <v>0</v>
@@ -24373,10 +24376,10 @@
     </row>
     <row r="107" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A107" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B107" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C107" s="5" t="b">
         <v>0</v>
@@ -24429,10 +24432,10 @@
     </row>
     <row r="108" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A108" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B108" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C108" s="5" t="b">
         <v>0</v>
@@ -24485,10 +24488,10 @@
     </row>
     <row r="109" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A109" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B109" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C109" s="5" t="b">
         <v>0</v>
@@ -24541,10 +24544,10 @@
     </row>
     <row r="110" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A110" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B110" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C110" s="5" t="b">
         <v>0</v>
@@ -24597,10 +24600,10 @@
     </row>
     <row r="111" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A111" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B111" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C111" s="5" t="b">
         <v>0</v>
@@ -24653,10 +24656,10 @@
     </row>
     <row r="112" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A112" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B112" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C112" s="5" t="b">
         <v>0</v>
@@ -24709,10 +24712,10 @@
     </row>
     <row r="113" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A113" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B113" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C113" s="5" t="b">
         <v>0</v>
@@ -24765,10 +24768,10 @@
     </row>
     <row r="114" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A114" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B114" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C114" s="5" t="b">
         <v>0</v>
@@ -24821,10 +24824,10 @@
     </row>
     <row r="115" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A115" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B115" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C115" s="5" t="b">
         <v>0</v>
@@ -24877,10 +24880,10 @@
     </row>
     <row r="116" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A116" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B116" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C116" s="5" t="b">
         <v>0</v>
@@ -24933,10 +24936,10 @@
     </row>
     <row r="117" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A117" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B117" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C117" s="5" t="b">
         <v>0</v>
@@ -24989,10 +24992,10 @@
     </row>
     <row r="118" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A118" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B118" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C118" s="5" t="b">
         <v>0</v>
@@ -25045,10 +25048,10 @@
     </row>
     <row r="119" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A119" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B119" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C119" s="5" t="b">
         <v>0</v>
@@ -25101,10 +25104,10 @@
     </row>
     <row r="120" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A120" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B120" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C120" s="5" t="b">
         <v>0</v>
@@ -25157,10 +25160,10 @@
     </row>
     <row r="121" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A121" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B121" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C121" s="5" t="b">
         <v>0</v>
@@ -25213,10 +25216,10 @@
     </row>
     <row r="122" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A122" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B122" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C122" s="5" t="b">
         <v>0</v>
@@ -25269,10 +25272,10 @@
     </row>
     <row r="123" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A123" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B123" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C123" s="5" t="b">
         <v>0</v>
@@ -25325,10 +25328,10 @@
     </row>
     <row r="124" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A124" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B124" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C124" s="5" t="b">
         <v>0</v>
@@ -25381,10 +25384,10 @@
     </row>
     <row r="125" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A125" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B125" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C125" s="5" t="b">
         <v>0</v>
@@ -25437,10 +25440,10 @@
     </row>
     <row r="126" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A126" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B126" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C126" s="5" t="b">
         <v>0</v>
@@ -25493,10 +25496,10 @@
     </row>
     <row r="127" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A127" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B127" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C127" s="5" t="b">
         <v>0</v>
@@ -25549,10 +25552,10 @@
     </row>
     <row r="128" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A128" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B128" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C128" s="5" t="b">
         <v>0</v>
@@ -25605,10 +25608,10 @@
     </row>
     <row r="129" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A129" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B129" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C129" s="5" t="b">
         <v>0</v>
@@ -25661,10 +25664,10 @@
     </row>
     <row r="130" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A130" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B130" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C130" s="5" t="b">
         <v>0</v>
@@ -25717,10 +25720,10 @@
     </row>
     <row r="131" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A131" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B131" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C131" s="5" t="b">
         <v>0</v>
@@ -25773,10 +25776,10 @@
     </row>
     <row r="132" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A132" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B132" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C132" s="5" t="b">
         <v>0</v>
@@ -25829,10 +25832,10 @@
     </row>
     <row r="133" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A133" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B133" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C133" s="5" t="b">
         <v>0</v>
@@ -25885,10 +25888,10 @@
     </row>
     <row r="134" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A134" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B134" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C134" s="5" t="b">
         <v>0</v>
@@ -25941,10 +25944,10 @@
     </row>
     <row r="135" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A135" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B135" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C135" s="5" t="b">
         <v>0</v>
@@ -25997,10 +26000,10 @@
     </row>
     <row r="136" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A136" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B136" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C136" s="5" t="b">
         <v>0</v>
@@ -26053,10 +26056,10 @@
     </row>
     <row r="137" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A137" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B137" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C137" s="5" t="b">
         <v>0</v>
@@ -26109,10 +26112,10 @@
     </row>
     <row r="138" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A138" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B138" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C138" s="5" t="b">
         <v>0</v>
@@ -26165,10 +26168,10 @@
     </row>
     <row r="139" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A139" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B139" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C139" s="5" t="b">
         <v>0</v>
@@ -26221,10 +26224,10 @@
     </row>
     <row r="140" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A140" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B140" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C140" s="5" t="b">
         <v>0</v>
@@ -26277,10 +26280,10 @@
     </row>
     <row r="141" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A141" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B141" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C141" s="5" t="b">
         <v>0</v>
@@ -26333,10 +26336,10 @@
     </row>
     <row r="142" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A142" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B142" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C142" s="5" t="b">
         <v>0</v>
@@ -26389,10 +26392,10 @@
     </row>
     <row r="143" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A143" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B143" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C143" s="5" t="b">
         <v>0</v>
@@ -26445,10 +26448,10 @@
     </row>
     <row r="144" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A144" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B144" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C144" s="5" t="b">
         <v>0</v>
@@ -26501,10 +26504,10 @@
     </row>
     <row r="145" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A145" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B145" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C145" s="5" t="b">
         <v>0</v>
@@ -26557,10 +26560,10 @@
     </row>
     <row r="146" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A146" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B146" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C146" s="5" t="b">
         <v>0</v>
@@ -26613,10 +26616,10 @@
     </row>
     <row r="147" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A147" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B147" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C147" s="5" t="b">
         <v>0</v>
@@ -26669,10 +26672,10 @@
     </row>
     <row r="148" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A148" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B148" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C148" s="5" t="b">
         <v>0</v>
@@ -26725,10 +26728,10 @@
     </row>
     <row r="149" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A149" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B149" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C149" s="5" t="b">
         <v>0</v>
@@ -26781,10 +26784,10 @@
     </row>
     <row r="150" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A150" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B150" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C150" s="5" t="b">
         <v>0</v>
@@ -26837,10 +26840,10 @@
     </row>
     <row r="151" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A151" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B151" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C151" s="5" t="b">
         <v>0</v>
@@ -26893,10 +26896,10 @@
     </row>
     <row r="152" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A152" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B152" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C152" s="5" t="b">
         <v>0</v>
@@ -26949,10 +26952,10 @@
     </row>
     <row r="153" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A153" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B153" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C153" s="5" t="b">
         <v>0</v>
@@ -27005,10 +27008,10 @@
     </row>
     <row r="154" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A154" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B154" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C154" s="5" t="b">
         <v>0</v>
@@ -27061,10 +27064,10 @@
     </row>
     <row r="155" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A155" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B155" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C155" s="5" t="b">
         <v>0</v>
@@ -27117,10 +27120,10 @@
     </row>
     <row r="156" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A156" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B156" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C156" s="5" t="b">
         <v>0</v>
@@ -27173,10 +27176,10 @@
     </row>
     <row r="157" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A157" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B157" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C157" s="5" t="b">
         <v>0</v>
@@ -27229,10 +27232,10 @@
     </row>
     <row r="158" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A158" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B158" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C158" s="5" t="b">
         <v>0</v>
@@ -27285,10 +27288,10 @@
     </row>
     <row r="159" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A159" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B159" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C159" s="5" t="b">
         <v>0</v>
@@ -27341,10 +27344,10 @@
     </row>
     <row r="160" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A160" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B160" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C160" s="5" t="b">
         <v>0</v>
@@ -27397,10 +27400,10 @@
     </row>
     <row r="161" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A161" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B161" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C161" s="5" t="b">
         <v>0</v>
@@ -27453,10 +27456,10 @@
     </row>
     <row r="162" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A162" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B162" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C162" s="5" t="b">
         <v>0</v>
@@ -27509,10 +27512,10 @@
     </row>
     <row r="163" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A163" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B163" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C163" s="5" t="b">
         <v>0</v>
@@ -27565,10 +27568,10 @@
     </row>
     <row r="164" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A164" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B164" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C164" s="5" t="b">
         <v>0</v>
@@ -27621,10 +27624,10 @@
     </row>
     <row r="165" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A165" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B165" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C165" s="5" t="b">
         <v>0</v>
@@ -27677,10 +27680,10 @@
     </row>
     <row r="166" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A166" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B166" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C166" s="5" t="b">
         <v>0</v>
@@ -27733,10 +27736,10 @@
     </row>
     <row r="167" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A167" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B167" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C167" s="5" t="b">
         <v>0</v>
@@ -27789,10 +27792,10 @@
     </row>
     <row r="168" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A168" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B168" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C168" s="5" t="b">
         <v>0</v>
@@ -27845,10 +27848,10 @@
     </row>
     <row r="169" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A169" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B169" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C169" s="5" t="b">
         <v>0</v>
@@ -27901,10 +27904,10 @@
     </row>
     <row r="170" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A170" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B170" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C170" s="5" t="b">
         <v>0</v>
@@ -27957,10 +27960,10 @@
     </row>
     <row r="171" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A171" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B171" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C171" s="5" t="b">
         <v>0</v>
@@ -28013,10 +28016,10 @@
     </row>
     <row r="172" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A172" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B172" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C172" s="5" t="b">
         <v>0</v>
@@ -28069,10 +28072,10 @@
     </row>
     <row r="173" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A173" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B173" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C173" s="5" t="b">
         <v>0</v>
@@ -28125,10 +28128,10 @@
     </row>
     <row r="174" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A174" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B174" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C174" s="5" t="b">
         <v>0</v>
@@ -28181,10 +28184,10 @@
     </row>
     <row r="175" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A175" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B175" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C175" s="5" t="b">
         <v>0</v>
@@ -28237,10 +28240,10 @@
     </row>
     <row r="176" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A176" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B176" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C176" s="5" t="b">
         <v>0</v>
@@ -28293,10 +28296,10 @@
     </row>
     <row r="177" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A177" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B177" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C177" s="5" t="b">
         <v>0</v>
@@ -28349,10 +28352,10 @@
     </row>
     <row r="178" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A178" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B178" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C178" s="5" t="b">
         <v>0</v>
@@ -28405,10 +28408,10 @@
     </row>
     <row r="179" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A179" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B179" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C179" s="5" t="b">
         <v>0</v>
@@ -28461,10 +28464,10 @@
     </row>
     <row r="180" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A180" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B180" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C180" s="5" t="b">
         <v>0</v>
@@ -28517,10 +28520,10 @@
     </row>
     <row r="181" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A181" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B181" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C181" s="5" t="b">
         <v>0</v>
@@ -28573,10 +28576,10 @@
     </row>
     <row r="182" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A182" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B182" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C182" s="5" t="b">
         <v>0</v>
@@ -28629,10 +28632,10 @@
     </row>
     <row r="183" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A183" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B183" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C183" s="5" t="b">
         <v>0</v>
@@ -28685,10 +28688,10 @@
     </row>
     <row r="184" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A184" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B184" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C184" s="5" t="b">
         <v>0</v>
@@ -28741,10 +28744,10 @@
     </row>
     <row r="185" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A185" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B185" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C185" s="5" t="b">
         <v>0</v>
@@ -28797,10 +28800,10 @@
     </row>
     <row r="186" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A186" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B186" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C186" s="5" t="b">
         <v>0</v>
@@ -28853,10 +28856,10 @@
     </row>
     <row r="187" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A187" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B187" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C187" s="5" t="b">
         <v>0</v>
@@ -28909,10 +28912,10 @@
     </row>
     <row r="188" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A188" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B188" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C188" s="5" t="b">
         <v>0</v>
@@ -28965,10 +28968,10 @@
     </row>
     <row r="189" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A189" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B189" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C189" s="5" t="b">
         <v>0</v>
@@ -29021,10 +29024,10 @@
     </row>
     <row r="190" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A190" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B190" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C190" s="5" t="b">
         <v>0</v>
@@ -29077,10 +29080,10 @@
     </row>
     <row r="191" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A191" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B191" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C191" s="5" t="b">
         <v>0</v>
@@ -29133,10 +29136,10 @@
     </row>
     <row r="192" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A192" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B192" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C192" s="5" t="b">
         <v>0</v>
@@ -29189,10 +29192,10 @@
     </row>
     <row r="193" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A193" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B193" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C193" s="5" t="b">
         <v>0</v>
@@ -29245,10 +29248,10 @@
     </row>
     <row r="194" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A194" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B194" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C194" s="5" t="b">
         <v>0</v>
@@ -29301,10 +29304,10 @@
     </row>
     <row r="195" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A195" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B195" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C195" s="5" t="b">
         <v>0</v>
@@ -29357,10 +29360,10 @@
     </row>
     <row r="196" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A196" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B196" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C196" s="5" t="b">
         <v>0</v>
@@ -29413,10 +29416,10 @@
     </row>
     <row r="197" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A197" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B197" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C197" s="5" t="b">
         <v>0</v>
@@ -29469,10 +29472,10 @@
     </row>
     <row r="198" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A198" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B198" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C198" s="5" t="b">
         <v>0</v>
@@ -29525,10 +29528,10 @@
     </row>
     <row r="199" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A199" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B199" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C199" s="5" t="b">
         <v>0</v>
@@ -29581,10 +29584,10 @@
     </row>
     <row r="200" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A200" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B200" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C200" s="5" t="b">
         <v>0</v>
@@ -29637,10 +29640,10 @@
     </row>
     <row r="201" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A201" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B201" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C201" s="5" t="b">
         <v>0</v>
@@ -29693,10 +29696,10 @@
     </row>
     <row r="202" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A202" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B202" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C202" s="5" t="b">
         <v>0</v>
@@ -29749,10 +29752,10 @@
     </row>
     <row r="203" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A203" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B203" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C203" s="5" t="b">
         <v>0</v>
@@ -29805,10 +29808,10 @@
     </row>
     <row r="204" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A204" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B204" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C204" s="5" t="b">
         <v>0</v>
@@ -29861,10 +29864,10 @@
     </row>
     <row r="205" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A205" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B205" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C205" s="5" t="b">
         <v>0</v>
@@ -29917,10 +29920,10 @@
     </row>
     <row r="206" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A206" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B206" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C206" s="5" t="b">
         <v>0</v>
@@ -29973,10 +29976,10 @@
     </row>
     <row r="207" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A207" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B207" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C207" s="5" t="b">
         <v>0</v>
@@ -30029,10 +30032,10 @@
     </row>
     <row r="208" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A208" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B208" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C208" s="5" t="b">
         <v>0</v>
@@ -30085,10 +30088,10 @@
     </row>
     <row r="209" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A209" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B209" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C209" s="5" t="b">
         <v>0</v>
@@ -30141,10 +30144,10 @@
     </row>
     <row r="210" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A210" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B210" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C210" s="5" t="b">
         <v>0</v>
@@ -30197,10 +30200,10 @@
     </row>
     <row r="211" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A211" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B211" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C211" s="5" t="b">
         <v>0</v>
@@ -30253,10 +30256,10 @@
     </row>
     <row r="212" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A212" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B212" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C212" s="5" t="b">
         <v>0</v>
@@ -30309,10 +30312,10 @@
     </row>
     <row r="213" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A213" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B213" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C213" s="5" t="b">
         <v>0</v>
@@ -30365,10 +30368,10 @@
     </row>
     <row r="214" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A214" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B214" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C214" s="5" t="b">
         <v>0</v>
@@ -30421,10 +30424,10 @@
     </row>
     <row r="215" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A215" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B215" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C215" s="5" t="b">
         <v>0</v>
@@ -30477,10 +30480,10 @@
     </row>
     <row r="216" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A216" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B216" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C216" s="5" t="b">
         <v>0</v>
@@ -30533,10 +30536,10 @@
     </row>
     <row r="217" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A217" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B217" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C217" s="5" t="b">
         <v>0</v>
@@ -30589,10 +30592,10 @@
     </row>
     <row r="218" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A218" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B218" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C218" s="5" t="b">
         <v>0</v>
@@ -30645,10 +30648,10 @@
     </row>
     <row r="219" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A219" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B219" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C219" s="5" t="b">
         <v>0</v>
@@ -30701,10 +30704,10 @@
     </row>
     <row r="220" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A220" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B220" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C220" s="5" t="b">
         <v>0</v>
@@ -30757,10 +30760,10 @@
     </row>
     <row r="221" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A221" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B221" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C221" s="5" t="b">
         <v>0</v>
@@ -30813,10 +30816,10 @@
     </row>
     <row r="222" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A222" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B222" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C222" s="5" t="b">
         <v>0</v>
@@ -30869,10 +30872,10 @@
     </row>
     <row r="223" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A223" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B223" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C223" s="5" t="b">
         <v>0</v>
@@ -30925,10 +30928,10 @@
     </row>
     <row r="224" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A224" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B224" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C224" s="5" t="b">
         <v>0</v>
@@ -30981,10 +30984,10 @@
     </row>
     <row r="225" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A225" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B225" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C225" s="5" t="b">
         <v>0</v>
@@ -31037,10 +31040,10 @@
     </row>
     <row r="226" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A226" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B226" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C226" s="5" t="b">
         <v>0</v>
@@ -31093,10 +31096,10 @@
     </row>
     <row r="227" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A227" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B227" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C227" s="5" t="b">
         <v>0</v>
@@ -31149,10 +31152,10 @@
     </row>
     <row r="228" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A228" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B228" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C228" s="5" t="b">
         <v>0</v>
@@ -31205,10 +31208,10 @@
     </row>
     <row r="229" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A229" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B229" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C229" s="5" t="b">
         <v>0</v>
@@ -31261,10 +31264,10 @@
     </row>
     <row r="230" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A230" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B230" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C230" s="5" t="b">
         <v>0</v>
@@ -31317,10 +31320,10 @@
     </row>
     <row r="231" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A231" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B231" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C231" s="5" t="b">
         <v>0</v>
@@ -31373,10 +31376,10 @@
     </row>
     <row r="232" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A232" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B232" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C232" s="5" t="b">
         <v>0</v>
@@ -31429,10 +31432,10 @@
     </row>
     <row r="233" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A233" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B233" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C233" s="5" t="b">
         <v>0</v>
@@ -31485,10 +31488,10 @@
     </row>
     <row r="234" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A234" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B234" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C234" s="5" t="b">
         <v>0</v>
@@ -31541,10 +31544,10 @@
     </row>
     <row r="235" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A235" s="3" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B235" s="3" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C235" s="5" t="b">
         <v>0</v>

</xml_diff>

<commit_message>
generated all the reports on 2024-08-20
</commit_message>
<xml_diff>
--- a/report/merged_configurations.xlsx
+++ b/report/merged_configurations.xlsx
@@ -18203,7 +18203,7 @@
         <v>23</v>
       </c>
       <c r="D232" s="3" t="s">
-        <v>41</v>
+        <v>24</v>
       </c>
       <c r="E232" s="3" t="s">
         <v>1188</v>
@@ -18264,7 +18264,7 @@
         <v>23</v>
       </c>
       <c r="D233" s="3" t="s">
-        <v>41</v>
+        <v>24</v>
       </c>
       <c r="E233" s="3" t="s">
         <v>1198</v>

</xml_diff>

<commit_message>
generated all the reports on 2024-08-26
</commit_message>
<xml_diff>
--- a/report/merged_configurations.xlsx
+++ b/report/merged_configurations.xlsx
@@ -4143,7 +4143,7 @@
         <v>26</v>
       </c>
       <c r="G2" s="4">
-        <v>45368.95833333333</v>
+        <v>45369</v>
       </c>
       <c r="H2" s="3" t="s">
         <v>27</v>
@@ -4164,7 +4164,7 @@
         <v>32</v>
       </c>
       <c r="N2" s="4">
-        <v>45168.91666666667</v>
+        <v>45169</v>
       </c>
       <c r="O2" s="3" t="s">
         <v>33</v>
@@ -4204,7 +4204,7 @@
         <v>26</v>
       </c>
       <c r="G3" s="4">
-        <v>45368.95833333333</v>
+        <v>45369</v>
       </c>
       <c r="H3" s="3" t="s">
         <v>39</v>
@@ -4225,7 +4225,7 @@
         <v>32</v>
       </c>
       <c r="N3" s="4">
-        <v>45168.91666666667</v>
+        <v>45169</v>
       </c>
       <c r="O3" s="3" t="s">
         <v>33</v>
@@ -4265,7 +4265,7 @@
         <v>43</v>
       </c>
       <c r="G4" s="4">
-        <v>45495.91666666667</v>
+        <v>45496</v>
       </c>
       <c r="H4" s="3" t="s">
         <v>44</v>
@@ -4326,7 +4326,7 @@
         <v>43</v>
       </c>
       <c r="G5" s="4">
-        <v>45495.91666666667</v>
+        <v>45496</v>
       </c>
       <c r="H5" s="3" t="s">
         <v>45</v>
@@ -4406,7 +4406,7 @@
         <v>61</v>
       </c>
       <c r="N6" s="4">
-        <v>44973.95833333333</v>
+        <v>44974</v>
       </c>
       <c r="O6" s="3" t="s">
         <v>33</v>
@@ -4465,7 +4465,7 @@
         <v>66</v>
       </c>
       <c r="N7" s="4">
-        <v>44973.95833333333</v>
+        <v>44974</v>
       </c>
       <c r="O7" s="3" t="s">
         <v>33</v>
@@ -4505,7 +4505,7 @@
         <v>69</v>
       </c>
       <c r="G8" s="4">
-        <v>44376.91666666667</v>
+        <v>44377</v>
       </c>
       <c r="H8" s="3" t="s">
         <v>70</v>
@@ -4566,7 +4566,7 @@
         <v>69</v>
       </c>
       <c r="G9" s="4">
-        <v>44376.91666666667</v>
+        <v>44377</v>
       </c>
       <c r="H9" s="3" t="s">
         <v>78</v>
@@ -4627,7 +4627,7 @@
         <v>43</v>
       </c>
       <c r="G10" s="4">
-        <v>45221.91666666667</v>
+        <v>45222</v>
       </c>
       <c r="H10" s="3" t="s">
         <v>81</v>
@@ -4682,7 +4682,7 @@
         <v>43</v>
       </c>
       <c r="G11" s="4">
-        <v>45221.91666666667</v>
+        <v>45222</v>
       </c>
       <c r="H11" s="3" t="s">
         <v>89</v>
@@ -4737,7 +4737,7 @@
         <v>43</v>
       </c>
       <c r="G12" s="4">
-        <v>45117.91666666667</v>
+        <v>45118</v>
       </c>
       <c r="H12" s="3" t="s">
         <v>92</v>
@@ -4758,7 +4758,7 @@
         <v>95</v>
       </c>
       <c r="N12" s="4">
-        <v>44973.95833333333</v>
+        <v>44974</v>
       </c>
       <c r="O12" s="3" t="s">
         <v>33</v>
@@ -4798,7 +4798,7 @@
         <v>43</v>
       </c>
       <c r="G13" s="4">
-        <v>45371.95833333333</v>
+        <v>45372</v>
       </c>
       <c r="H13" s="3" t="s">
         <v>100</v>
@@ -4857,7 +4857,7 @@
         <v>43</v>
       </c>
       <c r="G14" s="4">
-        <v>45371.95833333333</v>
+        <v>45372</v>
       </c>
       <c r="H14" s="3" t="s">
         <v>111</v>
@@ -4916,7 +4916,7 @@
         <v>43</v>
       </c>
       <c r="G15" s="4">
-        <v>45260.95833333333</v>
+        <v>45261</v>
       </c>
       <c r="H15" s="3" t="s">
         <v>115</v>
@@ -4977,7 +4977,7 @@
         <v>43</v>
       </c>
       <c r="G16" s="4">
-        <v>45260.95833333333</v>
+        <v>45261</v>
       </c>
       <c r="H16" s="3" t="s">
         <v>128</v>
@@ -5038,7 +5038,7 @@
         <v>134</v>
       </c>
       <c r="G17" s="4">
-        <v>44636.95833333333</v>
+        <v>44637</v>
       </c>
       <c r="H17" s="3" t="s">
         <v>135</v>
@@ -5099,7 +5099,7 @@
         <v>134</v>
       </c>
       <c r="G18" s="4">
-        <v>44636.95833333333</v>
+        <v>44637</v>
       </c>
       <c r="H18" s="3" t="s">
         <v>147</v>
@@ -5160,7 +5160,7 @@
         <v>150</v>
       </c>
       <c r="G19" s="4">
-        <v>44678.91666666667</v>
+        <v>44679</v>
       </c>
       <c r="H19" s="3" t="s">
         <v>151</v>
@@ -5221,7 +5221,7 @@
         <v>150</v>
       </c>
       <c r="G20" s="4">
-        <v>44408.91666666667</v>
+        <v>44409</v>
       </c>
       <c r="H20" s="3" t="s">
         <v>160</v>
@@ -5282,7 +5282,7 @@
         <v>150</v>
       </c>
       <c r="G21" s="4">
-        <v>44678.91666666667</v>
+        <v>44679</v>
       </c>
       <c r="H21" s="3" t="s">
         <v>163</v>
@@ -5343,7 +5343,7 @@
         <v>150</v>
       </c>
       <c r="G22" s="4">
-        <v>44678.91666666667</v>
+        <v>44679</v>
       </c>
       <c r="H22" s="3" t="s">
         <v>166</v>
@@ -5404,7 +5404,7 @@
         <v>150</v>
       </c>
       <c r="G23" s="4">
-        <v>44408.91666666667</v>
+        <v>44409</v>
       </c>
       <c r="H23" s="3" t="s">
         <v>170</v>
@@ -5465,7 +5465,7 @@
         <v>150</v>
       </c>
       <c r="G24" s="4">
-        <v>44408.91666666667</v>
+        <v>44409</v>
       </c>
       <c r="H24" s="3" t="s">
         <v>173</v>
@@ -5526,7 +5526,7 @@
         <v>150</v>
       </c>
       <c r="G25" s="4">
-        <v>44408.91666666667</v>
+        <v>44409</v>
       </c>
       <c r="H25" s="3" t="s">
         <v>176</v>
@@ -5587,7 +5587,7 @@
         <v>150</v>
       </c>
       <c r="G26" s="4">
-        <v>44408.91666666667</v>
+        <v>44409</v>
       </c>
       <c r="H26" s="3" t="s">
         <v>179</v>
@@ -5648,7 +5648,7 @@
         <v>150</v>
       </c>
       <c r="G27" s="4">
-        <v>44408.91666666667</v>
+        <v>44409</v>
       </c>
       <c r="H27" s="3" t="s">
         <v>182</v>
@@ -5709,7 +5709,7 @@
         <v>150</v>
       </c>
       <c r="G28" s="4">
-        <v>44408.91666666667</v>
+        <v>44409</v>
       </c>
       <c r="H28" s="3" t="s">
         <v>185</v>
@@ -5770,7 +5770,7 @@
         <v>150</v>
       </c>
       <c r="G29" s="4">
-        <v>44408.91666666667</v>
+        <v>44409</v>
       </c>
       <c r="H29" s="3" t="s">
         <v>188</v>
@@ -5831,7 +5831,7 @@
         <v>150</v>
       </c>
       <c r="G30" s="4">
-        <v>44408.91666666667</v>
+        <v>44409</v>
       </c>
       <c r="H30" s="3" t="s">
         <v>185</v>
@@ -5892,7 +5892,7 @@
         <v>150</v>
       </c>
       <c r="G31" s="4">
-        <v>44408.91666666667</v>
+        <v>44409</v>
       </c>
       <c r="H31" s="3" t="s">
         <v>191</v>
@@ -5953,7 +5953,7 @@
         <v>150</v>
       </c>
       <c r="G32" s="4">
-        <v>44408.91666666667</v>
+        <v>44409</v>
       </c>
       <c r="H32" s="3" t="s">
         <v>194</v>
@@ -6014,7 +6014,7 @@
         <v>150</v>
       </c>
       <c r="G33" s="4">
-        <v>44408.91666666667</v>
+        <v>44409</v>
       </c>
       <c r="H33" s="3" t="s">
         <v>197</v>
@@ -6075,7 +6075,7 @@
         <v>150</v>
       </c>
       <c r="G34" s="4">
-        <v>44408.91666666667</v>
+        <v>44409</v>
       </c>
       <c r="H34" s="3" t="s">
         <v>200</v>
@@ -6136,7 +6136,7 @@
         <v>150</v>
       </c>
       <c r="G35" s="4">
-        <v>44678.91666666667</v>
+        <v>44679</v>
       </c>
       <c r="H35" s="3" t="s">
         <v>203</v>
@@ -6197,7 +6197,7 @@
         <v>150</v>
       </c>
       <c r="G36" s="4">
-        <v>44678.91666666667</v>
+        <v>44679</v>
       </c>
       <c r="H36" s="3" t="s">
         <v>206</v>
@@ -6258,7 +6258,7 @@
         <v>150</v>
       </c>
       <c r="G37" s="4">
-        <v>44678.91666666667</v>
+        <v>44679</v>
       </c>
       <c r="H37" s="3" t="s">
         <v>209</v>
@@ -6319,7 +6319,7 @@
         <v>150</v>
       </c>
       <c r="G38" s="4">
-        <v>44678.91666666667</v>
+        <v>44679</v>
       </c>
       <c r="H38" s="3" t="s">
         <v>212</v>
@@ -6380,7 +6380,7 @@
         <v>217</v>
       </c>
       <c r="G39" s="4">
-        <v>44678.91666666667</v>
+        <v>44679</v>
       </c>
       <c r="H39" s="3" t="s">
         <v>218</v>
@@ -6441,7 +6441,7 @@
         <v>217</v>
       </c>
       <c r="G40" s="4">
-        <v>44678.91666666667</v>
+        <v>44679</v>
       </c>
       <c r="H40" s="3" t="s">
         <v>219</v>
@@ -6502,7 +6502,7 @@
         <v>233</v>
       </c>
       <c r="G41" s="4">
-        <v>44454.91666666667</v>
+        <v>44455</v>
       </c>
       <c r="H41" s="3" t="s">
         <v>234</v>
@@ -6523,7 +6523,7 @@
         <v>238</v>
       </c>
       <c r="N41" s="4">
-        <v>44454.91666666667</v>
+        <v>44455</v>
       </c>
       <c r="O41" s="3" t="s">
         <v>239</v>
@@ -6537,7 +6537,7 @@
       <c r="R41" s="3"/>
       <c r="S41" s="3"/>
       <c r="T41" s="4">
-        <v>44729.91666666667</v>
+        <v>44730</v>
       </c>
       <c r="U41" s="3" t="s">
         <v>241</v>
@@ -6563,7 +6563,7 @@
         <v>233</v>
       </c>
       <c r="G42" s="4">
-        <v>44454.91666666667</v>
+        <v>44455</v>
       </c>
       <c r="H42" s="3" t="s">
         <v>244</v>
@@ -6584,7 +6584,7 @@
         <v>245</v>
       </c>
       <c r="N42" s="4">
-        <v>44454.91666666667</v>
+        <v>44455</v>
       </c>
       <c r="O42" s="3" t="s">
         <v>239</v>
@@ -6598,7 +6598,7 @@
       <c r="R42" s="3"/>
       <c r="S42" s="3"/>
       <c r="T42" s="4">
-        <v>44729.91666666667</v>
+        <v>44730</v>
       </c>
       <c r="U42" s="3" t="s">
         <v>241</v>
@@ -6624,7 +6624,7 @@
         <v>217</v>
       </c>
       <c r="G43" s="4">
-        <v>44594.95833333333</v>
+        <v>44595</v>
       </c>
       <c r="H43" s="3" t="s">
         <v>248</v>
@@ -6685,7 +6685,7 @@
         <v>217</v>
       </c>
       <c r="G44" s="4">
-        <v>44594.95833333333</v>
+        <v>44595</v>
       </c>
       <c r="H44" s="3" t="s">
         <v>258</v>
@@ -6746,7 +6746,7 @@
         <v>262</v>
       </c>
       <c r="G45" s="4">
-        <v>44671.91666666667</v>
+        <v>44672</v>
       </c>
       <c r="H45" s="3" t="s">
         <v>263</v>
@@ -6767,13 +6767,13 @@
         <v>267</v>
       </c>
       <c r="N45" s="4">
-        <v>44146.95833333333</v>
+        <v>44147</v>
       </c>
       <c r="O45" s="4">
-        <v>44636.95833333333</v>
+        <v>44637</v>
       </c>
       <c r="P45" s="4">
-        <v>44671.91666666667</v>
+        <v>44672</v>
       </c>
       <c r="Q45" s="3" t="s">
         <v>268</v>
@@ -6807,7 +6807,7 @@
         <v>262</v>
       </c>
       <c r="G46" s="4">
-        <v>44671.91666666667</v>
+        <v>44672</v>
       </c>
       <c r="H46" s="3" t="s">
         <v>271</v>
@@ -6828,13 +6828,13 @@
         <v>267</v>
       </c>
       <c r="N46" s="4">
-        <v>44146.95833333333</v>
+        <v>44147</v>
       </c>
       <c r="O46" s="4">
-        <v>44636.95833333333</v>
+        <v>44637</v>
       </c>
       <c r="P46" s="4">
-        <v>44671.91666666667</v>
+        <v>44672</v>
       </c>
       <c r="Q46" s="3" t="s">
         <v>268</v>
@@ -6868,7 +6868,7 @@
         <v>262</v>
       </c>
       <c r="G47" s="4">
-        <v>44671.91666666667</v>
+        <v>44672</v>
       </c>
       <c r="H47" s="3" t="s">
         <v>273</v>
@@ -6889,13 +6889,13 @@
         <v>267</v>
       </c>
       <c r="N47" s="4">
-        <v>44146.95833333333</v>
+        <v>44147</v>
       </c>
       <c r="O47" s="4">
-        <v>44636.95833333333</v>
+        <v>44637</v>
       </c>
       <c r="P47" s="4">
-        <v>44671.91666666667</v>
+        <v>44672</v>
       </c>
       <c r="Q47" s="3" t="s">
         <v>268</v>
@@ -6929,7 +6929,7 @@
         <v>262</v>
       </c>
       <c r="G48" s="4">
-        <v>44671.91666666667</v>
+        <v>44672</v>
       </c>
       <c r="H48" s="3" t="s">
         <v>276</v>
@@ -6950,13 +6950,13 @@
         <v>267</v>
       </c>
       <c r="N48" s="4">
-        <v>44146.95833333333</v>
+        <v>44147</v>
       </c>
       <c r="O48" s="4">
-        <v>44636.95833333333</v>
+        <v>44637</v>
       </c>
       <c r="P48" s="4">
-        <v>44671.91666666667</v>
+        <v>44672</v>
       </c>
       <c r="Q48" s="3" t="s">
         <v>268</v>
@@ -6990,7 +6990,7 @@
         <v>43</v>
       </c>
       <c r="G49" s="4">
-        <v>43283.91666666667</v>
+        <v>43284</v>
       </c>
       <c r="H49" s="3" t="s">
         <v>279</v>
@@ -7051,7 +7051,7 @@
         <v>43</v>
       </c>
       <c r="G50" s="4">
-        <v>43808.95833333333</v>
+        <v>43809</v>
       </c>
       <c r="H50" s="3" t="s">
         <v>292</v>
@@ -7112,7 +7112,7 @@
         <v>43</v>
       </c>
       <c r="G51" s="4">
-        <v>43430.95833333333</v>
+        <v>43431</v>
       </c>
       <c r="H51" s="3" t="s">
         <v>295</v>
@@ -7173,7 +7173,7 @@
         <v>43</v>
       </c>
       <c r="G52" s="4">
-        <v>43808.95833333333</v>
+        <v>43809</v>
       </c>
       <c r="H52" s="3" t="s">
         <v>306</v>
@@ -7234,7 +7234,7 @@
         <v>43</v>
       </c>
       <c r="G53" s="4">
-        <v>43502.95833333333</v>
+        <v>43503</v>
       </c>
       <c r="H53" s="3" t="s">
         <v>310</v>
@@ -7295,7 +7295,7 @@
         <v>43</v>
       </c>
       <c r="G54" s="4">
-        <v>43502.95833333333</v>
+        <v>43503</v>
       </c>
       <c r="H54" s="3" t="s">
         <v>320</v>
@@ -7356,7 +7356,7 @@
         <v>43</v>
       </c>
       <c r="G55" s="4">
-        <v>43283.91666666667</v>
+        <v>43284</v>
       </c>
       <c r="H55" s="3" t="s">
         <v>323</v>
@@ -7417,7 +7417,7 @@
         <v>43</v>
       </c>
       <c r="G56" s="4">
-        <v>43808.95833333333</v>
+        <v>43809</v>
       </c>
       <c r="H56" s="3" t="s">
         <v>331</v>
@@ -7478,7 +7478,7 @@
         <v>334</v>
       </c>
       <c r="G57" s="4">
-        <v>43502.95833333333</v>
+        <v>43503</v>
       </c>
       <c r="H57" s="3" t="s">
         <v>335</v>
@@ -7539,7 +7539,7 @@
         <v>43</v>
       </c>
       <c r="G58" s="4">
-        <v>43283.91666666667</v>
+        <v>43284</v>
       </c>
       <c r="H58" s="3" t="s">
         <v>347</v>
@@ -7600,7 +7600,7 @@
         <v>43</v>
       </c>
       <c r="G59" s="4">
-        <v>43283.91666666667</v>
+        <v>43284</v>
       </c>
       <c r="H59" s="3" t="s">
         <v>357</v>
@@ -7661,7 +7661,7 @@
         <v>360</v>
       </c>
       <c r="G60" s="4">
-        <v>43803.95833333333</v>
+        <v>43804</v>
       </c>
       <c r="H60" s="3" t="s">
         <v>361</v>
@@ -7722,7 +7722,7 @@
         <v>360</v>
       </c>
       <c r="G61" s="4">
-        <v>43803.95833333333</v>
+        <v>43804</v>
       </c>
       <c r="H61" s="3" t="s">
         <v>373</v>
@@ -7783,7 +7783,7 @@
         <v>43</v>
       </c>
       <c r="G62" s="4">
-        <v>43808.95833333333</v>
+        <v>43809</v>
       </c>
       <c r="H62" s="3" t="s">
         <v>376</v>
@@ -7844,7 +7844,7 @@
         <v>43</v>
       </c>
       <c r="G63" s="4">
-        <v>43283.91666666667</v>
+        <v>43284</v>
       </c>
       <c r="H63" s="3" t="s">
         <v>383</v>
@@ -7905,7 +7905,7 @@
         <v>43</v>
       </c>
       <c r="G64" s="4">
-        <v>43411.95833333333</v>
+        <v>43412</v>
       </c>
       <c r="H64" s="3" t="s">
         <v>391</v>
@@ -7966,7 +7966,7 @@
         <v>43</v>
       </c>
       <c r="G65" s="4">
-        <v>43411.95833333333</v>
+        <v>43412</v>
       </c>
       <c r="H65" s="3" t="s">
         <v>395</v>
@@ -8027,7 +8027,7 @@
         <v>43</v>
       </c>
       <c r="G66" s="4">
-        <v>43943.91666666667</v>
+        <v>43944</v>
       </c>
       <c r="H66" s="3" t="s">
         <v>398</v>
@@ -8088,7 +8088,7 @@
         <v>43</v>
       </c>
       <c r="G67" s="4">
-        <v>43502.95833333333</v>
+        <v>43503</v>
       </c>
       <c r="H67" s="3" t="s">
         <v>406</v>
@@ -8149,7 +8149,7 @@
         <v>43</v>
       </c>
       <c r="G68" s="4">
-        <v>43502.95833333333</v>
+        <v>43503</v>
       </c>
       <c r="H68" s="3" t="s">
         <v>413</v>
@@ -8210,7 +8210,7 @@
         <v>43</v>
       </c>
       <c r="G69" s="4">
-        <v>43502.95833333333</v>
+        <v>43503</v>
       </c>
       <c r="H69" s="3" t="s">
         <v>416</v>
@@ -8271,7 +8271,7 @@
         <v>43</v>
       </c>
       <c r="G70" s="4">
-        <v>43502.95833333333</v>
+        <v>43503</v>
       </c>
       <c r="H70" s="3" t="s">
         <v>424</v>
@@ -8332,7 +8332,7 @@
         <v>43</v>
       </c>
       <c r="G71" s="4">
-        <v>43502.95833333333</v>
+        <v>43503</v>
       </c>
       <c r="H71" s="3" t="s">
         <v>427</v>
@@ -8393,7 +8393,7 @@
         <v>430</v>
       </c>
       <c r="G72" s="4">
-        <v>45193.91666666667</v>
+        <v>45194</v>
       </c>
       <c r="H72" s="3" t="s">
         <v>431</v>
@@ -8454,7 +8454,7 @@
         <v>430</v>
       </c>
       <c r="G73" s="4">
-        <v>45193.91666666667</v>
+        <v>45194</v>
       </c>
       <c r="H73" s="3" t="s">
         <v>442</v>
@@ -8515,7 +8515,7 @@
         <v>445</v>
       </c>
       <c r="G74" s="4">
-        <v>43465.95833333333</v>
+        <v>43466</v>
       </c>
       <c r="H74" s="3" t="s">
         <v>446</v>
@@ -8576,7 +8576,7 @@
         <v>445</v>
       </c>
       <c r="G75" s="4">
-        <v>43465.95833333333</v>
+        <v>43466</v>
       </c>
       <c r="H75" s="3" t="s">
         <v>456</v>
@@ -8637,7 +8637,7 @@
         <v>459</v>
       </c>
       <c r="G76" s="4">
-        <v>43943.91666666667</v>
+        <v>43944</v>
       </c>
       <c r="H76" s="3" t="s">
         <v>460</v>
@@ -8698,7 +8698,7 @@
         <v>459</v>
       </c>
       <c r="G77" s="4">
-        <v>43943.91666666667</v>
+        <v>43944</v>
       </c>
       <c r="H77" s="3" t="s">
         <v>472</v>
@@ -8759,7 +8759,7 @@
         <v>459</v>
       </c>
       <c r="G78" s="4">
-        <v>43943.91666666667</v>
+        <v>43944</v>
       </c>
       <c r="H78" s="3" t="s">
         <v>476</v>
@@ -8820,7 +8820,7 @@
         <v>459</v>
       </c>
       <c r="G79" s="4">
-        <v>43943.91666666667</v>
+        <v>43944</v>
       </c>
       <c r="H79" s="3" t="s">
         <v>480</v>
@@ -8881,7 +8881,7 @@
         <v>43</v>
       </c>
       <c r="G80" s="4">
-        <v>44531.95833333333</v>
+        <v>44532</v>
       </c>
       <c r="H80" s="3" t="s">
         <v>485</v>
@@ -8942,7 +8942,7 @@
         <v>43</v>
       </c>
       <c r="G81" s="4">
-        <v>43502.95833333333</v>
+        <v>43503</v>
       </c>
       <c r="H81" s="3" t="s">
         <v>499</v>
@@ -9003,7 +9003,7 @@
         <v>43</v>
       </c>
       <c r="G82" s="4">
-        <v>43502.95833333333</v>
+        <v>43503</v>
       </c>
       <c r="H82" s="3" t="s">
         <v>512</v>
@@ -9064,7 +9064,7 @@
         <v>43</v>
       </c>
       <c r="G83" s="4">
-        <v>43502.95833333333</v>
+        <v>43503</v>
       </c>
       <c r="H83" s="3" t="s">
         <v>520</v>
@@ -9125,7 +9125,7 @@
         <v>523</v>
       </c>
       <c r="G84" s="4">
-        <v>43999.91666666667</v>
+        <v>44000</v>
       </c>
       <c r="H84" s="3" t="s">
         <v>524</v>
@@ -9186,7 +9186,7 @@
         <v>523</v>
       </c>
       <c r="G85" s="4">
-        <v>43999.91666666667</v>
+        <v>44000</v>
       </c>
       <c r="H85" s="3" t="s">
         <v>536</v>
@@ -9247,7 +9247,7 @@
         <v>523</v>
       </c>
       <c r="G86" s="4">
-        <v>43999.91666666667</v>
+        <v>44000</v>
       </c>
       <c r="H86" s="3" t="s">
         <v>539</v>
@@ -9308,7 +9308,7 @@
         <v>523</v>
       </c>
       <c r="G87" s="4">
-        <v>43999.91666666667</v>
+        <v>44000</v>
       </c>
       <c r="H87" s="3" t="s">
         <v>544</v>
@@ -9369,7 +9369,7 @@
         <v>547</v>
       </c>
       <c r="G88" s="4">
-        <v>43300.91666666667</v>
+        <v>43301</v>
       </c>
       <c r="H88" s="3" t="s">
         <v>548</v>
@@ -9430,7 +9430,7 @@
         <v>547</v>
       </c>
       <c r="G89" s="4">
-        <v>43300.91666666667</v>
+        <v>43301</v>
       </c>
       <c r="H89" s="3" t="s">
         <v>557</v>
@@ -9491,7 +9491,7 @@
         <v>547</v>
       </c>
       <c r="G90" s="4">
-        <v>43300.91666666667</v>
+        <v>43301</v>
       </c>
       <c r="H90" s="3" t="s">
         <v>561</v>
@@ -9552,7 +9552,7 @@
         <v>547</v>
       </c>
       <c r="G91" s="4">
-        <v>43300.91666666667</v>
+        <v>43301</v>
       </c>
       <c r="H91" s="3" t="s">
         <v>567</v>
@@ -9613,7 +9613,7 @@
         <v>547</v>
       </c>
       <c r="G92" s="4">
-        <v>43276.91666666667</v>
+        <v>43277</v>
       </c>
       <c r="H92" s="3" t="s">
         <v>570</v>
@@ -9674,7 +9674,7 @@
         <v>43</v>
       </c>
       <c r="G93" s="4">
-        <v>43241.91666666667</v>
+        <v>43242</v>
       </c>
       <c r="H93" s="3" t="s">
         <v>575</v>
@@ -9735,7 +9735,7 @@
         <v>43</v>
       </c>
       <c r="G94" s="4">
-        <v>43241.91666666667</v>
+        <v>43242</v>
       </c>
       <c r="H94" s="3" t="s">
         <v>583</v>
@@ -9796,7 +9796,7 @@
         <v>43</v>
       </c>
       <c r="G95" s="4">
-        <v>43241.91666666667</v>
+        <v>43242</v>
       </c>
       <c r="H95" s="3" t="s">
         <v>586</v>
@@ -9857,7 +9857,7 @@
         <v>43</v>
       </c>
       <c r="G96" s="4">
-        <v>43430.95833333333</v>
+        <v>43431</v>
       </c>
       <c r="H96" s="3" t="s">
         <v>596</v>
@@ -9918,7 +9918,7 @@
         <v>43</v>
       </c>
       <c r="G97" s="4">
-        <v>43430.95833333333</v>
+        <v>43431</v>
       </c>
       <c r="H97" s="3" t="s">
         <v>606</v>
@@ -9979,7 +9979,7 @@
         <v>43</v>
       </c>
       <c r="G98" s="4">
-        <v>43430.95833333333</v>
+        <v>43431</v>
       </c>
       <c r="H98" s="3" t="s">
         <v>608</v>
@@ -10040,7 +10040,7 @@
         <v>43</v>
       </c>
       <c r="G99" s="4">
-        <v>43430.95833333333</v>
+        <v>43431</v>
       </c>
       <c r="H99" s="3" t="s">
         <v>610</v>
@@ -10101,7 +10101,7 @@
         <v>43</v>
       </c>
       <c r="G100" s="4">
-        <v>43430.95833333333</v>
+        <v>43431</v>
       </c>
       <c r="H100" s="3" t="s">
         <v>612</v>
@@ -10162,7 +10162,7 @@
         <v>43</v>
       </c>
       <c r="G101" s="4">
-        <v>43430.95833333333</v>
+        <v>43431</v>
       </c>
       <c r="H101" s="3" t="s">
         <v>614</v>
@@ -10223,7 +10223,7 @@
         <v>43</v>
       </c>
       <c r="G102" s="4">
-        <v>43430.95833333333</v>
+        <v>43431</v>
       </c>
       <c r="H102" s="3" t="s">
         <v>616</v>
@@ -10284,7 +10284,7 @@
         <v>43</v>
       </c>
       <c r="G103" s="4">
-        <v>43430.95833333333</v>
+        <v>43431</v>
       </c>
       <c r="H103" s="3" t="s">
         <v>619</v>
@@ -10345,7 +10345,7 @@
         <v>43</v>
       </c>
       <c r="G104" s="4">
-        <v>43430.95833333333</v>
+        <v>43431</v>
       </c>
       <c r="H104" s="3" t="s">
         <v>621</v>
@@ -10406,7 +10406,7 @@
         <v>43</v>
       </c>
       <c r="G105" s="4">
-        <v>43430.95833333333</v>
+        <v>43431</v>
       </c>
       <c r="H105" s="3" t="s">
         <v>623</v>
@@ -10467,7 +10467,7 @@
         <v>43</v>
       </c>
       <c r="G106" s="4">
-        <v>43430.95833333333</v>
+        <v>43431</v>
       </c>
       <c r="H106" s="3" t="s">
         <v>625</v>
@@ -10528,7 +10528,7 @@
         <v>43</v>
       </c>
       <c r="G107" s="4">
-        <v>43430.95833333333</v>
+        <v>43431</v>
       </c>
       <c r="H107" s="3" t="s">
         <v>627</v>
@@ -10589,7 +10589,7 @@
         <v>43</v>
       </c>
       <c r="G108" s="4">
-        <v>43430.95833333333</v>
+        <v>43431</v>
       </c>
       <c r="H108" s="3" t="s">
         <v>629</v>
@@ -10650,7 +10650,7 @@
         <v>43</v>
       </c>
       <c r="G109" s="4">
-        <v>43430.95833333333</v>
+        <v>43431</v>
       </c>
       <c r="H109" s="3" t="s">
         <v>631</v>
@@ -10711,7 +10711,7 @@
         <v>43</v>
       </c>
       <c r="G110" s="4">
-        <v>43430.95833333333</v>
+        <v>43431</v>
       </c>
       <c r="H110" s="3" t="s">
         <v>633</v>
@@ -10772,7 +10772,7 @@
         <v>43</v>
       </c>
       <c r="G111" s="4">
-        <v>43430.95833333333</v>
+        <v>43431</v>
       </c>
       <c r="H111" s="3" t="s">
         <v>635</v>
@@ -10833,7 +10833,7 @@
         <v>638</v>
       </c>
       <c r="G112" s="4">
-        <v>43943.91666666667</v>
+        <v>43944</v>
       </c>
       <c r="H112" s="3" t="s">
         <v>639</v>
@@ -10894,7 +10894,7 @@
         <v>334</v>
       </c>
       <c r="G113" s="4">
-        <v>44230.95833333333</v>
+        <v>44231</v>
       </c>
       <c r="H113" s="3" t="s">
         <v>647</v>
@@ -10955,7 +10955,7 @@
         <v>334</v>
       </c>
       <c r="G114" s="4">
-        <v>44230.95833333333</v>
+        <v>44231</v>
       </c>
       <c r="H114" s="3" t="s">
         <v>658</v>
@@ -11016,7 +11016,7 @@
         <v>217</v>
       </c>
       <c r="G115" s="4">
-        <v>44307.91666666667</v>
+        <v>44308</v>
       </c>
       <c r="H115" s="3" t="s">
         <v>661</v>
@@ -11040,10 +11040,10 @@
         <v>667</v>
       </c>
       <c r="O115" s="4">
-        <v>44265.95833333333</v>
+        <v>44266</v>
       </c>
       <c r="P115" s="4">
-        <v>44307.91666666667</v>
+        <v>44308</v>
       </c>
       <c r="Q115" s="3" t="s">
         <v>668</v>
@@ -11077,7 +11077,7 @@
         <v>217</v>
       </c>
       <c r="G116" s="4">
-        <v>44307.91666666667</v>
+        <v>44308</v>
       </c>
       <c r="H116" s="3" t="s">
         <v>672</v>
@@ -11101,10 +11101,10 @@
         <v>667</v>
       </c>
       <c r="O116" s="4">
-        <v>44265.95833333333</v>
+        <v>44266</v>
       </c>
       <c r="P116" s="4">
-        <v>44307.91666666667</v>
+        <v>44308</v>
       </c>
       <c r="Q116" s="3" t="s">
         <v>668</v>
@@ -11138,7 +11138,7 @@
         <v>217</v>
       </c>
       <c r="G117" s="4">
-        <v>44307.91666666667</v>
+        <v>44308</v>
       </c>
       <c r="H117" s="3" t="s">
         <v>676</v>
@@ -11159,13 +11159,13 @@
         <v>666</v>
       </c>
       <c r="N117" s="4">
-        <v>43788.95833333333</v>
+        <v>43789</v>
       </c>
       <c r="O117" s="4">
-        <v>44265.95833333333</v>
+        <v>44266</v>
       </c>
       <c r="P117" s="4">
-        <v>44307.91666666667</v>
+        <v>44308</v>
       </c>
       <c r="Q117" s="3" t="s">
         <v>668</v>
@@ -11199,7 +11199,7 @@
         <v>680</v>
       </c>
       <c r="G118" s="4">
-        <v>43251.91666666667</v>
+        <v>43252</v>
       </c>
       <c r="H118" s="3" t="s">
         <v>681</v>
@@ -11260,7 +11260,7 @@
         <v>690</v>
       </c>
       <c r="G119" s="4">
-        <v>43251.91666666667</v>
+        <v>43252</v>
       </c>
       <c r="H119" s="3" t="s">
         <v>691</v>
@@ -11319,7 +11319,7 @@
         <v>43</v>
       </c>
       <c r="G120" s="4">
-        <v>42816.95833333333</v>
+        <v>42817</v>
       </c>
       <c r="H120" s="3" t="s">
         <v>695</v>
@@ -11378,7 +11378,7 @@
         <v>43</v>
       </c>
       <c r="G121" s="4">
-        <v>42824.91666666667</v>
+        <v>42825</v>
       </c>
       <c r="H121" s="3" t="s">
         <v>700</v>
@@ -11439,7 +11439,7 @@
         <v>43</v>
       </c>
       <c r="G122" s="4">
-        <v>44468.91666666667</v>
+        <v>44469</v>
       </c>
       <c r="H122" s="3" t="s">
         <v>702</v>
@@ -11500,7 +11500,7 @@
         <v>43</v>
       </c>
       <c r="G123" s="4">
-        <v>44468.91666666667</v>
+        <v>44469</v>
       </c>
       <c r="H123" s="3" t="s">
         <v>709</v>
@@ -11561,7 +11561,7 @@
         <v>43</v>
       </c>
       <c r="G124" s="4">
-        <v>44468.91666666667</v>
+        <v>44469</v>
       </c>
       <c r="H124" s="3" t="s">
         <v>711</v>
@@ -11622,7 +11622,7 @@
         <v>43</v>
       </c>
       <c r="G125" s="4">
-        <v>44468.91666666667</v>
+        <v>44469</v>
       </c>
       <c r="H125" s="3" t="s">
         <v>713</v>
@@ -11683,7 +11683,7 @@
         <v>43</v>
       </c>
       <c r="G126" s="4">
-        <v>44468.91666666667</v>
+        <v>44469</v>
       </c>
       <c r="H126" s="3" t="s">
         <v>715</v>
@@ -11744,7 +11744,7 @@
         <v>43</v>
       </c>
       <c r="G127" s="4">
-        <v>44468.91666666667</v>
+        <v>44469</v>
       </c>
       <c r="H127" s="3" t="s">
         <v>717</v>
@@ -11805,7 +11805,7 @@
         <v>43</v>
       </c>
       <c r="G128" s="4">
-        <v>44468.91666666667</v>
+        <v>44469</v>
       </c>
       <c r="H128" s="3" t="s">
         <v>719</v>
@@ -11866,7 +11866,7 @@
         <v>43</v>
       </c>
       <c r="G129" s="4">
-        <v>44468.91666666667</v>
+        <v>44469</v>
       </c>
       <c r="H129" s="3" t="s">
         <v>721</v>
@@ -11927,7 +11927,7 @@
         <v>43</v>
       </c>
       <c r="G130" s="4">
-        <v>44468.91666666667</v>
+        <v>44469</v>
       </c>
       <c r="H130" s="3" t="s">
         <v>723</v>
@@ -11988,7 +11988,7 @@
         <v>43</v>
       </c>
       <c r="G131" s="4">
-        <v>44468.91666666667</v>
+        <v>44469</v>
       </c>
       <c r="H131" s="3" t="s">
         <v>725</v>
@@ -12049,7 +12049,7 @@
         <v>43</v>
       </c>
       <c r="G132" s="4">
-        <v>44468.91666666667</v>
+        <v>44469</v>
       </c>
       <c r="H132" s="3" t="s">
         <v>727</v>
@@ -12110,7 +12110,7 @@
         <v>43</v>
       </c>
       <c r="G133" s="4">
-        <v>44468.91666666667</v>
+        <v>44469</v>
       </c>
       <c r="H133" s="3" t="s">
         <v>731</v>
@@ -12171,7 +12171,7 @@
         <v>43</v>
       </c>
       <c r="G134" s="4">
-        <v>44468.91666666667</v>
+        <v>44469</v>
       </c>
       <c r="H134" s="3" t="s">
         <v>734</v>
@@ -12232,7 +12232,7 @@
         <v>43</v>
       </c>
       <c r="G135" s="4">
-        <v>44468.91666666667</v>
+        <v>44469</v>
       </c>
       <c r="H135" s="3" t="s">
         <v>736</v>
@@ -12293,7 +12293,7 @@
         <v>43</v>
       </c>
       <c r="G136" s="4">
-        <v>44468.91666666667</v>
+        <v>44469</v>
       </c>
       <c r="H136" s="3" t="s">
         <v>738</v>
@@ -12354,7 +12354,7 @@
         <v>43</v>
       </c>
       <c r="G137" s="4">
-        <v>44468.91666666667</v>
+        <v>44469</v>
       </c>
       <c r="H137" s="3" t="s">
         <v>740</v>
@@ -12415,7 +12415,7 @@
         <v>43</v>
       </c>
       <c r="G138" s="4">
-        <v>44468.91666666667</v>
+        <v>44469</v>
       </c>
       <c r="H138" s="3" t="s">
         <v>742</v>
@@ -12476,7 +12476,7 @@
         <v>43</v>
       </c>
       <c r="G139" s="4">
-        <v>44468.91666666667</v>
+        <v>44469</v>
       </c>
       <c r="H139" s="3" t="s">
         <v>744</v>
@@ -12537,7 +12537,7 @@
         <v>43</v>
       </c>
       <c r="G140" s="4">
-        <v>44468.91666666667</v>
+        <v>44469</v>
       </c>
       <c r="H140" s="3" t="s">
         <v>746</v>
@@ -12598,7 +12598,7 @@
         <v>43</v>
       </c>
       <c r="G141" s="4">
-        <v>44468.91666666667</v>
+        <v>44469</v>
       </c>
       <c r="H141" s="3" t="s">
         <v>748</v>
@@ -12659,7 +12659,7 @@
         <v>43</v>
       </c>
       <c r="G142" s="4">
-        <v>44468.91666666667</v>
+        <v>44469</v>
       </c>
       <c r="H142" s="3" t="s">
         <v>750</v>
@@ -12842,7 +12842,7 @@
         <v>69</v>
       </c>
       <c r="G145" s="4">
-        <v>44307.91666666667</v>
+        <v>44308</v>
       </c>
       <c r="H145" s="3" t="s">
         <v>770</v>
@@ -12863,13 +12863,13 @@
         <v>773</v>
       </c>
       <c r="N145" s="4">
-        <v>44031.91666666667</v>
+        <v>44032</v>
       </c>
       <c r="O145" s="4">
-        <v>44265.95833333333</v>
+        <v>44266</v>
       </c>
       <c r="P145" s="4">
-        <v>44307.91666666667</v>
+        <v>44308</v>
       </c>
       <c r="Q145" s="3" t="s">
         <v>766</v>
@@ -12903,7 +12903,7 @@
         <v>69</v>
       </c>
       <c r="G146" s="4">
-        <v>44307.91666666667</v>
+        <v>44308</v>
       </c>
       <c r="H146" s="3" t="s">
         <v>776</v>
@@ -12924,13 +12924,13 @@
         <v>779</v>
       </c>
       <c r="N146" s="4">
-        <v>44396.91666666667</v>
+        <v>44397</v>
       </c>
       <c r="O146" s="4">
-        <v>44265.95833333333</v>
+        <v>44266</v>
       </c>
       <c r="P146" s="4">
-        <v>44307.91666666667</v>
+        <v>44308</v>
       </c>
       <c r="Q146" s="3" t="s">
         <v>766</v>
@@ -12964,7 +12964,7 @@
         <v>150</v>
       </c>
       <c r="G147" s="4">
-        <v>44408.91666666667</v>
+        <v>44409</v>
       </c>
       <c r="H147" s="3" t="s">
         <v>782</v>
@@ -13025,7 +13025,7 @@
         <v>638</v>
       </c>
       <c r="G148" s="4">
-        <v>44166.95833333333</v>
+        <v>44167</v>
       </c>
       <c r="H148" s="3" t="s">
         <v>786</v>
@@ -13086,7 +13086,7 @@
         <v>638</v>
       </c>
       <c r="G149" s="4">
-        <v>44166.95833333333</v>
+        <v>44167</v>
       </c>
       <c r="H149" s="3" t="s">
         <v>797</v>
@@ -13147,7 +13147,7 @@
         <v>638</v>
       </c>
       <c r="G150" s="4">
-        <v>44166.95833333333</v>
+        <v>44167</v>
       </c>
       <c r="H150" s="3" t="s">
         <v>800</v>
@@ -13208,7 +13208,7 @@
         <v>638</v>
       </c>
       <c r="G151" s="4">
-        <v>44166.95833333333</v>
+        <v>44167</v>
       </c>
       <c r="H151" s="3" t="s">
         <v>803</v>
@@ -13269,7 +13269,7 @@
         <v>638</v>
       </c>
       <c r="G152" s="4">
-        <v>44166.95833333333</v>
+        <v>44167</v>
       </c>
       <c r="H152" s="3" t="s">
         <v>806</v>
@@ -13330,7 +13330,7 @@
         <v>638</v>
       </c>
       <c r="G153" s="4">
-        <v>44166.95833333333</v>
+        <v>44167</v>
       </c>
       <c r="H153" s="3" t="s">
         <v>809</v>
@@ -13391,7 +13391,7 @@
         <v>638</v>
       </c>
       <c r="G154" s="4">
-        <v>44166.95833333333</v>
+        <v>44167</v>
       </c>
       <c r="H154" s="3" t="s">
         <v>812</v>
@@ -13452,7 +13452,7 @@
         <v>638</v>
       </c>
       <c r="G155" s="4">
-        <v>44166.95833333333</v>
+        <v>44167</v>
       </c>
       <c r="H155" s="3" t="s">
         <v>815</v>
@@ -13513,7 +13513,7 @@
         <v>638</v>
       </c>
       <c r="G156" s="4">
-        <v>44166.95833333333</v>
+        <v>44167</v>
       </c>
       <c r="H156" s="3" t="s">
         <v>818</v>
@@ -13574,7 +13574,7 @@
         <v>638</v>
       </c>
       <c r="G157" s="4">
-        <v>44166.95833333333</v>
+        <v>44167</v>
       </c>
       <c r="H157" s="3" t="s">
         <v>821</v>
@@ -13635,7 +13635,7 @@
         <v>638</v>
       </c>
       <c r="G158" s="4">
-        <v>44166.95833333333</v>
+        <v>44167</v>
       </c>
       <c r="H158" s="3" t="s">
         <v>824</v>
@@ -13696,7 +13696,7 @@
         <v>638</v>
       </c>
       <c r="G159" s="4">
-        <v>44166.95833333333</v>
+        <v>44167</v>
       </c>
       <c r="H159" s="3" t="s">
         <v>827</v>
@@ -13757,7 +13757,7 @@
         <v>638</v>
       </c>
       <c r="G160" s="4">
-        <v>44166.95833333333</v>
+        <v>44167</v>
       </c>
       <c r="H160" s="3" t="s">
         <v>830</v>
@@ -13818,7 +13818,7 @@
         <v>638</v>
       </c>
       <c r="G161" s="4">
-        <v>44166.95833333333</v>
+        <v>44167</v>
       </c>
       <c r="H161" s="3" t="s">
         <v>833</v>
@@ -13879,7 +13879,7 @@
         <v>638</v>
       </c>
       <c r="G162" s="4">
-        <v>44166.95833333333</v>
+        <v>44167</v>
       </c>
       <c r="H162" s="3" t="s">
         <v>836</v>
@@ -13940,7 +13940,7 @@
         <v>638</v>
       </c>
       <c r="G163" s="4">
-        <v>44166.95833333333</v>
+        <v>44167</v>
       </c>
       <c r="H163" s="3" t="s">
         <v>839</v>
@@ -14001,7 +14001,7 @@
         <v>638</v>
       </c>
       <c r="G164" s="4">
-        <v>44166.95833333333</v>
+        <v>44167</v>
       </c>
       <c r="H164" s="3" t="s">
         <v>842</v>
@@ -14062,7 +14062,7 @@
         <v>638</v>
       </c>
       <c r="G165" s="4">
-        <v>44166.95833333333</v>
+        <v>44167</v>
       </c>
       <c r="H165" s="3" t="s">
         <v>845</v>
@@ -14123,7 +14123,7 @@
         <v>638</v>
       </c>
       <c r="G166" s="4">
-        <v>44166.95833333333</v>
+        <v>44167</v>
       </c>
       <c r="H166" s="3" t="s">
         <v>848</v>
@@ -14184,7 +14184,7 @@
         <v>638</v>
       </c>
       <c r="G167" s="4">
-        <v>44166.95833333333</v>
+        <v>44167</v>
       </c>
       <c r="H167" s="3" t="s">
         <v>851</v>
@@ -14245,7 +14245,7 @@
         <v>638</v>
       </c>
       <c r="G168" s="4">
-        <v>44166.95833333333</v>
+        <v>44167</v>
       </c>
       <c r="H168" s="3" t="s">
         <v>854</v>
@@ -14306,7 +14306,7 @@
         <v>638</v>
       </c>
       <c r="G169" s="4">
-        <v>44166.95833333333</v>
+        <v>44167</v>
       </c>
       <c r="H169" s="3" t="s">
         <v>857</v>
@@ -14367,7 +14367,7 @@
         <v>638</v>
       </c>
       <c r="G170" s="4">
-        <v>44166.95833333333</v>
+        <v>44167</v>
       </c>
       <c r="H170" s="3" t="s">
         <v>860</v>
@@ -14428,7 +14428,7 @@
         <v>638</v>
       </c>
       <c r="G171" s="4">
-        <v>44166.95833333333</v>
+        <v>44167</v>
       </c>
       <c r="H171" s="3" t="s">
         <v>863</v>
@@ -14489,7 +14489,7 @@
         <v>638</v>
       </c>
       <c r="G172" s="4">
-        <v>44166.95833333333</v>
+        <v>44167</v>
       </c>
       <c r="H172" s="3" t="s">
         <v>866</v>
@@ -14550,7 +14550,7 @@
         <v>638</v>
       </c>
       <c r="G173" s="4">
-        <v>44166.95833333333</v>
+        <v>44167</v>
       </c>
       <c r="H173" s="3" t="s">
         <v>869</v>
@@ -14611,7 +14611,7 @@
         <v>638</v>
       </c>
       <c r="G174" s="4">
-        <v>44166.95833333333</v>
+        <v>44167</v>
       </c>
       <c r="H174" s="3" t="s">
         <v>872</v>
@@ -14672,7 +14672,7 @@
         <v>638</v>
       </c>
       <c r="G175" s="4">
-        <v>44166.95833333333</v>
+        <v>44167</v>
       </c>
       <c r="H175" s="3" t="s">
         <v>875</v>
@@ -14733,7 +14733,7 @@
         <v>638</v>
       </c>
       <c r="G176" s="4">
-        <v>44166.95833333333</v>
+        <v>44167</v>
       </c>
       <c r="H176" s="3" t="s">
         <v>878</v>
@@ -14794,7 +14794,7 @@
         <v>638</v>
       </c>
       <c r="G177" s="4">
-        <v>44166.95833333333</v>
+        <v>44167</v>
       </c>
       <c r="H177" s="3" t="s">
         <v>881</v>
@@ -14855,7 +14855,7 @@
         <v>638</v>
       </c>
       <c r="G178" s="4">
-        <v>44166.95833333333</v>
+        <v>44167</v>
       </c>
       <c r="H178" s="3" t="s">
         <v>884</v>
@@ -14916,7 +14916,7 @@
         <v>638</v>
       </c>
       <c r="G179" s="4">
-        <v>44166.95833333333</v>
+        <v>44167</v>
       </c>
       <c r="H179" s="3" t="s">
         <v>887</v>
@@ -14977,7 +14977,7 @@
         <v>638</v>
       </c>
       <c r="G180" s="4">
-        <v>44166.95833333333</v>
+        <v>44167</v>
       </c>
       <c r="H180" s="3" t="s">
         <v>890</v>
@@ -15038,7 +15038,7 @@
         <v>638</v>
       </c>
       <c r="G181" s="4">
-        <v>44166.95833333333</v>
+        <v>44167</v>
       </c>
       <c r="H181" s="3" t="s">
         <v>893</v>
@@ -15099,7 +15099,7 @@
         <v>638</v>
       </c>
       <c r="G182" s="4">
-        <v>44166.95833333333</v>
+        <v>44167</v>
       </c>
       <c r="H182" s="3" t="s">
         <v>896</v>
@@ -15160,7 +15160,7 @@
         <v>638</v>
       </c>
       <c r="G183" s="4">
-        <v>44166.95833333333</v>
+        <v>44167</v>
       </c>
       <c r="H183" s="3" t="s">
         <v>898</v>
@@ -15221,7 +15221,7 @@
         <v>638</v>
       </c>
       <c r="G184" s="4">
-        <v>44166.95833333333</v>
+        <v>44167</v>
       </c>
       <c r="H184" s="3" t="s">
         <v>900</v>
@@ -15282,7 +15282,7 @@
         <v>638</v>
       </c>
       <c r="G185" s="4">
-        <v>44166.95833333333</v>
+        <v>44167</v>
       </c>
       <c r="H185" s="3" t="s">
         <v>903</v>
@@ -15343,7 +15343,7 @@
         <v>638</v>
       </c>
       <c r="G186" s="4">
-        <v>44166.95833333333</v>
+        <v>44167</v>
       </c>
       <c r="H186" s="3" t="s">
         <v>905</v>
@@ -15404,7 +15404,7 @@
         <v>638</v>
       </c>
       <c r="G187" s="4">
-        <v>44166.95833333333</v>
+        <v>44167</v>
       </c>
       <c r="H187" s="3" t="s">
         <v>907</v>
@@ -15465,7 +15465,7 @@
         <v>638</v>
       </c>
       <c r="G188" s="4">
-        <v>44166.95833333333</v>
+        <v>44167</v>
       </c>
       <c r="H188" s="3" t="s">
         <v>910</v>
@@ -15587,7 +15587,7 @@
         <v>69</v>
       </c>
       <c r="G190" s="4">
-        <v>44546.95833333333</v>
+        <v>44547</v>
       </c>
       <c r="H190" s="3" t="s">
         <v>921</v>
@@ -15620,7 +15620,7 @@
         <v>928</v>
       </c>
       <c r="R190" s="4">
-        <v>45238.95833333333</v>
+        <v>45239</v>
       </c>
       <c r="S190" s="3"/>
       <c r="T190" s="3" t="s">
@@ -15650,7 +15650,7 @@
         <v>69</v>
       </c>
       <c r="G191" s="4">
-        <v>44546.95833333333</v>
+        <v>44547</v>
       </c>
       <c r="H191" s="3" t="s">
         <v>922</v>
@@ -15683,7 +15683,7 @@
         <v>928</v>
       </c>
       <c r="R191" s="4">
-        <v>45238.95833333333</v>
+        <v>45239</v>
       </c>
       <c r="S191" s="3"/>
       <c r="T191" s="3" t="s">
@@ -15713,7 +15713,7 @@
         <v>933</v>
       </c>
       <c r="G192" s="4">
-        <v>44531.95833333333</v>
+        <v>44532</v>
       </c>
       <c r="H192" s="3" t="s">
         <v>485</v>
@@ -15835,7 +15835,7 @@
         <v>933</v>
       </c>
       <c r="G194" s="4">
-        <v>44594.95833333333</v>
+        <v>44595</v>
       </c>
       <c r="H194" s="3" t="s">
         <v>955</v>
@@ -15896,7 +15896,7 @@
         <v>43</v>
       </c>
       <c r="G195" s="4">
-        <v>44895.95833333333</v>
+        <v>44896</v>
       </c>
       <c r="H195" s="3" t="s">
         <v>966</v>
@@ -15917,13 +15917,13 @@
         <v>970</v>
       </c>
       <c r="N195" s="4">
-        <v>44452.91666666667</v>
+        <v>44453</v>
       </c>
       <c r="O195" s="4">
-        <v>44874.95833333333</v>
+        <v>44875</v>
       </c>
       <c r="P195" s="4">
-        <v>44895.95833333333</v>
+        <v>44896</v>
       </c>
       <c r="Q195" s="3" t="s">
         <v>971</v>
@@ -15957,7 +15957,7 @@
         <v>43</v>
       </c>
       <c r="G196" s="4">
-        <v>44895.95833333333</v>
+        <v>44896</v>
       </c>
       <c r="H196" s="3" t="s">
         <v>974</v>
@@ -15978,13 +15978,13 @@
         <v>970</v>
       </c>
       <c r="N196" s="4">
-        <v>44452.91666666667</v>
+        <v>44453</v>
       </c>
       <c r="O196" s="4">
-        <v>44874.95833333333</v>
+        <v>44875</v>
       </c>
       <c r="P196" s="4">
-        <v>44895.95833333333</v>
+        <v>44896</v>
       </c>
       <c r="Q196" s="3" t="s">
         <v>971</v>
@@ -16018,7 +16018,7 @@
         <v>43</v>
       </c>
       <c r="G197" s="4">
-        <v>44895.95833333333</v>
+        <v>44896</v>
       </c>
       <c r="H197" s="3" t="s">
         <v>977</v>
@@ -16079,7 +16079,7 @@
         <v>43</v>
       </c>
       <c r="G198" s="4">
-        <v>44895.95833333333</v>
+        <v>44896</v>
       </c>
       <c r="H198" s="3" t="s">
         <v>985</v>
@@ -16140,7 +16140,7 @@
         <v>217</v>
       </c>
       <c r="G199" s="4">
-        <v>44640.95833333333</v>
+        <v>44641</v>
       </c>
       <c r="H199" s="3" t="s">
         <v>988</v>
@@ -16205,7 +16205,7 @@
         <v>217</v>
       </c>
       <c r="G200" s="4">
-        <v>44640.95833333333</v>
+        <v>44641</v>
       </c>
       <c r="H200" s="3" t="s">
         <v>989</v>
@@ -16270,7 +16270,7 @@
         <v>69</v>
       </c>
       <c r="G201" s="4">
-        <v>44734.91666666667</v>
+        <v>44735</v>
       </c>
       <c r="H201" s="3" t="s">
         <v>1002</v>
@@ -16331,7 +16331,7 @@
         <v>69</v>
       </c>
       <c r="G202" s="4">
-        <v>44734.91666666667</v>
+        <v>44735</v>
       </c>
       <c r="H202" s="3" t="s">
         <v>1013</v>
@@ -16392,7 +16392,7 @@
         <v>43</v>
       </c>
       <c r="G203" s="4">
-        <v>44895.95833333333</v>
+        <v>44896</v>
       </c>
       <c r="H203" s="3" t="s">
         <v>1017</v>
@@ -16417,7 +16417,7 @@
         <v>33</v>
       </c>
       <c r="P203" s="4">
-        <v>44895.95833333333</v>
+        <v>44896</v>
       </c>
       <c r="Q203" s="3" t="s">
         <v>1021</v>
@@ -16425,7 +16425,7 @@
       <c r="R203" s="3"/>
       <c r="S203" s="3"/>
       <c r="T203" s="4">
-        <v>44844.91666666667</v>
+        <v>44845</v>
       </c>
       <c r="U203" s="3" t="s">
         <v>1022</v>
@@ -16451,7 +16451,7 @@
         <v>43</v>
       </c>
       <c r="G204" s="4">
-        <v>44895.95833333333</v>
+        <v>44896</v>
       </c>
       <c r="H204" s="3" t="s">
         <v>1025</v>
@@ -16476,7 +16476,7 @@
         <v>33</v>
       </c>
       <c r="P204" s="4">
-        <v>44895.95833333333</v>
+        <v>44896</v>
       </c>
       <c r="Q204" s="3" t="s">
         <v>1021</v>
@@ -16484,7 +16484,7 @@
       <c r="R204" s="3"/>
       <c r="S204" s="3"/>
       <c r="T204" s="4">
-        <v>44844.91666666667</v>
+        <v>44845</v>
       </c>
       <c r="U204" s="3" t="s">
         <v>1022</v>
@@ -16510,7 +16510,7 @@
         <v>1029</v>
       </c>
       <c r="G205" s="4">
-        <v>44914.95833333333</v>
+        <v>44915</v>
       </c>
       <c r="H205" s="3" t="s">
         <v>1030</v>
@@ -16531,7 +16531,7 @@
         <v>1035</v>
       </c>
       <c r="N205" s="4">
-        <v>44950.95833333333</v>
+        <v>44951</v>
       </c>
       <c r="O205" s="3" t="s">
         <v>33</v>
@@ -16543,7 +16543,7 @@
         <v>1036</v>
       </c>
       <c r="R205" s="4">
-        <v>45427.91666666667</v>
+        <v>45428</v>
       </c>
       <c r="S205" s="3" t="s">
         <v>33</v>
@@ -16575,7 +16575,7 @@
         <v>1039</v>
       </c>
       <c r="G206" s="4">
-        <v>44914.95833333333</v>
+        <v>44915</v>
       </c>
       <c r="H206" s="3" t="s">
         <v>1040</v>
@@ -16596,7 +16596,7 @@
         <v>1045</v>
       </c>
       <c r="N206" s="4">
-        <v>44950.95833333333</v>
+        <v>44951</v>
       </c>
       <c r="O206" s="3" t="s">
         <v>33</v>
@@ -16640,7 +16640,7 @@
         <v>43</v>
       </c>
       <c r="G207" s="4">
-        <v>45238.95833333333</v>
+        <v>45239</v>
       </c>
       <c r="H207" s="3" t="s">
         <v>1048</v>
@@ -16661,10 +16661,10 @@
         <v>1051</v>
       </c>
       <c r="N207" s="4">
-        <v>44811.91666666667</v>
+        <v>44812</v>
       </c>
       <c r="O207" s="4">
-        <v>45238.95833333333</v>
+        <v>45239</v>
       </c>
       <c r="P207" s="3" t="s">
         <v>33</v>
@@ -16701,7 +16701,7 @@
         <v>43</v>
       </c>
       <c r="G208" s="4">
-        <v>45238.95833333333</v>
+        <v>45239</v>
       </c>
       <c r="H208" s="3" t="s">
         <v>1055</v>
@@ -16722,10 +16722,10 @@
         <v>1051</v>
       </c>
       <c r="N208" s="4">
-        <v>44811.91666666667</v>
+        <v>44812</v>
       </c>
       <c r="O208" s="4">
-        <v>45238.95833333333</v>
+        <v>45239</v>
       </c>
       <c r="P208" s="3" t="s">
         <v>33</v>
@@ -16813,7 +16813,7 @@
         <v>43</v>
       </c>
       <c r="G210" s="4">
-        <v>45488.91666666667</v>
+        <v>45489</v>
       </c>
       <c r="H210" s="3" t="s">
         <v>1065</v>
@@ -16874,7 +16874,7 @@
         <v>43</v>
       </c>
       <c r="G211" s="4">
-        <v>45488.91666666667</v>
+        <v>45489</v>
       </c>
       <c r="H211" s="3" t="s">
         <v>1074</v>
@@ -16935,7 +16935,7 @@
         <v>43</v>
       </c>
       <c r="G212" s="4">
-        <v>44874.95833333333</v>
+        <v>44875</v>
       </c>
       <c r="H212" s="3" t="s">
         <v>1077</v>
@@ -16968,7 +16968,7 @@
         <v>1084</v>
       </c>
       <c r="R212" s="4">
-        <v>45460.91666666667</v>
+        <v>45461</v>
       </c>
       <c r="S212" s="3"/>
       <c r="T212" s="3" t="s">
@@ -16998,7 +16998,7 @@
         <v>43</v>
       </c>
       <c r="G213" s="4">
-        <v>44874.95833333333</v>
+        <v>44875</v>
       </c>
       <c r="H213" s="3" t="s">
         <v>1078</v>
@@ -17031,7 +17031,7 @@
         <v>1084</v>
       </c>
       <c r="R213" s="4">
-        <v>45460.91666666667</v>
+        <v>45461</v>
       </c>
       <c r="S213" s="3"/>
       <c r="T213" s="3" t="s">
@@ -17061,7 +17061,7 @@
         <v>43</v>
       </c>
       <c r="G214" s="4">
-        <v>45130.91666666667</v>
+        <v>45131</v>
       </c>
       <c r="H214" s="3" t="s">
         <v>1089</v>
@@ -17082,10 +17082,10 @@
         <v>1092</v>
       </c>
       <c r="N214" s="4">
-        <v>44872.95833333333</v>
+        <v>44873</v>
       </c>
       <c r="O214" s="4">
-        <v>45238.95833333333</v>
+        <v>45239</v>
       </c>
       <c r="P214" s="3" t="s">
         <v>33</v>
@@ -17122,7 +17122,7 @@
         <v>43</v>
       </c>
       <c r="G215" s="4">
-        <v>45130.91666666667</v>
+        <v>45131</v>
       </c>
       <c r="H215" s="3" t="s">
         <v>1096</v>
@@ -17143,10 +17143,10 @@
         <v>1092</v>
       </c>
       <c r="N215" s="4">
-        <v>44872.95833333333</v>
+        <v>44873</v>
       </c>
       <c r="O215" s="4">
-        <v>45238.95833333333</v>
+        <v>45239</v>
       </c>
       <c r="P215" s="3" t="s">
         <v>33</v>
@@ -17183,7 +17183,7 @@
         <v>547</v>
       </c>
       <c r="G216" s="4">
-        <v>45329.95833333333</v>
+        <v>45330</v>
       </c>
       <c r="H216" s="3" t="s">
         <v>1099</v>
@@ -17244,7 +17244,7 @@
         <v>547</v>
       </c>
       <c r="G217" s="4">
-        <v>45329.95833333333</v>
+        <v>45330</v>
       </c>
       <c r="H217" s="3" t="s">
         <v>1100</v>
@@ -17305,7 +17305,7 @@
         <v>43</v>
       </c>
       <c r="G218" s="4">
-        <v>45307.95833333333</v>
+        <v>45308</v>
       </c>
       <c r="H218" s="3" t="s">
         <v>1113</v>
@@ -17360,7 +17360,7 @@
         <v>43</v>
       </c>
       <c r="G219" s="4">
-        <v>45307.95833333333</v>
+        <v>45308</v>
       </c>
       <c r="H219" s="3" t="s">
         <v>1122</v>
@@ -17415,7 +17415,7 @@
         <v>1039</v>
       </c>
       <c r="G220" s="4">
-        <v>45322.95833333333</v>
+        <v>45323</v>
       </c>
       <c r="H220" s="3" t="s">
         <v>1125</v>
@@ -17476,7 +17476,7 @@
         <v>1039</v>
       </c>
       <c r="G221" s="4">
-        <v>45322.95833333333</v>
+        <v>45323</v>
       </c>
       <c r="H221" s="3" t="s">
         <v>1136</v>
@@ -17537,7 +17537,7 @@
         <v>1039</v>
       </c>
       <c r="G222" s="4">
-        <v>45392.91666666667</v>
+        <v>45393</v>
       </c>
       <c r="H222" s="3" t="s">
         <v>1141</v>
@@ -17598,7 +17598,7 @@
         <v>43</v>
       </c>
       <c r="G223" s="4">
-        <v>45369.95833333333</v>
+        <v>45370</v>
       </c>
       <c r="H223" s="3" t="s">
         <v>1146</v>
@@ -17631,7 +17631,7 @@
         <v>1153</v>
       </c>
       <c r="R223" s="4">
-        <v>45466.91666666667</v>
+        <v>45467</v>
       </c>
       <c r="S223" s="3"/>
       <c r="T223" s="3" t="s">
@@ -17661,7 +17661,7 @@
         <v>43</v>
       </c>
       <c r="G224" s="4">
-        <v>45369.95833333333</v>
+        <v>45370</v>
       </c>
       <c r="H224" s="3" t="s">
         <v>1147</v>
@@ -17694,7 +17694,7 @@
         <v>1153</v>
       </c>
       <c r="R224" s="4">
-        <v>45460.91666666667</v>
+        <v>45461</v>
       </c>
       <c r="S224" s="3"/>
       <c r="T224" s="3" t="s">
@@ -17724,7 +17724,7 @@
         <v>1158</v>
       </c>
       <c r="G225" s="4">
-        <v>45077.91666666667</v>
+        <v>45078</v>
       </c>
       <c r="H225" s="3" t="s">
         <v>1159</v>
@@ -17785,7 +17785,7 @@
         <v>1158</v>
       </c>
       <c r="G226" s="4">
-        <v>45077.91666666667</v>
+        <v>45078</v>
       </c>
       <c r="H226" s="3" t="s">
         <v>1167</v>
@@ -17846,7 +17846,7 @@
         <v>1158</v>
       </c>
       <c r="G227" s="4">
-        <v>45077.91666666667</v>
+        <v>45078</v>
       </c>
       <c r="H227" s="3" t="s">
         <v>1170</v>
@@ -17907,7 +17907,7 @@
         <v>1039</v>
       </c>
       <c r="G228" s="4">
-        <v>45389.91666666667</v>
+        <v>45390</v>
       </c>
       <c r="H228" s="3" t="s">
         <v>1173</v>
@@ -17928,7 +17928,7 @@
         <v>1045</v>
       </c>
       <c r="N228" s="4">
-        <v>45371.95833333333</v>
+        <v>45372</v>
       </c>
       <c r="O228" s="3" t="s">
         <v>33</v>
@@ -17940,7 +17940,7 @@
         <v>1036</v>
       </c>
       <c r="R228" s="4">
-        <v>45427.91666666667</v>
+        <v>45428</v>
       </c>
       <c r="S228" s="3" t="s">
         <v>33</v>
@@ -17972,7 +17972,7 @@
         <v>1158</v>
       </c>
       <c r="G229" s="4">
-        <v>45077.91666666667</v>
+        <v>45078</v>
       </c>
       <c r="H229" s="3" t="s">
         <v>1177</v>
@@ -18033,7 +18033,7 @@
         <v>1158</v>
       </c>
       <c r="G230" s="4">
-        <v>45077.91666666667</v>
+        <v>45078</v>
       </c>
       <c r="H230" s="3" t="s">
         <v>1180</v>
@@ -18094,7 +18094,7 @@
         <v>1158</v>
       </c>
       <c r="G231" s="4">
-        <v>45077.91666666667</v>
+        <v>45078</v>
       </c>
       <c r="H231" s="3" t="s">
         <v>1186</v>
@@ -18155,7 +18155,7 @@
         <v>43</v>
       </c>
       <c r="G232" s="4">
-        <v>45411.91666666667</v>
+        <v>45412</v>
       </c>
       <c r="H232" s="3" t="s">
         <v>1189</v>
@@ -18216,7 +18216,7 @@
         <v>43</v>
       </c>
       <c r="G233" s="4">
-        <v>45411.91666666667</v>
+        <v>45412</v>
       </c>
       <c r="H233" s="3" t="s">
         <v>1190</v>
@@ -18277,7 +18277,7 @@
         <v>43</v>
       </c>
       <c r="G234" s="4">
-        <v>45502.91666666667</v>
+        <v>45503</v>
       </c>
       <c r="H234" s="3" t="s">
         <v>1202</v>
@@ -18338,7 +18338,7 @@
         <v>43</v>
       </c>
       <c r="G235" s="4">
-        <v>45502.91666666667</v>
+        <v>45503</v>
       </c>
       <c r="H235" s="3" t="s">
         <v>1203</v>

</xml_diff>

<commit_message>
generated all the reports on 2024-09-06
</commit_message>
<xml_diff>
--- a/report/merged_configurations.xlsx
+++ b/report/merged_configurations.xlsx
@@ -137,54 +137,54 @@
     <t>Applicatieprofiel Schuldbeheer</t>
   </si>
   <si>
+    <t>ap-schuldbeheer-config.md</t>
+  </si>
+  <si>
+    <t>[{"name":"Agentschap Digitaal Vlaanderen","resourceReference":"https://data.vlaanderen.be/id/organisatie/OVO002949"}]</t>
+  </si>
+  <si>
+    <t>[{"name":"Applicatieprofiel Schuldbeheer","resourceReference":"https://data.vlaanderen.be/doc/applicatieprofiel/schuldbeheer"}]</t>
+  </si>
+  <si>
+    <t>[{"name":"Vocabularium Schuldbeheer","resourceReference":"https://data.vlaanderen.be/ns/schuldbeheer"}]</t>
+  </si>
+  <si>
+    <t>[{"name":"Verslag Business Werkgroep - 4 maart 2024","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-schuldbeheer/standaardenregister/reports/20240304_BusinessWorkshop_Verslag_OSLOSchuldbeheer.pdf"},{"name":"Verslag Werksessie Lokale Besturen - 16 april 2024","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-schuldbeheer/standaardenregister/reports/20240416_WerksessieLokaleBesturen_Verslag_OSLOSchuldbeheer.pdf"},{"name":"Verslag Eerste Thematische Werkgroep - 16 mei 2024","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-schuldbeheer/standaardenregister/reports/20240516_ThematicWorkshop1_Verslag_OSLOSchuldbeheer.pdf"},{"name":"Verslag Tweede Thematische Werkgroep - 11 juni 2024","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-schuldbeheer/standaardenregister/reports/20240611_ThematicWorkshop2_Verslag_OSLOSchuldbeheer.pdf"},{"name":"Verslag Derde Thematische Werkgroep - 2 juli 2024","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-schuldbeheer/standaardenregister/reports/20240702_ThematicWorkshop3_Verslag_OSLOSchuldbeheer.pdf"}]</t>
+  </si>
+  <si>
+    <t>Charter Schuldbeheer</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-schuldbeheer/standaardenregister/charter/Projectcharter_OSLOSchuldbeheer.pdf</t>
+  </si>
+  <si>
+    <t>[{"name":"Presentatie Business Werkgroep - 4 maart 2024","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-schuldbeheer/standaardenregister/presentations/20240304_BusinessWorkshop_Presentatie_OSLOSchuldbeheer.pptx"},{"name":"Presentatie Werksessie Lokale Besturen - 16 april 2024","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-schuldbeheer/standaardenregister/presentations/20240416_PresentatieWerksessieLokaleBesturen.pptx"},{"name":"Presentatie Eerste Thematische Werkgroep - 16 mei 2024","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-schuldbeheer/standaardenregister/presentations/20240516_ThematicWorkshop1_Powerpoint_OSLOSchuldbeheer.pptx"},{"name":"Presentatie Tweede Thematische Werkgroep - 11 juni 2024","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-schuldbeheer/standaardenregister/presentations/20240611_ThematicWorkshop2_Powerpoint_OSLOSchuldbeheer.pptx"},{"name":"Presentatie Derde Thematische Werkgroep - 2 juli 2024","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-schuldbeheer/standaardenregister/presentations/20240702_ThematicWorkshop3_Powerpoint_OSLOSchuldbeheer.pptx"}]</t>
+  </si>
+  <si>
+    <t>21 maart 2024</t>
+  </si>
+  <si>
+    <t>OSLOthema-schuldbeheer</t>
+  </si>
+  <si>
+    <t>{"name":"Charter Schuldbeheer","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-schuldbeheer/standaardenregister/charter/Projectcharter_OSLOSchuldbeheer.pdf"}</t>
+  </si>
+  <si>
+    <t>Vocabularium Schuldbeheer</t>
+  </si>
+  <si>
+    <t>voc-schuldbeheer-config.md</t>
+  </si>
+  <si>
+    <t>Applicatieprofiel Kabels en Leidingen</t>
+  </si>
+  <si>
+    <t>Aanbevolen</t>
+  </si>
+  <si>
     <t>standaard-in-ontwikkeling</t>
   </si>
   <si>
-    <t>ap-schuldbeheer-config.md</t>
-  </si>
-  <si>
-    <t>[{"name":"Agentschap Digitaal Vlaanderen","resourceReference":"https://data.vlaanderen.be/id/organisatie/OVO002949"}]</t>
-  </si>
-  <si>
-    <t>[{"name":"Applicatieprofiel Schuldbeheer","resourceReference":"https://data.vlaanderen.be/doc/applicatieprofiel/schuldbeheer"}]</t>
-  </si>
-  <si>
-    <t>[{"name":"Vocabularium Schuldbeheer","resourceReference":"https://data.vlaanderen.be/ns/schuldbeheer"}]</t>
-  </si>
-  <si>
-    <t>[{"name":"Verslag Business Werkgroep - 4 maart 2024","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-schuldbeheer/standaardenregister/reports/20240304_BusinessWorkshop_Verslag_OSLOSchuldbeheer.pdf"},{"name":"Verslag Werksessie Lokale Besturen - 16 april 2024","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-schuldbeheer/standaardenregister/reports/20240416_WerksessieLokaleBesturen_Verslag_OSLOSchuldbeheer.pdf"},{"name":"Verslag Eerste Thematische Werkgroep - 16 mei 2024","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-schuldbeheer/standaardenregister/reports/20240516_ThematicWorkshop1_Verslag_OSLOSchuldbeheer.pdf"},{"name":"Verslag Tweede Thematische Werkgroep - 11 juni 2024","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-schuldbeheer/standaardenregister/reports/20240611_ThematicWorkshop2_Verslag_OSLOSchuldbeheer.pdf"},{"name":"Verslag Derde Thematische Werkgroep - 2 juli 2024","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-schuldbeheer/standaardenregister/reports/20240702_ThematicWorkshop3_Verslag_OSLOSchuldbeheer.pdf"}]</t>
-  </si>
-  <si>
-    <t>Charter Schuldbeheer</t>
-  </si>
-  <si>
-    <t>https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-schuldbeheer/standaardenregister/charter/Projectcharter_OSLOSchuldbeheer.pdf</t>
-  </si>
-  <si>
-    <t>[{"name":"Presentatie Business Werkgroep - 4 maart 2024","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-schuldbeheer/standaardenregister/presentations/20240304_BusinessWorkshop_Presentatie_OSLOSchuldbeheer.pptx"},{"name":"Presentatie Werksessie Lokale Besturen - 16 april 2024","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-schuldbeheer/standaardenregister/presentations/20240416_PresentatieWerksessieLokaleBesturen.pptx"},{"name":"Presentatie Eerste Thematische Werkgroep - 16 mei 2024","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-schuldbeheer/standaardenregister/presentations/20240516_ThematicWorkshop1_Powerpoint_OSLOSchuldbeheer.pptx"},{"name":"Presentatie Tweede Thematische Werkgroep - 11 juni 2024","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-schuldbeheer/standaardenregister/presentations/20240611_ThematicWorkshop2_Powerpoint_OSLOSchuldbeheer.pptx"},{"name":"Presentatie Derde Thematische Werkgroep - 2 juli 2024","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-schuldbeheer/standaardenregister/presentations/20240702_ThematicWorkshop3_Powerpoint_OSLOSchuldbeheer.pptx"}]</t>
-  </si>
-  <si>
-    <t>21 maart 2024</t>
-  </si>
-  <si>
-    <t>OSLOthema-schuldbeheer</t>
-  </si>
-  <si>
-    <t>{"name":"Charter Schuldbeheer","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-schuldbeheer/standaardenregister/charter/Projectcharter_OSLOSchuldbeheer.pdf"}</t>
-  </si>
-  <si>
-    <t>Vocabularium Schuldbeheer</t>
-  </si>
-  <si>
-    <t>voc-schuldbeheer-config.md</t>
-  </si>
-  <si>
-    <t>Applicatieprofiel Kabels en Leidingen</t>
-  </si>
-  <si>
-    <t>Aanbevolen</t>
-  </si>
-  <si>
     <t>kabels-en-leidingen-description.md</t>
   </si>
   <si>
@@ -587,7 +587,7 @@
     <t>Applicatieprofiel Ruimtelijke Bereiken</t>
   </si>
   <si>
-    <t>[{"name":"Applicatieprofiel Ruimtelijke bereiken","resourceReference":"https://data.vlaanderen.be/doc/applicatieprofiel/bodem-en-ondergrond/ruimtelijke-bereiken/ontwerpstandaard/2021-08-01"}]</t>
+    <t>[{"name":"Applicatieprofiel Ruimtelijke bereiken","resourceReference":"https://data.vlaanderen.be/ns/ruimtelijke-bereiken/"}]</t>
   </si>
   <si>
     <t>[{"name":"Applicatieprofiel Bodem","resourceReference":"https://data.vlaanderen.be/doc/applicatieprofiel/bodem-en-ondergrond/bodem/ontwerpstandaard/2021-08-01"},{"name":"Applicatieprofiel Bodem en Ondergrond","resourceReference":"https://data.vlaanderen.be/doc/applicatieprofiel/bodem-en-ondergrond/bodem-en-ondergrond/kandidaatstandaard/2022-04-28"},{"name":"Applicatieprofiel Bodem en Ondergrond Interpretaties","resourceReference":"https://data.vlaanderen.be/doc/applicatieprofiel/bodem-en-ondergrond/bo-interpretaties/ontwerpstandaard/2021-08-01"},{"name":"Applicatieprofiel Bodem en Ondergrond Observaties","resourceReference":"https://data.vlaanderen.be/doc/applicatieprofiel/bodem-en-ondergrond/bo-observaties/ontwerpstandaard/2021-08-01"},{"name":"Applicatieprofiel Grondboringen","resourceReference":"https://data.vlaanderen.be/doc/applicatieprofiel/bodem-en-ondergrond/grondboringen/ontwerpstandaard/2021-08-01"},{"name":"Applicatieprofiel Grondwatermeetnet","resourceReference":"https://data.vlaanderen.be/doc/applicatieprofiel/bodem-en-ondergrond/grondwatermeetnet/ontwerpstandaard/2021-08-01"},{"name":"Applicatieprofiel Observaties en Metingen","resourceReference":"https://data.vlaanderen.be/doc/applicatieprofiel/observaties-en-metingen/kandidaatstandaard/2022-04-28"},{"name":"Applicatieprofiel Sensoren en Bemonstering","resourceReference":"https://data.vlaanderen.be/doc/applicatieprofiel/sensoren-en-bemonstering/kandidaatstandaard/2022-04-28"},{"name":"Applicatieprofiel Sonderingen","resourceReference":"https://data.vlaanderen.be/doc/applicatieprofiel/bodem-en-ondergrond/sonderingen/ontwerpstandaard/2021-08-01"},{"name":"Vocabularium Bodem","resourceReference":"https://data.vlaanderen.be/doc/vocabularium/bodem-en-ondergrond/bodem/ontwerpstandaard/2021-08-01"},{"name":"Vocabularium Bodem en Ondergrond","resourceReference":"https://data.vlaanderen.be/doc/vocabularium/bodem-en-ondergrond/bodem-en-ondergrond/kandidaatstandaard/2022-04-28"},{"name":"Vocabularium Bodem en Ondergrond Interpretaties","resourceReference":"https://data.vlaanderen.be/doc/vocabularium/bodem-en-ondergrond/bo-interpretaties/ontwerpstandaard/2021-08-01"},{"name":"Vocabularium Bodem en Ondergrond Observaties","resourceReference":"https://data.vlaanderen.be/doc/vocabularium/bodem-en-ondergrond/bo-observaties/ontwerpstandaard/2021-08-01"},{"name":"Vocabularium Grondboringen","resourceReference":"https://data.vlaanderen.be/doc/vocabularium/bodem-en-ondergrond/grondboringen/ontwerpstandaard/2021-08-01"},{"name":"Vocabularium Grondboringen","resourceReference":"https://data.vlaanderen.be/doc/vocabularium/bodem-en-ondergrond/grondboringen/ontwerpstandaard/2021-08-01"},{"name":"Vocabularium Observaties en Metingen","resourceReference":"https://data.vlaanderen.be/doc/vocabularium/observaties-en-metingen/kandidaatstandaard/2022-04-28"},{"name":"Vocabularium Ruimtelijke bereiken","resourceReference":"https://data.vlaanderen.be/doc/vocabularium/bodem-en-ondergrond/ruimtelijke-bereiken/ontwerpstandaard/2021-08-01"},{"name":"Vocabularium Sensoren en Bemonstering","resourceReference":"https://data.vlaanderen.be/doc/vocabularium/sensoren-en-bemonstering/kandidaatstandaard/2022-04-28"},{"name":"Vocabularium Sonderingen","resourceReference":"https://data.vlaanderen.be/doc/vocabularium/bodem-en-ondergrond/sonderingen/ontwerpstandaard/2021-08-01"}]</t>
@@ -4256,37 +4256,37 @@
         <v>23</v>
       </c>
       <c r="D4" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="F4" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="G4" s="4">
+        <v>45540</v>
+      </c>
+      <c r="H4" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="G4" s="4">
-        <v>45496</v>
-      </c>
-      <c r="H4" s="3" t="s">
+      <c r="I4" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="I4" s="3" t="s">
+      <c r="J4" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="J4" s="3" t="s">
+      <c r="K4" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="K4" s="3" t="s">
+      <c r="L4" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="L4" s="3" t="s">
+      <c r="M4" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="M4" s="3" t="s">
+      <c r="N4" s="3" t="s">
         <v>49</v>
-      </c>
-      <c r="N4" s="3" t="s">
-        <v>50</v>
       </c>
       <c r="O4" s="3" t="s">
         <v>33</v>
@@ -4295,20 +4295,22 @@
         <v>33</v>
       </c>
       <c r="Q4" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="R4" s="3"/>
+        <v>50</v>
+      </c>
+      <c r="R4" s="4">
+        <v>45540</v>
+      </c>
       <c r="S4" s="3"/>
       <c r="T4" s="3" t="s">
         <v>35</v>
       </c>
       <c r="U4" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>38</v>
@@ -4317,37 +4319,37 @@
         <v>23</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>41</v>
+        <v>24</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F5" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="G5" s="4">
+        <v>45540</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="I5" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="G5" s="4">
-        <v>45496</v>
-      </c>
-      <c r="H5" s="3" t="s">
+      <c r="J5" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="I5" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="J5" s="3" t="s">
+      <c r="K5" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="K5" s="3" t="s">
+      <c r="L5" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="L5" s="3" t="s">
+      <c r="M5" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="M5" s="3" t="s">
+      <c r="N5" s="3" t="s">
         <v>49</v>
-      </c>
-      <c r="N5" s="3" t="s">
-        <v>50</v>
       </c>
       <c r="O5" s="3" t="s">
         <v>33</v>
@@ -4356,35 +4358,37 @@
         <v>33</v>
       </c>
       <c r="Q5" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="R5" s="3"/>
+        <v>50</v>
+      </c>
+      <c r="R5" s="4">
+        <v>45540</v>
+      </c>
       <c r="S5" s="3"/>
       <c r="T5" s="3" t="s">
         <v>35</v>
       </c>
       <c r="U5" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>22</v>
       </c>
       <c r="C6" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D6" s="3" t="s">
         <v>56</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>41</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>57</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G6" s="3"/>
       <c r="H6" s="3" t="s">
@@ -4434,16 +4438,16 @@
         <v>38</v>
       </c>
       <c r="C7" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D7" s="3" t="s">
         <v>56</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>41</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>57</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G7" s="3"/>
       <c r="H7" s="3" t="s">
@@ -4496,7 +4500,7 @@
         <v>23</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>41</v>
+        <v>56</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>68</v>
@@ -4557,7 +4561,7 @@
         <v>23</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>41</v>
+        <v>56</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>68</v>
@@ -4618,13 +4622,13 @@
         <v>23</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>41</v>
+        <v>56</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>80</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G10" s="4">
         <v>45222</v>
@@ -4673,13 +4677,13 @@
         <v>23</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>41</v>
+        <v>56</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>80</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G11" s="4">
         <v>45222</v>
@@ -4728,13 +4732,13 @@
         <v>23</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>41</v>
+        <v>56</v>
       </c>
       <c r="E12" s="3" t="s">
         <v>91</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G12" s="4">
         <v>45118</v>
@@ -4789,13 +4793,13 @@
         <v>23</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>41</v>
+        <v>56</v>
       </c>
       <c r="E13" s="3" t="s">
         <v>99</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G13" s="4">
         <v>45372</v>
@@ -4848,13 +4852,13 @@
         <v>23</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>41</v>
+        <v>56</v>
       </c>
       <c r="E14" s="3" t="s">
         <v>110</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G14" s="4">
         <v>45372</v>
@@ -4913,7 +4917,7 @@
         <v>114</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G15" s="4">
         <v>45261</v>
@@ -4974,7 +4978,7 @@
         <v>127</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G16" s="4">
         <v>45261</v>
@@ -5151,7 +5155,7 @@
         <v>23</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>41</v>
+        <v>56</v>
       </c>
       <c r="E19" s="3" t="s">
         <v>149</v>
@@ -5212,7 +5216,7 @@
         <v>23</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>41</v>
+        <v>56</v>
       </c>
       <c r="E20" s="3" t="s">
         <v>149</v>
@@ -5395,7 +5399,7 @@
         <v>23</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>41</v>
+        <v>56</v>
       </c>
       <c r="E23" s="3" t="s">
         <v>149</v>
@@ -5456,7 +5460,7 @@
         <v>23</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>41</v>
+        <v>56</v>
       </c>
       <c r="E24" s="3" t="s">
         <v>149</v>
@@ -5517,7 +5521,7 @@
         <v>23</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>41</v>
+        <v>56</v>
       </c>
       <c r="E25" s="3" t="s">
         <v>149</v>
@@ -5578,7 +5582,7 @@
         <v>23</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>41</v>
+        <v>56</v>
       </c>
       <c r="E26" s="3" t="s">
         <v>149</v>
@@ -5639,7 +5643,7 @@
         <v>23</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>41</v>
+        <v>56</v>
       </c>
       <c r="E27" s="3" t="s">
         <v>149</v>
@@ -5700,7 +5704,7 @@
         <v>23</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>41</v>
+        <v>56</v>
       </c>
       <c r="E28" s="3" t="s">
         <v>149</v>
@@ -5761,7 +5765,7 @@
         <v>23</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>41</v>
+        <v>56</v>
       </c>
       <c r="E29" s="3" t="s">
         <v>149</v>
@@ -5822,7 +5826,7 @@
         <v>23</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>41</v>
+        <v>56</v>
       </c>
       <c r="E30" s="3" t="s">
         <v>149</v>
@@ -5883,7 +5887,7 @@
         <v>23</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>41</v>
+        <v>56</v>
       </c>
       <c r="E31" s="3" t="s">
         <v>149</v>
@@ -5892,7 +5896,7 @@
         <v>150</v>
       </c>
       <c r="G31" s="4">
-        <v>44409</v>
+        <v>45539</v>
       </c>
       <c r="H31" s="3" t="s">
         <v>191</v>
@@ -5944,7 +5948,7 @@
         <v>23</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>41</v>
+        <v>56</v>
       </c>
       <c r="E32" s="3" t="s">
         <v>149</v>
@@ -6005,7 +6009,7 @@
         <v>23</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>41</v>
+        <v>56</v>
       </c>
       <c r="E33" s="3" t="s">
         <v>149</v>
@@ -6066,7 +6070,7 @@
         <v>23</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>41</v>
+        <v>56</v>
       </c>
       <c r="E34" s="3" t="s">
         <v>149</v>
@@ -6127,7 +6131,7 @@
         <v>23</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>41</v>
+        <v>56</v>
       </c>
       <c r="E35" s="3" t="s">
         <v>149</v>
@@ -6188,7 +6192,7 @@
         <v>23</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>41</v>
+        <v>56</v>
       </c>
       <c r="E36" s="3" t="s">
         <v>149</v>
@@ -6249,7 +6253,7 @@
         <v>23</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>41</v>
+        <v>56</v>
       </c>
       <c r="E37" s="3" t="s">
         <v>149</v>
@@ -6310,7 +6314,7 @@
         <v>23</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>41</v>
+        <v>56</v>
       </c>
       <c r="E38" s="3" t="s">
         <v>149</v>
@@ -6987,7 +6991,7 @@
         <v>278</v>
       </c>
       <c r="F49" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G49" s="4">
         <v>43284</v>
@@ -7048,7 +7052,7 @@
         <v>291</v>
       </c>
       <c r="F50" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G50" s="4">
         <v>43809</v>
@@ -7109,7 +7113,7 @@
         <v>294</v>
       </c>
       <c r="F51" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G51" s="4">
         <v>43431</v>
@@ -7170,7 +7174,7 @@
         <v>305</v>
       </c>
       <c r="F52" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G52" s="4">
         <v>43809</v>
@@ -7231,7 +7235,7 @@
         <v>309</v>
       </c>
       <c r="F53" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G53" s="4">
         <v>43503</v>
@@ -7292,7 +7296,7 @@
         <v>319</v>
       </c>
       <c r="F54" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G54" s="4">
         <v>43503</v>
@@ -7353,7 +7357,7 @@
         <v>322</v>
       </c>
       <c r="F55" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G55" s="4">
         <v>43284</v>
@@ -7414,7 +7418,7 @@
         <v>330</v>
       </c>
       <c r="F56" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G56" s="4">
         <v>43809</v>
@@ -7536,7 +7540,7 @@
         <v>346</v>
       </c>
       <c r="F58" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G58" s="4">
         <v>43284</v>
@@ -7597,7 +7601,7 @@
         <v>356</v>
       </c>
       <c r="F59" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G59" s="4">
         <v>43284</v>
@@ -7780,7 +7784,7 @@
         <v>375</v>
       </c>
       <c r="F62" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G62" s="4">
         <v>43809</v>
@@ -7841,7 +7845,7 @@
         <v>382</v>
       </c>
       <c r="F63" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G63" s="4">
         <v>43284</v>
@@ -7902,7 +7906,7 @@
         <v>390</v>
       </c>
       <c r="F64" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G64" s="4">
         <v>43412</v>
@@ -7963,7 +7967,7 @@
         <v>394</v>
       </c>
       <c r="F65" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G65" s="4">
         <v>43412</v>
@@ -8024,7 +8028,7 @@
         <v>397</v>
       </c>
       <c r="F66" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G66" s="4">
         <v>43944</v>
@@ -8085,7 +8089,7 @@
         <v>405</v>
       </c>
       <c r="F67" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G67" s="4">
         <v>43503</v>
@@ -8146,7 +8150,7 @@
         <v>412</v>
       </c>
       <c r="F68" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G68" s="4">
         <v>43503</v>
@@ -8207,7 +8211,7 @@
         <v>415</v>
       </c>
       <c r="F69" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G69" s="4">
         <v>43503</v>
@@ -8268,7 +8272,7 @@
         <v>423</v>
       </c>
       <c r="F70" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G70" s="4">
         <v>43503</v>
@@ -8329,7 +8333,7 @@
         <v>426</v>
       </c>
       <c r="F71" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G71" s="4">
         <v>43503</v>
@@ -8878,7 +8882,7 @@
         <v>484</v>
       </c>
       <c r="F80" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G80" s="4">
         <v>44532</v>
@@ -8939,7 +8943,7 @@
         <v>498</v>
       </c>
       <c r="F81" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G81" s="4">
         <v>43503</v>
@@ -9000,7 +9004,7 @@
         <v>511</v>
       </c>
       <c r="F82" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G82" s="4">
         <v>43503</v>
@@ -9061,7 +9065,7 @@
         <v>519</v>
       </c>
       <c r="F83" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G83" s="4">
         <v>43503</v>
@@ -9671,7 +9675,7 @@
         <v>574</v>
       </c>
       <c r="F93" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G93" s="4">
         <v>43242</v>
@@ -9732,7 +9736,7 @@
         <v>574</v>
       </c>
       <c r="F94" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G94" s="4">
         <v>43242</v>
@@ -9793,7 +9797,7 @@
         <v>585</v>
       </c>
       <c r="F95" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G95" s="4">
         <v>43242</v>
@@ -9854,7 +9858,7 @@
         <v>595</v>
       </c>
       <c r="F96" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G96" s="4">
         <v>43431</v>
@@ -9915,7 +9919,7 @@
         <v>595</v>
       </c>
       <c r="F97" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G97" s="4">
         <v>43431</v>
@@ -9976,7 +9980,7 @@
         <v>595</v>
       </c>
       <c r="F98" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G98" s="4">
         <v>43431</v>
@@ -10037,7 +10041,7 @@
         <v>595</v>
       </c>
       <c r="F99" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G99" s="4">
         <v>43431</v>
@@ -10098,7 +10102,7 @@
         <v>595</v>
       </c>
       <c r="F100" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G100" s="4">
         <v>43431</v>
@@ -10159,7 +10163,7 @@
         <v>595</v>
       </c>
       <c r="F101" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G101" s="4">
         <v>43431</v>
@@ -10220,7 +10224,7 @@
         <v>595</v>
       </c>
       <c r="F102" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G102" s="4">
         <v>43431</v>
@@ -10281,7 +10285,7 @@
         <v>618</v>
       </c>
       <c r="F103" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G103" s="4">
         <v>43431</v>
@@ -10342,7 +10346,7 @@
         <v>618</v>
       </c>
       <c r="F104" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G104" s="4">
         <v>43431</v>
@@ -10403,7 +10407,7 @@
         <v>618</v>
       </c>
       <c r="F105" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G105" s="4">
         <v>43431</v>
@@ -10464,7 +10468,7 @@
         <v>618</v>
       </c>
       <c r="F106" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G106" s="4">
         <v>43431</v>
@@ -10525,7 +10529,7 @@
         <v>618</v>
       </c>
       <c r="F107" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G107" s="4">
         <v>43431</v>
@@ -10586,7 +10590,7 @@
         <v>618</v>
       </c>
       <c r="F108" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G108" s="4">
         <v>43431</v>
@@ -10647,7 +10651,7 @@
         <v>618</v>
       </c>
       <c r="F109" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G109" s="4">
         <v>43431</v>
@@ -10708,7 +10712,7 @@
         <v>618</v>
       </c>
       <c r="F110" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G110" s="4">
         <v>43431</v>
@@ -10769,7 +10773,7 @@
         <v>618</v>
       </c>
       <c r="F111" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G111" s="4">
         <v>43431</v>
@@ -11316,7 +11320,7 @@
       </c>
       <c r="E120" s="3"/>
       <c r="F120" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G120" s="4">
         <v>42817</v>
@@ -11375,7 +11379,7 @@
       </c>
       <c r="E121" s="3"/>
       <c r="F121" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G121" s="4">
         <v>42825</v>
@@ -11436,7 +11440,7 @@
         <v>618</v>
       </c>
       <c r="F122" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G122" s="4">
         <v>44469</v>
@@ -11497,7 +11501,7 @@
         <v>618</v>
       </c>
       <c r="F123" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G123" s="4">
         <v>44469</v>
@@ -11558,7 +11562,7 @@
         <v>618</v>
       </c>
       <c r="F124" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G124" s="4">
         <v>44469</v>
@@ -11619,7 +11623,7 @@
         <v>618</v>
       </c>
       <c r="F125" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G125" s="4">
         <v>44469</v>
@@ -11680,7 +11684,7 @@
         <v>618</v>
       </c>
       <c r="F126" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G126" s="4">
         <v>44469</v>
@@ -11741,7 +11745,7 @@
         <v>618</v>
       </c>
       <c r="F127" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G127" s="4">
         <v>44469</v>
@@ -11802,7 +11806,7 @@
         <v>618</v>
       </c>
       <c r="F128" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G128" s="4">
         <v>44469</v>
@@ -11863,7 +11867,7 @@
         <v>618</v>
       </c>
       <c r="F129" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G129" s="4">
         <v>44469</v>
@@ -11924,7 +11928,7 @@
         <v>618</v>
       </c>
       <c r="F130" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G130" s="4">
         <v>44469</v>
@@ -11985,7 +11989,7 @@
         <v>618</v>
       </c>
       <c r="F131" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G131" s="4">
         <v>44469</v>
@@ -12046,7 +12050,7 @@
         <v>618</v>
       </c>
       <c r="F132" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G132" s="4">
         <v>44469</v>
@@ -12107,7 +12111,7 @@
         <v>730</v>
       </c>
       <c r="F133" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G133" s="4">
         <v>44469</v>
@@ -12168,7 +12172,7 @@
         <v>733</v>
       </c>
       <c r="F134" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G134" s="4">
         <v>44469</v>
@@ -12229,7 +12233,7 @@
         <v>733</v>
       </c>
       <c r="F135" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G135" s="4">
         <v>44469</v>
@@ -12290,7 +12294,7 @@
         <v>733</v>
       </c>
       <c r="F136" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G136" s="4">
         <v>44469</v>
@@ -12351,7 +12355,7 @@
         <v>733</v>
       </c>
       <c r="F137" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G137" s="4">
         <v>44469</v>
@@ -12412,7 +12416,7 @@
         <v>733</v>
       </c>
       <c r="F138" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G138" s="4">
         <v>44469</v>
@@ -12473,7 +12477,7 @@
         <v>733</v>
       </c>
       <c r="F139" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G139" s="4">
         <v>44469</v>
@@ -12534,7 +12538,7 @@
         <v>733</v>
       </c>
       <c r="F140" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G140" s="4">
         <v>44469</v>
@@ -12595,7 +12599,7 @@
         <v>733</v>
       </c>
       <c r="F141" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G141" s="4">
         <v>44469</v>
@@ -12656,7 +12660,7 @@
         <v>733</v>
       </c>
       <c r="F142" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G142" s="4">
         <v>44469</v>
@@ -12711,7 +12715,7 @@
         <v>33</v>
       </c>
       <c r="D143" s="3" t="s">
-        <v>41</v>
+        <v>56</v>
       </c>
       <c r="E143" s="3" t="s">
         <v>752</v>
@@ -12772,7 +12776,7 @@
         <v>33</v>
       </c>
       <c r="D144" s="3" t="s">
-        <v>41</v>
+        <v>56</v>
       </c>
       <c r="E144" s="3" t="s">
         <v>761</v>
@@ -15517,7 +15521,7 @@
         <v>33</v>
       </c>
       <c r="D189" s="3" t="s">
-        <v>41</v>
+        <v>56</v>
       </c>
       <c r="E189" s="3" t="s">
         <v>912</v>
@@ -15765,13 +15769,13 @@
         <v>23</v>
       </c>
       <c r="D193" s="3" t="s">
-        <v>41</v>
+        <v>56</v>
       </c>
       <c r="E193" s="3" t="s">
         <v>944</v>
       </c>
       <c r="F193" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G193" s="3" t="s">
         <v>33</v>
@@ -15893,7 +15897,7 @@
         <v>965</v>
       </c>
       <c r="F195" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G195" s="4">
         <v>44896</v>
@@ -15954,7 +15958,7 @@
         <v>965</v>
       </c>
       <c r="F196" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G196" s="4">
         <v>44896</v>
@@ -16015,7 +16019,7 @@
         <v>976</v>
       </c>
       <c r="F197" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G197" s="4">
         <v>44896</v>
@@ -16076,7 +16080,7 @@
         <v>976</v>
       </c>
       <c r="F198" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G198" s="4">
         <v>44896</v>
@@ -16389,7 +16393,7 @@
         <v>1016</v>
       </c>
       <c r="F203" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G203" s="4">
         <v>44896</v>
@@ -16448,7 +16452,7 @@
         <v>1024</v>
       </c>
       <c r="F204" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G204" s="4">
         <v>44896</v>
@@ -16566,7 +16570,7 @@
         <v>23</v>
       </c>
       <c r="D206" s="3" t="s">
-        <v>41</v>
+        <v>56</v>
       </c>
       <c r="E206" s="3" t="s">
         <v>1028</v>
@@ -16637,7 +16641,7 @@
         <v>91</v>
       </c>
       <c r="F207" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G207" s="4">
         <v>45239</v>
@@ -16698,7 +16702,7 @@
         <v>91</v>
       </c>
       <c r="F208" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G208" s="4">
         <v>45239</v>
@@ -16753,11 +16757,11 @@
         <v>23</v>
       </c>
       <c r="D209" s="3" t="s">
-        <v>41</v>
+        <v>56</v>
       </c>
       <c r="E209" s="3"/>
       <c r="F209" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G209" s="3"/>
       <c r="H209" s="3" t="s">
@@ -16804,13 +16808,13 @@
         <v>23</v>
       </c>
       <c r="D210" s="3" t="s">
-        <v>41</v>
+        <v>56</v>
       </c>
       <c r="E210" s="3" t="s">
         <v>1064</v>
       </c>
       <c r="F210" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G210" s="4">
         <v>45489</v>
@@ -16865,13 +16869,13 @@
         <v>23</v>
       </c>
       <c r="D211" s="3" t="s">
-        <v>41</v>
+        <v>56</v>
       </c>
       <c r="E211" s="3" t="s">
         <v>1064</v>
       </c>
       <c r="F211" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G211" s="4">
         <v>45489</v>
@@ -16932,7 +16936,7 @@
         <v>1076</v>
       </c>
       <c r="F212" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G212" s="4">
         <v>44875</v>
@@ -16995,7 +16999,7 @@
         <v>1087</v>
       </c>
       <c r="F213" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G213" s="4">
         <v>44875</v>
@@ -17058,7 +17062,7 @@
         <v>91</v>
       </c>
       <c r="F214" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G214" s="4">
         <v>45131</v>
@@ -17119,7 +17123,7 @@
         <v>91</v>
       </c>
       <c r="F215" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G215" s="4">
         <v>45131</v>
@@ -17296,13 +17300,13 @@
         <v>23</v>
       </c>
       <c r="D218" s="3" t="s">
-        <v>41</v>
+        <v>56</v>
       </c>
       <c r="E218" s="3" t="s">
         <v>91</v>
       </c>
       <c r="F218" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G218" s="4">
         <v>45308</v>
@@ -17351,13 +17355,13 @@
         <v>23</v>
       </c>
       <c r="D219" s="3" t="s">
-        <v>41</v>
+        <v>56</v>
       </c>
       <c r="E219" s="3" t="s">
         <v>91</v>
       </c>
       <c r="F219" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G219" s="4">
         <v>45308</v>
@@ -17595,7 +17599,7 @@
         <v>1145</v>
       </c>
       <c r="F223" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G223" s="4">
         <v>45370</v>
@@ -17658,7 +17662,7 @@
         <v>1145</v>
       </c>
       <c r="F224" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G224" s="4">
         <v>45370</v>
@@ -18152,7 +18156,7 @@
         <v>1188</v>
       </c>
       <c r="F232" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G232" s="4">
         <v>45412</v>
@@ -18176,7 +18180,7 @@
         <v>1194</v>
       </c>
       <c r="N232" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="O232" s="3" t="s">
         <v>33</v>
@@ -18213,7 +18217,7 @@
         <v>1198</v>
       </c>
       <c r="F233" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G233" s="4">
         <v>45412</v>
@@ -18237,7 +18241,7 @@
         <v>1194</v>
       </c>
       <c r="N233" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="O233" s="3" t="s">
         <v>33</v>
@@ -18268,13 +18272,13 @@
         <v>1200</v>
       </c>
       <c r="D234" s="3" t="s">
-        <v>41</v>
+        <v>56</v>
       </c>
       <c r="E234" s="3" t="s">
         <v>1201</v>
       </c>
       <c r="F234" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G234" s="4">
         <v>45503</v>
@@ -18329,13 +18333,13 @@
         <v>1200</v>
       </c>
       <c r="D235" s="3" t="s">
-        <v>41</v>
+        <v>56</v>
       </c>
       <c r="E235" s="3" t="s">
         <v>1201</v>
       </c>
       <c r="F235" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G235" s="4">
         <v>45503</v>
@@ -18601,8 +18605,8 @@
       <c r="M4" s="6" t="b">
         <v>0</v>
       </c>
-      <c r="N4" s="6" t="b">
-        <v>0</v>
+      <c r="N4" s="5" t="b">
+        <v>1</v>
       </c>
       <c r="O4" s="6" t="b">
         <v>0</v>
@@ -18619,7 +18623,7 @@
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B5" s="5" t="b">
         <v>1</v>
@@ -18657,8 +18661,8 @@
       <c r="M5" s="6" t="b">
         <v>0</v>
       </c>
-      <c r="N5" s="6" t="b">
-        <v>0</v>
+      <c r="N5" s="5" t="b">
+        <v>1</v>
       </c>
       <c r="O5" s="6" t="b">
         <v>0</v>
@@ -18675,7 +18679,7 @@
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B6" s="5" t="b">
         <v>1</v>

</xml_diff>

<commit_message>
generated all the reports on 2024-09-18
</commit_message>
<xml_diff>
--- a/report/merged_configurations.xlsx
+++ b/report/merged_configurations.xlsx
@@ -17978,7 +17978,9 @@
       <c r="Q232" s="3" t="s">
         <v>1125</v>
       </c>
-      <c r="R232" s="3"/>
+      <c r="R232" s="4">
+        <v>45534</v>
+      </c>
       <c r="S232" s="3"/>
       <c r="T232" s="3" t="s">
         <v>35</v>
@@ -18039,7 +18041,9 @@
       <c r="Q233" s="3" t="s">
         <v>1125</v>
       </c>
-      <c r="R233" s="3"/>
+      <c r="R233" s="4">
+        <v>45534</v>
+      </c>
       <c r="S233" s="3"/>
       <c r="T233" s="3" t="s">
         <v>35</v>
@@ -31160,8 +31164,8 @@
       <c r="M232" s="6" t="b">
         <v>0</v>
       </c>
-      <c r="N232" s="6" t="b">
-        <v>0</v>
+      <c r="N232" s="5" t="b">
+        <v>1</v>
       </c>
       <c r="O232" s="6" t="b">
         <v>0</v>
@@ -31216,8 +31220,8 @@
       <c r="M233" s="6" t="b">
         <v>0</v>
       </c>
-      <c r="N233" s="6" t="b">
-        <v>0</v>
+      <c r="N233" s="5" t="b">
+        <v>1</v>
       </c>
       <c r="O233" s="6" t="b">
         <v>0</v>

</xml_diff>

<commit_message>
generated all the reports on 2024-11-06
</commit_message>
<xml_diff>
--- a/report/merged_configurations.xlsx
+++ b/report/merged_configurations.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3967" uniqueCount="1160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3967" uniqueCount="1161">
   <si>
     <t>title</t>
   </si>
@@ -3144,6 +3144,9 @@
   </si>
   <si>
     <t>Implementatiemodel Kwaliteit Wegen en Wegmarkeringen</t>
+  </si>
+  <si>
+    <t>[{"name":"stad Roeselare","resourceReference":"https://data.vlaanderen.be/id/organisatie/OVO002220"}]</t>
   </si>
   <si>
     <t>[{"name":"Implementatiemodel Kwaliteit Wegen en Wegmarkeringen","resourceReference":"https://implementatie.data.vlaanderen.be/doc/implementatiemodel/kwaliteit-wegen-en-wegmarkeringen/"}]</t>
@@ -16909,28 +16912,28 @@
         <v>90</v>
       </c>
       <c r="F214" s="3" t="s">
-        <v>42</v>
+        <v>1044</v>
       </c>
       <c r="G214" s="4">
         <v>45131</v>
       </c>
       <c r="H214" s="3" t="s">
-        <v>1044</v>
+        <v>1045</v>
       </c>
       <c r="I214" s="3" t="s">
         <v>28</v>
       </c>
       <c r="J214" s="3" t="s">
-        <v>1045</v>
+        <v>1046</v>
       </c>
       <c r="K214" s="3" t="s">
         <v>30</v>
       </c>
       <c r="L214" s="3" t="s">
-        <v>1046</v>
+        <v>1047</v>
       </c>
       <c r="M214" s="3" t="s">
-        <v>1047</v>
+        <v>1048</v>
       </c>
       <c r="N214" s="4">
         <v>44873</v>
@@ -16942,7 +16945,7 @@
         <v>33</v>
       </c>
       <c r="Q214" s="3" t="s">
-        <v>1048</v>
+        <v>1049</v>
       </c>
       <c r="R214" s="3"/>
       <c r="S214" s="3"/>
@@ -16950,12 +16953,12 @@
         <v>35</v>
       </c>
       <c r="U214" s="3" t="s">
-        <v>1049</v>
+        <v>1050</v>
       </c>
     </row>
     <row r="215" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A215" s="3" t="s">
-        <v>1050</v>
+        <v>1051</v>
       </c>
       <c r="B215" s="3" t="s">
         <v>38</v>
@@ -16970,28 +16973,28 @@
         <v>90</v>
       </c>
       <c r="F215" s="3" t="s">
-        <v>42</v>
+        <v>1044</v>
       </c>
       <c r="G215" s="4">
         <v>45131</v>
       </c>
       <c r="H215" s="3" t="s">
-        <v>1051</v>
+        <v>1052</v>
       </c>
       <c r="I215" s="3" t="s">
         <v>28</v>
       </c>
       <c r="J215" s="3" t="s">
-        <v>1045</v>
+        <v>1046</v>
       </c>
       <c r="K215" s="3" t="s">
         <v>30</v>
       </c>
       <c r="L215" s="3" t="s">
-        <v>1046</v>
+        <v>1047</v>
       </c>
       <c r="M215" s="3" t="s">
-        <v>1047</v>
+        <v>1048</v>
       </c>
       <c r="N215" s="4">
         <v>44873</v>
@@ -17003,7 +17006,7 @@
         <v>33</v>
       </c>
       <c r="Q215" s="3" t="s">
-        <v>1048</v>
+        <v>1049</v>
       </c>
       <c r="R215" s="3"/>
       <c r="S215" s="3"/>
@@ -17011,12 +17014,12 @@
         <v>35</v>
       </c>
       <c r="U215" s="3" t="s">
-        <v>1049</v>
+        <v>1050</v>
       </c>
     </row>
     <row r="216" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A216" s="3" t="s">
-        <v>1052</v>
+        <v>1053</v>
       </c>
       <c r="B216" s="3" t="s">
         <v>22</v>
@@ -17028,7 +17031,7 @@
         <v>24</v>
       </c>
       <c r="E216" s="3" t="s">
-        <v>1053</v>
+        <v>1054</v>
       </c>
       <c r="F216" s="3" t="s">
         <v>521</v>
@@ -17037,22 +17040,22 @@
         <v>45330</v>
       </c>
       <c r="H216" s="3" t="s">
-        <v>1054</v>
+        <v>1055</v>
       </c>
       <c r="I216" s="3" t="s">
-        <v>1055</v>
+        <v>1056</v>
       </c>
       <c r="J216" s="3" t="s">
-        <v>1056</v>
+        <v>1057</v>
       </c>
       <c r="K216" s="3" t="s">
-        <v>1057</v>
+        <v>1058</v>
       </c>
       <c r="L216" s="3" t="s">
-        <v>1058</v>
+        <v>1059</v>
       </c>
       <c r="M216" s="3" t="s">
-        <v>1059</v>
+        <v>1060</v>
       </c>
       <c r="N216" s="4">
         <v>45237</v>
@@ -17064,7 +17067,7 @@
         <v>33</v>
       </c>
       <c r="Q216" s="3" t="s">
-        <v>1060</v>
+        <v>1061</v>
       </c>
       <c r="R216" s="3"/>
       <c r="S216" s="3"/>
@@ -17072,12 +17075,12 @@
         <v>35</v>
       </c>
       <c r="U216" s="3" t="s">
-        <v>1061</v>
+        <v>1062</v>
       </c>
     </row>
     <row r="217" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A217" s="3" t="s">
-        <v>1062</v>
+        <v>1063</v>
       </c>
       <c r="B217" s="3" t="s">
         <v>38</v>
@@ -17089,7 +17092,7 @@
         <v>24</v>
       </c>
       <c r="E217" s="3" t="s">
-        <v>1063</v>
+        <v>1064</v>
       </c>
       <c r="F217" s="3" t="s">
         <v>521</v>
@@ -17098,22 +17101,22 @@
         <v>45330</v>
       </c>
       <c r="H217" s="3" t="s">
+        <v>1056</v>
+      </c>
+      <c r="I217" s="3" t="s">
         <v>1055</v>
       </c>
-      <c r="I217" s="3" t="s">
-        <v>1054</v>
-      </c>
       <c r="J217" s="3" t="s">
-        <v>1056</v>
+        <v>1057</v>
       </c>
       <c r="K217" s="3" t="s">
-        <v>1057</v>
+        <v>1058</v>
       </c>
       <c r="L217" s="3" t="s">
-        <v>1058</v>
+        <v>1059</v>
       </c>
       <c r="M217" s="3" t="s">
-        <v>1059</v>
+        <v>1060</v>
       </c>
       <c r="N217" s="4">
         <v>45237</v>
@@ -17125,7 +17128,7 @@
         <v>33</v>
       </c>
       <c r="Q217" s="3" t="s">
-        <v>1060</v>
+        <v>1061</v>
       </c>
       <c r="R217" s="3"/>
       <c r="S217" s="3"/>
@@ -17133,15 +17136,15 @@
         <v>35</v>
       </c>
       <c r="U217" s="3" t="s">
-        <v>1061</v>
+        <v>1062</v>
       </c>
     </row>
     <row r="218" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A218" s="3" t="s">
-        <v>1064</v>
+        <v>1065</v>
       </c>
       <c r="B218" s="3" t="s">
-        <v>1065</v>
+        <v>1066</v>
       </c>
       <c r="C218" s="3" t="s">
         <v>23</v>
@@ -17159,28 +17162,28 @@
         <v>45308</v>
       </c>
       <c r="H218" s="3" t="s">
-        <v>1066</v>
+        <v>1067</v>
       </c>
       <c r="I218" s="3" t="s">
         <v>28</v>
       </c>
       <c r="J218" s="3" t="s">
-        <v>1067</v>
+        <v>1068</v>
       </c>
       <c r="K218" s="3" t="s">
-        <v>1068</v>
+        <v>1069</v>
       </c>
       <c r="L218" s="3" t="s">
-        <v>1069</v>
+        <v>1070</v>
       </c>
       <c r="M218" s="3" t="s">
-        <v>1070</v>
+        <v>1071</v>
       </c>
       <c r="N218" s="3"/>
       <c r="O218" s="3"/>
       <c r="P218" s="3"/>
       <c r="Q218" s="3" t="s">
-        <v>1071</v>
+        <v>1072</v>
       </c>
       <c r="R218" s="3"/>
       <c r="S218" s="3"/>
@@ -17188,15 +17191,15 @@
         <v>35</v>
       </c>
       <c r="U218" s="3" t="s">
-        <v>1072</v>
+        <v>1073</v>
       </c>
     </row>
     <row r="219" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A219" s="3" t="s">
-        <v>1073</v>
+        <v>1074</v>
       </c>
       <c r="B219" s="3" t="s">
-        <v>1074</v>
+        <v>1075</v>
       </c>
       <c r="C219" s="3" t="s">
         <v>23</v>
@@ -17214,28 +17217,28 @@
         <v>45308</v>
       </c>
       <c r="H219" s="3" t="s">
-        <v>1075</v>
+        <v>1076</v>
       </c>
       <c r="I219" s="3" t="s">
         <v>28</v>
       </c>
       <c r="J219" s="3" t="s">
-        <v>1067</v>
+        <v>1068</v>
       </c>
       <c r="K219" s="3" t="s">
-        <v>1068</v>
+        <v>1069</v>
       </c>
       <c r="L219" s="3" t="s">
-        <v>1069</v>
+        <v>1070</v>
       </c>
       <c r="M219" s="3" t="s">
-        <v>1070</v>
+        <v>1071</v>
       </c>
       <c r="N219" s="3"/>
       <c r="O219" s="3"/>
       <c r="P219" s="3"/>
       <c r="Q219" s="3" t="s">
-        <v>1071</v>
+        <v>1072</v>
       </c>
       <c r="R219" s="3"/>
       <c r="S219" s="3"/>
@@ -17243,12 +17246,12 @@
         <v>35</v>
       </c>
       <c r="U219" s="3" t="s">
-        <v>1072</v>
+        <v>1073</v>
       </c>
     </row>
     <row r="220" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A220" s="3" t="s">
-        <v>1076</v>
+        <v>1077</v>
       </c>
       <c r="B220" s="3" t="s">
         <v>22</v>
@@ -17260,7 +17263,7 @@
         <v>24</v>
       </c>
       <c r="E220" s="3" t="s">
-        <v>1077</v>
+        <v>1078</v>
       </c>
       <c r="F220" s="3" t="s">
         <v>996</v>
@@ -17269,22 +17272,22 @@
         <v>45323</v>
       </c>
       <c r="H220" s="3" t="s">
-        <v>1078</v>
+        <v>1079</v>
       </c>
       <c r="I220" s="3" t="s">
-        <v>1079</v>
+        <v>1080</v>
       </c>
       <c r="J220" s="3" t="s">
-        <v>1080</v>
+        <v>1081</v>
       </c>
       <c r="K220" s="3" t="s">
-        <v>1081</v>
+        <v>1082</v>
       </c>
       <c r="L220" s="3" t="s">
-        <v>1082</v>
+        <v>1083</v>
       </c>
       <c r="M220" s="3" t="s">
-        <v>1083</v>
+        <v>1084</v>
       </c>
       <c r="N220" s="4">
         <v>45316</v>
@@ -17296,7 +17299,7 @@
         <v>33</v>
       </c>
       <c r="Q220" s="3" t="s">
-        <v>1084</v>
+        <v>1085</v>
       </c>
       <c r="R220" s="3"/>
       <c r="S220" s="3"/>
@@ -17304,12 +17307,12 @@
         <v>35</v>
       </c>
       <c r="U220" s="3" t="s">
-        <v>1085</v>
+        <v>1086</v>
       </c>
     </row>
     <row r="221" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A221" s="3" t="s">
-        <v>1086</v>
+        <v>1087</v>
       </c>
       <c r="B221" s="3" t="s">
         <v>38</v>
@@ -17321,7 +17324,7 @@
         <v>24</v>
       </c>
       <c r="E221" s="3" t="s">
-        <v>1087</v>
+        <v>1088</v>
       </c>
       <c r="F221" s="3" t="s">
         <v>996</v>
@@ -17330,22 +17333,22 @@
         <v>45323</v>
       </c>
       <c r="H221" s="3" t="s">
-        <v>1088</v>
+        <v>1089</v>
       </c>
       <c r="I221" s="3" t="s">
-        <v>1089</v>
+        <v>1090</v>
       </c>
       <c r="J221" s="3" t="s">
-        <v>1090</v>
+        <v>1091</v>
       </c>
       <c r="K221" s="3" t="s">
-        <v>1081</v>
+        <v>1082</v>
       </c>
       <c r="L221" s="3" t="s">
-        <v>1082</v>
+        <v>1083</v>
       </c>
       <c r="M221" s="3" t="s">
-        <v>1083</v>
+        <v>1084</v>
       </c>
       <c r="N221" s="4">
         <v>45316</v>
@@ -17357,7 +17360,7 @@
         <v>33</v>
       </c>
       <c r="Q221" s="3" t="s">
-        <v>1084</v>
+        <v>1085</v>
       </c>
       <c r="R221" s="3"/>
       <c r="S221" s="3"/>
@@ -17365,12 +17368,12 @@
         <v>35</v>
       </c>
       <c r="U221" s="3" t="s">
-        <v>1085</v>
+        <v>1086</v>
       </c>
     </row>
     <row r="222" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A222" s="3" t="s">
-        <v>1091</v>
+        <v>1092</v>
       </c>
       <c r="B222" s="3" t="s">
         <v>38</v>
@@ -17382,7 +17385,7 @@
         <v>24</v>
       </c>
       <c r="E222" s="3" t="s">
-        <v>1092</v>
+        <v>1093</v>
       </c>
       <c r="F222" s="3" t="s">
         <v>996</v>
@@ -17391,22 +17394,22 @@
         <v>45393</v>
       </c>
       <c r="H222" s="3" t="s">
-        <v>1093</v>
+        <v>1094</v>
       </c>
       <c r="I222" s="3" t="s">
-        <v>1094</v>
+        <v>1095</v>
       </c>
       <c r="J222" s="3" t="s">
-        <v>1095</v>
+        <v>1096</v>
       </c>
       <c r="K222" s="3" t="s">
-        <v>1081</v>
+        <v>1082</v>
       </c>
       <c r="L222" s="3" t="s">
-        <v>1082</v>
+        <v>1083</v>
       </c>
       <c r="M222" s="3" t="s">
-        <v>1083</v>
+        <v>1084</v>
       </c>
       <c r="N222" s="4">
         <v>45316</v>
@@ -17418,7 +17421,7 @@
         <v>33</v>
       </c>
       <c r="Q222" s="3" t="s">
-        <v>1084</v>
+        <v>1085</v>
       </c>
       <c r="R222" s="3"/>
       <c r="S222" s="3"/>
@@ -17426,12 +17429,12 @@
         <v>35</v>
       </c>
       <c r="U222" s="3" t="s">
-        <v>1085</v>
+        <v>1086</v>
       </c>
     </row>
     <row r="223" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A223" s="3" t="s">
-        <v>1096</v>
+        <v>1097</v>
       </c>
       <c r="B223" s="3" t="s">
         <v>22</v>
@@ -17443,7 +17446,7 @@
         <v>24</v>
       </c>
       <c r="E223" s="3" t="s">
-        <v>1097</v>
+        <v>1098</v>
       </c>
       <c r="F223" s="3" t="s">
         <v>42</v>
@@ -17452,22 +17455,22 @@
         <v>45370</v>
       </c>
       <c r="H223" s="3" t="s">
-        <v>1098</v>
+        <v>1099</v>
       </c>
       <c r="I223" s="3" t="s">
-        <v>1099</v>
+        <v>1100</v>
       </c>
       <c r="J223" s="3" t="s">
-        <v>1100</v>
+        <v>1101</v>
       </c>
       <c r="K223" s="3" t="s">
-        <v>1101</v>
+        <v>1102</v>
       </c>
       <c r="L223" s="3" t="s">
-        <v>1102</v>
+        <v>1103</v>
       </c>
       <c r="M223" s="3" t="s">
-        <v>1103</v>
+        <v>1104</v>
       </c>
       <c r="N223" s="4">
         <v>45279</v>
@@ -17479,7 +17482,7 @@
         <v>33</v>
       </c>
       <c r="Q223" s="3" t="s">
-        <v>1104</v>
+        <v>1105</v>
       </c>
       <c r="R223" s="4">
         <v>45467</v>
@@ -17489,12 +17492,12 @@
         <v>35</v>
       </c>
       <c r="U223" s="3" t="s">
-        <v>1105</v>
+        <v>1106</v>
       </c>
     </row>
     <row r="224" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A224" s="3" t="s">
-        <v>1106</v>
+        <v>1107</v>
       </c>
       <c r="B224" s="3" t="s">
         <v>38</v>
@@ -17506,7 +17509,7 @@
         <v>24</v>
       </c>
       <c r="E224" s="3" t="s">
-        <v>1097</v>
+        <v>1098</v>
       </c>
       <c r="F224" s="3" t="s">
         <v>42</v>
@@ -17515,22 +17518,22 @@
         <v>45370</v>
       </c>
       <c r="H224" s="3" t="s">
+        <v>1100</v>
+      </c>
+      <c r="I224" s="3" t="s">
         <v>1099</v>
       </c>
-      <c r="I224" s="3" t="s">
-        <v>1098</v>
-      </c>
       <c r="J224" s="3" t="s">
-        <v>1100</v>
+        <v>1101</v>
       </c>
       <c r="K224" s="3" t="s">
-        <v>1101</v>
+        <v>1102</v>
       </c>
       <c r="L224" s="3" t="s">
-        <v>1102</v>
+        <v>1103</v>
       </c>
       <c r="M224" s="3" t="s">
-        <v>1103</v>
+        <v>1104</v>
       </c>
       <c r="N224" s="4">
         <v>45279</v>
@@ -17542,7 +17545,7 @@
         <v>33</v>
       </c>
       <c r="Q224" s="3" t="s">
-        <v>1104</v>
+        <v>1105</v>
       </c>
       <c r="R224" s="4">
         <v>45461</v>
@@ -17552,12 +17555,12 @@
         <v>35</v>
       </c>
       <c r="U224" s="3" t="s">
-        <v>1105</v>
+        <v>1106</v>
       </c>
     </row>
     <row r="225" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A225" s="3" t="s">
-        <v>1107</v>
+        <v>1108</v>
       </c>
       <c r="B225" s="3" t="s">
         <v>38</v>
@@ -17569,31 +17572,31 @@
         <v>24</v>
       </c>
       <c r="E225" s="3" t="s">
-        <v>1108</v>
+        <v>1109</v>
       </c>
       <c r="F225" s="3" t="s">
-        <v>1109</v>
+        <v>1110</v>
       </c>
       <c r="G225" s="4">
         <v>45078</v>
       </c>
       <c r="H225" s="3" t="s">
-        <v>1110</v>
+        <v>1111</v>
       </c>
       <c r="I225" s="3" t="s">
-        <v>1111</v>
+        <v>1112</v>
       </c>
       <c r="J225" s="3" t="s">
-        <v>1111</v>
+        <v>1112</v>
       </c>
       <c r="K225" s="3" t="s">
         <v>35</v>
       </c>
       <c r="L225" s="3" t="s">
+        <v>1113</v>
+      </c>
+      <c r="M225" s="3" t="s">
         <v>1112</v>
-      </c>
-      <c r="M225" s="3" t="s">
-        <v>1111</v>
       </c>
       <c r="N225" s="4">
         <v>44851</v>
@@ -17605,7 +17608,7 @@
         <v>33</v>
       </c>
       <c r="Q225" s="3" t="s">
-        <v>1113</v>
+        <v>1114</v>
       </c>
       <c r="R225" s="3"/>
       <c r="S225" s="3"/>
@@ -17613,12 +17616,12 @@
         <v>35</v>
       </c>
       <c r="U225" s="3" t="s">
-        <v>1114</v>
+        <v>1115</v>
       </c>
     </row>
     <row r="226" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A226" s="3" t="s">
-        <v>1115</v>
+        <v>1116</v>
       </c>
       <c r="B226" s="3" t="s">
         <v>22</v>
@@ -17630,31 +17633,31 @@
         <v>24</v>
       </c>
       <c r="E226" s="3" t="s">
-        <v>1116</v>
+        <v>1117</v>
       </c>
       <c r="F226" s="3" t="s">
-        <v>1109</v>
+        <v>1110</v>
       </c>
       <c r="G226" s="4">
         <v>45078</v>
       </c>
       <c r="H226" s="3" t="s">
-        <v>1117</v>
+        <v>1118</v>
       </c>
       <c r="I226" s="3" t="s">
-        <v>1111</v>
+        <v>1112</v>
       </c>
       <c r="J226" s="3" t="s">
-        <v>1111</v>
+        <v>1112</v>
       </c>
       <c r="K226" s="3" t="s">
         <v>35</v>
       </c>
       <c r="L226" s="3" t="s">
+        <v>1113</v>
+      </c>
+      <c r="M226" s="3" t="s">
         <v>1112</v>
-      </c>
-      <c r="M226" s="3" t="s">
-        <v>1111</v>
       </c>
       <c r="N226" s="4">
         <v>44851</v>
@@ -17666,7 +17669,7 @@
         <v>33</v>
       </c>
       <c r="Q226" s="3" t="s">
-        <v>1113</v>
+        <v>1114</v>
       </c>
       <c r="R226" s="3"/>
       <c r="S226" s="3"/>
@@ -17674,12 +17677,12 @@
         <v>35</v>
       </c>
       <c r="U226" s="3" t="s">
-        <v>1114</v>
+        <v>1115</v>
       </c>
     </row>
     <row r="227" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A227" s="3" t="s">
-        <v>1118</v>
+        <v>1119</v>
       </c>
       <c r="B227" s="3" t="s">
         <v>38</v>
@@ -17691,31 +17694,31 @@
         <v>24</v>
       </c>
       <c r="E227" s="3" t="s">
-        <v>1119</v>
+        <v>1120</v>
       </c>
       <c r="F227" s="3" t="s">
-        <v>1109</v>
+        <v>1110</v>
       </c>
       <c r="G227" s="4">
         <v>45078</v>
       </c>
       <c r="H227" s="3" t="s">
-        <v>1120</v>
+        <v>1121</v>
       </c>
       <c r="I227" s="3" t="s">
-        <v>1111</v>
+        <v>1112</v>
       </c>
       <c r="J227" s="3" t="s">
-        <v>1111</v>
+        <v>1112</v>
       </c>
       <c r="K227" s="3" t="s">
         <v>35</v>
       </c>
       <c r="L227" s="3" t="s">
+        <v>1113</v>
+      </c>
+      <c r="M227" s="3" t="s">
         <v>1112</v>
-      </c>
-      <c r="M227" s="3" t="s">
-        <v>1111</v>
       </c>
       <c r="N227" s="4">
         <v>44851</v>
@@ -17727,7 +17730,7 @@
         <v>33</v>
       </c>
       <c r="Q227" s="3" t="s">
-        <v>1113</v>
+        <v>1114</v>
       </c>
       <c r="R227" s="3"/>
       <c r="S227" s="3"/>
@@ -17735,12 +17738,12 @@
         <v>35</v>
       </c>
       <c r="U227" s="3" t="s">
-        <v>1114</v>
+        <v>1115</v>
       </c>
     </row>
     <row r="228" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A228" s="3" t="s">
-        <v>1121</v>
+        <v>1122</v>
       </c>
       <c r="B228" s="3" t="s">
         <v>22</v>
@@ -17752,7 +17755,7 @@
         <v>24</v>
       </c>
       <c r="E228" s="3" t="s">
-        <v>1122</v>
+        <v>1123</v>
       </c>
       <c r="F228" s="3" t="s">
         <v>996</v>
@@ -17761,10 +17764,10 @@
         <v>45390</v>
       </c>
       <c r="H228" s="3" t="s">
-        <v>1123</v>
+        <v>1124</v>
       </c>
       <c r="I228" s="3" t="s">
-        <v>1124</v>
+        <v>1125</v>
       </c>
       <c r="J228" s="3" t="s">
         <v>999</v>
@@ -17805,7 +17808,7 @@
     </row>
     <row r="229" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A229" s="3" t="s">
-        <v>1125</v>
+        <v>1126</v>
       </c>
       <c r="B229" s="3" t="s">
         <v>22</v>
@@ -17817,31 +17820,31 @@
         <v>24</v>
       </c>
       <c r="E229" s="3" t="s">
-        <v>1126</v>
+        <v>1127</v>
       </c>
       <c r="F229" s="3" t="s">
-        <v>1109</v>
+        <v>1110</v>
       </c>
       <c r="G229" s="4">
         <v>45078</v>
       </c>
       <c r="H229" s="3" t="s">
-        <v>1127</v>
+        <v>1128</v>
       </c>
       <c r="I229" s="3" t="s">
-        <v>1111</v>
+        <v>1112</v>
       </c>
       <c r="J229" s="3" t="s">
-        <v>1111</v>
+        <v>1112</v>
       </c>
       <c r="K229" s="3" t="s">
         <v>35</v>
       </c>
       <c r="L229" s="3" t="s">
+        <v>1113</v>
+      </c>
+      <c r="M229" s="3" t="s">
         <v>1112</v>
-      </c>
-      <c r="M229" s="3" t="s">
-        <v>1111</v>
       </c>
       <c r="N229" s="4">
         <v>44851</v>
@@ -17853,7 +17856,7 @@
         <v>33</v>
       </c>
       <c r="Q229" s="3" t="s">
-        <v>1113</v>
+        <v>1114</v>
       </c>
       <c r="R229" s="3"/>
       <c r="S229" s="3"/>
@@ -17861,12 +17864,12 @@
         <v>35</v>
       </c>
       <c r="U229" s="3" t="s">
-        <v>1114</v>
+        <v>1115</v>
       </c>
     </row>
     <row r="230" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A230" s="3" t="s">
-        <v>1128</v>
+        <v>1129</v>
       </c>
       <c r="B230" s="3" t="s">
         <v>22</v>
@@ -17878,31 +17881,31 @@
         <v>24</v>
       </c>
       <c r="E230" s="3" t="s">
-        <v>1129</v>
+        <v>1130</v>
       </c>
       <c r="F230" s="3" t="s">
-        <v>1109</v>
+        <v>1110</v>
       </c>
       <c r="G230" s="4">
         <v>45078</v>
       </c>
       <c r="H230" s="3" t="s">
-        <v>1130</v>
+        <v>1131</v>
       </c>
       <c r="I230" s="3" t="s">
-        <v>1131</v>
+        <v>1132</v>
       </c>
       <c r="J230" s="3" t="s">
-        <v>1132</v>
+        <v>1133</v>
       </c>
       <c r="K230" s="3" t="s">
         <v>35</v>
       </c>
       <c r="L230" s="3" t="s">
-        <v>1112</v>
+        <v>1113</v>
       </c>
       <c r="M230" s="3" t="s">
-        <v>1133</v>
+        <v>1134</v>
       </c>
       <c r="N230" s="4">
         <v>44851</v>
@@ -17914,7 +17917,7 @@
         <v>33</v>
       </c>
       <c r="Q230" s="3" t="s">
-        <v>1113</v>
+        <v>1114</v>
       </c>
       <c r="R230" s="3"/>
       <c r="S230" s="3"/>
@@ -17922,12 +17925,12 @@
         <v>35</v>
       </c>
       <c r="U230" s="3" t="s">
-        <v>1114</v>
+        <v>1115</v>
       </c>
     </row>
     <row r="231" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A231" s="3" t="s">
-        <v>1134</v>
+        <v>1135</v>
       </c>
       <c r="B231" s="3" t="s">
         <v>38</v>
@@ -17939,31 +17942,31 @@
         <v>24</v>
       </c>
       <c r="E231" s="3" t="s">
-        <v>1135</v>
+        <v>1136</v>
       </c>
       <c r="F231" s="3" t="s">
-        <v>1109</v>
+        <v>1110</v>
       </c>
       <c r="G231" s="4">
         <v>45078</v>
       </c>
       <c r="H231" s="3" t="s">
-        <v>1136</v>
+        <v>1137</v>
       </c>
       <c r="I231" s="3" t="s">
-        <v>1131</v>
+        <v>1132</v>
       </c>
       <c r="J231" s="3" t="s">
-        <v>1132</v>
+        <v>1133</v>
       </c>
       <c r="K231" s="3" t="s">
         <v>35</v>
       </c>
       <c r="L231" s="3" t="s">
-        <v>1112</v>
+        <v>1113</v>
       </c>
       <c r="M231" s="3" t="s">
-        <v>1133</v>
+        <v>1134</v>
       </c>
       <c r="N231" s="4">
         <v>44851</v>
@@ -17975,7 +17978,7 @@
         <v>33</v>
       </c>
       <c r="Q231" s="3" t="s">
-        <v>1113</v>
+        <v>1114</v>
       </c>
       <c r="R231" s="3"/>
       <c r="S231" s="3"/>
@@ -17983,12 +17986,12 @@
         <v>35</v>
       </c>
       <c r="U231" s="3" t="s">
-        <v>1114</v>
+        <v>1115</v>
       </c>
     </row>
     <row r="232" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A232" s="3" t="s">
-        <v>1137</v>
+        <v>1138</v>
       </c>
       <c r="B232" s="3" t="s">
         <v>22</v>
@@ -18000,7 +18003,7 @@
         <v>24</v>
       </c>
       <c r="E232" s="3" t="s">
-        <v>1138</v>
+        <v>1139</v>
       </c>
       <c r="F232" s="3" t="s">
         <v>42</v>
@@ -18009,22 +18012,22 @@
         <v>45412</v>
       </c>
       <c r="H232" s="3" t="s">
-        <v>1139</v>
+        <v>1140</v>
       </c>
       <c r="I232" s="3" t="s">
-        <v>1140</v>
+        <v>1141</v>
       </c>
       <c r="J232" s="3" t="s">
-        <v>1141</v>
+        <v>1142</v>
       </c>
       <c r="K232" s="3" t="s">
-        <v>1142</v>
+        <v>1143</v>
       </c>
       <c r="L232" s="3" t="s">
-        <v>1143</v>
+        <v>1144</v>
       </c>
       <c r="M232" s="3" t="s">
-        <v>1144</v>
+        <v>1145</v>
       </c>
       <c r="N232" s="4">
         <v>45372</v>
@@ -18036,7 +18039,7 @@
         <v>33</v>
       </c>
       <c r="Q232" s="3" t="s">
-        <v>1145</v>
+        <v>1146</v>
       </c>
       <c r="R232" s="4">
         <v>45534</v>
@@ -18046,12 +18049,12 @@
         <v>35</v>
       </c>
       <c r="U232" s="3" t="s">
-        <v>1146</v>
+        <v>1147</v>
       </c>
     </row>
     <row r="233" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A233" s="3" t="s">
-        <v>1147</v>
+        <v>1148</v>
       </c>
       <c r="B233" s="3" t="s">
         <v>38</v>
@@ -18063,7 +18066,7 @@
         <v>24</v>
       </c>
       <c r="E233" s="3" t="s">
-        <v>1148</v>
+        <v>1149</v>
       </c>
       <c r="F233" s="3" t="s">
         <v>42</v>
@@ -18072,22 +18075,22 @@
         <v>45412</v>
       </c>
       <c r="H233" s="3" t="s">
+        <v>1141</v>
+      </c>
+      <c r="I233" s="3" t="s">
         <v>1140</v>
       </c>
-      <c r="I233" s="3" t="s">
-        <v>1139</v>
-      </c>
       <c r="J233" s="3" t="s">
-        <v>1141</v>
+        <v>1142</v>
       </c>
       <c r="K233" s="3" t="s">
-        <v>1142</v>
+        <v>1143</v>
       </c>
       <c r="L233" s="3" t="s">
-        <v>1143</v>
+        <v>1144</v>
       </c>
       <c r="M233" s="3" t="s">
-        <v>1144</v>
+        <v>1145</v>
       </c>
       <c r="N233" s="4">
         <v>45372</v>
@@ -18099,7 +18102,7 @@
         <v>33</v>
       </c>
       <c r="Q233" s="3" t="s">
-        <v>1145</v>
+        <v>1146</v>
       </c>
       <c r="R233" s="4">
         <v>45534</v>
@@ -18109,24 +18112,24 @@
         <v>35</v>
       </c>
       <c r="U233" s="3" t="s">
-        <v>1146</v>
+        <v>1147</v>
       </c>
     </row>
     <row r="234" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A234" s="3" t="s">
-        <v>1149</v>
+        <v>1150</v>
       </c>
       <c r="B234" s="3" t="s">
         <v>22</v>
       </c>
       <c r="C234" s="3" t="s">
-        <v>1150</v>
+        <v>1151</v>
       </c>
       <c r="D234" s="3" t="s">
         <v>55</v>
       </c>
       <c r="E234" s="3" t="s">
-        <v>1151</v>
+        <v>1152</v>
       </c>
       <c r="F234" s="3" t="s">
         <v>42</v>
@@ -18135,22 +18138,22 @@
         <v>45503</v>
       </c>
       <c r="H234" s="3" t="s">
-        <v>1152</v>
+        <v>1153</v>
       </c>
       <c r="I234" s="3" t="s">
-        <v>1153</v>
+        <v>1154</v>
       </c>
       <c r="J234" s="3" t="s">
-        <v>1154</v>
+        <v>1155</v>
       </c>
       <c r="K234" s="3" t="s">
-        <v>1155</v>
+        <v>1156</v>
       </c>
       <c r="L234" s="3" t="s">
-        <v>1156</v>
+        <v>1157</v>
       </c>
       <c r="M234" s="3" t="s">
-        <v>1157</v>
+        <v>1158</v>
       </c>
       <c r="N234" s="4">
         <v>45169</v>
@@ -18170,24 +18173,24 @@
         <v>35</v>
       </c>
       <c r="U234" s="3" t="s">
-        <v>1158</v>
+        <v>1159</v>
       </c>
     </row>
     <row r="235" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A235" s="3" t="s">
-        <v>1159</v>
+        <v>1160</v>
       </c>
       <c r="B235" s="3" t="s">
         <v>38</v>
       </c>
       <c r="C235" s="3" t="s">
-        <v>1150</v>
+        <v>1151</v>
       </c>
       <c r="D235" s="3" t="s">
         <v>55</v>
       </c>
       <c r="E235" s="3" t="s">
-        <v>1151</v>
+        <v>1152</v>
       </c>
       <c r="F235" s="3" t="s">
         <v>42</v>
@@ -18196,22 +18199,22 @@
         <v>45503</v>
       </c>
       <c r="H235" s="3" t="s">
-        <v>1153</v>
+        <v>1154</v>
       </c>
       <c r="I235" s="3" t="s">
-        <v>1153</v>
+        <v>1154</v>
       </c>
       <c r="J235" s="3" t="s">
-        <v>1154</v>
+        <v>1155</v>
       </c>
       <c r="K235" s="3" t="s">
-        <v>1155</v>
+        <v>1156</v>
       </c>
       <c r="L235" s="3" t="s">
-        <v>1156</v>
+        <v>1157</v>
       </c>
       <c r="M235" s="3" t="s">
-        <v>1157</v>
+        <v>1158</v>
       </c>
       <c r="N235" s="4">
         <v>45169</v>
@@ -18231,7 +18234,7 @@
         <v>35</v>
       </c>
       <c r="U235" s="3" t="s">
-        <v>1158</v>
+        <v>1159</v>
       </c>
     </row>
   </sheetData>
@@ -30234,7 +30237,7 @@
     </row>
     <row r="215" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A215" s="3" t="s">
-        <v>1050</v>
+        <v>1051</v>
       </c>
       <c r="B215" s="5" t="b">
         <v>1</v>
@@ -30290,7 +30293,7 @@
     </row>
     <row r="216" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A216" s="3" t="s">
-        <v>1052</v>
+        <v>1053</v>
       </c>
       <c r="B216" s="5" t="b">
         <v>1</v>
@@ -30346,7 +30349,7 @@
     </row>
     <row r="217" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A217" s="3" t="s">
-        <v>1062</v>
+        <v>1063</v>
       </c>
       <c r="B217" s="5" t="b">
         <v>1</v>
@@ -30402,7 +30405,7 @@
     </row>
     <row r="218" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A218" s="3" t="s">
-        <v>1064</v>
+        <v>1065</v>
       </c>
       <c r="B218" s="5" t="b">
         <v>1</v>
@@ -30458,7 +30461,7 @@
     </row>
     <row r="219" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A219" s="3" t="s">
-        <v>1073</v>
+        <v>1074</v>
       </c>
       <c r="B219" s="5" t="b">
         <v>1</v>
@@ -30514,7 +30517,7 @@
     </row>
     <row r="220" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A220" s="3" t="s">
-        <v>1076</v>
+        <v>1077</v>
       </c>
       <c r="B220" s="5" t="b">
         <v>1</v>
@@ -30570,7 +30573,7 @@
     </row>
     <row r="221" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A221" s="3" t="s">
-        <v>1086</v>
+        <v>1087</v>
       </c>
       <c r="B221" s="5" t="b">
         <v>1</v>
@@ -30626,7 +30629,7 @@
     </row>
     <row r="222" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A222" s="3" t="s">
-        <v>1091</v>
+        <v>1092</v>
       </c>
       <c r="B222" s="5" t="b">
         <v>1</v>
@@ -30682,7 +30685,7 @@
     </row>
     <row r="223" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A223" s="3" t="s">
-        <v>1096</v>
+        <v>1097</v>
       </c>
       <c r="B223" s="5" t="b">
         <v>1</v>
@@ -30738,7 +30741,7 @@
     </row>
     <row r="224" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A224" s="3" t="s">
-        <v>1106</v>
+        <v>1107</v>
       </c>
       <c r="B224" s="5" t="b">
         <v>1</v>
@@ -30794,7 +30797,7 @@
     </row>
     <row r="225" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A225" s="3" t="s">
-        <v>1107</v>
+        <v>1108</v>
       </c>
       <c r="B225" s="5" t="b">
         <v>1</v>
@@ -30850,7 +30853,7 @@
     </row>
     <row r="226" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A226" s="3" t="s">
-        <v>1115</v>
+        <v>1116</v>
       </c>
       <c r="B226" s="5" t="b">
         <v>1</v>
@@ -30906,7 +30909,7 @@
     </row>
     <row r="227" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A227" s="3" t="s">
-        <v>1118</v>
+        <v>1119</v>
       </c>
       <c r="B227" s="5" t="b">
         <v>1</v>
@@ -30962,7 +30965,7 @@
     </row>
     <row r="228" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A228" s="3" t="s">
-        <v>1121</v>
+        <v>1122</v>
       </c>
       <c r="B228" s="5" t="b">
         <v>1</v>
@@ -31018,7 +31021,7 @@
     </row>
     <row r="229" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A229" s="3" t="s">
-        <v>1125</v>
+        <v>1126</v>
       </c>
       <c r="B229" s="5" t="b">
         <v>1</v>
@@ -31074,7 +31077,7 @@
     </row>
     <row r="230" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A230" s="3" t="s">
-        <v>1128</v>
+        <v>1129</v>
       </c>
       <c r="B230" s="5" t="b">
         <v>1</v>
@@ -31130,7 +31133,7 @@
     </row>
     <row r="231" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A231" s="3" t="s">
-        <v>1134</v>
+        <v>1135</v>
       </c>
       <c r="B231" s="5" t="b">
         <v>1</v>
@@ -31186,7 +31189,7 @@
     </row>
     <row r="232" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A232" s="3" t="s">
-        <v>1137</v>
+        <v>1138</v>
       </c>
       <c r="B232" s="5" t="b">
         <v>1</v>
@@ -31242,7 +31245,7 @@
     </row>
     <row r="233" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A233" s="3" t="s">
-        <v>1147</v>
+        <v>1148</v>
       </c>
       <c r="B233" s="5" t="b">
         <v>1</v>
@@ -31298,7 +31301,7 @@
     </row>
     <row r="234" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A234" s="3" t="s">
-        <v>1149</v>
+        <v>1150</v>
       </c>
       <c r="B234" s="5" t="b">
         <v>1</v>
@@ -31354,7 +31357,7 @@
     </row>
     <row r="235" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A235" s="3" t="s">
-        <v>1159</v>
+        <v>1160</v>
       </c>
       <c r="B235" s="5" t="b">
         <v>1</v>

</xml_diff>

<commit_message>
generated all the reports on 2024-11-08
</commit_message>
<xml_diff>
--- a/report/merged_configurations.xlsx
+++ b/report/merged_configurations.xlsx
@@ -251,25 +251,25 @@
     <t>ap-ruimtelijke-indicatoren-description.md</t>
   </si>
   <si>
-    <t>[{"name":"Ruimtelijke Indicatoren Applicatieprofiel","resourceReference":"https://data.vlaanderen.be/doc/applicatieprofiel/ruimtelijke-indicatoren/ontwerpstandaard/2024-01-22/"}]</t>
-  </si>
-  <si>
-    <t>[{"name":"OSLO Ruimtelijke Indicatoren - verslag - business werkgroep - 27 september 2023","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-slimRuimtelijkPlannen/standaardenregister/reports/Verslag business werkgroep SRP 2023-09-27.pdf"},{"name":"OSLO Ruimtelijke Indicatoren - verslag - thematische werkgroep 1 - 25 oktober 2023","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-slimRuimtelijkPlannen/standaardenregister/reports/Verslag thematische werkgroep 1 SRP 2023-10-25.pdf"},{"name":"OSLO Ruimtelijke Indicatoren - verslag - thematische werkgroep 2 - 30 november 2023","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-slimRuimtelijkPlannen/standaardenregister/reports/Verslag thematische werkgroep 2 SRP 2023-11-30.pdf"},{"name":"OSLO Ruimtelijke Indicatoren - verslag - thematische werkgroep 3 - 21 december 2023","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-slimRuimtelijkPlannen/standaardenregister/reports/Verslag thematische werkgroep 3 SRP 2023-12-21.pdf"},{"name":"OSLO Ruimtelijke Indicatoren - verslag - thematische werkgroep 4 - februari 2024","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-slimRuimtelijkPlannen/standaardenregister/reports/Verslag thematische werkgroep 4 SRP 2024-02-01.pdf"}]</t>
+    <t>[{"name":"Ruimtelijke Indicatoren Applicatieprofiel","resourceReference":"https://data.vlaanderen.be/doc/applicatieprofiel/ruimtelijke-indicatoren"}]</t>
+  </si>
+  <si>
+    <t>[{"name":"OSLO Ruimtelijke Indicatoren - verslag - business werkgroep - 27 september 2023","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-slimRuimtelijkPlannen/standaardenregister/reports/Verslag business werkgroep SRP 2023-09-27.pdf"},{"name":"OSLO Ruimtelijke Indicatoren - verslag - thematische werkgroep 1 - 25 oktober 2023","resourceReference":"https://github.com/Informatievlaanderen/OSLOthema-slimRuimtelijkPlannen/raw/a53dd0439d01fd35e587c2587c3504fcff5f104c/reports/Verslag%20thematische%20werkgroep%201%20SRP%202023-09-25.pdf"},{"name":"OSLO Ruimtelijke Indicatoren - verslag - thematische werkgroep 2 - 30 november 2023","resourceReference":"https://github.com/Informatievlaanderen/OSLOthema-slimRuimtelijkPlannen/raw/a53dd0439d01fd35e587c2587c3504fcff5f104c/reports/Verslag%20thematische%20werkgroep%202%20SRP%202023-11-30.docx"},{"name":"OSLO Ruimtelijke Indicatoren - verslag - thematische werkgroep 3 - 21 december 2023","resourceReference":"https://github.com/Informatievlaanderen/OSLOthema-slimRuimtelijkPlannen/raw/a53dd0439d01fd35e587c2587c3504fcff5f104c/reports/Verslag%20thematische%20werkgroep%203%20SRP%202023-12-21.pdf"},{"name":"OSLO Ruimtelijke Indicatoren - verslag - thematische werkgroep 4 - februari 2024","resourceReference":"https://github.com/Informatievlaanderen/OSLOthema-slimRuimtelijkPlannen/raw/a53dd0439d01fd35e587c2587c3504fcff5f104c/reports/Verslag%20thematische%20werkgroep%204%20SRP%202024-02-01.pdf"}]</t>
   </si>
   <si>
     <t>Projectcharter</t>
   </si>
   <si>
-    <t>https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-slimRuimtelijkPlannen/standaardenregister/charter/Werkgroep-charter-OSLO_SlimRuimtelijkPlannen.docx</t>
-  </si>
-  <si>
-    <t>[{"name":"OSLO Ruimtelijke Indicatoren - presentatie - business werkgroep - 27 september 2023","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-slimRuimtelijkPlannen/standaardenregister/presentations/Presentatie business werkgroep SRP 2023-09-27.pdf"},{"name":"OSLO Ruimtelijke Indicatoren - presentatie - thematische werkgroep 1 - 25 oktober 2023","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-slimRuimtelijkPlannen/standaardenregister/presentations/Presentatie thematische werkgroep 1 SRP 2023-10-25.pdf"},{"name":"OSLO Ruimtelijke Indicatoren - presentatie - thematische werkgroep 2 - 30 november 2023","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-slimRuimtelijkPlannen/standaardenregister/presentations/Presentatie thematische werkgroep 2 SRP 2023-11-30.pdf"},{"name":"OSLO Ruimtelijke Indicatoren - presentatie - thematische werkgroep 3 - 21 december 2023","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-slimRuimtelijkPlannen/standaardenregister/presentations/Presentatie thematische werkgroep 3 SRP 2023-12-21.pdf"},{"name":"OSLO Ruimtelijke Indicatoren - presentatie - thematische werkgroep 4 - 1 februari 2024","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-slimRuimtelijkPlannen/standaardenregister/presentations/Presentatie thematische werkgroep 4 SRP 2024-02-01.pdf"}]</t>
+    <t>https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-slimRuimtelijkPlannen/refs/heads/standaardenregister/charter/Werkgroep-charter-OSLO_SlimRuimtelijkPlannen.docx</t>
+  </si>
+  <si>
+    <t>[{"name":"OSLO Ruimtelijke Indicatoren - presentatie - business werkgroep - 27 september 2023","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-slimRuimtelijkPlannen/refs/heads/standaardenregister/presentations/Presentatie%20business%20werkgroep%20SRP%202023-09-27.pdf"},{"name":"OSLO Ruimtelijke Indicatoren - presentatie - thematische werkgroep 1 - 25 oktober 2023","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-slimRuimtelijkPlannen/refs/heads/standaardenregister/presentations/Presentatie%20thematische%20werkgroep%201%20SRP%202023-10-25.pdf"},{"name":"OSLO Ruimtelijke Indicatoren - presentatie - thematische werkgroep 2 - 30 november 2023","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-slimRuimtelijkPlannen/refs/heads/standaardenregister/presentations/Presentatie%20thematische%20werkgroep%202%20SRP%202023-11-30.pdf"},{"name":"OSLO Ruimtelijke Indicatoren - presentatie - thematische werkgroep 3 - 21 december 2023","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-slimRuimtelijkPlannen/refs/heads/standaardenregister/presentations/Presentatie%20thematische%20werkgroep%203%20SRP%202023-12-21.pdf"},{"name":"OSLO Ruimtelijke Indicatoren - presentatie - thematische werkgroep 4 - 1 februari 2024","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-slimRuimtelijkPlannen/refs/heads/standaardenregister/presentations/Presentatie%20thematische%20werkgroep%204%20SRP%202024-02-01.pdf"}]</t>
   </si>
   <si>
     <t>OSLOthema-slimRuimtelijkPlannen</t>
   </si>
   <si>
-    <t>{"name":"Projectcharter","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-slimRuimtelijkPlannen/standaardenregister/charter/Werkgroep-charter-OSLO_SlimRuimtelijkPlannen.docx"}</t>
+    <t>{"name":"Projectcharter","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-slimRuimtelijkPlannen/refs/heads/standaardenregister/charter/Werkgroep-charter-OSLO_SlimRuimtelijkPlannen.docx"}</t>
   </si>
   <si>
     <t>Vocabularium Ruimtelijke Indicatoren</t>
@@ -278,7 +278,7 @@
     <t>voc-ruimtelijke-indicatoren-description.md</t>
   </si>
   <si>
-    <t>[{"name":"Ruimtelijke Indicatoren Vocabularium","resourceReference":"https://data.vlaanderen.be/doc/vocabularium/ruimtelijke-indicatoren/ontwerpstandaard/2024-01-22"}]</t>
+    <t>[{"name":"Ruimtelijke Indicatoren Vocabularium","resourceReference":"https://data.vlaanderen.be/ns/ruimtelijke-indicatoren"}]</t>
   </si>
   <si>
     <t>OSLO Voorwaarden Dienstverlening</t>
@@ -308,6 +308,9 @@
     <t>Applicatieprofiel Incentiveringsplatform</t>
   </si>
   <si>
+    <t>erkende-standaard</t>
+  </si>
+  <si>
     <t>ap-Incentiveringsplatform.md</t>
   </si>
   <si>
@@ -342,9 +345,6 @@
   </si>
   <si>
     <t>Applicatieprofiel Verkeersmetingen</t>
-  </si>
-  <si>
-    <t>erkende-standaard</t>
   </si>
   <si>
     <t>ap-Verkeersmetingen.md</t>
@@ -4472,7 +4472,7 @@
         <v>23</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>55</v>
+        <v>24</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>78</v>
@@ -4481,7 +4481,7 @@
         <v>42</v>
       </c>
       <c r="G10" s="4">
-        <v>45222</v>
+        <v>45372</v>
       </c>
       <c r="H10" s="3" t="s">
         <v>79</v>
@@ -4527,7 +4527,7 @@
         <v>23</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>55</v>
+        <v>24</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>87</v>
@@ -4536,7 +4536,7 @@
         <v>42</v>
       </c>
       <c r="G11" s="4">
-        <v>45222</v>
+        <v>45372</v>
       </c>
       <c r="H11" s="3" t="s">
         <v>88</v>
@@ -4643,10 +4643,10 @@
         <v>23</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>55</v>
+        <v>98</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="F13" s="3" t="s">
         <v>42</v>
@@ -4655,22 +4655,22 @@
         <v>45372</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="I13" s="3" t="s">
         <v>28</v>
       </c>
       <c r="J13" s="3" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="K13" s="3" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="L13" s="3" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="M13" s="3" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="N13" s="4">
         <v>45001</v>
@@ -4678,9 +4678,11 @@
       <c r="O13" s="4">
         <v>45372</v>
       </c>
-      <c r="P13" s="3"/>
+      <c r="P13" s="4">
+        <v>45568</v>
+      </c>
       <c r="Q13" s="3" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="R13" s="3"/>
       <c r="S13" s="3"/>
@@ -4688,12 +4690,12 @@
         <v>35</v>
       </c>
       <c r="U13" s="3" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>38</v>
@@ -4702,10 +4704,10 @@
         <v>23</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>55</v>
+        <v>98</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="F14" s="3" t="s">
         <v>42</v>
@@ -4714,22 +4716,22 @@
         <v>45372</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="I14" s="3" t="s">
         <v>28</v>
       </c>
       <c r="J14" s="3" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="K14" s="3" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="L14" s="3" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="M14" s="3" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="N14" s="4">
         <v>45001</v>
@@ -4737,9 +4739,11 @@
       <c r="O14" s="4">
         <v>45372</v>
       </c>
-      <c r="P14" s="3"/>
+      <c r="P14" s="4">
+        <v>45568</v>
+      </c>
       <c r="Q14" s="3" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="R14" s="3"/>
       <c r="S14" s="3"/>
@@ -4747,12 +4751,12 @@
         <v>35</v>
       </c>
       <c r="U14" s="3" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>22</v>
@@ -4761,7 +4765,7 @@
         <v>23</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="E15" s="3" t="s">
         <v>111</v>
@@ -4822,7 +4826,7 @@
         <v>23</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="E16" s="3" t="s">
         <v>125</v>
@@ -4883,7 +4887,7 @@
         <v>23</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="E17" s="3" t="s">
         <v>131</v>
@@ -4944,7 +4948,7 @@
         <v>23</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="E18" s="3" t="s">
         <v>142</v>
@@ -6225,7 +6229,7 @@
         <v>23</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="E39" s="3" t="s">
         <v>225</v>
@@ -6286,7 +6290,7 @@
         <v>23</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="E40" s="3" t="s">
         <v>236</v>
@@ -6591,7 +6595,7 @@
         <v>264</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="E45" s="3" t="s">
         <v>265</v>
@@ -6652,7 +6656,7 @@
         <v>23</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="E46" s="3" t="s">
         <v>265</v>
@@ -6713,7 +6717,7 @@
         <v>264</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="E47" s="3" t="s">
         <v>265</v>
@@ -6774,7 +6778,7 @@
         <v>264</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="E48" s="3" t="s">
         <v>279</v>
@@ -6835,7 +6839,7 @@
         <v>23</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="E49" s="3" t="s">
         <v>282</v>
@@ -6957,7 +6961,7 @@
         <v>23</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="E51" s="3" t="s">
         <v>295</v>
@@ -7079,7 +7083,7 @@
         <v>23</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="E53" s="3" t="s">
         <v>308</v>
@@ -7140,7 +7144,7 @@
         <v>23</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="E54" s="3" t="s">
         <v>315</v>
@@ -7201,7 +7205,7 @@
         <v>23</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="E55" s="3" t="s">
         <v>318</v>
@@ -7323,7 +7327,7 @@
         <v>23</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="E57" s="3" t="s">
         <v>330</v>
@@ -7384,7 +7388,7 @@
         <v>23</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="E58" s="3" t="s">
         <v>340</v>
@@ -7506,7 +7510,7 @@
         <v>23</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="E60" s="3" t="s">
         <v>352</v>
@@ -7567,7 +7571,7 @@
         <v>23</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="E61" s="3" t="s">
         <v>362</v>
@@ -7689,7 +7693,7 @@
         <v>23</v>
       </c>
       <c r="D63" s="3" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="E63" s="3" t="s">
         <v>372</v>
@@ -7933,7 +7937,7 @@
         <v>23</v>
       </c>
       <c r="D67" s="3" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="E67" s="3" t="s">
         <v>394</v>
@@ -7994,7 +7998,7 @@
         <v>23</v>
       </c>
       <c r="D68" s="3" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="E68" s="3" t="s">
         <v>401</v>
@@ -8055,7 +8059,7 @@
         <v>23</v>
       </c>
       <c r="D69" s="3" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="E69" s="3" t="s">
         <v>404</v>
@@ -8116,7 +8120,7 @@
         <v>23</v>
       </c>
       <c r="D70" s="3" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="E70" s="3" t="s">
         <v>411</v>
@@ -8177,7 +8181,7 @@
         <v>23</v>
       </c>
       <c r="D71" s="3" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="E71" s="3" t="s">
         <v>414</v>
@@ -8238,7 +8242,7 @@
         <v>23</v>
       </c>
       <c r="D72" s="3" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="E72" s="3" t="s">
         <v>417</v>
@@ -8299,7 +8303,7 @@
         <v>23</v>
       </c>
       <c r="D73" s="3" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="E73" s="3" t="s">
         <v>428</v>
@@ -8482,7 +8486,7 @@
         <v>23</v>
       </c>
       <c r="D76" s="3" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="E76" s="3" t="s">
         <v>444</v>
@@ -8543,7 +8547,7 @@
         <v>23</v>
       </c>
       <c r="D77" s="3" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="E77" s="3" t="s">
         <v>455</v>
@@ -8604,7 +8608,7 @@
         <v>23</v>
       </c>
       <c r="D78" s="3" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="E78" s="3" t="s">
         <v>459</v>
@@ -8665,7 +8669,7 @@
         <v>23</v>
       </c>
       <c r="D79" s="3" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="E79" s="3" t="s">
         <v>463</v>
@@ -8787,7 +8791,7 @@
         <v>23</v>
       </c>
       <c r="D81" s="3" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="E81" s="3" t="s">
         <v>479</v>
@@ -8848,7 +8852,7 @@
         <v>23</v>
       </c>
       <c r="D82" s="3" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="E82" s="3" t="s">
         <v>489</v>
@@ -8909,7 +8913,7 @@
         <v>23</v>
       </c>
       <c r="D83" s="3" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="E83" s="3" t="s">
         <v>496</v>
@@ -8970,7 +8974,7 @@
         <v>23</v>
       </c>
       <c r="D84" s="3" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="E84" s="3" t="s">
         <v>499</v>
@@ -9031,7 +9035,7 @@
         <v>23</v>
       </c>
       <c r="D85" s="3" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="E85" s="3" t="s">
         <v>509</v>
@@ -9092,7 +9096,7 @@
         <v>23</v>
       </c>
       <c r="D86" s="3" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="E86" s="3" t="s">
         <v>512</v>
@@ -9153,7 +9157,7 @@
         <v>23</v>
       </c>
       <c r="D87" s="3" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="E87" s="3" t="s">
         <v>517</v>
@@ -9214,7 +9218,7 @@
         <v>23</v>
       </c>
       <c r="D88" s="3" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="E88" s="3" t="s">
         <v>520</v>
@@ -9275,7 +9279,7 @@
         <v>529</v>
       </c>
       <c r="D89" s="3" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="E89" s="3" t="s">
         <v>530</v>
@@ -9336,7 +9340,7 @@
         <v>23</v>
       </c>
       <c r="D90" s="3" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="E90" s="3" t="s">
         <v>534</v>
@@ -9397,7 +9401,7 @@
         <v>529</v>
       </c>
       <c r="D91" s="3" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="E91" s="3" t="s">
         <v>540</v>
@@ -9458,7 +9462,7 @@
         <v>529</v>
       </c>
       <c r="D92" s="3" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="E92" s="3" t="s">
         <v>543</v>
@@ -9519,7 +9523,7 @@
         <v>547</v>
       </c>
       <c r="D93" s="3" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="E93" s="3" t="s">
         <v>548</v>
@@ -9580,7 +9584,7 @@
         <v>547</v>
       </c>
       <c r="D94" s="3" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="E94" s="3" t="s">
         <v>548</v>
@@ -9641,7 +9645,7 @@
         <v>23</v>
       </c>
       <c r="D95" s="3" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="E95" s="3" t="s">
         <v>558</v>
@@ -9702,7 +9706,7 @@
         <v>23</v>
       </c>
       <c r="D96" s="3" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="E96" s="3" t="s">
         <v>567</v>
@@ -9763,7 +9767,7 @@
         <v>23</v>
       </c>
       <c r="D97" s="3" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="E97" s="3" t="s">
         <v>567</v>
@@ -9824,7 +9828,7 @@
         <v>23</v>
       </c>
       <c r="D98" s="3" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="E98" s="3" t="s">
         <v>567</v>
@@ -9885,7 +9889,7 @@
         <v>23</v>
       </c>
       <c r="D99" s="3" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="E99" s="3" t="s">
         <v>567</v>
@@ -9946,7 +9950,7 @@
         <v>23</v>
       </c>
       <c r="D100" s="3" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="E100" s="3" t="s">
         <v>567</v>
@@ -10007,7 +10011,7 @@
         <v>23</v>
       </c>
       <c r="D101" s="3" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="E101" s="3" t="s">
         <v>567</v>
@@ -10068,7 +10072,7 @@
         <v>23</v>
       </c>
       <c r="D102" s="3" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="E102" s="3" t="s">
         <v>567</v>
@@ -10129,7 +10133,7 @@
         <v>23</v>
       </c>
       <c r="D103" s="3" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="E103" s="3" t="s">
         <v>587</v>
@@ -10190,7 +10194,7 @@
         <v>23</v>
       </c>
       <c r="D104" s="3" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="E104" s="3" t="s">
         <v>587</v>
@@ -10251,7 +10255,7 @@
         <v>23</v>
       </c>
       <c r="D105" s="3" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="E105" s="3" t="s">
         <v>587</v>
@@ -10312,7 +10316,7 @@
         <v>23</v>
       </c>
       <c r="D106" s="3" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="E106" s="3" t="s">
         <v>587</v>
@@ -10373,7 +10377,7 @@
         <v>23</v>
       </c>
       <c r="D107" s="3" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="E107" s="3" t="s">
         <v>587</v>
@@ -10434,7 +10438,7 @@
         <v>23</v>
       </c>
       <c r="D108" s="3" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="E108" s="3" t="s">
         <v>587</v>
@@ -10495,7 +10499,7 @@
         <v>23</v>
       </c>
       <c r="D109" s="3" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="E109" s="3" t="s">
         <v>587</v>
@@ -10556,7 +10560,7 @@
         <v>23</v>
       </c>
       <c r="D110" s="3" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="E110" s="3" t="s">
         <v>587</v>
@@ -10617,7 +10621,7 @@
         <v>23</v>
       </c>
       <c r="D111" s="3" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="E111" s="3" t="s">
         <v>587</v>
@@ -10739,7 +10743,7 @@
         <v>23</v>
       </c>
       <c r="D113" s="3" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="E113" s="3" t="s">
         <v>616</v>
@@ -10800,7 +10804,7 @@
         <v>23</v>
       </c>
       <c r="D114" s="3" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="E114" s="3" t="s">
         <v>616</v>
@@ -10861,7 +10865,7 @@
         <v>264</v>
       </c>
       <c r="D115" s="3" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="E115" s="3" t="s">
         <v>627</v>
@@ -10922,7 +10926,7 @@
         <v>264</v>
       </c>
       <c r="D116" s="3" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="E116" s="3" t="s">
         <v>637</v>
@@ -10983,7 +10987,7 @@
         <v>23</v>
       </c>
       <c r="D117" s="3" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="E117" s="3" t="s">
         <v>641</v>
@@ -11345,7 +11349,7 @@
         <v>23</v>
       </c>
       <c r="D123" s="3" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="E123" s="3" t="s">
         <v>587</v>
@@ -11406,7 +11410,7 @@
         <v>23</v>
       </c>
       <c r="D124" s="3" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="E124" s="3" t="s">
         <v>587</v>
@@ -11467,7 +11471,7 @@
         <v>23</v>
       </c>
       <c r="D125" s="3" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="E125" s="3" t="s">
         <v>587</v>
@@ -11528,7 +11532,7 @@
         <v>23</v>
       </c>
       <c r="D126" s="3" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="E126" s="3" t="s">
         <v>587</v>
@@ -11589,7 +11593,7 @@
         <v>23</v>
       </c>
       <c r="D127" s="3" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="E127" s="3" t="s">
         <v>587</v>
@@ -11650,7 +11654,7 @@
         <v>23</v>
       </c>
       <c r="D128" s="3" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="E128" s="3" t="s">
         <v>587</v>
@@ -11711,7 +11715,7 @@
         <v>23</v>
       </c>
       <c r="D129" s="3" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="E129" s="3" t="s">
         <v>587</v>
@@ -11772,7 +11776,7 @@
         <v>23</v>
       </c>
       <c r="D130" s="3" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="E130" s="3" t="s">
         <v>587</v>
@@ -11833,7 +11837,7 @@
         <v>23</v>
       </c>
       <c r="D131" s="3" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="E131" s="3" t="s">
         <v>587</v>
@@ -11894,7 +11898,7 @@
         <v>23</v>
       </c>
       <c r="D132" s="3" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="E132" s="3" t="s">
         <v>587</v>
@@ -11955,7 +11959,7 @@
         <v>23</v>
       </c>
       <c r="D133" s="3" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="E133" s="3" t="s">
         <v>587</v>
@@ -12016,7 +12020,7 @@
         <v>23</v>
       </c>
       <c r="D134" s="3" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="E134" s="3" t="s">
         <v>704</v>
@@ -12077,7 +12081,7 @@
         <v>23</v>
       </c>
       <c r="D135" s="3" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="E135" s="3" t="s">
         <v>707</v>
@@ -12138,7 +12142,7 @@
         <v>23</v>
       </c>
       <c r="D136" s="3" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="E136" s="3" t="s">
         <v>707</v>
@@ -12199,7 +12203,7 @@
         <v>23</v>
       </c>
       <c r="D137" s="3" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="E137" s="3" t="s">
         <v>707</v>
@@ -12260,7 +12264,7 @@
         <v>23</v>
       </c>
       <c r="D138" s="3" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="E138" s="3" t="s">
         <v>707</v>
@@ -12321,7 +12325,7 @@
         <v>23</v>
       </c>
       <c r="D139" s="3" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="E139" s="3" t="s">
         <v>707</v>
@@ -12382,7 +12386,7 @@
         <v>23</v>
       </c>
       <c r="D140" s="3" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="E140" s="3" t="s">
         <v>707</v>
@@ -12443,7 +12447,7 @@
         <v>23</v>
       </c>
       <c r="D141" s="3" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="E141" s="3" t="s">
         <v>707</v>
@@ -12504,7 +12508,7 @@
         <v>23</v>
       </c>
       <c r="D142" s="3" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="E142" s="3" t="s">
         <v>707</v>
@@ -12565,7 +12569,7 @@
         <v>23</v>
       </c>
       <c r="D143" s="3" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="E143" s="3" t="s">
         <v>707</v>
@@ -12748,7 +12752,7 @@
         <v>264</v>
       </c>
       <c r="D146" s="3" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="E146" s="3" t="s">
         <v>743</v>
@@ -12809,7 +12813,7 @@
         <v>264</v>
       </c>
       <c r="D147" s="3" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="E147" s="3" t="s">
         <v>743</v>
@@ -12870,7 +12874,7 @@
         <v>23</v>
       </c>
       <c r="D148" s="3" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="E148" s="3" t="s">
         <v>756</v>
@@ -12931,7 +12935,7 @@
         <v>23</v>
       </c>
       <c r="D149" s="3" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="E149" s="3" t="s">
         <v>764</v>
@@ -12992,7 +12996,7 @@
         <v>23</v>
       </c>
       <c r="D150" s="3" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="E150" s="3" t="s">
         <v>767</v>
@@ -13053,7 +13057,7 @@
         <v>23</v>
       </c>
       <c r="D151" s="3" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="E151" s="3" t="s">
         <v>770</v>
@@ -13114,7 +13118,7 @@
         <v>23</v>
       </c>
       <c r="D152" s="3" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="E152" s="3" t="s">
         <v>773</v>
@@ -13175,7 +13179,7 @@
         <v>23</v>
       </c>
       <c r="D153" s="3" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="E153" s="3" t="s">
         <v>776</v>
@@ -13236,7 +13240,7 @@
         <v>23</v>
       </c>
       <c r="D154" s="3" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="E154" s="3" t="s">
         <v>779</v>
@@ -13297,7 +13301,7 @@
         <v>23</v>
       </c>
       <c r="D155" s="3" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="E155" s="3" t="s">
         <v>782</v>
@@ -13358,7 +13362,7 @@
         <v>23</v>
       </c>
       <c r="D156" s="3" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="E156" s="3" t="s">
         <v>785</v>
@@ -13419,7 +13423,7 @@
         <v>23</v>
       </c>
       <c r="D157" s="3" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="E157" s="3" t="s">
         <v>788</v>
@@ -13480,7 +13484,7 @@
         <v>23</v>
       </c>
       <c r="D158" s="3" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="E158" s="3" t="s">
         <v>791</v>
@@ -13541,7 +13545,7 @@
         <v>23</v>
       </c>
       <c r="D159" s="3" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="E159" s="3" t="s">
         <v>794</v>
@@ -13602,7 +13606,7 @@
         <v>23</v>
       </c>
       <c r="D160" s="3" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="E160" s="3" t="s">
         <v>797</v>
@@ -13663,7 +13667,7 @@
         <v>23</v>
       </c>
       <c r="D161" s="3" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="E161" s="3" t="s">
         <v>800</v>
@@ -13724,7 +13728,7 @@
         <v>23</v>
       </c>
       <c r="D162" s="3" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="E162" s="3" t="s">
         <v>803</v>
@@ -13785,7 +13789,7 @@
         <v>23</v>
       </c>
       <c r="D163" s="3" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="E163" s="3" t="s">
         <v>806</v>
@@ -13846,7 +13850,7 @@
         <v>23</v>
       </c>
       <c r="D164" s="3" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="E164" s="3" t="s">
         <v>809</v>
@@ -13907,7 +13911,7 @@
         <v>23</v>
       </c>
       <c r="D165" s="3" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="E165" s="3" t="s">
         <v>812</v>
@@ -13968,7 +13972,7 @@
         <v>23</v>
       </c>
       <c r="D166" s="3" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="E166" s="3" t="s">
         <v>815</v>
@@ -14029,7 +14033,7 @@
         <v>23</v>
       </c>
       <c r="D167" s="3" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="E167" s="3" t="s">
         <v>818</v>
@@ -14090,7 +14094,7 @@
         <v>23</v>
       </c>
       <c r="D168" s="3" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="E168" s="3" t="s">
         <v>821</v>
@@ -14151,7 +14155,7 @@
         <v>23</v>
       </c>
       <c r="D169" s="3" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="E169" s="3" t="s">
         <v>824</v>
@@ -14212,7 +14216,7 @@
         <v>23</v>
       </c>
       <c r="D170" s="3" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="E170" s="3" t="s">
         <v>827</v>
@@ -14273,7 +14277,7 @@
         <v>23</v>
       </c>
       <c r="D171" s="3" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="E171" s="3" t="s">
         <v>830</v>
@@ -14334,7 +14338,7 @@
         <v>23</v>
       </c>
       <c r="D172" s="3" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="E172" s="3" t="s">
         <v>833</v>
@@ -14395,7 +14399,7 @@
         <v>23</v>
       </c>
       <c r="D173" s="3" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="E173" s="3" t="s">
         <v>836</v>
@@ -14456,7 +14460,7 @@
         <v>23</v>
       </c>
       <c r="D174" s="3" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="E174" s="3" t="s">
         <v>839</v>
@@ -14517,7 +14521,7 @@
         <v>23</v>
       </c>
       <c r="D175" s="3" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="E175" s="3" t="s">
         <v>842</v>
@@ -14578,7 +14582,7 @@
         <v>23</v>
       </c>
       <c r="D176" s="3" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="E176" s="3" t="s">
         <v>845</v>
@@ -14639,7 +14643,7 @@
         <v>23</v>
       </c>
       <c r="D177" s="3" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="E177" s="3" t="s">
         <v>848</v>
@@ -14700,7 +14704,7 @@
         <v>23</v>
       </c>
       <c r="D178" s="3" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="E178" s="3" t="s">
         <v>851</v>
@@ -14761,7 +14765,7 @@
         <v>23</v>
       </c>
       <c r="D179" s="3" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="E179" s="3" t="s">
         <v>854</v>
@@ -14822,7 +14826,7 @@
         <v>23</v>
       </c>
       <c r="D180" s="3" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="E180" s="3" t="s">
         <v>857</v>
@@ -14883,7 +14887,7 @@
         <v>23</v>
       </c>
       <c r="D181" s="3" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="E181" s="3" t="s">
         <v>860</v>
@@ -14944,7 +14948,7 @@
         <v>23</v>
       </c>
       <c r="D182" s="3" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="E182" s="3" t="s">
         <v>863</v>
@@ -15005,7 +15009,7 @@
         <v>23</v>
       </c>
       <c r="D183" s="3" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="E183" s="3" t="s">
         <v>863</v>
@@ -15066,7 +15070,7 @@
         <v>23</v>
       </c>
       <c r="D184" s="3" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="E184" s="3" t="s">
         <v>863</v>
@@ -15127,7 +15131,7 @@
         <v>23</v>
       </c>
       <c r="D185" s="3" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="E185" s="3" t="s">
         <v>863</v>
@@ -15188,7 +15192,7 @@
         <v>23</v>
       </c>
       <c r="D186" s="3" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="E186" s="3" t="s">
         <v>863</v>
@@ -15249,7 +15253,7 @@
         <v>23</v>
       </c>
       <c r="D187" s="3" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="E187" s="3" t="s">
         <v>863</v>
@@ -15310,7 +15314,7 @@
         <v>23</v>
       </c>
       <c r="D188" s="3" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="E188" s="3" t="s">
         <v>863</v>
@@ -15558,7 +15562,7 @@
         <v>23</v>
       </c>
       <c r="D192" s="3" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="E192" s="3" t="s">
         <v>468</v>
@@ -15680,7 +15684,7 @@
         <v>23</v>
       </c>
       <c r="D194" s="3" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="E194" s="3" t="s">
         <v>917</v>
@@ -15741,7 +15745,7 @@
         <v>23</v>
       </c>
       <c r="D195" s="3" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="E195" s="3" t="s">
         <v>926</v>
@@ -15802,7 +15806,7 @@
         <v>23</v>
       </c>
       <c r="D196" s="3" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="E196" s="3" t="s">
         <v>926</v>
@@ -15863,7 +15867,7 @@
         <v>23</v>
       </c>
       <c r="D197" s="3" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="E197" s="3" t="s">
         <v>937</v>
@@ -15924,7 +15928,7 @@
         <v>23</v>
       </c>
       <c r="D198" s="3" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="E198" s="3" t="s">
         <v>937</v>
@@ -16237,7 +16241,7 @@
         <v>23</v>
       </c>
       <c r="D203" s="3" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="E203" s="3" t="s">
         <v>973</v>
@@ -16296,7 +16300,7 @@
         <v>23</v>
       </c>
       <c r="D204" s="3" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="E204" s="3" t="s">
         <v>981</v>
@@ -16485,7 +16489,7 @@
         <v>23</v>
       </c>
       <c r="D207" s="3" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="E207" s="3" t="s">
         <v>90</v>
@@ -16546,7 +16550,7 @@
         <v>23</v>
       </c>
       <c r="D208" s="3" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="E208" s="3" t="s">
         <v>90</v>
@@ -18960,8 +18964,8 @@
       <c r="L13" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="M13" s="6" t="b">
-        <v>0</v>
+      <c r="M13" s="5" t="b">
+        <v>1</v>
       </c>
       <c r="N13" s="6" t="b">
         <v>0</v>
@@ -18981,7 +18985,7 @@
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B14" s="5" t="b">
         <v>1</v>
@@ -19016,8 +19020,8 @@
       <c r="L14" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="M14" s="6" t="b">
-        <v>0</v>
+      <c r="M14" s="5" t="b">
+        <v>1</v>
       </c>
       <c r="N14" s="6" t="b">
         <v>0</v>
@@ -19037,7 +19041,7 @@
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B15" s="5" t="b">
         <v>1</v>

</xml_diff>

<commit_message>
generated all the reports on 2024-12-15
</commit_message>
<xml_diff>
--- a/report/merged_configurations.xlsx
+++ b/report/merged_configurations.xlsx
@@ -128,10 +128,10 @@
     <t>Applicatieprofiel Erosiepoel</t>
   </si>
   <si>
-    <t>[{"name":"Applicatieprofiel Erosiepoel","resourceReference":"https://test.data.vlaanderen.be/doc/applicatieprofiel/erosiepoel/ontwerpstandaard/2024-11-29/"}]</t>
-  </si>
-  <si>
-    <t>[{"name":"Vocabularium Erosiepoel","resourceReference":"https://test.data.vlaanderen.be/ns/erosiepoel/"}]</t>
+    <t>[{"name":"Applicatieprofiel Erosiepoel","resourceReference":"https://data.vlaanderen.be/doc/applicatieprofiel/erosiepoel"}]</t>
+  </si>
+  <si>
+    <t>[{"name":"Vocabularium Erosiepoel","resourceReference":"https://data.vlaanderen.be/ns/erosiepoel/"}]</t>
   </si>
   <si>
     <t>https://github.com/Informatievlaanderen/OSLOthema-modderstromen/blob/standaardenregister/charter/Werkgroep%20charter%20OSLO_ModderstroomMonitoring%20-%20OSLO.docx</t>

</xml_diff>

<commit_message>
generated all the reports on 2025-01-19
</commit_message>
<xml_diff>
--- a/report/merged_configurations.xlsx
+++ b/report/merged_configurations.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4552" uniqueCount="1224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4540" uniqueCount="1224">
   <si>
     <t>title</t>
   </si>
@@ -18812,7 +18812,7 @@
         <v>41</v>
       </c>
       <c r="D221" s="3" t="s">
-        <v>89</v>
+        <v>74</v>
       </c>
       <c r="E221" s="3" t="s">
         <v>1106</v>
@@ -18844,8 +18844,8 @@
       <c r="N221" s="4">
         <v>45239</v>
       </c>
-      <c r="O221" s="3" t="s">
-        <v>81</v>
+      <c r="O221" s="4">
+        <v>45631</v>
       </c>
       <c r="P221" s="3"/>
       <c r="Q221" s="3" t="s">
@@ -18879,7 +18879,7 @@
         <v>41</v>
       </c>
       <c r="D222" s="3" t="s">
-        <v>89</v>
+        <v>74</v>
       </c>
       <c r="E222" s="3" t="s">
         <v>1106</v>
@@ -18911,8 +18911,8 @@
       <c r="N222" s="4">
         <v>45239</v>
       </c>
-      <c r="O222" s="3" t="s">
-        <v>81</v>
+      <c r="O222" s="4">
+        <v>45631</v>
       </c>
       <c r="P222" s="3"/>
       <c r="Q222" s="3" t="s">
@@ -18946,7 +18946,7 @@
         <v>41</v>
       </c>
       <c r="D223" s="3" t="s">
-        <v>89</v>
+        <v>74</v>
       </c>
       <c r="E223" s="3" t="s">
         <v>484</v>
@@ -18978,8 +18978,8 @@
       <c r="N223" s="4">
         <v>45334</v>
       </c>
-      <c r="O223" s="3" t="s">
-        <v>81</v>
+      <c r="O223" s="4">
+        <v>45631</v>
       </c>
       <c r="P223" s="3"/>
       <c r="Q223" s="3" t="s">
@@ -19013,7 +19013,7 @@
         <v>41</v>
       </c>
       <c r="D224" s="3" t="s">
-        <v>89</v>
+        <v>74</v>
       </c>
       <c r="E224" s="3" t="s">
         <v>484</v>
@@ -19045,8 +19045,8 @@
       <c r="N224" s="4">
         <v>45334</v>
       </c>
-      <c r="O224" s="3" t="s">
-        <v>81</v>
+      <c r="O224" s="4">
+        <v>45631</v>
       </c>
       <c r="P224" s="3"/>
       <c r="Q224" s="3" t="s">
@@ -19222,7 +19222,7 @@
         <v>41</v>
       </c>
       <c r="D227" s="3" t="s">
-        <v>89</v>
+        <v>74</v>
       </c>
       <c r="E227" s="3" t="s">
         <v>1046</v>
@@ -19251,11 +19251,11 @@
       <c r="M227" s="4">
         <v>45316</v>
       </c>
-      <c r="N227" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="O227" s="3" t="s">
-        <v>81</v>
+      <c r="N227" s="4">
+        <v>45603</v>
+      </c>
+      <c r="O227" s="4">
+        <v>45631</v>
       </c>
       <c r="P227" s="3"/>
       <c r="Q227" s="3" t="s">
@@ -19289,7 +19289,7 @@
         <v>41</v>
       </c>
       <c r="D228" s="3" t="s">
-        <v>89</v>
+        <v>74</v>
       </c>
       <c r="E228" s="3" t="s">
         <v>1046</v>
@@ -19318,11 +19318,11 @@
       <c r="M228" s="4">
         <v>45316</v>
       </c>
-      <c r="N228" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="O228" s="3" t="s">
-        <v>81</v>
+      <c r="N228" s="4">
+        <v>45603</v>
+      </c>
+      <c r="O228" s="4">
+        <v>45631</v>
       </c>
       <c r="P228" s="3"/>
       <c r="Q228" s="3" t="s">
@@ -19356,7 +19356,7 @@
         <v>41</v>
       </c>
       <c r="D229" s="3" t="s">
-        <v>89</v>
+        <v>74</v>
       </c>
       <c r="E229" s="3" t="s">
         <v>1046</v>
@@ -19385,11 +19385,11 @@
       <c r="M229" s="4">
         <v>45316</v>
       </c>
-      <c r="N229" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="O229" s="3" t="s">
-        <v>81</v>
+      <c r="N229" s="4">
+        <v>45603</v>
+      </c>
+      <c r="O229" s="4">
+        <v>45631</v>
       </c>
       <c r="P229" s="3"/>
       <c r="Q229" s="3" t="s">
@@ -19762,7 +19762,7 @@
         <v>41</v>
       </c>
       <c r="D235" s="3" t="s">
-        <v>89</v>
+        <v>74</v>
       </c>
       <c r="E235" s="3" t="s">
         <v>1046</v>
@@ -19791,11 +19791,11 @@
       <c r="M235" s="4">
         <v>45372</v>
       </c>
-      <c r="N235" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="O235" s="3" t="s">
-        <v>81</v>
+      <c r="N235" s="4">
+        <v>45603</v>
+      </c>
+      <c r="O235" s="4">
+        <v>45631</v>
       </c>
       <c r="P235" s="4">
         <v>45428</v>
@@ -32666,8 +32666,8 @@
       <c r="L221" s="6" t="b">
         <v>1</v>
       </c>
-      <c r="M221" s="5" t="b">
-        <v>0</v>
+      <c r="M221" s="6" t="b">
+        <v>1</v>
       </c>
       <c r="N221" s="5" t="b">
         <v>0</v>
@@ -32722,8 +32722,8 @@
       <c r="L222" s="6" t="b">
         <v>1</v>
       </c>
-      <c r="M222" s="5" t="b">
-        <v>0</v>
+      <c r="M222" s="6" t="b">
+        <v>1</v>
       </c>
       <c r="N222" s="5" t="b">
         <v>0</v>
@@ -32778,8 +32778,8 @@
       <c r="L223" s="6" t="b">
         <v>1</v>
       </c>
-      <c r="M223" s="5" t="b">
-        <v>0</v>
+      <c r="M223" s="6" t="b">
+        <v>1</v>
       </c>
       <c r="N223" s="5" t="b">
         <v>0</v>
@@ -32834,8 +32834,8 @@
       <c r="L224" s="6" t="b">
         <v>1</v>
       </c>
-      <c r="M224" s="5" t="b">
-        <v>0</v>
+      <c r="M224" s="6" t="b">
+        <v>1</v>
       </c>
       <c r="N224" s="5" t="b">
         <v>0</v>
@@ -32999,11 +32999,11 @@
       <c r="K227" s="6" t="b">
         <v>1</v>
       </c>
-      <c r="L227" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="M227" s="5" t="b">
-        <v>0</v>
+      <c r="L227" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="M227" s="6" t="b">
+        <v>1</v>
       </c>
       <c r="N227" s="5" t="b">
         <v>0</v>
@@ -33055,11 +33055,11 @@
       <c r="K228" s="6" t="b">
         <v>1</v>
       </c>
-      <c r="L228" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="M228" s="5" t="b">
-        <v>0</v>
+      <c r="L228" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="M228" s="6" t="b">
+        <v>1</v>
       </c>
       <c r="N228" s="5" t="b">
         <v>0</v>
@@ -33111,11 +33111,11 @@
       <c r="K229" s="6" t="b">
         <v>1</v>
       </c>
-      <c r="L229" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="M229" s="5" t="b">
-        <v>0</v>
+      <c r="L229" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="M229" s="6" t="b">
+        <v>1</v>
       </c>
       <c r="N229" s="5" t="b">
         <v>0</v>
@@ -33447,11 +33447,11 @@
       <c r="K235" s="6" t="b">
         <v>1</v>
       </c>
-      <c r="L235" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="M235" s="5" t="b">
-        <v>0</v>
+      <c r="L235" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="M235" s="6" t="b">
+        <v>1</v>
       </c>
       <c r="N235" s="6" t="b">
         <v>1</v>

</xml_diff>

<commit_message>
generated all the reports on 2025-03-23
</commit_message>
<xml_diff>
--- a/report/merged_configurations.xlsx
+++ b/report/merged_configurations.xlsx
@@ -3500,13 +3500,13 @@
     <t>[{"name":"Verslag Thematische Werkgroep I - 16 januari 2024","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-overlijdensaangifte/standaardenregister/reports/20240116__ThematicWorkshop1_Verslag_OSLOOverlijdensaangifte.pdf"},{"name":"Verslag Thematische Werkgroep II - 20 februari 2024","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-overlijdensaangifte/standaardenregister/reports/20240220_ThematicWorkshop2_Verslag_OSLOOverlijdensaangifte.pdf"},{"name":"Verslag Thematische Werkgroep III - 12 maart 2024","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-overlijdensaangifte/standaardenregister/reports/20240312_ThematicWorkshop3_Verslag_OSLOOverlijdensaangifte.pdf"},{"name":"Verslag Thematische Werkgroep IV - 23 april 2024","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-overlijdensaangifte/standaardenregister/reports/20240423_ThematicWorkshop4_Verslag_OSLOOverlijdensaangifte.pdf"}]</t>
   </si>
   <si>
-    <t>Applicatieprofiel Kindfiche</t>
-  </si>
-  <si>
-    <t>kind-fiche-description.md</t>
-  </si>
-  <si>
-    <t>[{"name":"Applicatieprofiel Kindfiche","resourceReference":"https://data.vlaanderen.be/doc/applicatieprofiel/kindfiche/"}]</t>
+    <t>Applicatieprofiel Dienstverlening Aan Personen</t>
+  </si>
+  <si>
+    <t>dienstverlening-aan-personen-description.md</t>
+  </si>
+  <si>
+    <t>[{"name":"Applicatieprofiel Dienstverlening Aan Personen","resourceReference":"https://data.vlaanderen.be/doc/applicatieprofiel/dienstverlening-aan-personen/"}]</t>
   </si>
   <si>
     <t>[{"name":"Vocabularium Kindfiche","resourceReference":"https://data.vlaanderen.be/ns/kindfiche/"}]</t>

</xml_diff>

<commit_message>
generated all the reports on 2025-03-30
</commit_message>
<xml_diff>
--- a/report/merged_configurations.xlsx
+++ b/report/merged_configurations.xlsx
@@ -2147,10 +2147,10 @@
     <t>{"name":"Charter OSLO Iteratie Cultureel Erfgoed","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-cultureelErfgoed/standaardenregister/charter/Werkgroep_charter_OSLO_iteratie_CE.pdf"}</t>
   </si>
   <si>
-    <t>[{"name":"Verslag Business Werkgroep - 24 september 2024","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-cultureelErfgoed/standaardenregister/reports/20240924_BusinessWorkshop_Verslag_OSLOiteratieCE.pdf"},{"name":"Verslag Thematische Werkgroep 1 - 22 oktober 2024","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-cultureelErfgoed/standaardenregister/reports/20241022_ThematicWorkshop1_Verslag_OSLOiteratieCE.pdf"},{"name":"Verslag Thematische Werkgroep 2 - 19 november 2024","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-cultureelErfgoed/standaardenregister/reports/20241119_ThematicWorkshop2_Verslag_OSLOiteratieCE.pdf"},{"name":"Verslag Thematische Werkgroep 3 - 19 december 2024","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-cultureelErfgoed/standaardenregister/reports/20241219_ThematicWorkshop3_Verslag_OSLOiteratieCE.pdf"}]</t>
-  </si>
-  <si>
-    <t>[{"name":"Presentatie Business Werkgroep - 24 september 2024","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-cultureelErfgoed/standaardenregister/presentations/20240924_BusinessWorkshop_Slides_OSLOiteratieCE.pdf"},{"name":"Presentatie Thematische Werkgroep 1 - 22 oktober 2024","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-cultureelErfgoed/standaardenregister/presentations/20241022_ThematicWorkshop1_Slides_OSLOiteratieCE.pdf"},{"name":"Presentatie Thematische Werkgroep 2 - 19 november 2024","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-cultureelErfgoed/standaardenregister/presentations/20241119_ThematicWorkshop2_Slides_OSLOiteratieCE.pdf"},{"name":"Presentatie Thematische Werkgroep 3 - 19 december 2024","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-cultureelErfgoed/standaardenregister/presentations/20241219_ThematicWorkshop3_Slides_OSLOiteratieCE.pdf"}]</t>
+    <t>[{"name":"Verslag Business Werkgroep - 24 september 2024","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-cultureelErfgoed/standaardenregister/reports/20240924_BusinessWorkshop_Verslag_OSLOiteratieCE.pdf"},{"name":"Verslag Thematische Werkgroep 1 - 22 oktober 2024","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-cultureelErfgoed/standaardenregister/reports/20241022_ThematicWorkshop1_Verslag_OSLOiteratieCE.pdf"},{"name":"Verslag Thematische Werkgroep 2 - 19 november 2024","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-cultureelErfgoed/standaardenregister/reports/20241119_ThematicWorkshop2_Verslag_OSLOiteratieCE.pdf"},{"name":"Verslag Thematische Werkgroep 3 - 19 december 2024","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-cultureelErfgoed/standaardenregister/reports/20241219_ThematicWorkshop3_Verslag_OSLOiteratieCE.pdf"},{"name":"Verslag Thematische Werkgroep 4 - 21 januari 2025","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-cultureelErfgoed/standaardenregister/reports/20250121_ThematicWorkshop4_Verslag_OSLOiteratieCE.pdf"}]</t>
+  </si>
+  <si>
+    <t>[{"name":"Presentatie Business Werkgroep - 24 september 2024","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-cultureelErfgoed/standaardenregister/presentations/20240924_BusinessWorkshop_Slides_OSLOiteratieCE.pdf"},{"name":"Presentatie Thematische Werkgroep 1 - 22 oktober 2024","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-cultureelErfgoed/standaardenregister/presentations/20241022_ThematicWorkshop1_Slides_OSLOiteratieCE.pdf"},{"name":"Presentatie Thematische Werkgroep 2 - 19 november 2024","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-cultureelErfgoed/standaardenregister/presentations/20241119_ThematicWorkshop2_Slides_OSLOiteratieCE.pdf"},{"name":"Presentatie Thematische Werkgroep 3 - 19 december 2024","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-cultureelErfgoed/standaardenregister/presentations/20241219_ThematicWorkshop3_Slides_OSLOiteratieCE.pdf"},{"name":"Presentatie Thematische Werkgroep 4 - 21 januari 2025","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-cultureelErfgoed/standaardenregister/presentations/20250121_ThematicWorkshop4_Slides_OSLOiteratieCE.pdf"}]</t>
   </si>
   <si>
     <t>Charter OSLO Iteratie Cultureel Erfgoed</t>
@@ -12519,7 +12519,7 @@
         <v>85</v>
       </c>
       <c r="Q127" s="4">
-        <v>45736</v>
+        <v>45743</v>
       </c>
       <c r="R127" s="3" t="s">
         <v>28</v>

</xml_diff>

<commit_message>
generated all the reports on 2025-05-04
</commit_message>
<xml_diff>
--- a/report/merged_configurations.xlsx
+++ b/report/merged_configurations.xlsx
@@ -155,190 +155,190 @@
     <t>Aanbevolen (vrijwillig)</t>
   </si>
   <si>
+    <t>kandidaat-standaard</t>
+  </si>
+  <si>
+    <t>[null]</t>
+  </si>
+  <si>
+    <t>description.md</t>
+  </si>
+  <si>
+    <t>[{"name":"Vocabularium Hulp- en Dienstverlening aan Gedetineerden","resourceReference":"https://data.vlaanderen.be/ns/hulp-dienstverlening-gedetineerden/"}]</t>
+  </si>
+  <si>
+    <t>[{"name":"Applicatieprofiel Hulp- en Dienstverlening aan Gedetineerden","resourceReference":"https://data.vlaanderen.be/doc/applicatieprofiel/hulp-dienstverlening-gedetineerden/"}]</t>
+  </si>
+  <si>
+    <t>{"name":"Charter","resourceReference":"https://github.com/Informatievlaanderen/OSLOthema-hulpEnDienstverleningAanGedetineerden/blob/standaardenregister/charter/Werkgroep%20charter%20OSLO_AJH%20HDG.docx"}</t>
+  </si>
+  <si>
+    <t>[{"name":"Verslag business werkgroep -  30 mei 2024","resourceReference":"https://github.com/Informatievlaanderen/OSLOthema-hulpEnDienstverleningAanGedetineerden/blob/standaardenregister/reports/Verslag%20business%20werkgroep%20-%20HDG.pdf"},{"name":"Verslag thematische werkgroep 1 -  25 juni 2024","resourceReference":"https://github.com/Informatievlaanderen/OSLOthema-hulpEnDienstverleningAanGedetineerden/blob/standaardenregister/reports/Verslag%20thematische%20werkgroep%201%20-%20HDG.pdf"},{"name":"Verslag thematische werkgroep 2 -  16 september 2024","resourceReference":"https://github.com/Informatievlaanderen/OSLOthema-hulpEnDienstverleningAanGedetineerden/blob/standaardenregister/reports/Verslag%20thematische%20werkgroep%202%20-%20HDG.pdf"},{"name":"Verslag thematische werkgroep 3 -  22 oktober 2024","resourceReference":"https://github.com/Informatievlaanderen/OSLOthema-hulpEnDienstverleningAanGedetineerden/blob/standaardenregister/reports/Verslag%20thematische%20werkgroep%203%20-%20HDG.pdf"},{"name":"Verslag thematische werkgroep 4 -  25 november 2024","resourceReference":"https://github.com/Informatievlaanderen/OSLOthema-hulpEnDienstverleningAanGedetineerden/blob/standaardenregister/reports/Verslag%20thematische%20werkgroep%204%20-%2025%20november%202024.pdf"}]</t>
+  </si>
+  <si>
+    <t>[{"name":"Presentatie business werkgroep - 30 mei 2024","resourceReference":"https://github.com/Informatievlaanderen/OSLOthema-hulpEnDienstverleningAanGedetineerden/blob/standaardenregister/presentations/Presentatie%20business%20werkgroep%20-%20HDG.pdf"},{"name":"Presentatie thematische werkgroep 1 - 25 juni 2024","resourceReference":"https://github.com/Informatievlaanderen/OSLOthema-hulpEnDienstverleningAanGedetineerden/blob/standaardenregister/presentations/Presentatie%20thematische%20werkgroep%201%20-%20HDG.pdf"},{"name":"Presentatie thematische werkgroep 2 - 16 september 2024","resourceReference":"https://github.com/Informatievlaanderen/OSLOthema-hulpEnDienstverleningAanGedetineerden/blob/standaardenregister/presentations/Presentatie%20thematische%20werkgroep%202%20-%20HDG.pdf"},{"name":"Presentatie thematische werkgroep 3 - 22 oktober 2024","resourceReference":"https://github.com/Informatievlaanderen/OSLOthema-hulpEnDienstverleningAanGedetineerden/blob/standaardenregister/presentations/Presentatie%20thematische%20werkgroep%203%20-%20HDG.pdf"},{"name":"Presentatie thematische werkgroep 4 - 25 november 2024","resourceReference":"https://github.com/Informatievlaanderen/OSLOthema-hulpEnDienstverleningAanGedetineerden/blob/standaardenregister/presentations/Presentatie%20thematische%20werkgroep%204%20-%20HDG.pdf"}]</t>
+  </si>
+  <si>
+    <t>[{"name":"Agentschap Digitaal Vlaanderen","resourceReference":"https://data.vlaanderen.be/id/organisatie/OVO002949"}]</t>
+  </si>
+  <si>
+    <t>Charter</t>
+  </si>
+  <si>
+    <t>https://github.com/Informatievlaanderen/OSLOthema-hulpEnDienstverleningAanGedetineerden/blob/standaardenregister/charter/Werkgroep%20charter%20OSLO_AJH%20HDG.docx</t>
+  </si>
+  <si>
+    <t>Applicatieprofiel Hulp- en Dienstverlening aan Gedetineerden</t>
+  </si>
+  <si>
+    <t>Applicatieprofiel</t>
+  </si>
+  <si>
+    <t>[{"name":"Applicatieprofiel Hulp- en Dienstverlening aan Gedetineerden","resourceReference":"https://data.vlaanderen.be/doc/applicatieprofiel/hulp-dienstverlening-gedetineerden"}]</t>
+  </si>
+  <si>
+    <t>[{"name":"Business werkgroep -  30 mei 2024","resourceReference":"https://github.com/Informatievlaanderen/OSLOthema-hulpEnDienstverleningAanGedetineerden/blob/standaardenregister/reports/Verslag%20business%20werkgroep%20-%20HDG.pdf"},{"name":"Verslag thematische werkgroep 1 -  25 juni 2024","resourceReference":"https://github.com/Informatievlaanderen/OSLOthema-hulpEnDienstverleningAanGedetineerden/blob/standaardenregister/reports/Verslag%20thematische%20werkgroep%201%20-%20HDG.pdf"},{"name":"Verslag thematische werkgroep 2 -  16 september 2024","resourceReference":"https://github.com/Informatievlaanderen/OSLOthema-hulpEnDienstverleningAanGedetineerden/blob/standaardenregister/reports/Verslag%20thematische%20werkgroep%202%20-%20HDG.pdf"},{"name":"Verslag thematische werkgroep 3 -  22 oktober 2024","resourceReference":"https://github.com/Informatievlaanderen/OSLOthema-hulpEnDienstverleningAanGedetineerden/blob/standaardenregister/reports/Verslag%20thematische%20werkgroep%203%20-%20HDG.pdf"},{"name":"Verslag thematische werkgroep 4 -  25 november 2024","resourceReference":"https://github.com/Informatievlaanderen/OSLOthema-hulpEnDienstverleningAanGedetineerden/blob/standaardenregister/reports/Verslag%20thematische%20werkgroep%204%20-%2025%20november%202024.pdf"}]</t>
+  </si>
+  <si>
+    <t>Applicatieprofiel Erosiepoel</t>
+  </si>
+  <si>
+    <t>[{"name":"Applicatieprofiel Erosiepoel","resourceReference":"https://data.vlaanderen.be/doc/applicatieprofiel/erosiepoel"}]</t>
+  </si>
+  <si>
+    <t>[{"name":"Vocabularium Erosiepoel","resourceReference":"https://data.vlaanderen.be/ns/erosiepoel/"}]</t>
+  </si>
+  <si>
+    <t>{"name":"Charter","resourceReference":"https://github.com/Informatievlaanderen/OSLOthema-modderstromen/blob/standaardenregister/charter/Werkgroep%20charter%20OSLO_ModderstroomMonitoring%20-%20OSLO.docx"}</t>
+  </si>
+  <si>
+    <t>[{"name":"Verslag thematische werkgroep 1 -  20 juni 2024","resourceReference":"https://github.com/Informatievlaanderen/OSLOthema-modderstromen/blob/standaardenregister/reports/ThematischeWerkgroep1.pdf"},{"name":"Verslag thematische werkgroep 2 -  6 september 2024","resourceReference":"https://github.com/Informatievlaanderen/OSLOthema-modderstromen/blob/standaardenregister/reports/ThematischeWerkgroep2.pdf"},{"name":"Verslag thematische werkgroep 3 -  28 november 2024","resourceReference":"https://github.com/Informatievlaanderen/OSLOthema-modderstromen/blob/standaardenregister/reports/ThematischeWerkgroep3.pdf"}]</t>
+  </si>
+  <si>
+    <t>[{"name":"Presentatie thematische werkgroep 1 - 20 juni 2024","resourceReference":"https://github.com/Informatievlaanderen/OSLOthema-modderstromen/blob/standaardenregister/presentations/ThematischeWerkgroep1.pdf"},{"name":"Presentatie thematische werkgroep 2 - 6 september 2024","resourceReference":"https://github.com/Informatievlaanderen/OSLOthema-modderstromen/blob/standaardenregister/presentations/ThematischeWerkgroep2.pdf"},{"name":"Presentatie thematische werkgroep 3 - 28 november 2024","resourceReference":"https://github.com/Informatievlaanderen/OSLOthema-modderstromen/blob/standaardenregister/presentations/ThematischeWerkgroep3.pdf"}]</t>
+  </si>
+  <si>
+    <t>https://github.com/Informatievlaanderen/OSLOthema-modderstromen/blob/standaardenregister/charter/Werkgroep%20charter%20OSLO_ModderstroomMonitoring%20-%20OSLO.docx</t>
+  </si>
+  <si>
+    <t>Vocabularium Erosiepoel</t>
+  </si>
+  <si>
+    <t>Applicatieprofiel Mobiliteit: Intelligente Toegang</t>
+  </si>
+  <si>
+    <t>[{"name":"Applicationprofiel Mobiliteit: Intelligente Toegang","resourceReference":"https://data.vlaanderen.be/doc/applicatieprofiel/mobiliteit-intelligente-toegang"}]</t>
+  </si>
+  <si>
+    <t>[{"name":"Vocabularium Mobiliteit: Intelligente Toegang","resourceReference":"https://data.vlaanderen.be/doc/vocabularium/mobiliteit-intelligente-toegang"}]</t>
+  </si>
+  <si>
+    <t>{"name":"Charter OSLO Citerra","resourceReference":"https://github.com/Informatievlaanderen/OSLOthema-citerra/blob/standaardenregister/charter/Werkgroep%20charter%20OSLO_Citerra.docx"}</t>
+  </si>
+  <si>
+    <t>[{"name":"Verslag business werkgroep - 27 februari 2024","resourceReference":"https://github.com/Informatievlaanderen/OSLOthema-citerra/blob/standaardenregister/reports/20240227_BW_Verslag_CoTCiterra.pdf"},{"name":"Verslag thematische werkgroep 1 - 5 juni 2024","resourceReference":"https://github.com/Informatievlaanderen/OSLOthema-citerra/blob/standaardenregister/reports/20240905_ThematischeWerkgroep1_Verslag_OSLOCiterra.pdf"},{"name":"Verslag thematische werkgroep 2 -  3 oktober 2024","resourceReference":"https://github.com/Informatievlaanderen/OSLOthema-citerra/blob/standaardenregister/reports/20241003_ThematischeWerkgroep2_Verslag_OSLOCiterra.pdf"},{"name":"Verslag thematische werkgroep 3 -  14 november 2024","resourceReference":"https://github.com/Informatievlaanderen/OSLOthema-citerra/blob/standaardenregister/reports/20241114_ThematischeWerkgroep3_Verslag_OSLOCiterra.pdf"}]</t>
+  </si>
+  <si>
+    <t>[{"name":"Presentatie thematische werkgroep 1 - 5 juni 2024","resourceReference":"https://github.com/Informatievlaanderen/OSLOthema-citerra/blob/standaardenregister/presentations/20240905_ThematicWorkshop1_Powerpoint_OSLOCiterra.pptx"},{"name":"Presentatie thematische werkgroep 2 - 3 oktober 2024","resourceReference":"https://github.com/Informatievlaanderen/OSLOthema-citerra/blob/standaardenregister/presentations/20241003_ThematicWorkshop2_Powerpoint_OSLOCiterra.pptx"},{"name":"Presentatie thematische werkgroep 3 - 14 november 2024","resourceReference":"https://github.com/Informatievlaanderen/OSLOthema-citerra/blob/standaardenregister/presentations/20241114_ThematicWorkshop3_Powerpoint_OSLOCiterra.pptx"}]</t>
+  </si>
+  <si>
+    <t>Charter OSLO Citerra</t>
+  </si>
+  <si>
+    <t>https://github.com/Informatievlaanderen/OSLOthema-citerra/blob/standaardenregister/charter/Werkgroep%20charter%20OSLO_Citerra.docx</t>
+  </si>
+  <si>
+    <t>Vocabularium Mobiliteit: Intelligente Toegang</t>
+  </si>
+  <si>
+    <t>[{"name":"Applicatieprofiel Mobiliteit: Intelligente Toegang","resourceReference":"https://data.vlaanderen.be/doc/applicatieprofiel/mobiliteit-intelligente-toegang"}]</t>
+  </si>
+  <si>
+    <t>Applicatieprofiel Omgevingsvergunning</t>
+  </si>
+  <si>
+    <t>erkende-standaard</t>
+  </si>
+  <si>
+    <t>["Departement Omgeving"]</t>
+  </si>
+  <si>
+    <t>omgevingsvergunning-description.md</t>
+  </si>
+  <si>
+    <t>[{"name":"Omgevingsvergunning Applicatieprofiel","resourceReference":"https://data.vlaanderen.be/doc/applicatieprofiel/omgevingsvergunning"}]</t>
+  </si>
+  <si>
+    <t>{"name":"Charter","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-omgevingsvergunning/standaardenregister/charter/Werkgroep charter OSLO_omgevingsvergunningen.pdf"}</t>
+  </si>
+  <si>
+    <t>[{"name":"Verslag business werkgroep - 28 augustus 2023","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-omgevingsvergunning/standaardenregister/reports/Verslag Business werkgroep Omgevingsvergunning 2023-08-28.pdf"},{"name":"Verslag thematische werkgroep 1 - 6 november 2023","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-omgevingsvergunning/standaardenregister/reports/Verslag Thematische werkgroep 1 Omgevingsvergunning 2023-11-06.pdf"},{"name":"Verslag thematische werkgroep 2 - 11 december 2023","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-omgevingsvergunning/standaardenregister/reports/Verslag Thematische werkgroep 2 Omgevingsvergunning 2023-12-11.pdf"},{"name":"Verslag thematische werkgroep 3 - 15 januari 2024","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-omgevingsvergunning/standaardenregister/reports/Verslag Thematische werkgroep 3 Omgevingsvergunning 2024-1-15.pdf"},{"name":"Verslag thematische werkgroep 4 - 19 februari 2024","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-omgevingsvergunning/standaardenregister/reports/Verslag Thematische werkgroep 4 Omgevingsvergunning 2024-2-19.pdf"}]</t>
+  </si>
+  <si>
+    <t>[{"name":"Presentatie business werkgroep - 28 augustus 2023","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-omgevingsvergunning/standaardenregister/presentations/Presentatie Business Werkgroep Omgevingsvergunning 2023-08-28.pdf"},{"name":"Presentatie thematische werkgroep 1 - 6 november 2023","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-omgevingsvergunning/standaardenregister/presentations/Presentatie Thematische werkgroep 1 Omgevingsvergunning 2023-11-06.pdf"},{"name":"Presentatie thematische werkgroep 2 - 11 december 2023","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-omgevingsvergunning/standaardenregister/presentations/Presentatie thematische werkgroep 2 Omgevingsvergunning 2023-12-11.pdf"},{"name":"Presentatie thematische werkgroep 3 - 15 januari 2024","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-omgevingsvergunning/standaardenregister/presentations/Presentatie thematische werkgroep 3 Omgevingsvergunning 2024-1-15.pdf"},{"name":"Presentatie thematische werkgroep 4 - 19 februari 2024","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-omgevingsvergunning/standaardenregister/presentations/Presentatie Thematische werkgroep 4 Omgevingsvergunning 2024-2-19.pdf"}]</t>
+  </si>
+  <si>
+    <t>TBD</t>
+  </si>
+  <si>
+    <t>[{"name":"Departement Omgeving","resourceReference":"https://data.vlaanderen.be/doc/organisatie/OVO003323"}]</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-omgevingsvergunning/standaardenregister/charter/Werkgroep charter OSLO_omgevingsvergunningen.pdf</t>
+  </si>
+  <si>
+    <t>OSLOthema-omgevingsvergunning</t>
+  </si>
+  <si>
+    <t>Vocabularium Omgevingsvergunning</t>
+  </si>
+  <si>
+    <t>[{"name":"Omgevingsvergunning Vocabularium","resourceReference":"https://data.vlaanderen.be/ns/omgevingsvergunning"}]</t>
+  </si>
+  <si>
+    <t>Applicatieprofiel Schuldbeheer</t>
+  </si>
+  <si>
+    <t>ap-schuldbeheer-config.md</t>
+  </si>
+  <si>
+    <t>[{"name":"Applicatieprofiel Schuldbeheer","resourceReference":"https://data.vlaanderen.be/doc/applicatieprofiel/schuldbeheer"}]</t>
+  </si>
+  <si>
+    <t>[{"name":"Vocabularium Schuldbeheer","resourceReference":"https://data.vlaanderen.be/ns/schuldbeheer"}]</t>
+  </si>
+  <si>
+    <t>{"name":"Charter Schuldbeheer","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-schuldbeheer/standaardenregister/charter/Projectcharter_OSLOSchuldbeheer.pdf"}</t>
+  </si>
+  <si>
+    <t>[{"name":"Verslag Business Werkgroep - 4 maart 2024","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-schuldbeheer/standaardenregister/reports/20240304_BusinessWorkshop_Verslag_OSLOSchuldbeheer.pdf"},{"name":"Verslag Werksessie Lokale Besturen - 16 april 2024","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-schuldbeheer/standaardenregister/reports/20240416_WerksessieLokaleBesturen_Verslag_OSLOSchuldbeheer.pdf"},{"name":"Verslag Eerste Thematische Werkgroep - 16 mei 2024","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-schuldbeheer/standaardenregister/reports/20240516_ThematicWorkshop1_Verslag_OSLOSchuldbeheer.pdf"},{"name":"Verslag Tweede Thematische Werkgroep - 11 juni 2024","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-schuldbeheer/standaardenregister/reports/20240611_ThematicWorkshop2_Verslag_OSLOSchuldbeheer.pdf"},{"name":"Verslag Derde Thematische Werkgroep - 2 juli 2024","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-schuldbeheer/standaardenregister/reports/20240702_ThematicWorkshop3_Verslag_OSLOSchuldbeheer.pdf"}]</t>
+  </si>
+  <si>
+    <t>[{"name":"Presentatie Business Werkgroep - 4 maart 2024","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-schuldbeheer/standaardenregister/presentations/20240304_BusinessWorkshop_Presentatie_OSLOSchuldbeheer.pptx"},{"name":"Presentatie Werksessie Lokale Besturen - 16 april 2024","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-schuldbeheer/standaardenregister/presentations/20240416_PresentatieWerksessieLokaleBesturen.pptx"},{"name":"Presentatie Eerste Thematische Werkgroep - 16 mei 2024","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-schuldbeheer/standaardenregister/presentations/20240516_ThematicWorkshop1_Powerpoint_OSLOSchuldbeheer.pptx"},{"name":"Presentatie Tweede Thematische Werkgroep - 11 juni 2024","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-schuldbeheer/standaardenregister/presentations/20240611_ThematicWorkshop2_Powerpoint_OSLOSchuldbeheer.pptx"},{"name":"Presentatie Derde Thematische Werkgroep - 2 juli 2024","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-schuldbeheer/standaardenregister/presentations/20240702_ThematicWorkshop3_Powerpoint_OSLOSchuldbeheer.pptx"}]</t>
+  </si>
+  <si>
+    <t>Charter Schuldbeheer</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-schuldbeheer/standaardenregister/charter/Projectcharter_OSLOSchuldbeheer.pdf</t>
+  </si>
+  <si>
+    <t>OSLOthema-schuldbeheer</t>
+  </si>
+  <si>
+    <t>Vocabularium Schuldbeheer</t>
+  </si>
+  <si>
+    <t>voc-schuldbeheer-config.md</t>
+  </si>
+  <si>
+    <t>Applicatieprofiel Kabels en Leidingen</t>
+  </si>
+  <si>
+    <t>Aanbevolen</t>
+  </si>
+  <si>
     <t>standaard-in-ontwikkeling</t>
-  </si>
-  <si>
-    <t>[null]</t>
-  </si>
-  <si>
-    <t>description.md</t>
-  </si>
-  <si>
-    <t>[{"name":"Vocabularium Hulp- en Dienstverlening aan Gedetineerden","resourceReference":"https://data.vlaanderen.be/ns/hulp-dienstverlening-gedetineerden/"}]</t>
-  </si>
-  <si>
-    <t>[{"name":"Applicatieprofiel Hulp- en Dienstverlening aan Gedetineerden","resourceReference":"https://data.vlaanderen.be/doc/applicatieprofiel/hulp-dienstverlening-gedetineerden/"}]</t>
-  </si>
-  <si>
-    <t>{"name":"Charter","resourceReference":"https://github.com/Informatievlaanderen/OSLOthema-hulpEnDienstverleningAanGedetineerden/blob/standaardenregister/charter/Werkgroep%20charter%20OSLO_AJH%20HDG.docx"}</t>
-  </si>
-  <si>
-    <t>[{"name":"Verslag business werkgroep -  30 mei 2024","resourceReference":"https://github.com/Informatievlaanderen/OSLOthema-hulpEnDienstverleningAanGedetineerden/blob/standaardenregister/reports/Verslag%20business%20werkgroep%20-%20HDG.pdf"},{"name":"Verslag thematische werkgroep 1 -  25 juni 2024","resourceReference":"https://github.com/Informatievlaanderen/OSLOthema-hulpEnDienstverleningAanGedetineerden/blob/standaardenregister/reports/Verslag%20thematische%20werkgroep%201%20-%20HDG.pdf"},{"name":"Verslag thematische werkgroep 2 -  16 september 2024","resourceReference":"https://github.com/Informatievlaanderen/OSLOthema-hulpEnDienstverleningAanGedetineerden/blob/standaardenregister/reports/Verslag%20thematische%20werkgroep%202%20-%20HDG.pdf"},{"name":"Verslag thematische werkgroep 3 -  22 oktober 2024","resourceReference":"https://github.com/Informatievlaanderen/OSLOthema-hulpEnDienstverleningAanGedetineerden/blob/standaardenregister/reports/Verslag%20thematische%20werkgroep%203%20-%20HDG.pdf"},{"name":"Verslag thematische werkgroep 4 -  25 november 2024","resourceReference":"https://github.com/Informatievlaanderen/OSLOthema-hulpEnDienstverleningAanGedetineerden/blob/standaardenregister/reports/Verslag%20thematische%20werkgroep%204%20-%2025%20november%202024.pdf"}]</t>
-  </si>
-  <si>
-    <t>[{"name":"Presentatie business werkgroep - 30 mei 2024","resourceReference":"https://github.com/Informatievlaanderen/OSLOthema-hulpEnDienstverleningAanGedetineerden/blob/standaardenregister/presentations/Presentatie%20business%20werkgroep%20-%20HDG.pdf"},{"name":"Presentatie thematische werkgroep 1 - 25 juni 2024","resourceReference":"https://github.com/Informatievlaanderen/OSLOthema-hulpEnDienstverleningAanGedetineerden/blob/standaardenregister/presentations/Presentatie%20thematische%20werkgroep%201%20-%20HDG.pdf"},{"name":"Presentatie thematische werkgroep 2 - 16 september 2024","resourceReference":"https://github.com/Informatievlaanderen/OSLOthema-hulpEnDienstverleningAanGedetineerden/blob/standaardenregister/presentations/Presentatie%20thematische%20werkgroep%202%20-%20HDG.pdf"},{"name":"Presentatie thematische werkgroep 3 - 22 oktober 2024","resourceReference":"https://github.com/Informatievlaanderen/OSLOthema-hulpEnDienstverleningAanGedetineerden/blob/standaardenregister/presentations/Presentatie%20thematische%20werkgroep%203%20-%20HDG.pdf"},{"name":"Presentatie thematische werkgroep 4 - 25 november 2024","resourceReference":"https://github.com/Informatievlaanderen/OSLOthema-hulpEnDienstverleningAanGedetineerden/blob/standaardenregister/presentations/Presentatie%20thematische%20werkgroep%204%20-%20HDG.pdf"}]</t>
-  </si>
-  <si>
-    <t>[{"name":"Agentschap Digitaal Vlaanderen","resourceReference":"https://data.vlaanderen.be/id/organisatie/OVO002949"}]</t>
-  </si>
-  <si>
-    <t>Charter</t>
-  </si>
-  <si>
-    <t>https://github.com/Informatievlaanderen/OSLOthema-hulpEnDienstverleningAanGedetineerden/blob/standaardenregister/charter/Werkgroep%20charter%20OSLO_AJH%20HDG.docx</t>
-  </si>
-  <si>
-    <t>Applicatieprofiel Hulp- en Dienstverlening aan Gedetineerden</t>
-  </si>
-  <si>
-    <t>Applicatieprofiel</t>
-  </si>
-  <si>
-    <t>[{"name":"Applicatieprofiel Hulp- en Dienstverlening aan Gedetineerden","resourceReference":"https://data.vlaanderen.be/doc/applicatieprofiel/hulp-dienstverlening-gedetineerden"}]</t>
-  </si>
-  <si>
-    <t>[{"name":"Business werkgroep -  30 mei 2024","resourceReference":"https://github.com/Informatievlaanderen/OSLOthema-hulpEnDienstverleningAanGedetineerden/blob/standaardenregister/reports/Verslag%20business%20werkgroep%20-%20HDG.pdf"},{"name":"Verslag thematische werkgroep 1 -  25 juni 2024","resourceReference":"https://github.com/Informatievlaanderen/OSLOthema-hulpEnDienstverleningAanGedetineerden/blob/standaardenregister/reports/Verslag%20thematische%20werkgroep%201%20-%20HDG.pdf"},{"name":"Verslag thematische werkgroep 2 -  16 september 2024","resourceReference":"https://github.com/Informatievlaanderen/OSLOthema-hulpEnDienstverleningAanGedetineerden/blob/standaardenregister/reports/Verslag%20thematische%20werkgroep%202%20-%20HDG.pdf"},{"name":"Verslag thematische werkgroep 3 -  22 oktober 2024","resourceReference":"https://github.com/Informatievlaanderen/OSLOthema-hulpEnDienstverleningAanGedetineerden/blob/standaardenregister/reports/Verslag%20thematische%20werkgroep%203%20-%20HDG.pdf"},{"name":"Verslag thematische werkgroep 4 -  25 november 2024","resourceReference":"https://github.com/Informatievlaanderen/OSLOthema-hulpEnDienstverleningAanGedetineerden/blob/standaardenregister/reports/Verslag%20thematische%20werkgroep%204%20-%2025%20november%202024.pdf"}]</t>
-  </si>
-  <si>
-    <t>Applicatieprofiel Erosiepoel</t>
-  </si>
-  <si>
-    <t>[{"name":"Applicatieprofiel Erosiepoel","resourceReference":"https://data.vlaanderen.be/doc/applicatieprofiel/erosiepoel"}]</t>
-  </si>
-  <si>
-    <t>[{"name":"Vocabularium Erosiepoel","resourceReference":"https://data.vlaanderen.be/ns/erosiepoel/"}]</t>
-  </si>
-  <si>
-    <t>{"name":"Charter","resourceReference":"https://github.com/Informatievlaanderen/OSLOthema-modderstromen/blob/standaardenregister/charter/Werkgroep%20charter%20OSLO_ModderstroomMonitoring%20-%20OSLO.docx"}</t>
-  </si>
-  <si>
-    <t>[{"name":"Verslag thematische werkgroep 1 -  20 juni 2024","resourceReference":"https://github.com/Informatievlaanderen/OSLOthema-modderstromen/blob/standaardenregister/reports/ThematischeWerkgroep1.pdf"},{"name":"Verslag thematische werkgroep 2 -  6 september 2024","resourceReference":"https://github.com/Informatievlaanderen/OSLOthema-modderstromen/blob/standaardenregister/reports/ThematischeWerkgroep2.pdf"},{"name":"Verslag thematische werkgroep 3 -  28 november 2024","resourceReference":"https://github.com/Informatievlaanderen/OSLOthema-modderstromen/blob/standaardenregister/reports/ThematischeWerkgroep3.pdf"}]</t>
-  </si>
-  <si>
-    <t>[{"name":"Presentatie thematische werkgroep 1 - 20 juni 2024","resourceReference":"https://github.com/Informatievlaanderen/OSLOthema-modderstromen/blob/standaardenregister/presentations/ThematischeWerkgroep1.pdf"},{"name":"Presentatie thematische werkgroep 2 - 6 september 2024","resourceReference":"https://github.com/Informatievlaanderen/OSLOthema-modderstromen/blob/standaardenregister/presentations/ThematischeWerkgroep2.pdf"},{"name":"Presentatie thematische werkgroep 3 - 28 november 2024","resourceReference":"https://github.com/Informatievlaanderen/OSLOthema-modderstromen/blob/standaardenregister/presentations/ThematischeWerkgroep3.pdf"}]</t>
-  </si>
-  <si>
-    <t>https://github.com/Informatievlaanderen/OSLOthema-modderstromen/blob/standaardenregister/charter/Werkgroep%20charter%20OSLO_ModderstroomMonitoring%20-%20OSLO.docx</t>
-  </si>
-  <si>
-    <t>Vocabularium Erosiepoel</t>
-  </si>
-  <si>
-    <t>Applicatieprofiel Mobiliteit: Intelligente Toegang</t>
-  </si>
-  <si>
-    <t>[{"name":"Applicationprofiel Mobiliteit: Intelligente Toegang","resourceReference":"https://data.vlaanderen.be/doc/applicatieprofiel/mobiliteit-intelligente-toegang"}]</t>
-  </si>
-  <si>
-    <t>[{"name":"Vocabularium Mobiliteit: Intelligente Toegang","resourceReference":"https://data.vlaanderen.be/doc/vocabularium/mobiliteit-intelligente-toegang"}]</t>
-  </si>
-  <si>
-    <t>{"name":"Charter OSLO Citerra","resourceReference":"https://github.com/Informatievlaanderen/OSLOthema-citerra/blob/standaardenregister/charter/Werkgroep%20charter%20OSLO_Citerra.docx"}</t>
-  </si>
-  <si>
-    <t>[{"name":"Verslag business werkgroep - 27 februari 2024","resourceReference":"https://github.com/Informatievlaanderen/OSLOthema-citerra/blob/standaardenregister/reports/20240227_BW_Verslag_CoTCiterra.pdf"},{"name":"Verslag thematische werkgroep 1 - 5 juni 2024","resourceReference":"https://github.com/Informatievlaanderen/OSLOthema-citerra/blob/standaardenregister/reports/20240905_ThematischeWerkgroep1_Verslag_OSLOCiterra.pdf"},{"name":"Verslag thematische werkgroep 2 -  3 oktober 2024","resourceReference":"https://github.com/Informatievlaanderen/OSLOthema-citerra/blob/standaardenregister/reports/20241003_ThematischeWerkgroep2_Verslag_OSLOCiterra.pdf"},{"name":"Verslag thematische werkgroep 3 -  14 november 2024","resourceReference":"https://github.com/Informatievlaanderen/OSLOthema-citerra/blob/standaardenregister/reports/20241114_ThematischeWerkgroep3_Verslag_OSLOCiterra.pdf"}]</t>
-  </si>
-  <si>
-    <t>[{"name":"Presentatie thematische werkgroep 1 - 5 juni 2024","resourceReference":"https://github.com/Informatievlaanderen/OSLOthema-citerra/blob/standaardenregister/presentations/20240905_ThematicWorkshop1_Powerpoint_OSLOCiterra.pptx"},{"name":"Presentatie thematische werkgroep 2 - 3 oktober 2024","resourceReference":"https://github.com/Informatievlaanderen/OSLOthema-citerra/blob/standaardenregister/presentations/20241003_ThematicWorkshop2_Powerpoint_OSLOCiterra.pptx"},{"name":"Presentatie thematische werkgroep 3 - 14 november 2024","resourceReference":"https://github.com/Informatievlaanderen/OSLOthema-citerra/blob/standaardenregister/presentations/20241114_ThematicWorkshop3_Powerpoint_OSLOCiterra.pptx"}]</t>
-  </si>
-  <si>
-    <t>Charter OSLO Citerra</t>
-  </si>
-  <si>
-    <t>https://github.com/Informatievlaanderen/OSLOthema-citerra/blob/standaardenregister/charter/Werkgroep%20charter%20OSLO_Citerra.docx</t>
-  </si>
-  <si>
-    <t>Vocabularium Mobiliteit: Intelligente Toegang</t>
-  </si>
-  <si>
-    <t>[{"name":"Applicatieprofiel Mobiliteit: Intelligente Toegang","resourceReference":"https://data.vlaanderen.be/doc/applicatieprofiel/mobiliteit-intelligente-toegang"}]</t>
-  </si>
-  <si>
-    <t>Applicatieprofiel Omgevingsvergunning</t>
-  </si>
-  <si>
-    <t>erkende-standaard</t>
-  </si>
-  <si>
-    <t>["Departement Omgeving"]</t>
-  </si>
-  <si>
-    <t>omgevingsvergunning-description.md</t>
-  </si>
-  <si>
-    <t>[{"name":"Omgevingsvergunning Applicatieprofiel","resourceReference":"https://data.vlaanderen.be/doc/applicatieprofiel/omgevingsvergunning"}]</t>
-  </si>
-  <si>
-    <t>{"name":"Charter","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-omgevingsvergunning/standaardenregister/charter/Werkgroep charter OSLO_omgevingsvergunningen.pdf"}</t>
-  </si>
-  <si>
-    <t>[{"name":"Verslag business werkgroep - 28 augustus 2023","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-omgevingsvergunning/standaardenregister/reports/Verslag Business werkgroep Omgevingsvergunning 2023-08-28.pdf"},{"name":"Verslag thematische werkgroep 1 - 6 november 2023","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-omgevingsvergunning/standaardenregister/reports/Verslag Thematische werkgroep 1 Omgevingsvergunning 2023-11-06.pdf"},{"name":"Verslag thematische werkgroep 2 - 11 december 2023","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-omgevingsvergunning/standaardenregister/reports/Verslag Thematische werkgroep 2 Omgevingsvergunning 2023-12-11.pdf"},{"name":"Verslag thematische werkgroep 3 - 15 januari 2024","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-omgevingsvergunning/standaardenregister/reports/Verslag Thematische werkgroep 3 Omgevingsvergunning 2024-1-15.pdf"},{"name":"Verslag thematische werkgroep 4 - 19 februari 2024","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-omgevingsvergunning/standaardenregister/reports/Verslag Thematische werkgroep 4 Omgevingsvergunning 2024-2-19.pdf"}]</t>
-  </si>
-  <si>
-    <t>[{"name":"Presentatie business werkgroep - 28 augustus 2023","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-omgevingsvergunning/standaardenregister/presentations/Presentatie Business Werkgroep Omgevingsvergunning 2023-08-28.pdf"},{"name":"Presentatie thematische werkgroep 1 - 6 november 2023","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-omgevingsvergunning/standaardenregister/presentations/Presentatie Thematische werkgroep 1 Omgevingsvergunning 2023-11-06.pdf"},{"name":"Presentatie thematische werkgroep 2 - 11 december 2023","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-omgevingsvergunning/standaardenregister/presentations/Presentatie thematische werkgroep 2 Omgevingsvergunning 2023-12-11.pdf"},{"name":"Presentatie thematische werkgroep 3 - 15 januari 2024","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-omgevingsvergunning/standaardenregister/presentations/Presentatie thematische werkgroep 3 Omgevingsvergunning 2024-1-15.pdf"},{"name":"Presentatie thematische werkgroep 4 - 19 februari 2024","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-omgevingsvergunning/standaardenregister/presentations/Presentatie Thematische werkgroep 4 Omgevingsvergunning 2024-2-19.pdf"}]</t>
-  </si>
-  <si>
-    <t>TBD</t>
-  </si>
-  <si>
-    <t>[{"name":"Departement Omgeving","resourceReference":"https://data.vlaanderen.be/doc/organisatie/OVO003323"}]</t>
-  </si>
-  <si>
-    <t>https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-omgevingsvergunning/standaardenregister/charter/Werkgroep charter OSLO_omgevingsvergunningen.pdf</t>
-  </si>
-  <si>
-    <t>OSLOthema-omgevingsvergunning</t>
-  </si>
-  <si>
-    <t>Vocabularium Omgevingsvergunning</t>
-  </si>
-  <si>
-    <t>[{"name":"Omgevingsvergunning Vocabularium","resourceReference":"https://data.vlaanderen.be/ns/omgevingsvergunning"}]</t>
-  </si>
-  <si>
-    <t>Applicatieprofiel Schuldbeheer</t>
-  </si>
-  <si>
-    <t>kandidaat-standaard</t>
-  </si>
-  <si>
-    <t>ap-schuldbeheer-config.md</t>
-  </si>
-  <si>
-    <t>[{"name":"Applicatieprofiel Schuldbeheer","resourceReference":"https://data.vlaanderen.be/doc/applicatieprofiel/schuldbeheer"}]</t>
-  </si>
-  <si>
-    <t>[{"name":"Vocabularium Schuldbeheer","resourceReference":"https://data.vlaanderen.be/ns/schuldbeheer"}]</t>
-  </si>
-  <si>
-    <t>{"name":"Charter Schuldbeheer","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-schuldbeheer/standaardenregister/charter/Projectcharter_OSLOSchuldbeheer.pdf"}</t>
-  </si>
-  <si>
-    <t>[{"name":"Verslag Business Werkgroep - 4 maart 2024","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-schuldbeheer/standaardenregister/reports/20240304_BusinessWorkshop_Verslag_OSLOSchuldbeheer.pdf"},{"name":"Verslag Werksessie Lokale Besturen - 16 april 2024","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-schuldbeheer/standaardenregister/reports/20240416_WerksessieLokaleBesturen_Verslag_OSLOSchuldbeheer.pdf"},{"name":"Verslag Eerste Thematische Werkgroep - 16 mei 2024","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-schuldbeheer/standaardenregister/reports/20240516_ThematicWorkshop1_Verslag_OSLOSchuldbeheer.pdf"},{"name":"Verslag Tweede Thematische Werkgroep - 11 juni 2024","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-schuldbeheer/standaardenregister/reports/20240611_ThematicWorkshop2_Verslag_OSLOSchuldbeheer.pdf"},{"name":"Verslag Derde Thematische Werkgroep - 2 juli 2024","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-schuldbeheer/standaardenregister/reports/20240702_ThematicWorkshop3_Verslag_OSLOSchuldbeheer.pdf"}]</t>
-  </si>
-  <si>
-    <t>[{"name":"Presentatie Business Werkgroep - 4 maart 2024","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-schuldbeheer/standaardenregister/presentations/20240304_BusinessWorkshop_Presentatie_OSLOSchuldbeheer.pptx"},{"name":"Presentatie Werksessie Lokale Besturen - 16 april 2024","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-schuldbeheer/standaardenregister/presentations/20240416_PresentatieWerksessieLokaleBesturen.pptx"},{"name":"Presentatie Eerste Thematische Werkgroep - 16 mei 2024","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-schuldbeheer/standaardenregister/presentations/20240516_ThematicWorkshop1_Powerpoint_OSLOSchuldbeheer.pptx"},{"name":"Presentatie Tweede Thematische Werkgroep - 11 juni 2024","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-schuldbeheer/standaardenregister/presentations/20240611_ThematicWorkshop2_Powerpoint_OSLOSchuldbeheer.pptx"},{"name":"Presentatie Derde Thematische Werkgroep - 2 juli 2024","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-schuldbeheer/standaardenregister/presentations/20240702_ThematicWorkshop3_Powerpoint_OSLOSchuldbeheer.pptx"}]</t>
-  </si>
-  <si>
-    <t>Charter Schuldbeheer</t>
-  </si>
-  <si>
-    <t>https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-schuldbeheer/standaardenregister/charter/Projectcharter_OSLOSchuldbeheer.pdf</t>
-  </si>
-  <si>
-    <t>OSLOthema-schuldbeheer</t>
-  </si>
-  <si>
-    <t>Vocabularium Schuldbeheer</t>
-  </si>
-  <si>
-    <t>voc-schuldbeheer-config.md</t>
-  </si>
-  <si>
-    <t>Applicatieprofiel Kabels en Leidingen</t>
-  </si>
-  <si>
-    <t>Aanbevolen</t>
   </si>
   <si>
     <t>kabels-en-leidingen-description.md</t>
@@ -4935,7 +4935,7 @@
         <v>46</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>95</v>
+        <v>47</v>
       </c>
       <c r="E14" s="3" t="s">
         <v>40</v>
@@ -4947,22 +4947,22 @@
         <v>45540</v>
       </c>
       <c r="H14" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="I14" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="I14" s="3" t="s">
+      <c r="J14" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="J14" s="3" t="s">
+      <c r="K14" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="K14" s="3" t="s">
+      <c r="L14" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="L14" s="3" t="s">
+      <c r="M14" s="3" t="s">
         <v>100</v>
-      </c>
-      <c r="M14" s="3" t="s">
-        <v>101</v>
       </c>
       <c r="N14" s="4">
         <v>45372</v>
@@ -4984,18 +4984,18 @@
         <v>55</v>
       </c>
       <c r="U14" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="V14" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="V14" s="3" t="s">
+      <c r="W14" s="3" t="s">
         <v>103</v>
-      </c>
-      <c r="W14" s="3" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="15" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>45</v>
@@ -5004,7 +5004,7 @@
         <v>46</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>95</v>
+        <v>47</v>
       </c>
       <c r="E15" s="3" t="s">
         <v>40</v>
@@ -5016,22 +5016,22 @@
         <v>45540</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="I15" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="J15" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="K15" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="J15" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="K15" s="3" t="s">
+      <c r="L15" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="L15" s="3" t="s">
+      <c r="M15" s="3" t="s">
         <v>100</v>
-      </c>
-      <c r="M15" s="3" t="s">
-        <v>101</v>
       </c>
       <c r="N15" s="4">
         <v>45372</v>
@@ -5053,27 +5053,27 @@
         <v>55</v>
       </c>
       <c r="U15" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="V15" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="V15" s="3" t="s">
+      <c r="W15" s="3" t="s">
         <v>103</v>
-      </c>
-      <c r="W15" s="3" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="16" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>59</v>
       </c>
       <c r="C16" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="D16" s="3" t="s">
         <v>108</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>47</v>
       </c>
       <c r="E16" s="3" t="s">
         <v>40</v>
@@ -5135,10 +5135,10 @@
         <v>45</v>
       </c>
       <c r="C17" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="D17" s="3" t="s">
         <v>108</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>47</v>
       </c>
       <c r="E17" s="3" t="s">
         <v>40</v>
@@ -5203,7 +5203,7 @@
         <v>46</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>47</v>
+        <v>108</v>
       </c>
       <c r="E18" s="3" t="s">
         <v>40</v>
@@ -5270,7 +5270,7 @@
         <v>46</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>47</v>
+        <v>108</v>
       </c>
       <c r="E19" s="3" t="s">
         <v>40</v>
@@ -5475,7 +5475,7 @@
         <v>46</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>47</v>
+        <v>108</v>
       </c>
       <c r="E22" s="3" t="s">
         <v>40</v>
@@ -5952,7 +5952,7 @@
         <v>46</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>47</v>
+        <v>108</v>
       </c>
       <c r="E29" s="3" t="s">
         <v>198</v>
@@ -6019,7 +6019,7 @@
         <v>46</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>47</v>
+        <v>108</v>
       </c>
       <c r="E30" s="3" t="s">
         <v>198</v>
@@ -6086,7 +6086,7 @@
         <v>46</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>95</v>
+        <v>47</v>
       </c>
       <c r="E31" s="3" t="s">
         <v>198</v>
@@ -6153,7 +6153,7 @@
         <v>46</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>95</v>
+        <v>47</v>
       </c>
       <c r="E32" s="3" t="s">
         <v>198</v>
@@ -6220,7 +6220,7 @@
         <v>46</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>47</v>
+        <v>108</v>
       </c>
       <c r="E33" s="3" t="s">
         <v>198</v>
@@ -6287,7 +6287,7 @@
         <v>46</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>47</v>
+        <v>108</v>
       </c>
       <c r="E34" s="3" t="s">
         <v>198</v>
@@ -6354,7 +6354,7 @@
         <v>46</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>47</v>
+        <v>108</v>
       </c>
       <c r="E35" s="3" t="s">
         <v>198</v>
@@ -6421,7 +6421,7 @@
         <v>46</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>47</v>
+        <v>108</v>
       </c>
       <c r="E36" s="3" t="s">
         <v>198</v>
@@ -6488,7 +6488,7 @@
         <v>46</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>47</v>
+        <v>108</v>
       </c>
       <c r="E37" s="3" t="s">
         <v>198</v>
@@ -6555,7 +6555,7 @@
         <v>46</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>47</v>
+        <v>108</v>
       </c>
       <c r="E38" s="3" t="s">
         <v>198</v>
@@ -6622,7 +6622,7 @@
         <v>46</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>47</v>
+        <v>108</v>
       </c>
       <c r="E39" s="3" t="s">
         <v>198</v>
@@ -6689,7 +6689,7 @@
         <v>46</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>47</v>
+        <v>108</v>
       </c>
       <c r="E40" s="3" t="s">
         <v>198</v>
@@ -6756,7 +6756,7 @@
         <v>46</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>47</v>
+        <v>108</v>
       </c>
       <c r="E41" s="3" t="s">
         <v>198</v>
@@ -6823,7 +6823,7 @@
         <v>46</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>47</v>
+        <v>108</v>
       </c>
       <c r="E42" s="3" t="s">
         <v>198</v>
@@ -6890,7 +6890,7 @@
         <v>46</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>47</v>
+        <v>108</v>
       </c>
       <c r="E43" s="3" t="s">
         <v>198</v>
@@ -6957,7 +6957,7 @@
         <v>46</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>47</v>
+        <v>108</v>
       </c>
       <c r="E44" s="3" t="s">
         <v>198</v>
@@ -7024,7 +7024,7 @@
         <v>46</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>47</v>
+        <v>108</v>
       </c>
       <c r="E45" s="3" t="s">
         <v>198</v>
@@ -7091,7 +7091,7 @@
         <v>46</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>47</v>
+        <v>108</v>
       </c>
       <c r="E46" s="3" t="s">
         <v>198</v>
@@ -7158,7 +7158,7 @@
         <v>46</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>47</v>
+        <v>108</v>
       </c>
       <c r="E47" s="3" t="s">
         <v>198</v>
@@ -7225,7 +7225,7 @@
         <v>46</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>47</v>
+        <v>108</v>
       </c>
       <c r="E48" s="3" t="s">
         <v>198</v>
@@ -7426,7 +7426,7 @@
         <v>46</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>95</v>
+        <v>47</v>
       </c>
       <c r="E51" s="3" t="s">
         <v>292</v>
@@ -7493,7 +7493,7 @@
         <v>46</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>95</v>
+        <v>47</v>
       </c>
       <c r="E52" s="3" t="s">
         <v>292</v>
@@ -7560,7 +7560,7 @@
         <v>46</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>95</v>
+        <v>47</v>
       </c>
       <c r="E53" s="3" t="s">
         <v>183</v>
@@ -7627,7 +7627,7 @@
         <v>46</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>95</v>
+        <v>47</v>
       </c>
       <c r="E54" s="3" t="s">
         <v>183</v>
@@ -8029,7 +8029,7 @@
         <v>347</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>95</v>
+        <v>47</v>
       </c>
       <c r="E60" s="3" t="s">
         <v>40</v>
@@ -8163,7 +8163,7 @@
         <v>46</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>95</v>
+        <v>47</v>
       </c>
       <c r="E62" s="3" t="s">
         <v>40</v>
@@ -8431,7 +8431,7 @@
         <v>46</v>
       </c>
       <c r="D66" s="3" t="s">
-        <v>95</v>
+        <v>47</v>
       </c>
       <c r="E66" s="3" t="s">
         <v>40</v>
@@ -8632,7 +8632,7 @@
         <v>46</v>
       </c>
       <c r="D69" s="3" t="s">
-        <v>95</v>
+        <v>47</v>
       </c>
       <c r="E69" s="3" t="s">
         <v>40</v>
@@ -8833,7 +8833,7 @@
         <v>46</v>
       </c>
       <c r="D72" s="3" t="s">
-        <v>95</v>
+        <v>47</v>
       </c>
       <c r="E72" s="3" t="s">
         <v>40</v>
@@ -8967,7 +8967,7 @@
         <v>46</v>
       </c>
       <c r="D74" s="3" t="s">
-        <v>95</v>
+        <v>47</v>
       </c>
       <c r="E74" s="3" t="s">
         <v>40</v>
@@ -9034,7 +9034,7 @@
         <v>46</v>
       </c>
       <c r="D75" s="3" t="s">
-        <v>95</v>
+        <v>47</v>
       </c>
       <c r="E75" s="3" t="s">
         <v>40</v>
@@ -9101,7 +9101,7 @@
         <v>46</v>
       </c>
       <c r="D76" s="3" t="s">
-        <v>95</v>
+        <v>47</v>
       </c>
       <c r="E76" s="3" t="s">
         <v>40</v>
@@ -9637,7 +9637,7 @@
         <v>46</v>
       </c>
       <c r="D84" s="3" t="s">
-        <v>95</v>
+        <v>47</v>
       </c>
       <c r="E84" s="3" t="s">
         <v>490</v>
@@ -9704,7 +9704,7 @@
         <v>46</v>
       </c>
       <c r="D85" s="3" t="s">
-        <v>95</v>
+        <v>47</v>
       </c>
       <c r="E85" s="3" t="s">
         <v>490</v>
@@ -12183,7 +12183,7 @@
         <v>46</v>
       </c>
       <c r="D122" s="3" t="s">
-        <v>95</v>
+        <v>47</v>
       </c>
       <c r="E122" s="3" t="s">
         <v>670</v>
@@ -12585,7 +12585,7 @@
         <v>46</v>
       </c>
       <c r="D128" s="3" t="s">
-        <v>47</v>
+        <v>108</v>
       </c>
       <c r="E128" s="3" t="s">
         <v>183</v>
@@ -12654,7 +12654,7 @@
         <v>46</v>
       </c>
       <c r="D129" s="3" t="s">
-        <v>95</v>
+        <v>47</v>
       </c>
       <c r="E129" s="3" t="s">
         <v>719</v>
@@ -12721,7 +12721,7 @@
         <v>46</v>
       </c>
       <c r="D130" s="3" t="s">
-        <v>95</v>
+        <v>47</v>
       </c>
       <c r="E130" s="3" t="s">
         <v>719</v>
@@ -14325,7 +14325,7 @@
         <v>88</v>
       </c>
       <c r="D154" s="3" t="s">
-        <v>47</v>
+        <v>108</v>
       </c>
       <c r="E154" s="3" t="s">
         <v>40</v>
@@ -14392,7 +14392,7 @@
         <v>88</v>
       </c>
       <c r="D155" s="3" t="s">
-        <v>47</v>
+        <v>108</v>
       </c>
       <c r="E155" s="3" t="s">
         <v>40</v>
@@ -17340,7 +17340,7 @@
         <v>88</v>
       </c>
       <c r="D199" s="3" t="s">
-        <v>47</v>
+        <v>108</v>
       </c>
       <c r="E199" s="3" t="s">
         <v>40</v>
@@ -17407,7 +17407,7 @@
         <v>46</v>
       </c>
       <c r="D200" s="3" t="s">
-        <v>95</v>
+        <v>47</v>
       </c>
       <c r="E200" s="3" t="s">
         <v>40</v>
@@ -17476,7 +17476,7 @@
         <v>46</v>
       </c>
       <c r="D201" s="3" t="s">
-        <v>95</v>
+        <v>47</v>
       </c>
       <c r="E201" s="3" t="s">
         <v>40</v>
@@ -17612,7 +17612,7 @@
         <v>46</v>
       </c>
       <c r="D203" s="3" t="s">
-        <v>47</v>
+        <v>108</v>
       </c>
       <c r="E203" s="3" t="s">
         <v>40</v>
@@ -18014,7 +18014,7 @@
         <v>46</v>
       </c>
       <c r="D209" s="3" t="s">
-        <v>95</v>
+        <v>47</v>
       </c>
       <c r="E209" s="3" t="s">
         <v>183</v>
@@ -18085,7 +18085,7 @@
         <v>46</v>
       </c>
       <c r="D210" s="3" t="s">
-        <v>95</v>
+        <v>47</v>
       </c>
       <c r="E210" s="3" t="s">
         <v>183</v>
@@ -18156,7 +18156,7 @@
         <v>46</v>
       </c>
       <c r="D211" s="3" t="s">
-        <v>95</v>
+        <v>47</v>
       </c>
       <c r="E211" s="3" t="s">
         <v>40</v>
@@ -18223,7 +18223,7 @@
         <v>46</v>
       </c>
       <c r="D212" s="3" t="s">
-        <v>95</v>
+        <v>47</v>
       </c>
       <c r="E212" s="3" t="s">
         <v>40</v>
@@ -18420,7 +18420,7 @@
         <v>46</v>
       </c>
       <c r="D215" s="3" t="s">
-        <v>95</v>
+        <v>47</v>
       </c>
       <c r="E215" s="3" t="s">
         <v>1052</v>
@@ -18491,7 +18491,7 @@
         <v>46</v>
       </c>
       <c r="D216" s="3" t="s">
-        <v>47</v>
+        <v>108</v>
       </c>
       <c r="E216" s="3" t="s">
         <v>1052</v>
@@ -18696,7 +18696,7 @@
         <v>46</v>
       </c>
       <c r="D219" s="3" t="s">
-        <v>47</v>
+        <v>108</v>
       </c>
       <c r="E219" s="3" t="s">
         <v>40</v>
@@ -18753,7 +18753,7 @@
         <v>46</v>
       </c>
       <c r="D220" s="3" t="s">
-        <v>47</v>
+        <v>108</v>
       </c>
       <c r="E220" s="3" t="s">
         <v>40</v>
@@ -18820,7 +18820,7 @@
         <v>46</v>
       </c>
       <c r="D221" s="3" t="s">
-        <v>47</v>
+        <v>108</v>
       </c>
       <c r="E221" s="3" t="s">
         <v>40</v>
@@ -19636,7 +19636,7 @@
         <v>46</v>
       </c>
       <c r="D233" s="3" t="s">
-        <v>95</v>
+        <v>47</v>
       </c>
       <c r="E233" s="3" t="s">
         <v>40</v>
@@ -19705,7 +19705,7 @@
         <v>46</v>
       </c>
       <c r="D234" s="3" t="s">
-        <v>95</v>
+        <v>47</v>
       </c>
       <c r="E234" s="3" t="s">
         <v>40</v>
@@ -19774,7 +19774,7 @@
         <v>46</v>
       </c>
       <c r="D235" s="3" t="s">
-        <v>95</v>
+        <v>47</v>
       </c>
       <c r="E235" s="3" t="s">
         <v>1177</v>
@@ -19841,7 +19841,7 @@
         <v>46</v>
       </c>
       <c r="D236" s="3" t="s">
-        <v>95</v>
+        <v>47</v>
       </c>
       <c r="E236" s="3" t="s">
         <v>1177</v>
@@ -19908,7 +19908,7 @@
         <v>46</v>
       </c>
       <c r="D237" s="3" t="s">
-        <v>95</v>
+        <v>47</v>
       </c>
       <c r="E237" s="3" t="s">
         <v>1177</v>
@@ -20046,7 +20046,7 @@
         <v>46</v>
       </c>
       <c r="D239" s="3" t="s">
-        <v>95</v>
+        <v>47</v>
       </c>
       <c r="E239" s="3" t="s">
         <v>1177</v>
@@ -20113,7 +20113,7 @@
         <v>46</v>
       </c>
       <c r="D240" s="3" t="s">
-        <v>95</v>
+        <v>47</v>
       </c>
       <c r="E240" s="3" t="s">
         <v>1177</v>
@@ -20180,7 +20180,7 @@
         <v>46</v>
       </c>
       <c r="D241" s="3" t="s">
-        <v>95</v>
+        <v>47</v>
       </c>
       <c r="E241" s="3" t="s">
         <v>1177</v>
@@ -20247,7 +20247,7 @@
         <v>46</v>
       </c>
       <c r="D242" s="3" t="s">
-        <v>95</v>
+        <v>47</v>
       </c>
       <c r="E242" s="3" t="s">
         <v>40</v>
@@ -20316,7 +20316,7 @@
         <v>46</v>
       </c>
       <c r="D243" s="3" t="s">
-        <v>95</v>
+        <v>47</v>
       </c>
       <c r="E243" s="3" t="s">
         <v>40</v>
@@ -20385,7 +20385,7 @@
         <v>1220</v>
       </c>
       <c r="D244" s="3" t="s">
-        <v>47</v>
+        <v>108</v>
       </c>
       <c r="E244" s="3" t="s">
         <v>40</v>
@@ -20452,7 +20452,7 @@
         <v>1220</v>
       </c>
       <c r="D245" s="3" t="s">
-        <v>47</v>
+        <v>108</v>
       </c>
       <c r="E245" s="3" t="s">
         <v>40</v>
@@ -21446,7 +21446,7 @@
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B15" s="6" t="b">
         <v>1</v>
@@ -21502,7 +21502,7 @@
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B16" s="6" t="b">
         <v>1</v>

</xml_diff>

<commit_message>
generated all the reports on 2025-06-22
</commit_message>
<xml_diff>
--- a/report/merged_configurations.xlsx
+++ b/report/merged_configurations.xlsx
@@ -131,19 +131,19 @@
     <t>[{"name":"Vocabularium Thermografische Gebouwanalyse","resourceReference":"https://data.vlaanderen.be/ns/thermografische-gebouwanalyse"}]</t>
   </si>
   <si>
-    <t>[{"name":"Charter Thermografische Beeldanalyse","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-thermAI/standaardenregister/charter/Charter_OSLO_thermAI.pdf"}]</t>
-  </si>
-  <si>
-    <t>[{"name":"Verslag Business werkgroep - 18-02-2025","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-thermAI/standaardenregister/reports/Business%20werkgroep%20CoT%20ThermAI%202025-02-18.pdf"},{"name":"Verslag Thematische Werkgroep 1 - 18-03-2025","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-thermAI/standaardenregister/reports/Thematische%20werkgroep%201%20-%20CoT%20ThermAI%202025-03-18.pdf"},{"name":"Verslag Thematische Werkgroep 2 - 15-04-2025","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-thermAI/standaardenregister/reports/Thematische%20werkgroep%202%20-%20CoT%20ThermAI%202025-04-15.pdf"}]</t>
-  </si>
-  <si>
-    <t>[{"name":"Presentatie Business Werkgroep - 18-02-2025","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-thermAI/standaardenregister/presentations/ThermAI%20Business%20Werkgroep%20(1).pdf"},{"name":"Presentatie Thematische Werkgroep 1 - 18-03-2025","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-thermAI/standaardenregister/presentations/Thematische%20werkgroep%201%20-%20ThermAI.pdf"},{"name":"Presentatie Thematische Werkgroep 2 - 15-04-2025","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-thermAI/standaardenregister/presentations/Thematische%20werkgroep%202%20-%20ThermAI.pdf"}]</t>
+    <t>[{"name":"Charter Thermografische Gebouwanalyse","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-thermAI/standaardenregister/charter/Charter_OSLO_thermAI.pdf"}]</t>
+  </si>
+  <si>
+    <t>[{"name":"Verslag Business werkgroep - 18-02-2025","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-thermAI/standaardenregister/reports/Business%20werkgroep%20CoT%20ThermAI%202025-02-18.pdf"},{"name":"Verslag Thematische Werkgroep 1 - 18-03-2025","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-thermAI/standaardenregister/reports/Thematische%20werkgroep%201%20-%20CoT%20ThermAI%202025-03-18.pdf"},{"name":"Verslag Thematische Werkgroep 2 - 15-04-2025","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-thermAI/standaardenregister/reports/Thematische%20werkgroep%202%20-%20CoT%20ThermAI%202025-04-15.pdf"},{"name":"Verslag Thematische Werkgroep 3 - 15-05-2025","resourceReference":"https://github.com/Informatievlaanderen/OSLOthema-thermAI/blob/standaardenregister/reports/Verslag%20Thematische%20werkgroep%203%20-%20CoT%20ThermAI%202025-04-15.docx.pdf"}]</t>
+  </si>
+  <si>
+    <t>[{"name":"Presentatie Business Werkgroep - 18-02-2025","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-thermAI/standaardenregister/presentations/ThermAI%20Business%20Werkgroep%20(1).pdf"},{"name":"Presentatie Thematische Werkgroep 1 - 18-03-2025","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-thermAI/standaardenregister/presentations/Thematische%20werkgroep%201%20-%20ThermAI.pdf"},{"name":"Presentatie Thematische Werkgroep 2 - 15-04-2025","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-thermAI/standaardenregister/presentations/Thematische%20werkgroep%202%20-%20ThermAI.pdf"},{"name":"Presentatie Thematische Werkgroep 3 - 15-05-2025","resourceReference":"https://github.com/Informatievlaanderen/OSLOthema-thermAI/blob/standaardenregister/presentations/Slides%20-%20Thematische%20werkgroep%203%20-%20ThermAI.pdf"}]</t>
   </si>
   <si>
     <t>2024-12-1</t>
   </si>
   <si>
-    <t>["Charter Thermografische Beeldanalyse"]</t>
+    <t>["Charter Thermografische Gebouwanalyse"]</t>
   </si>
   <si>
     <t>["https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-thermAI/standaardenregister/charter/Charter_OSLO_thermAI.pdf"]</t>
@@ -191,7 +191,7 @@
     <t>[{"name":"Vocabularium Energiehuis","resourceReference":"https://data.vlaanderen.be/doc/applicatieprofiel/energiehuis"},{"name":"Codelijst informatievoorziening thema's","resourceReference":"https://data.vlaanderen.be/id/conceptscheme/InformatievoorzieningThema"},{"name":"Codelijst adviesverlening types","resourceReference":"https://data.vlaanderen.be/id/conceptscheme/AdviesverleningType"},{"name":"Codelijst begeleiding types","resourceReference":"https://data.vlaanderen.be/id/conceptscheme/BegeleidingType"}]</t>
   </si>
   <si>
-    <t>{"name":"Charter OSLO Energiehuis","resourceReference":"https://data.vlaanderen.be/doc/applicatieprofiel/energiehuis"}</t>
+    <t>{"name":"Charter OSLO Energiehuis","resourceReference":"https://github.com/Informatievlaanderen/OSLOthema-energiehuis/blob/standaardenregister/Charter%20OSLO_Energiehuis.pdf"}</t>
   </si>
   <si>
     <t>[{"name":"Verslag business werkgroep - 11-09-2024","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-energiehuis/standaardenregister/reports/Verslag%20-%20Business%20Werkgroep%20-%20Energiehuis%20-%2020240911.pdf"},{"name":"Verslag thematische werkgroep 1 - 16-10-2024","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-energiehuis/standaardenregister/reports/Verslag%20-%20Thematische%20Werkgroep%201%20-%20Energiehuis%20-%2020241016.pdf"},{"name":"Verslag thematische werkgroep 2 - 14-11-2024","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-energiehuis/standaardenregister/reports/Verslag%20-%20Thematische%20Werkgroep%202%20-%20Energiehuis%20-%2020241114.pdf"},{"name":"Verslag thematische werkgroep 3 - 09-12-2024","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-energiehuis/standaardenregister/reports/Verslag%20-%20Thematische%20Werkgroep%203%20-%20Energiehuis%20-%2020241209.pdf"},{"name":"Verslag thematische werkgroep 4 - 16-01-2025","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-energiehuis/standaardenregister/reports/Verslag%20-%20Thematische%20Werkgroep%204%20-%20Energiehuis%20-%2020250116.pdf"}]</t>
@@ -203,7 +203,7 @@
     <t>Charter OSLO Energiehuis</t>
   </si>
   <si>
-    <t>https://data.vlaanderen.be/doc/applicatieprofiel/energiehuis</t>
+    <t>https://github.com/Informatievlaanderen/OSLOthema-energiehuis/blob/standaardenregister/Charter%20OSLO_Energiehuis.pdf</t>
   </si>
   <si>
     <t>Vocabularium Energiehuis</t>
@@ -3821,19 +3821,19 @@
     <t>[{"name":"Vocabularium Rooilijnplannen","resourceReference":"https://data.vlaanderen.be/ns/rooilijnplannen/"}]</t>
   </si>
   <si>
-    <t>{"name":"Charter Rooilijnplannen","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-rooilijnplannen/blob/standaardenregister/charter/Werkgroep%20charter%20OSLO_Rooilijnplannen1%20(3).pdf"}</t>
-  </si>
-  <si>
-    <t>[{"name":"Verslag Business Werkgroep - 12 december 2024","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-rooilijnplannen/blob/standaardenregister/reports/Verslag%20Business%20werkgroep%20OSLO%20Rooilijnplannen.pdf"},{"name":"Verslag Thematische Werkgroep 1 - 23 januari 2025","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-rooilijnplannen/blob/standaardenregister/reports/Verslag%20Thematische%20werkgroep%201%20Rooilijnen.pdf"},{"name":"Verslag Thematische Werkgroep 2 - 20 februari 2025","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-rooilijnplannen/blob/standaardenregister/reports/Verslag%20TW2%20OSLO%20Rooilijnen.pdf"},{"name":"Verslag Thematische Werkgroep 3 - 3 april 2025","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-rooilijnplannen/blob/standaardenregister/reports/Verslag%20TW3%20OSLO%20Rooilijnen.pdf"}]</t>
-  </si>
-  <si>
-    <t>[{"name":"Presentatie Business Werkgroep -  12 december 2024","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-rooilijnplannen/blob/standaardenregister/presentations/Business%20Werkgroep%20presentatie%20Rooilijnplannen.pdf"},{"name":"Presentatie Thematische Werkgroep 1 - 23 januari 2025","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-rooilijnplannen/blob/standaardenregister/presentations/Presentatie%20thematische%20werkgroep%201%20-%20Rooilijnen.pdf"},{"name":"Presentatie Thematische Werkgroep 2 - 20 februari 2025","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-rooilijnplannen/blob/standaardenregister/presentations/Presentatie%20thematische%20werkgroep%202%20-%20Rooilijnen.pdf"},{"name":"Presentatie Thematische Werkgroep 3 - 3 april 2025","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-rooilijnplannen/blob/standaardenregister/presentations/Presentatie%20thematische%20werkgroep%203%20-%20Rooilijnen.pdf"}]</t>
+    <t>{"name":"Charter Rooilijnplannen","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-rooilijnplannen/standaardenregister/charter/Werkgroep%20charter%20OSLO_Rooilijnplannen1%20(3).pdf"}</t>
+  </si>
+  <si>
+    <t>[{"name":"Verslag Business Werkgroep - 12 december 2024","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-rooilijnplannen/standaardenregister/reports/Verslag%20Business%20werkgroep%20OSLO%20Rooilijnplannen.pdf"},{"name":"Verslag Thematische Werkgroep 1 - 23 januari 2025","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-rooilijnplannen/standaardenregister/reports/Verslag%20Thematische%20werkgroep%201%20Rooilijnen.pdf"},{"name":"Verslag Thematische Werkgroep 2 - 20 februari 2025","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-rooilijnplannen/standaardenregister/reports/Verslag%20TW2%20OSLO%20Rooilijnen.pdf"},{"name":"Verslag Thematische Werkgroep 3 - 3 april 2025","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-rooilijnplannen/standaardenregister/reports/Verslag%20TW3%20OSLO%20Rooilijnen.pdf"}]</t>
+  </si>
+  <si>
+    <t>[{"name":"Presentatie Business Werkgroep -  12 december 2024","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-rooilijnplannen/standaardenregister/presentations/Business%20Werkgroep%20presentatie%20Rooilijnplannen.pdf"},{"name":"Presentatie Thematische Werkgroep 1 - 23 januari 2025","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-rooilijnplannen/standaardenregister/presentations/Presentatie%20thematische%20werkgroep%201%20-%20Rooilijnen.pdf"},{"name":"Presentatie Thematische Werkgroep 2 - 20 februari 2025","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-rooilijnplannen/standaardenregister/presentations/Presentatie%20thematische%20werkgroep%202%20-%20Rooilijnen.pdf"},{"name":"Presentatie Thematische Werkgroep 3 - 3 april 2025","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-rooilijnplannen/standaardenregister/presentations/Presentatie%20thematische%20werkgroep%203%20-%20Rooilijnen.pdf"}]</t>
   </si>
   <si>
     <t>Charter Rooilijnplannen</t>
   </si>
   <si>
-    <t>https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-rooilijnplannen/blob/standaardenregister/charter/Werkgroep%20charter%20OSLO_Rooilijnplannen1%20(3).pdf</t>
+    <t>https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-rooilijnplannen/standaardenregister/charter/Werkgroep%20charter%20OSLO_Rooilijnplannen1%20(3).pdf</t>
   </si>
   <si>
     <t>Vocabularium Rooilijnplannen</t>
@@ -20507,7 +20507,7 @@
         <v>26</v>
       </c>
       <c r="F254" s="4">
-        <v>45813</v>
+        <v>45809</v>
       </c>
       <c r="G254" s="3" t="s">
         <v>1266</v>
@@ -20575,7 +20575,7 @@
         <v>26</v>
       </c>
       <c r="F255" s="4">
-        <v>45813</v>
+        <v>45809</v>
       </c>
       <c r="G255" s="3" t="s">
         <v>1266</v>

</xml_diff>

<commit_message>
generated all the reports on 2025-07-13
</commit_message>
<xml_diff>
--- a/report/merged_configurations.xlsx
+++ b/report/merged_configurations.xlsx
@@ -107,10 +107,10 @@
     <t>{}</t>
   </si>
   <si>
-    <t>[{"name":"Verslag Business Werkgroep - 24 februari 2025","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-EnergieManagementSystem/standaardenregister/reports/Verslag Business werkgroep EMS.pdf"},{"name":"Verslag Thematische Werkgroep I - 24 maart 2025","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-EnergieManagementSystem/standaardenregister/reports/Verslag Thematische werkgroep 1 EMS.pdf"},{"name":"Verslag Thematische Werkgroep II - 28 april 2025","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-EnergieManagementSystem/standaardenregister/reports/Thematische werkgroep 2 - EMS.pdf"}]</t>
-  </si>
-  <si>
-    <t>[{"name":"Presentatie Business Werkgroep - 24 februari 2025","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-EnergieManagementSystem/standaardenregister/presentations/Business Werkgroep presentatie EMS.pdf"},{"name":"Presentatie Thematische Werkgroep I - 24 maart 2025","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-EnergieManagementSystem/standaardenregister/presentations/Thematische werkgroep 1 presentatie EMS.pdf"},{"name":"Presentatie Thematische Werkgroep II - 28 april 2025","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-EnergieManagementSystem/standaardenregister/presentations/Thematische werkgroep 2 presentatie EMS.pdf"}]</t>
+    <t>[{"name":"Verslag Business Werkgroep - 24 februari 2025","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-EnergieManagementSystem/standaardenregister/reports/Verslag Business werkgroep EMS.pdf"},{"name":"Verslag Thematische Werkgroep I - 24 maart 2025","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-EnergieManagementSystem/standaardenregister/reports/Verslag Thematische werkgroep 1 EMS.pdf"},{"name":"Verslag Thematische Werkgroep II - 28 april 2025","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-EnergieManagementSystem/standaardenregister/reports/Thematische werkgroep 2 - EMS.pdf"},{"name":"Verslag Thematische Werkgroep III - 23 juni 2025","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-EnergieManagementSystem/standaardenregister/reports/Verslag thematische werkgroep 3 - EMS.pdf"}]</t>
+  </si>
+  <si>
+    <t>[{"name":"Presentatie Business Werkgroep - 24 februari 2025","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-EnergieManagementSystem/standaardenregister/presentations/Business Werkgroep presentatie EMS.pdf"},{"name":"Presentatie Thematische Werkgroep I - 24 maart 2025","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-EnergieManagementSystem/standaardenregister/presentations/Thematische werkgroep 1 presentatie EMS.pdf"},{"name":"Presentatie Thematische Werkgroep II - 28 april 2025","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-EnergieManagementSystem/standaardenregister/presentations/Thematische werkgroep 2 presentatie EMS.pdf"},{"name":"Presentatie Thematische Werkgroep III - 23 juni 2025","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-EnergieManagementSystem/standaardenregister/presentations/Thematische werkgroep 3 presentatie EMS.pdf"}]</t>
   </si>
   <si>
     <t>undefined</t>
@@ -3728,7 +3728,7 @@
     <t>{"name":"Charter Zaalreservatie","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-zaalreservatie/standaardenregister/charter/Charter%20Zaalreservatie.pdf"}</t>
   </si>
   <si>
-    <t>[{"name":"Verslag Business Werkgroep - 14 januari 2025","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-zaalreservatie/standaardenregister/reports/Verslag%20BW%20OSLO%20Zaalreservatie.pdf"},{"name":"Verslag Thematische Werkgroep 1 - 18 februari 2025","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-zaalreservatie/standaardenregister/reports/Verslag%20TW1%20OSLO%20Zaalreservatie.pdf"},{"name":"Verslag Thematische Werkgroep 2 - 18 maart 2025","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-zaalreservatie/standaardenregister/reports/Verslag%20TW2%20OSLO%20Zaalreservatie.pdf"},{"name":"Verslag Thematische Werkgroep 3 - 22 april 2025","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-zaalreservatie/standaardenregister/reports/Verslag%20TW3%20OSLO%20Zaalreservatie.pdf"}]</t>
+    <t>[{"name":"Verslag Business Werkgroep - 14 januari 2025","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-zaalreservatie/standaardenregister/reports/Verslag%20BW%20OSLO%20Zaalreservatie.pdf"},{"name":"Verslag Thematische Werkgroep 1 - 18 februari 2025","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-zaalreservatie/standaardenregister/reports/Verslag%20TW1%20OSLO%20Zaalreservatie.pdf"},{"name":"Verslag Thematische Werkgroep 2 - 18 maart 2025","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-zaalreservatie/standaardenregister/reports/Verslag%20TW2%20OSLO%20Zaalreservatie.pdf"},{"name":"Verslag Thematische Werkgroep 3 - 22 april 2025","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-zaalreservatie/standaardenregister/reports/Verslag%20TW3%20OSLO%20Zaalreservatie.pdf"},{"name":"Verslag Thematische Werkgroep 4 - 20 mei 2025","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-zaalreservatie/standaardenregister/reports/Verslag%20TW4%20OSLO%20Zaalreservatie.pdf"}]</t>
   </si>
   <si>
     <t>[{"name":"Presentatie Business Werkgroep -  14 januari 2025","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-zaalreservatie/standaardenregister/presentations/Business%20Werkgroep%20Zaalreservatie.pdf"},{"name":"Presentatie Thematische Werkgroep 1 - 18 februari 2025","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-zaalreservatie/standaardenregister/presentations/Thematische%20werkgroep%201%20OSLO%20Zaalreservatie.pdf"},{"name":"Presentatie Thematische Werkgroep 2 - 18 maart 2025","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-zaalreservatie/standaardenregister/presentations/Thematische%20werkgroep%202%20OSLO%20Zaalreservatie.pdf"},{"name":"Presentatie Thematische Werkgroep 3 - 22 april 2025","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-zaalreservatie/standaardenregister/presentations/Thematische%20werkgroep%203%20OSLO%20Zaalreservatie.pdf"},{"name":"Presentatie Thematische Werkgroep 4 - 20 mei 2025","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-zaalreservatie/standaardenregister/presentations/Thematische%20werkgroep%204%20OSLO%20Zaalreservatie.pdf"}]</t>
@@ -3812,10 +3812,10 @@
     <t>{"name":"Charter Rooilijnplannen","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-rooilijnplannen/standaardenregister/charter/Werkgroep%20charter%20OSLO_Rooilijnplannen1%20(3).pdf"}</t>
   </si>
   <si>
-    <t>[{"name":"Verslag Business Werkgroep - 12 december 2024","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-rooilijnplannen/standaardenregister/reports/Verslag%20Business%20werkgroep%20OSLO%20Rooilijnplannen.pdf"},{"name":"Verslag Thematische Werkgroep 1 - 23 januari 2025","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-rooilijnplannen/standaardenregister/reports/Verslag%20Thematische%20werkgroep%201%20Rooilijnen.pdf"},{"name":"Verslag Thematische Werkgroep 2 - 20 februari 2025","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-rooilijnplannen/standaardenregister/reports/Verslag%20TW2%20OSLO%20Rooilijnen.pdf"},{"name":"Verslag Thematische Werkgroep 3 - 3 april 2025","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-rooilijnplannen/standaardenregister/reports/Verslag%20TW3%20OSLO%20Rooilijnen.pdf"}]</t>
-  </si>
-  <si>
-    <t>[{"name":"Presentatie Business Werkgroep -  12 december 2024","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-rooilijnplannen/standaardenregister/presentations/Business%20Werkgroep%20presentatie%20Rooilijnplannen.pdf"},{"name":"Presentatie Thematische Werkgroep 1 - 23 januari 2025","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-rooilijnplannen/standaardenregister/presentations/Presentatie%20thematische%20werkgroep%201%20-%20Rooilijnen.pdf"},{"name":"Presentatie Thematische Werkgroep 2 - 20 februari 2025","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-rooilijnplannen/standaardenregister/presentations/Presentatie%20thematische%20werkgroep%202%20-%20Rooilijnen.pdf"},{"name":"Presentatie Thematische Werkgroep 3 - 3 april 2025","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-rooilijnplannen/standaardenregister/presentations/Presentatie%20thematische%20werkgroep%203%20-%20Rooilijnen.pdf"}]</t>
+    <t>[{"name":"Verslag Business Werkgroep - 12 december 2024","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-rooilijnplannen/standaardenregister/reports/Verslag%20Business%20werkgroep%20OSLO%20Rooilijnplannen.pdf"},{"name":"Verslag Thematische Werkgroep 1 - 23 januari 2025","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-rooilijnplannen/standaardenregister/reports/Verslag%20Thematische%20werkgroep%201%20Rooilijnen.pdf"},{"name":"Verslag Thematische Werkgroep 2 - 20 februari 2025","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-rooilijnplannen/standaardenregister/reports/Verslag%20TW2%20OSLO%20Rooilijnen.pdf"},{"name":"Verslag Thematische Werkgroep 3 - 3 april 2025","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-rooilijnplannen/standaardenregister/reports/Verslag%20TW3%20OSLO%20Rooilijnen.pdf"},{"name":"Verslag Thematische Werkgroep 4 - 18 juni 2025","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-rooilijnplannen/standaardenregister/reports/Verslag%20TW4%20OSLO%20Rooilijnen.pdf"}]</t>
+  </si>
+  <si>
+    <t>[{"name":"Presentatie Business Werkgroep -  12 december 2024","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-rooilijnplannen/standaardenregister/presentations/Business%20Werkgroep%20presentatie%20Rooilijnplannen.pdf"},{"name":"Presentatie Thematische Werkgroep 1 - 23 januari 2025","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-rooilijnplannen/standaardenregister/presentations/Presentatie%20thematische%20werkgroep%201%20-%20Rooilijnen.pdf"},{"name":"Presentatie Thematische Werkgroep 2 - 20 februari 2025","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-rooilijnplannen/standaardenregister/presentations/Presentatie%20thematische%20werkgroep%202%20-%20Rooilijnen.pdf"},{"name":"Presentatie Thematische Werkgroep 3 - 3 april 2025","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-rooilijnplannen/standaardenregister/presentations/Presentatie%20thematische%20werkgroep%203%20-%20Rooilijnen.pdf"},{"name":"Presentatie Thematische Werkgroep 4 - 18 juni 2025","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-rooilijnplannen/standaardenregister/presentations/Presentatie%20thematische%20werkgroep%204%20-%20Rooilijnen.pdf"}]</t>
   </si>
   <si>
     <t>Charter Rooilijnplannen</t>

</xml_diff>

<commit_message>
generated all the reports on 2025-07-20
</commit_message>
<xml_diff>
--- a/report/merged_configurations.xlsx
+++ b/report/merged_configurations.xlsx
@@ -128,10 +128,10 @@
     <t>[{"name":"Applicatieprofiel Thermografische Gebouwanalyse","resourceReference":"https://data.vlaanderen.be/doc/applicatieprofiel/thermografische-gebouwanalyse"}]</t>
   </si>
   <si>
-    <t>[{"name":"Vocabularium Thermografische Gebouwanalyse","resourceReference":"https://data.vlaanderen.be/ns/thermografische-gebouwanalyse"}]</t>
-  </si>
-  <si>
-    <t>[{"name":"Charter Thermografische Gebouwanalyse","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-thermAI/standaardenregister/charter/Charter_OSLO_thermAI.pdf"}]</t>
+    <t>[{"name":"Modelleerrapport","resourceReference":"https://github.com/Informatievlaanderen/OSLOthema-thermAI/blob/main/resources/ModelleerrapportThermAI.pdf"},{"name":"Datavoorbeelden","resourceReference":"https://github.com/Informatievlaanderen/OSLOthema-thermAI/tree/main/resources/Datavoorbeelden"}]</t>
+  </si>
+  <si>
+    <t>{"name":"Charter Thermografische Gebouwanalyse","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-thermAI/standaardenregister/charter/Charter_OSLO_thermAI.pdf"}</t>
   </si>
   <si>
     <t>[{"name":"Verslag Business werkgroep - 18-02-2025","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-thermAI/standaardenregister/reports/Business%20werkgroep%20CoT%20ThermAI%202025-02-18.pdf"},{"name":"Verslag Thematische Werkgroep 1 - 18-03-2025","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-thermAI/standaardenregister/reports/Thematische%20werkgroep%201%20-%20CoT%20ThermAI%202025-03-18.pdf"},{"name":"Verslag Thematische Werkgroep 2 - 15-04-2025","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-thermAI/standaardenregister/reports/Thematische%20werkgroep%202%20-%20CoT%20ThermAI%202025-04-15.pdf"},{"name":"Verslag Thematische Werkgroep 3 - 15-05-2025","resourceReference":"https://github.com/Informatievlaanderen/OSLOthema-thermAI/blob/standaardenregister/reports/Verslag%20Thematische%20werkgroep%203%20-%20CoT%20ThermAI%202025-04-15.docx.pdf"}]</t>
@@ -143,10 +143,10 @@
     <t>2024-12-1</t>
   </si>
   <si>
-    <t>["Charter Thermografische Gebouwanalyse"]</t>
-  </si>
-  <si>
-    <t>["https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-thermAI/standaardenregister/charter/Charter_OSLO_thermAI.pdf"]</t>
+    <t>Charter Thermografische Gebouwanalyse</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-thermAI/standaardenregister/charter/Charter_OSLO_thermAI.pdf</t>
   </si>
   <si>
     <t>Applicatieprofiel Leermiddelen</t>
@@ -3785,10 +3785,10 @@
     <t>[{"name":"Charter Verkeersmeldingen","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-SmartInnovationFactory/standaardenregister/charter/Charter_OSLO_SIF.pdf"}]</t>
   </si>
   <si>
-    <t>[{"name":"Verslag Business Werkgroep - 25 maart 2025","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-SmartInnovationFactory/standaardenregister/reports/Verslag%20BW%20OSLO%20SIF.pdf"},{"name":"Verslag Thematische Werkgroep 1 - 29 april 2025","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-SmartInnovationFactory/standaardenregister/reports/Verslag%20TW1%20OSLO%20SIF.pdf"}]</t>
-  </si>
-  <si>
-    <t>[{"name":"Presentatie Business Werkgroep -  25 maart 2025","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-SmartInnovationFactory/standaardenregister/presentations/BW%20Presentatie%20SIF.pdf"},{"name":"Presentatie Thematische Werkgroep 1 - 29 april 2025","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-SmartInnovationFactory/standaardenregister/presentations/20250429_OSLOSIF_PresentatieThematischeWerkgroep1.pdf"}]</t>
+    <t>[{"name":"Verslag Business Werkgroep - 25 maart 2025","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-SmartInnovationFactory/standaardenregister/reports/Verslag%20BW%20OSLO%20SIF.pdf"},{"name":"Verslag Thematische Werkgroep 1 - 29 april 2025","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-SmartInnovationFactory/standaardenregister/reports/Verslag%20TW1%20OSLO%20SIF.pdf"},{"name":"Verslag Thematische Werkgroep 2 - 10 juni 2025","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-SmartInnovationFactory/standaardenregister/reports/20250610_OSLOSIF_VerslagThematischeWerkgroep2.pdf"}]</t>
+  </si>
+  <si>
+    <t>[{"name":"Presentatie Business Werkgroep -  25 maart 2025","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-SmartInnovationFactory/standaardenregister/presentations/BW%20Presentatie%20SIF.pdf"},{"name":"Presentatie Thematische Werkgroep 1 - 29 april 2025","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-SmartInnovationFactory/standaardenregister/presentations/20250429_OSLOSIF_PresentatieThematischeWerkgroep1.pdf"},{"name":"Presentatie Thematische Werkgroep 2 - 10 juni 2025","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-SmartInnovationFactory/standaardenregister/presentations/20250610_OSLOSIF_PresentatieThematischeWerkgroep2.pdf"},{"name":"Presentatie Thematische Werkgroep 3 - 24 juni 2025","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-SmartInnovationFactory/standaardenregister/presentations/20250624_OSLOSIF_PresentatieThematischeWerkgroep3.pdf"}]</t>
   </si>
   <si>
     <t>["Charter Verkeersmeldingen"]</t>
@@ -4407,7 +4407,7 @@
       <c r="N3" s="3"/>
       <c r="O3" s="3"/>
       <c r="P3" s="4">
-        <v>45799</v>
+        <v>45854</v>
       </c>
       <c r="Q3" s="4">
         <v>45911</v>
@@ -4681,13 +4681,13 @@
         <v>24</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>35</v>
+        <v>56</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>71</v>
       </c>
       <c r="F8" s="4">
-        <v>45625</v>
+        <v>45856</v>
       </c>
       <c r="G8" s="3" t="s">
         <v>72</v>
@@ -4747,13 +4747,13 @@
         <v>24</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>35</v>
+        <v>56</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>71</v>
       </c>
       <c r="F9" s="4">
-        <v>45625</v>
+        <v>45856</v>
       </c>
       <c r="G9" s="3" t="s">
         <v>72</v>

</xml_diff>

<commit_message>
generated all the reports on 2025-08-10
</commit_message>
<xml_diff>
--- a/report/merged_configurations.xlsx
+++ b/report/merged_configurations.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4746" uniqueCount="1280">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4746" uniqueCount="1278">
   <si>
     <t>title</t>
   </si>
@@ -2957,9 +2957,6 @@
     <t>Applicatieprofiel DCAT-AP VL 2.0</t>
   </si>
   <si>
-    <t>[{"name":"Digitaal Vlaanderen","resourceReference":"https://data.vlaanderen.be/id/organisatie/OVO002949"}]</t>
-  </si>
-  <si>
     <t>[{"name":"DCAT-AP 1.2","resourceReference":"https://joinup.ec.europa.eu/release/dcat-ap/12"},{"name":"DCAT-AP 2.0","resourceReference":"https://github.com/SEMICeu/DCAT-AP/tree/2.0.1/releases/2.0.1"},{"name":"Applicatieprofiel metadata DCAT","resourceReference":"https://data.vlaanderen.be/doc/applicatieprofiel/metadata-dcat"},{"name":"W3C DCAT","resourceReference":"https://www.w3.org/TR/vocab-dcat/"},{"name":"W3C Review DCAT","resourceReference":"https://w3c.github.io/dxwg/dcat/"}]</t>
   </si>
   <si>
@@ -3777,9 +3774,6 @@
   </si>
   <si>
     <t>[{"name":"Applicatieprofiel Openbare Nutsvoorzieningkasten","resourceReference":"https://data.vlaanderen.be/doc/applicatieprofiel/openbare-nutsvoorzieningkasten/"}]</t>
-  </si>
-  <si>
-    <t>[{"name":"Vocabularium Openbare Nutsvoorzieningkasten","resourceReference":"https://data.vlaanderen.be/ns/openbare-nutsvoorzieningkasten/"}]</t>
   </si>
   <si>
     <t>[{"name":"Verslag Business werkgroep OSLO SHOK","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-SHOK/standaardenregister/reports/Verslag Business werkgroep OSLO SHOK.pdf"},{"name":"Verslag Thematische Werkgroep 1 OSLO SHOK","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-SHOK/standaardenregister/reports/Verslag Thematische Werkgroep 1 - OSLO SHOK.pdf"},{"name":"Verslag Thematische werkgroep 2 OSLO SHOK","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-SHOK/standaardenregister/reports/OSLO SHOK - Verslag Thematische werkgroep 2.pdf"},{"name":"Verslag Thematische werkgroep 3 OSLO SHOK","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-SHOK/standaardenregister/reports/Verslag Thematische Werkgroep 3 - OSLO SHOK.pdf"}]</t>
@@ -4875,7 +4869,7 @@
         <v>39</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>40</v>
+        <v>64</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>80</v>
@@ -4884,7 +4878,7 @@
         <v>42</v>
       </c>
       <c r="G10" s="4">
-        <v>45572</v>
+        <v>45861</v>
       </c>
       <c r="H10" s="3" t="s">
         <v>94</v>
@@ -4903,9 +4897,15 @@
       </c>
       <c r="M10" s="3"/>
       <c r="N10" s="3"/>
-      <c r="O10" s="3"/>
-      <c r="P10" s="3"/>
-      <c r="Q10" s="3"/>
+      <c r="O10" s="4">
+        <v>45828</v>
+      </c>
+      <c r="P10" s="4">
+        <v>45666</v>
+      </c>
+      <c r="Q10" s="4">
+        <v>45756</v>
+      </c>
       <c r="R10" s="3"/>
       <c r="S10" s="3" t="s">
         <v>36</v>
@@ -4934,7 +4934,7 @@
         <v>39</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>40</v>
+        <v>64</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>80</v>
@@ -4943,7 +4943,7 @@
         <v>42</v>
       </c>
       <c r="G11" s="4">
-        <v>45572</v>
+        <v>45861</v>
       </c>
       <c r="H11" s="3" t="s">
         <v>95</v>
@@ -4962,9 +4962,15 @@
       </c>
       <c r="M11" s="3"/>
       <c r="N11" s="3"/>
-      <c r="O11" s="3"/>
-      <c r="P11" s="3"/>
-      <c r="Q11" s="3"/>
+      <c r="O11" s="4">
+        <v>45828</v>
+      </c>
+      <c r="P11" s="4">
+        <v>45666</v>
+      </c>
+      <c r="Q11" s="4">
+        <v>45756</v>
+      </c>
       <c r="R11" s="3"/>
       <c r="S11" s="3" t="s">
         <v>36</v>
@@ -17893,7 +17899,7 @@
         <v>548</v>
       </c>
       <c r="F204" s="3" t="s">
-        <v>981</v>
+        <v>42</v>
       </c>
       <c r="G204" s="4">
         <v>44532</v>
@@ -17902,16 +17908,16 @@
         <v>549</v>
       </c>
       <c r="I204" s="3" t="s">
+        <v>981</v>
+      </c>
+      <c r="J204" s="3" t="s">
         <v>982</v>
       </c>
-      <c r="J204" s="3" t="s">
+      <c r="K204" s="3" t="s">
         <v>983</v>
       </c>
-      <c r="K204" s="3" t="s">
+      <c r="L204" s="3" t="s">
         <v>984</v>
-      </c>
-      <c r="L204" s="3" t="s">
-        <v>985</v>
       </c>
       <c r="M204" s="4">
         <v>44351</v>
@@ -17934,7 +17940,7 @@
         <v>554</v>
       </c>
       <c r="U204" s="3" t="s">
-        <v>986</v>
+        <v>985</v>
       </c>
       <c r="V204" s="3" t="s">
         <v>556</v>
@@ -17945,7 +17951,7 @@
     </row>
     <row r="205" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A205" s="3" t="s">
-        <v>987</v>
+        <v>986</v>
       </c>
       <c r="B205" s="3" t="s">
         <v>38</v>
@@ -17957,7 +17963,7 @@
         <v>53</v>
       </c>
       <c r="E205" s="3" t="s">
-        <v>988</v>
+        <v>987</v>
       </c>
       <c r="F205" s="3" t="s">
         <v>42</v>
@@ -17966,22 +17972,22 @@
         <v>24</v>
       </c>
       <c r="H205" s="3" t="s">
-        <v>989</v>
+        <v>988</v>
       </c>
       <c r="I205" s="3" t="s">
         <v>28</v>
       </c>
       <c r="J205" s="3" t="s">
+        <v>989</v>
+      </c>
+      <c r="K205" s="3" t="s">
         <v>990</v>
       </c>
-      <c r="K205" s="3" t="s">
+      <c r="L205" s="3" t="s">
         <v>991</v>
       </c>
-      <c r="L205" s="3" t="s">
+      <c r="M205" s="3" t="s">
         <v>992</v>
-      </c>
-      <c r="M205" s="3" t="s">
-        <v>993</v>
       </c>
       <c r="N205" s="3" t="s">
         <v>24</v>
@@ -17998,21 +18004,21 @@
         <v>36</v>
       </c>
       <c r="T205" s="3" t="s">
+        <v>993</v>
+      </c>
+      <c r="U205" s="3" t="s">
         <v>994</v>
-      </c>
-      <c r="U205" s="3" t="s">
-        <v>995</v>
       </c>
       <c r="V205" s="3" t="s">
         <v>177</v>
       </c>
       <c r="W205" s="3" t="s">
-        <v>996</v>
+        <v>995</v>
       </c>
     </row>
     <row r="206" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A206" s="3" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
       <c r="B206" s="3" t="s">
         <v>38</v>
@@ -18024,28 +18030,28 @@
         <v>64</v>
       </c>
       <c r="E206" s="3" t="s">
-        <v>998</v>
+        <v>997</v>
       </c>
       <c r="F206" s="3" t="s">
-        <v>981</v>
+        <v>42</v>
       </c>
       <c r="G206" s="4">
         <v>44595</v>
       </c>
       <c r="H206" s="3" t="s">
+        <v>998</v>
+      </c>
+      <c r="I206" s="3" t="s">
         <v>999</v>
-      </c>
-      <c r="I206" s="3" t="s">
-        <v>1000</v>
       </c>
       <c r="J206" s="3" t="s">
         <v>28</v>
       </c>
       <c r="K206" s="3" t="s">
+        <v>1000</v>
+      </c>
+      <c r="L206" s="3" t="s">
         <v>1001</v>
-      </c>
-      <c r="L206" s="3" t="s">
-        <v>1002</v>
       </c>
       <c r="M206" s="4">
         <v>44455</v>
@@ -18065,21 +18071,21 @@
         <v>36</v>
       </c>
       <c r="T206" s="3" t="s">
+        <v>1002</v>
+      </c>
+      <c r="U206" s="3" t="s">
         <v>1003</v>
-      </c>
-      <c r="U206" s="3" t="s">
-        <v>1004</v>
       </c>
       <c r="V206" s="3" t="s">
         <v>556</v>
       </c>
       <c r="W206" s="3" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="207" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A207" s="3" t="s">
-        <v>1006</v>
+        <v>1005</v>
       </c>
       <c r="B207" s="3" t="s">
         <v>38</v>
@@ -18091,7 +18097,7 @@
         <v>64</v>
       </c>
       <c r="E207" s="3" t="s">
-        <v>1007</v>
+        <v>1006</v>
       </c>
       <c r="F207" s="3" t="s">
         <v>42</v>
@@ -18100,19 +18106,19 @@
         <v>44896</v>
       </c>
       <c r="H207" s="3" t="s">
+        <v>1007</v>
+      </c>
+      <c r="I207" s="3" t="s">
         <v>1008</v>
       </c>
-      <c r="I207" s="3" t="s">
+      <c r="J207" s="3" t="s">
         <v>1009</v>
       </c>
-      <c r="J207" s="3" t="s">
+      <c r="K207" s="3" t="s">
         <v>1010</v>
       </c>
-      <c r="K207" s="3" t="s">
+      <c r="L207" s="3" t="s">
         <v>1011</v>
-      </c>
-      <c r="L207" s="3" t="s">
-        <v>1012</v>
       </c>
       <c r="M207" s="4">
         <v>44453</v>
@@ -18135,18 +18141,18 @@
         <v>87</v>
       </c>
       <c r="U207" s="3" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="V207" s="3" t="s">
         <v>110</v>
       </c>
       <c r="W207" s="3" t="s">
-        <v>1014</v>
+        <v>1013</v>
       </c>
     </row>
     <row r="208" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A208" s="3" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
       <c r="B208" s="3" t="s">
         <v>61</v>
@@ -18158,7 +18164,7 @@
         <v>64</v>
       </c>
       <c r="E208" s="3" t="s">
-        <v>1007</v>
+        <v>1006</v>
       </c>
       <c r="F208" s="3" t="s">
         <v>42</v>
@@ -18167,19 +18173,19 @@
         <v>44896</v>
       </c>
       <c r="H208" s="3" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
       <c r="I208" s="3" t="s">
+        <v>1008</v>
+      </c>
+      <c r="J208" s="3" t="s">
         <v>1009</v>
       </c>
-      <c r="J208" s="3" t="s">
+      <c r="K208" s="3" t="s">
         <v>1010</v>
       </c>
-      <c r="K208" s="3" t="s">
+      <c r="L208" s="3" t="s">
         <v>1011</v>
-      </c>
-      <c r="L208" s="3" t="s">
-        <v>1012</v>
       </c>
       <c r="M208" s="4">
         <v>44453</v>
@@ -18202,18 +18208,18 @@
         <v>87</v>
       </c>
       <c r="U208" s="3" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="V208" s="3" t="s">
         <v>110</v>
       </c>
       <c r="W208" s="3" t="s">
-        <v>1014</v>
+        <v>1013</v>
       </c>
     </row>
     <row r="209" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A209" s="3" t="s">
-        <v>1017</v>
+        <v>1016</v>
       </c>
       <c r="B209" s="3" t="s">
         <v>38</v>
@@ -18225,7 +18231,7 @@
         <v>64</v>
       </c>
       <c r="E209" s="3" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
       <c r="F209" s="3" t="s">
         <v>42</v>
@@ -18234,19 +18240,19 @@
         <v>44896</v>
       </c>
       <c r="H209" s="3" t="s">
-        <v>1019</v>
+        <v>1018</v>
       </c>
       <c r="I209" s="3" t="s">
         <v>28</v>
       </c>
       <c r="J209" s="3" t="s">
+        <v>1019</v>
+      </c>
+      <c r="K209" s="3" t="s">
         <v>1020</v>
       </c>
-      <c r="K209" s="3" t="s">
+      <c r="L209" s="3" t="s">
         <v>1021</v>
-      </c>
-      <c r="L209" s="3" t="s">
-        <v>1022</v>
       </c>
       <c r="M209" s="4">
         <v>44518</v>
@@ -18269,18 +18275,18 @@
         <v>164</v>
       </c>
       <c r="U209" s="3" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="V209" s="3" t="s">
         <v>556</v>
       </c>
       <c r="W209" s="3" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
     </row>
     <row r="210" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A210" s="3" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
       <c r="B210" s="3" t="s">
         <v>61</v>
@@ -18292,7 +18298,7 @@
         <v>64</v>
       </c>
       <c r="E210" s="3" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
       <c r="F210" s="3" t="s">
         <v>42</v>
@@ -18301,19 +18307,19 @@
         <v>44896</v>
       </c>
       <c r="H210" s="3" t="s">
-        <v>1026</v>
+        <v>1025</v>
       </c>
       <c r="I210" s="3" t="s">
         <v>28</v>
       </c>
       <c r="J210" s="3" t="s">
+        <v>1019</v>
+      </c>
+      <c r="K210" s="3" t="s">
         <v>1020</v>
       </c>
-      <c r="K210" s="3" t="s">
+      <c r="L210" s="3" t="s">
         <v>1021</v>
-      </c>
-      <c r="L210" s="3" t="s">
-        <v>1022</v>
       </c>
       <c r="M210" s="4">
         <v>44518</v>
@@ -18336,18 +18342,18 @@
         <v>164</v>
       </c>
       <c r="U210" s="3" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="V210" s="3" t="s">
         <v>177</v>
       </c>
       <c r="W210" s="3" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
     </row>
     <row r="211" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A211" s="3" t="s">
-        <v>1027</v>
+        <v>1026</v>
       </c>
       <c r="B211" s="3" t="s">
         <v>38</v>
@@ -18359,7 +18365,7 @@
         <v>40</v>
       </c>
       <c r="E211" s="3" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
       <c r="F211" s="3" t="s">
         <v>305</v>
@@ -18368,19 +18374,19 @@
         <v>44641</v>
       </c>
       <c r="H211" s="3" t="s">
+        <v>1028</v>
+      </c>
+      <c r="I211" s="3" t="s">
         <v>1029</v>
       </c>
-      <c r="I211" s="3" t="s">
+      <c r="J211" s="3" t="s">
         <v>1030</v>
       </c>
-      <c r="J211" s="3" t="s">
+      <c r="K211" s="3" t="s">
         <v>1031</v>
       </c>
-      <c r="K211" s="3" t="s">
+      <c r="L211" s="3" t="s">
         <v>1032</v>
-      </c>
-      <c r="L211" s="3" t="s">
-        <v>1033</v>
       </c>
       <c r="M211" s="4">
         <v>44531</v>
@@ -18404,21 +18410,21 @@
         <v>36</v>
       </c>
       <c r="T211" s="3" t="s">
+        <v>1033</v>
+      </c>
+      <c r="U211" s="3" t="s">
         <v>1034</v>
-      </c>
-      <c r="U211" s="3" t="s">
-        <v>1035</v>
       </c>
       <c r="V211" s="3" t="s">
         <v>313</v>
       </c>
       <c r="W211" s="3" t="s">
-        <v>1036</v>
+        <v>1035</v>
       </c>
     </row>
     <row r="212" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A212" s="3" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
       <c r="B212" s="3" t="s">
         <v>61</v>
@@ -18430,7 +18436,7 @@
         <v>40</v>
       </c>
       <c r="E212" s="3" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="F212" s="3" t="s">
         <v>305</v>
@@ -18439,19 +18445,19 @@
         <v>44641</v>
       </c>
       <c r="H212" s="3" t="s">
+        <v>1029</v>
+      </c>
+      <c r="I212" s="3" t="s">
+        <v>1028</v>
+      </c>
+      <c r="J212" s="3" t="s">
         <v>1030</v>
       </c>
-      <c r="I212" s="3" t="s">
-        <v>1029</v>
-      </c>
-      <c r="J212" s="3" t="s">
+      <c r="K212" s="3" t="s">
         <v>1031</v>
       </c>
-      <c r="K212" s="3" t="s">
+      <c r="L212" s="3" t="s">
         <v>1032</v>
-      </c>
-      <c r="L212" s="3" t="s">
-        <v>1033</v>
       </c>
       <c r="M212" s="4">
         <v>44531</v>
@@ -18475,21 +18481,21 @@
         <v>36</v>
       </c>
       <c r="T212" s="3" t="s">
+        <v>1033</v>
+      </c>
+      <c r="U212" s="3" t="s">
         <v>1034</v>
-      </c>
-      <c r="U212" s="3" t="s">
-        <v>1035</v>
       </c>
       <c r="V212" s="3" t="s">
         <v>313</v>
       </c>
       <c r="W212" s="3" t="s">
-        <v>1036</v>
+        <v>1035</v>
       </c>
     </row>
     <row r="213" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A213" s="3" t="s">
-        <v>1039</v>
+        <v>1038</v>
       </c>
       <c r="B213" s="3" t="s">
         <v>38</v>
@@ -18501,7 +18507,7 @@
         <v>40</v>
       </c>
       <c r="E213" s="3" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
       <c r="F213" s="3" t="s">
         <v>149</v>
@@ -18510,19 +18516,19 @@
         <v>44735</v>
       </c>
       <c r="H213" s="3" t="s">
+        <v>1040</v>
+      </c>
+      <c r="I213" s="3" t="s">
         <v>1041</v>
       </c>
-      <c r="I213" s="3" t="s">
+      <c r="J213" s="3" t="s">
         <v>1042</v>
       </c>
-      <c r="J213" s="3" t="s">
+      <c r="K213" s="3" t="s">
         <v>1043</v>
       </c>
-      <c r="K213" s="3" t="s">
+      <c r="L213" s="3" t="s">
         <v>1044</v>
-      </c>
-      <c r="L213" s="3" t="s">
-        <v>1045</v>
       </c>
       <c r="M213" s="4">
         <v>44013</v>
@@ -18542,21 +18548,21 @@
         <v>36</v>
       </c>
       <c r="T213" s="3" t="s">
+        <v>1045</v>
+      </c>
+      <c r="U213" s="3" t="s">
         <v>1046</v>
-      </c>
-      <c r="U213" s="3" t="s">
-        <v>1047</v>
       </c>
       <c r="V213" s="3" t="s">
         <v>417</v>
       </c>
       <c r="W213" s="3" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
     </row>
     <row r="214" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A214" s="3" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
       <c r="B214" s="3" t="s">
         <v>61</v>
@@ -18568,7 +18574,7 @@
         <v>40</v>
       </c>
       <c r="E214" s="3" t="s">
-        <v>1050</v>
+        <v>1049</v>
       </c>
       <c r="F214" s="3" t="s">
         <v>149</v>
@@ -18577,19 +18583,19 @@
         <v>44735</v>
       </c>
       <c r="H214" s="3" t="s">
+        <v>1050</v>
+      </c>
+      <c r="I214" s="3" t="s">
         <v>1051</v>
       </c>
-      <c r="I214" s="3" t="s">
-        <v>1052</v>
-      </c>
       <c r="J214" s="3" t="s">
+        <v>1042</v>
+      </c>
+      <c r="K214" s="3" t="s">
         <v>1043</v>
       </c>
-      <c r="K214" s="3" t="s">
+      <c r="L214" s="3" t="s">
         <v>1044</v>
-      </c>
-      <c r="L214" s="3" t="s">
-        <v>1045</v>
       </c>
       <c r="M214" s="4">
         <v>44013</v>
@@ -18609,21 +18615,21 @@
         <v>36</v>
       </c>
       <c r="T214" s="3" t="s">
+        <v>1045</v>
+      </c>
+      <c r="U214" s="3" t="s">
         <v>1046</v>
-      </c>
-      <c r="U214" s="3" t="s">
-        <v>1047</v>
       </c>
       <c r="V214" s="3" t="s">
         <v>417</v>
       </c>
       <c r="W214" s="3" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
     </row>
     <row r="215" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A215" s="3" t="s">
-        <v>1053</v>
+        <v>1052</v>
       </c>
       <c r="B215" s="3" t="s">
         <v>38</v>
@@ -18635,7 +18641,7 @@
         <v>64</v>
       </c>
       <c r="E215" s="3" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
       <c r="F215" s="3" t="s">
         <v>42</v>
@@ -18644,19 +18650,19 @@
         <v>44896</v>
       </c>
       <c r="H215" s="3" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
       <c r="I215" s="3" t="s">
         <v>28</v>
       </c>
       <c r="J215" s="3" t="s">
+        <v>1055</v>
+      </c>
+      <c r="K215" s="3" t="s">
         <v>1056</v>
       </c>
-      <c r="K215" s="3" t="s">
+      <c r="L215" s="3" t="s">
         <v>1057</v>
-      </c>
-      <c r="L215" s="3" t="s">
-        <v>1058</v>
       </c>
       <c r="M215" s="3"/>
       <c r="N215" s="3" t="s">
@@ -18677,18 +18683,18 @@
         <v>87</v>
       </c>
       <c r="U215" s="3" t="s">
-        <v>1059</v>
+        <v>1058</v>
       </c>
       <c r="V215" s="3" t="s">
         <v>110</v>
       </c>
       <c r="W215" s="3" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
     </row>
     <row r="216" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A216" s="3" t="s">
-        <v>1061</v>
+        <v>1060</v>
       </c>
       <c r="B216" s="3" t="s">
         <v>61</v>
@@ -18700,7 +18706,7 @@
         <v>64</v>
       </c>
       <c r="E216" s="3" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
       <c r="F216" s="3" t="s">
         <v>42</v>
@@ -18709,19 +18715,19 @@
         <v>44896</v>
       </c>
       <c r="H216" s="3" t="s">
-        <v>1063</v>
+        <v>1062</v>
       </c>
       <c r="I216" s="3" t="s">
         <v>28</v>
       </c>
       <c r="J216" s="3" t="s">
-        <v>1064</v>
+        <v>1063</v>
       </c>
       <c r="K216" s="3" t="s">
+        <v>1056</v>
+      </c>
+      <c r="L216" s="3" t="s">
         <v>1057</v>
-      </c>
-      <c r="L216" s="3" t="s">
-        <v>1058</v>
       </c>
       <c r="M216" s="3"/>
       <c r="N216" s="3" t="s">
@@ -18742,18 +18748,18 @@
         <v>87</v>
       </c>
       <c r="U216" s="3" t="s">
-        <v>1059</v>
+        <v>1058</v>
       </c>
       <c r="V216" s="3" t="s">
         <v>110</v>
       </c>
       <c r="W216" s="3" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
     </row>
     <row r="217" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A217" s="3" t="s">
-        <v>1065</v>
+        <v>1064</v>
       </c>
       <c r="B217" s="3" t="s">
         <v>61</v>
@@ -18765,28 +18771,28 @@
         <v>40</v>
       </c>
       <c r="E217" s="3" t="s">
+        <v>1065</v>
+      </c>
+      <c r="F217" s="3" t="s">
         <v>1066</v>
-      </c>
-      <c r="F217" s="3" t="s">
-        <v>1067</v>
       </c>
       <c r="G217" s="4">
         <v>44915</v>
       </c>
       <c r="H217" s="3" t="s">
+        <v>1067</v>
+      </c>
+      <c r="I217" s="3" t="s">
         <v>1068</v>
       </c>
-      <c r="I217" s="3" t="s">
+      <c r="J217" s="3" t="s">
         <v>1069</v>
       </c>
-      <c r="J217" s="3" t="s">
+      <c r="K217" s="3" t="s">
         <v>1070</v>
       </c>
-      <c r="K217" s="3" t="s">
+      <c r="L217" s="3" t="s">
         <v>1071</v>
-      </c>
-      <c r="L217" s="3" t="s">
-        <v>1072</v>
       </c>
       <c r="M217" s="4">
         <v>44951</v>
@@ -18810,21 +18816,21 @@
         <v>36</v>
       </c>
       <c r="T217" s="3" t="s">
+        <v>1072</v>
+      </c>
+      <c r="U217" s="3" t="s">
         <v>1073</v>
       </c>
-      <c r="U217" s="3" t="s">
+      <c r="V217" s="3" t="s">
         <v>1074</v>
       </c>
-      <c r="V217" s="3" t="s">
+      <c r="W217" s="3" t="s">
         <v>1075</v>
-      </c>
-      <c r="W217" s="3" t="s">
-        <v>1076</v>
       </c>
     </row>
     <row r="218" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A218" s="3" t="s">
-        <v>1077</v>
+        <v>1076</v>
       </c>
       <c r="B218" s="3" t="s">
         <v>38</v>
@@ -18836,28 +18842,28 @@
         <v>53</v>
       </c>
       <c r="E218" s="3" t="s">
-        <v>1066</v>
+        <v>1065</v>
       </c>
       <c r="F218" s="3" t="s">
-        <v>1078</v>
+        <v>1077</v>
       </c>
       <c r="G218" s="4">
         <v>44915</v>
       </c>
       <c r="H218" s="3" t="s">
+        <v>1078</v>
+      </c>
+      <c r="I218" s="3" t="s">
         <v>1079</v>
       </c>
-      <c r="I218" s="3" t="s">
+      <c r="J218" s="3" t="s">
         <v>1080</v>
       </c>
-      <c r="J218" s="3" t="s">
+      <c r="K218" s="3" t="s">
         <v>1081</v>
       </c>
-      <c r="K218" s="3" t="s">
+      <c r="L218" s="3" t="s">
         <v>1082</v>
-      </c>
-      <c r="L218" s="3" t="s">
-        <v>1083</v>
       </c>
       <c r="M218" s="4">
         <v>44951</v>
@@ -18881,21 +18887,21 @@
         <v>36</v>
       </c>
       <c r="T218" s="3" t="s">
+        <v>1083</v>
+      </c>
+      <c r="U218" s="3" t="s">
         <v>1084</v>
       </c>
-      <c r="U218" s="3" t="s">
-        <v>1085</v>
-      </c>
       <c r="V218" s="3" t="s">
+        <v>1074</v>
+      </c>
+      <c r="W218" s="3" t="s">
         <v>1075</v>
-      </c>
-      <c r="W218" s="3" t="s">
-        <v>1076</v>
       </c>
     </row>
     <row r="219" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A219" s="3" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
       <c r="B219" s="3" t="s">
         <v>38</v>
@@ -18916,19 +18922,19 @@
         <v>45239</v>
       </c>
       <c r="H219" s="3" t="s">
-        <v>1087</v>
+        <v>1086</v>
       </c>
       <c r="I219" s="3" t="s">
         <v>28</v>
       </c>
       <c r="J219" s="3" t="s">
+        <v>1087</v>
+      </c>
+      <c r="K219" s="3" t="s">
         <v>1088</v>
       </c>
-      <c r="K219" s="3" t="s">
+      <c r="L219" s="3" t="s">
         <v>1089</v>
-      </c>
-      <c r="L219" s="3" t="s">
-        <v>1090</v>
       </c>
       <c r="M219" s="4">
         <v>44812</v>
@@ -18951,18 +18957,18 @@
         <v>87</v>
       </c>
       <c r="U219" s="3" t="s">
-        <v>1091</v>
+        <v>1090</v>
       </c>
       <c r="V219" s="3" t="s">
         <v>177</v>
       </c>
       <c r="W219" s="3" t="s">
-        <v>1092</v>
+        <v>1091</v>
       </c>
     </row>
     <row r="220" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A220" s="3" t="s">
-        <v>1093</v>
+        <v>1092</v>
       </c>
       <c r="B220" s="3" t="s">
         <v>61</v>
@@ -18983,19 +18989,19 @@
         <v>45239</v>
       </c>
       <c r="H220" s="3" t="s">
-        <v>1094</v>
+        <v>1093</v>
       </c>
       <c r="I220" s="3" t="s">
         <v>28</v>
       </c>
       <c r="J220" s="3" t="s">
-        <v>1095</v>
+        <v>1094</v>
       </c>
       <c r="K220" s="3" t="s">
+        <v>1088</v>
+      </c>
+      <c r="L220" s="3" t="s">
         <v>1089</v>
-      </c>
-      <c r="L220" s="3" t="s">
-        <v>1090</v>
       </c>
       <c r="M220" s="4">
         <v>44812</v>
@@ -19018,18 +19024,18 @@
         <v>87</v>
       </c>
       <c r="U220" s="3" t="s">
-        <v>1091</v>
+        <v>1090</v>
       </c>
       <c r="V220" s="3" t="s">
         <v>313</v>
       </c>
       <c r="W220" s="3" t="s">
-        <v>1092</v>
+        <v>1091</v>
       </c>
     </row>
     <row r="221" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A221" s="3" t="s">
-        <v>1096</v>
+        <v>1095</v>
       </c>
       <c r="B221" s="3" t="s">
         <v>727</v>
@@ -19041,7 +19047,7 @@
         <v>807</v>
       </c>
       <c r="E221" s="3" t="s">
-        <v>1097</v>
+        <v>1096</v>
       </c>
       <c r="F221" s="3" t="s">
         <v>512</v>
@@ -19050,10 +19056,10 @@
         <v>45477</v>
       </c>
       <c r="H221" s="3" t="s">
+        <v>1097</v>
+      </c>
+      <c r="I221" s="3" t="s">
         <v>1098</v>
-      </c>
-      <c r="I221" s="3" t="s">
-        <v>1099</v>
       </c>
       <c r="J221" s="3" t="s">
         <v>28</v>
@@ -19065,22 +19071,22 @@
         <v>28</v>
       </c>
       <c r="M221" s="3" t="s">
-        <v>1100</v>
+        <v>1099</v>
       </c>
       <c r="N221" s="3" t="s">
-        <v>1100</v>
+        <v>1099</v>
       </c>
       <c r="O221" s="3" t="s">
-        <v>1100</v>
+        <v>1099</v>
       </c>
       <c r="P221" s="3" t="s">
-        <v>1100</v>
+        <v>1099</v>
       </c>
       <c r="Q221" s="3" t="s">
         <v>36</v>
       </c>
       <c r="R221" s="3" t="s">
-        <v>1100</v>
+        <v>1099</v>
       </c>
       <c r="S221" s="3" t="s">
         <v>36</v>
@@ -19095,7 +19101,7 @@
         <v>177</v>
       </c>
       <c r="W221" s="3" t="s">
-        <v>1101</v>
+        <v>1100</v>
       </c>
     </row>
     <row r="222" spans="1:23" x14ac:dyDescent="0.25">
@@ -19169,7 +19175,7 @@
     </row>
     <row r="223" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A223" s="3" t="s">
-        <v>1102</v>
+        <v>1101</v>
       </c>
       <c r="B223" s="3" t="s">
         <v>38</v>
@@ -19181,7 +19187,7 @@
         <v>53</v>
       </c>
       <c r="E223" s="3" t="s">
-        <v>1103</v>
+        <v>1102</v>
       </c>
       <c r="F223" s="3" t="s">
         <v>42</v>
@@ -19190,19 +19196,19 @@
         <v>45489</v>
       </c>
       <c r="H223" s="3" t="s">
-        <v>1104</v>
+        <v>1103</v>
       </c>
       <c r="I223" s="3" t="s">
         <v>28</v>
       </c>
       <c r="J223" s="3" t="s">
+        <v>1104</v>
+      </c>
+      <c r="K223" s="3" t="s">
         <v>1105</v>
       </c>
-      <c r="K223" s="3" t="s">
+      <c r="L223" s="3" t="s">
         <v>1106</v>
-      </c>
-      <c r="L223" s="3" t="s">
-        <v>1107</v>
       </c>
       <c r="M223" s="4">
         <v>44951</v>
@@ -19222,21 +19228,21 @@
         <v>36</v>
       </c>
       <c r="T223" s="3" t="s">
+        <v>1107</v>
+      </c>
+      <c r="U223" s="3" t="s">
         <v>1108</v>
-      </c>
-      <c r="U223" s="3" t="s">
-        <v>1109</v>
       </c>
       <c r="V223" s="3" t="s">
         <v>110</v>
       </c>
       <c r="W223" s="3" t="s">
-        <v>1110</v>
+        <v>1109</v>
       </c>
     </row>
     <row r="224" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A224" s="3" t="s">
-        <v>1111</v>
+        <v>1110</v>
       </c>
       <c r="B224" s="3" t="s">
         <v>61</v>
@@ -19248,7 +19254,7 @@
         <v>53</v>
       </c>
       <c r="E224" s="3" t="s">
-        <v>1103</v>
+        <v>1102</v>
       </c>
       <c r="F224" s="3" t="s">
         <v>42</v>
@@ -19257,19 +19263,19 @@
         <v>45489</v>
       </c>
       <c r="H224" s="3" t="s">
-        <v>1112</v>
+        <v>1111</v>
       </c>
       <c r="I224" s="3" t="s">
         <v>28</v>
       </c>
       <c r="J224" s="3" t="s">
+        <v>1104</v>
+      </c>
+      <c r="K224" s="3" t="s">
         <v>1105</v>
       </c>
-      <c r="K224" s="3" t="s">
+      <c r="L224" s="3" t="s">
         <v>1106</v>
-      </c>
-      <c r="L224" s="3" t="s">
-        <v>1107</v>
       </c>
       <c r="M224" s="4">
         <v>44951</v>
@@ -19289,21 +19295,21 @@
         <v>36</v>
       </c>
       <c r="T224" s="3" t="s">
+        <v>1107</v>
+      </c>
+      <c r="U224" s="3" t="s">
         <v>1108</v>
-      </c>
-      <c r="U224" s="3" t="s">
-        <v>1109</v>
       </c>
       <c r="V224" s="3" t="s">
         <v>110</v>
       </c>
       <c r="W224" s="3" t="s">
-        <v>1110</v>
+        <v>1109</v>
       </c>
     </row>
     <row r="225" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A225" s="3" t="s">
-        <v>1113</v>
+        <v>1112</v>
       </c>
       <c r="B225" s="3" t="s">
         <v>38</v>
@@ -19315,7 +19321,7 @@
         <v>64</v>
       </c>
       <c r="E225" s="3" t="s">
-        <v>1114</v>
+        <v>1113</v>
       </c>
       <c r="F225" s="3" t="s">
         <v>42</v>
@@ -19324,19 +19330,19 @@
         <v>44875</v>
       </c>
       <c r="H225" s="3" t="s">
+        <v>1114</v>
+      </c>
+      <c r="I225" s="3" t="s">
         <v>1115</v>
       </c>
-      <c r="I225" s="3" t="s">
+      <c r="J225" s="3" t="s">
         <v>1116</v>
       </c>
-      <c r="J225" s="3" t="s">
+      <c r="K225" s="3" t="s">
         <v>1117</v>
       </c>
-      <c r="K225" s="3" t="s">
+      <c r="L225" s="3" t="s">
         <v>1118</v>
-      </c>
-      <c r="L225" s="3" t="s">
-        <v>1119</v>
       </c>
       <c r="M225" s="4">
         <v>44875</v>
@@ -19358,21 +19364,21 @@
         <v>36</v>
       </c>
       <c r="T225" s="3" t="s">
+        <v>1119</v>
+      </c>
+      <c r="U225" s="3" t="s">
         <v>1120</v>
-      </c>
-      <c r="U225" s="3" t="s">
-        <v>1121</v>
       </c>
       <c r="V225" s="3" t="s">
         <v>110</v>
       </c>
       <c r="W225" s="3" t="s">
-        <v>1122</v>
+        <v>1121</v>
       </c>
     </row>
     <row r="226" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A226" s="3" t="s">
-        <v>1123</v>
+        <v>1122</v>
       </c>
       <c r="B226" s="3" t="s">
         <v>61</v>
@@ -19384,7 +19390,7 @@
         <v>64</v>
       </c>
       <c r="E226" s="3" t="s">
-        <v>1124</v>
+        <v>1123</v>
       </c>
       <c r="F226" s="3" t="s">
         <v>42</v>
@@ -19393,19 +19399,19 @@
         <v>44875</v>
       </c>
       <c r="H226" s="3" t="s">
+        <v>1115</v>
+      </c>
+      <c r="I226" s="3" t="s">
+        <v>1114</v>
+      </c>
+      <c r="J226" s="3" t="s">
         <v>1116</v>
       </c>
-      <c r="I226" s="3" t="s">
-        <v>1115</v>
-      </c>
-      <c r="J226" s="3" t="s">
+      <c r="K226" s="3" t="s">
         <v>1117</v>
       </c>
-      <c r="K226" s="3" t="s">
+      <c r="L226" s="3" t="s">
         <v>1118</v>
-      </c>
-      <c r="L226" s="3" t="s">
-        <v>1119</v>
       </c>
       <c r="M226" s="4">
         <v>44875</v>
@@ -19427,21 +19433,21 @@
         <v>36</v>
       </c>
       <c r="T226" s="3" t="s">
+        <v>1119</v>
+      </c>
+      <c r="U226" s="3" t="s">
         <v>1120</v>
-      </c>
-      <c r="U226" s="3" t="s">
-        <v>1121</v>
       </c>
       <c r="V226" s="3" t="s">
         <v>110</v>
       </c>
       <c r="W226" s="3" t="s">
-        <v>1122</v>
+        <v>1121</v>
       </c>
     </row>
     <row r="227" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A227" s="3" t="s">
-        <v>1125</v>
+        <v>1124</v>
       </c>
       <c r="B227" s="3" t="s">
         <v>727</v>
@@ -19456,25 +19462,25 @@
         <v>171</v>
       </c>
       <c r="F227" s="3" t="s">
-        <v>1126</v>
+        <v>1125</v>
       </c>
       <c r="G227" s="4">
         <v>45131</v>
       </c>
       <c r="H227" s="3" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
       <c r="I227" s="3" t="s">
         <v>28</v>
       </c>
       <c r="J227" s="3" t="s">
+        <v>1127</v>
+      </c>
+      <c r="K227" s="3" t="s">
         <v>1128</v>
       </c>
-      <c r="K227" s="3" t="s">
+      <c r="L227" s="3" t="s">
         <v>1129</v>
-      </c>
-      <c r="L227" s="3" t="s">
-        <v>1130</v>
       </c>
       <c r="M227" s="4">
         <v>44873</v>
@@ -19497,18 +19503,18 @@
         <v>87</v>
       </c>
       <c r="U227" s="3" t="s">
-        <v>1131</v>
+        <v>1130</v>
       </c>
       <c r="V227" s="3" t="s">
         <v>110</v>
       </c>
       <c r="W227" s="3" t="s">
-        <v>1132</v>
+        <v>1131</v>
       </c>
     </row>
     <row r="228" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A228" s="3" t="s">
-        <v>1133</v>
+        <v>1132</v>
       </c>
       <c r="B228" s="3" t="s">
         <v>61</v>
@@ -19523,25 +19529,25 @@
         <v>171</v>
       </c>
       <c r="F228" s="3" t="s">
-        <v>1126</v>
+        <v>1125</v>
       </c>
       <c r="G228" s="4">
         <v>45131</v>
       </c>
       <c r="H228" s="3" t="s">
-        <v>1134</v>
+        <v>1133</v>
       </c>
       <c r="I228" s="3" t="s">
         <v>28</v>
       </c>
       <c r="J228" s="3" t="s">
+        <v>1127</v>
+      </c>
+      <c r="K228" s="3" t="s">
         <v>1128</v>
       </c>
-      <c r="K228" s="3" t="s">
+      <c r="L228" s="3" t="s">
         <v>1129</v>
-      </c>
-      <c r="L228" s="3" t="s">
-        <v>1130</v>
       </c>
       <c r="M228" s="4">
         <v>44873</v>
@@ -19564,18 +19570,18 @@
         <v>87</v>
       </c>
       <c r="U228" s="3" t="s">
-        <v>1131</v>
+        <v>1130</v>
       </c>
       <c r="V228" s="3" t="s">
         <v>110</v>
       </c>
       <c r="W228" s="3" t="s">
-        <v>1132</v>
+        <v>1131</v>
       </c>
     </row>
     <row r="229" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A229" s="3" t="s">
-        <v>1135</v>
+        <v>1134</v>
       </c>
       <c r="B229" s="3" t="s">
         <v>38</v>
@@ -19587,7 +19593,7 @@
         <v>64</v>
       </c>
       <c r="E229" s="3" t="s">
-        <v>1136</v>
+        <v>1135</v>
       </c>
       <c r="F229" s="3" t="s">
         <v>602</v>
@@ -19596,19 +19602,19 @@
         <v>45330</v>
       </c>
       <c r="H229" s="3" t="s">
+        <v>1136</v>
+      </c>
+      <c r="I229" s="3" t="s">
         <v>1137</v>
       </c>
-      <c r="I229" s="3" t="s">
+      <c r="J229" s="3" t="s">
         <v>1138</v>
       </c>
-      <c r="J229" s="3" t="s">
+      <c r="K229" s="3" t="s">
         <v>1139</v>
       </c>
-      <c r="K229" s="3" t="s">
+      <c r="L229" s="3" t="s">
         <v>1140</v>
-      </c>
-      <c r="L229" s="3" t="s">
-        <v>1141</v>
       </c>
       <c r="M229" s="4">
         <v>45237</v>
@@ -19628,21 +19634,21 @@
         <v>36</v>
       </c>
       <c r="T229" s="3" t="s">
+        <v>1141</v>
+      </c>
+      <c r="U229" s="3" t="s">
         <v>1142</v>
-      </c>
-      <c r="U229" s="3" t="s">
-        <v>1143</v>
       </c>
       <c r="V229" s="3" t="s">
         <v>417</v>
       </c>
       <c r="W229" s="3" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
     </row>
     <row r="230" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A230" s="3" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
       <c r="B230" s="3" t="s">
         <v>61</v>
@@ -19654,7 +19660,7 @@
         <v>64</v>
       </c>
       <c r="E230" s="3" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
       <c r="F230" s="3" t="s">
         <v>602</v>
@@ -19663,19 +19669,19 @@
         <v>45330</v>
       </c>
       <c r="H230" s="3" t="s">
+        <v>1137</v>
+      </c>
+      <c r="I230" s="3" t="s">
+        <v>1136</v>
+      </c>
+      <c r="J230" s="3" t="s">
         <v>1138</v>
       </c>
-      <c r="I230" s="3" t="s">
-        <v>1137</v>
-      </c>
-      <c r="J230" s="3" t="s">
+      <c r="K230" s="3" t="s">
         <v>1139</v>
       </c>
-      <c r="K230" s="3" t="s">
+      <c r="L230" s="3" t="s">
         <v>1140</v>
-      </c>
-      <c r="L230" s="3" t="s">
-        <v>1141</v>
       </c>
       <c r="M230" s="4">
         <v>45237</v>
@@ -19695,21 +19701,21 @@
         <v>36</v>
       </c>
       <c r="T230" s="3" t="s">
+        <v>1141</v>
+      </c>
+      <c r="U230" s="3" t="s">
         <v>1142</v>
-      </c>
-      <c r="U230" s="3" t="s">
-        <v>1143</v>
       </c>
       <c r="V230" s="3" t="s">
         <v>417</v>
       </c>
       <c r="W230" s="3" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
     </row>
     <row r="231" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A231" s="3" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
       <c r="B231" s="3" t="s">
         <v>38</v>
@@ -19721,7 +19727,7 @@
         <v>64</v>
       </c>
       <c r="E231" s="3" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
       <c r="F231" s="3" t="s">
         <v>42</v>
@@ -19730,19 +19736,19 @@
         <v>45308</v>
       </c>
       <c r="H231" s="3" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
       <c r="I231" s="3" t="s">
         <v>28</v>
       </c>
       <c r="J231" s="3" t="s">
+        <v>1149</v>
+      </c>
+      <c r="K231" s="3" t="s">
         <v>1150</v>
       </c>
-      <c r="K231" s="3" t="s">
+      <c r="L231" s="3" t="s">
         <v>1151</v>
-      </c>
-      <c r="L231" s="3" t="s">
-        <v>1152</v>
       </c>
       <c r="M231" s="4">
         <v>45239</v>
@@ -19766,21 +19772,21 @@
         <v>36</v>
       </c>
       <c r="T231" s="3" t="s">
+        <v>1152</v>
+      </c>
+      <c r="U231" s="3" t="s">
         <v>1153</v>
-      </c>
-      <c r="U231" s="3" t="s">
-        <v>1154</v>
       </c>
       <c r="V231" s="3" t="s">
         <v>188</v>
       </c>
       <c r="W231" s="3" t="s">
-        <v>1155</v>
+        <v>1154</v>
       </c>
     </row>
     <row r="232" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A232" s="3" t="s">
-        <v>1156</v>
+        <v>1155</v>
       </c>
       <c r="B232" s="3" t="s">
         <v>61</v>
@@ -19792,7 +19798,7 @@
         <v>64</v>
       </c>
       <c r="E232" s="3" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
       <c r="F232" s="3" t="s">
         <v>42</v>
@@ -19801,19 +19807,19 @@
         <v>45308</v>
       </c>
       <c r="H232" s="3" t="s">
-        <v>1157</v>
+        <v>1156</v>
       </c>
       <c r="I232" s="3" t="s">
         <v>28</v>
       </c>
       <c r="J232" s="3" t="s">
+        <v>1149</v>
+      </c>
+      <c r="K232" s="3" t="s">
         <v>1150</v>
       </c>
-      <c r="K232" s="3" t="s">
+      <c r="L232" s="3" t="s">
         <v>1151</v>
-      </c>
-      <c r="L232" s="3" t="s">
-        <v>1152</v>
       </c>
       <c r="M232" s="4">
         <v>45239</v>
@@ -19837,21 +19843,21 @@
         <v>36</v>
       </c>
       <c r="T232" s="3" t="s">
+        <v>1152</v>
+      </c>
+      <c r="U232" s="3" t="s">
         <v>1153</v>
-      </c>
-      <c r="U232" s="3" t="s">
-        <v>1154</v>
       </c>
       <c r="V232" s="3" t="s">
         <v>188</v>
       </c>
       <c r="W232" s="3" t="s">
-        <v>1155</v>
+        <v>1154</v>
       </c>
     </row>
     <row r="233" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A233" s="3" t="s">
-        <v>1158</v>
+        <v>1157</v>
       </c>
       <c r="B233" s="3" t="s">
         <v>38</v>
@@ -19863,28 +19869,28 @@
         <v>64</v>
       </c>
       <c r="E233" s="3" t="s">
-        <v>1159</v>
+        <v>1158</v>
       </c>
       <c r="F233" s="3" t="s">
-        <v>1078</v>
+        <v>1077</v>
       </c>
       <c r="G233" s="4">
         <v>45323</v>
       </c>
       <c r="H233" s="3" t="s">
+        <v>1159</v>
+      </c>
+      <c r="I233" s="3" t="s">
         <v>1160</v>
       </c>
-      <c r="I233" s="3" t="s">
+      <c r="J233" s="3" t="s">
         <v>1161</v>
       </c>
-      <c r="J233" s="3" t="s">
+      <c r="K233" s="3" t="s">
         <v>1162</v>
       </c>
-      <c r="K233" s="3" t="s">
+      <c r="L233" s="3" t="s">
         <v>1163</v>
-      </c>
-      <c r="L233" s="3" t="s">
-        <v>1164</v>
       </c>
       <c r="M233" s="4">
         <v>45316</v>
@@ -19904,21 +19910,21 @@
         <v>36</v>
       </c>
       <c r="T233" s="3" t="s">
+        <v>1164</v>
+      </c>
+      <c r="U233" s="3" t="s">
         <v>1165</v>
-      </c>
-      <c r="U233" s="3" t="s">
-        <v>1166</v>
       </c>
       <c r="V233" s="3" t="s">
         <v>89</v>
       </c>
       <c r="W233" s="3" t="s">
-        <v>1167</v>
+        <v>1166</v>
       </c>
     </row>
     <row r="234" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A234" s="3" t="s">
-        <v>1168</v>
+        <v>1167</v>
       </c>
       <c r="B234" s="3" t="s">
         <v>61</v>
@@ -19930,28 +19936,28 @@
         <v>64</v>
       </c>
       <c r="E234" s="3" t="s">
-        <v>1169</v>
+        <v>1168</v>
       </c>
       <c r="F234" s="3" t="s">
-        <v>1078</v>
+        <v>1077</v>
       </c>
       <c r="G234" s="4">
         <v>45323</v>
       </c>
       <c r="H234" s="3" t="s">
+        <v>1169</v>
+      </c>
+      <c r="I234" s="3" t="s">
         <v>1170</v>
       </c>
-      <c r="I234" s="3" t="s">
+      <c r="J234" s="3" t="s">
         <v>1171</v>
       </c>
-      <c r="J234" s="3" t="s">
-        <v>1172</v>
-      </c>
       <c r="K234" s="3" t="s">
+        <v>1162</v>
+      </c>
+      <c r="L234" s="3" t="s">
         <v>1163</v>
-      </c>
-      <c r="L234" s="3" t="s">
-        <v>1164</v>
       </c>
       <c r="M234" s="4">
         <v>45316</v>
@@ -19971,21 +19977,21 @@
         <v>36</v>
       </c>
       <c r="T234" s="3" t="s">
+        <v>1164</v>
+      </c>
+      <c r="U234" s="3" t="s">
         <v>1165</v>
-      </c>
-      <c r="U234" s="3" t="s">
-        <v>1166</v>
       </c>
       <c r="V234" s="3" t="s">
         <v>89</v>
       </c>
       <c r="W234" s="3" t="s">
-        <v>1167</v>
+        <v>1166</v>
       </c>
     </row>
     <row r="235" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A235" s="3" t="s">
-        <v>1173</v>
+        <v>1172</v>
       </c>
       <c r="B235" s="3" t="s">
         <v>61</v>
@@ -19997,28 +20003,28 @@
         <v>64</v>
       </c>
       <c r="E235" s="3" t="s">
-        <v>1174</v>
+        <v>1173</v>
       </c>
       <c r="F235" s="3" t="s">
-        <v>1078</v>
+        <v>1077</v>
       </c>
       <c r="G235" s="4">
         <v>45393</v>
       </c>
       <c r="H235" s="3" t="s">
+        <v>1174</v>
+      </c>
+      <c r="I235" s="3" t="s">
         <v>1175</v>
       </c>
-      <c r="I235" s="3" t="s">
+      <c r="J235" s="3" t="s">
         <v>1176</v>
       </c>
-      <c r="J235" s="3" t="s">
-        <v>1177</v>
-      </c>
       <c r="K235" s="3" t="s">
+        <v>1162</v>
+      </c>
+      <c r="L235" s="3" t="s">
         <v>1163</v>
-      </c>
-      <c r="L235" s="3" t="s">
-        <v>1164</v>
       </c>
       <c r="M235" s="4">
         <v>45316</v>
@@ -20038,21 +20044,21 @@
         <v>36</v>
       </c>
       <c r="T235" s="3" t="s">
+        <v>1164</v>
+      </c>
+      <c r="U235" s="3" t="s">
         <v>1165</v>
-      </c>
-      <c r="U235" s="3" t="s">
-        <v>1166</v>
       </c>
       <c r="V235" s="3" t="s">
         <v>89</v>
       </c>
       <c r="W235" s="3" t="s">
-        <v>1167</v>
+        <v>1166</v>
       </c>
     </row>
     <row r="236" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A236" s="3" t="s">
-        <v>1178</v>
+        <v>1177</v>
       </c>
       <c r="B236" s="3" t="s">
         <v>38</v>
@@ -20064,7 +20070,7 @@
         <v>40</v>
       </c>
       <c r="E236" s="3" t="s">
-        <v>1179</v>
+        <v>1178</v>
       </c>
       <c r="F236" s="3" t="s">
         <v>42</v>
@@ -20073,19 +20079,19 @@
         <v>45370</v>
       </c>
       <c r="H236" s="3" t="s">
+        <v>1179</v>
+      </c>
+      <c r="I236" s="3" t="s">
         <v>1180</v>
       </c>
-      <c r="I236" s="3" t="s">
+      <c r="J236" s="3" t="s">
         <v>1181</v>
       </c>
-      <c r="J236" s="3" t="s">
+      <c r="K236" s="3" t="s">
         <v>1182</v>
       </c>
-      <c r="K236" s="3" t="s">
+      <c r="L236" s="3" t="s">
         <v>1183</v>
-      </c>
-      <c r="L236" s="3" t="s">
-        <v>1184</v>
       </c>
       <c r="M236" s="4">
         <v>45279</v>
@@ -20107,21 +20113,21 @@
         <v>36</v>
       </c>
       <c r="T236" s="3" t="s">
+        <v>1184</v>
+      </c>
+      <c r="U236" s="3" t="s">
         <v>1185</v>
-      </c>
-      <c r="U236" s="3" t="s">
-        <v>1186</v>
       </c>
       <c r="V236" s="3" t="s">
         <v>89</v>
       </c>
       <c r="W236" s="3" t="s">
-        <v>1187</v>
+        <v>1186</v>
       </c>
     </row>
     <row r="237" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A237" s="3" t="s">
-        <v>1188</v>
+        <v>1187</v>
       </c>
       <c r="B237" s="3" t="s">
         <v>61</v>
@@ -20133,7 +20139,7 @@
         <v>40</v>
       </c>
       <c r="E237" s="3" t="s">
-        <v>1179</v>
+        <v>1178</v>
       </c>
       <c r="F237" s="3" t="s">
         <v>42</v>
@@ -20142,19 +20148,19 @@
         <v>45370</v>
       </c>
       <c r="H237" s="3" t="s">
+        <v>1180</v>
+      </c>
+      <c r="I237" s="3" t="s">
+        <v>1179</v>
+      </c>
+      <c r="J237" s="3" t="s">
         <v>1181</v>
       </c>
-      <c r="I237" s="3" t="s">
-        <v>1180</v>
-      </c>
-      <c r="J237" s="3" t="s">
+      <c r="K237" s="3" t="s">
         <v>1182</v>
       </c>
-      <c r="K237" s="3" t="s">
+      <c r="L237" s="3" t="s">
         <v>1183</v>
-      </c>
-      <c r="L237" s="3" t="s">
-        <v>1184</v>
       </c>
       <c r="M237" s="4">
         <v>45279</v>
@@ -20176,21 +20182,21 @@
         <v>36</v>
       </c>
       <c r="T237" s="3" t="s">
+        <v>1184</v>
+      </c>
+      <c r="U237" s="3" t="s">
         <v>1185</v>
-      </c>
-      <c r="U237" s="3" t="s">
-        <v>1186</v>
       </c>
       <c r="V237" s="3" t="s">
         <v>89</v>
       </c>
       <c r="W237" s="3" t="s">
-        <v>1187</v>
+        <v>1186</v>
       </c>
     </row>
     <row r="238" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A238" s="3" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
       <c r="B238" s="3" t="s">
         <v>61</v>
@@ -20202,28 +20208,28 @@
         <v>40</v>
       </c>
       <c r="E238" s="3" t="s">
+        <v>1189</v>
+      </c>
+      <c r="F238" s="3" t="s">
         <v>1190</v>
-      </c>
-      <c r="F238" s="3" t="s">
-        <v>1191</v>
       </c>
       <c r="G238" s="4">
         <v>45078</v>
       </c>
       <c r="H238" s="3" t="s">
+        <v>1191</v>
+      </c>
+      <c r="I238" s="3" t="s">
         <v>1192</v>
       </c>
-      <c r="I238" s="3" t="s">
+      <c r="J238" s="3" t="s">
+        <v>1192</v>
+      </c>
+      <c r="K238" s="3" t="s">
         <v>1193</v>
       </c>
-      <c r="J238" s="3" t="s">
-        <v>1193</v>
-      </c>
-      <c r="K238" s="3" t="s">
-        <v>1194</v>
-      </c>
       <c r="L238" s="3" t="s">
-        <v>1193</v>
+        <v>1192</v>
       </c>
       <c r="M238" s="4">
         <v>44851</v>
@@ -20246,18 +20252,18 @@
         <v>36</v>
       </c>
       <c r="U238" s="3" t="s">
-        <v>1195</v>
+        <v>1194</v>
       </c>
       <c r="V238" s="3" t="s">
         <v>177</v>
       </c>
       <c r="W238" s="3" t="s">
-        <v>1196</v>
+        <v>1195</v>
       </c>
     </row>
     <row r="239" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A239" s="3" t="s">
-        <v>1197</v>
+        <v>1196</v>
       </c>
       <c r="B239" s="3" t="s">
         <v>38</v>
@@ -20269,28 +20275,28 @@
         <v>40</v>
       </c>
       <c r="E239" s="3" t="s">
-        <v>1198</v>
+        <v>1197</v>
       </c>
       <c r="F239" s="3" t="s">
-        <v>1191</v>
+        <v>1190</v>
       </c>
       <c r="G239" s="4">
         <v>45078</v>
       </c>
       <c r="H239" s="3" t="s">
-        <v>1199</v>
+        <v>1198</v>
       </c>
       <c r="I239" s="3" t="s">
+        <v>1192</v>
+      </c>
+      <c r="J239" s="3" t="s">
+        <v>1192</v>
+      </c>
+      <c r="K239" s="3" t="s">
         <v>1193</v>
       </c>
-      <c r="J239" s="3" t="s">
-        <v>1193</v>
-      </c>
-      <c r="K239" s="3" t="s">
-        <v>1194</v>
-      </c>
       <c r="L239" s="3" t="s">
-        <v>1193</v>
+        <v>1192</v>
       </c>
       <c r="M239" s="4">
         <v>44851</v>
@@ -20313,18 +20319,18 @@
         <v>36</v>
       </c>
       <c r="U239" s="3" t="s">
-        <v>1195</v>
+        <v>1194</v>
       </c>
       <c r="V239" s="3" t="s">
         <v>177</v>
       </c>
       <c r="W239" s="3" t="s">
-        <v>1196</v>
+        <v>1195</v>
       </c>
     </row>
     <row r="240" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A240" s="3" t="s">
-        <v>1200</v>
+        <v>1199</v>
       </c>
       <c r="B240" s="3" t="s">
         <v>61</v>
@@ -20336,28 +20342,28 @@
         <v>40</v>
       </c>
       <c r="E240" s="3" t="s">
-        <v>1201</v>
+        <v>1200</v>
       </c>
       <c r="F240" s="3" t="s">
-        <v>1191</v>
+        <v>1190</v>
       </c>
       <c r="G240" s="4">
         <v>45078</v>
       </c>
       <c r="H240" s="3" t="s">
-        <v>1202</v>
+        <v>1201</v>
       </c>
       <c r="I240" s="3" t="s">
+        <v>1192</v>
+      </c>
+      <c r="J240" s="3" t="s">
+        <v>1192</v>
+      </c>
+      <c r="K240" s="3" t="s">
         <v>1193</v>
       </c>
-      <c r="J240" s="3" t="s">
-        <v>1193</v>
-      </c>
-      <c r="K240" s="3" t="s">
-        <v>1194</v>
-      </c>
       <c r="L240" s="3" t="s">
-        <v>1193</v>
+        <v>1192</v>
       </c>
       <c r="M240" s="4">
         <v>44851</v>
@@ -20380,18 +20386,18 @@
         <v>36</v>
       </c>
       <c r="U240" s="3" t="s">
-        <v>1195</v>
+        <v>1194</v>
       </c>
       <c r="V240" s="3" t="s">
         <v>177</v>
       </c>
       <c r="W240" s="3" t="s">
-        <v>1196</v>
+        <v>1195</v>
       </c>
     </row>
     <row r="241" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A241" s="3" t="s">
-        <v>1203</v>
+        <v>1202</v>
       </c>
       <c r="B241" s="3" t="s">
         <v>38</v>
@@ -20403,28 +20409,28 @@
         <v>64</v>
       </c>
       <c r="E241" s="3" t="s">
-        <v>1204</v>
+        <v>1203</v>
       </c>
       <c r="F241" s="3" t="s">
-        <v>1078</v>
+        <v>1077</v>
       </c>
       <c r="G241" s="4">
         <v>45390</v>
       </c>
       <c r="H241" s="3" t="s">
+        <v>1204</v>
+      </c>
+      <c r="I241" s="3" t="s">
         <v>1205</v>
       </c>
-      <c r="I241" s="3" t="s">
-        <v>1206</v>
-      </c>
       <c r="J241" s="3" t="s">
+        <v>1080</v>
+      </c>
+      <c r="K241" s="3" t="s">
         <v>1081</v>
       </c>
-      <c r="K241" s="3" t="s">
+      <c r="L241" s="3" t="s">
         <v>1082</v>
-      </c>
-      <c r="L241" s="3" t="s">
-        <v>1083</v>
       </c>
       <c r="M241" s="4">
         <v>45372</v>
@@ -20448,21 +20454,21 @@
         <v>36</v>
       </c>
       <c r="T241" s="3" t="s">
+        <v>1083</v>
+      </c>
+      <c r="U241" s="3" t="s">
         <v>1084</v>
       </c>
-      <c r="U241" s="3" t="s">
-        <v>1085</v>
-      </c>
       <c r="V241" s="3" t="s">
+        <v>1074</v>
+      </c>
+      <c r="W241" s="3" t="s">
         <v>1075</v>
-      </c>
-      <c r="W241" s="3" t="s">
-        <v>1076</v>
       </c>
     </row>
     <row r="242" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A242" s="3" t="s">
-        <v>1207</v>
+        <v>1206</v>
       </c>
       <c r="B242" s="3" t="s">
         <v>38</v>
@@ -20474,28 +20480,28 @@
         <v>40</v>
       </c>
       <c r="E242" s="3" t="s">
-        <v>1208</v>
+        <v>1207</v>
       </c>
       <c r="F242" s="3" t="s">
-        <v>1191</v>
+        <v>1190</v>
       </c>
       <c r="G242" s="4">
         <v>45078</v>
       </c>
       <c r="H242" s="3" t="s">
-        <v>1209</v>
+        <v>1208</v>
       </c>
       <c r="I242" s="3" t="s">
+        <v>1192</v>
+      </c>
+      <c r="J242" s="3" t="s">
+        <v>1192</v>
+      </c>
+      <c r="K242" s="3" t="s">
         <v>1193</v>
       </c>
-      <c r="J242" s="3" t="s">
-        <v>1193</v>
-      </c>
-      <c r="K242" s="3" t="s">
-        <v>1194</v>
-      </c>
       <c r="L242" s="3" t="s">
-        <v>1193</v>
+        <v>1192</v>
       </c>
       <c r="M242" s="4">
         <v>44851</v>
@@ -20518,18 +20524,18 @@
         <v>36</v>
       </c>
       <c r="U242" s="3" t="s">
-        <v>1195</v>
+        <v>1194</v>
       </c>
       <c r="V242" s="3" t="s">
         <v>177</v>
       </c>
       <c r="W242" s="3" t="s">
-        <v>1196</v>
+        <v>1195</v>
       </c>
     </row>
     <row r="243" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A243" s="3" t="s">
-        <v>1210</v>
+        <v>1209</v>
       </c>
       <c r="B243" s="3" t="s">
         <v>38</v>
@@ -20541,28 +20547,28 @@
         <v>40</v>
       </c>
       <c r="E243" s="3" t="s">
-        <v>1211</v>
+        <v>1210</v>
       </c>
       <c r="F243" s="3" t="s">
-        <v>1191</v>
+        <v>1190</v>
       </c>
       <c r="G243" s="4">
         <v>45078</v>
       </c>
       <c r="H243" s="3" t="s">
+        <v>1211</v>
+      </c>
+      <c r="I243" s="3" t="s">
         <v>1212</v>
       </c>
-      <c r="I243" s="3" t="s">
+      <c r="J243" s="3" t="s">
         <v>1213</v>
       </c>
-      <c r="J243" s="3" t="s">
+      <c r="K243" s="3" t="s">
+        <v>1193</v>
+      </c>
+      <c r="L243" s="3" t="s">
         <v>1214</v>
-      </c>
-      <c r="K243" s="3" t="s">
-        <v>1194</v>
-      </c>
-      <c r="L243" s="3" t="s">
-        <v>1215</v>
       </c>
       <c r="M243" s="4">
         <v>44851</v>
@@ -20585,18 +20591,18 @@
         <v>36</v>
       </c>
       <c r="U243" s="3" t="s">
-        <v>1195</v>
+        <v>1194</v>
       </c>
       <c r="V243" s="3" t="s">
         <v>100</v>
       </c>
       <c r="W243" s="3" t="s">
-        <v>1196</v>
+        <v>1195</v>
       </c>
     </row>
     <row r="244" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A244" s="3" t="s">
-        <v>1216</v>
+        <v>1215</v>
       </c>
       <c r="B244" s="3" t="s">
         <v>61</v>
@@ -20608,28 +20614,28 @@
         <v>40</v>
       </c>
       <c r="E244" s="3" t="s">
-        <v>1217</v>
+        <v>1216</v>
       </c>
       <c r="F244" s="3" t="s">
-        <v>1191</v>
+        <v>1190</v>
       </c>
       <c r="G244" s="4">
         <v>45078</v>
       </c>
       <c r="H244" s="3" t="s">
-        <v>1218</v>
+        <v>1217</v>
       </c>
       <c r="I244" s="3" t="s">
+        <v>1212</v>
+      </c>
+      <c r="J244" s="3" t="s">
         <v>1213</v>
       </c>
-      <c r="J244" s="3" t="s">
+      <c r="K244" s="3" t="s">
+        <v>1193</v>
+      </c>
+      <c r="L244" s="3" t="s">
         <v>1214</v>
-      </c>
-      <c r="K244" s="3" t="s">
-        <v>1194</v>
-      </c>
-      <c r="L244" s="3" t="s">
-        <v>1215</v>
       </c>
       <c r="M244" s="4">
         <v>44851</v>
@@ -20652,18 +20658,18 @@
         <v>36</v>
       </c>
       <c r="U244" s="3" t="s">
-        <v>1195</v>
+        <v>1194</v>
       </c>
       <c r="V244" s="3" t="s">
         <v>100</v>
       </c>
       <c r="W244" s="3" t="s">
-        <v>1196</v>
+        <v>1195</v>
       </c>
     </row>
     <row r="245" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A245" s="3" t="s">
-        <v>1219</v>
+        <v>1218</v>
       </c>
       <c r="B245" s="3" t="s">
         <v>38</v>
@@ -20675,7 +20681,7 @@
         <v>64</v>
       </c>
       <c r="E245" s="3" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="F245" s="3" t="s">
         <v>42</v>
@@ -20684,19 +20690,19 @@
         <v>45412</v>
       </c>
       <c r="H245" s="3" t="s">
+        <v>1220</v>
+      </c>
+      <c r="I245" s="3" t="s">
         <v>1221</v>
       </c>
-      <c r="I245" s="3" t="s">
+      <c r="J245" s="3" t="s">
         <v>1222</v>
       </c>
-      <c r="J245" s="3" t="s">
+      <c r="K245" s="3" t="s">
         <v>1223</v>
       </c>
-      <c r="K245" s="3" t="s">
+      <c r="L245" s="3" t="s">
         <v>1224</v>
-      </c>
-      <c r="L245" s="3" t="s">
-        <v>1225</v>
       </c>
       <c r="M245" s="4">
         <v>45372</v>
@@ -20720,21 +20726,21 @@
         <v>36</v>
       </c>
       <c r="T245" s="3" t="s">
+        <v>1225</v>
+      </c>
+      <c r="U245" s="3" t="s">
         <v>1226</v>
-      </c>
-      <c r="U245" s="3" t="s">
-        <v>1227</v>
       </c>
       <c r="V245" s="3" t="s">
         <v>100</v>
       </c>
       <c r="W245" s="3" t="s">
-        <v>1228</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="246" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A246" s="3" t="s">
-        <v>1229</v>
+        <v>1228</v>
       </c>
       <c r="B246" s="3" t="s">
         <v>61</v>
@@ -20746,7 +20752,7 @@
         <v>64</v>
       </c>
       <c r="E246" s="3" t="s">
-        <v>1230</v>
+        <v>1229</v>
       </c>
       <c r="F246" s="3" t="s">
         <v>42</v>
@@ -20755,19 +20761,19 @@
         <v>45412</v>
       </c>
       <c r="H246" s="3" t="s">
+        <v>1221</v>
+      </c>
+      <c r="I246" s="3" t="s">
+        <v>1220</v>
+      </c>
+      <c r="J246" s="3" t="s">
         <v>1222</v>
       </c>
-      <c r="I246" s="3" t="s">
-        <v>1221</v>
-      </c>
-      <c r="J246" s="3" t="s">
+      <c r="K246" s="3" t="s">
         <v>1223</v>
       </c>
-      <c r="K246" s="3" t="s">
+      <c r="L246" s="3" t="s">
         <v>1224</v>
-      </c>
-      <c r="L246" s="3" t="s">
-        <v>1225</v>
       </c>
       <c r="M246" s="4">
         <v>45372</v>
@@ -20791,21 +20797,21 @@
         <v>36</v>
       </c>
       <c r="T246" s="3" t="s">
+        <v>1225</v>
+      </c>
+      <c r="U246" s="3" t="s">
         <v>1226</v>
-      </c>
-      <c r="U246" s="3" t="s">
-        <v>1227</v>
       </c>
       <c r="V246" s="3" t="s">
         <v>100</v>
       </c>
       <c r="W246" s="3" t="s">
-        <v>1228</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="247" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A247" s="3" t="s">
-        <v>1231</v>
+        <v>1230</v>
       </c>
       <c r="B247" s="3" t="s">
         <v>38</v>
@@ -20817,7 +20823,7 @@
         <v>53</v>
       </c>
       <c r="E247" s="3" t="s">
-        <v>1232</v>
+        <v>1231</v>
       </c>
       <c r="F247" s="3" t="s">
         <v>42</v>
@@ -20826,19 +20832,19 @@
         <v>45503</v>
       </c>
       <c r="H247" s="3" t="s">
+        <v>1232</v>
+      </c>
+      <c r="I247" s="3" t="s">
         <v>1233</v>
       </c>
-      <c r="I247" s="3" t="s">
+      <c r="J247" s="3" t="s">
         <v>1234</v>
       </c>
-      <c r="J247" s="3" t="s">
+      <c r="K247" s="3" t="s">
         <v>1235</v>
       </c>
-      <c r="K247" s="3" t="s">
+      <c r="L247" s="3" t="s">
         <v>1236</v>
-      </c>
-      <c r="L247" s="3" t="s">
-        <v>1237</v>
       </c>
       <c r="M247" s="4">
         <v>45169</v>
@@ -20858,10 +20864,10 @@
         <v>36</v>
       </c>
       <c r="T247" s="3" t="s">
+        <v>1237</v>
+      </c>
+      <c r="U247" s="3" t="s">
         <v>1238</v>
-      </c>
-      <c r="U247" s="3" t="s">
-        <v>1239</v>
       </c>
       <c r="V247" s="3" t="s">
         <v>110</v>
@@ -20872,7 +20878,7 @@
     </row>
     <row r="248" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A248" s="3" t="s">
-        <v>1240</v>
+        <v>1239</v>
       </c>
       <c r="B248" s="3" t="s">
         <v>61</v>
@@ -20884,7 +20890,7 @@
         <v>53</v>
       </c>
       <c r="E248" s="3" t="s">
-        <v>1232</v>
+        <v>1231</v>
       </c>
       <c r="F248" s="3" t="s">
         <v>42</v>
@@ -20893,19 +20899,19 @@
         <v>45503</v>
       </c>
       <c r="H248" s="3" t="s">
+        <v>1233</v>
+      </c>
+      <c r="I248" s="3" t="s">
+        <v>1233</v>
+      </c>
+      <c r="J248" s="3" t="s">
         <v>1234</v>
       </c>
-      <c r="I248" s="3" t="s">
-        <v>1234</v>
-      </c>
-      <c r="J248" s="3" t="s">
+      <c r="K248" s="3" t="s">
         <v>1235</v>
       </c>
-      <c r="K248" s="3" t="s">
+      <c r="L248" s="3" t="s">
         <v>1236</v>
-      </c>
-      <c r="L248" s="3" t="s">
-        <v>1237</v>
       </c>
       <c r="M248" s="4">
         <v>45169</v>
@@ -20925,10 +20931,10 @@
         <v>36</v>
       </c>
       <c r="T248" s="3" t="s">
+        <v>1237</v>
+      </c>
+      <c r="U248" s="3" t="s">
         <v>1238</v>
-      </c>
-      <c r="U248" s="3" t="s">
-        <v>1239</v>
       </c>
       <c r="V248" s="3" t="s">
         <v>110</v>
@@ -20939,7 +20945,7 @@
     </row>
     <row r="249" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A249" s="3" t="s">
-        <v>1241</v>
+        <v>1240</v>
       </c>
       <c r="B249" s="3" t="s">
         <v>38</v>
@@ -20951,7 +20957,7 @@
         <v>40</v>
       </c>
       <c r="E249" s="3" t="s">
-        <v>1242</v>
+        <v>1241</v>
       </c>
       <c r="F249" s="3" t="s">
         <v>42</v>
@@ -20960,19 +20966,19 @@
         <v>45839</v>
       </c>
       <c r="H249" s="3" t="s">
+        <v>1242</v>
+      </c>
+      <c r="I249" s="3" t="s">
         <v>1243</v>
       </c>
-      <c r="I249" s="3" t="s">
+      <c r="J249" s="3" t="s">
         <v>1244</v>
       </c>
-      <c r="J249" s="3" t="s">
+      <c r="K249" s="3" t="s">
         <v>1245</v>
       </c>
-      <c r="K249" s="3" t="s">
+      <c r="L249" s="3" t="s">
         <v>1246</v>
-      </c>
-      <c r="L249" s="3" t="s">
-        <v>1247</v>
       </c>
       <c r="M249" s="4">
         <v>45666</v>
@@ -20994,10 +21000,10 @@
         <v>36</v>
       </c>
       <c r="T249" s="3" t="s">
+        <v>1247</v>
+      </c>
+      <c r="U249" s="3" t="s">
         <v>1248</v>
-      </c>
-      <c r="U249" s="3" t="s">
-        <v>1249</v>
       </c>
       <c r="V249" s="3" t="s">
         <v>51</v>
@@ -21008,7 +21014,7 @@
     </row>
     <row r="250" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A250" s="3" t="s">
-        <v>1250</v>
+        <v>1249</v>
       </c>
       <c r="B250" s="3" t="s">
         <v>61</v>
@@ -21020,7 +21026,7 @@
         <v>40</v>
       </c>
       <c r="E250" s="3" t="s">
-        <v>1242</v>
+        <v>1241</v>
       </c>
       <c r="F250" s="3" t="s">
         <v>42</v>
@@ -21029,19 +21035,19 @@
         <v>45839</v>
       </c>
       <c r="H250" s="3" t="s">
+        <v>1243</v>
+      </c>
+      <c r="I250" s="3" t="s">
+        <v>1242</v>
+      </c>
+      <c r="J250" s="3" t="s">
         <v>1244</v>
       </c>
-      <c r="I250" s="3" t="s">
-        <v>1243</v>
-      </c>
-      <c r="J250" s="3" t="s">
-        <v>1245</v>
-      </c>
       <c r="K250" s="3" t="s">
-        <v>1251</v>
+        <v>1250</v>
       </c>
       <c r="L250" s="3" t="s">
-        <v>1247</v>
+        <v>1246</v>
       </c>
       <c r="M250" s="4">
         <v>45666</v>
@@ -21063,10 +21069,10 @@
         <v>36</v>
       </c>
       <c r="T250" s="3" t="s">
-        <v>1248</v>
+        <v>1247</v>
       </c>
       <c r="U250" s="3" t="s">
-        <v>1252</v>
+        <v>1251</v>
       </c>
       <c r="V250" s="3" t="s">
         <v>51</v>
@@ -21077,7 +21083,7 @@
     </row>
     <row r="251" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A251" s="3" t="s">
-        <v>1253</v>
+        <v>1252</v>
       </c>
       <c r="B251" s="3" t="s">
         <v>38</v>
@@ -21096,19 +21102,19 @@
         <v>45803</v>
       </c>
       <c r="H251" s="3" t="s">
+        <v>1253</v>
+      </c>
+      <c r="I251" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="J251" s="3" t="s">
         <v>1254</v>
       </c>
-      <c r="I251" s="3" t="s">
+      <c r="K251" s="3" t="s">
         <v>1255</v>
       </c>
-      <c r="J251" s="3" t="s">
+      <c r="L251" s="3" t="s">
         <v>1256</v>
-      </c>
-      <c r="K251" s="3" t="s">
-        <v>1257</v>
-      </c>
-      <c r="L251" s="3" t="s">
-        <v>1258</v>
       </c>
       <c r="M251" s="4">
         <v>45645</v>
@@ -21119,17 +21125,19 @@
       <c r="O251" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="P251" s="3"/>
+      <c r="P251" s="4">
+        <v>45866</v>
+      </c>
       <c r="Q251" s="3"/>
       <c r="R251" s="3"/>
       <c r="S251" s="3" t="s">
         <v>36</v>
       </c>
       <c r="T251" s="3" t="s">
-        <v>1259</v>
+        <v>1257</v>
       </c>
       <c r="U251" s="3" t="s">
-        <v>1260</v>
+        <v>1258</v>
       </c>
       <c r="V251" s="3" t="s">
         <v>51</v>
@@ -21140,7 +21148,7 @@
     </row>
     <row r="252" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A252" s="3" t="s">
-        <v>1261</v>
+        <v>1259</v>
       </c>
       <c r="B252" s="3" t="s">
         <v>727</v>
@@ -21152,7 +21160,7 @@
         <v>53</v>
       </c>
       <c r="E252" s="3" t="s">
-        <v>1262</v>
+        <v>1260</v>
       </c>
       <c r="F252" s="3" t="s">
         <v>42</v>
@@ -21161,19 +21169,19 @@
         <v>45812</v>
       </c>
       <c r="H252" s="3" t="s">
-        <v>1263</v>
+        <v>1261</v>
       </c>
       <c r="I252" s="3" t="s">
         <v>28</v>
       </c>
       <c r="J252" s="3" t="s">
+        <v>1262</v>
+      </c>
+      <c r="K252" s="3" t="s">
+        <v>1263</v>
+      </c>
+      <c r="L252" s="3" t="s">
         <v>1264</v>
-      </c>
-      <c r="K252" s="3" t="s">
-        <v>1265</v>
-      </c>
-      <c r="L252" s="3" t="s">
-        <v>1266</v>
       </c>
       <c r="M252" s="4">
         <v>45743</v>
@@ -21197,10 +21205,10 @@
         <v>36</v>
       </c>
       <c r="T252" s="3" t="s">
-        <v>1267</v>
+        <v>1265</v>
       </c>
       <c r="U252" s="3" t="s">
-        <v>1268</v>
+        <v>1266</v>
       </c>
       <c r="V252" s="3" t="s">
         <v>51</v>
@@ -21211,7 +21219,7 @@
     </row>
     <row r="253" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A253" s="3" t="s">
-        <v>1269</v>
+        <v>1267</v>
       </c>
       <c r="B253" s="3" t="s">
         <v>38</v>
@@ -21220,10 +21228,10 @@
         <v>39</v>
       </c>
       <c r="D253" s="3" t="s">
-        <v>1270</v>
+        <v>1268</v>
       </c>
       <c r="E253" s="3" t="s">
-        <v>1271</v>
+        <v>1269</v>
       </c>
       <c r="F253" s="3" t="s">
         <v>42</v>
@@ -21232,19 +21240,19 @@
         <v>45809</v>
       </c>
       <c r="H253" s="3" t="s">
+        <v>1270</v>
+      </c>
+      <c r="I253" s="3" t="s">
+        <v>1271</v>
+      </c>
+      <c r="J253" s="3" t="s">
         <v>1272</v>
       </c>
-      <c r="I253" s="3" t="s">
+      <c r="K253" s="3" t="s">
         <v>1273</v>
       </c>
-      <c r="J253" s="3" t="s">
+      <c r="L253" s="3" t="s">
         <v>1274</v>
-      </c>
-      <c r="K253" s="3" t="s">
-        <v>1275</v>
-      </c>
-      <c r="L253" s="3" t="s">
-        <v>1276</v>
       </c>
       <c r="M253" s="4">
         <v>45666</v>
@@ -21268,10 +21276,10 @@
         <v>36</v>
       </c>
       <c r="T253" s="3" t="s">
-        <v>1277</v>
+        <v>1275</v>
       </c>
       <c r="U253" s="3" t="s">
-        <v>1278</v>
+        <v>1276</v>
       </c>
       <c r="V253" s="3" t="s">
         <v>51</v>
@@ -21282,7 +21290,7 @@
     </row>
     <row r="254" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A254" s="3" t="s">
-        <v>1279</v>
+        <v>1277</v>
       </c>
       <c r="B254" s="3" t="s">
         <v>61</v>
@@ -21291,10 +21299,10 @@
         <v>39</v>
       </c>
       <c r="D254" s="3" t="s">
-        <v>1270</v>
+        <v>1268</v>
       </c>
       <c r="E254" s="3" t="s">
-        <v>1271</v>
+        <v>1269</v>
       </c>
       <c r="F254" s="3" t="s">
         <v>42</v>
@@ -21303,19 +21311,19 @@
         <v>45809</v>
       </c>
       <c r="H254" s="3" t="s">
+        <v>1271</v>
+      </c>
+      <c r="I254" s="3" t="s">
+        <v>1270</v>
+      </c>
+      <c r="J254" s="3" t="s">
+        <v>1272</v>
+      </c>
+      <c r="K254" s="3" t="s">
         <v>1273</v>
       </c>
-      <c r="I254" s="3" t="s">
-        <v>1272</v>
-      </c>
-      <c r="J254" s="3" t="s">
+      <c r="L254" s="3" t="s">
         <v>1274</v>
-      </c>
-      <c r="K254" s="3" t="s">
-        <v>1275</v>
-      </c>
-      <c r="L254" s="3" t="s">
-        <v>1276</v>
       </c>
       <c r="M254" s="4">
         <v>45666</v>
@@ -21339,10 +21347,10 @@
         <v>36</v>
       </c>
       <c r="T254" s="3" t="s">
-        <v>1277</v>
+        <v>1275</v>
       </c>
       <c r="U254" s="3" t="s">
-        <v>1278</v>
+        <v>1276</v>
       </c>
       <c r="V254" s="3" t="s">
         <v>51</v>
@@ -21906,14 +21914,14 @@
       <c r="L10" s="6" t="b">
         <v>0</v>
       </c>
-      <c r="M10" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="N10" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="O10" s="6" t="b">
-        <v>0</v>
+      <c r="M10" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="N10" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="O10" s="5" t="b">
+        <v>1</v>
       </c>
       <c r="P10" s="6" t="b">
         <v>0</v>
@@ -21962,14 +21970,14 @@
       <c r="L11" s="6" t="b">
         <v>0</v>
       </c>
-      <c r="M11" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="N11" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="O11" s="6" t="b">
-        <v>0</v>
+      <c r="M11" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="N11" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="O11" s="5" t="b">
+        <v>1</v>
       </c>
       <c r="P11" s="6" t="b">
         <v>0</v>
@@ -32791,7 +32799,7 @@
     </row>
     <row r="205" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A205" s="3" t="s">
-        <v>987</v>
+        <v>986</v>
       </c>
       <c r="B205" s="5" t="b">
         <v>1</v>
@@ -32847,7 +32855,7 @@
     </row>
     <row r="206" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A206" s="3" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
       <c r="B206" s="5" t="b">
         <v>1</v>
@@ -32903,7 +32911,7 @@
     </row>
     <row r="207" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A207" s="3" t="s">
-        <v>1006</v>
+        <v>1005</v>
       </c>
       <c r="B207" s="5" t="b">
         <v>1</v>
@@ -32959,7 +32967,7 @@
     </row>
     <row r="208" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A208" s="3" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
       <c r="B208" s="5" t="b">
         <v>1</v>
@@ -33015,7 +33023,7 @@
     </row>
     <row r="209" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A209" s="3" t="s">
-        <v>1017</v>
+        <v>1016</v>
       </c>
       <c r="B209" s="5" t="b">
         <v>1</v>
@@ -33071,7 +33079,7 @@
     </row>
     <row r="210" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A210" s="3" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
       <c r="B210" s="5" t="b">
         <v>1</v>
@@ -33127,7 +33135,7 @@
     </row>
     <row r="211" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A211" s="3" t="s">
-        <v>1027</v>
+        <v>1026</v>
       </c>
       <c r="B211" s="5" t="b">
         <v>1</v>
@@ -33183,7 +33191,7 @@
     </row>
     <row r="212" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A212" s="3" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
       <c r="B212" s="5" t="b">
         <v>1</v>
@@ -33239,7 +33247,7 @@
     </row>
     <row r="213" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A213" s="3" t="s">
-        <v>1039</v>
+        <v>1038</v>
       </c>
       <c r="B213" s="5" t="b">
         <v>1</v>
@@ -33295,7 +33303,7 @@
     </row>
     <row r="214" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A214" s="3" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
       <c r="B214" s="5" t="b">
         <v>1</v>
@@ -33351,7 +33359,7 @@
     </row>
     <row r="215" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A215" s="3" t="s">
-        <v>1053</v>
+        <v>1052</v>
       </c>
       <c r="B215" s="5" t="b">
         <v>1</v>
@@ -33407,7 +33415,7 @@
     </row>
     <row r="216" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A216" s="3" t="s">
-        <v>1061</v>
+        <v>1060</v>
       </c>
       <c r="B216" s="5" t="b">
         <v>1</v>
@@ -33463,7 +33471,7 @@
     </row>
     <row r="217" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A217" s="3" t="s">
-        <v>1065</v>
+        <v>1064</v>
       </c>
       <c r="B217" s="5" t="b">
         <v>1</v>
@@ -33519,7 +33527,7 @@
     </row>
     <row r="218" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A218" s="3" t="s">
-        <v>1077</v>
+        <v>1076</v>
       </c>
       <c r="B218" s="5" t="b">
         <v>1</v>
@@ -33575,7 +33583,7 @@
     </row>
     <row r="219" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A219" s="3" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
       <c r="B219" s="5" t="b">
         <v>1</v>
@@ -33631,7 +33639,7 @@
     </row>
     <row r="220" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A220" s="3" t="s">
-        <v>1093</v>
+        <v>1092</v>
       </c>
       <c r="B220" s="5" t="b">
         <v>1</v>
@@ -33687,7 +33695,7 @@
     </row>
     <row r="221" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A221" s="3" t="s">
-        <v>1096</v>
+        <v>1095</v>
       </c>
       <c r="B221" s="5" t="b">
         <v>1</v>
@@ -33799,7 +33807,7 @@
     </row>
     <row r="223" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A223" s="3" t="s">
-        <v>1102</v>
+        <v>1101</v>
       </c>
       <c r="B223" s="5" t="b">
         <v>1</v>
@@ -33855,7 +33863,7 @@
     </row>
     <row r="224" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A224" s="3" t="s">
-        <v>1111</v>
+        <v>1110</v>
       </c>
       <c r="B224" s="5" t="b">
         <v>1</v>
@@ -33911,7 +33919,7 @@
     </row>
     <row r="225" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A225" s="3" t="s">
-        <v>1113</v>
+        <v>1112</v>
       </c>
       <c r="B225" s="5" t="b">
         <v>1</v>
@@ -33967,7 +33975,7 @@
     </row>
     <row r="226" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A226" s="3" t="s">
-        <v>1123</v>
+        <v>1122</v>
       </c>
       <c r="B226" s="5" t="b">
         <v>1</v>
@@ -34023,7 +34031,7 @@
     </row>
     <row r="227" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A227" s="3" t="s">
-        <v>1125</v>
+        <v>1124</v>
       </c>
       <c r="B227" s="5" t="b">
         <v>1</v>
@@ -34079,7 +34087,7 @@
     </row>
     <row r="228" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A228" s="3" t="s">
-        <v>1133</v>
+        <v>1132</v>
       </c>
       <c r="B228" s="5" t="b">
         <v>1</v>
@@ -34135,7 +34143,7 @@
     </row>
     <row r="229" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A229" s="3" t="s">
-        <v>1135</v>
+        <v>1134</v>
       </c>
       <c r="B229" s="5" t="b">
         <v>1</v>
@@ -34191,7 +34199,7 @@
     </row>
     <row r="230" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A230" s="3" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
       <c r="B230" s="5" t="b">
         <v>1</v>
@@ -34247,7 +34255,7 @@
     </row>
     <row r="231" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A231" s="3" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
       <c r="B231" s="5" t="b">
         <v>1</v>
@@ -34303,7 +34311,7 @@
     </row>
     <row r="232" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A232" s="3" t="s">
-        <v>1156</v>
+        <v>1155</v>
       </c>
       <c r="B232" s="5" t="b">
         <v>1</v>
@@ -34359,7 +34367,7 @@
     </row>
     <row r="233" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A233" s="3" t="s">
-        <v>1158</v>
+        <v>1157</v>
       </c>
       <c r="B233" s="5" t="b">
         <v>1</v>
@@ -34415,7 +34423,7 @@
     </row>
     <row r="234" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A234" s="3" t="s">
-        <v>1168</v>
+        <v>1167</v>
       </c>
       <c r="B234" s="5" t="b">
         <v>1</v>
@@ -34471,7 +34479,7 @@
     </row>
     <row r="235" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A235" s="3" t="s">
-        <v>1173</v>
+        <v>1172</v>
       </c>
       <c r="B235" s="5" t="b">
         <v>1</v>
@@ -34527,7 +34535,7 @@
     </row>
     <row r="236" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A236" s="3" t="s">
-        <v>1178</v>
+        <v>1177</v>
       </c>
       <c r="B236" s="5" t="b">
         <v>1</v>
@@ -34583,7 +34591,7 @@
     </row>
     <row r="237" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A237" s="3" t="s">
-        <v>1188</v>
+        <v>1187</v>
       </c>
       <c r="B237" s="5" t="b">
         <v>1</v>
@@ -34639,7 +34647,7 @@
     </row>
     <row r="238" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A238" s="3" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
       <c r="B238" s="5" t="b">
         <v>1</v>
@@ -34695,7 +34703,7 @@
     </row>
     <row r="239" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A239" s="3" t="s">
-        <v>1197</v>
+        <v>1196</v>
       </c>
       <c r="B239" s="5" t="b">
         <v>1</v>
@@ -34751,7 +34759,7 @@
     </row>
     <row r="240" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A240" s="3" t="s">
-        <v>1200</v>
+        <v>1199</v>
       </c>
       <c r="B240" s="5" t="b">
         <v>1</v>
@@ -34807,7 +34815,7 @@
     </row>
     <row r="241" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A241" s="3" t="s">
-        <v>1203</v>
+        <v>1202</v>
       </c>
       <c r="B241" s="5" t="b">
         <v>1</v>
@@ -34863,7 +34871,7 @@
     </row>
     <row r="242" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A242" s="3" t="s">
-        <v>1207</v>
+        <v>1206</v>
       </c>
       <c r="B242" s="5" t="b">
         <v>1</v>
@@ -34919,7 +34927,7 @@
     </row>
     <row r="243" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A243" s="3" t="s">
-        <v>1210</v>
+        <v>1209</v>
       </c>
       <c r="B243" s="5" t="b">
         <v>1</v>
@@ -34975,7 +34983,7 @@
     </row>
     <row r="244" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A244" s="3" t="s">
-        <v>1216</v>
+        <v>1215</v>
       </c>
       <c r="B244" s="5" t="b">
         <v>1</v>
@@ -35031,7 +35039,7 @@
     </row>
     <row r="245" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A245" s="3" t="s">
-        <v>1219</v>
+        <v>1218</v>
       </c>
       <c r="B245" s="5" t="b">
         <v>1</v>
@@ -35087,7 +35095,7 @@
     </row>
     <row r="246" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A246" s="3" t="s">
-        <v>1229</v>
+        <v>1228</v>
       </c>
       <c r="B246" s="5" t="b">
         <v>1</v>
@@ -35143,7 +35151,7 @@
     </row>
     <row r="247" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A247" s="3" t="s">
-        <v>1231</v>
+        <v>1230</v>
       </c>
       <c r="B247" s="5" t="b">
         <v>1</v>
@@ -35199,7 +35207,7 @@
     </row>
     <row r="248" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A248" s="3" t="s">
-        <v>1240</v>
+        <v>1239</v>
       </c>
       <c r="B248" s="5" t="b">
         <v>1</v>
@@ -35255,7 +35263,7 @@
     </row>
     <row r="249" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A249" s="3" t="s">
-        <v>1241</v>
+        <v>1240</v>
       </c>
       <c r="B249" s="5" t="b">
         <v>1</v>
@@ -35311,7 +35319,7 @@
     </row>
     <row r="250" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A250" s="3" t="s">
-        <v>1250</v>
+        <v>1249</v>
       </c>
       <c r="B250" s="5" t="b">
         <v>1</v>
@@ -35367,7 +35375,7 @@
     </row>
     <row r="251" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A251" s="3" t="s">
-        <v>1253</v>
+        <v>1252</v>
       </c>
       <c r="B251" s="5" t="b">
         <v>1</v>
@@ -35384,8 +35392,8 @@
       <c r="F251" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="G251" s="5" t="b">
-        <v>1</v>
+      <c r="G251" s="6" t="b">
+        <v>0</v>
       </c>
       <c r="H251" s="5" t="b">
         <v>1</v>
@@ -35405,8 +35413,8 @@
       <c r="M251" s="6" t="b">
         <v>0</v>
       </c>
-      <c r="N251" s="6" t="b">
-        <v>0</v>
+      <c r="N251" s="5" t="b">
+        <v>1</v>
       </c>
       <c r="O251" s="6" t="b">
         <v>0</v>
@@ -35423,7 +35431,7 @@
     </row>
     <row r="252" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A252" s="3" t="s">
-        <v>1261</v>
+        <v>1259</v>
       </c>
       <c r="B252" s="5" t="b">
         <v>1</v>
@@ -35479,7 +35487,7 @@
     </row>
     <row r="253" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A253" s="3" t="s">
-        <v>1269</v>
+        <v>1267</v>
       </c>
       <c r="B253" s="5" t="b">
         <v>1</v>
@@ -35535,7 +35543,7 @@
     </row>
     <row r="254" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A254" s="3" t="s">
-        <v>1279</v>
+        <v>1277</v>
       </c>
       <c r="B254" s="5" t="b">
         <v>1</v>

</xml_diff>

<commit_message>
generated all the reports on 2025-08-24
</commit_message>
<xml_diff>
--- a/report/merged_configurations.xlsx
+++ b/report/merged_configurations.xlsx
@@ -3821,34 +3821,34 @@
     <t>Applicatieprofiel Rooilijnplannen</t>
   </si>
   <si>
+    <t>rooilijnplannen-description.md</t>
+  </si>
+  <si>
+    <t>[{"name":"Applicatieprofiel Rooilijnplannen","resourceReference":"https://data.vlaanderen.be/doc/applicatieprofiel/rooilijnplannen/"}]</t>
+  </si>
+  <si>
+    <t>[{"name":"Vocabularium Rooilijnplannen","resourceReference":"https://data.vlaanderen.be/ns/rooilijnplannen/"}]</t>
+  </si>
+  <si>
+    <t>[{"name":"Verslag Business Werkgroep - 12 december 2024","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-rooilijnplannen/standaardenregister/reports/Verslag%20Business%20werkgroep%20OSLO%20Rooilijnplannen.pdf"},{"name":"Verslag Thematische Werkgroep 1 - 23 januari 2025","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-rooilijnplannen/standaardenregister/reports/Verslag%20Thematische%20werkgroep%201%20Rooilijnen.pdf"},{"name":"Verslag Thematische Werkgroep 2 - 20 februari 2025","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-rooilijnplannen/standaardenregister/reports/Verslag%20TW2%20OSLO%20Rooilijnen.pdf"},{"name":"Verslag Thematische Werkgroep 3 - 3 april 2025","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-rooilijnplannen/standaardenregister/reports/Verslag%20TW3%20OSLO%20Rooilijnen.pdf"},{"name":"Verslag Thematische Werkgroep 4 - 18 juni 2025","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-rooilijnplannen/standaardenregister/reports/Verslag%20TW4%20OSLO%20Rooilijnen.pdf"}]</t>
+  </si>
+  <si>
+    <t>{"name":"Charter Rooilijnplannen","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-rooilijnplannen/standaardenregister/charter/Werkgroep%20charter%20OSLO_Rooilijnplannen1%20(3).pdf"}</t>
+  </si>
+  <si>
+    <t>[{"name":"Presentatie Business Werkgroep -  12 december 2024","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-rooilijnplannen/standaardenregister/presentations/Business%20Werkgroep%20presentatie%20Rooilijnplannen.pdf"},{"name":"Presentatie Thematische Werkgroep 1 - 23 januari 2025","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-rooilijnplannen/standaardenregister/presentations/Presentatie%20thematische%20werkgroep%201%20-%20Rooilijnen.pdf"},{"name":"Presentatie Thematische Werkgroep 2 - 20 februari 2025","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-rooilijnplannen/standaardenregister/presentations/Presentatie%20thematische%20werkgroep%202%20-%20Rooilijnen.pdf"},{"name":"Presentatie Thematische Werkgroep 3 - 3 april 2025","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-rooilijnplannen/standaardenregister/presentations/Presentatie%20thematische%20werkgroep%203%20-%20Rooilijnen.pdf"},{"name":"Presentatie Thematische Werkgroep 4 - 18 juni 2025","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-rooilijnplannen/standaardenregister/presentations/Presentatie%20thematische%20werkgroep%204%20-%20Rooilijnen.pdf"}]</t>
+  </si>
+  <si>
+    <t>Charter Rooilijnplannen</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-rooilijnplannen/standaardenregister/charter/Werkgroep%20charter%20OSLO_Rooilijnplannen1%20(3).pdf</t>
+  </si>
+  <si>
+    <t>Vocabularium Rooilijnplannen</t>
+  </si>
+  <si>
     <t>https://data.vlaanderen.be/doc/concept/StandaardStatus/KandidaatStandaard</t>
-  </si>
-  <si>
-    <t>rooilijnplannen-description.md</t>
-  </si>
-  <si>
-    <t>[{"name":"Applicatieprofiel Rooilijnplannen","resourceReference":"https://data.vlaanderen.be/doc/applicatieprofiel/rooilijnplannen/"}]</t>
-  </si>
-  <si>
-    <t>[{"name":"Vocabularium Rooilijnplannen","resourceReference":"https://data.vlaanderen.be/ns/rooilijnplannen/"}]</t>
-  </si>
-  <si>
-    <t>[{"name":"Verslag Business Werkgroep - 12 december 2024","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-rooilijnplannen/standaardenregister/reports/Verslag%20Business%20werkgroep%20OSLO%20Rooilijnplannen.pdf"},{"name":"Verslag Thematische Werkgroep 1 - 23 januari 2025","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-rooilijnplannen/standaardenregister/reports/Verslag%20Thematische%20werkgroep%201%20Rooilijnen.pdf"},{"name":"Verslag Thematische Werkgroep 2 - 20 februari 2025","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-rooilijnplannen/standaardenregister/reports/Verslag%20TW2%20OSLO%20Rooilijnen.pdf"},{"name":"Verslag Thematische Werkgroep 3 - 3 april 2025","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-rooilijnplannen/standaardenregister/reports/Verslag%20TW3%20OSLO%20Rooilijnen.pdf"},{"name":"Verslag Thematische Werkgroep 4 - 18 juni 2025","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-rooilijnplannen/standaardenregister/reports/Verslag%20TW4%20OSLO%20Rooilijnen.pdf"}]</t>
-  </si>
-  <si>
-    <t>{"name":"Charter Rooilijnplannen","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-rooilijnplannen/standaardenregister/charter/Werkgroep%20charter%20OSLO_Rooilijnplannen1%20(3).pdf"}</t>
-  </si>
-  <si>
-    <t>[{"name":"Presentatie Business Werkgroep -  12 december 2024","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-rooilijnplannen/standaardenregister/presentations/Business%20Werkgroep%20presentatie%20Rooilijnplannen.pdf"},{"name":"Presentatie Thematische Werkgroep 1 - 23 januari 2025","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-rooilijnplannen/standaardenregister/presentations/Presentatie%20thematische%20werkgroep%201%20-%20Rooilijnen.pdf"},{"name":"Presentatie Thematische Werkgroep 2 - 20 februari 2025","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-rooilijnplannen/standaardenregister/presentations/Presentatie%20thematische%20werkgroep%202%20-%20Rooilijnen.pdf"},{"name":"Presentatie Thematische Werkgroep 3 - 3 april 2025","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-rooilijnplannen/standaardenregister/presentations/Presentatie%20thematische%20werkgroep%203%20-%20Rooilijnen.pdf"},{"name":"Presentatie Thematische Werkgroep 4 - 18 juni 2025","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-rooilijnplannen/standaardenregister/presentations/Presentatie%20thematische%20werkgroep%204%20-%20Rooilijnen.pdf"}]</t>
-  </si>
-  <si>
-    <t>Charter Rooilijnplannen</t>
-  </si>
-  <si>
-    <t>https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-rooilijnplannen/standaardenregister/charter/Werkgroep%20charter%20OSLO_Rooilijnplannen1%20(3).pdf</t>
-  </si>
-  <si>
-    <t>Vocabularium Rooilijnplannen</t>
   </si>
 </sst>
 </file>
@@ -4513,7 +4513,7 @@
         <v>45870</v>
       </c>
       <c r="Q4" s="4">
-        <v>46010</v>
+        <v>45989</v>
       </c>
       <c r="R4" s="3"/>
       <c r="S4" s="3" t="s">
@@ -4578,7 +4578,7 @@
         <v>45870</v>
       </c>
       <c r="Q5" s="4">
-        <v>46010</v>
+        <v>45989</v>
       </c>
       <c r="R5" s="3"/>
       <c r="S5" s="3" t="s">
@@ -21243,10 +21243,10 @@
         <v>39</v>
       </c>
       <c r="D253" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="E253" s="3" t="s">
         <v>1269</v>
-      </c>
-      <c r="E253" s="3" t="s">
-        <v>1270</v>
       </c>
       <c r="F253" s="3" t="s">
         <v>42</v>
@@ -21255,19 +21255,19 @@
         <v>45809</v>
       </c>
       <c r="H253" s="3" t="s">
+        <v>1270</v>
+      </c>
+      <c r="I253" s="3" t="s">
         <v>1271</v>
       </c>
-      <c r="I253" s="3" t="s">
+      <c r="J253" s="3" t="s">
         <v>1272</v>
       </c>
-      <c r="J253" s="3" t="s">
+      <c r="K253" s="3" t="s">
         <v>1273</v>
       </c>
-      <c r="K253" s="3" t="s">
+      <c r="L253" s="3" t="s">
         <v>1274</v>
-      </c>
-      <c r="L253" s="3" t="s">
-        <v>1275</v>
       </c>
       <c r="M253" s="4">
         <v>45666</v>
@@ -21291,10 +21291,10 @@
         <v>36</v>
       </c>
       <c r="T253" s="3" t="s">
+        <v>1275</v>
+      </c>
+      <c r="U253" s="3" t="s">
         <v>1276</v>
-      </c>
-      <c r="U253" s="3" t="s">
-        <v>1277</v>
       </c>
       <c r="V253" s="3" t="s">
         <v>51</v>
@@ -21305,7 +21305,7 @@
     </row>
     <row r="254" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A254" s="3" t="s">
-        <v>1278</v>
+        <v>1277</v>
       </c>
       <c r="B254" s="3" t="s">
         <v>61</v>
@@ -21314,10 +21314,10 @@
         <v>39</v>
       </c>
       <c r="D254" s="3" t="s">
+        <v>1278</v>
+      </c>
+      <c r="E254" s="3" t="s">
         <v>1269</v>
-      </c>
-      <c r="E254" s="3" t="s">
-        <v>1270</v>
       </c>
       <c r="F254" s="3" t="s">
         <v>42</v>
@@ -21326,19 +21326,19 @@
         <v>45809</v>
       </c>
       <c r="H254" s="3" t="s">
+        <v>1271</v>
+      </c>
+      <c r="I254" s="3" t="s">
+        <v>1270</v>
+      </c>
+      <c r="J254" s="3" t="s">
         <v>1272</v>
       </c>
-      <c r="I254" s="3" t="s">
-        <v>1271</v>
-      </c>
-      <c r="J254" s="3" t="s">
+      <c r="K254" s="3" t="s">
         <v>1273</v>
       </c>
-      <c r="K254" s="3" t="s">
+      <c r="L254" s="3" t="s">
         <v>1274</v>
-      </c>
-      <c r="L254" s="3" t="s">
-        <v>1275</v>
       </c>
       <c r="M254" s="4">
         <v>45666</v>
@@ -21362,10 +21362,10 @@
         <v>36</v>
       </c>
       <c r="T254" s="3" t="s">
+        <v>1275</v>
+      </c>
+      <c r="U254" s="3" t="s">
         <v>1276</v>
-      </c>
-      <c r="U254" s="3" t="s">
-        <v>1277</v>
       </c>
       <c r="V254" s="3" t="s">
         <v>51</v>
@@ -35558,7 +35558,7 @@
     </row>
     <row r="254" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A254" s="3" t="s">
-        <v>1278</v>
+        <v>1277</v>
       </c>
       <c r="B254" s="5" t="b">
         <v>1</v>

</xml_diff>

<commit_message>
generated all the reports on 2025-09-07
</commit_message>
<xml_diff>
--- a/report/merged_configurations.xlsx
+++ b/report/merged_configurations.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4746" uniqueCount="1279">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4744" uniqueCount="1279">
   <si>
     <t>title</t>
   </si>
@@ -21005,10 +21005,10 @@
         <v>24</v>
       </c>
       <c r="P249" s="4">
-        <v>45839</v>
-      </c>
-      <c r="Q249" s="3" t="s">
-        <v>24</v>
+        <v>45860</v>
+      </c>
+      <c r="Q249" s="4">
+        <v>45952</v>
       </c>
       <c r="R249" s="3"/>
       <c r="S249" s="3" t="s">
@@ -21074,10 +21074,10 @@
         <v>24</v>
       </c>
       <c r="P250" s="4">
-        <v>45839</v>
-      </c>
-      <c r="Q250" s="3" t="s">
-        <v>24</v>
+        <v>45860</v>
+      </c>
+      <c r="Q250" s="4">
+        <v>45952</v>
       </c>
       <c r="R250" s="3"/>
       <c r="S250" s="3" t="s">
@@ -35319,8 +35319,8 @@
       <c r="N249" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="O249" s="6" t="b">
-        <v>0</v>
+      <c r="O249" s="5" t="b">
+        <v>1</v>
       </c>
       <c r="P249" s="6" t="b">
         <v>0</v>
@@ -35375,8 +35375,8 @@
       <c r="N250" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="O250" s="6" t="b">
-        <v>0</v>
+      <c r="O250" s="5" t="b">
+        <v>1</v>
       </c>
       <c r="P250" s="6" t="b">
         <v>0</v>

</xml_diff>

<commit_message>
generated all the reports on 2025-09-14
</commit_message>
<xml_diff>
--- a/report/merged_configurations.xlsx
+++ b/report/merged_configurations.xlsx
@@ -425,31 +425,31 @@
     <t>Applicatieprofiel Kabels en Leidingen</t>
   </si>
   <si>
+    <t>kabels-en-leidingen-description.md</t>
+  </si>
+  <si>
+    <t>[{"name":"Kabels en Leidingen Applicatieprofiel","resourceReference":"https://data.vlaanderen.be/doc/applicatieprofiel/kabels-en-leidingen"},{"name":"Cables and Pipes Application profile","resourceReference":"https://data.vlaanderen.be/doc/applicatieprofiel/kabels-en-leidingen/index_en.html"},{"name":"Câbles et Conduites Profil d'application","resourceReference":"https://data.vlaanderen.be/doc/applicatieprofiel/kabels-en-leidingen/index_fr.html"}]</t>
+  </si>
+  <si>
+    <t>[{"name":"Verslag business werkgroep - 24 april 2023","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-imkl/standaardenregister/reports/Verslag Business Workshop IMKL.pdf"},{"name":"Verslag thematische werkgroep 1 - 25 mei 2023","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-imkl/standaardenregister/reports/Verslag Thematische Werkgroep 1 IMKL.pdf"},{"name":"Verslag thematische werkgroep 2 - 29 juni 2023","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-imkl/standaardenregister/reports/Verslag Thematische Werkgroep 2 IMKL.pdf"},{"name":"Verslag thematische werkgroep 3 - 7 september 2023","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-imkl/standaardenregister/reports/Verslag Thematische Werkgroep 3 IMKL.pdf"},{"name":"Verslag thematische werkgroep 4 - 5 oktober 2023","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-imkl/standaardenregister/reports/Verslag Thematische Werkgroep 4 IMKL.pdf"},{"name":"Verslag Webinar Publieke Review IMKL - 28 november 2023","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-imkl/standaardenregister/reports/Verslag Webinar IMKL 28.11.2023.pdf"},{"name":"Technisch Rapport NL","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-imkl/standaardenregister/reports/Technisch rapport OSLO IMKL - NL (3).pdf"},{"name":"Technisch Rapport FR","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-imkl/standaardenregister/reports/Technisch rapport OSLO IMKL - FR.pdf"}]</t>
+  </si>
+  <si>
+    <t>{"name":"Charter","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-imkl/standaardenregister/charter/Charter OSLO IMKL.docx"}</t>
+  </si>
+  <si>
+    <t>[{"name":"Presentatie business werkgroep - 24 april 2023","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-imkl/standaardenregister/presentations/Business Werkgroep presentatie IMKL - 24 april 2023.pdf"},{"name":"Presentatie thematische werkgroep 1 - 25 mei 2023","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-imkl/standaardenregister/presentations/Presentatie eerste thematische werkgroep - IMKL -  25 mei 2023.pdf"},{"name":"Presentatie thematische werkgroep 2 - 29 juni 2023","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-imkl/standaardenregister/presentations/Presentatie tweede thematische werkgroep - IMKL -  29 juni 2023.pdf"},{"name":"Presentatie thematische werkgroep 3 - 7 september 2023","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-imkl/standaardenregister/presentations/Presentatie derde thematische werkgroep - IMKL - 7 september  2023.pdf"},{"name":"Presentatie thematische werkgroep 4 - 5 oktober 2023","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-imkl/standaardenregister/presentations/Presentatie vierde thematische werkgroep - IMKL - 5 oktober 2023.pdf"},{"name":"Presentatie Webinar Publieke Review IMKL - 28 november 2023","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-imkl/standaardenregister/presentations/Presentatie Webinar Publieke Review.pdf"}]</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-imkl/standaardenregister/charter/Charter OSLO IMKL.docx</t>
+  </si>
+  <si>
+    <t>OSLOthema-imkl</t>
+  </si>
+  <si>
+    <t>Vocabularium Nutsvoorzieningen</t>
+  </si>
+  <si>
     <t>https://data.vlaanderen.be/id/concept/StandaardStatus/OntwerpStandaard</t>
-  </si>
-  <si>
-    <t>kabels-en-leidingen-description.md</t>
-  </si>
-  <si>
-    <t>[{"name":"Kabels en Leidingen Applicatieprofiel","resourceReference":"https://data.vlaanderen.be/doc/applicatieprofiel/kabels-en-leidingen"},{"name":"Cables and Pipes Application profile","resourceReference":"https://data.vlaanderen.be/doc/applicatieprofiel/kabels-en-leidingen/index_en.html"},{"name":"Câbles et Conduites Profil d'application","resourceReference":"https://data.vlaanderen.be/doc/applicatieprofiel/kabels-en-leidingen/index_fr.html"}]</t>
-  </si>
-  <si>
-    <t>[{"name":"Verslag business werkgroep - 24 april 2023","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-imkl/standaardenregister/reports/Verslag Business Workshop IMKL.pdf"},{"name":"Verslag thematische werkgroep 1 - 25 mei 2023","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-imkl/standaardenregister/reports/Verslag Thematische Werkgroep 1 IMKL.pdf"},{"name":"Verslag thematische werkgroep 2 - 29 juni 2023","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-imkl/standaardenregister/reports/Verslag Thematische Werkgroep 2 IMKL.pdf"},{"name":"Verslag thematische werkgroep 3 - 7 september 2023","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-imkl/standaardenregister/reports/Verslag Thematische Werkgroep 3 IMKL.pdf"},{"name":"Verslag thematische werkgroep 4 - 5 oktober 2023","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-imkl/standaardenregister/reports/Verslag Thematische Werkgroep 4 IMKL.pdf"},{"name":"Verslag Webinar Publieke Review IMKL - 28 november 2023","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-imkl/standaardenregister/reports/Verslag Webinar IMKL 28.11.2023.pdf"},{"name":"Technisch Rapport NL","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-imkl/standaardenregister/reports/Technisch rapport OSLO IMKL - NL (3).pdf"},{"name":"Technisch Rapport FR","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-imkl/standaardenregister/reports/Technisch rapport OSLO IMKL - FR.pdf"}]</t>
-  </si>
-  <si>
-    <t>{"name":"Charter","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-imkl/standaardenregister/charter/Charter OSLO IMKL.docx"}</t>
-  </si>
-  <si>
-    <t>[{"name":"Presentatie business werkgroep - 24 april 2023","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-imkl/standaardenregister/presentations/Business Werkgroep presentatie IMKL - 24 april 2023.pdf"},{"name":"Presentatie thematische werkgroep 1 - 25 mei 2023","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-imkl/standaardenregister/presentations/Presentatie eerste thematische werkgroep - IMKL -  25 mei 2023.pdf"},{"name":"Presentatie thematische werkgroep 2 - 29 juni 2023","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-imkl/standaardenregister/presentations/Presentatie tweede thematische werkgroep - IMKL -  29 juni 2023.pdf"},{"name":"Presentatie thematische werkgroep 3 - 7 september 2023","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-imkl/standaardenregister/presentations/Presentatie derde thematische werkgroep - IMKL - 7 september  2023.pdf"},{"name":"Presentatie thematische werkgroep 4 - 5 oktober 2023","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-imkl/standaardenregister/presentations/Presentatie vierde thematische werkgroep - IMKL - 5 oktober 2023.pdf"},{"name":"Presentatie Webinar Publieke Review IMKL - 28 november 2023","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-imkl/standaardenregister/presentations/Presentatie Webinar Publieke Review.pdf"}]</t>
-  </si>
-  <si>
-    <t>https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-imkl/standaardenregister/charter/Charter OSLO IMKL.docx</t>
-  </si>
-  <si>
-    <t>OSLOthema-imkl</t>
-  </si>
-  <si>
-    <t>Vocabularium Nutsvoorzieningen</t>
   </si>
   <si>
     <t>[{"name":"Nutsvoorzieningen Vocabularium","resourceReference":"https://data.vlaanderen.be/ns/nutsvoorzieningen"},{"name":"Utility Services Vocabularium","resourceReference":"https://data.vlaanderen.be/ns/nutsvoorzieningen/index_en.html"},{"name":"Câbles et Conduites Vocabulaire","resourceReference":"https://data.vlaanderen.be/doc/applicatieprofiel/kabels-en-leidingen/index_fr.html"}]</t>
@@ -5404,31 +5404,29 @@
         <v>39</v>
       </c>
       <c r="D18" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="E18" s="3" t="s">
         <v>137</v>
-      </c>
-      <c r="E18" s="3" t="s">
-        <v>138</v>
       </c>
       <c r="F18" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="G18" s="4">
-        <v>44974</v>
-      </c>
+      <c r="G18" s="3"/>
       <c r="H18" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="I18" s="3" t="s">
         <v>28</v>
       </c>
       <c r="J18" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="K18" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="K18" s="3" t="s">
+      <c r="L18" s="3" t="s">
         <v>141</v>
-      </c>
-      <c r="L18" s="3" t="s">
-        <v>142</v>
       </c>
       <c r="M18" s="4">
         <v>44974</v>
@@ -5451,18 +5449,18 @@
         <v>87</v>
       </c>
       <c r="U18" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="V18" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="W18" s="3" t="s">
         <v>143</v>
-      </c>
-      <c r="V18" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="W18" s="3" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="19" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>61</v>
@@ -5471,10 +5469,10 @@
         <v>39</v>
       </c>
       <c r="D19" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="E19" s="3" t="s">
         <v>137</v>
-      </c>
-      <c r="E19" s="3" t="s">
-        <v>138</v>
       </c>
       <c r="F19" s="3" t="s">
         <v>42</v>
@@ -5489,10 +5487,10 @@
         <v>28</v>
       </c>
       <c r="J19" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="K19" s="3" t="s">
         <v>140</v>
-      </c>
-      <c r="K19" s="3" t="s">
-        <v>141</v>
       </c>
       <c r="L19" s="3" t="s">
         <v>147</v>
@@ -5518,13 +5516,13 @@
         <v>87</v>
       </c>
       <c r="U19" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="V19" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="W19" s="3" t="s">
         <v>143</v>
-      </c>
-      <c r="V19" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="W19" s="3" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="20" spans="1:23" x14ac:dyDescent="0.25">
@@ -5538,7 +5536,7 @@
         <v>39</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>137</v>
+        <v>145</v>
       </c>
       <c r="E20" s="3" t="s">
         <v>149</v>
@@ -5605,7 +5603,7 @@
         <v>39</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>137</v>
+        <v>145</v>
       </c>
       <c r="E21" s="3" t="s">
         <v>149</v>
@@ -5810,7 +5808,7 @@
         <v>39</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>137</v>
+        <v>145</v>
       </c>
       <c r="E24" s="3" t="s">
         <v>172</v>
@@ -6287,7 +6285,7 @@
         <v>39</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>137</v>
+        <v>145</v>
       </c>
       <c r="E31" s="3" t="s">
         <v>227</v>
@@ -6354,7 +6352,7 @@
         <v>39</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>137</v>
+        <v>145</v>
       </c>
       <c r="E32" s="3" t="s">
         <v>227</v>
@@ -6973,7 +6971,7 @@
         <v>39</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>137</v>
+        <v>145</v>
       </c>
       <c r="E41" s="3" t="s">
         <v>227</v>
@@ -7040,7 +7038,7 @@
         <v>39</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>137</v>
+        <v>145</v>
       </c>
       <c r="E42" s="3" t="s">
         <v>227</v>
@@ -7245,7 +7243,7 @@
         <v>39</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>137</v>
+        <v>145</v>
       </c>
       <c r="E45" s="3" t="s">
         <v>227</v>
@@ -7312,7 +7310,7 @@
         <v>39</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>137</v>
+        <v>145</v>
       </c>
       <c r="E46" s="3" t="s">
         <v>227</v>
@@ -17703,7 +17701,7 @@
         <v>24</v>
       </c>
       <c r="D201" s="3" t="s">
-        <v>137</v>
+        <v>145</v>
       </c>
       <c r="E201" s="3" t="s">
         <v>962</v>
@@ -17975,7 +17973,7 @@
         <v>39</v>
       </c>
       <c r="D205" s="3" t="s">
-        <v>137</v>
+        <v>145</v>
       </c>
       <c r="E205" s="3" t="s">
         <v>988</v>
@@ -18854,7 +18852,7 @@
         <v>39</v>
       </c>
       <c r="D218" s="3" t="s">
-        <v>137</v>
+        <v>145</v>
       </c>
       <c r="E218" s="3" t="s">
         <v>1066</v>
@@ -19199,7 +19197,7 @@
         <v>39</v>
       </c>
       <c r="D223" s="3" t="s">
-        <v>137</v>
+        <v>145</v>
       </c>
       <c r="E223" s="3" t="s">
         <v>1103</v>
@@ -19266,7 +19264,7 @@
         <v>39</v>
       </c>
       <c r="D224" s="3" t="s">
-        <v>137</v>
+        <v>145</v>
       </c>
       <c r="E224" s="3" t="s">
         <v>1103</v>
@@ -20835,7 +20833,7 @@
         <v>39</v>
       </c>
       <c r="D247" s="3" t="s">
-        <v>137</v>
+        <v>145</v>
       </c>
       <c r="E247" s="3" t="s">
         <v>1232</v>
@@ -20902,7 +20900,7 @@
         <v>39</v>
       </c>
       <c r="D248" s="3" t="s">
-        <v>137</v>
+        <v>145</v>
       </c>
       <c r="E248" s="3" t="s">
         <v>1232</v>
@@ -21107,7 +21105,7 @@
         <v>39</v>
       </c>
       <c r="D251" s="3" t="s">
-        <v>137</v>
+        <v>145</v>
       </c>
       <c r="E251" s="3"/>
       <c r="F251" s="3" t="s">
@@ -22347,8 +22345,8 @@
       <c r="B18" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="C18" s="5" t="b">
-        <v>1</v>
+      <c r="C18" s="6" t="b">
+        <v>0</v>
       </c>
       <c r="D18" s="5" t="b">
         <v>1</v>
@@ -22398,7 +22396,7 @@
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B19" s="5" t="b">
         <v>1</v>

</xml_diff>

<commit_message>
generated all the reports on 2025-11-02
</commit_message>
<xml_diff>
--- a/report/merged_configurations.xlsx
+++ b/report/merged_configurations.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5029" uniqueCount="1285">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5053" uniqueCount="1285">
   <si>
     <t>title</t>
   </si>
@@ -4274,7 +4274,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X255"/>
+  <dimension ref="A1:X256"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="24" width="44" customWidth="1"/>
@@ -22230,6 +22230,78 @@
         <v>36</v>
       </c>
     </row>
+    <row r="256" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A256" s="3" t="s">
+        <v>432</v>
+      </c>
+      <c r="B256" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="C256" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="D256" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="E256" s="3" t="s">
+        <v>433</v>
+      </c>
+      <c r="F256" s="3" t="s">
+        <v>434</v>
+      </c>
+      <c r="G256" s="3" t="s">
+        <v>435</v>
+      </c>
+      <c r="H256" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="I256" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="J256" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="K256" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="L256" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="M256" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="N256" s="3" t="s">
+        <v>436</v>
+      </c>
+      <c r="O256" s="3" t="s">
+        <v>437</v>
+      </c>
+      <c r="P256" s="3" t="s">
+        <v>438</v>
+      </c>
+      <c r="Q256" s="3" t="s">
+        <v>439</v>
+      </c>
+      <c r="R256" s="3" t="s">
+        <v>440</v>
+      </c>
+      <c r="S256" s="3" t="s">
+        <v>441</v>
+      </c>
+      <c r="T256" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="U256" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="V256" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="W256" s="3" t="s">
+        <v>442</v>
+      </c>
+      <c r="X256" s="3"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
@@ -22238,7 +22310,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R255"/>
+  <dimension ref="A1:R256"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="18" width="44" customWidth="1"/>
@@ -36524,6 +36596,62 @@
         <v>1</v>
       </c>
     </row>
+    <row r="256" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A256" s="3" t="s">
+        <v>432</v>
+      </c>
+      <c r="B256" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="C256" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="D256" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="E256" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="F256" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="G256" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="H256" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="I256" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="J256" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="K256" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="L256" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="M256" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="N256" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="O256" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="P256" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q256" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="R256" s="6" t="b">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>

</xml_diff>

<commit_message>
generated all the reports on 2025-11-09
</commit_message>
<xml_diff>
--- a/report/merged_configurations.xlsx
+++ b/report/merged_configurations.xlsx
@@ -2513,19 +2513,19 @@
     <t>https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-metadataVoorServices/standaardenregister/charter/Charter_OSLO_DCAT3.0.pdf</t>
   </si>
   <si>
-    <t>[{"name":"Verslag webinar 1 - 17 september 2025","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-metadataVoorServices/standaardenregister/reports/Verslag%20webinar%20één%20-%2017%20september%202025.pdf"}]</t>
-  </si>
-  <si>
-    <t>[{"name":"Presentatie webinar 1 - 17 september 2025","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-metadataVoorServices/standaardenregister/presentations/Presentatie%20webinar%20één%20-%2017%20september%202025.pdf"}]</t>
+    <t>[{"name":"Verslag webinar 1 - 17 september 2025","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-metadataVoorServices/standaardenregister/reports/Verslag%20webinar%20één%20-%2017%20september%202025.pdf"},{"name":"Verslag webinar 2 - 21 oktober 2025","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-metadataVoorServices/standaardenregister/reports/Verslag_Webinar_2_DCAT-AP.3.0.pdf"}]</t>
+  </si>
+  <si>
+    <t>[{"name":"Presentatie webinar 1 - 17 september 2025","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-metadataVoorServices/standaardenregister/presentations/Presentatie%20webinar%20één%20-%2017%20september%202025.pdf"},{"name":"Presentatie webinar 2 - 21 oktober 2025","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-metadataVoorServices/standaardenregister/presentations/Presentatie_webinar_2_OLSO_DCAT-AP3.0.pdf"}]</t>
   </si>
   <si>
     <t>{"name":"Charter OSLO DCAT-AP 3.0","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-metadataVoorServices/standaardenregister/charter/Charter_OSLO_DCAT3.0.pdf"}</t>
   </si>
   <si>
-    <t>Vocabularium metadata DCAT-AP 3.0</t>
-  </si>
-  <si>
-    <t>[{"name":"Vocabularium metadata DCAT-AP 3.0","resourceReference":"https://data.vlaanderen.be/doc/vocabularium/metadata-dcat/ontwerpstandaard/2025-09-16/"}]</t>
+    <t>Vocabularium metadata DCAT 3.0</t>
+  </si>
+  <si>
+    <t>[{"name":"Vocabularium metadata DCAT 3.0","resourceReference":"https://data.vlaanderen.be/doc/vocabularium/metadata-dcat/ontwerpstandaard/2025-09-16/"}]</t>
   </si>
   <si>
     <t>wegenenverkeer implementatiemodel AIM Object</t>
@@ -15449,7 +15449,7 @@
         <v>836</v>
       </c>
       <c r="B160" s="3" t="s">
-        <v>25</v>
+        <v>71</v>
       </c>
       <c r="C160" s="3" t="s">
         <v>26</v>

</xml_diff>

<commit_message>
generated all the reports on 2025-11-23
</commit_message>
<xml_diff>
--- a/report/merged_configurations.xlsx
+++ b/report/merged_configurations.xlsx
@@ -2504,7 +2504,7 @@
     <t>metadata.md</t>
   </si>
   <si>
-    <t>[{"name":"Applicatieprofiel metadata DCAT-AP 3.0","resourceReference":"https://data.vlaanderen.be/doc/applicatieprofiel/metadata-dcat/ontwerpstandaard/2025-09-16/"}]</t>
+    <t>[{"name":"Applicatieprofiel metadata DCAT-AP 3.0","resourceReference":"https://data.vlaanderen.be/doc/applicatieprofiel/metadata-dcat/"}]</t>
   </si>
   <si>
     <t>Charter OSLO DCAT-AP 3.0</t>
@@ -2525,7 +2525,7 @@
     <t>Vocabularium metadata DCAT 3.0</t>
   </si>
   <si>
-    <t>[{"name":"Vocabularium metadata DCAT 3.0","resourceReference":"https://data.vlaanderen.be/doc/vocabularium/metadata-dcat/ontwerpstandaard/2025-09-16/"}]</t>
+    <t>[{"name":"Vocabularium metadata DCAT 3.0","resourceReference":"https://data.vlaanderen.be/doc/vocabularium/metadata-dcat/"}]</t>
   </si>
   <si>
     <t>wegenenverkeer implementatiemodel AIM Object</t>

</xml_diff>

<commit_message>
generated all the reports on 2025-12-28
</commit_message>
<xml_diff>
--- a/report/merged_configurations.xlsx
+++ b/report/merged_configurations.xlsx
@@ -164,7 +164,7 @@
     <t>{"name":"Charter Thermografische Gebouwanalyse","resourceReference":"https://raw.githubusercontent.com/Informatievlaanderen/OSLOthema-thermAI/standaardenregister/charter/Charter_OSLO_thermAI.pdf"}</t>
   </si>
   <si>
-    <t>Applicatieprofiel Leermiddelen- en doelen</t>
+    <t>Applicatieprofiel Leermiddelen en -doelen</t>
   </si>
   <si>
     <t>[{"name":"Departement Onderwijs en Vorming","resourceReference":"https://data.vlaanderen.be/id/organisatie/OVO000049"}]</t>
@@ -173,7 +173,7 @@
     <t>ap-leermiddelen-config.md</t>
   </si>
   <si>
-    <t>[{"name":"Applicatieprofiel Leermiddelen- en doelen","resourceReference":"https://data.vlaanderen.be/doc/applicatieprofiel/leermiddelen"}]</t>
+    <t>[{"name":"Applicatieprofiel Leermiddelen en -doelen","resourceReference":"https://data.vlaanderen.be/doc/applicatieprofiel/leermiddelen"}]</t>
   </si>
   <si>
     <t>Charter OSLO Leermiddelen- en doelen</t>

</xml_diff>

<commit_message>
generated all the reports on 2026-02-15
</commit_message>
<xml_diff>
--- a/report/merged_configurations.xlsx
+++ b/report/merged_configurations.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5301" uniqueCount="1281">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5353" uniqueCount="1281">
   <si>
     <t>title</t>
   </si>
@@ -4262,7 +4262,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y256"/>
+  <dimension ref="A1:Y258"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="25" width="44" customWidth="1"/>
@@ -23071,6 +23071,160 @@
         <v>446</v>
       </c>
       <c r="Y256" s="3"/>
+    </row>
+    <row r="257" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A257" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B257" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C257" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D257" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E257" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="F257" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="G257" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="H257" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="I257" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="J257" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="K257" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="L257" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="M257" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="N257" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="O257" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="P257" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q257" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="R257" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="S257" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="T257" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="U257" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="V257" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="W257" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="X257" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="Y257" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="258" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A258" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B258" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C258" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D258" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E258" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="F258" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="G258" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="H258" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="I258" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="J258" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="K258" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="L258" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="M258" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="N258" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="O258" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="P258" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q258" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="R258" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="S258" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="T258" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="U258" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="V258" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="W258" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="X258" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="Y258" s="3" t="s">
+        <v>37</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -23080,7 +23234,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R256"/>
+  <dimension ref="A1:R258"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="18" width="44" customWidth="1"/>
@@ -37422,6 +37576,118 @@
         <v>0</v>
       </c>
     </row>
+    <row r="257" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A257" s="3" t="s">
+        <v>436</v>
+      </c>
+      <c r="B257" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="C257" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D257" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="E257" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="F257" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="G257" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="H257" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="I257" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="J257" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="K257" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="L257" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="M257" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="N257" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="O257" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="P257" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q257" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="R257" s="6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="258" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A258" s="3" t="s">
+        <v>436</v>
+      </c>
+      <c r="B258" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="C258" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D258" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="E258" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="F258" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="G258" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="H258" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="I258" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="J258" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="K258" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="L258" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="M258" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="N258" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="O258" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="P258" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q258" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="R258" s="6" t="b">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>

</xml_diff>